<commit_message>
🔄 Actualización automática del mapa (2025-07-18 07:34:25)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_NEW.xlsx
+++ b/mapa_interactivo_NEW.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P54"/>
+  <dimension ref="A1:P58"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4527,6 +4527,310 @@
         </is>
       </c>
     </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>6437</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>7/17/2025</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>MILLER 4590</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>808400306</t>
+        </is>
+      </c>
+      <c r="F55" t="inlineStr">
+        <is>
+          <t>NEW</t>
+        </is>
+      </c>
+      <c r="G55" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H55" t="inlineStr">
+        <is>
+          <t>Columna corroida</t>
+        </is>
+      </c>
+      <c r="I55" t="n">
+        <v>1</v>
+      </c>
+      <c r="J55" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K55" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L55" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M55" t="n">
+        <v>-58.495482</v>
+      </c>
+      <c r="N55" t="n">
+        <v>-34.552614</v>
+      </c>
+      <c r="O55" t="inlineStr">
+        <is>
+          <t>Saavedra</t>
+        </is>
+      </c>
+      <c r="P55" t="inlineStr">
+        <is>
+          <t>Capital Norte</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>6447</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>7/17/2025</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>CIUDAD DE LA PAZ 1535</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>13</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>808400333</t>
+        </is>
+      </c>
+      <c r="F56" t="inlineStr">
+        <is>
+          <t>NEW</t>
+        </is>
+      </c>
+      <c r="G56" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H56" t="inlineStr">
+        <is>
+          <t>Picada</t>
+        </is>
+      </c>
+      <c r="I56" t="n">
+        <v>1</v>
+      </c>
+      <c r="J56" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K56" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L56" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M56" t="n">
+        <v>-58.453124</v>
+      </c>
+      <c r="N56" t="n">
+        <v>-34.567382</v>
+      </c>
+      <c r="O56" t="inlineStr">
+        <is>
+          <t>Colegiales</t>
+        </is>
+      </c>
+      <c r="P56" t="inlineStr">
+        <is>
+          <t>Capital Norte</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>-519</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>7/17/2025</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>Vilela 2687</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>808400334</t>
+        </is>
+      </c>
+      <c r="F57" t="inlineStr">
+        <is>
+          <t>NEW</t>
+        </is>
+      </c>
+      <c r="G57" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H57" t="inlineStr">
+        <is>
+          <t>CAmbiar columna 114 picada en base</t>
+        </is>
+      </c>
+      <c r="I57" t="n">
+        <v>1</v>
+      </c>
+      <c r="J57" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K57" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L57" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M57" t="n">
+        <v>-58.472968</v>
+      </c>
+      <c r="N57" t="n">
+        <v>-34.546898</v>
+      </c>
+      <c r="O57" t="inlineStr">
+        <is>
+          <t>Saavedra</t>
+        </is>
+      </c>
+      <c r="P57" t="inlineStr">
+        <is>
+          <t>Capital Norte</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>-520</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>7/17/2025</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>Pedraza Manuela 4101</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>808400353</t>
+        </is>
+      </c>
+      <c r="F58" t="inlineStr">
+        <is>
+          <t>NEW</t>
+        </is>
+      </c>
+      <c r="G58" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H58" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Podrida en la base </t>
+        </is>
+      </c>
+      <c r="I58" t="n">
+        <v>1</v>
+      </c>
+      <c r="J58" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K58" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L58" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M58" t="n">
+        <v>-58.481569</v>
+      </c>
+      <c r="N58" t="n">
+        <v>-34.559853</v>
+      </c>
+      <c r="O58" t="inlineStr">
+        <is>
+          <t>Saavedra</t>
+        </is>
+      </c>
+      <c r="P58" t="inlineStr">
+        <is>
+          <t>Capital Norte</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-07-18 14:02:00)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_NEW.xlsx
+++ b/mapa_interactivo_NEW.xlsx
@@ -1444,12 +1444,12 @@
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
+          <t>Pendiente</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t xml:space="preserve">Cambiar columna 114 base corroida columna con movimiento </t>
+          <t>Retirar columna ya traspasaron el nodo</t>
         </is>
       </c>
       <c r="I14" t="n">

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-07-21 07:31:02)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_NEW.xlsx
+++ b/mapa_interactivo_NEW.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P58"/>
+  <dimension ref="A1:P57"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2250,7 +2250,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>5700</t>
+          <t>6173</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -2260,17 +2260,17 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>ESTOMBA 2119</t>
+          <t>ARMENIA 2321</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>805507349</t>
+          <t>805507398</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
@@ -2285,7 +2285,7 @@
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>Aplomar</t>
+          <t>Picada volvio a entrar como caso 6325</t>
         </is>
       </c>
       <c r="I25" t="n">
@@ -2293,7 +2293,7 @@
       </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K25" t="inlineStr">
@@ -2307,46 +2307,46 @@
         </is>
       </c>
       <c r="M25" t="n">
-        <v>-58.471481</v>
+        <v>-58.420549</v>
       </c>
       <c r="N25" t="n">
-        <v>-34.570441</v>
+        <v>-34.585103</v>
       </c>
       <c r="O25" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P25" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>6173</t>
+          <t>5715</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>4/29/2025</t>
+          <t>5/1/2025</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>ARMENIA 2321</t>
+          <t>CUENCA 4690</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>805507398</t>
+          <t>805579094</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
@@ -2361,7 +2361,7 @@
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>Picada volvio a entrar como caso 6325</t>
+          <t>Aplomar poste</t>
         </is>
       </c>
       <c r="I26" t="n">
@@ -2369,7 +2369,7 @@
       </c>
       <c r="J26" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K26" t="inlineStr">
@@ -2379,30 +2379,30 @@
       </c>
       <c r="L26" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M26" t="n">
-        <v>-58.420549</v>
+        <v>-58.506061</v>
       </c>
       <c r="N26" t="n">
-        <v>-34.585103</v>
+        <v>-34.588887</v>
       </c>
       <c r="O26" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P26" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>5715</t>
+          <t>5719</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -2412,7 +2412,7 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>CUENCA 4690</t>
+          <t>CABEZON, JOSE LEON 2440</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
@@ -2422,7 +2422,7 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>805579094</t>
+          <t>805579157</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
@@ -2437,7 +2437,7 @@
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>Aplomar poste</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I27" t="n">
@@ -2445,7 +2445,7 @@
       </c>
       <c r="J27" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K27" t="inlineStr">
@@ -2455,14 +2455,14 @@
       </c>
       <c r="L27" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M27" t="n">
-        <v>-58.506061</v>
+        <v>-58.499967</v>
       </c>
       <c r="N27" t="n">
-        <v>-34.588887</v>
+        <v>-34.57974</v>
       </c>
       <c r="O27" t="inlineStr">
         <is>
@@ -2478,7 +2478,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>5719</t>
+          <t>5720</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -2488,7 +2488,7 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>CABEZON, JOSE LEON 2440</t>
+          <t>CABEZON, JOSE LEON 2398</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
@@ -2498,7 +2498,7 @@
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>805579157</t>
+          <t>805579172</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
@@ -2535,10 +2535,10 @@
         </is>
       </c>
       <c r="M28" t="n">
-        <v>-58.499967</v>
+        <v>-58.499355</v>
       </c>
       <c r="N28" t="n">
-        <v>-34.57974</v>
+        <v>-34.579354</v>
       </c>
       <c r="O28" t="inlineStr">
         <is>
@@ -2554,7 +2554,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>5720</t>
+          <t>6333</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -2564,17 +2564,17 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>CABEZON, JOSE LEON 2398</t>
+          <t>ORTEGA Y GASSET 1816</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>805579172</t>
+          <t>805655342</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
@@ -2611,46 +2611,46 @@
         </is>
       </c>
       <c r="M29" t="n">
-        <v>-58.499355</v>
+        <v>-58.432556</v>
       </c>
       <c r="N29" t="n">
-        <v>-34.579354</v>
+        <v>-34.570279</v>
       </c>
       <c r="O29" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P29" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>6333</t>
+          <t>5847</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>5/1/2025</t>
+          <t>5/8/2025</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>ORTEGA Y GASSET 1816</t>
+          <t>JURAMENTO 5321</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>805655342</t>
+          <t>805791839</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
@@ -2687,46 +2687,46 @@
         </is>
       </c>
       <c r="M30" t="n">
-        <v>-58.432556</v>
+        <v>-58.485193</v>
       </c>
       <c r="N30" t="n">
-        <v>-34.570279</v>
+        <v>-34.579621</v>
       </c>
       <c r="O30" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P30" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>5847</t>
+          <t>232</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>5/8/2025</t>
+          <t>5/9/2025</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>JURAMENTO 5321</t>
+          <t>Gorostiaga 2286</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>805791839</t>
+          <t>805791858</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
@@ -2763,46 +2763,46 @@
         </is>
       </c>
       <c r="M31" t="n">
-        <v>-58.485193</v>
+        <v>-58.441563</v>
       </c>
       <c r="N31" t="n">
-        <v>-34.579621</v>
+        <v>-34.569743</v>
       </c>
       <c r="O31" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P31" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>232</t>
+          <t>5826</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>5/9/2025</t>
+          <t>5/19/2025</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Gorostiaga 2286</t>
+          <t>ALBARELLOS AV. 3180</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>805791858</t>
+          <t>806926466</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
@@ -2817,7 +2817,7 @@
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Columna (metal) inclinada</t>
         </is>
       </c>
       <c r="I32" t="n">
@@ -2825,7 +2825,7 @@
       </c>
       <c r="J32" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K32" t="inlineStr">
@@ -2835,30 +2835,30 @@
       </c>
       <c r="L32" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M32" t="n">
-        <v>-58.441563</v>
+        <v>-58.513552</v>
       </c>
       <c r="N32" t="n">
-        <v>-34.569743</v>
+        <v>-34.579829</v>
       </c>
       <c r="O32" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P32" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>5826</t>
+          <t>5825</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -2868,7 +2868,7 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>ALBARELLOS AV. 3180</t>
+          <t>PAZ, GRAL. AV. 5602</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
@@ -2878,7 +2878,7 @@
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>806926466</t>
+          <t>806926472</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
@@ -2893,7 +2893,7 @@
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>Columna (metal) inclinada</t>
+          <t>reparar rienda cortada - ver foto no es la misma que albarellos</t>
         </is>
       </c>
       <c r="I33" t="n">
@@ -2901,7 +2901,7 @@
       </c>
       <c r="J33" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Tensor</t>
         </is>
       </c>
       <c r="K33" t="inlineStr">
@@ -2915,10 +2915,10 @@
         </is>
       </c>
       <c r="M33" t="n">
-        <v>-58.513552</v>
+        <v>-58.513685</v>
       </c>
       <c r="N33" t="n">
-        <v>-34.579829</v>
+        <v>-34.579838</v>
       </c>
       <c r="O33" t="inlineStr">
         <is>
@@ -2934,17 +2934,17 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>5825</t>
+          <t>5875</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>5/19/2025</t>
+          <t>5/27/2025</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>PAZ, GRAL. AV. 5602</t>
+          <t>MONROE 4096</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
@@ -2954,7 +2954,7 @@
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>806926472</t>
+          <t>806975680</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
@@ -2969,7 +2969,7 @@
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>reparar rienda cortada - ver foto no es la misma que albarellos</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I34" t="n">
@@ -2977,7 +2977,7 @@
       </c>
       <c r="J34" t="inlineStr">
         <is>
-          <t>Tensor</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K34" t="inlineStr">
@@ -2987,18 +2987,18 @@
       </c>
       <c r="L34" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M34" t="n">
-        <v>-58.513685</v>
+        <v>-58.476106</v>
       </c>
       <c r="N34" t="n">
-        <v>-34.579838</v>
+        <v>-34.568373</v>
       </c>
       <c r="O34" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P34" t="inlineStr">
@@ -3010,27 +3010,27 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>5875</t>
+          <t>807044192</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>5/27/2025</t>
+          <t>5/29/2025</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>MONROE 4096</t>
+          <t>O'Higgins 4379</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>806975680</t>
+          <t>807044192</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
@@ -3045,7 +3045,7 @@
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t xml:space="preserve">Poste </t>
         </is>
       </c>
       <c r="I35" t="n">
@@ -3053,7 +3053,7 @@
       </c>
       <c r="J35" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Desmonte</t>
         </is>
       </c>
       <c r="K35" t="inlineStr">
@@ -3063,18 +3063,18 @@
       </c>
       <c r="L35" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M35" t="n">
-        <v>-58.476106</v>
+        <v>-58.468425</v>
       </c>
       <c r="N35" t="n">
-        <v>-34.568373</v>
+        <v>-34.54124</v>
       </c>
       <c r="O35" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P35" t="inlineStr">
@@ -3086,27 +3086,27 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>807044192</t>
+          <t>6020</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>5/29/2025</t>
+          <t>6/5/2025</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>O'Higgins 4379</t>
+          <t>RAVIGNANI, EMILIO, DR. 2036</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>807044192</t>
+          <t>807215465</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
@@ -3121,7 +3121,7 @@
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t xml:space="preserve">Poste </t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I36" t="n">
@@ -3129,7 +3129,7 @@
       </c>
       <c r="J36" t="inlineStr">
         <is>
-          <t>Desmonte</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K36" t="inlineStr">
@@ -3139,50 +3139,50 @@
       </c>
       <c r="L36" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M36" t="n">
-        <v>-58.468425</v>
+        <v>-58.436298</v>
       </c>
       <c r="N36" t="n">
-        <v>-34.54124</v>
+        <v>-34.578972</v>
       </c>
       <c r="O36" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P36" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>6020</t>
+          <t>6144</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>6/5/2025</t>
+          <t>6/11/2025</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>RAVIGNANI, EMILIO, DR. 2036</t>
+          <t>TURIN 2990</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>807215465</t>
+          <t>807458282</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
@@ -3219,26 +3219,26 @@
         </is>
       </c>
       <c r="M37" t="n">
-        <v>-58.436298</v>
+        <v>-58.480925</v>
       </c>
       <c r="N37" t="n">
-        <v>-34.578972</v>
+        <v>-34.585471</v>
       </c>
       <c r="O37" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P37" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>6144</t>
+          <t>6143</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
@@ -3248,7 +3248,7 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>TURIN 2990</t>
+          <t>SOLANO LOPEZ, F., MARISCAL 2845</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
@@ -3258,7 +3258,7 @@
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>807458282</t>
+          <t>807458296</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
@@ -3295,10 +3295,10 @@
         </is>
       </c>
       <c r="M38" t="n">
-        <v>-58.480925</v>
+        <v>-58.495071</v>
       </c>
       <c r="N38" t="n">
-        <v>-34.585471</v>
+        <v>-34.593122</v>
       </c>
       <c r="O38" t="inlineStr">
         <is>
@@ -3314,7 +3314,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>6143</t>
+          <t>6141</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
@@ -3324,17 +3324,17 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>SOLANO LOPEZ, F., MARISCAL 2845</t>
+          <t>EL PAMPERO 2618</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>807458296</t>
+          <t>807458310</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
@@ -3371,10 +3371,10 @@
         </is>
       </c>
       <c r="M39" t="n">
-        <v>-58.495071</v>
+        <v>-58.481942</v>
       </c>
       <c r="N39" t="n">
-        <v>-34.593122</v>
+        <v>-34.602989</v>
       </c>
       <c r="O39" t="inlineStr">
         <is>
@@ -3390,17 +3390,17 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>6141</t>
+          <t>-478</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>6/11/2025</t>
+          <t>6/15/2025</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>EL PAMPERO 2618</t>
+          <t>Chivilcoy 4875</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
@@ -3410,7 +3410,7 @@
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>807458310</t>
+          <t>807508509</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
@@ -3425,7 +3425,7 @@
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Poste podrido</t>
         </is>
       </c>
       <c r="I40" t="n">
@@ -3443,14 +3443,14 @@
       </c>
       <c r="L40" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M40" t="n">
-        <v>-58.481942</v>
+        <v>-58.517389</v>
       </c>
       <c r="N40" t="n">
-        <v>-34.602989</v>
+        <v>-34.593541</v>
       </c>
       <c r="O40" t="inlineStr">
         <is>
@@ -3466,27 +3466,27 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>-478</t>
+          <t>6171</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>6/15/2025</t>
+          <t>6/18/2025</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Chivilcoy 4875</t>
+          <t>CABELLO 3486</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>807508509</t>
+          <t>807658640</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
@@ -3501,7 +3501,7 @@
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>Poste podrido</t>
+          <t>Columna inclinada evaluar con inspector un corrimiento</t>
         </is>
       </c>
       <c r="I41" t="n">
@@ -3519,40 +3519,40 @@
       </c>
       <c r="L41" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M41" t="n">
-        <v>-58.517389</v>
+        <v>-58.409579</v>
       </c>
       <c r="N41" t="n">
-        <v>-34.593541</v>
+        <v>-34.581134</v>
       </c>
       <c r="O41" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P41" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>6171</t>
+          <t>6230</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>6/18/2025</t>
+          <t>6/24/2025</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>CABELLO 3486</t>
+          <t>Santa maria de oro	2722</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
@@ -3562,7 +3562,7 @@
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>807658640</t>
+          <t>807763066</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
@@ -3577,7 +3577,7 @@
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>Columna inclinada evaluar con inspector un corrimiento</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I42" t="n">
@@ -3599,10 +3599,10 @@
         </is>
       </c>
       <c r="M42" t="n">
-        <v>-58.409579</v>
+        <v>-58.422315</v>
       </c>
       <c r="N42" t="n">
-        <v>-34.581134</v>
+        <v>-34.576988</v>
       </c>
       <c r="O42" t="inlineStr">
         <is>
@@ -3618,7 +3618,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>6230</t>
+          <t>6231</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
@@ -3628,7 +3628,7 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Santa maria de oro	2722</t>
+          <t>Ciudad de la Paz 275</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
@@ -3638,7 +3638,7 @@
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>807763066</t>
+          <t>807763070</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
@@ -3653,7 +3653,7 @@
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Aplomar o cambiar</t>
         </is>
       </c>
       <c r="I43" t="n">
@@ -3671,14 +3671,14 @@
       </c>
       <c r="L43" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M43" t="n">
-        <v>-58.422315</v>
+        <v>-58.441049</v>
       </c>
       <c r="N43" t="n">
-        <v>-34.576988</v>
+        <v>-34.574625</v>
       </c>
       <c r="O43" t="inlineStr">
         <is>
@@ -3694,7 +3694,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>6231</t>
+          <t>6235</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
@@ -3704,17 +3704,17 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Ciudad de la Paz 275</t>
+          <t>HUERGO 389</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>807763070</t>
+          <t>807763078</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
@@ -3729,7 +3729,7 @@
       </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t>Aplomar o cambiar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I44" t="n">
@@ -3747,14 +3747,14 @@
       </c>
       <c r="L44" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M44" t="n">
-        <v>-58.441049</v>
+        <v>-58.432722</v>
       </c>
       <c r="N44" t="n">
-        <v>-34.574625</v>
+        <v>-34.572371</v>
       </c>
       <c r="O44" t="inlineStr">
         <is>
@@ -3770,27 +3770,27 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>6235</t>
+          <t>6295</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>6/24/2025</t>
+          <t>6/30/2025</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>HUERGO 389</t>
+          <t>SOLER 6017</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>807763078</t>
+          <t>807851636</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
@@ -3827,10 +3827,10 @@
         </is>
       </c>
       <c r="M45" t="n">
-        <v>-58.432722</v>
+        <v>-58.436808</v>
       </c>
       <c r="N45" t="n">
-        <v>-34.572371</v>
+        <v>-34.577464</v>
       </c>
       <c r="O45" t="inlineStr">
         <is>
@@ -3846,17 +3846,17 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>6295</t>
+          <t>6331</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>6/30/2025</t>
+          <t>7/3/2025</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>SOLER 6017</t>
+          <t>PARAGUAY 4259</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
@@ -3866,7 +3866,7 @@
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>807851636</t>
+          <t>807965788</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
@@ -3903,10 +3903,10 @@
         </is>
       </c>
       <c r="M46" t="n">
-        <v>-58.436808</v>
+        <v>-58.421822</v>
       </c>
       <c r="N46" t="n">
-        <v>-34.577464</v>
+        <v>-34.58645</v>
       </c>
       <c r="O46" t="inlineStr">
         <is>
@@ -3922,7 +3922,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>6331</t>
+          <t>6332</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
@@ -3932,7 +3932,7 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>PARAGUAY 4259</t>
+          <t>ARAOZ 2560</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
@@ -3942,7 +3942,7 @@
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>807965788</t>
+          <t>807965818</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
@@ -3979,10 +3979,10 @@
         </is>
       </c>
       <c r="M47" t="n">
-        <v>-58.421822</v>
+        <v>-58.414507</v>
       </c>
       <c r="N47" t="n">
-        <v>-34.58645</v>
+        <v>-34.585377</v>
       </c>
       <c r="O47" t="inlineStr">
         <is>
@@ -3998,7 +3998,7 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>6332</t>
+          <t>6336</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
@@ -4008,7 +4008,7 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>ARAOZ 2560</t>
+          <t>PARAGUAY 4291</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
@@ -4018,7 +4018,7 @@
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>807965818</t>
+          <t>807965819</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
@@ -4055,10 +4055,10 @@
         </is>
       </c>
       <c r="M48" t="n">
-        <v>-58.414507</v>
+        <v>-58.422084</v>
       </c>
       <c r="N48" t="n">
-        <v>-34.585377</v>
+        <v>-34.58625</v>
       </c>
       <c r="O48" t="inlineStr">
         <is>
@@ -4074,7 +4074,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>6336</t>
+          <t>6337</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
@@ -4084,7 +4084,7 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>PARAGUAY 4291</t>
+          <t>PARAGUAY 4383</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
@@ -4094,7 +4094,7 @@
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>807965819</t>
+          <t>807965926</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
@@ -4131,10 +4131,10 @@
         </is>
       </c>
       <c r="M49" t="n">
-        <v>-58.422084</v>
+        <v>-58.422931</v>
       </c>
       <c r="N49" t="n">
-        <v>-34.58625</v>
+        <v>-34.585597</v>
       </c>
       <c r="O49" t="inlineStr">
         <is>
@@ -4150,27 +4150,27 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>6337</t>
+          <t>6363</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>7/3/2025</t>
+          <t>7/8/2025</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>PARAGUAY 4383</t>
+          <t>MOLDES 3730</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>807965926</t>
+          <t>808099415</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
@@ -4185,7 +4185,7 @@
       </c>
       <c r="H50" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Poste inclinado</t>
         </is>
       </c>
       <c r="I50" t="n">
@@ -4193,7 +4193,7 @@
       </c>
       <c r="J50" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K50" t="inlineStr">
@@ -4203,50 +4203,50 @@
       </c>
       <c r="L50" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M50" t="n">
-        <v>-58.422931</v>
+        <v>-58.47192</v>
       </c>
       <c r="N50" t="n">
-        <v>-34.585597</v>
+        <v>-34.549398</v>
       </c>
       <c r="O50" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P50" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>6363</t>
+          <t>-503</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>7/8/2025</t>
+          <t>7/10/2025</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>MOLDES 3730</t>
+          <t>Salguero 842</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>808099415</t>
+          <t>808148673</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
@@ -4261,7 +4261,7 @@
       </c>
       <c r="H51" t="inlineStr">
         <is>
-          <t>Poste inclinado</t>
+          <t>Cambiar columna picada en la base</t>
         </is>
       </c>
       <c r="I51" t="n">
@@ -4269,7 +4269,7 @@
       </c>
       <c r="J51" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K51" t="inlineStr">
@@ -4279,30 +4279,30 @@
       </c>
       <c r="L51" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M51" t="n">
-        <v>-58.47192</v>
+        <v>-58.419166</v>
       </c>
       <c r="N51" t="n">
-        <v>-34.549398</v>
+        <v>-34.600265</v>
       </c>
       <c r="O51" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P51" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>-503</t>
+          <t>-504</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
@@ -4312,17 +4312,17 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>Salguero 842</t>
+          <t>Ohiggins 1611</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>808148673</t>
+          <t>808148679</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
@@ -4337,7 +4337,7 @@
       </c>
       <c r="H52" t="inlineStr">
         <is>
-          <t>Cambiar columna picada en la base</t>
+          <t>Columna podrida en la base</t>
         </is>
       </c>
       <c r="I52" t="n">
@@ -4350,7 +4350,7 @@
       </c>
       <c r="K52" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L52" t="inlineStr">
@@ -4359,36 +4359,36 @@
         </is>
       </c>
       <c r="M52" t="n">
-        <v>-58.419166</v>
+        <v>-58.448993</v>
       </c>
       <c r="N52" t="n">
-        <v>-34.600265</v>
+        <v>-34.564383</v>
       </c>
       <c r="O52" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P52" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>-504</t>
+          <t>6392</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>7/10/2025</t>
+          <t>7/14/2025</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>Ohiggins 1611</t>
+          <t>MOLDES 1808</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
@@ -4398,7 +4398,7 @@
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>808148679</t>
+          <t>808194266</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
@@ -4413,7 +4413,7 @@
       </c>
       <c r="H53" t="inlineStr">
         <is>
-          <t>Columna podrida en la base</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I53" t="n">
@@ -4426,7 +4426,7 @@
       </c>
       <c r="K53" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L53" t="inlineStr">
@@ -4435,10 +4435,10 @@
         </is>
       </c>
       <c r="M53" t="n">
-        <v>-58.448993</v>
+        <v>-58.45719</v>
       </c>
       <c r="N53" t="n">
-        <v>-34.564383</v>
+        <v>-34.566365</v>
       </c>
       <c r="O53" t="inlineStr">
         <is>
@@ -4454,27 +4454,27 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>6392</t>
+          <t>6437</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>7/14/2025</t>
+          <t>7/17/2025</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>MOLDES 1808</t>
+          <t>MILLER 4590</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>808194266</t>
+          <t>808400306</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
@@ -4489,7 +4489,7 @@
       </c>
       <c r="H54" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Columna corroida</t>
         </is>
       </c>
       <c r="I54" t="n">
@@ -4511,14 +4511,14 @@
         </is>
       </c>
       <c r="M54" t="n">
-        <v>-58.45719</v>
+        <v>-58.495482</v>
       </c>
       <c r="N54" t="n">
-        <v>-34.566365</v>
+        <v>-34.552614</v>
       </c>
       <c r="O54" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P54" t="inlineStr">
@@ -4530,7 +4530,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>6437</t>
+          <t>6447</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
@@ -4540,17 +4540,17 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>MILLER 4590</t>
+          <t>CIUDAD DE LA PAZ 1535</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>808400306</t>
+          <t>808400333</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
@@ -4565,7 +4565,7 @@
       </c>
       <c r="H55" t="inlineStr">
         <is>
-          <t>Columna corroida</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I55" t="n">
@@ -4587,14 +4587,14 @@
         </is>
       </c>
       <c r="M55" t="n">
-        <v>-58.495482</v>
+        <v>-58.453124</v>
       </c>
       <c r="N55" t="n">
-        <v>-34.552614</v>
+        <v>-34.567382</v>
       </c>
       <c r="O55" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P55" t="inlineStr">
@@ -4606,7 +4606,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>6447</t>
+          <t>-519</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
@@ -4616,17 +4616,17 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>CIUDAD DE LA PAZ 1535</t>
+          <t>Vilela 2687</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>808400333</t>
+          <t>808400334</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
@@ -4641,7 +4641,7 @@
       </c>
       <c r="H56" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>CAmbiar columna 114 picada en base</t>
         </is>
       </c>
       <c r="I56" t="n">
@@ -4663,14 +4663,14 @@
         </is>
       </c>
       <c r="M56" t="n">
-        <v>-58.453124</v>
+        <v>-58.472968</v>
       </c>
       <c r="N56" t="n">
-        <v>-34.567382</v>
+        <v>-34.546898</v>
       </c>
       <c r="O56" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P56" t="inlineStr">
@@ -4682,7 +4682,7 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>-519</t>
+          <t>-520</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
@@ -4692,7 +4692,7 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>Vilela 2687</t>
+          <t>Pedraza Manuela 4101</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
@@ -4702,7 +4702,7 @@
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>808400334</t>
+          <t>808400353</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
@@ -4717,7 +4717,7 @@
       </c>
       <c r="H57" t="inlineStr">
         <is>
-          <t>CAmbiar columna 114 picada en base</t>
+          <t xml:space="preserve">Podrida en la base </t>
         </is>
       </c>
       <c r="I57" t="n">
@@ -4739,10 +4739,10 @@
         </is>
       </c>
       <c r="M57" t="n">
-        <v>-58.472968</v>
+        <v>-58.481569</v>
       </c>
       <c r="N57" t="n">
-        <v>-34.546898</v>
+        <v>-34.559853</v>
       </c>
       <c r="O57" t="inlineStr">
         <is>
@@ -4750,82 +4750,6 @@
         </is>
       </c>
       <c r="P57" t="inlineStr">
-        <is>
-          <t>Capital Norte</t>
-        </is>
-      </c>
-    </row>
-    <row r="58">
-      <c r="A58" t="inlineStr">
-        <is>
-          <t>-520</t>
-        </is>
-      </c>
-      <c r="B58" t="inlineStr">
-        <is>
-          <t>7/17/2025</t>
-        </is>
-      </c>
-      <c r="C58" t="inlineStr">
-        <is>
-          <t>Pedraza Manuela 4101</t>
-        </is>
-      </c>
-      <c r="D58" t="inlineStr">
-        <is>
-          <t>12</t>
-        </is>
-      </c>
-      <c r="E58" t="inlineStr">
-        <is>
-          <t>808400353</t>
-        </is>
-      </c>
-      <c r="F58" t="inlineStr">
-        <is>
-          <t>NEW</t>
-        </is>
-      </c>
-      <c r="G58" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H58" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Podrida en la base </t>
-        </is>
-      </c>
-      <c r="I58" t="n">
-        <v>1</v>
-      </c>
-      <c r="J58" t="inlineStr">
-        <is>
-          <t>Cambio</t>
-        </is>
-      </c>
-      <c r="K58" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L58" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
-      <c r="M58" t="n">
-        <v>-58.481569</v>
-      </c>
-      <c r="N58" t="n">
-        <v>-34.559853</v>
-      </c>
-      <c r="O58" t="inlineStr">
-        <is>
-          <t>Saavedra</t>
-        </is>
-      </c>
-      <c r="P58" t="inlineStr">
         <is>
           <t>Capital Norte</t>
         </is>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-07-23 07:17:22)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_NEW.xlsx
+++ b/mapa_interactivo_NEW.xlsx
@@ -1870,7 +1870,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>5601</t>
+          <t>5590</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -1880,17 +1880,17 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>JURAMENTO 3964</t>
+          <t>O'HIGGINS 2441</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>804732274</t>
+          <t>804732275</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
@@ -1927,14 +1927,14 @@
         </is>
       </c>
       <c r="M20" t="n">
-        <v>-58.471885</v>
+        <v>-58.45573</v>
       </c>
       <c r="N20" t="n">
-        <v>-34.571063</v>
+        <v>-34.556576</v>
       </c>
       <c r="O20" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P20" t="inlineStr">
@@ -1946,17 +1946,17 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>5590</t>
+          <t>5624</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>4/15/2025</t>
+          <t>4/22/2025</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>O'HIGGINS 2441</t>
+          <t>PINO, VIRREY DEL 3456</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
@@ -1966,7 +1966,7 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>804732275</t>
+          <t>804876043</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
@@ -1981,7 +1981,7 @@
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Desmonte de poste</t>
         </is>
       </c>
       <c r="I21" t="n">
@@ -1989,7 +1989,7 @@
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Desmonte</t>
         </is>
       </c>
       <c r="K21" t="inlineStr">
@@ -1999,18 +1999,18 @@
       </c>
       <c r="L21" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M21" t="n">
-        <v>-58.45573</v>
+        <v>-58.464354</v>
       </c>
       <c r="N21" t="n">
-        <v>-34.556576</v>
+        <v>-34.572486</v>
       </c>
       <c r="O21" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P21" t="inlineStr">
@@ -2022,27 +2022,27 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>5721</t>
+          <t>804922177</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>4/14/2025</t>
+          <t>4/24/2025</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>AVALOS 1935</t>
+          <t>Moldes 1717</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>804839238</t>
+          <t>804922177</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
@@ -2057,15 +2057,15 @@
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>Aplomo de columna  - VIRARDI</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I22" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J22" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K22" t="inlineStr">
@@ -2079,14 +2079,14 @@
         </is>
       </c>
       <c r="M22" t="n">
-        <v>-58.482268</v>
+        <v>-58.45643</v>
       </c>
       <c r="N22" t="n">
-        <v>-34.578975</v>
+        <v>-34.567121</v>
       </c>
       <c r="O22" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P22" t="inlineStr">
@@ -2098,27 +2098,27 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>5624</t>
+          <t>5656</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>4/22/2025</t>
+          <t>4/24/2025</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>PINO, VIRREY DEL 3456</t>
+          <t>ECHEVERRIA 5893</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>804876043</t>
+          <t>804922184</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
@@ -2133,7 +2133,7 @@
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>Desmonte de poste</t>
+          <t>Poste con base quebrada</t>
         </is>
       </c>
       <c r="I23" t="n">
@@ -2155,14 +2155,14 @@
         </is>
       </c>
       <c r="M23" t="n">
-        <v>-58.464354</v>
+        <v>-58.489627</v>
       </c>
       <c r="N23" t="n">
-        <v>-34.572486</v>
+        <v>-34.583761</v>
       </c>
       <c r="O23" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P23" t="inlineStr">
@@ -2174,27 +2174,27 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>5656</t>
+          <t>6173</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>4/24/2025</t>
+          <t>4/29/2025</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>ECHEVERRIA 5893</t>
+          <t>ARMENIA 2321</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>804922184</t>
+          <t>805507398</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
@@ -2209,7 +2209,7 @@
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>Poste con base quebrada</t>
+          <t>Picada volvio a entrar como caso 6325</t>
         </is>
       </c>
       <c r="I24" t="n">
@@ -2217,7 +2217,7 @@
       </c>
       <c r="J24" t="inlineStr">
         <is>
-          <t>Desmonte</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K24" t="inlineStr">
@@ -2227,50 +2227,50 @@
       </c>
       <c r="L24" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M24" t="n">
-        <v>-58.489627</v>
+        <v>-58.420549</v>
       </c>
       <c r="N24" t="n">
-        <v>-34.583761</v>
+        <v>-34.585103</v>
       </c>
       <c r="O24" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P24" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>6173</t>
+          <t>5715</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>4/29/2025</t>
+          <t>5/1/2025</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>ARMENIA 2321</t>
+          <t>CUENCA 4690</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>805507398</t>
+          <t>805579094</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
@@ -2285,7 +2285,7 @@
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>Picada volvio a entrar como caso 6325</t>
+          <t>Aplomar poste</t>
         </is>
       </c>
       <c r="I25" t="n">
@@ -2293,7 +2293,7 @@
       </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K25" t="inlineStr">
@@ -2303,30 +2303,30 @@
       </c>
       <c r="L25" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M25" t="n">
-        <v>-58.420549</v>
+        <v>-58.506061</v>
       </c>
       <c r="N25" t="n">
-        <v>-34.585103</v>
+        <v>-34.588887</v>
       </c>
       <c r="O25" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P25" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>5715</t>
+          <t>5719</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -2336,7 +2336,7 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>CUENCA 4690</t>
+          <t>CABEZON, JOSE LEON 2440</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
@@ -2346,7 +2346,7 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>805579094</t>
+          <t>805579157</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
@@ -2361,7 +2361,7 @@
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>Aplomar poste</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I26" t="n">
@@ -2369,7 +2369,7 @@
       </c>
       <c r="J26" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K26" t="inlineStr">
@@ -2379,14 +2379,14 @@
       </c>
       <c r="L26" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M26" t="n">
-        <v>-58.506061</v>
+        <v>-58.499967</v>
       </c>
       <c r="N26" t="n">
-        <v>-34.588887</v>
+        <v>-34.57974</v>
       </c>
       <c r="O26" t="inlineStr">
         <is>
@@ -2402,7 +2402,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>5719</t>
+          <t>6333</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -2412,17 +2412,17 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>CABEZON, JOSE LEON 2440</t>
+          <t>ORTEGA Y GASSET 1816</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>805579157</t>
+          <t>805655342</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
@@ -2459,46 +2459,46 @@
         </is>
       </c>
       <c r="M27" t="n">
-        <v>-58.499967</v>
+        <v>-58.432556</v>
       </c>
       <c r="N27" t="n">
-        <v>-34.57974</v>
+        <v>-34.570279</v>
       </c>
       <c r="O27" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P27" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>5720</t>
+          <t>805707165</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>5/1/2025</t>
+          <t>5/7/2025</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>CABEZON, JOSE LEON 2398</t>
+          <t>Baez 793</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>805579172</t>
+          <t>805707165</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
@@ -2513,7 +2513,7 @@
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>DESMONTAR COLUMNA DE 7 MTS Y TRANSFERIR A COMUNITARIA</t>
         </is>
       </c>
       <c r="I28" t="n">
@@ -2531,50 +2531,50 @@
       </c>
       <c r="L28" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M28" t="n">
-        <v>-58.499355</v>
+        <v>-58.436165</v>
       </c>
       <c r="N28" t="n">
-        <v>-34.579354</v>
+        <v>-34.569081</v>
       </c>
       <c r="O28" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P28" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>6333</t>
+          <t>5847</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>5/1/2025</t>
+          <t>5/8/2025</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>ORTEGA Y GASSET 1816</t>
+          <t>JURAMENTO 5321</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>805655342</t>
+          <t>805791839</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
@@ -2611,46 +2611,46 @@
         </is>
       </c>
       <c r="M29" t="n">
-        <v>-58.432556</v>
+        <v>-58.485193</v>
       </c>
       <c r="N29" t="n">
-        <v>-34.570279</v>
+        <v>-34.579621</v>
       </c>
       <c r="O29" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P29" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>5847</t>
+          <t>232</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>5/8/2025</t>
+          <t>5/9/2025</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>JURAMENTO 5321</t>
+          <t>Gorostiaga 2286</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>805791839</t>
+          <t>805791858</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
@@ -2687,46 +2687,46 @@
         </is>
       </c>
       <c r="M30" t="n">
-        <v>-58.485193</v>
+        <v>-58.441563</v>
       </c>
       <c r="N30" t="n">
-        <v>-34.579621</v>
+        <v>-34.569743</v>
       </c>
       <c r="O30" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P30" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>232</t>
+          <t>5826</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>5/9/2025</t>
+          <t>5/19/2025</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Gorostiaga 2286</t>
+          <t>ALBARELLOS AV. 3180</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>805791858</t>
+          <t>806926466</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
@@ -2741,7 +2741,7 @@
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Columna (metal) inclinada</t>
         </is>
       </c>
       <c r="I31" t="n">
@@ -2749,7 +2749,7 @@
       </c>
       <c r="J31" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K31" t="inlineStr">
@@ -2759,30 +2759,30 @@
       </c>
       <c r="L31" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M31" t="n">
-        <v>-58.441563</v>
+        <v>-58.513552</v>
       </c>
       <c r="N31" t="n">
-        <v>-34.569743</v>
+        <v>-34.579829</v>
       </c>
       <c r="O31" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P31" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>5826</t>
+          <t>5825</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
@@ -2792,7 +2792,7 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>ALBARELLOS AV. 3180</t>
+          <t>PAZ, GRAL. AV. 5602</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
@@ -2802,7 +2802,7 @@
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>806926466</t>
+          <t>806926472</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
@@ -2817,7 +2817,7 @@
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>Columna (metal) inclinada</t>
+          <t>reparar rienda cortada - ver foto no es la misma que albarellos</t>
         </is>
       </c>
       <c r="I32" t="n">
@@ -2825,7 +2825,7 @@
       </c>
       <c r="J32" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Tensor</t>
         </is>
       </c>
       <c r="K32" t="inlineStr">
@@ -2839,10 +2839,10 @@
         </is>
       </c>
       <c r="M32" t="n">
-        <v>-58.513552</v>
+        <v>-58.513685</v>
       </c>
       <c r="N32" t="n">
-        <v>-34.579829</v>
+        <v>-34.579838</v>
       </c>
       <c r="O32" t="inlineStr">
         <is>
@@ -2858,17 +2858,17 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>5825</t>
+          <t>5875</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>5/19/2025</t>
+          <t>5/27/2025</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>PAZ, GRAL. AV. 5602</t>
+          <t>MONROE 4096</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
@@ -2878,7 +2878,7 @@
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>806926472</t>
+          <t>806975680</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
@@ -2893,7 +2893,7 @@
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>reparar rienda cortada - ver foto no es la misma que albarellos</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I33" t="n">
@@ -2901,7 +2901,7 @@
       </c>
       <c r="J33" t="inlineStr">
         <is>
-          <t>Tensor</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K33" t="inlineStr">
@@ -2911,18 +2911,18 @@
       </c>
       <c r="L33" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M33" t="n">
-        <v>-58.513685</v>
+        <v>-58.476106</v>
       </c>
       <c r="N33" t="n">
-        <v>-34.579838</v>
+        <v>-34.568373</v>
       </c>
       <c r="O33" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P33" t="inlineStr">
@@ -2934,27 +2934,27 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>5875</t>
+          <t>807044192</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>5/27/2025</t>
+          <t>5/29/2025</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>MONROE 4096</t>
+          <t>O'Higgins 4379</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>806975680</t>
+          <t>807044192</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
@@ -2969,7 +2969,7 @@
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t xml:space="preserve">Poste </t>
         </is>
       </c>
       <c r="I34" t="n">
@@ -2977,7 +2977,7 @@
       </c>
       <c r="J34" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Desmonte</t>
         </is>
       </c>
       <c r="K34" t="inlineStr">
@@ -2987,18 +2987,18 @@
       </c>
       <c r="L34" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M34" t="n">
-        <v>-58.476106</v>
+        <v>-58.468425</v>
       </c>
       <c r="N34" t="n">
-        <v>-34.568373</v>
+        <v>-34.54124</v>
       </c>
       <c r="O34" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P34" t="inlineStr">
@@ -3010,27 +3010,27 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>807044192</t>
+          <t>6020</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>5/29/2025</t>
+          <t>6/5/2025</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>O'Higgins 4379</t>
+          <t>RAVIGNANI, EMILIO, DR. 2036</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>807044192</t>
+          <t>807215465</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
@@ -3045,7 +3045,7 @@
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t xml:space="preserve">Poste </t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I35" t="n">
@@ -3053,7 +3053,7 @@
       </c>
       <c r="J35" t="inlineStr">
         <is>
-          <t>Desmonte</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K35" t="inlineStr">
@@ -3063,50 +3063,50 @@
       </c>
       <c r="L35" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M35" t="n">
-        <v>-58.468425</v>
+        <v>-58.436298</v>
       </c>
       <c r="N35" t="n">
-        <v>-34.54124</v>
+        <v>-34.578972</v>
       </c>
       <c r="O35" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P35" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>6020</t>
+          <t>6144</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>6/5/2025</t>
+          <t>6/11/2025</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>RAVIGNANI, EMILIO, DR. 2036</t>
+          <t>TURIN 2990</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>807215465</t>
+          <t>807458282</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
@@ -3143,26 +3143,26 @@
         </is>
       </c>
       <c r="M36" t="n">
-        <v>-58.436298</v>
+        <v>-58.480925</v>
       </c>
       <c r="N36" t="n">
-        <v>-34.578972</v>
+        <v>-34.585471</v>
       </c>
       <c r="O36" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P36" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>6144</t>
+          <t>6143</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
@@ -3172,7 +3172,7 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>TURIN 2990</t>
+          <t>SOLANO LOPEZ, F., MARISCAL 2845</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
@@ -3182,7 +3182,7 @@
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>807458282</t>
+          <t>807458296</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
@@ -3219,10 +3219,10 @@
         </is>
       </c>
       <c r="M37" t="n">
-        <v>-58.480925</v>
+        <v>-58.495071</v>
       </c>
       <c r="N37" t="n">
-        <v>-34.585471</v>
+        <v>-34.593122</v>
       </c>
       <c r="O37" t="inlineStr">
         <is>
@@ -3238,7 +3238,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>6143</t>
+          <t>6141</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
@@ -3248,17 +3248,17 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>SOLANO LOPEZ, F., MARISCAL 2845</t>
+          <t>EL PAMPERO 2618</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>807458296</t>
+          <t>807458310</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
@@ -3295,10 +3295,10 @@
         </is>
       </c>
       <c r="M38" t="n">
-        <v>-58.495071</v>
+        <v>-58.481942</v>
       </c>
       <c r="N38" t="n">
-        <v>-34.593122</v>
+        <v>-34.602989</v>
       </c>
       <c r="O38" t="inlineStr">
         <is>
@@ -3314,17 +3314,17 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>6141</t>
+          <t>-478</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>6/11/2025</t>
+          <t>6/15/2025</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>EL PAMPERO 2618</t>
+          <t>Chivilcoy 4875</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
@@ -3334,7 +3334,7 @@
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>807458310</t>
+          <t>807508509</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
@@ -3349,7 +3349,7 @@
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Poste podrido</t>
         </is>
       </c>
       <c r="I39" t="n">
@@ -3367,14 +3367,14 @@
       </c>
       <c r="L39" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M39" t="n">
-        <v>-58.481942</v>
+        <v>-58.517389</v>
       </c>
       <c r="N39" t="n">
-        <v>-34.602989</v>
+        <v>-34.593541</v>
       </c>
       <c r="O39" t="inlineStr">
         <is>
@@ -3390,27 +3390,27 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>-478</t>
+          <t>6171</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>6/15/2025</t>
+          <t>6/18/2025</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Chivilcoy 4875</t>
+          <t>CABELLO 3486</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>807508509</t>
+          <t>807658640</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
@@ -3425,7 +3425,7 @@
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t>Poste podrido</t>
+          <t>Columna inclinada evaluar con inspector un corrimiento</t>
         </is>
       </c>
       <c r="I40" t="n">
@@ -3443,40 +3443,40 @@
       </c>
       <c r="L40" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M40" t="n">
-        <v>-58.517389</v>
+        <v>-58.409579</v>
       </c>
       <c r="N40" t="n">
-        <v>-34.593541</v>
+        <v>-34.581134</v>
       </c>
       <c r="O40" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P40" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>6171</t>
+          <t>6230</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>6/18/2025</t>
+          <t>6/24/2025</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>CABELLO 3486</t>
+          <t>Santa maria de oro	2722</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
@@ -3486,7 +3486,7 @@
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>807658640</t>
+          <t>807763066</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
@@ -3501,7 +3501,7 @@
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>Columna inclinada evaluar con inspector un corrimiento</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I41" t="n">
@@ -3523,10 +3523,10 @@
         </is>
       </c>
       <c r="M41" t="n">
-        <v>-58.409579</v>
+        <v>-58.422315</v>
       </c>
       <c r="N41" t="n">
-        <v>-34.581134</v>
+        <v>-34.576988</v>
       </c>
       <c r="O41" t="inlineStr">
         <is>
@@ -3542,7 +3542,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>6230</t>
+          <t>6231</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
@@ -3552,7 +3552,7 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Santa maria de oro	2722</t>
+          <t>Ciudad de la Paz 275</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
@@ -3562,7 +3562,7 @@
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>807763066</t>
+          <t>807763070</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
@@ -3577,7 +3577,7 @@
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Aplomar o cambiar</t>
         </is>
       </c>
       <c r="I42" t="n">
@@ -3595,14 +3595,14 @@
       </c>
       <c r="L42" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M42" t="n">
-        <v>-58.422315</v>
+        <v>-58.441049</v>
       </c>
       <c r="N42" t="n">
-        <v>-34.576988</v>
+        <v>-34.574625</v>
       </c>
       <c r="O42" t="inlineStr">
         <is>
@@ -3618,7 +3618,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>6231</t>
+          <t>6235</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
@@ -3628,17 +3628,17 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Ciudad de la Paz 275</t>
+          <t>HUERGO 389</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>807763070</t>
+          <t>807763078</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
@@ -3653,7 +3653,7 @@
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>Aplomar o cambiar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I43" t="n">
@@ -3671,14 +3671,14 @@
       </c>
       <c r="L43" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M43" t="n">
-        <v>-58.441049</v>
+        <v>-58.432722</v>
       </c>
       <c r="N43" t="n">
-        <v>-34.574625</v>
+        <v>-34.572371</v>
       </c>
       <c r="O43" t="inlineStr">
         <is>
@@ -3694,27 +3694,27 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>6235</t>
+          <t>6295</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>6/24/2025</t>
+          <t>6/30/2025</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>HUERGO 389</t>
+          <t>SOLER 6017</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>807763078</t>
+          <t>807851636</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
@@ -3751,10 +3751,10 @@
         </is>
       </c>
       <c r="M44" t="n">
-        <v>-58.432722</v>
+        <v>-58.436808</v>
       </c>
       <c r="N44" t="n">
-        <v>-34.572371</v>
+        <v>-34.577464</v>
       </c>
       <c r="O44" t="inlineStr">
         <is>
@@ -3770,17 +3770,17 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>6295</t>
+          <t>6331</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>6/30/2025</t>
+          <t>7/3/2025</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>SOLER 6017</t>
+          <t>PARAGUAY 4259</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
@@ -3790,7 +3790,7 @@
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>807851636</t>
+          <t>807965788</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
@@ -3827,10 +3827,10 @@
         </is>
       </c>
       <c r="M45" t="n">
-        <v>-58.436808</v>
+        <v>-58.421822</v>
       </c>
       <c r="N45" t="n">
-        <v>-34.577464</v>
+        <v>-34.58645</v>
       </c>
       <c r="O45" t="inlineStr">
         <is>
@@ -3846,7 +3846,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>6331</t>
+          <t>6332</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
@@ -3856,7 +3856,7 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>PARAGUAY 4259</t>
+          <t>ARAOZ 2560</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
@@ -3866,7 +3866,7 @@
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>807965788</t>
+          <t>807965818</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
@@ -3903,10 +3903,10 @@
         </is>
       </c>
       <c r="M46" t="n">
-        <v>-58.421822</v>
+        <v>-58.414507</v>
       </c>
       <c r="N46" t="n">
-        <v>-34.58645</v>
+        <v>-34.585377</v>
       </c>
       <c r="O46" t="inlineStr">
         <is>
@@ -3922,7 +3922,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>6332</t>
+          <t>6336</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
@@ -3932,7 +3932,7 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>ARAOZ 2560</t>
+          <t>PARAGUAY 4291</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
@@ -3942,7 +3942,7 @@
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>807965818</t>
+          <t>807965819</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
@@ -3979,10 +3979,10 @@
         </is>
       </c>
       <c r="M47" t="n">
-        <v>-58.414507</v>
+        <v>-58.422084</v>
       </c>
       <c r="N47" t="n">
-        <v>-34.585377</v>
+        <v>-34.58625</v>
       </c>
       <c r="O47" t="inlineStr">
         <is>
@@ -3998,7 +3998,7 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>6336</t>
+          <t>6337</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
@@ -4008,7 +4008,7 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>PARAGUAY 4291</t>
+          <t>PARAGUAY 4383</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
@@ -4018,7 +4018,7 @@
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>807965819</t>
+          <t>807965926</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
@@ -4055,10 +4055,10 @@
         </is>
       </c>
       <c r="M48" t="n">
-        <v>-58.422084</v>
+        <v>-58.422931</v>
       </c>
       <c r="N48" t="n">
-        <v>-34.58625</v>
+        <v>-34.585597</v>
       </c>
       <c r="O48" t="inlineStr">
         <is>
@@ -4074,27 +4074,27 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>6337</t>
+          <t>6363</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>7/3/2025</t>
+          <t>7/8/2025</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>PARAGUAY 4383</t>
+          <t>MOLDES 3730</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>807965926</t>
+          <t>808099415</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
@@ -4109,7 +4109,7 @@
       </c>
       <c r="H49" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Poste inclinado</t>
         </is>
       </c>
       <c r="I49" t="n">
@@ -4117,7 +4117,7 @@
       </c>
       <c r="J49" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K49" t="inlineStr">
@@ -4127,50 +4127,50 @@
       </c>
       <c r="L49" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M49" t="n">
-        <v>-58.422931</v>
+        <v>-58.47192</v>
       </c>
       <c r="N49" t="n">
-        <v>-34.585597</v>
+        <v>-34.549398</v>
       </c>
       <c r="O49" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P49" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>6363</t>
+          <t>-503</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>7/8/2025</t>
+          <t>7/10/2025</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>MOLDES 3730</t>
+          <t>Salguero 842</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>808099415</t>
+          <t>808148673</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
@@ -4185,7 +4185,7 @@
       </c>
       <c r="H50" t="inlineStr">
         <is>
-          <t>Poste inclinado</t>
+          <t>Cambiar columna picada en la base</t>
         </is>
       </c>
       <c r="I50" t="n">
@@ -4193,7 +4193,7 @@
       </c>
       <c r="J50" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K50" t="inlineStr">
@@ -4203,30 +4203,30 @@
       </c>
       <c r="L50" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M50" t="n">
-        <v>-58.47192</v>
+        <v>-58.419166</v>
       </c>
       <c r="N50" t="n">
-        <v>-34.549398</v>
+        <v>-34.600265</v>
       </c>
       <c r="O50" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P50" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>-503</t>
+          <t>-504</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
@@ -4236,17 +4236,17 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Salguero 842</t>
+          <t>Ohiggins 1611</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>808148673</t>
+          <t>808148679</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
@@ -4261,7 +4261,7 @@
       </c>
       <c r="H51" t="inlineStr">
         <is>
-          <t>Cambiar columna picada en la base</t>
+          <t>Columna podrida en la base</t>
         </is>
       </c>
       <c r="I51" t="n">
@@ -4274,7 +4274,7 @@
       </c>
       <c r="K51" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L51" t="inlineStr">
@@ -4283,36 +4283,36 @@
         </is>
       </c>
       <c r="M51" t="n">
-        <v>-58.419166</v>
+        <v>-58.448993</v>
       </c>
       <c r="N51" t="n">
-        <v>-34.600265</v>
+        <v>-34.564383</v>
       </c>
       <c r="O51" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P51" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>-504</t>
+          <t>6392</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>7/10/2025</t>
+          <t>7/14/2025</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>Ohiggins 1611</t>
+          <t>MOLDES 1808</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
@@ -4322,7 +4322,7 @@
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>808148679</t>
+          <t>808194266</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
@@ -4337,7 +4337,7 @@
       </c>
       <c r="H52" t="inlineStr">
         <is>
-          <t>Columna podrida en la base</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I52" t="n">
@@ -4350,7 +4350,7 @@
       </c>
       <c r="K52" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L52" t="inlineStr">
@@ -4359,10 +4359,10 @@
         </is>
       </c>
       <c r="M52" t="n">
-        <v>-58.448993</v>
+        <v>-58.45719</v>
       </c>
       <c r="N52" t="n">
-        <v>-34.564383</v>
+        <v>-34.566365</v>
       </c>
       <c r="O52" t="inlineStr">
         <is>
@@ -4378,27 +4378,27 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>6392</t>
+          <t>6437</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>7/14/2025</t>
+          <t>7/17/2025</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>MOLDES 1808</t>
+          <t>MILLER 4590</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>808194266</t>
+          <t>808400306</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
@@ -4413,7 +4413,7 @@
       </c>
       <c r="H53" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Columna corroida</t>
         </is>
       </c>
       <c r="I53" t="n">
@@ -4435,14 +4435,14 @@
         </is>
       </c>
       <c r="M53" t="n">
-        <v>-58.45719</v>
+        <v>-58.495482</v>
       </c>
       <c r="N53" t="n">
-        <v>-34.566365</v>
+        <v>-34.552614</v>
       </c>
       <c r="O53" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P53" t="inlineStr">
@@ -4454,7 +4454,7 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>6437</t>
+          <t>6447</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
@@ -4464,17 +4464,17 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>MILLER 4590</t>
+          <t>CIUDAD DE LA PAZ 1535</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>808400306</t>
+          <t>808400333</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
@@ -4489,7 +4489,7 @@
       </c>
       <c r="H54" t="inlineStr">
         <is>
-          <t>Columna corroida</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I54" t="n">
@@ -4511,14 +4511,14 @@
         </is>
       </c>
       <c r="M54" t="n">
-        <v>-58.495482</v>
+        <v>-58.453124</v>
       </c>
       <c r="N54" t="n">
-        <v>-34.552614</v>
+        <v>-34.567382</v>
       </c>
       <c r="O54" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P54" t="inlineStr">
@@ -4530,7 +4530,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>6447</t>
+          <t>-519</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
@@ -4540,17 +4540,17 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>CIUDAD DE LA PAZ 1535</t>
+          <t>Vilela 2687</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>808400333</t>
+          <t>808400334</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
@@ -4565,7 +4565,7 @@
       </c>
       <c r="H55" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>CAmbiar columna 114 picada en base</t>
         </is>
       </c>
       <c r="I55" t="n">
@@ -4587,14 +4587,14 @@
         </is>
       </c>
       <c r="M55" t="n">
-        <v>-58.453124</v>
+        <v>-58.472968</v>
       </c>
       <c r="N55" t="n">
-        <v>-34.567382</v>
+        <v>-34.546898</v>
       </c>
       <c r="O55" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P55" t="inlineStr">
@@ -4606,7 +4606,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>-519</t>
+          <t>-520</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
@@ -4616,7 +4616,7 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>Vilela 2687</t>
+          <t>Pedraza Manuela 4101</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
@@ -4626,7 +4626,7 @@
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>808400334</t>
+          <t>808400353</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
@@ -4641,7 +4641,7 @@
       </c>
       <c r="H56" t="inlineStr">
         <is>
-          <t>CAmbiar columna 114 picada en base</t>
+          <t xml:space="preserve">Podrida en la base </t>
         </is>
       </c>
       <c r="I56" t="n">
@@ -4663,10 +4663,10 @@
         </is>
       </c>
       <c r="M56" t="n">
-        <v>-58.472968</v>
+        <v>-58.481569</v>
       </c>
       <c r="N56" t="n">
-        <v>-34.546898</v>
+        <v>-34.559853</v>
       </c>
       <c r="O56" t="inlineStr">
         <is>
@@ -4682,27 +4682,27 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>-520</t>
+          <t>-525</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>7/17/2025</t>
+          <t>7/22/2025</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>Pedraza Manuela 4101</t>
+          <t>Zabala 3567</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>808400353</t>
+          <t>808480549</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
@@ -4717,7 +4717,7 @@
       </c>
       <c r="H57" t="inlineStr">
         <is>
-          <t xml:space="preserve">Podrida en la base </t>
+          <t>Corroida en base para recambio</t>
         </is>
       </c>
       <c r="I57" t="n">
@@ -4739,14 +4739,14 @@
         </is>
       </c>
       <c r="M57" t="n">
-        <v>-58.481569</v>
+        <v>-58.457492</v>
       </c>
       <c r="N57" t="n">
-        <v>-34.559853</v>
+        <v>-34.579336</v>
       </c>
       <c r="O57" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P57" t="inlineStr">

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-07-23 11:53:17)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_NEW.xlsx
+++ b/mapa_interactivo_NEW.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P57"/>
+  <dimension ref="A1:P62"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2022,7 +2022,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>804922177</t>
+          <t>804922147</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -2032,7 +2032,7 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Moldes 1717</t>
+          <t>Av. Álvarez Thomas 1171</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
@@ -2042,7 +2042,7 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>804922177</t>
+          <t>804922147</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
@@ -2061,7 +2061,7 @@
         </is>
       </c>
       <c r="I22" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J22" t="inlineStr">
         <is>
@@ -2079,10 +2079,10 @@
         </is>
       </c>
       <c r="M22" t="n">
-        <v>-58.45643</v>
+        <v>-58.45793</v>
       </c>
       <c r="N22" t="n">
-        <v>-34.567121</v>
+        <v>-34.578334</v>
       </c>
       <c r="O22" t="inlineStr">
         <is>
@@ -2098,7 +2098,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>5656</t>
+          <t>804922171</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -2108,17 +2108,17 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>ECHEVERRIA 5893</t>
+          <t>Virrey Arredondo 3581</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>804922184</t>
+          <t>804922171</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
@@ -2133,7 +2133,7 @@
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>Poste con base quebrada</t>
+          <t>Aplomar</t>
         </is>
       </c>
       <c r="I23" t="n">
@@ -2141,7 +2141,7 @@
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>Desmonte</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K23" t="inlineStr">
@@ -2151,18 +2151,18 @@
       </c>
       <c r="L23" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M23" t="n">
-        <v>-58.489627</v>
+        <v>-58.459513</v>
       </c>
       <c r="N23" t="n">
-        <v>-34.583761</v>
+        <v>-34.578019</v>
       </c>
       <c r="O23" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P23" t="inlineStr">
@@ -2174,27 +2174,27 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>6173</t>
+          <t>804922177</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>4/29/2025</t>
+          <t>4/24/2025</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>ARMENIA 2321</t>
+          <t>Moldes 1717</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>805507398</t>
+          <t>804922177</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
@@ -2209,7 +2209,7 @@
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>Picada volvio a entrar como caso 6325</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I24" t="n">
@@ -2231,36 +2231,36 @@
         </is>
       </c>
       <c r="M24" t="n">
-        <v>-58.420549</v>
+        <v>-58.45643</v>
       </c>
       <c r="N24" t="n">
-        <v>-34.585103</v>
+        <v>-34.567121</v>
       </c>
       <c r="O24" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P24" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>5715</t>
+          <t>5656</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>5/1/2025</t>
+          <t>4/24/2025</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>CUENCA 4690</t>
+          <t>ECHEVERRIA 5893</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
@@ -2270,7 +2270,7 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>805579094</t>
+          <t>804922184</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
@@ -2285,7 +2285,7 @@
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>Aplomar poste</t>
+          <t>Poste con base quebrada</t>
         </is>
       </c>
       <c r="I25" t="n">
@@ -2293,7 +2293,7 @@
       </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Desmonte</t>
         </is>
       </c>
       <c r="K25" t="inlineStr">
@@ -2307,10 +2307,10 @@
         </is>
       </c>
       <c r="M25" t="n">
-        <v>-58.506061</v>
+        <v>-58.489627</v>
       </c>
       <c r="N25" t="n">
-        <v>-34.588887</v>
+        <v>-34.583761</v>
       </c>
       <c r="O25" t="inlineStr">
         <is>
@@ -2326,27 +2326,27 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>5719</t>
+          <t>6173</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>5/1/2025</t>
+          <t>4/29/2025</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>CABEZON, JOSE LEON 2440</t>
+          <t>ARMENIA 2321</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>805579157</t>
+          <t>805507398</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
@@ -2361,7 +2361,7 @@
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Picada volvio a entrar como caso 6325</t>
         </is>
       </c>
       <c r="I26" t="n">
@@ -2383,26 +2383,26 @@
         </is>
       </c>
       <c r="M26" t="n">
-        <v>-58.499967</v>
+        <v>-58.420549</v>
       </c>
       <c r="N26" t="n">
-        <v>-34.57974</v>
+        <v>-34.585103</v>
       </c>
       <c r="O26" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P26" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>6333</t>
+          <t>5715</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -2412,17 +2412,17 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>ORTEGA Y GASSET 1816</t>
+          <t>CUENCA 4690</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>805655342</t>
+          <t>805579094</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
@@ -2437,7 +2437,7 @@
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Aplomar poste</t>
         </is>
       </c>
       <c r="I27" t="n">
@@ -2445,7 +2445,7 @@
       </c>
       <c r="J27" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K27" t="inlineStr">
@@ -2455,50 +2455,50 @@
       </c>
       <c r="L27" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M27" t="n">
-        <v>-58.432556</v>
+        <v>-58.506061</v>
       </c>
       <c r="N27" t="n">
-        <v>-34.570279</v>
+        <v>-34.588887</v>
       </c>
       <c r="O27" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P27" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>805707165</t>
+          <t>5719</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>5/7/2025</t>
+          <t>5/1/2025</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Baez 793</t>
+          <t>CABEZON, JOSE LEON 2440</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>805707165</t>
+          <t>805579157</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
@@ -2513,7 +2513,7 @@
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>DESMONTAR COLUMNA DE 7 MTS Y TRANSFERIR A COMUNITARIA</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I28" t="n">
@@ -2531,50 +2531,50 @@
       </c>
       <c r="L28" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M28" t="n">
-        <v>-58.436165</v>
+        <v>-58.499967</v>
       </c>
       <c r="N28" t="n">
-        <v>-34.569081</v>
+        <v>-34.57974</v>
       </c>
       <c r="O28" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P28" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>5847</t>
+          <t>6333</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>5/8/2025</t>
+          <t>5/1/2025</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>JURAMENTO 5321</t>
+          <t>ORTEGA Y GASSET 1816</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>805791839</t>
+          <t>805655342</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
@@ -2611,36 +2611,36 @@
         </is>
       </c>
       <c r="M29" t="n">
-        <v>-58.485193</v>
+        <v>-58.432556</v>
       </c>
       <c r="N29" t="n">
-        <v>-34.579621</v>
+        <v>-34.570279</v>
       </c>
       <c r="O29" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P29" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>232</t>
+          <t>805707165</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>5/9/2025</t>
+          <t>5/7/2025</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Gorostiaga 2286</t>
+          <t>Baez 793</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
@@ -2650,7 +2650,7 @@
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>805791858</t>
+          <t>805707165</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
@@ -2665,7 +2665,7 @@
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>DESMONTAR COLUMNA DE 7 MTS Y TRANSFERIR A COMUNITARIA</t>
         </is>
       </c>
       <c r="I30" t="n">
@@ -2683,14 +2683,14 @@
       </c>
       <c r="L30" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M30" t="n">
-        <v>-58.441563</v>
+        <v>-58.436165</v>
       </c>
       <c r="N30" t="n">
-        <v>-34.569743</v>
+        <v>-34.569081</v>
       </c>
       <c r="O30" t="inlineStr">
         <is>
@@ -2706,17 +2706,17 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>5826</t>
+          <t>5847</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>5/19/2025</t>
+          <t>5/8/2025</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>ALBARELLOS AV. 3180</t>
+          <t>JURAMENTO 5321</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
@@ -2726,7 +2726,7 @@
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>806926466</t>
+          <t>805791839</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
@@ -2741,7 +2741,7 @@
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>Columna (metal) inclinada</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I31" t="n">
@@ -2749,7 +2749,7 @@
       </c>
       <c r="J31" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K31" t="inlineStr">
@@ -2759,14 +2759,14 @@
       </c>
       <c r="L31" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M31" t="n">
-        <v>-58.513552</v>
+        <v>-58.485193</v>
       </c>
       <c r="N31" t="n">
-        <v>-34.579829</v>
+        <v>-34.579621</v>
       </c>
       <c r="O31" t="inlineStr">
         <is>
@@ -2782,27 +2782,27 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>5825</t>
+          <t>232</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>5/19/2025</t>
+          <t>5/9/2025</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>PAZ, GRAL. AV. 5602</t>
+          <t>Gorostiaga 2286</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>806926472</t>
+          <t>805791858</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
@@ -2817,7 +2817,7 @@
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>reparar rienda cortada - ver foto no es la misma que albarellos</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I32" t="n">
@@ -2825,7 +2825,7 @@
       </c>
       <c r="J32" t="inlineStr">
         <is>
-          <t>Tensor</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K32" t="inlineStr">
@@ -2835,40 +2835,40 @@
       </c>
       <c r="L32" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M32" t="n">
-        <v>-58.513685</v>
+        <v>-58.441563</v>
       </c>
       <c r="N32" t="n">
-        <v>-34.579838</v>
+        <v>-34.569743</v>
       </c>
       <c r="O32" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P32" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>5875</t>
+          <t>5826</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>5/27/2025</t>
+          <t>5/19/2025</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>MONROE 4096</t>
+          <t>ALBARELLOS AV. 3180</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
@@ -2878,7 +2878,7 @@
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>806975680</t>
+          <t>806926466</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
@@ -2893,7 +2893,7 @@
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Columna (metal) inclinada</t>
         </is>
       </c>
       <c r="I33" t="n">
@@ -2901,7 +2901,7 @@
       </c>
       <c r="J33" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K33" t="inlineStr">
@@ -2911,18 +2911,18 @@
       </c>
       <c r="L33" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M33" t="n">
-        <v>-58.476106</v>
+        <v>-58.513552</v>
       </c>
       <c r="N33" t="n">
-        <v>-34.568373</v>
+        <v>-34.579829</v>
       </c>
       <c r="O33" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P33" t="inlineStr">
@@ -2934,27 +2934,27 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>807044192</t>
+          <t>5825</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>5/29/2025</t>
+          <t>5/19/2025</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>O'Higgins 4379</t>
+          <t>PAZ, GRAL. AV. 5602</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>807044192</t>
+          <t>806926472</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
@@ -2969,7 +2969,7 @@
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t xml:space="preserve">Poste </t>
+          <t>reparar rienda cortada - ver foto no es la misma que albarellos</t>
         </is>
       </c>
       <c r="I34" t="n">
@@ -2977,7 +2977,7 @@
       </c>
       <c r="J34" t="inlineStr">
         <is>
-          <t>Desmonte</t>
+          <t>Tensor</t>
         </is>
       </c>
       <c r="K34" t="inlineStr">
@@ -2987,18 +2987,18 @@
       </c>
       <c r="L34" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M34" t="n">
-        <v>-58.468425</v>
+        <v>-58.513685</v>
       </c>
       <c r="N34" t="n">
-        <v>-34.54124</v>
+        <v>-34.579838</v>
       </c>
       <c r="O34" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P34" t="inlineStr">
@@ -3010,27 +3010,27 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>6020</t>
+          <t>5875</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>6/5/2025</t>
+          <t>5/27/2025</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>RAVIGNANI, EMILIO, DR. 2036</t>
+          <t>MONROE 4096</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>807215465</t>
+          <t>806975680</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
@@ -3067,46 +3067,46 @@
         </is>
       </c>
       <c r="M35" t="n">
-        <v>-58.436298</v>
+        <v>-58.476106</v>
       </c>
       <c r="N35" t="n">
-        <v>-34.578972</v>
+        <v>-34.568373</v>
       </c>
       <c r="O35" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P35" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>6144</t>
+          <t>807044192</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>6/11/2025</t>
+          <t>5/29/2025</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>TURIN 2990</t>
+          <t>O'Higgins 4379</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>807458282</t>
+          <t>807044192</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
@@ -3121,7 +3121,7 @@
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t xml:space="preserve">Poste </t>
         </is>
       </c>
       <c r="I36" t="n">
@@ -3129,7 +3129,7 @@
       </c>
       <c r="J36" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Desmonte</t>
         </is>
       </c>
       <c r="K36" t="inlineStr">
@@ -3139,18 +3139,18 @@
       </c>
       <c r="L36" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M36" t="n">
-        <v>-58.480925</v>
+        <v>-58.468425</v>
       </c>
       <c r="N36" t="n">
-        <v>-34.585471</v>
+        <v>-34.54124</v>
       </c>
       <c r="O36" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P36" t="inlineStr">
@@ -3162,27 +3162,27 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>6143</t>
+          <t>6020</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>6/11/2025</t>
+          <t>6/5/2025</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>SOLANO LOPEZ, F., MARISCAL 2845</t>
+          <t>RAVIGNANI, EMILIO, DR. 2036</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>807458296</t>
+          <t>807215465</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
@@ -3219,26 +3219,26 @@
         </is>
       </c>
       <c r="M37" t="n">
-        <v>-58.495071</v>
+        <v>-58.436298</v>
       </c>
       <c r="N37" t="n">
-        <v>-34.593122</v>
+        <v>-34.578972</v>
       </c>
       <c r="O37" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P37" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>6141</t>
+          <t>6144</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
@@ -3248,17 +3248,17 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>EL PAMPERO 2618</t>
+          <t>TURIN 2990</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>807458310</t>
+          <t>807458282</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
@@ -3295,10 +3295,10 @@
         </is>
       </c>
       <c r="M38" t="n">
-        <v>-58.481942</v>
+        <v>-58.480925</v>
       </c>
       <c r="N38" t="n">
-        <v>-34.602989</v>
+        <v>-34.585471</v>
       </c>
       <c r="O38" t="inlineStr">
         <is>
@@ -3314,27 +3314,27 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>-478</t>
+          <t>6143</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>6/15/2025</t>
+          <t>6/11/2025</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Chivilcoy 4875</t>
+          <t>SOLANO LOPEZ, F., MARISCAL 2845</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>807508509</t>
+          <t>807458296</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
@@ -3349,7 +3349,7 @@
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>Poste podrido</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I39" t="n">
@@ -3367,14 +3367,14 @@
       </c>
       <c r="L39" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M39" t="n">
-        <v>-58.517389</v>
+        <v>-58.495071</v>
       </c>
       <c r="N39" t="n">
-        <v>-34.593541</v>
+        <v>-34.593122</v>
       </c>
       <c r="O39" t="inlineStr">
         <is>
@@ -3390,27 +3390,27 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>6171</t>
+          <t>6141</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>6/18/2025</t>
+          <t>6/11/2025</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>CABELLO 3486</t>
+          <t>EL PAMPERO 2618</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>807658640</t>
+          <t>807458310</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
@@ -3425,7 +3425,7 @@
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t>Columna inclinada evaluar con inspector un corrimiento</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I40" t="n">
@@ -3447,46 +3447,46 @@
         </is>
       </c>
       <c r="M40" t="n">
-        <v>-58.409579</v>
+        <v>-58.481942</v>
       </c>
       <c r="N40" t="n">
-        <v>-34.581134</v>
+        <v>-34.602989</v>
       </c>
       <c r="O40" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P40" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>6230</t>
+          <t>-478</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>6/24/2025</t>
+          <t>6/15/2025</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Santa maria de oro	2722</t>
+          <t>Chivilcoy 4875</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>807763066</t>
+          <t>807508509</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
@@ -3501,7 +3501,7 @@
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Poste podrido</t>
         </is>
       </c>
       <c r="I41" t="n">
@@ -3519,40 +3519,40 @@
       </c>
       <c r="L41" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M41" t="n">
-        <v>-58.422315</v>
+        <v>-58.517389</v>
       </c>
       <c r="N41" t="n">
-        <v>-34.576988</v>
+        <v>-34.593541</v>
       </c>
       <c r="O41" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P41" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>6231</t>
+          <t>6171</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>6/24/2025</t>
+          <t>6/18/2025</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Ciudad de la Paz 275</t>
+          <t>CABELLO 3486</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
@@ -3562,7 +3562,7 @@
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>807763070</t>
+          <t>807658640</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
@@ -3577,7 +3577,7 @@
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>Aplomar o cambiar</t>
+          <t>Columna inclinada evaluar con inspector un corrimiento</t>
         </is>
       </c>
       <c r="I42" t="n">
@@ -3595,14 +3595,14 @@
       </c>
       <c r="L42" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M42" t="n">
-        <v>-58.441049</v>
+        <v>-58.409579</v>
       </c>
       <c r="N42" t="n">
-        <v>-34.574625</v>
+        <v>-34.581134</v>
       </c>
       <c r="O42" t="inlineStr">
         <is>
@@ -3618,7 +3618,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>6235</t>
+          <t>6230</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
@@ -3628,17 +3628,17 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>HUERGO 389</t>
+          <t>Santa maria de oro	2722</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>807763078</t>
+          <t>807763066</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
@@ -3675,10 +3675,10 @@
         </is>
       </c>
       <c r="M43" t="n">
-        <v>-58.432722</v>
+        <v>-58.422315</v>
       </c>
       <c r="N43" t="n">
-        <v>-34.572371</v>
+        <v>-34.576988</v>
       </c>
       <c r="O43" t="inlineStr">
         <is>
@@ -3694,17 +3694,17 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>6295</t>
+          <t>6231</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>6/30/2025</t>
+          <t>6/24/2025</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>SOLER 6017</t>
+          <t>Ciudad de la Paz 275</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
@@ -3714,7 +3714,7 @@
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>807851636</t>
+          <t>807763070</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
@@ -3729,7 +3729,7 @@
       </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Aplomar o cambiar</t>
         </is>
       </c>
       <c r="I44" t="n">
@@ -3747,14 +3747,14 @@
       </c>
       <c r="L44" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M44" t="n">
-        <v>-58.436808</v>
+        <v>-58.441049</v>
       </c>
       <c r="N44" t="n">
-        <v>-34.577464</v>
+        <v>-34.574625</v>
       </c>
       <c r="O44" t="inlineStr">
         <is>
@@ -3770,27 +3770,27 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>6331</t>
+          <t>6235</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>7/3/2025</t>
+          <t>6/24/2025</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>PARAGUAY 4259</t>
+          <t>HUERGO 389</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>807965788</t>
+          <t>807763078</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
@@ -3827,10 +3827,10 @@
         </is>
       </c>
       <c r="M45" t="n">
-        <v>-58.421822</v>
+        <v>-58.432722</v>
       </c>
       <c r="N45" t="n">
-        <v>-34.58645</v>
+        <v>-34.572371</v>
       </c>
       <c r="O45" t="inlineStr">
         <is>
@@ -3846,17 +3846,17 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>6332</t>
+          <t>6295</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>7/3/2025</t>
+          <t>6/30/2025</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>ARAOZ 2560</t>
+          <t>SOLER 6017</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
@@ -3866,7 +3866,7 @@
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>807965818</t>
+          <t>807851636</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
@@ -3903,10 +3903,10 @@
         </is>
       </c>
       <c r="M46" t="n">
-        <v>-58.414507</v>
+        <v>-58.436808</v>
       </c>
       <c r="N46" t="n">
-        <v>-34.585377</v>
+        <v>-34.577464</v>
       </c>
       <c r="O46" t="inlineStr">
         <is>
@@ -3922,7 +3922,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>6336</t>
+          <t>6331</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
@@ -3932,7 +3932,7 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>PARAGUAY 4291</t>
+          <t>PARAGUAY 4259</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
@@ -3942,7 +3942,7 @@
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>807965819</t>
+          <t>807965788</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
@@ -3979,10 +3979,10 @@
         </is>
       </c>
       <c r="M47" t="n">
-        <v>-58.422084</v>
+        <v>-58.421822</v>
       </c>
       <c r="N47" t="n">
-        <v>-34.58625</v>
+        <v>-34.58645</v>
       </c>
       <c r="O47" t="inlineStr">
         <is>
@@ -3998,7 +3998,7 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>6337</t>
+          <t>6332</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
@@ -4008,7 +4008,7 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>PARAGUAY 4383</t>
+          <t>ARAOZ 2560</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
@@ -4018,7 +4018,7 @@
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>807965926</t>
+          <t>807965818</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
@@ -4055,10 +4055,10 @@
         </is>
       </c>
       <c r="M48" t="n">
-        <v>-58.422931</v>
+        <v>-58.414507</v>
       </c>
       <c r="N48" t="n">
-        <v>-34.585597</v>
+        <v>-34.585377</v>
       </c>
       <c r="O48" t="inlineStr">
         <is>
@@ -4074,27 +4074,27 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>6363</t>
+          <t>6336</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>7/8/2025</t>
+          <t>7/3/2025</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>MOLDES 3730</t>
+          <t>PARAGUAY 4291</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>808099415</t>
+          <t>807965819</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
@@ -4109,7 +4109,7 @@
       </c>
       <c r="H49" t="inlineStr">
         <is>
-          <t>Poste inclinado</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I49" t="n">
@@ -4117,7 +4117,7 @@
       </c>
       <c r="J49" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K49" t="inlineStr">
@@ -4127,50 +4127,50 @@
       </c>
       <c r="L49" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M49" t="n">
-        <v>-58.47192</v>
+        <v>-58.422084</v>
       </c>
       <c r="N49" t="n">
-        <v>-34.549398</v>
+        <v>-34.58625</v>
       </c>
       <c r="O49" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P49" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>-503</t>
+          <t>6337</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>7/10/2025</t>
+          <t>7/3/2025</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Salguero 842</t>
+          <t>PARAGUAY 4383</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>808148673</t>
+          <t>807965926</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
@@ -4185,7 +4185,7 @@
       </c>
       <c r="H50" t="inlineStr">
         <is>
-          <t>Cambiar columna picada en la base</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I50" t="n">
@@ -4207,14 +4207,14 @@
         </is>
       </c>
       <c r="M50" t="n">
-        <v>-58.419166</v>
+        <v>-58.422931</v>
       </c>
       <c r="N50" t="n">
-        <v>-34.600265</v>
+        <v>-34.585597</v>
       </c>
       <c r="O50" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P50" t="inlineStr">
@@ -4226,27 +4226,27 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>-504</t>
+          <t>6363</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>7/10/2025</t>
+          <t>7/8/2025</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Ohiggins 1611</t>
+          <t>MOLDES 3730</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>808148679</t>
+          <t>808099415</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
@@ -4261,7 +4261,7 @@
       </c>
       <c r="H51" t="inlineStr">
         <is>
-          <t>Columna podrida en la base</t>
+          <t>Poste inclinado</t>
         </is>
       </c>
       <c r="I51" t="n">
@@ -4269,28 +4269,28 @@
       </c>
       <c r="J51" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K51" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L51" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M51" t="n">
-        <v>-58.448993</v>
+        <v>-58.47192</v>
       </c>
       <c r="N51" t="n">
-        <v>-34.564383</v>
+        <v>-34.549398</v>
       </c>
       <c r="O51" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P51" t="inlineStr">
@@ -4302,27 +4302,27 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>6392</t>
+          <t>-503</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>7/14/2025</t>
+          <t>7/10/2025</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>MOLDES 1808</t>
+          <t>Salguero 842</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>808194266</t>
+          <t>808148673</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
@@ -4337,7 +4337,7 @@
       </c>
       <c r="H52" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambiar columna picada en la base</t>
         </is>
       </c>
       <c r="I52" t="n">
@@ -4359,46 +4359,46 @@
         </is>
       </c>
       <c r="M52" t="n">
-        <v>-58.45719</v>
+        <v>-58.419166</v>
       </c>
       <c r="N52" t="n">
-        <v>-34.566365</v>
+        <v>-34.600265</v>
       </c>
       <c r="O52" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P52" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>6437</t>
+          <t>-504</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>7/17/2025</t>
+          <t>7/10/2025</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>MILLER 4590</t>
+          <t>Ohiggins 1611</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>808400306</t>
+          <t>808148679</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
@@ -4413,7 +4413,7 @@
       </c>
       <c r="H53" t="inlineStr">
         <is>
-          <t>Columna corroida</t>
+          <t>Columna podrida en la base</t>
         </is>
       </c>
       <c r="I53" t="n">
@@ -4426,7 +4426,7 @@
       </c>
       <c r="K53" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L53" t="inlineStr">
@@ -4435,14 +4435,14 @@
         </is>
       </c>
       <c r="M53" t="n">
-        <v>-58.495482</v>
+        <v>-58.448993</v>
       </c>
       <c r="N53" t="n">
-        <v>-34.552614</v>
+        <v>-34.564383</v>
       </c>
       <c r="O53" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P53" t="inlineStr">
@@ -4454,17 +4454,17 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>6447</t>
+          <t>6392</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>7/17/2025</t>
+          <t>7/14/2025</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>CIUDAD DE LA PAZ 1535</t>
+          <t>MOLDES 1808</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
@@ -4474,7 +4474,7 @@
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>808400333</t>
+          <t>808194266</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
@@ -4511,10 +4511,10 @@
         </is>
       </c>
       <c r="M54" t="n">
-        <v>-58.453124</v>
+        <v>-58.45719</v>
       </c>
       <c r="N54" t="n">
-        <v>-34.567382</v>
+        <v>-34.566365</v>
       </c>
       <c r="O54" t="inlineStr">
         <is>
@@ -4530,7 +4530,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>-519</t>
+          <t>6437</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
@@ -4540,7 +4540,7 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>Vilela 2687</t>
+          <t>MILLER 4590</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
@@ -4550,7 +4550,7 @@
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>808400334</t>
+          <t>808400306</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
@@ -4565,7 +4565,7 @@
       </c>
       <c r="H55" t="inlineStr">
         <is>
-          <t>CAmbiar columna 114 picada en base</t>
+          <t>Columna corroida</t>
         </is>
       </c>
       <c r="I55" t="n">
@@ -4587,10 +4587,10 @@
         </is>
       </c>
       <c r="M55" t="n">
-        <v>-58.472968</v>
+        <v>-58.495482</v>
       </c>
       <c r="N55" t="n">
-        <v>-34.546898</v>
+        <v>-34.552614</v>
       </c>
       <c r="O55" t="inlineStr">
         <is>
@@ -4606,7 +4606,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>-520</t>
+          <t>6447</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
@@ -4616,17 +4616,17 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>Pedraza Manuela 4101</t>
+          <t>CIUDAD DE LA PAZ 1535</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>808400353</t>
+          <t>808400333</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
@@ -4641,7 +4641,7 @@
       </c>
       <c r="H56" t="inlineStr">
         <is>
-          <t xml:space="preserve">Podrida en la base </t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I56" t="n">
@@ -4663,14 +4663,14 @@
         </is>
       </c>
       <c r="M56" t="n">
-        <v>-58.481569</v>
+        <v>-58.453124</v>
       </c>
       <c r="N56" t="n">
-        <v>-34.559853</v>
+        <v>-34.567382</v>
       </c>
       <c r="O56" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P56" t="inlineStr">
@@ -4682,74 +4682,454 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
+          <t>-519</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>7/17/2025</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>Vilela 2687</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>808400334</t>
+        </is>
+      </c>
+      <c r="F57" t="inlineStr">
+        <is>
+          <t>NEW</t>
+        </is>
+      </c>
+      <c r="G57" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H57" t="inlineStr">
+        <is>
+          <t>CAmbiar columna 114 picada en base</t>
+        </is>
+      </c>
+      <c r="I57" t="n">
+        <v>1</v>
+      </c>
+      <c r="J57" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K57" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L57" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M57" t="n">
+        <v>-58.472968</v>
+      </c>
+      <c r="N57" t="n">
+        <v>-34.546898</v>
+      </c>
+      <c r="O57" t="inlineStr">
+        <is>
+          <t>Saavedra</t>
+        </is>
+      </c>
+      <c r="P57" t="inlineStr">
+        <is>
+          <t>Capital Norte</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>-520</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>7/17/2025</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>Pedraza Manuela 4101</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>808400353</t>
+        </is>
+      </c>
+      <c r="F58" t="inlineStr">
+        <is>
+          <t>NEW</t>
+        </is>
+      </c>
+      <c r="G58" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H58" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Podrida en la base </t>
+        </is>
+      </c>
+      <c r="I58" t="n">
+        <v>1</v>
+      </c>
+      <c r="J58" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K58" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L58" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M58" t="n">
+        <v>-58.481569</v>
+      </c>
+      <c r="N58" t="n">
+        <v>-34.559853</v>
+      </c>
+      <c r="O58" t="inlineStr">
+        <is>
+          <t>Saavedra</t>
+        </is>
+      </c>
+      <c r="P58" t="inlineStr">
+        <is>
+          <t>Capital Norte</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
           <t>-525</t>
         </is>
       </c>
-      <c r="B57" t="inlineStr">
+      <c r="B59" t="inlineStr">
         <is>
           <t>7/22/2025</t>
         </is>
       </c>
-      <c r="C57" t="inlineStr">
+      <c r="C59" t="inlineStr">
         <is>
           <t>Zabala 3567</t>
         </is>
       </c>
-      <c r="D57" t="inlineStr">
+      <c r="D59" t="inlineStr">
         <is>
           <t>15</t>
         </is>
       </c>
-      <c r="E57" t="inlineStr">
+      <c r="E59" t="inlineStr">
         <is>
           <t>808480549</t>
         </is>
       </c>
-      <c r="F57" t="inlineStr">
-        <is>
-          <t>NEW</t>
-        </is>
-      </c>
-      <c r="G57" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H57" t="inlineStr">
+      <c r="F59" t="inlineStr">
+        <is>
+          <t>NEW</t>
+        </is>
+      </c>
+      <c r="G59" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H59" t="inlineStr">
         <is>
           <t>Corroida en base para recambio</t>
         </is>
       </c>
-      <c r="I57" t="n">
-        <v>1</v>
-      </c>
-      <c r="J57" t="inlineStr">
+      <c r="I59" t="n">
+        <v>1</v>
+      </c>
+      <c r="J59" t="inlineStr">
         <is>
           <t>Cambio</t>
         </is>
       </c>
-      <c r="K57" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L57" t="inlineStr">
+      <c r="K59" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L59" t="inlineStr">
         <is>
           <t>Pasante</t>
         </is>
       </c>
-      <c r="M57" t="n">
+      <c r="M59" t="n">
         <v>-58.457492</v>
       </c>
-      <c r="N57" t="n">
+      <c r="N59" t="n">
         <v>-34.579336</v>
       </c>
-      <c r="O57" t="inlineStr">
+      <c r="O59" t="inlineStr">
         <is>
           <t>Colegiales</t>
         </is>
       </c>
-      <c r="P57" t="inlineStr">
+      <c r="P59" t="inlineStr">
+        <is>
+          <t>Capital Norte</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>-526</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>7/23/2025</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>Moldes 1813</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>13</t>
+        </is>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>808488825</t>
+        </is>
+      </c>
+      <c r="F60" t="inlineStr">
+        <is>
+          <t>NEW</t>
+        </is>
+      </c>
+      <c r="G60" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H60" t="inlineStr">
+        <is>
+          <t>Cambiar</t>
+        </is>
+      </c>
+      <c r="I60" t="n">
+        <v>1</v>
+      </c>
+      <c r="J60" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K60" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L60" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M60" t="n">
+        <v>-58.457145</v>
+      </c>
+      <c r="N60" t="n">
+        <v>-34.56629</v>
+      </c>
+      <c r="O60" t="inlineStr">
+        <is>
+          <t>Colegiales</t>
+        </is>
+      </c>
+      <c r="P60" t="inlineStr">
+        <is>
+          <t>Capital Norte</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>-527</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>7/23/2025</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>Moldes 1761</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>13</t>
+        </is>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>808488822</t>
+        </is>
+      </c>
+      <c r="F61" t="inlineStr">
+        <is>
+          <t>NEW</t>
+        </is>
+      </c>
+      <c r="G61" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H61" t="inlineStr">
+        <is>
+          <t>Picada</t>
+        </is>
+      </c>
+      <c r="I61" t="n">
+        <v>1</v>
+      </c>
+      <c r="J61" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K61" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L61" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M61" t="n">
+        <v>-58.456734</v>
+      </c>
+      <c r="N61" t="n">
+        <v>-34.566768</v>
+      </c>
+      <c r="O61" t="inlineStr">
+        <is>
+          <t>Colegiales</t>
+        </is>
+      </c>
+      <c r="P61" t="inlineStr">
+        <is>
+          <t>Capital Norte</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>-528</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>7/23/2025</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>Moldes 1743</t>
+        </is>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>13</t>
+        </is>
+      </c>
+      <c r="E62" t="inlineStr">
+        <is>
+          <t>808488806</t>
+        </is>
+      </c>
+      <c r="F62" t="inlineStr">
+        <is>
+          <t>NEW</t>
+        </is>
+      </c>
+      <c r="G62" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H62" t="inlineStr">
+        <is>
+          <t>Picada</t>
+        </is>
+      </c>
+      <c r="I62" t="n">
+        <v>1</v>
+      </c>
+      <c r="J62" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K62" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L62" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M62" t="n">
+        <v>-58.456563</v>
+      </c>
+      <c r="N62" t="n">
+        <v>-34.566967</v>
+      </c>
+      <c r="O62" t="inlineStr">
+        <is>
+          <t>Colegiales</t>
+        </is>
+      </c>
+      <c r="P62" t="inlineStr">
         <is>
           <t>Capital Norte</t>
         </is>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-07-23 15:06:53)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_NEW.xlsx
+++ b/mapa_interactivo_NEW.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P62"/>
+  <dimension ref="A1:P59"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2174,7 +2174,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>804922177</t>
+          <t>5656</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -2184,17 +2184,17 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Moldes 1717</t>
+          <t>ECHEVERRIA 5893</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>804922177</t>
+          <t>804922184</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
@@ -2209,7 +2209,7 @@
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Poste con base quebrada</t>
         </is>
       </c>
       <c r="I24" t="n">
@@ -2217,7 +2217,7 @@
       </c>
       <c r="J24" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Desmonte</t>
         </is>
       </c>
       <c r="K24" t="inlineStr">
@@ -2227,18 +2227,18 @@
       </c>
       <c r="L24" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M24" t="n">
-        <v>-58.45643</v>
+        <v>-58.489627</v>
       </c>
       <c r="N24" t="n">
-        <v>-34.567121</v>
+        <v>-34.583761</v>
       </c>
       <c r="O24" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P24" t="inlineStr">
@@ -2250,27 +2250,27 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>5656</t>
+          <t>6173</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>4/24/2025</t>
+          <t>4/29/2025</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>ECHEVERRIA 5893</t>
+          <t>ARMENIA 2321</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>804922184</t>
+          <t>805507398</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
@@ -2285,7 +2285,7 @@
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>Poste con base quebrada</t>
+          <t>Picada volvio a entrar como caso 6325</t>
         </is>
       </c>
       <c r="I25" t="n">
@@ -2293,7 +2293,7 @@
       </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t>Desmonte</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K25" t="inlineStr">
@@ -2303,50 +2303,50 @@
       </c>
       <c r="L25" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M25" t="n">
-        <v>-58.489627</v>
+        <v>-58.420549</v>
       </c>
       <c r="N25" t="n">
-        <v>-34.583761</v>
+        <v>-34.585103</v>
       </c>
       <c r="O25" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P25" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>6173</t>
+          <t>5715</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>4/29/2025</t>
+          <t>5/1/2025</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>ARMENIA 2321</t>
+          <t>CUENCA 4690</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>805507398</t>
+          <t>805579094</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
@@ -2361,7 +2361,7 @@
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>Picada volvio a entrar como caso 6325</t>
+          <t>Aplomar poste</t>
         </is>
       </c>
       <c r="I26" t="n">
@@ -2369,7 +2369,7 @@
       </c>
       <c r="J26" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K26" t="inlineStr">
@@ -2379,30 +2379,30 @@
       </c>
       <c r="L26" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M26" t="n">
-        <v>-58.420549</v>
+        <v>-58.506061</v>
       </c>
       <c r="N26" t="n">
-        <v>-34.585103</v>
+        <v>-34.588887</v>
       </c>
       <c r="O26" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P26" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>5715</t>
+          <t>5719</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -2412,7 +2412,7 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>CUENCA 4690</t>
+          <t>CABEZON, JOSE LEON 2440</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
@@ -2422,7 +2422,7 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>805579094</t>
+          <t>805579157</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
@@ -2437,7 +2437,7 @@
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>Aplomar poste</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I27" t="n">
@@ -2445,7 +2445,7 @@
       </c>
       <c r="J27" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K27" t="inlineStr">
@@ -2455,14 +2455,14 @@
       </c>
       <c r="L27" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M27" t="n">
-        <v>-58.506061</v>
+        <v>-58.499967</v>
       </c>
       <c r="N27" t="n">
-        <v>-34.588887</v>
+        <v>-34.57974</v>
       </c>
       <c r="O27" t="inlineStr">
         <is>
@@ -2478,7 +2478,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>5719</t>
+          <t>6333</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -2488,17 +2488,17 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>CABEZON, JOSE LEON 2440</t>
+          <t>ORTEGA Y GASSET 1816</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>805579157</t>
+          <t>805655342</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
@@ -2535,36 +2535,36 @@
         </is>
       </c>
       <c r="M28" t="n">
-        <v>-58.499967</v>
+        <v>-58.432556</v>
       </c>
       <c r="N28" t="n">
-        <v>-34.57974</v>
+        <v>-34.570279</v>
       </c>
       <c r="O28" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P28" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>6333</t>
+          <t>805707165</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>5/1/2025</t>
+          <t>5/7/2025</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>ORTEGA Y GASSET 1816</t>
+          <t>Baez 793</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
@@ -2574,7 +2574,7 @@
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>805655342</t>
+          <t>805707165</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
@@ -2589,7 +2589,7 @@
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>DESMONTAR COLUMNA DE 7 MTS Y TRANSFERIR A COMUNITARIA</t>
         </is>
       </c>
       <c r="I29" t="n">
@@ -2607,14 +2607,14 @@
       </c>
       <c r="L29" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M29" t="n">
-        <v>-58.432556</v>
+        <v>-58.436165</v>
       </c>
       <c r="N29" t="n">
-        <v>-34.570279</v>
+        <v>-34.569081</v>
       </c>
       <c r="O29" t="inlineStr">
         <is>
@@ -2630,27 +2630,27 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>805707165</t>
+          <t>5847</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>5/7/2025</t>
+          <t>5/8/2025</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Baez 793</t>
+          <t>JURAMENTO 5321</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>805707165</t>
+          <t>805791839</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
@@ -2665,7 +2665,7 @@
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>DESMONTAR COLUMNA DE 7 MTS Y TRANSFERIR A COMUNITARIA</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I30" t="n">
@@ -2683,50 +2683,50 @@
       </c>
       <c r="L30" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M30" t="n">
-        <v>-58.436165</v>
+        <v>-58.485193</v>
       </c>
       <c r="N30" t="n">
-        <v>-34.569081</v>
+        <v>-34.579621</v>
       </c>
       <c r="O30" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P30" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>5847</t>
+          <t>232</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>5/8/2025</t>
+          <t>5/9/2025</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>JURAMENTO 5321</t>
+          <t>Gorostiaga 2286</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>805791839</t>
+          <t>805791858</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
@@ -2763,46 +2763,46 @@
         </is>
       </c>
       <c r="M31" t="n">
-        <v>-58.485193</v>
+        <v>-58.441563</v>
       </c>
       <c r="N31" t="n">
-        <v>-34.579621</v>
+        <v>-34.569743</v>
       </c>
       <c r="O31" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P31" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>232</t>
+          <t>5826</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>5/9/2025</t>
+          <t>5/19/2025</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Gorostiaga 2286</t>
+          <t>ALBARELLOS AV. 3180</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>805791858</t>
+          <t>806926466</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
@@ -2817,7 +2817,7 @@
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Columna (metal) inclinada</t>
         </is>
       </c>
       <c r="I32" t="n">
@@ -2825,7 +2825,7 @@
       </c>
       <c r="J32" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K32" t="inlineStr">
@@ -2835,30 +2835,30 @@
       </c>
       <c r="L32" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M32" t="n">
-        <v>-58.441563</v>
+        <v>-58.513552</v>
       </c>
       <c r="N32" t="n">
-        <v>-34.569743</v>
+        <v>-34.579829</v>
       </c>
       <c r="O32" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P32" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>5826</t>
+          <t>5825</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -2868,7 +2868,7 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>ALBARELLOS AV. 3180</t>
+          <t>PAZ, GRAL. AV. 5602</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
@@ -2878,7 +2878,7 @@
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>806926466</t>
+          <t>806926472</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
@@ -2893,7 +2893,7 @@
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>Columna (metal) inclinada</t>
+          <t>reparar rienda cortada - ver foto no es la misma que albarellos</t>
         </is>
       </c>
       <c r="I33" t="n">
@@ -2901,7 +2901,7 @@
       </c>
       <c r="J33" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Tensor</t>
         </is>
       </c>
       <c r="K33" t="inlineStr">
@@ -2915,10 +2915,10 @@
         </is>
       </c>
       <c r="M33" t="n">
-        <v>-58.513552</v>
+        <v>-58.513685</v>
       </c>
       <c r="N33" t="n">
-        <v>-34.579829</v>
+        <v>-34.579838</v>
       </c>
       <c r="O33" t="inlineStr">
         <is>
@@ -2934,17 +2934,17 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>5825</t>
+          <t>5875</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>5/19/2025</t>
+          <t>5/27/2025</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>PAZ, GRAL. AV. 5602</t>
+          <t>MONROE 4096</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
@@ -2954,7 +2954,7 @@
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>806926472</t>
+          <t>806975680</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
@@ -2969,7 +2969,7 @@
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>reparar rienda cortada - ver foto no es la misma que albarellos</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I34" t="n">
@@ -2977,7 +2977,7 @@
       </c>
       <c r="J34" t="inlineStr">
         <is>
-          <t>Tensor</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K34" t="inlineStr">
@@ -2987,18 +2987,18 @@
       </c>
       <c r="L34" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M34" t="n">
-        <v>-58.513685</v>
+        <v>-58.476106</v>
       </c>
       <c r="N34" t="n">
-        <v>-34.579838</v>
+        <v>-34.568373</v>
       </c>
       <c r="O34" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P34" t="inlineStr">
@@ -3010,27 +3010,27 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>5875</t>
+          <t>807044192</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>5/27/2025</t>
+          <t>5/29/2025</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>MONROE 4096</t>
+          <t>O'Higgins 4379</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>806975680</t>
+          <t>807044192</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
@@ -3045,7 +3045,7 @@
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t xml:space="preserve">Poste </t>
         </is>
       </c>
       <c r="I35" t="n">
@@ -3053,7 +3053,7 @@
       </c>
       <c r="J35" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Desmonte</t>
         </is>
       </c>
       <c r="K35" t="inlineStr">
@@ -3063,18 +3063,18 @@
       </c>
       <c r="L35" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M35" t="n">
-        <v>-58.476106</v>
+        <v>-58.468425</v>
       </c>
       <c r="N35" t="n">
-        <v>-34.568373</v>
+        <v>-34.54124</v>
       </c>
       <c r="O35" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P35" t="inlineStr">
@@ -3086,27 +3086,27 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>807044192</t>
+          <t>6020</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>5/29/2025</t>
+          <t>6/5/2025</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>O'Higgins 4379</t>
+          <t>RAVIGNANI, EMILIO, DR. 2036</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>807044192</t>
+          <t>807215465</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
@@ -3121,7 +3121,7 @@
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t xml:space="preserve">Poste </t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I36" t="n">
@@ -3129,7 +3129,7 @@
       </c>
       <c r="J36" t="inlineStr">
         <is>
-          <t>Desmonte</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K36" t="inlineStr">
@@ -3139,50 +3139,50 @@
       </c>
       <c r="L36" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M36" t="n">
-        <v>-58.468425</v>
+        <v>-58.436298</v>
       </c>
       <c r="N36" t="n">
-        <v>-34.54124</v>
+        <v>-34.578972</v>
       </c>
       <c r="O36" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P36" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>6020</t>
+          <t>6144</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>6/5/2025</t>
+          <t>6/11/2025</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>RAVIGNANI, EMILIO, DR. 2036</t>
+          <t>TURIN 2990</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>807215465</t>
+          <t>807458282</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
@@ -3219,26 +3219,26 @@
         </is>
       </c>
       <c r="M37" t="n">
-        <v>-58.436298</v>
+        <v>-58.480925</v>
       </c>
       <c r="N37" t="n">
-        <v>-34.578972</v>
+        <v>-34.585471</v>
       </c>
       <c r="O37" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P37" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>6144</t>
+          <t>6143</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
@@ -3248,7 +3248,7 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>TURIN 2990</t>
+          <t>SOLANO LOPEZ, F., MARISCAL 2845</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
@@ -3258,7 +3258,7 @@
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>807458282</t>
+          <t>807458296</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
@@ -3295,10 +3295,10 @@
         </is>
       </c>
       <c r="M38" t="n">
-        <v>-58.480925</v>
+        <v>-58.495071</v>
       </c>
       <c r="N38" t="n">
-        <v>-34.585471</v>
+        <v>-34.593122</v>
       </c>
       <c r="O38" t="inlineStr">
         <is>
@@ -3314,7 +3314,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>6143</t>
+          <t>6141</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
@@ -3324,17 +3324,17 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>SOLANO LOPEZ, F., MARISCAL 2845</t>
+          <t>EL PAMPERO 2618</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>807458296</t>
+          <t>807458310</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
@@ -3371,10 +3371,10 @@
         </is>
       </c>
       <c r="M39" t="n">
-        <v>-58.495071</v>
+        <v>-58.481942</v>
       </c>
       <c r="N39" t="n">
-        <v>-34.593122</v>
+        <v>-34.602989</v>
       </c>
       <c r="O39" t="inlineStr">
         <is>
@@ -3390,17 +3390,17 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>6141</t>
+          <t>-478</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>6/11/2025</t>
+          <t>6/15/2025</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>EL PAMPERO 2618</t>
+          <t>Chivilcoy 4875</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
@@ -3410,7 +3410,7 @@
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>807458310</t>
+          <t>807508509</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
@@ -3425,7 +3425,7 @@
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Poste podrido</t>
         </is>
       </c>
       <c r="I40" t="n">
@@ -3443,14 +3443,14 @@
       </c>
       <c r="L40" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M40" t="n">
-        <v>-58.481942</v>
+        <v>-58.517389</v>
       </c>
       <c r="N40" t="n">
-        <v>-34.602989</v>
+        <v>-34.593541</v>
       </c>
       <c r="O40" t="inlineStr">
         <is>
@@ -3466,27 +3466,27 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>-478</t>
+          <t>6171</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>6/15/2025</t>
+          <t>6/18/2025</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Chivilcoy 4875</t>
+          <t>CABELLO 3486</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>807508509</t>
+          <t>807658640</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
@@ -3501,7 +3501,7 @@
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>Poste podrido</t>
+          <t>Columna inclinada evaluar con inspector un corrimiento</t>
         </is>
       </c>
       <c r="I41" t="n">
@@ -3519,40 +3519,40 @@
       </c>
       <c r="L41" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M41" t="n">
-        <v>-58.517389</v>
+        <v>-58.409579</v>
       </c>
       <c r="N41" t="n">
-        <v>-34.593541</v>
+        <v>-34.581134</v>
       </c>
       <c r="O41" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P41" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>6171</t>
+          <t>6230</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>6/18/2025</t>
+          <t>6/24/2025</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>CABELLO 3486</t>
+          <t>Santa maria de oro	2722</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
@@ -3562,7 +3562,7 @@
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>807658640</t>
+          <t>807763066</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
@@ -3577,7 +3577,7 @@
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>Columna inclinada evaluar con inspector un corrimiento</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I42" t="n">
@@ -3599,10 +3599,10 @@
         </is>
       </c>
       <c r="M42" t="n">
-        <v>-58.409579</v>
+        <v>-58.422315</v>
       </c>
       <c r="N42" t="n">
-        <v>-34.581134</v>
+        <v>-34.576988</v>
       </c>
       <c r="O42" t="inlineStr">
         <is>
@@ -3618,7 +3618,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>6230</t>
+          <t>6231</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
@@ -3628,7 +3628,7 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Santa maria de oro	2722</t>
+          <t>Ciudad de la Paz 275</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
@@ -3638,7 +3638,7 @@
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>807763066</t>
+          <t>807763070</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
@@ -3653,7 +3653,7 @@
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Aplomar o cambiar</t>
         </is>
       </c>
       <c r="I43" t="n">
@@ -3671,14 +3671,14 @@
       </c>
       <c r="L43" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M43" t="n">
-        <v>-58.422315</v>
+        <v>-58.441049</v>
       </c>
       <c r="N43" t="n">
-        <v>-34.576988</v>
+        <v>-34.574625</v>
       </c>
       <c r="O43" t="inlineStr">
         <is>
@@ -3694,7 +3694,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>6231</t>
+          <t>6235</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
@@ -3704,17 +3704,17 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Ciudad de la Paz 275</t>
+          <t>HUERGO 389</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>807763070</t>
+          <t>807763078</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
@@ -3729,7 +3729,7 @@
       </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t>Aplomar o cambiar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I44" t="n">
@@ -3747,14 +3747,14 @@
       </c>
       <c r="L44" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M44" t="n">
-        <v>-58.441049</v>
+        <v>-58.432722</v>
       </c>
       <c r="N44" t="n">
-        <v>-34.574625</v>
+        <v>-34.572371</v>
       </c>
       <c r="O44" t="inlineStr">
         <is>
@@ -3770,27 +3770,27 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>6235</t>
+          <t>6295</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>6/24/2025</t>
+          <t>6/30/2025</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>HUERGO 389</t>
+          <t>SOLER 6017</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>807763078</t>
+          <t>807851636</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
@@ -3827,10 +3827,10 @@
         </is>
       </c>
       <c r="M45" t="n">
-        <v>-58.432722</v>
+        <v>-58.436808</v>
       </c>
       <c r="N45" t="n">
-        <v>-34.572371</v>
+        <v>-34.577464</v>
       </c>
       <c r="O45" t="inlineStr">
         <is>
@@ -3846,17 +3846,17 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>6295</t>
+          <t>6331</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>6/30/2025</t>
+          <t>7/3/2025</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>SOLER 6017</t>
+          <t>PARAGUAY 4259</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
@@ -3866,7 +3866,7 @@
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>807851636</t>
+          <t>807965788</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
@@ -3903,10 +3903,10 @@
         </is>
       </c>
       <c r="M46" t="n">
-        <v>-58.436808</v>
+        <v>-58.421822</v>
       </c>
       <c r="N46" t="n">
-        <v>-34.577464</v>
+        <v>-34.58645</v>
       </c>
       <c r="O46" t="inlineStr">
         <is>
@@ -3922,7 +3922,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>6331</t>
+          <t>6332</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
@@ -3932,7 +3932,7 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>PARAGUAY 4259</t>
+          <t>ARAOZ 2560</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
@@ -3942,7 +3942,7 @@
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>807965788</t>
+          <t>807965818</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
@@ -3979,10 +3979,10 @@
         </is>
       </c>
       <c r="M47" t="n">
-        <v>-58.421822</v>
+        <v>-58.414507</v>
       </c>
       <c r="N47" t="n">
-        <v>-34.58645</v>
+        <v>-34.585377</v>
       </c>
       <c r="O47" t="inlineStr">
         <is>
@@ -3998,7 +3998,7 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>6332</t>
+          <t>6336</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
@@ -4008,7 +4008,7 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>ARAOZ 2560</t>
+          <t>PARAGUAY 4291</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
@@ -4018,7 +4018,7 @@
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>807965818</t>
+          <t>807965819</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
@@ -4055,10 +4055,10 @@
         </is>
       </c>
       <c r="M48" t="n">
-        <v>-58.414507</v>
+        <v>-58.422084</v>
       </c>
       <c r="N48" t="n">
-        <v>-34.585377</v>
+        <v>-34.58625</v>
       </c>
       <c r="O48" t="inlineStr">
         <is>
@@ -4074,7 +4074,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>6336</t>
+          <t>6337</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
@@ -4084,7 +4084,7 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>PARAGUAY 4291</t>
+          <t>PARAGUAY 4383</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
@@ -4094,7 +4094,7 @@
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>807965819</t>
+          <t>807965926</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
@@ -4131,10 +4131,10 @@
         </is>
       </c>
       <c r="M49" t="n">
-        <v>-58.422084</v>
+        <v>-58.422931</v>
       </c>
       <c r="N49" t="n">
-        <v>-34.58625</v>
+        <v>-34.585597</v>
       </c>
       <c r="O49" t="inlineStr">
         <is>
@@ -4150,27 +4150,27 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>6337</t>
+          <t>6363</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>7/3/2025</t>
+          <t>7/8/2025</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>PARAGUAY 4383</t>
+          <t>MOLDES 3730</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>807965926</t>
+          <t>808099415</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
@@ -4185,7 +4185,7 @@
       </c>
       <c r="H50" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Poste inclinado</t>
         </is>
       </c>
       <c r="I50" t="n">
@@ -4193,7 +4193,7 @@
       </c>
       <c r="J50" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K50" t="inlineStr">
@@ -4203,50 +4203,50 @@
       </c>
       <c r="L50" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M50" t="n">
-        <v>-58.422931</v>
+        <v>-58.47192</v>
       </c>
       <c r="N50" t="n">
-        <v>-34.585597</v>
+        <v>-34.549398</v>
       </c>
       <c r="O50" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P50" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>6363</t>
+          <t>-503</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>7/8/2025</t>
+          <t>7/10/2025</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>MOLDES 3730</t>
+          <t>Salguero 842</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>808099415</t>
+          <t>808148673</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
@@ -4261,7 +4261,7 @@
       </c>
       <c r="H51" t="inlineStr">
         <is>
-          <t>Poste inclinado</t>
+          <t>Cambiar columna picada en la base</t>
         </is>
       </c>
       <c r="I51" t="n">
@@ -4269,7 +4269,7 @@
       </c>
       <c r="J51" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K51" t="inlineStr">
@@ -4279,30 +4279,30 @@
       </c>
       <c r="L51" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M51" t="n">
-        <v>-58.47192</v>
+        <v>-58.419166</v>
       </c>
       <c r="N51" t="n">
-        <v>-34.549398</v>
+        <v>-34.600265</v>
       </c>
       <c r="O51" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P51" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>-503</t>
+          <t>-504</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
@@ -4312,17 +4312,17 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>Salguero 842</t>
+          <t>Ohiggins 1611</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>808148673</t>
+          <t>808148679</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
@@ -4337,7 +4337,7 @@
       </c>
       <c r="H52" t="inlineStr">
         <is>
-          <t>Cambiar columna picada en la base</t>
+          <t>Columna podrida en la base</t>
         </is>
       </c>
       <c r="I52" t="n">
@@ -4350,7 +4350,7 @@
       </c>
       <c r="K52" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L52" t="inlineStr">
@@ -4359,36 +4359,36 @@
         </is>
       </c>
       <c r="M52" t="n">
-        <v>-58.419166</v>
+        <v>-58.448993</v>
       </c>
       <c r="N52" t="n">
-        <v>-34.600265</v>
+        <v>-34.564383</v>
       </c>
       <c r="O52" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P52" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>-504</t>
+          <t>6392</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>7/10/2025</t>
+          <t>7/14/2025</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>Ohiggins 1611</t>
+          <t>MOLDES 1808</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
@@ -4398,7 +4398,7 @@
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>808148679</t>
+          <t>808194266</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
@@ -4413,7 +4413,7 @@
       </c>
       <c r="H53" t="inlineStr">
         <is>
-          <t>Columna podrida en la base</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I53" t="n">
@@ -4426,7 +4426,7 @@
       </c>
       <c r="K53" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L53" t="inlineStr">
@@ -4435,10 +4435,10 @@
         </is>
       </c>
       <c r="M53" t="n">
-        <v>-58.448993</v>
+        <v>-58.45719</v>
       </c>
       <c r="N53" t="n">
-        <v>-34.564383</v>
+        <v>-34.566365</v>
       </c>
       <c r="O53" t="inlineStr">
         <is>
@@ -4454,27 +4454,27 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>6392</t>
+          <t>6437</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>7/14/2025</t>
+          <t>7/17/2025</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>MOLDES 1808</t>
+          <t>MILLER 4590</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>808194266</t>
+          <t>808400306</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
@@ -4489,7 +4489,7 @@
       </c>
       <c r="H54" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Columna corroida</t>
         </is>
       </c>
       <c r="I54" t="n">
@@ -4511,14 +4511,14 @@
         </is>
       </c>
       <c r="M54" t="n">
-        <v>-58.45719</v>
+        <v>-58.495482</v>
       </c>
       <c r="N54" t="n">
-        <v>-34.566365</v>
+        <v>-34.552614</v>
       </c>
       <c r="O54" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P54" t="inlineStr">
@@ -4530,7 +4530,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>6437</t>
+          <t>6447</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
@@ -4540,17 +4540,17 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>MILLER 4590</t>
+          <t>CIUDAD DE LA PAZ 1535</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>808400306</t>
+          <t>808400333</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
@@ -4565,7 +4565,7 @@
       </c>
       <c r="H55" t="inlineStr">
         <is>
-          <t>Columna corroida</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I55" t="n">
@@ -4587,14 +4587,14 @@
         </is>
       </c>
       <c r="M55" t="n">
-        <v>-58.495482</v>
+        <v>-58.453124</v>
       </c>
       <c r="N55" t="n">
-        <v>-34.552614</v>
+        <v>-34.567382</v>
       </c>
       <c r="O55" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P55" t="inlineStr">
@@ -4606,7 +4606,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>6447</t>
+          <t>-519</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
@@ -4616,17 +4616,17 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>CIUDAD DE LA PAZ 1535</t>
+          <t>Vilela 2687</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>808400333</t>
+          <t>808400334</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
@@ -4641,7 +4641,7 @@
       </c>
       <c r="H56" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>CAmbiar columna 114 picada en base</t>
         </is>
       </c>
       <c r="I56" t="n">
@@ -4663,14 +4663,14 @@
         </is>
       </c>
       <c r="M56" t="n">
-        <v>-58.453124</v>
+        <v>-58.472968</v>
       </c>
       <c r="N56" t="n">
-        <v>-34.567382</v>
+        <v>-34.546898</v>
       </c>
       <c r="O56" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P56" t="inlineStr">
@@ -4682,7 +4682,7 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>-519</t>
+          <t>-520</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
@@ -4692,7 +4692,7 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>Vilela 2687</t>
+          <t>Pedraza Manuela 4101</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
@@ -4702,7 +4702,7 @@
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>808400334</t>
+          <t>808400353</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
@@ -4717,7 +4717,7 @@
       </c>
       <c r="H57" t="inlineStr">
         <is>
-          <t>CAmbiar columna 114 picada en base</t>
+          <t xml:space="preserve">Podrida en la base </t>
         </is>
       </c>
       <c r="I57" t="n">
@@ -4739,10 +4739,10 @@
         </is>
       </c>
       <c r="M57" t="n">
-        <v>-58.472968</v>
+        <v>-58.481569</v>
       </c>
       <c r="N57" t="n">
-        <v>-34.546898</v>
+        <v>-34.559853</v>
       </c>
       <c r="O57" t="inlineStr">
         <is>
@@ -4758,27 +4758,27 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>-520</t>
+          <t>-525</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>7/17/2025</t>
+          <t>7/22/2025</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>Pedraza Manuela 4101</t>
+          <t>Zabala 3567</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>808400353</t>
+          <t>808480549</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
@@ -4793,7 +4793,7 @@
       </c>
       <c r="H58" t="inlineStr">
         <is>
-          <t xml:space="preserve">Podrida en la base </t>
+          <t>Corroida en base para recambio</t>
         </is>
       </c>
       <c r="I58" t="n">
@@ -4815,14 +4815,14 @@
         </is>
       </c>
       <c r="M58" t="n">
-        <v>-58.481569</v>
+        <v>-58.457492</v>
       </c>
       <c r="N58" t="n">
-        <v>-34.559853</v>
+        <v>-34.579336</v>
       </c>
       <c r="O58" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P58" t="inlineStr">
@@ -4834,27 +4834,27 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>-525</t>
+          <t>-526</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>7/22/2025</t>
+          <t>7/23/2025</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>Zabala 3567</t>
+          <t>Moldes 1813</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>808480549</t>
+          <t>808488825</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
@@ -4869,7 +4869,7 @@
       </c>
       <c r="H59" t="inlineStr">
         <is>
-          <t>Corroida en base para recambio</t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I59" t="n">
@@ -4891,10 +4891,10 @@
         </is>
       </c>
       <c r="M59" t="n">
-        <v>-58.457492</v>
+        <v>-58.457145</v>
       </c>
       <c r="N59" t="n">
-        <v>-34.579336</v>
+        <v>-34.56629</v>
       </c>
       <c r="O59" t="inlineStr">
         <is>
@@ -4902,234 +4902,6 @@
         </is>
       </c>
       <c r="P59" t="inlineStr">
-        <is>
-          <t>Capital Norte</t>
-        </is>
-      </c>
-    </row>
-    <row r="60">
-      <c r="A60" t="inlineStr">
-        <is>
-          <t>-526</t>
-        </is>
-      </c>
-      <c r="B60" t="inlineStr">
-        <is>
-          <t>7/23/2025</t>
-        </is>
-      </c>
-      <c r="C60" t="inlineStr">
-        <is>
-          <t>Moldes 1813</t>
-        </is>
-      </c>
-      <c r="D60" t="inlineStr">
-        <is>
-          <t>13</t>
-        </is>
-      </c>
-      <c r="E60" t="inlineStr">
-        <is>
-          <t>808488825</t>
-        </is>
-      </c>
-      <c r="F60" t="inlineStr">
-        <is>
-          <t>NEW</t>
-        </is>
-      </c>
-      <c r="G60" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H60" t="inlineStr">
-        <is>
-          <t>Cambiar</t>
-        </is>
-      </c>
-      <c r="I60" t="n">
-        <v>1</v>
-      </c>
-      <c r="J60" t="inlineStr">
-        <is>
-          <t>Cambio</t>
-        </is>
-      </c>
-      <c r="K60" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L60" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
-      <c r="M60" t="n">
-        <v>-58.457145</v>
-      </c>
-      <c r="N60" t="n">
-        <v>-34.56629</v>
-      </c>
-      <c r="O60" t="inlineStr">
-        <is>
-          <t>Colegiales</t>
-        </is>
-      </c>
-      <c r="P60" t="inlineStr">
-        <is>
-          <t>Capital Norte</t>
-        </is>
-      </c>
-    </row>
-    <row r="61">
-      <c r="A61" t="inlineStr">
-        <is>
-          <t>-527</t>
-        </is>
-      </c>
-      <c r="B61" t="inlineStr">
-        <is>
-          <t>7/23/2025</t>
-        </is>
-      </c>
-      <c r="C61" t="inlineStr">
-        <is>
-          <t>Moldes 1761</t>
-        </is>
-      </c>
-      <c r="D61" t="inlineStr">
-        <is>
-          <t>13</t>
-        </is>
-      </c>
-      <c r="E61" t="inlineStr">
-        <is>
-          <t>808488822</t>
-        </is>
-      </c>
-      <c r="F61" t="inlineStr">
-        <is>
-          <t>NEW</t>
-        </is>
-      </c>
-      <c r="G61" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H61" t="inlineStr">
-        <is>
-          <t>Picada</t>
-        </is>
-      </c>
-      <c r="I61" t="n">
-        <v>1</v>
-      </c>
-      <c r="J61" t="inlineStr">
-        <is>
-          <t>Cambio</t>
-        </is>
-      </c>
-      <c r="K61" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L61" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
-      <c r="M61" t="n">
-        <v>-58.456734</v>
-      </c>
-      <c r="N61" t="n">
-        <v>-34.566768</v>
-      </c>
-      <c r="O61" t="inlineStr">
-        <is>
-          <t>Colegiales</t>
-        </is>
-      </c>
-      <c r="P61" t="inlineStr">
-        <is>
-          <t>Capital Norte</t>
-        </is>
-      </c>
-    </row>
-    <row r="62">
-      <c r="A62" t="inlineStr">
-        <is>
-          <t>-528</t>
-        </is>
-      </c>
-      <c r="B62" t="inlineStr">
-        <is>
-          <t>7/23/2025</t>
-        </is>
-      </c>
-      <c r="C62" t="inlineStr">
-        <is>
-          <t>Moldes 1743</t>
-        </is>
-      </c>
-      <c r="D62" t="inlineStr">
-        <is>
-          <t>13</t>
-        </is>
-      </c>
-      <c r="E62" t="inlineStr">
-        <is>
-          <t>808488806</t>
-        </is>
-      </c>
-      <c r="F62" t="inlineStr">
-        <is>
-          <t>NEW</t>
-        </is>
-      </c>
-      <c r="G62" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H62" t="inlineStr">
-        <is>
-          <t>Picada</t>
-        </is>
-      </c>
-      <c r="I62" t="n">
-        <v>1</v>
-      </c>
-      <c r="J62" t="inlineStr">
-        <is>
-          <t>Cambio</t>
-        </is>
-      </c>
-      <c r="K62" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L62" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
-      <c r="M62" t="n">
-        <v>-58.456563</v>
-      </c>
-      <c r="N62" t="n">
-        <v>-34.566967</v>
-      </c>
-      <c r="O62" t="inlineStr">
-        <is>
-          <t>Colegiales</t>
-        </is>
-      </c>
-      <c r="P62" t="inlineStr">
         <is>
           <t>Capital Norte</t>
         </is>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-07-24 06:58:08)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_NEW.xlsx
+++ b/mapa_interactivo_NEW.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P59"/>
+  <dimension ref="A1:P58"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4831,82 +4831,6 @@
         </is>
       </c>
     </row>
-    <row r="59">
-      <c r="A59" t="inlineStr">
-        <is>
-          <t>-526</t>
-        </is>
-      </c>
-      <c r="B59" t="inlineStr">
-        <is>
-          <t>7/23/2025</t>
-        </is>
-      </c>
-      <c r="C59" t="inlineStr">
-        <is>
-          <t>Moldes 1813</t>
-        </is>
-      </c>
-      <c r="D59" t="inlineStr">
-        <is>
-          <t>13</t>
-        </is>
-      </c>
-      <c r="E59" t="inlineStr">
-        <is>
-          <t>808488825</t>
-        </is>
-      </c>
-      <c r="F59" t="inlineStr">
-        <is>
-          <t>NEW</t>
-        </is>
-      </c>
-      <c r="G59" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H59" t="inlineStr">
-        <is>
-          <t>Cambiar</t>
-        </is>
-      </c>
-      <c r="I59" t="n">
-        <v>1</v>
-      </c>
-      <c r="J59" t="inlineStr">
-        <is>
-          <t>Cambio</t>
-        </is>
-      </c>
-      <c r="K59" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L59" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
-      <c r="M59" t="n">
-        <v>-58.457145</v>
-      </c>
-      <c r="N59" t="n">
-        <v>-34.56629</v>
-      </c>
-      <c r="O59" t="inlineStr">
-        <is>
-          <t>Colegiales</t>
-        </is>
-      </c>
-      <c r="P59" t="inlineStr">
-        <is>
-          <t>Capital Norte</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-07-24 10:12:02)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_NEW.xlsx
+++ b/mapa_interactivo_NEW.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P58"/>
+  <dimension ref="A1:P57"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4378,27 +4378,27 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>6392</t>
+          <t>6437</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>7/14/2025</t>
+          <t>7/17/2025</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>MOLDES 1808</t>
+          <t>MILLER 4590</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>808194266</t>
+          <t>808400306</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
@@ -4413,7 +4413,7 @@
       </c>
       <c r="H53" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Columna corroida</t>
         </is>
       </c>
       <c r="I53" t="n">
@@ -4435,14 +4435,14 @@
         </is>
       </c>
       <c r="M53" t="n">
-        <v>-58.45719</v>
+        <v>-58.495482</v>
       </c>
       <c r="N53" t="n">
-        <v>-34.566365</v>
+        <v>-34.552614</v>
       </c>
       <c r="O53" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P53" t="inlineStr">
@@ -4454,7 +4454,7 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>6437</t>
+          <t>6447</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
@@ -4464,17 +4464,17 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>MILLER 4590</t>
+          <t>CIUDAD DE LA PAZ 1535</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>808400306</t>
+          <t>808400333</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
@@ -4489,7 +4489,7 @@
       </c>
       <c r="H54" t="inlineStr">
         <is>
-          <t>Columna corroida</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I54" t="n">
@@ -4511,14 +4511,14 @@
         </is>
       </c>
       <c r="M54" t="n">
-        <v>-58.495482</v>
+        <v>-58.453124</v>
       </c>
       <c r="N54" t="n">
-        <v>-34.552614</v>
+        <v>-34.567382</v>
       </c>
       <c r="O54" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P54" t="inlineStr">
@@ -4530,7 +4530,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>6447</t>
+          <t>-519</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
@@ -4540,17 +4540,17 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>CIUDAD DE LA PAZ 1535</t>
+          <t>Vilela 2687</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>808400333</t>
+          <t>808400334</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
@@ -4565,7 +4565,7 @@
       </c>
       <c r="H55" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>CAmbiar columna 114 picada en base</t>
         </is>
       </c>
       <c r="I55" t="n">
@@ -4587,14 +4587,14 @@
         </is>
       </c>
       <c r="M55" t="n">
-        <v>-58.453124</v>
+        <v>-58.472968</v>
       </c>
       <c r="N55" t="n">
-        <v>-34.567382</v>
+        <v>-34.546898</v>
       </c>
       <c r="O55" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P55" t="inlineStr">
@@ -4606,7 +4606,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>-519</t>
+          <t>-520</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
@@ -4616,7 +4616,7 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>Vilela 2687</t>
+          <t>Pedraza Manuela 4101</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
@@ -4626,7 +4626,7 @@
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>808400334</t>
+          <t>808400353</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
@@ -4641,7 +4641,7 @@
       </c>
       <c r="H56" t="inlineStr">
         <is>
-          <t>CAmbiar columna 114 picada en base</t>
+          <t xml:space="preserve">Podrida en la base </t>
         </is>
       </c>
       <c r="I56" t="n">
@@ -4663,10 +4663,10 @@
         </is>
       </c>
       <c r="M56" t="n">
-        <v>-58.472968</v>
+        <v>-58.481569</v>
       </c>
       <c r="N56" t="n">
-        <v>-34.546898</v>
+        <v>-34.559853</v>
       </c>
       <c r="O56" t="inlineStr">
         <is>
@@ -4682,27 +4682,27 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>-520</t>
+          <t>-525</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>7/17/2025</t>
+          <t>7/22/2025</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>Pedraza Manuela 4101</t>
+          <t>Zabala 3567</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>808400353</t>
+          <t>808480549</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
@@ -4717,7 +4717,7 @@
       </c>
       <c r="H57" t="inlineStr">
         <is>
-          <t xml:space="preserve">Podrida en la base </t>
+          <t>Corroida en base para recambio</t>
         </is>
       </c>
       <c r="I57" t="n">
@@ -4739,93 +4739,17 @@
         </is>
       </c>
       <c r="M57" t="n">
-        <v>-58.481569</v>
+        <v>-58.457492</v>
       </c>
       <c r="N57" t="n">
-        <v>-34.559853</v>
+        <v>-34.579336</v>
       </c>
       <c r="O57" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P57" t="inlineStr">
-        <is>
-          <t>Capital Norte</t>
-        </is>
-      </c>
-    </row>
-    <row r="58">
-      <c r="A58" t="inlineStr">
-        <is>
-          <t>-525</t>
-        </is>
-      </c>
-      <c r="B58" t="inlineStr">
-        <is>
-          <t>7/22/2025</t>
-        </is>
-      </c>
-      <c r="C58" t="inlineStr">
-        <is>
-          <t>Zabala 3567</t>
-        </is>
-      </c>
-      <c r="D58" t="inlineStr">
-        <is>
-          <t>15</t>
-        </is>
-      </c>
-      <c r="E58" t="inlineStr">
-        <is>
-          <t>808480549</t>
-        </is>
-      </c>
-      <c r="F58" t="inlineStr">
-        <is>
-          <t>NEW</t>
-        </is>
-      </c>
-      <c r="G58" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H58" t="inlineStr">
-        <is>
-          <t>Corroida en base para recambio</t>
-        </is>
-      </c>
-      <c r="I58" t="n">
-        <v>1</v>
-      </c>
-      <c r="J58" t="inlineStr">
-        <is>
-          <t>Cambio</t>
-        </is>
-      </c>
-      <c r="K58" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L58" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
-      <c r="M58" t="n">
-        <v>-58.457492</v>
-      </c>
-      <c r="N58" t="n">
-        <v>-34.579336</v>
-      </c>
-      <c r="O58" t="inlineStr">
-        <is>
-          <t>Colegiales</t>
-        </is>
-      </c>
-      <c r="P58" t="inlineStr">
         <is>
           <t>Capital Norte</t>
         </is>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-07-24 12:17:17)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_NEW.xlsx
+++ b/mapa_interactivo_NEW.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P57"/>
+  <dimension ref="A1:P58"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4755,6 +4755,82 @@
         </is>
       </c>
     </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>6484</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>7/24/2025</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>URIARTE 2396</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>14</t>
+        </is>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>808509373</t>
+        </is>
+      </c>
+      <c r="F58" t="inlineStr">
+        <is>
+          <t>NEW</t>
+        </is>
+      </c>
+      <c r="G58" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H58" t="inlineStr">
+        <is>
+          <t>Picada</t>
+        </is>
+      </c>
+      <c r="I58" t="n">
+        <v>1</v>
+      </c>
+      <c r="J58" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K58" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L58" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M58" t="n">
+        <v>-58.423934</v>
+      </c>
+      <c r="N58" t="n">
+        <v>-34.581562</v>
+      </c>
+      <c r="O58" t="inlineStr">
+        <is>
+          <t>Palermo</t>
+        </is>
+      </c>
+      <c r="P58" t="inlineStr">
+        <is>
+          <t>Capital Sur</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-07-25 11:59:38)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_NEW.xlsx
+++ b/mapa_interactivo_NEW.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P58"/>
+  <dimension ref="A1:P62"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -746,27 +746,27 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>5589</t>
+          <t>801645368</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>12/31/2023</t>
+          <t>12/13/2024</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>ARCOS 1520</t>
+          <t>San Blas 1809</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>799540526</t>
+          <t>801645368</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -776,7 +776,7 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
+          <t>Pendiente</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
@@ -787,22 +787,30 @@
       <c r="I5" t="n">
         <v>0</v>
       </c>
-      <c r="J5" t="inlineStr"/>
-      <c r="K5" t="inlineStr"/>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
       <c r="L5" t="inlineStr">
         <is>
           <t>Pasante</t>
         </is>
       </c>
       <c r="M5" t="n">
-        <v>-58.449125</v>
+        <v>-58.467767</v>
       </c>
       <c r="N5" t="n">
-        <v>-34.565958</v>
+        <v>-34.604588</v>
       </c>
       <c r="O5" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P5" t="inlineStr">
@@ -814,17 +822,17 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>4595</t>
+          <t>5589</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>1/15/2025</t>
+          <t>12/31/2023</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>PAROISSIEN 1806</t>
+          <t>ARCOS 1520</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -834,7 +842,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>802747617</t>
+          <t>799540526</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -844,41 +852,33 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>Aplomar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I6" t="n">
-        <v>1</v>
-      </c>
-      <c r="J6" t="inlineStr">
-        <is>
-          <t>Aplomo</t>
-        </is>
-      </c>
-      <c r="K6" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="J6" t="inlineStr"/>
+      <c r="K6" t="inlineStr"/>
       <c r="L6" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M6" t="n">
-        <v>-58.464172</v>
+        <v>-58.449125</v>
       </c>
       <c r="N6" t="n">
-        <v>-34.543845</v>
+        <v>-34.565958</v>
       </c>
       <c r="O6" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P6" t="inlineStr">
@@ -890,27 +890,27 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>4662</t>
+          <t>4595</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>1/21/2025</t>
+          <t>1/15/2025</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>ALTOLAGUIRRE 2397</t>
+          <t>PAROISSIEN 1806</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>802823938</t>
+          <t>802747617</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -925,7 +925,7 @@
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>Inclinada</t>
+          <t>Aplomar</t>
         </is>
       </c>
       <c r="I7" t="n">
@@ -943,18 +943,18 @@
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M7" t="n">
-        <v>-58.490766</v>
+        <v>-58.464172</v>
       </c>
       <c r="N7" t="n">
-        <v>-34.576987</v>
+        <v>-34.543845</v>
       </c>
       <c r="O7" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P7" t="inlineStr">
@@ -966,27 +966,27 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>4862</t>
+          <t>4662</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>1/23/2025</t>
+          <t>1/21/2025</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>ARCOS 2263</t>
+          <t>ALTOLAGUIRRE 2397</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>802857379</t>
+          <t>802823938</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -996,25 +996,25 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
+          <t>Pendiente</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>picada</t>
+          <t>Inclinada</t>
         </is>
       </c>
       <c r="I8" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L8" t="inlineStr">
@@ -1023,14 +1023,14 @@
         </is>
       </c>
       <c r="M8" t="n">
-        <v>-58.455082</v>
+        <v>-58.490766</v>
       </c>
       <c r="N8" t="n">
-        <v>-34.558883</v>
+        <v>-34.576987</v>
       </c>
       <c r="O8" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P8" t="inlineStr">
@@ -1042,27 +1042,27 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>6036</t>
+          <t>4862</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>2/24/2025</t>
+          <t>1/23/2025</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>MEDRANO 1715</t>
+          <t>ARCOS 2263</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>803608181</t>
+          <t>802857379</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -1072,10 +1072,14 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H9" t="inlineStr"/>
+          <t>Pendiente de Traspaso PROPIO</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>picada</t>
+        </is>
+      </c>
       <c r="I9" t="n">
         <v>0</v>
       </c>
@@ -1095,46 +1099,46 @@
         </is>
       </c>
       <c r="M9" t="n">
-        <v>-58.418236</v>
+        <v>-58.455082</v>
       </c>
       <c r="N9" t="n">
-        <v>-34.589859</v>
+        <v>-34.558883</v>
       </c>
       <c r="O9" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P9" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>5037</t>
+          <t>6036</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>3/7/2025</t>
+          <t>2/24/2025</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Monroe 3605</t>
+          <t>MEDRANO 1715</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>803825082</t>
+          <t>803608181</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
@@ -1147,22 +1151,18 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H10" t="inlineStr">
-        <is>
-          <t>Columna inclinada</t>
-        </is>
-      </c>
+      <c r="H10" t="inlineStr"/>
       <c r="I10" t="n">
         <v>0</v>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L10" t="inlineStr">
@@ -1171,46 +1171,46 @@
         </is>
       </c>
       <c r="M10" t="n">
-        <v>-58.471774</v>
+        <v>-58.418236</v>
       </c>
       <c r="N10" t="n">
-        <v>-34.565411</v>
+        <v>-34.589859</v>
       </c>
       <c r="O10" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P10" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>5053</t>
+          <t>803608480</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>3/11/2025</t>
+          <t>2/24/2025</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>MENDOZA 1153</t>
+          <t>GUATEMALA /ALT/ 4415</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>803969314</t>
+          <t>803608480</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
@@ -1225,7 +1225,7 @@
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t xml:space="preserve">Guatemala 4415 </t>
         </is>
       </c>
       <c r="I11" t="n">
@@ -1243,50 +1243,50 @@
       </c>
       <c r="L11" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M11" t="n">
-        <v>-58.44463</v>
+        <v>-58.421661</v>
       </c>
       <c r="N11" t="n">
-        <v>-34.553354</v>
+        <v>-34.588428</v>
       </c>
       <c r="O11" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P11" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>6071</t>
+          <t>5037</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>3/17/2025</t>
+          <t>3/7/2025</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>OSORIO 4994</t>
+          <t>Monroe 3605</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>804053324</t>
+          <t>803825082</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
@@ -1299,13 +1299,17 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H12" t="inlineStr"/>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>Columna inclinada</t>
+        </is>
+      </c>
       <c r="I12" t="n">
         <v>0</v>
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K12" t="inlineStr">
@@ -1319,14 +1323,14 @@
         </is>
       </c>
       <c r="M12" t="n">
-        <v>-58.466241</v>
+        <v>-58.471774</v>
       </c>
       <c r="N12" t="n">
-        <v>-34.595741</v>
+        <v>-34.565411</v>
       </c>
       <c r="O12" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P12" t="inlineStr">
@@ -1338,27 +1342,27 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>3348</t>
+          <t>5053</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>3/27/2025</t>
+          <t>3/11/2025</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>ESTOMBA 2626</t>
+          <t>MENDOZA 1153</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>804309704</t>
+          <t>803969314</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
@@ -1373,15 +1377,15 @@
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="I13" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>Desmonte</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K13" t="inlineStr">
@@ -1391,18 +1395,18 @@
       </c>
       <c r="L13" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M13" t="n">
-        <v>-58.47538</v>
+        <v>-58.44463</v>
       </c>
       <c r="N13" t="n">
-        <v>-34.566015</v>
+        <v>-34.553354</v>
       </c>
       <c r="O13" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P13" t="inlineStr">
@@ -1414,27 +1418,27 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>-312</t>
+          <t>6071</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>3/29/2025</t>
+          <t>3/17/2025</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>MATIENZO BENJAMIN /ALT/ 1831</t>
+          <t>OSORIO 4994</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>804333522</t>
+          <t>804053324</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
@@ -1447,11 +1451,7 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H14" t="inlineStr">
-        <is>
-          <t>Retirar columna ya traspasaron el nodo</t>
-        </is>
-      </c>
+      <c r="H14" t="inlineStr"/>
       <c r="I14" t="n">
         <v>0</v>
       </c>
@@ -1462,7 +1462,7 @@
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L14" t="inlineStr">
@@ -1471,36 +1471,36 @@
         </is>
       </c>
       <c r="M14" t="n">
-        <v>-58.434835</v>
+        <v>-58.466241</v>
       </c>
       <c r="N14" t="n">
-        <v>-34.569129</v>
+        <v>-34.595741</v>
       </c>
       <c r="O14" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P14" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>3430</t>
+          <t>3348</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>4/1/2025</t>
+          <t>3/27/2025</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>MONROE 3838</t>
+          <t>ESTOMBA 2626</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -1510,7 +1510,7 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>804468442</t>
+          <t>804309704</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
@@ -1525,7 +1525,7 @@
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>Reparar rienda</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I15" t="n">
@@ -1533,7 +1533,7 @@
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>Tensor</t>
+          <t>Desmonte</t>
         </is>
       </c>
       <c r="K15" t="inlineStr">
@@ -1543,14 +1543,14 @@
       </c>
       <c r="L15" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M15" t="n">
-        <v>-58.473659</v>
+        <v>-58.47538</v>
       </c>
       <c r="N15" t="n">
-        <v>-34.566979</v>
+        <v>-34.566015</v>
       </c>
       <c r="O15" t="inlineStr">
         <is>
@@ -1566,27 +1566,27 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>5464</t>
+          <t>-312</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>4/4/2025</t>
+          <t>3/29/2025</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>SUCRE, ANTONIO JOSE DE, MCAL. 3100</t>
+          <t>MATIENZO BENJAMIN /ALT/ 1831</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>804497880</t>
+          <t>804333522</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
@@ -1601,11 +1601,11 @@
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Retirar columna ya traspasaron el nodo</t>
         </is>
       </c>
       <c r="I16" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J16" t="inlineStr">
         <is>
@@ -1614,45 +1614,45 @@
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L16" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M16" t="n">
-        <v>-58.46161</v>
+        <v>-58.434835</v>
       </c>
       <c r="N16" t="n">
-        <v>-34.567849</v>
+        <v>-34.569129</v>
       </c>
       <c r="O16" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P16" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>5469</t>
+          <t>3430</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>4/4/2025</t>
+          <t>4/1/2025</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>ESTADO PLURINACIONAL DE BOLIVIA 5899</t>
+          <t>MONROE 3838</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
@@ -1662,7 +1662,7 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>804497887</t>
+          <t>804468442</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
@@ -1677,7 +1677,7 @@
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>Aplomar</t>
+          <t>Reparar rienda</t>
         </is>
       </c>
       <c r="I17" t="n">
@@ -1685,7 +1685,7 @@
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Tensor</t>
         </is>
       </c>
       <c r="K17" t="inlineStr">
@@ -1699,14 +1699,14 @@
         </is>
       </c>
       <c r="M17" t="n">
-        <v>-58.507746</v>
+        <v>-58.473659</v>
       </c>
       <c r="N17" t="n">
-        <v>-34.574217</v>
+        <v>-34.566979</v>
       </c>
       <c r="O17" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P17" t="inlineStr">
@@ -1718,7 +1718,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>5492</t>
+          <t>5464</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -1728,17 +1728,17 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>ESTADO PLURINACIONAL DE BOLIVIA 5920</t>
+          <t>SUCRE, ANTONIO JOSE DE, MCAL. 3100</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>804498035</t>
+          <t>804497880</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
@@ -1753,7 +1753,7 @@
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>aplomar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I18" t="n">
@@ -1761,7 +1761,7 @@
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K18" t="inlineStr">
@@ -1775,14 +1775,14 @@
         </is>
       </c>
       <c r="M18" t="n">
-        <v>-58.50751</v>
+        <v>-58.46161</v>
       </c>
       <c r="N18" t="n">
-        <v>-34.574543</v>
+        <v>-34.567849</v>
       </c>
       <c r="O18" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P18" t="inlineStr">
@@ -1794,17 +1794,17 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>5599</t>
+          <t>5469</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>4/15/2025</t>
+          <t>4/4/2025</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>ESTOMBA 4052</t>
+          <t>ESTADO PLURINACIONAL DE BOLIVIA 5899</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
@@ -1814,7 +1814,7 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>804732246</t>
+          <t>804497887</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
@@ -1829,7 +1829,7 @@
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>Columna PRFV quedo inclinada (la hicieron como estomba 4056)</t>
+          <t>Aplomar</t>
         </is>
       </c>
       <c r="I19" t="n">
@@ -1842,23 +1842,23 @@
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>Nodo TLC</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L19" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M19" t="n">
-        <v>-58.485407</v>
+        <v>-58.507746</v>
       </c>
       <c r="N19" t="n">
-        <v>-34.552985</v>
+        <v>-34.574217</v>
       </c>
       <c r="O19" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P19" t="inlineStr">
@@ -1870,27 +1870,27 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>5590</t>
+          <t>5492</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>4/15/2025</t>
+          <t>4/4/2025</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>O'HIGGINS 2441</t>
+          <t>ESTADO PLURINACIONAL DE BOLIVIA 5920</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>804732275</t>
+          <t>804498035</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
@@ -1905,7 +1905,7 @@
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>aplomar</t>
         </is>
       </c>
       <c r="I20" t="n">
@@ -1913,7 +1913,7 @@
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K20" t="inlineStr">
@@ -1923,18 +1923,18 @@
       </c>
       <c r="L20" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M20" t="n">
-        <v>-58.45573</v>
+        <v>-58.50751</v>
       </c>
       <c r="N20" t="n">
-        <v>-34.556576</v>
+        <v>-34.574543</v>
       </c>
       <c r="O20" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P20" t="inlineStr">
@@ -1946,27 +1946,27 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>5624</t>
+          <t>5599</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>4/22/2025</t>
+          <t>4/15/2025</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>PINO, VIRREY DEL 3456</t>
+          <t>ESTOMBA 4052</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>804876043</t>
+          <t>804732246</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
@@ -1981,7 +1981,7 @@
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>Desmonte de poste</t>
+          <t>Columna PRFV quedo inclinada (la hicieron como estomba 4056)</t>
         </is>
       </c>
       <c r="I21" t="n">
@@ -1989,28 +1989,28 @@
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>Desmonte</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo TLC</t>
         </is>
       </c>
       <c r="L21" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M21" t="n">
-        <v>-58.464354</v>
+        <v>-58.485407</v>
       </c>
       <c r="N21" t="n">
-        <v>-34.572486</v>
+        <v>-34.552985</v>
       </c>
       <c r="O21" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P21" t="inlineStr">
@@ -2022,17 +2022,17 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>804922147</t>
+          <t>5590</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>4/24/2025</t>
+          <t>4/15/2025</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Av. Álvarez Thomas 1171</t>
+          <t>O'HIGGINS 2441</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
@@ -2042,7 +2042,7 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>804922147</t>
+          <t>804732275</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
@@ -2061,7 +2061,7 @@
         </is>
       </c>
       <c r="I22" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J22" t="inlineStr">
         <is>
@@ -2079,14 +2079,14 @@
         </is>
       </c>
       <c r="M22" t="n">
-        <v>-58.45793</v>
+        <v>-58.45573</v>
       </c>
       <c r="N22" t="n">
-        <v>-34.578334</v>
+        <v>-34.556576</v>
       </c>
       <c r="O22" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P22" t="inlineStr">
@@ -2098,27 +2098,27 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>804922171</t>
+          <t>804787368</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>4/24/2025</t>
+          <t>4/17/2025</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Virrey Arredondo 3581</t>
+          <t>San Blas 2591</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>804922171</t>
+          <t>804787368</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
@@ -2133,7 +2133,7 @@
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>Aplomar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I23" t="n">
@@ -2141,7 +2141,7 @@
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K23" t="inlineStr">
@@ -2151,18 +2151,18 @@
       </c>
       <c r="L23" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M23" t="n">
-        <v>-58.459513</v>
+        <v>-58.477427</v>
       </c>
       <c r="N23" t="n">
-        <v>-34.578019</v>
+        <v>-34.609261</v>
       </c>
       <c r="O23" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P23" t="inlineStr">
@@ -2174,27 +2174,27 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>5656</t>
+          <t>5624</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>4/24/2025</t>
+          <t>4/22/2025</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>ECHEVERRIA 5893</t>
+          <t>PINO, VIRREY DEL 3456</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>804922184</t>
+          <t>804876043</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
@@ -2209,7 +2209,7 @@
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>Poste con base quebrada</t>
+          <t>Desmonte de poste</t>
         </is>
       </c>
       <c r="I24" t="n">
@@ -2231,14 +2231,14 @@
         </is>
       </c>
       <c r="M24" t="n">
-        <v>-58.489627</v>
+        <v>-58.464354</v>
       </c>
       <c r="N24" t="n">
-        <v>-34.583761</v>
+        <v>-34.572486</v>
       </c>
       <c r="O24" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P24" t="inlineStr">
@@ -2250,27 +2250,27 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>6173</t>
+          <t>804922147</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>4/29/2025</t>
+          <t>4/24/2025</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>ARMENIA 2321</t>
+          <t>Av. Álvarez Thomas 1171</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>805507398</t>
+          <t>804922147</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
@@ -2285,11 +2285,11 @@
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>Picada volvio a entrar como caso 6325</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I25" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J25" t="inlineStr">
         <is>
@@ -2307,46 +2307,46 @@
         </is>
       </c>
       <c r="M25" t="n">
-        <v>-58.420549</v>
+        <v>-58.45793</v>
       </c>
       <c r="N25" t="n">
-        <v>-34.585103</v>
+        <v>-34.578334</v>
       </c>
       <c r="O25" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P25" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>5715</t>
+          <t>804922171</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>5/1/2025</t>
+          <t>4/24/2025</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>CUENCA 4690</t>
+          <t>Virrey Arredondo 3581</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>805579094</t>
+          <t>804922171</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
@@ -2361,7 +2361,7 @@
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>Aplomar poste</t>
+          <t>Aplomar</t>
         </is>
       </c>
       <c r="I26" t="n">
@@ -2379,18 +2379,18 @@
       </c>
       <c r="L26" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M26" t="n">
-        <v>-58.506061</v>
+        <v>-58.459513</v>
       </c>
       <c r="N26" t="n">
-        <v>-34.588887</v>
+        <v>-34.578019</v>
       </c>
       <c r="O26" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P26" t="inlineStr">
@@ -2402,17 +2402,17 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>5719</t>
+          <t>5656</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>5/1/2025</t>
+          <t>4/24/2025</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>CABEZON, JOSE LEON 2440</t>
+          <t>ECHEVERRIA 5893</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
@@ -2422,7 +2422,7 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>805579157</t>
+          <t>804922184</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
@@ -2437,7 +2437,7 @@
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Poste con base quebrada</t>
         </is>
       </c>
       <c r="I27" t="n">
@@ -2445,7 +2445,7 @@
       </c>
       <c r="J27" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Desmonte</t>
         </is>
       </c>
       <c r="K27" t="inlineStr">
@@ -2455,14 +2455,14 @@
       </c>
       <c r="L27" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M27" t="n">
-        <v>-58.499967</v>
+        <v>-58.489627</v>
       </c>
       <c r="N27" t="n">
-        <v>-34.57974</v>
+        <v>-34.583761</v>
       </c>
       <c r="O27" t="inlineStr">
         <is>
@@ -2478,17 +2478,17 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>6333</t>
+          <t>804922192</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>5/1/2025</t>
+          <t>4/24/2025</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>ORTEGA Y GASSET 1816</t>
+          <t>Paraguay 4657</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
@@ -2498,7 +2498,7 @@
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>805655342</t>
+          <t>804922192</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
@@ -2535,10 +2535,10 @@
         </is>
       </c>
       <c r="M28" t="n">
-        <v>-58.432556</v>
+        <v>-58.425642</v>
       </c>
       <c r="N28" t="n">
-        <v>-34.570279</v>
+        <v>-34.583525</v>
       </c>
       <c r="O28" t="inlineStr">
         <is>
@@ -2554,17 +2554,17 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>805707165</t>
+          <t>6173</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>5/7/2025</t>
+          <t>4/29/2025</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Baez 793</t>
+          <t>ARMENIA 2321</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
@@ -2574,7 +2574,7 @@
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>805707165</t>
+          <t>805507398</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
@@ -2589,7 +2589,7 @@
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>DESMONTAR COLUMNA DE 7 MTS Y TRANSFERIR A COMUNITARIA</t>
+          <t>Picada volvio a entrar como caso 6325</t>
         </is>
       </c>
       <c r="I29" t="n">
@@ -2607,14 +2607,14 @@
       </c>
       <c r="L29" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M29" t="n">
-        <v>-58.436165</v>
+        <v>-58.420549</v>
       </c>
       <c r="N29" t="n">
-        <v>-34.569081</v>
+        <v>-34.585103</v>
       </c>
       <c r="O29" t="inlineStr">
         <is>
@@ -2630,17 +2630,17 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>5847</t>
+          <t>5715</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>5/8/2025</t>
+          <t>5/1/2025</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>JURAMENTO 5321</t>
+          <t>CUENCA 4690</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
@@ -2650,7 +2650,7 @@
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>805791839</t>
+          <t>805579094</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
@@ -2665,7 +2665,7 @@
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Aplomar poste</t>
         </is>
       </c>
       <c r="I30" t="n">
@@ -2673,7 +2673,7 @@
       </c>
       <c r="J30" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K30" t="inlineStr">
@@ -2683,14 +2683,14 @@
       </c>
       <c r="L30" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M30" t="n">
-        <v>-58.485193</v>
+        <v>-58.506061</v>
       </c>
       <c r="N30" t="n">
-        <v>-34.579621</v>
+        <v>-34.588887</v>
       </c>
       <c r="O30" t="inlineStr">
         <is>
@@ -2706,27 +2706,27 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>232</t>
+          <t>5719</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>5/9/2025</t>
+          <t>5/1/2025</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Gorostiaga 2286</t>
+          <t>CABEZON, JOSE LEON 2440</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>805791858</t>
+          <t>805579157</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
@@ -2763,46 +2763,46 @@
         </is>
       </c>
       <c r="M31" t="n">
-        <v>-58.441563</v>
+        <v>-58.499967</v>
       </c>
       <c r="N31" t="n">
-        <v>-34.569743</v>
+        <v>-34.57974</v>
       </c>
       <c r="O31" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P31" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>5826</t>
+          <t>6333</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>5/19/2025</t>
+          <t>5/1/2025</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>ALBARELLOS AV. 3180</t>
+          <t>ORTEGA Y GASSET 1816</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>806926466</t>
+          <t>805655342</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
@@ -2817,7 +2817,7 @@
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>Columna (metal) inclinada</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I32" t="n">
@@ -2825,7 +2825,7 @@
       </c>
       <c r="J32" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K32" t="inlineStr">
@@ -2835,50 +2835,50 @@
       </c>
       <c r="L32" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M32" t="n">
-        <v>-58.513552</v>
+        <v>-58.432556</v>
       </c>
       <c r="N32" t="n">
-        <v>-34.579829</v>
+        <v>-34.570279</v>
       </c>
       <c r="O32" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P32" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>5825</t>
+          <t>805707165</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>5/19/2025</t>
+          <t>5/7/2025</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>PAZ, GRAL. AV. 5602</t>
+          <t>Baez 793</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>806926472</t>
+          <t>805707165</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
@@ -2893,7 +2893,7 @@
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>reparar rienda cortada - ver foto no es la misma que albarellos</t>
+          <t>DESMONTAR COLUMNA DE 7 MTS Y TRANSFERIR A COMUNITARIA</t>
         </is>
       </c>
       <c r="I33" t="n">
@@ -2901,7 +2901,7 @@
       </c>
       <c r="J33" t="inlineStr">
         <is>
-          <t>Tensor</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K33" t="inlineStr">
@@ -2915,36 +2915,36 @@
         </is>
       </c>
       <c r="M33" t="n">
-        <v>-58.513685</v>
+        <v>-58.436165</v>
       </c>
       <c r="N33" t="n">
-        <v>-34.579838</v>
+        <v>-34.569081</v>
       </c>
       <c r="O33" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P33" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>5875</t>
+          <t>5847</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>5/27/2025</t>
+          <t>5/8/2025</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>MONROE 4096</t>
+          <t>JURAMENTO 5321</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
@@ -2954,7 +2954,7 @@
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>806975680</t>
+          <t>805791839</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
@@ -2991,14 +2991,14 @@
         </is>
       </c>
       <c r="M34" t="n">
-        <v>-58.476106</v>
+        <v>-58.485193</v>
       </c>
       <c r="N34" t="n">
-        <v>-34.568373</v>
+        <v>-34.579621</v>
       </c>
       <c r="O34" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P34" t="inlineStr">
@@ -3010,27 +3010,27 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>807044192</t>
+          <t>232</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>5/29/2025</t>
+          <t>5/9/2025</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>O'Higgins 4379</t>
+          <t>Gorostiaga 2286</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>807044192</t>
+          <t>805791858</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
@@ -3045,7 +3045,7 @@
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t xml:space="preserve">Poste </t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I35" t="n">
@@ -3053,7 +3053,7 @@
       </c>
       <c r="J35" t="inlineStr">
         <is>
-          <t>Desmonte</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K35" t="inlineStr">
@@ -3063,50 +3063,50 @@
       </c>
       <c r="L35" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M35" t="n">
-        <v>-58.468425</v>
+        <v>-58.441563</v>
       </c>
       <c r="N35" t="n">
-        <v>-34.54124</v>
+        <v>-34.569743</v>
       </c>
       <c r="O35" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P35" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>6020</t>
+          <t>5826</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>6/5/2025</t>
+          <t>5/19/2025</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>RAVIGNANI, EMILIO, DR. 2036</t>
+          <t>ALBARELLOS AV. 3180</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>807215465</t>
+          <t>806926466</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
@@ -3121,7 +3121,7 @@
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Columna (metal) inclinada</t>
         </is>
       </c>
       <c r="I36" t="n">
@@ -3129,7 +3129,7 @@
       </c>
       <c r="J36" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K36" t="inlineStr">
@@ -3139,50 +3139,50 @@
       </c>
       <c r="L36" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M36" t="n">
-        <v>-58.436298</v>
+        <v>-58.513552</v>
       </c>
       <c r="N36" t="n">
-        <v>-34.578972</v>
+        <v>-34.579829</v>
       </c>
       <c r="O36" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P36" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>6144</t>
+          <t>5825</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>6/11/2025</t>
+          <t>5/19/2025</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>TURIN 2990</t>
+          <t>PAZ, GRAL. AV. 5602</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>807458282</t>
+          <t>806926472</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
@@ -3197,7 +3197,7 @@
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>reparar rienda cortada - ver foto no es la misma que albarellos</t>
         </is>
       </c>
       <c r="I37" t="n">
@@ -3205,7 +3205,7 @@
       </c>
       <c r="J37" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Tensor</t>
         </is>
       </c>
       <c r="K37" t="inlineStr">
@@ -3215,14 +3215,14 @@
       </c>
       <c r="L37" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M37" t="n">
-        <v>-58.480925</v>
+        <v>-58.513685</v>
       </c>
       <c r="N37" t="n">
-        <v>-34.585471</v>
+        <v>-34.579838</v>
       </c>
       <c r="O37" t="inlineStr">
         <is>
@@ -3238,27 +3238,27 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>6143</t>
+          <t>5875</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>6/11/2025</t>
+          <t>5/27/2025</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>SOLANO LOPEZ, F., MARISCAL 2845</t>
+          <t>MONROE 4096</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>807458296</t>
+          <t>806975680</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
@@ -3295,14 +3295,14 @@
         </is>
       </c>
       <c r="M38" t="n">
-        <v>-58.495071</v>
+        <v>-58.476106</v>
       </c>
       <c r="N38" t="n">
-        <v>-34.593122</v>
+        <v>-34.568373</v>
       </c>
       <c r="O38" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P38" t="inlineStr">
@@ -3314,27 +3314,27 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>6141</t>
+          <t>807044192</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>6/11/2025</t>
+          <t>5/29/2025</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>EL PAMPERO 2618</t>
+          <t>O'Higgins 4379</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>807458310</t>
+          <t>807044192</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
@@ -3349,7 +3349,7 @@
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t xml:space="preserve">Poste </t>
         </is>
       </c>
       <c r="I39" t="n">
@@ -3357,7 +3357,7 @@
       </c>
       <c r="J39" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Desmonte</t>
         </is>
       </c>
       <c r="K39" t="inlineStr">
@@ -3367,18 +3367,18 @@
       </c>
       <c r="L39" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M39" t="n">
-        <v>-58.481942</v>
+        <v>-58.468425</v>
       </c>
       <c r="N39" t="n">
-        <v>-34.602989</v>
+        <v>-34.54124</v>
       </c>
       <c r="O39" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P39" t="inlineStr">
@@ -3390,27 +3390,27 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>-478</t>
+          <t>6020</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>6/15/2025</t>
+          <t>6/5/2025</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Chivilcoy 4875</t>
+          <t>RAVIGNANI, EMILIO, DR. 2036</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>807508509</t>
+          <t>807215465</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
@@ -3425,7 +3425,7 @@
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t>Poste podrido</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I40" t="n">
@@ -3443,50 +3443,50 @@
       </c>
       <c r="L40" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M40" t="n">
-        <v>-58.517389</v>
+        <v>-58.436298</v>
       </c>
       <c r="N40" t="n">
-        <v>-34.593541</v>
+        <v>-34.578972</v>
       </c>
       <c r="O40" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P40" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>6171</t>
+          <t>6144</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>6/18/2025</t>
+          <t>6/11/2025</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>CABELLO 3486</t>
+          <t>TURIN 2990</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>807658640</t>
+          <t>807458282</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
@@ -3501,7 +3501,7 @@
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>Columna inclinada evaluar con inspector un corrimiento</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I41" t="n">
@@ -3523,46 +3523,46 @@
         </is>
       </c>
       <c r="M41" t="n">
-        <v>-58.409579</v>
+        <v>-58.480925</v>
       </c>
       <c r="N41" t="n">
-        <v>-34.581134</v>
+        <v>-34.585471</v>
       </c>
       <c r="O41" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P41" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>6230</t>
+          <t>6143</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>6/24/2025</t>
+          <t>6/11/2025</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Santa maria de oro	2722</t>
+          <t>SOLANO LOPEZ, F., MARISCAL 2845</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>807763066</t>
+          <t>807458296</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
@@ -3599,46 +3599,46 @@
         </is>
       </c>
       <c r="M42" t="n">
-        <v>-58.422315</v>
+        <v>-58.495071</v>
       </c>
       <c r="N42" t="n">
-        <v>-34.576988</v>
+        <v>-34.593122</v>
       </c>
       <c r="O42" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P42" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>6231</t>
+          <t>6141</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>6/24/2025</t>
+          <t>6/11/2025</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Ciudad de la Paz 275</t>
+          <t>EL PAMPERO 2618</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>807763070</t>
+          <t>807458310</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
@@ -3653,7 +3653,7 @@
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>Aplomar o cambiar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I43" t="n">
@@ -3671,40 +3671,40 @@
       </c>
       <c r="L43" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M43" t="n">
-        <v>-58.441049</v>
+        <v>-58.481942</v>
       </c>
       <c r="N43" t="n">
-        <v>-34.574625</v>
+        <v>-34.602989</v>
       </c>
       <c r="O43" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P43" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>6235</t>
+          <t>-478</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>6/24/2025</t>
+          <t>6/15/2025</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>HUERGO 389</t>
+          <t>Chivilcoy 4875</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
@@ -3714,7 +3714,7 @@
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>807763078</t>
+          <t>807508509</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
@@ -3729,7 +3729,7 @@
       </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Poste podrido</t>
         </is>
       </c>
       <c r="I44" t="n">
@@ -3747,40 +3747,40 @@
       </c>
       <c r="L44" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M44" t="n">
-        <v>-58.432722</v>
+        <v>-58.517389</v>
       </c>
       <c r="N44" t="n">
-        <v>-34.572371</v>
+        <v>-34.593541</v>
       </c>
       <c r="O44" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P44" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>6295</t>
+          <t>6171</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>6/30/2025</t>
+          <t>6/18/2025</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>SOLER 6017</t>
+          <t>CABELLO 3486</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
@@ -3790,7 +3790,7 @@
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>807851636</t>
+          <t>807658640</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
@@ -3805,7 +3805,7 @@
       </c>
       <c r="H45" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Columna inclinada evaluar con inspector un corrimiento</t>
         </is>
       </c>
       <c r="I45" t="n">
@@ -3827,10 +3827,10 @@
         </is>
       </c>
       <c r="M45" t="n">
-        <v>-58.436808</v>
+        <v>-58.409579</v>
       </c>
       <c r="N45" t="n">
-        <v>-34.577464</v>
+        <v>-34.581134</v>
       </c>
       <c r="O45" t="inlineStr">
         <is>
@@ -3846,17 +3846,17 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>6331</t>
+          <t>6230</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>7/3/2025</t>
+          <t>6/24/2025</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>PARAGUAY 4259</t>
+          <t>Santa maria de oro	2722</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
@@ -3866,7 +3866,7 @@
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>807965788</t>
+          <t>807763066</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
@@ -3903,10 +3903,10 @@
         </is>
       </c>
       <c r="M46" t="n">
-        <v>-58.421822</v>
+        <v>-58.422315</v>
       </c>
       <c r="N46" t="n">
-        <v>-34.58645</v>
+        <v>-34.576988</v>
       </c>
       <c r="O46" t="inlineStr">
         <is>
@@ -3922,17 +3922,17 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>6332</t>
+          <t>6231</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>7/3/2025</t>
+          <t>6/24/2025</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>ARAOZ 2560</t>
+          <t>Ciudad de la Paz 275</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
@@ -3942,7 +3942,7 @@
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>807965818</t>
+          <t>807763070</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
@@ -3957,7 +3957,7 @@
       </c>
       <c r="H47" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Aplomar o cambiar</t>
         </is>
       </c>
       <c r="I47" t="n">
@@ -3975,14 +3975,14 @@
       </c>
       <c r="L47" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M47" t="n">
-        <v>-58.414507</v>
+        <v>-58.441049</v>
       </c>
       <c r="N47" t="n">
-        <v>-34.585377</v>
+        <v>-34.574625</v>
       </c>
       <c r="O47" t="inlineStr">
         <is>
@@ -3998,27 +3998,27 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>6336</t>
+          <t>6235</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>7/3/2025</t>
+          <t>6/24/2025</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>PARAGUAY 4291</t>
+          <t>HUERGO 389</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>807965819</t>
+          <t>807763078</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
@@ -4055,10 +4055,10 @@
         </is>
       </c>
       <c r="M48" t="n">
-        <v>-58.422084</v>
+        <v>-58.432722</v>
       </c>
       <c r="N48" t="n">
-        <v>-34.58625</v>
+        <v>-34.572371</v>
       </c>
       <c r="O48" t="inlineStr">
         <is>
@@ -4074,17 +4074,17 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>6337</t>
+          <t>6295</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>7/3/2025</t>
+          <t>6/30/2025</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>PARAGUAY 4383</t>
+          <t>SOLER 6017</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
@@ -4094,7 +4094,7 @@
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>807965926</t>
+          <t>807851636</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
@@ -4131,10 +4131,10 @@
         </is>
       </c>
       <c r="M49" t="n">
-        <v>-58.422931</v>
+        <v>-58.436808</v>
       </c>
       <c r="N49" t="n">
-        <v>-34.585597</v>
+        <v>-34.577464</v>
       </c>
       <c r="O49" t="inlineStr">
         <is>
@@ -4150,27 +4150,27 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>6363</t>
+          <t>6331</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>7/8/2025</t>
+          <t>7/3/2025</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>MOLDES 3730</t>
+          <t>PARAGUAY 4259</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>808099415</t>
+          <t>807965788</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
@@ -4185,7 +4185,7 @@
       </c>
       <c r="H50" t="inlineStr">
         <is>
-          <t>Poste inclinado</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I50" t="n">
@@ -4193,7 +4193,7 @@
       </c>
       <c r="J50" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K50" t="inlineStr">
@@ -4203,50 +4203,50 @@
       </c>
       <c r="L50" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M50" t="n">
-        <v>-58.47192</v>
+        <v>-58.421822</v>
       </c>
       <c r="N50" t="n">
-        <v>-34.549398</v>
+        <v>-34.58645</v>
       </c>
       <c r="O50" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P50" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>-503</t>
+          <t>6332</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>7/10/2025</t>
+          <t>7/3/2025</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Salguero 842</t>
+          <t>ARAOZ 2560</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>808148673</t>
+          <t>807965818</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
@@ -4261,7 +4261,7 @@
       </c>
       <c r="H51" t="inlineStr">
         <is>
-          <t>Cambiar columna picada en la base</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I51" t="n">
@@ -4283,14 +4283,14 @@
         </is>
       </c>
       <c r="M51" t="n">
-        <v>-58.419166</v>
+        <v>-58.414507</v>
       </c>
       <c r="N51" t="n">
-        <v>-34.600265</v>
+        <v>-34.585377</v>
       </c>
       <c r="O51" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P51" t="inlineStr">
@@ -4302,27 +4302,27 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>-504</t>
+          <t>6336</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>7/10/2025</t>
+          <t>7/3/2025</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>Ohiggins 1611</t>
+          <t>PARAGUAY 4291</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>808148679</t>
+          <t>807965819</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
@@ -4337,7 +4337,7 @@
       </c>
       <c r="H52" t="inlineStr">
         <is>
-          <t>Columna podrida en la base</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I52" t="n">
@@ -4350,7 +4350,7 @@
       </c>
       <c r="K52" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L52" t="inlineStr">
@@ -4359,46 +4359,46 @@
         </is>
       </c>
       <c r="M52" t="n">
-        <v>-58.448993</v>
+        <v>-58.422084</v>
       </c>
       <c r="N52" t="n">
-        <v>-34.564383</v>
+        <v>-34.58625</v>
       </c>
       <c r="O52" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P52" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>6437</t>
+          <t>6337</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>7/17/2025</t>
+          <t>7/3/2025</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>MILLER 4590</t>
+          <t>PARAGUAY 4383</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>808400306</t>
+          <t>807965926</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
@@ -4413,7 +4413,7 @@
       </c>
       <c r="H53" t="inlineStr">
         <is>
-          <t>Columna corroida</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I53" t="n">
@@ -4435,46 +4435,46 @@
         </is>
       </c>
       <c r="M53" t="n">
-        <v>-58.495482</v>
+        <v>-58.422931</v>
       </c>
       <c r="N53" t="n">
-        <v>-34.552614</v>
+        <v>-34.585597</v>
       </c>
       <c r="O53" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P53" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>6447</t>
+          <t>6363</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>7/17/2025</t>
+          <t>7/8/2025</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>CIUDAD DE LA PAZ 1535</t>
+          <t>MOLDES 3730</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>808400333</t>
+          <t>808099415</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
@@ -4489,7 +4489,7 @@
       </c>
       <c r="H54" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Poste inclinado</t>
         </is>
       </c>
       <c r="I54" t="n">
@@ -4497,7 +4497,7 @@
       </c>
       <c r="J54" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K54" t="inlineStr">
@@ -4507,18 +4507,18 @@
       </c>
       <c r="L54" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M54" t="n">
-        <v>-58.453124</v>
+        <v>-58.47192</v>
       </c>
       <c r="N54" t="n">
-        <v>-34.567382</v>
+        <v>-34.549398</v>
       </c>
       <c r="O54" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P54" t="inlineStr">
@@ -4530,27 +4530,27 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>-519</t>
+          <t>-503</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>7/17/2025</t>
+          <t>7/10/2025</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>Vilela 2687</t>
+          <t>Salguero 842</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>808400334</t>
+          <t>808148673</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
@@ -4565,7 +4565,7 @@
       </c>
       <c r="H55" t="inlineStr">
         <is>
-          <t>CAmbiar columna 114 picada en base</t>
+          <t>Cambiar columna picada en la base</t>
         </is>
       </c>
       <c r="I55" t="n">
@@ -4587,46 +4587,46 @@
         </is>
       </c>
       <c r="M55" t="n">
-        <v>-58.472968</v>
+        <v>-58.419166</v>
       </c>
       <c r="N55" t="n">
-        <v>-34.546898</v>
+        <v>-34.600265</v>
       </c>
       <c r="O55" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P55" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>-520</t>
+          <t>-504</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>7/17/2025</t>
+          <t>7/10/2025</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>Pedraza Manuela 4101</t>
+          <t>Ohiggins 1611</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>808400353</t>
+          <t>808148679</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
@@ -4641,7 +4641,7 @@
       </c>
       <c r="H56" t="inlineStr">
         <is>
-          <t xml:space="preserve">Podrida en la base </t>
+          <t>Columna podrida en la base</t>
         </is>
       </c>
       <c r="I56" t="n">
@@ -4654,7 +4654,7 @@
       </c>
       <c r="K56" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L56" t="inlineStr">
@@ -4663,14 +4663,14 @@
         </is>
       </c>
       <c r="M56" t="n">
-        <v>-58.481569</v>
+        <v>-58.448993</v>
       </c>
       <c r="N56" t="n">
-        <v>-34.559853</v>
+        <v>-34.564383</v>
       </c>
       <c r="O56" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P56" t="inlineStr">
@@ -4682,27 +4682,27 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>-525</t>
+          <t>6437</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>7/22/2025</t>
+          <t>7/17/2025</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>Zabala 3567</t>
+          <t>MILLER 4590</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>808480549</t>
+          <t>808400306</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
@@ -4717,7 +4717,7 @@
       </c>
       <c r="H57" t="inlineStr">
         <is>
-          <t>Corroida en base para recambio</t>
+          <t>Columna corroida</t>
         </is>
       </c>
       <c r="I57" t="n">
@@ -4739,14 +4739,14 @@
         </is>
       </c>
       <c r="M57" t="n">
-        <v>-58.457492</v>
+        <v>-58.495482</v>
       </c>
       <c r="N57" t="n">
-        <v>-34.579336</v>
+        <v>-34.552614</v>
       </c>
       <c r="O57" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P57" t="inlineStr">
@@ -4758,27 +4758,27 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>6484</t>
+          <t>6447</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>7/24/2025</t>
+          <t>7/17/2025</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>URIARTE 2396</t>
+          <t>CIUDAD DE LA PAZ 1535</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>808509373</t>
+          <t>808400333</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
@@ -4815,17 +4815,321 @@
         </is>
       </c>
       <c r="M58" t="n">
+        <v>-58.453124</v>
+      </c>
+      <c r="N58" t="n">
+        <v>-34.567382</v>
+      </c>
+      <c r="O58" t="inlineStr">
+        <is>
+          <t>Colegiales</t>
+        </is>
+      </c>
+      <c r="P58" t="inlineStr">
+        <is>
+          <t>Capital Norte</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>-519</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>7/17/2025</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>Vilela 2687</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>808400334</t>
+        </is>
+      </c>
+      <c r="F59" t="inlineStr">
+        <is>
+          <t>NEW</t>
+        </is>
+      </c>
+      <c r="G59" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H59" t="inlineStr">
+        <is>
+          <t>CAmbiar columna 114 picada en base</t>
+        </is>
+      </c>
+      <c r="I59" t="n">
+        <v>1</v>
+      </c>
+      <c r="J59" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K59" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L59" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M59" t="n">
+        <v>-58.472968</v>
+      </c>
+      <c r="N59" t="n">
+        <v>-34.546898</v>
+      </c>
+      <c r="O59" t="inlineStr">
+        <is>
+          <t>Saavedra</t>
+        </is>
+      </c>
+      <c r="P59" t="inlineStr">
+        <is>
+          <t>Capital Norte</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>-520</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>7/17/2025</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>Pedraza Manuela 4101</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>808400353</t>
+        </is>
+      </c>
+      <c r="F60" t="inlineStr">
+        <is>
+          <t>NEW</t>
+        </is>
+      </c>
+      <c r="G60" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H60" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Podrida en la base </t>
+        </is>
+      </c>
+      <c r="I60" t="n">
+        <v>1</v>
+      </c>
+      <c r="J60" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K60" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L60" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M60" t="n">
+        <v>-58.481569</v>
+      </c>
+      <c r="N60" t="n">
+        <v>-34.559853</v>
+      </c>
+      <c r="O60" t="inlineStr">
+        <is>
+          <t>Saavedra</t>
+        </is>
+      </c>
+      <c r="P60" t="inlineStr">
+        <is>
+          <t>Capital Norte</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>-525</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>7/22/2025</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>Zabala 3567</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>808480549</t>
+        </is>
+      </c>
+      <c r="F61" t="inlineStr">
+        <is>
+          <t>NEW</t>
+        </is>
+      </c>
+      <c r="G61" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H61" t="inlineStr">
+        <is>
+          <t>Corroida en base para recambio</t>
+        </is>
+      </c>
+      <c r="I61" t="n">
+        <v>1</v>
+      </c>
+      <c r="J61" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K61" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L61" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M61" t="n">
+        <v>-58.457492</v>
+      </c>
+      <c r="N61" t="n">
+        <v>-34.579336</v>
+      </c>
+      <c r="O61" t="inlineStr">
+        <is>
+          <t>Colegiales</t>
+        </is>
+      </c>
+      <c r="P61" t="inlineStr">
+        <is>
+          <t>Capital Norte</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>6484</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>7/24/2025</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>URIARTE 2396</t>
+        </is>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>14</t>
+        </is>
+      </c>
+      <c r="E62" t="inlineStr">
+        <is>
+          <t>808509373</t>
+        </is>
+      </c>
+      <c r="F62" t="inlineStr">
+        <is>
+          <t>NEW</t>
+        </is>
+      </c>
+      <c r="G62" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H62" t="inlineStr">
+        <is>
+          <t>Picada</t>
+        </is>
+      </c>
+      <c r="I62" t="n">
+        <v>1</v>
+      </c>
+      <c r="J62" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K62" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L62" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M62" t="n">
         <v>-58.423934</v>
       </c>
-      <c r="N58" t="n">
+      <c r="N62" t="n">
         <v>-34.581562</v>
       </c>
-      <c r="O58" t="inlineStr">
+      <c r="O62" t="inlineStr">
         <is>
           <t>Palermo</t>
         </is>
       </c>
-      <c r="P58" t="inlineStr">
+      <c r="P62" t="inlineStr">
         <is>
           <t>Capital Sur</t>
         </is>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-07-29 08:58:59)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_NEW.xlsx
+++ b/mapa_interactivo_NEW.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P62"/>
+  <dimension ref="A1:P68"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4378,27 +4378,27 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>6337</t>
+          <t>6363</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>7/3/2025</t>
+          <t>7/8/2025</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>PARAGUAY 4383</t>
+          <t>MOLDES 3730</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>807965926</t>
+          <t>808099415</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
@@ -4413,7 +4413,7 @@
       </c>
       <c r="H53" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Poste inclinado</t>
         </is>
       </c>
       <c r="I53" t="n">
@@ -4421,7 +4421,7 @@
       </c>
       <c r="J53" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K53" t="inlineStr">
@@ -4431,50 +4431,50 @@
       </c>
       <c r="L53" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M53" t="n">
-        <v>-58.422931</v>
+        <v>-58.47192</v>
       </c>
       <c r="N53" t="n">
-        <v>-34.585597</v>
+        <v>-34.549398</v>
       </c>
       <c r="O53" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P53" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>6363</t>
+          <t>-503</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>7/8/2025</t>
+          <t>7/10/2025</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>MOLDES 3730</t>
+          <t>Salguero 842</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>808099415</t>
+          <t>808148673</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
@@ -4489,7 +4489,7 @@
       </c>
       <c r="H54" t="inlineStr">
         <is>
-          <t>Poste inclinado</t>
+          <t>Cambiar columna picada en la base</t>
         </is>
       </c>
       <c r="I54" t="n">
@@ -4497,7 +4497,7 @@
       </c>
       <c r="J54" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K54" t="inlineStr">
@@ -4507,30 +4507,30 @@
       </c>
       <c r="L54" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M54" t="n">
-        <v>-58.47192</v>
+        <v>-58.419166</v>
       </c>
       <c r="N54" t="n">
-        <v>-34.549398</v>
+        <v>-34.600265</v>
       </c>
       <c r="O54" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P54" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>-503</t>
+          <t>6506</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
@@ -4540,17 +4540,17 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>Salguero 842</t>
+          <t>Ohiggins 1611</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>808148673</t>
+          <t>808148679</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
@@ -4565,7 +4565,7 @@
       </c>
       <c r="H55" t="inlineStr">
         <is>
-          <t>Cambiar columna picada en la base</t>
+          <t>Columna podrida en la base</t>
         </is>
       </c>
       <c r="I55" t="n">
@@ -4578,7 +4578,7 @@
       </c>
       <c r="K55" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L55" t="inlineStr">
@@ -4587,46 +4587,46 @@
         </is>
       </c>
       <c r="M55" t="n">
-        <v>-58.419166</v>
+        <v>-58.448993</v>
       </c>
       <c r="N55" t="n">
-        <v>-34.600265</v>
+        <v>-34.564383</v>
       </c>
       <c r="O55" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P55" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>-504</t>
+          <t>6437</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>7/10/2025</t>
+          <t>7/17/2025</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>Ohiggins 1611</t>
+          <t>MILLER 4590</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>808148679</t>
+          <t>808400306</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
@@ -4641,7 +4641,7 @@
       </c>
       <c r="H56" t="inlineStr">
         <is>
-          <t>Columna podrida en la base</t>
+          <t>Columna corroida</t>
         </is>
       </c>
       <c r="I56" t="n">
@@ -4654,7 +4654,7 @@
       </c>
       <c r="K56" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L56" t="inlineStr">
@@ -4663,14 +4663,14 @@
         </is>
       </c>
       <c r="M56" t="n">
-        <v>-58.448993</v>
+        <v>-58.495482</v>
       </c>
       <c r="N56" t="n">
-        <v>-34.564383</v>
+        <v>-34.552614</v>
       </c>
       <c r="O56" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P56" t="inlineStr">
@@ -4682,7 +4682,7 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>6437</t>
+          <t>6447</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
@@ -4692,17 +4692,17 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>MILLER 4590</t>
+          <t>CIUDAD DE LA PAZ 1535</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>808400306</t>
+          <t>808400333</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
@@ -4717,7 +4717,7 @@
       </c>
       <c r="H57" t="inlineStr">
         <is>
-          <t>Columna corroida</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I57" t="n">
@@ -4739,14 +4739,14 @@
         </is>
       </c>
       <c r="M57" t="n">
-        <v>-58.495482</v>
+        <v>-58.453124</v>
       </c>
       <c r="N57" t="n">
-        <v>-34.552614</v>
+        <v>-34.567382</v>
       </c>
       <c r="O57" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P57" t="inlineStr">
@@ -4758,7 +4758,7 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>6447</t>
+          <t>-519</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
@@ -4768,17 +4768,17 @@
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>CIUDAD DE LA PAZ 1535</t>
+          <t>Vilela 2687</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>808400333</t>
+          <t>808400334</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
@@ -4793,7 +4793,7 @@
       </c>
       <c r="H58" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>CAmbiar columna 114 picada en base</t>
         </is>
       </c>
       <c r="I58" t="n">
@@ -4815,14 +4815,14 @@
         </is>
       </c>
       <c r="M58" t="n">
-        <v>-58.453124</v>
+        <v>-58.472968</v>
       </c>
       <c r="N58" t="n">
-        <v>-34.567382</v>
+        <v>-34.546898</v>
       </c>
       <c r="O58" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P58" t="inlineStr">
@@ -4834,7 +4834,7 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>-519</t>
+          <t>-520</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
@@ -4844,7 +4844,7 @@
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>Vilela 2687</t>
+          <t>Pedraza Manuela 4101</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
@@ -4854,7 +4854,7 @@
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>808400334</t>
+          <t>808400353</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
@@ -4869,7 +4869,7 @@
       </c>
       <c r="H59" t="inlineStr">
         <is>
-          <t>CAmbiar columna 114 picada en base</t>
+          <t xml:space="preserve">Podrida en la base </t>
         </is>
       </c>
       <c r="I59" t="n">
@@ -4891,10 +4891,10 @@
         </is>
       </c>
       <c r="M59" t="n">
-        <v>-58.472968</v>
+        <v>-58.481569</v>
       </c>
       <c r="N59" t="n">
-        <v>-34.546898</v>
+        <v>-34.559853</v>
       </c>
       <c r="O59" t="inlineStr">
         <is>
@@ -4910,27 +4910,27 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>-520</t>
+          <t>-525</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>7/17/2025</t>
+          <t>7/22/2025</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>Pedraza Manuela 4101</t>
+          <t>Zabala 3567</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>808400353</t>
+          <t>808480549</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
@@ -4945,7 +4945,7 @@
       </c>
       <c r="H60" t="inlineStr">
         <is>
-          <t xml:space="preserve">Podrida en la base </t>
+          <t>Corroida en base para recambio</t>
         </is>
       </c>
       <c r="I60" t="n">
@@ -4967,14 +4967,14 @@
         </is>
       </c>
       <c r="M60" t="n">
-        <v>-58.481569</v>
+        <v>-58.457492</v>
       </c>
       <c r="N60" t="n">
-        <v>-34.559853</v>
+        <v>-34.579336</v>
       </c>
       <c r="O60" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P60" t="inlineStr">
@@ -4986,27 +4986,27 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>-525</t>
+          <t>6484</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>7/22/2025</t>
+          <t>7/24/2025</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>Zabala 3567</t>
+          <t>URIARTE 2396</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>808480549</t>
+          <t>808509373</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
@@ -5021,7 +5021,7 @@
       </c>
       <c r="H61" t="inlineStr">
         <is>
-          <t>Corroida en base para recambio</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I61" t="n">
@@ -5043,46 +5043,46 @@
         </is>
       </c>
       <c r="M61" t="n">
-        <v>-58.457492</v>
+        <v>-58.423934</v>
       </c>
       <c r="N61" t="n">
-        <v>-34.579336</v>
+        <v>-34.581562</v>
       </c>
       <c r="O61" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P61" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>6484</t>
+          <t>6502</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>7/24/2025</t>
+          <t>7/25/2025</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>URIARTE 2396</t>
+          <t>CIUDAD DE LA PAZ 1511</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>808509373</t>
+          <t>808571972</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
@@ -5119,17 +5119,469 @@
         </is>
       </c>
       <c r="M62" t="n">
-        <v>-58.423934</v>
+        <v>-58.452907</v>
       </c>
       <c r="N62" t="n">
-        <v>-34.581562</v>
+        <v>-34.567508</v>
       </c>
       <c r="O62" t="inlineStr">
         <is>
+          <t>Colegiales</t>
+        </is>
+      </c>
+      <c r="P62" t="inlineStr">
+        <is>
+          <t>Capital Norte</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>6504</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>7/25/2025</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>CIUDAD DE LA PAZ 1278</t>
+        </is>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>13</t>
+        </is>
+      </c>
+      <c r="E63" t="inlineStr">
+        <is>
+          <t>808571974</t>
+        </is>
+      </c>
+      <c r="F63" t="inlineStr">
+        <is>
+          <t>NEW</t>
+        </is>
+      </c>
+      <c r="G63" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H63" t="inlineStr">
+        <is>
+          <t>Inclinada</t>
+        </is>
+      </c>
+      <c r="I63" t="n">
+        <v>1</v>
+      </c>
+      <c r="J63" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K63" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L63" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M63" t="n">
+        <v>-58.450753</v>
+      </c>
+      <c r="N63" t="n">
+        <v>-34.5688</v>
+      </c>
+      <c r="O63" t="inlineStr">
+        <is>
+          <t>Colegiales</t>
+        </is>
+      </c>
+      <c r="P63" t="inlineStr">
+        <is>
+          <t>Capital Norte</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>6512</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>7/28/2025</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>GASCON 1195</t>
+        </is>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>14</t>
+        </is>
+      </c>
+      <c r="E64" t="inlineStr">
+        <is>
+          <t>808571975</t>
+        </is>
+      </c>
+      <c r="F64" t="inlineStr">
+        <is>
+          <t>NEW</t>
+        </is>
+      </c>
+      <c r="G64" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H64" t="inlineStr">
+        <is>
+          <t>Picada</t>
+        </is>
+      </c>
+      <c r="I64" t="n">
+        <v>1</v>
+      </c>
+      <c r="J64" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K64" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L64" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M64" t="n">
+        <v>-58.423127</v>
+      </c>
+      <c r="N64" t="n">
+        <v>-34.596476</v>
+      </c>
+      <c r="O64" t="inlineStr">
+        <is>
           <t>Palermo</t>
         </is>
       </c>
-      <c r="P62" t="inlineStr">
+      <c r="P64" t="inlineStr">
+        <is>
+          <t>Capital Sur</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>6513</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>7/28/2025</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>DORREGO 1925</t>
+        </is>
+      </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>14</t>
+        </is>
+      </c>
+      <c r="E65" t="inlineStr">
+        <is>
+          <t>808571976</t>
+        </is>
+      </c>
+      <c r="F65" t="inlineStr">
+        <is>
+          <t>NEW</t>
+        </is>
+      </c>
+      <c r="G65" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H65" t="inlineStr">
+        <is>
+          <t>Picada</t>
+        </is>
+      </c>
+      <c r="I65" t="n">
+        <v>1</v>
+      </c>
+      <c r="J65" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K65" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L65" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M65" t="n">
+        <v>-58.441281</v>
+      </c>
+      <c r="N65" t="n">
+        <v>-34.579867</v>
+      </c>
+      <c r="O65" t="inlineStr">
+        <is>
+          <t>Palermo</t>
+        </is>
+      </c>
+      <c r="P65" t="inlineStr">
+        <is>
+          <t>Capital Sur</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>6519</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>7/28/2025</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>SALGUERO, JERONIMO 2874</t>
+        </is>
+      </c>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>14</t>
+        </is>
+      </c>
+      <c r="E66" t="inlineStr">
+        <is>
+          <t>808571977</t>
+        </is>
+      </c>
+      <c r="F66" t="inlineStr">
+        <is>
+          <t>NEW</t>
+        </is>
+      </c>
+      <c r="G66" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H66" t="inlineStr">
+        <is>
+          <t>Reparar rienda</t>
+        </is>
+      </c>
+      <c r="I66" t="n">
+        <v>1</v>
+      </c>
+      <c r="J66" t="inlineStr">
+        <is>
+          <t>Tensor</t>
+        </is>
+      </c>
+      <c r="K66" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L66" t="inlineStr">
+        <is>
+          <t>Terminal</t>
+        </is>
+      </c>
+      <c r="M66" t="n">
+        <v>-58.407256</v>
+      </c>
+      <c r="N66" t="n">
+        <v>-34.578976</v>
+      </c>
+      <c r="O66" t="inlineStr">
+        <is>
+          <t>Palermo</t>
+        </is>
+      </c>
+      <c r="P66" t="inlineStr">
+        <is>
+          <t>Capital Sur</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>-534</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>7/28/2025</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>Jose Aaron Salmun Feijoo 325</t>
+        </is>
+      </c>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="E67" t="inlineStr">
+        <is>
+          <t>808571999</t>
+        </is>
+      </c>
+      <c r="F67" t="inlineStr">
+        <is>
+          <t>NEW</t>
+        </is>
+      </c>
+      <c r="G67" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H67" t="inlineStr">
+        <is>
+          <t>Cambiar terminal</t>
+        </is>
+      </c>
+      <c r="I67" t="n">
+        <v>0</v>
+      </c>
+      <c r="J67" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K67" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L67" t="inlineStr">
+        <is>
+          <t>Terminal</t>
+        </is>
+      </c>
+      <c r="M67" t="n">
+        <v>-58.3793</v>
+      </c>
+      <c r="N67" t="n">
+        <v>-34.636079</v>
+      </c>
+      <c r="O67" t="inlineStr">
+        <is>
+          <t>San Telmo</t>
+        </is>
+      </c>
+      <c r="P67" t="inlineStr">
+        <is>
+          <t>Capital Sur</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>-535</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>7/28/2025</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>Jose Aaron Salmun Feijoo 363</t>
+        </is>
+      </c>
+      <c r="D68" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="E68" t="inlineStr"/>
+      <c r="F68" t="inlineStr">
+        <is>
+          <t>NEW</t>
+        </is>
+      </c>
+      <c r="G68" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H68" t="inlineStr">
+        <is>
+          <t>Colocar prfv pasante</t>
+        </is>
+      </c>
+      <c r="I68" t="n">
+        <v>0</v>
+      </c>
+      <c r="J68" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K68" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L68" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M68" t="n">
+        <v>-58.379294</v>
+      </c>
+      <c r="N68" t="n">
+        <v>-34.636313</v>
+      </c>
+      <c r="O68" t="inlineStr">
+        <is>
+          <t>San Telmo</t>
+        </is>
+      </c>
+      <c r="P68" t="inlineStr">
         <is>
           <t>Capital Sur</t>
         </is>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-07-29 12:27:42)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_NEW.xlsx
+++ b/mapa_interactivo_NEW.xlsx
@@ -5536,7 +5536,11 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E68" t="inlineStr"/>
+      <c r="E68" t="inlineStr">
+        <is>
+          <t>ICD30238810</t>
+        </is>
+      </c>
       <c r="F68" t="inlineStr">
         <is>
           <t>NEW</t>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-07-30 06:58:25)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_NEW.xlsx
+++ b/mapa_interactivo_NEW.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P68"/>
+  <dimension ref="A1:P65"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2478,17 +2478,17 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>804922192</t>
+          <t>6173</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>4/24/2025</t>
+          <t>4/29/2025</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Paraguay 4657</t>
+          <t>ARMENIA 2321</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
@@ -2498,7 +2498,7 @@
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>804922192</t>
+          <t>805507398</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
@@ -2513,7 +2513,7 @@
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Picada volvio a entrar como caso 6325</t>
         </is>
       </c>
       <c r="I28" t="n">
@@ -2535,10 +2535,10 @@
         </is>
       </c>
       <c r="M28" t="n">
-        <v>-58.425642</v>
+        <v>-58.420549</v>
       </c>
       <c r="N28" t="n">
-        <v>-34.583525</v>
+        <v>-34.585103</v>
       </c>
       <c r="O28" t="inlineStr">
         <is>
@@ -2554,27 +2554,27 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>6173</t>
+          <t>5715</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>4/29/2025</t>
+          <t>5/1/2025</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>ARMENIA 2321</t>
+          <t>CUENCA 4690</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>805507398</t>
+          <t>805579094</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
@@ -2589,7 +2589,7 @@
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>Picada volvio a entrar como caso 6325</t>
+          <t>Aplomar poste</t>
         </is>
       </c>
       <c r="I29" t="n">
@@ -2597,7 +2597,7 @@
       </c>
       <c r="J29" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K29" t="inlineStr">
@@ -2607,30 +2607,30 @@
       </c>
       <c r="L29" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M29" t="n">
-        <v>-58.420549</v>
+        <v>-58.506061</v>
       </c>
       <c r="N29" t="n">
-        <v>-34.585103</v>
+        <v>-34.588887</v>
       </c>
       <c r="O29" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P29" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>5715</t>
+          <t>5719</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -2640,7 +2640,7 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>CUENCA 4690</t>
+          <t>CABEZON, JOSE LEON 2440</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
@@ -2650,7 +2650,7 @@
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>805579094</t>
+          <t>805579157</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
@@ -2665,7 +2665,7 @@
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>Aplomar poste</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I30" t="n">
@@ -2673,7 +2673,7 @@
       </c>
       <c r="J30" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K30" t="inlineStr">
@@ -2683,14 +2683,14 @@
       </c>
       <c r="L30" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M30" t="n">
-        <v>-58.506061</v>
+        <v>-58.499967</v>
       </c>
       <c r="N30" t="n">
-        <v>-34.588887</v>
+        <v>-34.57974</v>
       </c>
       <c r="O30" t="inlineStr">
         <is>
@@ -2706,7 +2706,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>5719</t>
+          <t>6333</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
@@ -2716,17 +2716,17 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>CABEZON, JOSE LEON 2440</t>
+          <t>ORTEGA Y GASSET 1816</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>805579157</t>
+          <t>805655342</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
@@ -2763,36 +2763,36 @@
         </is>
       </c>
       <c r="M31" t="n">
-        <v>-58.499967</v>
+        <v>-58.432556</v>
       </c>
       <c r="N31" t="n">
-        <v>-34.57974</v>
+        <v>-34.570279</v>
       </c>
       <c r="O31" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P31" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>6333</t>
+          <t>805707165</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>5/1/2025</t>
+          <t>5/7/2025</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>ORTEGA Y GASSET 1816</t>
+          <t>Baez 793</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
@@ -2802,7 +2802,7 @@
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>805655342</t>
+          <t>805707165</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
@@ -2817,7 +2817,7 @@
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>DESMONTAR COLUMNA DE 7 MTS Y TRANSFERIR A COMUNITARIA</t>
         </is>
       </c>
       <c r="I32" t="n">
@@ -2835,14 +2835,14 @@
       </c>
       <c r="L32" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M32" t="n">
-        <v>-58.432556</v>
+        <v>-58.436165</v>
       </c>
       <c r="N32" t="n">
-        <v>-34.570279</v>
+        <v>-34.569081</v>
       </c>
       <c r="O32" t="inlineStr">
         <is>
@@ -2858,27 +2858,27 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>805707165</t>
+          <t>5847</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>5/7/2025</t>
+          <t>5/8/2025</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Baez 793</t>
+          <t>JURAMENTO 5321</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>805707165</t>
+          <t>805791839</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
@@ -2893,7 +2893,7 @@
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>DESMONTAR COLUMNA DE 7 MTS Y TRANSFERIR A COMUNITARIA</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I33" t="n">
@@ -2911,50 +2911,50 @@
       </c>
       <c r="L33" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M33" t="n">
-        <v>-58.436165</v>
+        <v>-58.485193</v>
       </c>
       <c r="N33" t="n">
-        <v>-34.569081</v>
+        <v>-34.579621</v>
       </c>
       <c r="O33" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P33" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>5847</t>
+          <t>232</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>5/8/2025</t>
+          <t>5/9/2025</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>JURAMENTO 5321</t>
+          <t>Gorostiaga 2286</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>805791839</t>
+          <t>805791858</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
@@ -2991,46 +2991,46 @@
         </is>
       </c>
       <c r="M34" t="n">
-        <v>-58.485193</v>
+        <v>-58.441563</v>
       </c>
       <c r="N34" t="n">
-        <v>-34.579621</v>
+        <v>-34.569743</v>
       </c>
       <c r="O34" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P34" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>232</t>
+          <t>5826</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>5/9/2025</t>
+          <t>5/19/2025</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Gorostiaga 2286</t>
+          <t>ALBARELLOS AV. 3180</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>805791858</t>
+          <t>806926466</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
@@ -3045,7 +3045,7 @@
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Columna (metal) inclinada</t>
         </is>
       </c>
       <c r="I35" t="n">
@@ -3053,7 +3053,7 @@
       </c>
       <c r="J35" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K35" t="inlineStr">
@@ -3063,30 +3063,30 @@
       </c>
       <c r="L35" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M35" t="n">
-        <v>-58.441563</v>
+        <v>-58.513552</v>
       </c>
       <c r="N35" t="n">
-        <v>-34.569743</v>
+        <v>-34.579829</v>
       </c>
       <c r="O35" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P35" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>5826</t>
+          <t>5825</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
@@ -3096,7 +3096,7 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>ALBARELLOS AV. 3180</t>
+          <t>PAZ, GRAL. AV. 5602</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
@@ -3106,7 +3106,7 @@
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>806926466</t>
+          <t>806926472</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
@@ -3121,7 +3121,7 @@
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>Columna (metal) inclinada</t>
+          <t>reparar rienda cortada - ver foto no es la misma que albarellos</t>
         </is>
       </c>
       <c r="I36" t="n">
@@ -3129,7 +3129,7 @@
       </c>
       <c r="J36" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Tensor</t>
         </is>
       </c>
       <c r="K36" t="inlineStr">
@@ -3143,10 +3143,10 @@
         </is>
       </c>
       <c r="M36" t="n">
-        <v>-58.513552</v>
+        <v>-58.513685</v>
       </c>
       <c r="N36" t="n">
-        <v>-34.579829</v>
+        <v>-34.579838</v>
       </c>
       <c r="O36" t="inlineStr">
         <is>
@@ -3162,17 +3162,17 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>5825</t>
+          <t>5875</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>5/19/2025</t>
+          <t>5/27/2025</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>PAZ, GRAL. AV. 5602</t>
+          <t>MONROE 4096</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
@@ -3182,7 +3182,7 @@
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>806926472</t>
+          <t>806975680</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
@@ -3197,7 +3197,7 @@
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>reparar rienda cortada - ver foto no es la misma que albarellos</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I37" t="n">
@@ -3205,7 +3205,7 @@
       </c>
       <c r="J37" t="inlineStr">
         <is>
-          <t>Tensor</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K37" t="inlineStr">
@@ -3215,18 +3215,18 @@
       </c>
       <c r="L37" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M37" t="n">
-        <v>-58.513685</v>
+        <v>-58.476106</v>
       </c>
       <c r="N37" t="n">
-        <v>-34.579838</v>
+        <v>-34.568373</v>
       </c>
       <c r="O37" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P37" t="inlineStr">
@@ -3238,27 +3238,27 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>5875</t>
+          <t>807044192</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>5/27/2025</t>
+          <t>5/29/2025</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>MONROE 4096</t>
+          <t>O'Higgins 4379</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>806975680</t>
+          <t>807044192</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
@@ -3273,7 +3273,7 @@
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t xml:space="preserve">Poste </t>
         </is>
       </c>
       <c r="I38" t="n">
@@ -3281,7 +3281,7 @@
       </c>
       <c r="J38" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Desmonte</t>
         </is>
       </c>
       <c r="K38" t="inlineStr">
@@ -3291,18 +3291,18 @@
       </c>
       <c r="L38" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M38" t="n">
-        <v>-58.476106</v>
+        <v>-58.468425</v>
       </c>
       <c r="N38" t="n">
-        <v>-34.568373</v>
+        <v>-34.54124</v>
       </c>
       <c r="O38" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P38" t="inlineStr">
@@ -3314,27 +3314,27 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>807044192</t>
+          <t>6020</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>5/29/2025</t>
+          <t>6/5/2025</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>O'Higgins 4379</t>
+          <t>RAVIGNANI, EMILIO, DR. 2036</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>807044192</t>
+          <t>807215465</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
@@ -3349,7 +3349,7 @@
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t xml:space="preserve">Poste </t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I39" t="n">
@@ -3357,7 +3357,7 @@
       </c>
       <c r="J39" t="inlineStr">
         <is>
-          <t>Desmonte</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K39" t="inlineStr">
@@ -3367,50 +3367,50 @@
       </c>
       <c r="L39" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M39" t="n">
-        <v>-58.468425</v>
+        <v>-58.436298</v>
       </c>
       <c r="N39" t="n">
-        <v>-34.54124</v>
+        <v>-34.578972</v>
       </c>
       <c r="O39" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P39" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>6020</t>
+          <t>6144</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>6/5/2025</t>
+          <t>6/11/2025</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>RAVIGNANI, EMILIO, DR. 2036</t>
+          <t>TURIN 2990</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>807215465</t>
+          <t>807458282</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
@@ -3447,26 +3447,26 @@
         </is>
       </c>
       <c r="M40" t="n">
-        <v>-58.436298</v>
+        <v>-58.480925</v>
       </c>
       <c r="N40" t="n">
-        <v>-34.578972</v>
+        <v>-34.585471</v>
       </c>
       <c r="O40" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P40" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>6144</t>
+          <t>6143</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
@@ -3476,7 +3476,7 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>TURIN 2990</t>
+          <t>SOLANO LOPEZ, F., MARISCAL 2845</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
@@ -3486,7 +3486,7 @@
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>807458282</t>
+          <t>807458296</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
@@ -3523,10 +3523,10 @@
         </is>
       </c>
       <c r="M41" t="n">
-        <v>-58.480925</v>
+        <v>-58.495071</v>
       </c>
       <c r="N41" t="n">
-        <v>-34.585471</v>
+        <v>-34.593122</v>
       </c>
       <c r="O41" t="inlineStr">
         <is>
@@ -3542,7 +3542,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>6143</t>
+          <t>6141</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
@@ -3552,17 +3552,17 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>SOLANO LOPEZ, F., MARISCAL 2845</t>
+          <t>EL PAMPERO 2618</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>807458296</t>
+          <t>807458310</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
@@ -3599,10 +3599,10 @@
         </is>
       </c>
       <c r="M42" t="n">
-        <v>-58.495071</v>
+        <v>-58.481942</v>
       </c>
       <c r="N42" t="n">
-        <v>-34.593122</v>
+        <v>-34.602989</v>
       </c>
       <c r="O42" t="inlineStr">
         <is>
@@ -3618,17 +3618,17 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>6141</t>
+          <t>-478</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>6/11/2025</t>
+          <t>6/15/2025</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>EL PAMPERO 2618</t>
+          <t>Chivilcoy 4875</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
@@ -3638,7 +3638,7 @@
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>807458310</t>
+          <t>807508509</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
@@ -3653,7 +3653,7 @@
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Poste podrido</t>
         </is>
       </c>
       <c r="I43" t="n">
@@ -3671,14 +3671,14 @@
       </c>
       <c r="L43" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M43" t="n">
-        <v>-58.481942</v>
+        <v>-58.517389</v>
       </c>
       <c r="N43" t="n">
-        <v>-34.602989</v>
+        <v>-34.593541</v>
       </c>
       <c r="O43" t="inlineStr">
         <is>
@@ -3694,27 +3694,27 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>-478</t>
+          <t>6171</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>6/15/2025</t>
+          <t>6/18/2025</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Chivilcoy 4875</t>
+          <t>CABELLO 3486</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>807508509</t>
+          <t>807658640</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
@@ -3729,7 +3729,7 @@
       </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t>Poste podrido</t>
+          <t>Columna inclinada evaluar con inspector un corrimiento</t>
         </is>
       </c>
       <c r="I44" t="n">
@@ -3747,40 +3747,40 @@
       </c>
       <c r="L44" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M44" t="n">
-        <v>-58.517389</v>
+        <v>-58.409579</v>
       </c>
       <c r="N44" t="n">
-        <v>-34.593541</v>
+        <v>-34.581134</v>
       </c>
       <c r="O44" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P44" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>6171</t>
+          <t>6230</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>6/18/2025</t>
+          <t>6/24/2025</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>CABELLO 3486</t>
+          <t>Santa maria de oro	2722</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
@@ -3790,7 +3790,7 @@
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>807658640</t>
+          <t>807763066</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
@@ -3805,7 +3805,7 @@
       </c>
       <c r="H45" t="inlineStr">
         <is>
-          <t>Columna inclinada evaluar con inspector un corrimiento</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I45" t="n">
@@ -3827,10 +3827,10 @@
         </is>
       </c>
       <c r="M45" t="n">
-        <v>-58.409579</v>
+        <v>-58.422315</v>
       </c>
       <c r="N45" t="n">
-        <v>-34.581134</v>
+        <v>-34.576988</v>
       </c>
       <c r="O45" t="inlineStr">
         <is>
@@ -3846,7 +3846,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>6230</t>
+          <t>6231</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
@@ -3856,7 +3856,7 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Santa maria de oro	2722</t>
+          <t>Ciudad de la Paz 275</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
@@ -3866,7 +3866,7 @@
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>807763066</t>
+          <t>807763070</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
@@ -3881,7 +3881,7 @@
       </c>
       <c r="H46" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Aplomar o cambiar</t>
         </is>
       </c>
       <c r="I46" t="n">
@@ -3899,14 +3899,14 @@
       </c>
       <c r="L46" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M46" t="n">
-        <v>-58.422315</v>
+        <v>-58.441049</v>
       </c>
       <c r="N46" t="n">
-        <v>-34.576988</v>
+        <v>-34.574625</v>
       </c>
       <c r="O46" t="inlineStr">
         <is>
@@ -3922,7 +3922,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>6231</t>
+          <t>6235</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
@@ -3932,17 +3932,17 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Ciudad de la Paz 275</t>
+          <t>HUERGO 389</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>807763070</t>
+          <t>807763078</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
@@ -3957,7 +3957,7 @@
       </c>
       <c r="H47" t="inlineStr">
         <is>
-          <t>Aplomar o cambiar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I47" t="n">
@@ -3975,14 +3975,14 @@
       </c>
       <c r="L47" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M47" t="n">
-        <v>-58.441049</v>
+        <v>-58.432722</v>
       </c>
       <c r="N47" t="n">
-        <v>-34.574625</v>
+        <v>-34.572371</v>
       </c>
       <c r="O47" t="inlineStr">
         <is>
@@ -3998,27 +3998,27 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>6235</t>
+          <t>6295</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>6/24/2025</t>
+          <t>6/30/2025</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>HUERGO 389</t>
+          <t>SOLER 6017</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>807763078</t>
+          <t>807851636</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
@@ -4055,10 +4055,10 @@
         </is>
       </c>
       <c r="M48" t="n">
-        <v>-58.432722</v>
+        <v>-58.436808</v>
       </c>
       <c r="N48" t="n">
-        <v>-34.572371</v>
+        <v>-34.577464</v>
       </c>
       <c r="O48" t="inlineStr">
         <is>
@@ -4074,17 +4074,17 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>6295</t>
+          <t>6332</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>6/30/2025</t>
+          <t>7/3/2025</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>SOLER 6017</t>
+          <t>ARAOZ 2560</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
@@ -4094,7 +4094,7 @@
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>807851636</t>
+          <t>807965818</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
@@ -4131,10 +4131,10 @@
         </is>
       </c>
       <c r="M49" t="n">
-        <v>-58.436808</v>
+        <v>-58.414507</v>
       </c>
       <c r="N49" t="n">
-        <v>-34.577464</v>
+        <v>-34.585377</v>
       </c>
       <c r="O49" t="inlineStr">
         <is>
@@ -4150,27 +4150,27 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>6331</t>
+          <t>6363</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>7/3/2025</t>
+          <t>7/8/2025</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>PARAGUAY 4259</t>
+          <t>MOLDES 3730</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>807965788</t>
+          <t>808099415</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
@@ -4185,7 +4185,7 @@
       </c>
       <c r="H50" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Poste inclinado</t>
         </is>
       </c>
       <c r="I50" t="n">
@@ -4193,7 +4193,7 @@
       </c>
       <c r="J50" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K50" t="inlineStr">
@@ -4203,50 +4203,50 @@
       </c>
       <c r="L50" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M50" t="n">
-        <v>-58.421822</v>
+        <v>-58.47192</v>
       </c>
       <c r="N50" t="n">
-        <v>-34.58645</v>
+        <v>-34.549398</v>
       </c>
       <c r="O50" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P50" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>6332</t>
+          <t>-503</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>7/3/2025</t>
+          <t>7/10/2025</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>ARAOZ 2560</t>
+          <t>Salguero 842</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>807965818</t>
+          <t>808148673</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
@@ -4261,7 +4261,7 @@
       </c>
       <c r="H51" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambiar columna picada en la base</t>
         </is>
       </c>
       <c r="I51" t="n">
@@ -4283,14 +4283,14 @@
         </is>
       </c>
       <c r="M51" t="n">
-        <v>-58.414507</v>
+        <v>-58.419166</v>
       </c>
       <c r="N51" t="n">
-        <v>-34.585377</v>
+        <v>-34.600265</v>
       </c>
       <c r="O51" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P51" t="inlineStr">
@@ -4302,27 +4302,27 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>6336</t>
+          <t>6506</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>7/3/2025</t>
+          <t>7/10/2025</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>PARAGUAY 4291</t>
+          <t>Ohiggins 1611</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>807965819</t>
+          <t>808148679</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
@@ -4337,7 +4337,7 @@
       </c>
       <c r="H52" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Columna podrida en la base</t>
         </is>
       </c>
       <c r="I52" t="n">
@@ -4350,7 +4350,7 @@
       </c>
       <c r="K52" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L52" t="inlineStr">
@@ -4359,36 +4359,36 @@
         </is>
       </c>
       <c r="M52" t="n">
-        <v>-58.422084</v>
+        <v>-58.448993</v>
       </c>
       <c r="N52" t="n">
-        <v>-34.58625</v>
+        <v>-34.564383</v>
       </c>
       <c r="O52" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P52" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>6363</t>
+          <t>6437</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>7/8/2025</t>
+          <t>7/17/2025</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>MOLDES 3730</t>
+          <t>MILLER 4590</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
@@ -4398,7 +4398,7 @@
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>808099415</t>
+          <t>808400306</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
@@ -4413,7 +4413,7 @@
       </c>
       <c r="H53" t="inlineStr">
         <is>
-          <t>Poste inclinado</t>
+          <t>Columna corroida</t>
         </is>
       </c>
       <c r="I53" t="n">
@@ -4421,7 +4421,7 @@
       </c>
       <c r="J53" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K53" t="inlineStr">
@@ -4431,14 +4431,14 @@
       </c>
       <c r="L53" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M53" t="n">
-        <v>-58.47192</v>
+        <v>-58.495482</v>
       </c>
       <c r="N53" t="n">
-        <v>-34.549398</v>
+        <v>-34.552614</v>
       </c>
       <c r="O53" t="inlineStr">
         <is>
@@ -4454,27 +4454,27 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>-503</t>
+          <t>6447</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>7/10/2025</t>
+          <t>7/17/2025</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>Salguero 842</t>
+          <t>CIUDAD DE LA PAZ 1535</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>808148673</t>
+          <t>808400333</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
@@ -4489,7 +4489,7 @@
       </c>
       <c r="H54" t="inlineStr">
         <is>
-          <t>Cambiar columna picada en la base</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I54" t="n">
@@ -4511,46 +4511,46 @@
         </is>
       </c>
       <c r="M54" t="n">
-        <v>-58.419166</v>
+        <v>-58.453124</v>
       </c>
       <c r="N54" t="n">
-        <v>-34.600265</v>
+        <v>-34.567382</v>
       </c>
       <c r="O54" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P54" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>6506</t>
+          <t>-519</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>7/10/2025</t>
+          <t>7/17/2025</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>Ohiggins 1611</t>
+          <t>Vilela 2687</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>808148679</t>
+          <t>808400334</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
@@ -4565,7 +4565,7 @@
       </c>
       <c r="H55" t="inlineStr">
         <is>
-          <t>Columna podrida en la base</t>
+          <t>CAmbiar columna 114 picada en base</t>
         </is>
       </c>
       <c r="I55" t="n">
@@ -4578,7 +4578,7 @@
       </c>
       <c r="K55" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L55" t="inlineStr">
@@ -4587,14 +4587,14 @@
         </is>
       </c>
       <c r="M55" t="n">
-        <v>-58.448993</v>
+        <v>-58.472968</v>
       </c>
       <c r="N55" t="n">
-        <v>-34.564383</v>
+        <v>-34.546898</v>
       </c>
       <c r="O55" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P55" t="inlineStr">
@@ -4606,7 +4606,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>6437</t>
+          <t>6538</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
@@ -4616,7 +4616,7 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>MILLER 4590</t>
+          <t>Pedraza Manuela 4101</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
@@ -4626,7 +4626,7 @@
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>808400306</t>
+          <t>808400353</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
@@ -4641,7 +4641,7 @@
       </c>
       <c r="H56" t="inlineStr">
         <is>
-          <t>Columna corroida</t>
+          <t xml:space="preserve">Podrida en la base </t>
         </is>
       </c>
       <c r="I56" t="n">
@@ -4663,10 +4663,10 @@
         </is>
       </c>
       <c r="M56" t="n">
-        <v>-58.495482</v>
+        <v>-58.481569</v>
       </c>
       <c r="N56" t="n">
-        <v>-34.552614</v>
+        <v>-34.559853</v>
       </c>
       <c r="O56" t="inlineStr">
         <is>
@@ -4682,27 +4682,27 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>6447</t>
+          <t>-525</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>7/17/2025</t>
+          <t>7/22/2025</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>CIUDAD DE LA PAZ 1535</t>
+          <t>Zabala 3567</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>808400333</t>
+          <t>808480549</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
@@ -4717,7 +4717,7 @@
       </c>
       <c r="H57" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Corroida en base para recambio</t>
         </is>
       </c>
       <c r="I57" t="n">
@@ -4739,10 +4739,10 @@
         </is>
       </c>
       <c r="M57" t="n">
-        <v>-58.453124</v>
+        <v>-58.457492</v>
       </c>
       <c r="N57" t="n">
-        <v>-34.567382</v>
+        <v>-34.579336</v>
       </c>
       <c r="O57" t="inlineStr">
         <is>
@@ -4758,27 +4758,27 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>-519</t>
+          <t>6484</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>7/17/2025</t>
+          <t>7/24/2025</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>Vilela 2687</t>
+          <t>URIARTE 2396</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>808400334</t>
+          <t>808509373</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
@@ -4793,7 +4793,7 @@
       </c>
       <c r="H58" t="inlineStr">
         <is>
-          <t>CAmbiar columna 114 picada en base</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I58" t="n">
@@ -4815,46 +4815,46 @@
         </is>
       </c>
       <c r="M58" t="n">
-        <v>-58.472968</v>
+        <v>-58.423934</v>
       </c>
       <c r="N58" t="n">
-        <v>-34.546898</v>
+        <v>-34.581562</v>
       </c>
       <c r="O58" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P58" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>-520</t>
+          <t>6502</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>7/17/2025</t>
+          <t>7/25/2025</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>Pedraza Manuela 4101</t>
+          <t>CIUDAD DE LA PAZ 1511</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>808400353</t>
+          <t>808571972</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
@@ -4869,7 +4869,7 @@
       </c>
       <c r="H59" t="inlineStr">
         <is>
-          <t xml:space="preserve">Podrida en la base </t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I59" t="n">
@@ -4891,14 +4891,14 @@
         </is>
       </c>
       <c r="M59" t="n">
-        <v>-58.481569</v>
+        <v>-58.452907</v>
       </c>
       <c r="N59" t="n">
-        <v>-34.559853</v>
+        <v>-34.567508</v>
       </c>
       <c r="O59" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P59" t="inlineStr">
@@ -4910,27 +4910,27 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>-525</t>
+          <t>6504</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>7/22/2025</t>
+          <t>7/25/2025</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>Zabala 3567</t>
+          <t>CIUDAD DE LA PAZ 1278</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>808480549</t>
+          <t>808571974</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
@@ -4945,7 +4945,7 @@
       </c>
       <c r="H60" t="inlineStr">
         <is>
-          <t>Corroida en base para recambio</t>
+          <t>Inclinada</t>
         </is>
       </c>
       <c r="I60" t="n">
@@ -4967,10 +4967,10 @@
         </is>
       </c>
       <c r="M60" t="n">
-        <v>-58.457492</v>
+        <v>-58.450753</v>
       </c>
       <c r="N60" t="n">
-        <v>-34.579336</v>
+        <v>-34.5688</v>
       </c>
       <c r="O60" t="inlineStr">
         <is>
@@ -4986,17 +4986,17 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>6484</t>
+          <t>6512</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>7/24/2025</t>
+          <t>7/28/2025</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>URIARTE 2396</t>
+          <t>GASCON 1195</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
@@ -5006,7 +5006,7 @@
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>808509373</t>
+          <t>808571975</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
@@ -5043,10 +5043,10 @@
         </is>
       </c>
       <c r="M61" t="n">
-        <v>-58.423934</v>
+        <v>-58.423127</v>
       </c>
       <c r="N61" t="n">
-        <v>-34.581562</v>
+        <v>-34.596476</v>
       </c>
       <c r="O61" t="inlineStr">
         <is>
@@ -5062,27 +5062,27 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>6502</t>
+          <t>6513</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>7/25/2025</t>
+          <t>7/28/2025</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>CIUDAD DE LA PAZ 1511</t>
+          <t>DORREGO 1925</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>808571972</t>
+          <t>808571976</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
@@ -5119,46 +5119,46 @@
         </is>
       </c>
       <c r="M62" t="n">
-        <v>-58.452907</v>
+        <v>-58.441281</v>
       </c>
       <c r="N62" t="n">
-        <v>-34.567508</v>
+        <v>-34.579867</v>
       </c>
       <c r="O62" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P62" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>6504</t>
+          <t>6519</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>7/25/2025</t>
+          <t>7/28/2025</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>CIUDAD DE LA PAZ 1278</t>
+          <t>SALGUERO, JERONIMO 2874</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>808571974</t>
+          <t>808571977</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
@@ -5173,7 +5173,7 @@
       </c>
       <c r="H63" t="inlineStr">
         <is>
-          <t>Inclinada</t>
+          <t>Reparar rienda</t>
         </is>
       </c>
       <c r="I63" t="n">
@@ -5181,7 +5181,7 @@
       </c>
       <c r="J63" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Tensor</t>
         </is>
       </c>
       <c r="K63" t="inlineStr">
@@ -5191,30 +5191,30 @@
       </c>
       <c r="L63" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M63" t="n">
-        <v>-58.450753</v>
+        <v>-58.407256</v>
       </c>
       <c r="N63" t="n">
-        <v>-34.5688</v>
+        <v>-34.578976</v>
       </c>
       <c r="O63" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P63" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>6512</t>
+          <t>-534</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
@@ -5224,17 +5224,17 @@
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>GASCON 1195</t>
+          <t>Jose Aaron Salmun Feijoo 325</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>808571975</t>
+          <t>808571999</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
@@ -5249,11 +5249,11 @@
       </c>
       <c r="H64" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambiar terminal</t>
         </is>
       </c>
       <c r="I64" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J64" t="inlineStr">
         <is>
@@ -5267,18 +5267,18 @@
       </c>
       <c r="L64" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M64" t="n">
-        <v>-58.423127</v>
+        <v>-58.3793</v>
       </c>
       <c r="N64" t="n">
-        <v>-34.596476</v>
+        <v>-34.636079</v>
       </c>
       <c r="O64" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P64" t="inlineStr">
@@ -5290,7 +5290,7 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>6513</t>
+          <t>-535</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
@@ -5300,17 +5300,17 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>DORREGO 1925</t>
+          <t>Jose Aaron Salmun Feijoo 363</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>808571976</t>
+          <t>ICD30238810</t>
         </is>
       </c>
       <c r="F65" t="inlineStr">
@@ -5325,11 +5325,11 @@
       </c>
       <c r="H65" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Colocar prfv pasante</t>
         </is>
       </c>
       <c r="I65" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J65" t="inlineStr">
         <is>
@@ -5347,245 +5347,17 @@
         </is>
       </c>
       <c r="M65" t="n">
-        <v>-58.441281</v>
+        <v>-58.379294</v>
       </c>
       <c r="N65" t="n">
-        <v>-34.579867</v>
+        <v>-34.636313</v>
       </c>
       <c r="O65" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P65" t="inlineStr">
-        <is>
-          <t>Capital Sur</t>
-        </is>
-      </c>
-    </row>
-    <row r="66">
-      <c r="A66" t="inlineStr">
-        <is>
-          <t>6519</t>
-        </is>
-      </c>
-      <c r="B66" t="inlineStr">
-        <is>
-          <t>7/28/2025</t>
-        </is>
-      </c>
-      <c r="C66" t="inlineStr">
-        <is>
-          <t>SALGUERO, JERONIMO 2874</t>
-        </is>
-      </c>
-      <c r="D66" t="inlineStr">
-        <is>
-          <t>14</t>
-        </is>
-      </c>
-      <c r="E66" t="inlineStr">
-        <is>
-          <t>808571977</t>
-        </is>
-      </c>
-      <c r="F66" t="inlineStr">
-        <is>
-          <t>NEW</t>
-        </is>
-      </c>
-      <c r="G66" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H66" t="inlineStr">
-        <is>
-          <t>Reparar rienda</t>
-        </is>
-      </c>
-      <c r="I66" t="n">
-        <v>1</v>
-      </c>
-      <c r="J66" t="inlineStr">
-        <is>
-          <t>Tensor</t>
-        </is>
-      </c>
-      <c r="K66" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L66" t="inlineStr">
-        <is>
-          <t>Terminal</t>
-        </is>
-      </c>
-      <c r="M66" t="n">
-        <v>-58.407256</v>
-      </c>
-      <c r="N66" t="n">
-        <v>-34.578976</v>
-      </c>
-      <c r="O66" t="inlineStr">
-        <is>
-          <t>Palermo</t>
-        </is>
-      </c>
-      <c r="P66" t="inlineStr">
-        <is>
-          <t>Capital Sur</t>
-        </is>
-      </c>
-    </row>
-    <row r="67">
-      <c r="A67" t="inlineStr">
-        <is>
-          <t>-534</t>
-        </is>
-      </c>
-      <c r="B67" t="inlineStr">
-        <is>
-          <t>7/28/2025</t>
-        </is>
-      </c>
-      <c r="C67" t="inlineStr">
-        <is>
-          <t>Jose Aaron Salmun Feijoo 325</t>
-        </is>
-      </c>
-      <c r="D67" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="E67" t="inlineStr">
-        <is>
-          <t>808571999</t>
-        </is>
-      </c>
-      <c r="F67" t="inlineStr">
-        <is>
-          <t>NEW</t>
-        </is>
-      </c>
-      <c r="G67" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H67" t="inlineStr">
-        <is>
-          <t>Cambiar terminal</t>
-        </is>
-      </c>
-      <c r="I67" t="n">
-        <v>0</v>
-      </c>
-      <c r="J67" t="inlineStr">
-        <is>
-          <t>Cambio</t>
-        </is>
-      </c>
-      <c r="K67" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L67" t="inlineStr">
-        <is>
-          <t>Terminal</t>
-        </is>
-      </c>
-      <c r="M67" t="n">
-        <v>-58.3793</v>
-      </c>
-      <c r="N67" t="n">
-        <v>-34.636079</v>
-      </c>
-      <c r="O67" t="inlineStr">
-        <is>
-          <t>San Telmo</t>
-        </is>
-      </c>
-      <c r="P67" t="inlineStr">
-        <is>
-          <t>Capital Sur</t>
-        </is>
-      </c>
-    </row>
-    <row r="68">
-      <c r="A68" t="inlineStr">
-        <is>
-          <t>-535</t>
-        </is>
-      </c>
-      <c r="B68" t="inlineStr">
-        <is>
-          <t>7/28/2025</t>
-        </is>
-      </c>
-      <c r="C68" t="inlineStr">
-        <is>
-          <t>Jose Aaron Salmun Feijoo 363</t>
-        </is>
-      </c>
-      <c r="D68" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="E68" t="inlineStr">
-        <is>
-          <t>ICD30238810</t>
-        </is>
-      </c>
-      <c r="F68" t="inlineStr">
-        <is>
-          <t>NEW</t>
-        </is>
-      </c>
-      <c r="G68" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H68" t="inlineStr">
-        <is>
-          <t>Colocar prfv pasante</t>
-        </is>
-      </c>
-      <c r="I68" t="n">
-        <v>0</v>
-      </c>
-      <c r="J68" t="inlineStr">
-        <is>
-          <t>Cambio</t>
-        </is>
-      </c>
-      <c r="K68" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L68" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
-      <c r="M68" t="n">
-        <v>-58.379294</v>
-      </c>
-      <c r="N68" t="n">
-        <v>-34.636313</v>
-      </c>
-      <c r="O68" t="inlineStr">
-        <is>
-          <t>San Telmo</t>
-        </is>
-      </c>
-      <c r="P68" t="inlineStr">
         <is>
           <t>Capital Sur</t>
         </is>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-07-31 07:18:40)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_NEW.xlsx
+++ b/mapa_interactivo_NEW.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P65"/>
+  <dimension ref="A1:P66"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5363,6 +5363,82 @@
         </is>
       </c>
     </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>-538</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>7/31/2025</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>Malabia 964</t>
+        </is>
+      </c>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="E66" t="inlineStr">
+        <is>
+          <t>808609237</t>
+        </is>
+      </c>
+      <c r="F66" t="inlineStr">
+        <is>
+          <t>NEW</t>
+        </is>
+      </c>
+      <c r="G66" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H66" t="inlineStr">
+        <is>
+          <t>Cambiar poste mal estado por PRFV</t>
+        </is>
+      </c>
+      <c r="I66" t="n">
+        <v>1</v>
+      </c>
+      <c r="J66" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K66" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L66" t="inlineStr">
+        <is>
+          <t>Poste</t>
+        </is>
+      </c>
+      <c r="M66" t="n">
+        <v>-58.433634</v>
+      </c>
+      <c r="N66" t="n">
+        <v>-34.595018</v>
+      </c>
+      <c r="O66" t="inlineStr">
+        <is>
+          <t>Palermo</t>
+        </is>
+      </c>
+      <c r="P66" t="inlineStr">
+        <is>
+          <t>Capital Sur</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-07-31 14:41:43)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_NEW.xlsx
+++ b/mapa_interactivo_NEW.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P66"/>
+  <dimension ref="A1:P64"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5214,27 +5214,27 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>-534</t>
+          <t>-538</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>7/28/2025</t>
+          <t>7/31/2025</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>Jose Aaron Salmun Feijoo 325</t>
+          <t>Malabia 964</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>808571999</t>
+          <t>808609237</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
@@ -5249,11 +5249,11 @@
       </c>
       <c r="H64" t="inlineStr">
         <is>
-          <t>Cambiar terminal</t>
+          <t>Cambiar poste mal estado por PRFV</t>
         </is>
       </c>
       <c r="I64" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J64" t="inlineStr">
         <is>
@@ -5267,173 +5267,21 @@
       </c>
       <c r="L64" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M64" t="n">
-        <v>-58.3793</v>
+        <v>-58.433634</v>
       </c>
       <c r="N64" t="n">
-        <v>-34.636079</v>
+        <v>-34.595018</v>
       </c>
       <c r="O64" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P64" t="inlineStr">
-        <is>
-          <t>Capital Sur</t>
-        </is>
-      </c>
-    </row>
-    <row r="65">
-      <c r="A65" t="inlineStr">
-        <is>
-          <t>-535</t>
-        </is>
-      </c>
-      <c r="B65" t="inlineStr">
-        <is>
-          <t>7/28/2025</t>
-        </is>
-      </c>
-      <c r="C65" t="inlineStr">
-        <is>
-          <t>Jose Aaron Salmun Feijoo 363</t>
-        </is>
-      </c>
-      <c r="D65" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="E65" t="inlineStr">
-        <is>
-          <t>ICD30238810</t>
-        </is>
-      </c>
-      <c r="F65" t="inlineStr">
-        <is>
-          <t>NEW</t>
-        </is>
-      </c>
-      <c r="G65" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H65" t="inlineStr">
-        <is>
-          <t>Colocar prfv pasante</t>
-        </is>
-      </c>
-      <c r="I65" t="n">
-        <v>0</v>
-      </c>
-      <c r="J65" t="inlineStr">
-        <is>
-          <t>Cambio</t>
-        </is>
-      </c>
-      <c r="K65" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L65" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
-      <c r="M65" t="n">
-        <v>-58.379294</v>
-      </c>
-      <c r="N65" t="n">
-        <v>-34.636313</v>
-      </c>
-      <c r="O65" t="inlineStr">
-        <is>
-          <t>San Telmo</t>
-        </is>
-      </c>
-      <c r="P65" t="inlineStr">
-        <is>
-          <t>Capital Sur</t>
-        </is>
-      </c>
-    </row>
-    <row r="66">
-      <c r="A66" t="inlineStr">
-        <is>
-          <t>-538</t>
-        </is>
-      </c>
-      <c r="B66" t="inlineStr">
-        <is>
-          <t>7/31/2025</t>
-        </is>
-      </c>
-      <c r="C66" t="inlineStr">
-        <is>
-          <t>Malabia 964</t>
-        </is>
-      </c>
-      <c r="D66" t="inlineStr">
-        <is>
-          <t>15</t>
-        </is>
-      </c>
-      <c r="E66" t="inlineStr">
-        <is>
-          <t>808609237</t>
-        </is>
-      </c>
-      <c r="F66" t="inlineStr">
-        <is>
-          <t>NEW</t>
-        </is>
-      </c>
-      <c r="G66" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H66" t="inlineStr">
-        <is>
-          <t>Cambiar poste mal estado por PRFV</t>
-        </is>
-      </c>
-      <c r="I66" t="n">
-        <v>1</v>
-      </c>
-      <c r="J66" t="inlineStr">
-        <is>
-          <t>Cambio</t>
-        </is>
-      </c>
-      <c r="K66" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L66" t="inlineStr">
-        <is>
-          <t>Poste</t>
-        </is>
-      </c>
-      <c r="M66" t="n">
-        <v>-58.433634</v>
-      </c>
-      <c r="N66" t="n">
-        <v>-34.595018</v>
-      </c>
-      <c r="O66" t="inlineStr">
-        <is>
-          <t>Palermo</t>
-        </is>
-      </c>
-      <c r="P66" t="inlineStr">
         <is>
           <t>Capital Sur</t>
         </is>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-08-02 07:27:14)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_NEW.xlsx
+++ b/mapa_interactivo_NEW.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P64"/>
+  <dimension ref="A1:P67"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3010,17 +3010,17 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>5826</t>
+          <t>-406</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>5/19/2025</t>
+          <t>5/8/2025</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>ALBARELLOS AV. 3180</t>
+          <t>Olof palme 4144</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
@@ -3030,7 +3030,7 @@
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>806926466</t>
+          <t>805791925</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
@@ -3045,7 +3045,7 @@
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>Columna (metal) inclinada</t>
+          <t>Tensar 2 riendas a pique columna 168</t>
         </is>
       </c>
       <c r="I35" t="n">
@@ -3053,7 +3053,7 @@
       </c>
       <c r="J35" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Tensor</t>
         </is>
       </c>
       <c r="K35" t="inlineStr">
@@ -3067,14 +3067,14 @@
         </is>
       </c>
       <c r="M35" t="n">
-        <v>-58.513552</v>
+        <v>-58.488252</v>
       </c>
       <c r="N35" t="n">
-        <v>-34.579829</v>
+        <v>-34.553391</v>
       </c>
       <c r="O35" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P35" t="inlineStr">
@@ -3086,7 +3086,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>5825</t>
+          <t>5826</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
@@ -3096,7 +3096,7 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>PAZ, GRAL. AV. 5602</t>
+          <t>ALBARELLOS AV. 3180</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
@@ -3106,7 +3106,7 @@
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>806926472</t>
+          <t>806926466</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
@@ -3121,7 +3121,7 @@
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>reparar rienda cortada - ver foto no es la misma que albarellos</t>
+          <t>Columna (metal) inclinada</t>
         </is>
       </c>
       <c r="I36" t="n">
@@ -3129,7 +3129,7 @@
       </c>
       <c r="J36" t="inlineStr">
         <is>
-          <t>Tensor</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K36" t="inlineStr">
@@ -3143,10 +3143,10 @@
         </is>
       </c>
       <c r="M36" t="n">
-        <v>-58.513685</v>
+        <v>-58.513552</v>
       </c>
       <c r="N36" t="n">
-        <v>-34.579838</v>
+        <v>-34.579829</v>
       </c>
       <c r="O36" t="inlineStr">
         <is>
@@ -3162,17 +3162,17 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>5875</t>
+          <t>5825</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>5/27/2025</t>
+          <t>5/19/2025</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>MONROE 4096</t>
+          <t>PAZ, GRAL. AV. 5602</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
@@ -3182,7 +3182,7 @@
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>806975680</t>
+          <t>806926472</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
@@ -3197,7 +3197,7 @@
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>reparar rienda cortada - ver foto no es la misma que albarellos</t>
         </is>
       </c>
       <c r="I37" t="n">
@@ -3205,7 +3205,7 @@
       </c>
       <c r="J37" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Tensor</t>
         </is>
       </c>
       <c r="K37" t="inlineStr">
@@ -3215,18 +3215,18 @@
       </c>
       <c r="L37" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M37" t="n">
-        <v>-58.476106</v>
+        <v>-58.513685</v>
       </c>
       <c r="N37" t="n">
-        <v>-34.568373</v>
+        <v>-34.579838</v>
       </c>
       <c r="O37" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P37" t="inlineStr">
@@ -3238,27 +3238,27 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>807044192</t>
+          <t>5875</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>5/29/2025</t>
+          <t>5/27/2025</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>O'Higgins 4379</t>
+          <t>MONROE 4096</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>807044192</t>
+          <t>806975680</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
@@ -3273,7 +3273,7 @@
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t xml:space="preserve">Poste </t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I38" t="n">
@@ -3281,7 +3281,7 @@
       </c>
       <c r="J38" t="inlineStr">
         <is>
-          <t>Desmonte</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K38" t="inlineStr">
@@ -3291,18 +3291,18 @@
       </c>
       <c r="L38" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M38" t="n">
-        <v>-58.468425</v>
+        <v>-58.476106</v>
       </c>
       <c r="N38" t="n">
-        <v>-34.54124</v>
+        <v>-34.568373</v>
       </c>
       <c r="O38" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P38" t="inlineStr">
@@ -3314,27 +3314,27 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>6020</t>
+          <t>807044192</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>6/5/2025</t>
+          <t>5/29/2025</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>RAVIGNANI, EMILIO, DR. 2036</t>
+          <t>O'Higgins 4379</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>807215465</t>
+          <t>807044192</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
@@ -3349,7 +3349,7 @@
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t xml:space="preserve">Poste </t>
         </is>
       </c>
       <c r="I39" t="n">
@@ -3357,7 +3357,7 @@
       </c>
       <c r="J39" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Desmonte</t>
         </is>
       </c>
       <c r="K39" t="inlineStr">
@@ -3367,50 +3367,50 @@
       </c>
       <c r="L39" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M39" t="n">
-        <v>-58.436298</v>
+        <v>-58.468425</v>
       </c>
       <c r="N39" t="n">
-        <v>-34.578972</v>
+        <v>-34.54124</v>
       </c>
       <c r="O39" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P39" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>6144</t>
+          <t>6020</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>6/11/2025</t>
+          <t>6/5/2025</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>TURIN 2990</t>
+          <t>RAVIGNANI, EMILIO, DR. 2036</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>807458282</t>
+          <t>807215465</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
@@ -3447,26 +3447,26 @@
         </is>
       </c>
       <c r="M40" t="n">
-        <v>-58.480925</v>
+        <v>-58.436298</v>
       </c>
       <c r="N40" t="n">
-        <v>-34.585471</v>
+        <v>-34.578972</v>
       </c>
       <c r="O40" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P40" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>6143</t>
+          <t>6144</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
@@ -3476,7 +3476,7 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>SOLANO LOPEZ, F., MARISCAL 2845</t>
+          <t>TURIN 2990</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
@@ -3486,7 +3486,7 @@
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>807458296</t>
+          <t>807458282</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
@@ -3523,10 +3523,10 @@
         </is>
       </c>
       <c r="M41" t="n">
-        <v>-58.495071</v>
+        <v>-58.480925</v>
       </c>
       <c r="N41" t="n">
-        <v>-34.593122</v>
+        <v>-34.585471</v>
       </c>
       <c r="O41" t="inlineStr">
         <is>
@@ -3542,7 +3542,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>6141</t>
+          <t>6143</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
@@ -3552,17 +3552,17 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>EL PAMPERO 2618</t>
+          <t>SOLANO LOPEZ, F., MARISCAL 2845</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>807458310</t>
+          <t>807458296</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
@@ -3599,10 +3599,10 @@
         </is>
       </c>
       <c r="M42" t="n">
-        <v>-58.481942</v>
+        <v>-58.495071</v>
       </c>
       <c r="N42" t="n">
-        <v>-34.602989</v>
+        <v>-34.593122</v>
       </c>
       <c r="O42" t="inlineStr">
         <is>
@@ -3618,17 +3618,17 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>-478</t>
+          <t>6141</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>6/15/2025</t>
+          <t>6/11/2025</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Chivilcoy 4875</t>
+          <t>EL PAMPERO 2618</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
@@ -3638,7 +3638,7 @@
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>807508509</t>
+          <t>807458310</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
@@ -3653,7 +3653,7 @@
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>Poste podrido</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I43" t="n">
@@ -3671,14 +3671,14 @@
       </c>
       <c r="L43" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M43" t="n">
-        <v>-58.517389</v>
+        <v>-58.481942</v>
       </c>
       <c r="N43" t="n">
-        <v>-34.593541</v>
+        <v>-34.602989</v>
       </c>
       <c r="O43" t="inlineStr">
         <is>
@@ -3694,27 +3694,27 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>6171</t>
+          <t>-478</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>6/18/2025</t>
+          <t>6/15/2025</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>CABELLO 3486</t>
+          <t>Chivilcoy 4875</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>807658640</t>
+          <t>807508509</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
@@ -3729,7 +3729,7 @@
       </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t>Columna inclinada evaluar con inspector un corrimiento</t>
+          <t>Poste podrido</t>
         </is>
       </c>
       <c r="I44" t="n">
@@ -3747,40 +3747,40 @@
       </c>
       <c r="L44" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M44" t="n">
-        <v>-58.409579</v>
+        <v>-58.517389</v>
       </c>
       <c r="N44" t="n">
-        <v>-34.581134</v>
+        <v>-34.593541</v>
       </c>
       <c r="O44" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P44" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>6230</t>
+          <t>6171</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>6/24/2025</t>
+          <t>6/18/2025</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Santa maria de oro	2722</t>
+          <t>CABELLO 3486</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
@@ -3790,7 +3790,7 @@
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>807763066</t>
+          <t>807658640</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
@@ -3805,7 +3805,7 @@
       </c>
       <c r="H45" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Columna inclinada evaluar con inspector un corrimiento</t>
         </is>
       </c>
       <c r="I45" t="n">
@@ -3827,10 +3827,10 @@
         </is>
       </c>
       <c r="M45" t="n">
-        <v>-58.422315</v>
+        <v>-58.409579</v>
       </c>
       <c r="N45" t="n">
-        <v>-34.576988</v>
+        <v>-34.581134</v>
       </c>
       <c r="O45" t="inlineStr">
         <is>
@@ -3846,7 +3846,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>6231</t>
+          <t>6230</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
@@ -3856,7 +3856,7 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Ciudad de la Paz 275</t>
+          <t>Santa maria de oro	2722</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
@@ -3866,7 +3866,7 @@
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>807763070</t>
+          <t>807763066</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
@@ -3881,7 +3881,7 @@
       </c>
       <c r="H46" t="inlineStr">
         <is>
-          <t>Aplomar o cambiar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I46" t="n">
@@ -3899,14 +3899,14 @@
       </c>
       <c r="L46" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M46" t="n">
-        <v>-58.441049</v>
+        <v>-58.422315</v>
       </c>
       <c r="N46" t="n">
-        <v>-34.574625</v>
+        <v>-34.576988</v>
       </c>
       <c r="O46" t="inlineStr">
         <is>
@@ -3922,7 +3922,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>6235</t>
+          <t>6231</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
@@ -3932,17 +3932,17 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>HUERGO 389</t>
+          <t>Ciudad de la Paz 275</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>807763078</t>
+          <t>807763070</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
@@ -3957,7 +3957,7 @@
       </c>
       <c r="H47" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Aplomar o cambiar</t>
         </is>
       </c>
       <c r="I47" t="n">
@@ -3975,14 +3975,14 @@
       </c>
       <c r="L47" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M47" t="n">
-        <v>-58.432722</v>
+        <v>-58.441049</v>
       </c>
       <c r="N47" t="n">
-        <v>-34.572371</v>
+        <v>-34.574625</v>
       </c>
       <c r="O47" t="inlineStr">
         <is>
@@ -3998,27 +3998,27 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>6295</t>
+          <t>6235</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>6/30/2025</t>
+          <t>6/24/2025</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>SOLER 6017</t>
+          <t>HUERGO 389</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>807851636</t>
+          <t>807763078</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
@@ -4055,10 +4055,10 @@
         </is>
       </c>
       <c r="M48" t="n">
-        <v>-58.436808</v>
+        <v>-58.432722</v>
       </c>
       <c r="N48" t="n">
-        <v>-34.577464</v>
+        <v>-34.572371</v>
       </c>
       <c r="O48" t="inlineStr">
         <is>
@@ -4074,17 +4074,17 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>6332</t>
+          <t>6295</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>7/3/2025</t>
+          <t>6/30/2025</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>ARAOZ 2560</t>
+          <t>SOLER 6017</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
@@ -4094,7 +4094,7 @@
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>807965818</t>
+          <t>807851636</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
@@ -4131,10 +4131,10 @@
         </is>
       </c>
       <c r="M49" t="n">
-        <v>-58.414507</v>
+        <v>-58.436808</v>
       </c>
       <c r="N49" t="n">
-        <v>-34.585377</v>
+        <v>-34.577464</v>
       </c>
       <c r="O49" t="inlineStr">
         <is>
@@ -4150,27 +4150,27 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>6363</t>
+          <t>6332</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>7/8/2025</t>
+          <t>7/3/2025</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>MOLDES 3730</t>
+          <t>ARAOZ 2560</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>808099415</t>
+          <t>807965818</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
@@ -4185,7 +4185,7 @@
       </c>
       <c r="H50" t="inlineStr">
         <is>
-          <t>Poste inclinado</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I50" t="n">
@@ -4193,7 +4193,7 @@
       </c>
       <c r="J50" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K50" t="inlineStr">
@@ -4203,50 +4203,50 @@
       </c>
       <c r="L50" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M50" t="n">
-        <v>-58.47192</v>
+        <v>-58.414507</v>
       </c>
       <c r="N50" t="n">
-        <v>-34.549398</v>
+        <v>-34.585377</v>
       </c>
       <c r="O50" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P50" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>-503</t>
+          <t>6363</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>7/10/2025</t>
+          <t>7/8/2025</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Salguero 842</t>
+          <t>MOLDES 3730</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>808148673</t>
+          <t>808099415</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
@@ -4261,7 +4261,7 @@
       </c>
       <c r="H51" t="inlineStr">
         <is>
-          <t>Cambiar columna picada en la base</t>
+          <t>Poste inclinado</t>
         </is>
       </c>
       <c r="I51" t="n">
@@ -4269,7 +4269,7 @@
       </c>
       <c r="J51" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K51" t="inlineStr">
@@ -4279,30 +4279,30 @@
       </c>
       <c r="L51" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M51" t="n">
-        <v>-58.419166</v>
+        <v>-58.47192</v>
       </c>
       <c r="N51" t="n">
-        <v>-34.600265</v>
+        <v>-34.549398</v>
       </c>
       <c r="O51" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P51" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>6506</t>
+          <t>-503</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
@@ -4312,17 +4312,17 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>Ohiggins 1611</t>
+          <t>Salguero 842</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>808148679</t>
+          <t>808148673</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
@@ -4337,7 +4337,7 @@
       </c>
       <c r="H52" t="inlineStr">
         <is>
-          <t>Columna podrida en la base</t>
+          <t>Cambiar columna picada en la base</t>
         </is>
       </c>
       <c r="I52" t="n">
@@ -4350,7 +4350,7 @@
       </c>
       <c r="K52" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L52" t="inlineStr">
@@ -4359,46 +4359,46 @@
         </is>
       </c>
       <c r="M52" t="n">
-        <v>-58.448993</v>
+        <v>-58.419166</v>
       </c>
       <c r="N52" t="n">
-        <v>-34.564383</v>
+        <v>-34.600265</v>
       </c>
       <c r="O52" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P52" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>6437</t>
+          <t>6506</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>7/17/2025</t>
+          <t>7/10/2025</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>MILLER 4590</t>
+          <t>Ohiggins 1611</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>808400306</t>
+          <t>808148679</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
@@ -4413,7 +4413,7 @@
       </c>
       <c r="H53" t="inlineStr">
         <is>
-          <t>Columna corroida</t>
+          <t>Columna podrida en la base</t>
         </is>
       </c>
       <c r="I53" t="n">
@@ -4426,7 +4426,7 @@
       </c>
       <c r="K53" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L53" t="inlineStr">
@@ -4435,14 +4435,14 @@
         </is>
       </c>
       <c r="M53" t="n">
-        <v>-58.495482</v>
+        <v>-58.448993</v>
       </c>
       <c r="N53" t="n">
-        <v>-34.552614</v>
+        <v>-34.564383</v>
       </c>
       <c r="O53" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P53" t="inlineStr">
@@ -4454,7 +4454,7 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>6447</t>
+          <t>6437</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
@@ -4464,17 +4464,17 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>CIUDAD DE LA PAZ 1535</t>
+          <t>MILLER 4590</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>808400333</t>
+          <t>808400306</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
@@ -4489,7 +4489,7 @@
       </c>
       <c r="H54" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Columna corroida</t>
         </is>
       </c>
       <c r="I54" t="n">
@@ -4511,14 +4511,14 @@
         </is>
       </c>
       <c r="M54" t="n">
-        <v>-58.453124</v>
+        <v>-58.495482</v>
       </c>
       <c r="N54" t="n">
-        <v>-34.567382</v>
+        <v>-34.552614</v>
       </c>
       <c r="O54" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P54" t="inlineStr">
@@ -4530,7 +4530,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>-519</t>
+          <t>6447</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
@@ -4540,17 +4540,17 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>Vilela 2687</t>
+          <t>CIUDAD DE LA PAZ 1535</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>808400334</t>
+          <t>808400333</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
@@ -4565,7 +4565,7 @@
       </c>
       <c r="H55" t="inlineStr">
         <is>
-          <t>CAmbiar columna 114 picada en base</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I55" t="n">
@@ -4587,14 +4587,14 @@
         </is>
       </c>
       <c r="M55" t="n">
-        <v>-58.472968</v>
+        <v>-58.453124</v>
       </c>
       <c r="N55" t="n">
-        <v>-34.546898</v>
+        <v>-34.567382</v>
       </c>
       <c r="O55" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P55" t="inlineStr">
@@ -4606,7 +4606,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>6538</t>
+          <t>-519</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
@@ -4616,7 +4616,7 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>Pedraza Manuela 4101</t>
+          <t>Vilela 2687</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
@@ -4626,7 +4626,7 @@
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>808400353</t>
+          <t>808400334</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
@@ -4641,7 +4641,7 @@
       </c>
       <c r="H56" t="inlineStr">
         <is>
-          <t xml:space="preserve">Podrida en la base </t>
+          <t>CAmbiar columna 114 picada en base</t>
         </is>
       </c>
       <c r="I56" t="n">
@@ -4663,10 +4663,10 @@
         </is>
       </c>
       <c r="M56" t="n">
-        <v>-58.481569</v>
+        <v>-58.472968</v>
       </c>
       <c r="N56" t="n">
-        <v>-34.559853</v>
+        <v>-34.546898</v>
       </c>
       <c r="O56" t="inlineStr">
         <is>
@@ -4682,27 +4682,27 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>-525</t>
+          <t>6538</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>7/22/2025</t>
+          <t>7/17/2025</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>Zabala 3567</t>
+          <t>Pedraza Manuela 4101</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>808480549</t>
+          <t>808400353</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
@@ -4717,7 +4717,7 @@
       </c>
       <c r="H57" t="inlineStr">
         <is>
-          <t>Corroida en base para recambio</t>
+          <t xml:space="preserve">Podrida en la base </t>
         </is>
       </c>
       <c r="I57" t="n">
@@ -4739,14 +4739,14 @@
         </is>
       </c>
       <c r="M57" t="n">
-        <v>-58.457492</v>
+        <v>-58.481569</v>
       </c>
       <c r="N57" t="n">
-        <v>-34.579336</v>
+        <v>-34.559853</v>
       </c>
       <c r="O57" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P57" t="inlineStr">
@@ -4758,27 +4758,27 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>6484</t>
+          <t>-525</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>7/24/2025</t>
+          <t>7/22/2025</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>URIARTE 2396</t>
+          <t>Zabala 3567</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>808509373</t>
+          <t>808480549</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
@@ -4793,7 +4793,7 @@
       </c>
       <c r="H58" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Corroida en base para recambio</t>
         </is>
       </c>
       <c r="I58" t="n">
@@ -4815,46 +4815,46 @@
         </is>
       </c>
       <c r="M58" t="n">
-        <v>-58.423934</v>
+        <v>-58.457492</v>
       </c>
       <c r="N58" t="n">
-        <v>-34.581562</v>
+        <v>-34.579336</v>
       </c>
       <c r="O58" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P58" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>6502</t>
+          <t>6484</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>7/25/2025</t>
+          <t>7/24/2025</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>CIUDAD DE LA PAZ 1511</t>
+          <t>URIARTE 2396</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>808571972</t>
+          <t>808509373</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
@@ -4891,26 +4891,26 @@
         </is>
       </c>
       <c r="M59" t="n">
-        <v>-58.452907</v>
+        <v>-58.423934</v>
       </c>
       <c r="N59" t="n">
-        <v>-34.567508</v>
+        <v>-34.581562</v>
       </c>
       <c r="O59" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P59" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>6504</t>
+          <t>6502</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
@@ -4920,7 +4920,7 @@
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>CIUDAD DE LA PAZ 1278</t>
+          <t>CIUDAD DE LA PAZ 1511</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
@@ -4930,7 +4930,7 @@
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>808571974</t>
+          <t>808571972</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
@@ -4945,7 +4945,7 @@
       </c>
       <c r="H60" t="inlineStr">
         <is>
-          <t>Inclinada</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I60" t="n">
@@ -4967,10 +4967,10 @@
         </is>
       </c>
       <c r="M60" t="n">
-        <v>-58.450753</v>
+        <v>-58.452907</v>
       </c>
       <c r="N60" t="n">
-        <v>-34.5688</v>
+        <v>-34.567508</v>
       </c>
       <c r="O60" t="inlineStr">
         <is>
@@ -4986,27 +4986,27 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>6512</t>
+          <t>6504</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>7/28/2025</t>
+          <t>7/25/2025</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>GASCON 1195</t>
+          <t>CIUDAD DE LA PAZ 1278</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>808571975</t>
+          <t>808571974</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
@@ -5021,7 +5021,7 @@
       </c>
       <c r="H61" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Inclinada</t>
         </is>
       </c>
       <c r="I61" t="n">
@@ -5043,26 +5043,26 @@
         </is>
       </c>
       <c r="M61" t="n">
-        <v>-58.423127</v>
+        <v>-58.450753</v>
       </c>
       <c r="N61" t="n">
-        <v>-34.596476</v>
+        <v>-34.5688</v>
       </c>
       <c r="O61" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P61" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>6513</t>
+          <t>6512</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
@@ -5072,7 +5072,7 @@
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>DORREGO 1925</t>
+          <t>GASCON 1195</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
@@ -5082,7 +5082,7 @@
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>808571976</t>
+          <t>808571975</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
@@ -5119,10 +5119,10 @@
         </is>
       </c>
       <c r="M62" t="n">
-        <v>-58.441281</v>
+        <v>-58.423127</v>
       </c>
       <c r="N62" t="n">
-        <v>-34.579867</v>
+        <v>-34.596476</v>
       </c>
       <c r="O62" t="inlineStr">
         <is>
@@ -5138,7 +5138,7 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>6519</t>
+          <t>6513</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
@@ -5148,7 +5148,7 @@
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>SALGUERO, JERONIMO 2874</t>
+          <t>DORREGO 1925</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
@@ -5158,7 +5158,7 @@
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>808571977</t>
+          <t>808571976</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
@@ -5173,7 +5173,7 @@
       </c>
       <c r="H63" t="inlineStr">
         <is>
-          <t>Reparar rienda</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I63" t="n">
@@ -5181,7 +5181,7 @@
       </c>
       <c r="J63" t="inlineStr">
         <is>
-          <t>Tensor</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K63" t="inlineStr">
@@ -5191,14 +5191,14 @@
       </c>
       <c r="L63" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M63" t="n">
-        <v>-58.407256</v>
+        <v>-58.441281</v>
       </c>
       <c r="N63" t="n">
-        <v>-34.578976</v>
+        <v>-34.579867</v>
       </c>
       <c r="O63" t="inlineStr">
         <is>
@@ -5214,27 +5214,27 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>-538</t>
+          <t>6519</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>7/31/2025</t>
+          <t>7/28/2025</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>Malabia 964</t>
+          <t>SALGUERO, JERONIMO 2874</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>808609237</t>
+          <t>808571977</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
@@ -5249,7 +5249,7 @@
       </c>
       <c r="H64" t="inlineStr">
         <is>
-          <t>Cambiar poste mal estado por PRFV</t>
+          <t>Reparar rienda</t>
         </is>
       </c>
       <c r="I64" t="n">
@@ -5257,33 +5257,257 @@
       </c>
       <c r="J64" t="inlineStr">
         <is>
+          <t>Tensor</t>
+        </is>
+      </c>
+      <c r="K64" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L64" t="inlineStr">
+        <is>
+          <t>Terminal</t>
+        </is>
+      </c>
+      <c r="M64" t="n">
+        <v>-58.407256</v>
+      </c>
+      <c r="N64" t="n">
+        <v>-34.578976</v>
+      </c>
+      <c r="O64" t="inlineStr">
+        <is>
+          <t>Palermo</t>
+        </is>
+      </c>
+      <c r="P64" t="inlineStr">
+        <is>
+          <t>Capital Sur</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>-536</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>7/29/2025</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>Olof palme 4142</t>
+        </is>
+      </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="E65" t="inlineStr">
+        <is>
+          <t xml:space="preserve">ICD30249764 </t>
+        </is>
+      </c>
+      <c r="F65" t="inlineStr">
+        <is>
+          <t>NEW</t>
+        </is>
+      </c>
+      <c r="G65" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H65" t="inlineStr">
+        <is>
+          <t>Aplomar o desmontar poste</t>
+        </is>
+      </c>
+      <c r="I65" t="n">
+        <v>1</v>
+      </c>
+      <c r="J65" t="inlineStr">
+        <is>
+          <t>Desmonte</t>
+        </is>
+      </c>
+      <c r="K65" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L65" t="inlineStr">
+        <is>
+          <t>Poste</t>
+        </is>
+      </c>
+      <c r="M65" t="n">
+        <v>-58.488239</v>
+      </c>
+      <c r="N65" t="n">
+        <v>-34.55341</v>
+      </c>
+      <c r="O65" t="inlineStr">
+        <is>
+          <t>Saavedra</t>
+        </is>
+      </c>
+      <c r="P65" t="inlineStr">
+        <is>
+          <t>Capital Norte</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>-538</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>7/31/2025</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>Malabia 964</t>
+        </is>
+      </c>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="E66" t="inlineStr">
+        <is>
+          <t>808609237</t>
+        </is>
+      </c>
+      <c r="F66" t="inlineStr">
+        <is>
+          <t>NEW</t>
+        </is>
+      </c>
+      <c r="G66" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H66" t="inlineStr">
+        <is>
+          <t>Cambiar poste mal estado por PRFV</t>
+        </is>
+      </c>
+      <c r="I66" t="n">
+        <v>1</v>
+      </c>
+      <c r="J66" t="inlineStr">
+        <is>
           <t>Cambio</t>
         </is>
       </c>
-      <c r="K64" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L64" t="inlineStr">
+      <c r="K66" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L66" t="inlineStr">
         <is>
           <t>Poste</t>
         </is>
       </c>
-      <c r="M64" t="n">
+      <c r="M66" t="n">
         <v>-58.433634</v>
       </c>
-      <c r="N64" t="n">
+      <c r="N66" t="n">
         <v>-34.595018</v>
       </c>
-      <c r="O64" t="inlineStr">
+      <c r="O66" t="inlineStr">
         <is>
           <t>Palermo</t>
         </is>
       </c>
-      <c r="P64" t="inlineStr">
+      <c r="P66" t="inlineStr">
         <is>
           <t>Capital Sur</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>-543</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>8/1/2025</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>Pedro Ignacio Rivera 3258</t>
+        </is>
+      </c>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>13</t>
+        </is>
+      </c>
+      <c r="E67" t="inlineStr"/>
+      <c r="F67" t="inlineStr">
+        <is>
+          <t>NEW</t>
+        </is>
+      </c>
+      <c r="G67" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H67" t="inlineStr">
+        <is>
+          <t>Desmontar poste en desuso</t>
+        </is>
+      </c>
+      <c r="I67" t="n">
+        <v>1</v>
+      </c>
+      <c r="J67" t="inlineStr">
+        <is>
+          <t>Desmonte</t>
+        </is>
+      </c>
+      <c r="K67" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L67" t="inlineStr">
+        <is>
+          <t>Poste</t>
+        </is>
+      </c>
+      <c r="M67" t="n">
+        <v>-58.46967</v>
+      </c>
+      <c r="N67" t="n">
+        <v>-34.561676</v>
+      </c>
+      <c r="O67" t="inlineStr">
+        <is>
+          <t>Colegiales</t>
+        </is>
+      </c>
+      <c r="P67" t="inlineStr">
+        <is>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-08-04 13:06:54)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_NEW.xlsx
+++ b/mapa_interactivo_NEW.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P67"/>
+  <dimension ref="A1:P62"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1266,27 +1266,27 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>5037</t>
+          <t>5053</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>3/7/2025</t>
+          <t>3/11/2025</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Monroe 3605</t>
+          <t>MENDOZA 1153</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>803825082</t>
+          <t>803969314</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
@@ -1301,7 +1301,7 @@
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>Columna inclinada</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="I12" t="n">
@@ -1309,7 +1309,7 @@
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K12" t="inlineStr">
@@ -1319,18 +1319,18 @@
       </c>
       <c r="L12" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M12" t="n">
-        <v>-58.471774</v>
+        <v>-58.44463</v>
       </c>
       <c r="N12" t="n">
-        <v>-34.565411</v>
+        <v>-34.553354</v>
       </c>
       <c r="O12" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P12" t="inlineStr">
@@ -1342,27 +1342,27 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>5053</t>
+          <t>6071</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>3/11/2025</t>
+          <t>3/17/2025</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>MENDOZA 1153</t>
+          <t>OSORIO 4994</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>803969314</t>
+          <t>804053324</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
@@ -1375,11 +1375,7 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H13" t="inlineStr">
-        <is>
-          <t>Poste</t>
-        </is>
-      </c>
+      <c r="H13" t="inlineStr"/>
       <c r="I13" t="n">
         <v>0</v>
       </c>
@@ -1395,18 +1391,18 @@
       </c>
       <c r="L13" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M13" t="n">
-        <v>-58.44463</v>
+        <v>-58.466241</v>
       </c>
       <c r="N13" t="n">
-        <v>-34.553354</v>
+        <v>-34.595741</v>
       </c>
       <c r="O13" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P13" t="inlineStr">
@@ -1418,27 +1414,27 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>6071</t>
+          <t>3348</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>3/17/2025</t>
+          <t>3/27/2025</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>OSORIO 4994</t>
+          <t>ESTOMBA 2626</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>804053324</t>
+          <t>804309704</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
@@ -1451,13 +1447,17 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H14" t="inlineStr"/>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>Picada</t>
+        </is>
+      </c>
       <c r="I14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Desmonte</t>
         </is>
       </c>
       <c r="K14" t="inlineStr">
@@ -1471,14 +1471,14 @@
         </is>
       </c>
       <c r="M14" t="n">
-        <v>-58.466241</v>
+        <v>-58.47538</v>
       </c>
       <c r="N14" t="n">
-        <v>-34.595741</v>
+        <v>-34.566015</v>
       </c>
       <c r="O14" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P14" t="inlineStr">
@@ -1490,27 +1490,27 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>3348</t>
+          <t>-312</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>3/27/2025</t>
+          <t>3/29/2025</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>ESTOMBA 2626</t>
+          <t>MATIENZO BENJAMIN /ALT/ 1831</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>804309704</t>
+          <t>804333522</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
@@ -1525,20 +1525,20 @@
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Retirar columna ya traspasaron el nodo</t>
         </is>
       </c>
       <c r="I15" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>Desmonte</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L15" t="inlineStr">
@@ -1547,46 +1547,46 @@
         </is>
       </c>
       <c r="M15" t="n">
-        <v>-58.47538</v>
+        <v>-58.434835</v>
       </c>
       <c r="N15" t="n">
-        <v>-34.566015</v>
+        <v>-34.569129</v>
       </c>
       <c r="O15" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P15" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>-312</t>
+          <t>3430</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>3/29/2025</t>
+          <t>4/1/2025</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>MATIENZO BENJAMIN /ALT/ 1831</t>
+          <t>MONROE 3838</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>804333522</t>
+          <t>804468442</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
@@ -1601,68 +1601,68 @@
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>Retirar columna ya traspasaron el nodo</t>
+          <t>Reparar rienda</t>
         </is>
       </c>
       <c r="I16" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Tensor</t>
         </is>
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L16" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M16" t="n">
-        <v>-58.434835</v>
+        <v>-58.473659</v>
       </c>
       <c r="N16" t="n">
-        <v>-34.569129</v>
+        <v>-34.566979</v>
       </c>
       <c r="O16" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P16" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>3430</t>
+          <t>5464</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>4/1/2025</t>
+          <t>4/4/2025</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>MONROE 3838</t>
+          <t>SUCRE, ANTONIO JOSE DE, MCAL. 3100</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>804468442</t>
+          <t>804497880</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
@@ -1677,7 +1677,7 @@
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>Reparar rienda</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I17" t="n">
@@ -1685,7 +1685,7 @@
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>Tensor</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K17" t="inlineStr">
@@ -1699,10 +1699,10 @@
         </is>
       </c>
       <c r="M17" t="n">
-        <v>-58.473659</v>
+        <v>-58.46161</v>
       </c>
       <c r="N17" t="n">
-        <v>-34.566979</v>
+        <v>-34.567849</v>
       </c>
       <c r="O17" t="inlineStr">
         <is>
@@ -1718,7 +1718,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>5464</t>
+          <t>5469</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -1728,17 +1728,17 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>SUCRE, ANTONIO JOSE DE, MCAL. 3100</t>
+          <t>ESTADO PLURINACIONAL DE BOLIVIA 5899</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>804497880</t>
+          <t>804497887</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
@@ -1753,7 +1753,7 @@
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Aplomar</t>
         </is>
       </c>
       <c r="I18" t="n">
@@ -1761,7 +1761,7 @@
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K18" t="inlineStr">
@@ -1775,14 +1775,14 @@
         </is>
       </c>
       <c r="M18" t="n">
-        <v>-58.46161</v>
+        <v>-58.507746</v>
       </c>
       <c r="N18" t="n">
-        <v>-34.567849</v>
+        <v>-34.574217</v>
       </c>
       <c r="O18" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P18" t="inlineStr">
@@ -1794,7 +1794,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>5469</t>
+          <t>5492</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -1804,7 +1804,7 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>ESTADO PLURINACIONAL DE BOLIVIA 5899</t>
+          <t>ESTADO PLURINACIONAL DE BOLIVIA 5920</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
@@ -1814,7 +1814,7 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>804497887</t>
+          <t>804498035</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
@@ -1829,7 +1829,7 @@
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>Aplomar</t>
+          <t>aplomar</t>
         </is>
       </c>
       <c r="I19" t="n">
@@ -1851,10 +1851,10 @@
         </is>
       </c>
       <c r="M19" t="n">
-        <v>-58.507746</v>
+        <v>-58.50751</v>
       </c>
       <c r="N19" t="n">
-        <v>-34.574217</v>
+        <v>-34.574543</v>
       </c>
       <c r="O19" t="inlineStr">
         <is>
@@ -1870,17 +1870,17 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>5492</t>
+          <t>5599</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>4/4/2025</t>
+          <t>4/15/2025</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>ESTADO PLURINACIONAL DE BOLIVIA 5920</t>
+          <t>ESTOMBA 4052</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
@@ -1890,7 +1890,7 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>804498035</t>
+          <t>804732246</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
@@ -1905,7 +1905,7 @@
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>aplomar</t>
+          <t>Columna PRFV quedo inclinada (la hicieron como estomba 4056)</t>
         </is>
       </c>
       <c r="I20" t="n">
@@ -1918,23 +1918,23 @@
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo TLC</t>
         </is>
       </c>
       <c r="L20" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M20" t="n">
-        <v>-58.50751</v>
+        <v>-58.485407</v>
       </c>
       <c r="N20" t="n">
-        <v>-34.574543</v>
+        <v>-34.552985</v>
       </c>
       <c r="O20" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P20" t="inlineStr">
@@ -1946,7 +1946,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>5599</t>
+          <t>5590</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -1956,17 +1956,17 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>ESTOMBA 4052</t>
+          <t>O'HIGGINS 2441</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>804732246</t>
+          <t>804732275</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
@@ -1981,7 +1981,7 @@
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>Columna PRFV quedo inclinada (la hicieron como estomba 4056)</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I21" t="n">
@@ -1989,12 +1989,12 @@
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>Nodo TLC</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L21" t="inlineStr">
@@ -2003,10 +2003,10 @@
         </is>
       </c>
       <c r="M21" t="n">
-        <v>-58.485407</v>
+        <v>-58.45573</v>
       </c>
       <c r="N21" t="n">
-        <v>-34.552985</v>
+        <v>-34.556576</v>
       </c>
       <c r="O21" t="inlineStr">
         <is>
@@ -2022,27 +2022,27 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>5590</t>
+          <t>804787368</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>4/15/2025</t>
+          <t>4/17/2025</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>O'HIGGINS 2441</t>
+          <t>San Blas 2591</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>804732275</t>
+          <t>804787368</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
@@ -2079,14 +2079,14 @@
         </is>
       </c>
       <c r="M22" t="n">
-        <v>-58.45573</v>
+        <v>-58.477427</v>
       </c>
       <c r="N22" t="n">
-        <v>-34.556576</v>
+        <v>-34.609261</v>
       </c>
       <c r="O22" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P22" t="inlineStr">
@@ -2098,27 +2098,27 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>804787368</t>
+          <t>5624</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>4/17/2025</t>
+          <t>4/22/2025</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>San Blas 2591</t>
+          <t>PINO, VIRREY DEL 3456</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>804787368</t>
+          <t>804876043</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
@@ -2133,7 +2133,7 @@
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Desmonte de poste</t>
         </is>
       </c>
       <c r="I23" t="n">
@@ -2141,7 +2141,7 @@
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Desmonte</t>
         </is>
       </c>
       <c r="K23" t="inlineStr">
@@ -2151,18 +2151,18 @@
       </c>
       <c r="L23" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M23" t="n">
-        <v>-58.477427</v>
+        <v>-58.464354</v>
       </c>
       <c r="N23" t="n">
-        <v>-34.609261</v>
+        <v>-34.572486</v>
       </c>
       <c r="O23" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P23" t="inlineStr">
@@ -2174,17 +2174,17 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>5624</t>
+          <t>804922147</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>4/22/2025</t>
+          <t>4/24/2025</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>PINO, VIRREY DEL 3456</t>
+          <t>Av. Álvarez Thomas 1171</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
@@ -2194,7 +2194,7 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>804876043</t>
+          <t>804922147</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
@@ -2209,15 +2209,15 @@
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>Desmonte de poste</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I24" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J24" t="inlineStr">
         <is>
-          <t>Desmonte</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K24" t="inlineStr">
@@ -2227,14 +2227,14 @@
       </c>
       <c r="L24" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M24" t="n">
-        <v>-58.464354</v>
+        <v>-58.45793</v>
       </c>
       <c r="N24" t="n">
-        <v>-34.572486</v>
+        <v>-34.578334</v>
       </c>
       <c r="O24" t="inlineStr">
         <is>
@@ -2250,7 +2250,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>804922147</t>
+          <t>804922171</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -2260,7 +2260,7 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Av. Álvarez Thomas 1171</t>
+          <t>Virrey Arredondo 3581</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
@@ -2270,7 +2270,7 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>804922147</t>
+          <t>804922171</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
@@ -2285,15 +2285,15 @@
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Aplomar</t>
         </is>
       </c>
       <c r="I25" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K25" t="inlineStr">
@@ -2303,14 +2303,14 @@
       </c>
       <c r="L25" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M25" t="n">
-        <v>-58.45793</v>
+        <v>-58.459513</v>
       </c>
       <c r="N25" t="n">
-        <v>-34.578334</v>
+        <v>-34.578019</v>
       </c>
       <c r="O25" t="inlineStr">
         <is>
@@ -2326,7 +2326,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>804922171</t>
+          <t>5656</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -2336,17 +2336,17 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Virrey Arredondo 3581</t>
+          <t>ECHEVERRIA 5893</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>804922171</t>
+          <t>804922184</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
@@ -2361,7 +2361,7 @@
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>Aplomar</t>
+          <t>Poste con base quebrada</t>
         </is>
       </c>
       <c r="I26" t="n">
@@ -2369,7 +2369,7 @@
       </c>
       <c r="J26" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Desmonte</t>
         </is>
       </c>
       <c r="K26" t="inlineStr">
@@ -2379,18 +2379,18 @@
       </c>
       <c r="L26" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M26" t="n">
-        <v>-58.459513</v>
+        <v>-58.489627</v>
       </c>
       <c r="N26" t="n">
-        <v>-34.578019</v>
+        <v>-34.583761</v>
       </c>
       <c r="O26" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P26" t="inlineStr">
@@ -2402,27 +2402,27 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>5656</t>
+          <t>6173</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>4/24/2025</t>
+          <t>4/29/2025</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>ECHEVERRIA 5893</t>
+          <t>ARMENIA 2321</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>804922184</t>
+          <t>805507398</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
@@ -2437,7 +2437,7 @@
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>Poste con base quebrada</t>
+          <t>Picada volvio a entrar como caso 6325</t>
         </is>
       </c>
       <c r="I27" t="n">
@@ -2445,7 +2445,7 @@
       </c>
       <c r="J27" t="inlineStr">
         <is>
-          <t>Desmonte</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K27" t="inlineStr">
@@ -2455,50 +2455,50 @@
       </c>
       <c r="L27" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M27" t="n">
-        <v>-58.489627</v>
+        <v>-58.420549</v>
       </c>
       <c r="N27" t="n">
-        <v>-34.583761</v>
+        <v>-34.585103</v>
       </c>
       <c r="O27" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P27" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>6173</t>
+          <t>5715</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>4/29/2025</t>
+          <t>5/1/2025</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>ARMENIA 2321</t>
+          <t>CUENCA 4690</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>805507398</t>
+          <t>805579094</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
@@ -2513,7 +2513,7 @@
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>Picada volvio a entrar como caso 6325</t>
+          <t>Aplomar poste</t>
         </is>
       </c>
       <c r="I28" t="n">
@@ -2521,7 +2521,7 @@
       </c>
       <c r="J28" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K28" t="inlineStr">
@@ -2531,30 +2531,30 @@
       </c>
       <c r="L28" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M28" t="n">
-        <v>-58.420549</v>
+        <v>-58.506061</v>
       </c>
       <c r="N28" t="n">
-        <v>-34.585103</v>
+        <v>-34.588887</v>
       </c>
       <c r="O28" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P28" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>5715</t>
+          <t>5719</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -2564,7 +2564,7 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>CUENCA 4690</t>
+          <t>CABEZON, JOSE LEON 2440</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
@@ -2574,7 +2574,7 @@
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>805579094</t>
+          <t>805579157</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
@@ -2589,7 +2589,7 @@
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>Aplomar poste</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I29" t="n">
@@ -2597,7 +2597,7 @@
       </c>
       <c r="J29" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K29" t="inlineStr">
@@ -2607,14 +2607,14 @@
       </c>
       <c r="L29" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M29" t="n">
-        <v>-58.506061</v>
+        <v>-58.499967</v>
       </c>
       <c r="N29" t="n">
-        <v>-34.588887</v>
+        <v>-34.57974</v>
       </c>
       <c r="O29" t="inlineStr">
         <is>
@@ -2630,7 +2630,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>5719</t>
+          <t>6333</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -2640,17 +2640,17 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>CABEZON, JOSE LEON 2440</t>
+          <t>ORTEGA Y GASSET 1816</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>805579157</t>
+          <t>805655342</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
@@ -2687,36 +2687,36 @@
         </is>
       </c>
       <c r="M30" t="n">
-        <v>-58.499967</v>
+        <v>-58.432556</v>
       </c>
       <c r="N30" t="n">
-        <v>-34.57974</v>
+        <v>-34.570279</v>
       </c>
       <c r="O30" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P30" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>6333</t>
+          <t>805707165</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>5/1/2025</t>
+          <t>5/7/2025</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>ORTEGA Y GASSET 1816</t>
+          <t>Baez 793</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
@@ -2726,7 +2726,7 @@
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>805655342</t>
+          <t>805707165</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
@@ -2741,7 +2741,7 @@
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>DESMONTAR COLUMNA DE 7 MTS Y TRANSFERIR A COMUNITARIA</t>
         </is>
       </c>
       <c r="I31" t="n">
@@ -2759,14 +2759,14 @@
       </c>
       <c r="L31" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M31" t="n">
-        <v>-58.432556</v>
+        <v>-58.436165</v>
       </c>
       <c r="N31" t="n">
-        <v>-34.570279</v>
+        <v>-34.569081</v>
       </c>
       <c r="O31" t="inlineStr">
         <is>
@@ -2782,27 +2782,27 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>805707165</t>
+          <t>5847</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>5/7/2025</t>
+          <t>5/8/2025</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Baez 793</t>
+          <t>JURAMENTO 5321</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>805707165</t>
+          <t>805791839</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
@@ -2817,7 +2817,7 @@
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>DESMONTAR COLUMNA DE 7 MTS Y TRANSFERIR A COMUNITARIA</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I32" t="n">
@@ -2835,50 +2835,50 @@
       </c>
       <c r="L32" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M32" t="n">
-        <v>-58.436165</v>
+        <v>-58.485193</v>
       </c>
       <c r="N32" t="n">
-        <v>-34.569081</v>
+        <v>-34.579621</v>
       </c>
       <c r="O32" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P32" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>5847</t>
+          <t>232</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>5/8/2025</t>
+          <t>5/9/2025</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>JURAMENTO 5321</t>
+          <t>Gorostiaga 2286</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>805791839</t>
+          <t>805791858</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
@@ -2915,46 +2915,46 @@
         </is>
       </c>
       <c r="M33" t="n">
-        <v>-58.485193</v>
+        <v>-58.441563</v>
       </c>
       <c r="N33" t="n">
-        <v>-34.579621</v>
+        <v>-34.569743</v>
       </c>
       <c r="O33" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P33" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>232</t>
+          <t>-406</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>5/9/2025</t>
+          <t>5/8/2025</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Gorostiaga 2286</t>
+          <t>Olof palme 4144</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>805791858</t>
+          <t>805791925</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
@@ -2969,7 +2969,7 @@
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Tensar 2 riendas a pique columna 168</t>
         </is>
       </c>
       <c r="I34" t="n">
@@ -2977,7 +2977,7 @@
       </c>
       <c r="J34" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Tensor</t>
         </is>
       </c>
       <c r="K34" t="inlineStr">
@@ -2987,40 +2987,40 @@
       </c>
       <c r="L34" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M34" t="n">
-        <v>-58.441563</v>
+        <v>-58.488252</v>
       </c>
       <c r="N34" t="n">
-        <v>-34.569743</v>
+        <v>-34.553391</v>
       </c>
       <c r="O34" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P34" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>-406</t>
+          <t>5826</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>5/8/2025</t>
+          <t>5/19/2025</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Olof palme 4144</t>
+          <t>ALBARELLOS AV. 3180</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
@@ -3030,7 +3030,7 @@
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>805791925</t>
+          <t>806926466</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
@@ -3045,7 +3045,7 @@
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>Tensar 2 riendas a pique columna 168</t>
+          <t>Columna (metal) inclinada</t>
         </is>
       </c>
       <c r="I35" t="n">
@@ -3053,7 +3053,7 @@
       </c>
       <c r="J35" t="inlineStr">
         <is>
-          <t>Tensor</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K35" t="inlineStr">
@@ -3067,14 +3067,14 @@
         </is>
       </c>
       <c r="M35" t="n">
-        <v>-58.488252</v>
+        <v>-58.513552</v>
       </c>
       <c r="N35" t="n">
-        <v>-34.553391</v>
+        <v>-34.579829</v>
       </c>
       <c r="O35" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P35" t="inlineStr">
@@ -3086,7 +3086,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>5826</t>
+          <t>5825</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
@@ -3096,7 +3096,7 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>ALBARELLOS AV. 3180</t>
+          <t>PAZ, GRAL. AV. 5602</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
@@ -3106,7 +3106,7 @@
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>806926466</t>
+          <t>806926472</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
@@ -3121,7 +3121,7 @@
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>Columna (metal) inclinada</t>
+          <t>reparar rienda cortada - ver foto no es la misma que albarellos</t>
         </is>
       </c>
       <c r="I36" t="n">
@@ -3129,7 +3129,7 @@
       </c>
       <c r="J36" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Tensor</t>
         </is>
       </c>
       <c r="K36" t="inlineStr">
@@ -3143,10 +3143,10 @@
         </is>
       </c>
       <c r="M36" t="n">
-        <v>-58.513552</v>
+        <v>-58.513685</v>
       </c>
       <c r="N36" t="n">
-        <v>-34.579829</v>
+        <v>-34.579838</v>
       </c>
       <c r="O36" t="inlineStr">
         <is>
@@ -3162,27 +3162,27 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>5825</t>
+          <t>807044192</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>5/19/2025</t>
+          <t>5/29/2025</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>PAZ, GRAL. AV. 5602</t>
+          <t>O'Higgins 4379</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>806926472</t>
+          <t>807044192</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
@@ -3197,7 +3197,7 @@
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>reparar rienda cortada - ver foto no es la misma que albarellos</t>
+          <t xml:space="preserve">Poste </t>
         </is>
       </c>
       <c r="I37" t="n">
@@ -3205,7 +3205,7 @@
       </c>
       <c r="J37" t="inlineStr">
         <is>
-          <t>Tensor</t>
+          <t>Desmonte</t>
         </is>
       </c>
       <c r="K37" t="inlineStr">
@@ -3215,18 +3215,18 @@
       </c>
       <c r="L37" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M37" t="n">
-        <v>-58.513685</v>
+        <v>-58.468425</v>
       </c>
       <c r="N37" t="n">
-        <v>-34.579838</v>
+        <v>-34.54124</v>
       </c>
       <c r="O37" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P37" t="inlineStr">
@@ -3238,27 +3238,27 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>5875</t>
+          <t>6020</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>5/27/2025</t>
+          <t>6/5/2025</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>MONROE 4096</t>
+          <t>RAVIGNANI, EMILIO, DR. 2036</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>806975680</t>
+          <t>807215465</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
@@ -3295,46 +3295,46 @@
         </is>
       </c>
       <c r="M38" t="n">
-        <v>-58.476106</v>
+        <v>-58.436298</v>
       </c>
       <c r="N38" t="n">
-        <v>-34.568373</v>
+        <v>-34.578972</v>
       </c>
       <c r="O38" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P38" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>807044192</t>
+          <t>6144</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>5/29/2025</t>
+          <t>6/11/2025</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>O'Higgins 4379</t>
+          <t>TURIN 2990</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>807044192</t>
+          <t>807458282</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
@@ -3349,7 +3349,7 @@
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t xml:space="preserve">Poste </t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I39" t="n">
@@ -3357,7 +3357,7 @@
       </c>
       <c r="J39" t="inlineStr">
         <is>
-          <t>Desmonte</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K39" t="inlineStr">
@@ -3367,18 +3367,18 @@
       </c>
       <c r="L39" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M39" t="n">
-        <v>-58.468425</v>
+        <v>-58.480925</v>
       </c>
       <c r="N39" t="n">
-        <v>-34.54124</v>
+        <v>-34.585471</v>
       </c>
       <c r="O39" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P39" t="inlineStr">
@@ -3390,27 +3390,27 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>6020</t>
+          <t>6143</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>6/5/2025</t>
+          <t>6/11/2025</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>RAVIGNANI, EMILIO, DR. 2036</t>
+          <t>SOLANO LOPEZ, F., MARISCAL 2845</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>807215465</t>
+          <t>807458296</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
@@ -3447,26 +3447,26 @@
         </is>
       </c>
       <c r="M40" t="n">
-        <v>-58.436298</v>
+        <v>-58.495071</v>
       </c>
       <c r="N40" t="n">
-        <v>-34.578972</v>
+        <v>-34.593122</v>
       </c>
       <c r="O40" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P40" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>6144</t>
+          <t>6141</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
@@ -3476,17 +3476,17 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>TURIN 2990</t>
+          <t>EL PAMPERO 2618</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>807458282</t>
+          <t>807458310</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
@@ -3523,10 +3523,10 @@
         </is>
       </c>
       <c r="M41" t="n">
-        <v>-58.480925</v>
+        <v>-58.481942</v>
       </c>
       <c r="N41" t="n">
-        <v>-34.585471</v>
+        <v>-34.602989</v>
       </c>
       <c r="O41" t="inlineStr">
         <is>
@@ -3542,27 +3542,27 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>6143</t>
+          <t>-478</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>6/11/2025</t>
+          <t>6/15/2025</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>SOLANO LOPEZ, F., MARISCAL 2845</t>
+          <t>Chivilcoy 4875</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>807458296</t>
+          <t>807508509</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
@@ -3577,7 +3577,7 @@
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Poste podrido</t>
         </is>
       </c>
       <c r="I42" t="n">
@@ -3595,14 +3595,14 @@
       </c>
       <c r="L42" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M42" t="n">
-        <v>-58.495071</v>
+        <v>-58.517389</v>
       </c>
       <c r="N42" t="n">
-        <v>-34.593122</v>
+        <v>-34.593541</v>
       </c>
       <c r="O42" t="inlineStr">
         <is>
@@ -3618,27 +3618,27 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>6141</t>
+          <t>6171</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>6/11/2025</t>
+          <t>6/18/2025</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>EL PAMPERO 2618</t>
+          <t>CABELLO 3486</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>807458310</t>
+          <t>807658640</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
@@ -3653,7 +3653,7 @@
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Columna inclinada evaluar con inspector un corrimiento</t>
         </is>
       </c>
       <c r="I43" t="n">
@@ -3675,46 +3675,46 @@
         </is>
       </c>
       <c r="M43" t="n">
-        <v>-58.481942</v>
+        <v>-58.409579</v>
       </c>
       <c r="N43" t="n">
-        <v>-34.602989</v>
+        <v>-34.581134</v>
       </c>
       <c r="O43" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P43" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>-478</t>
+          <t>6230</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>6/15/2025</t>
+          <t>6/24/2025</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Chivilcoy 4875</t>
+          <t>Santa maria de oro	2722</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>807508509</t>
+          <t>807763066</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
@@ -3729,7 +3729,7 @@
       </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t>Poste podrido</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I44" t="n">
@@ -3747,40 +3747,40 @@
       </c>
       <c r="L44" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M44" t="n">
-        <v>-58.517389</v>
+        <v>-58.422315</v>
       </c>
       <c r="N44" t="n">
-        <v>-34.593541</v>
+        <v>-34.576988</v>
       </c>
       <c r="O44" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P44" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>6171</t>
+          <t>6231</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>6/18/2025</t>
+          <t>6/24/2025</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>CABELLO 3486</t>
+          <t>Ciudad de la Paz 275</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
@@ -3790,7 +3790,7 @@
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>807658640</t>
+          <t>807763070</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
@@ -3805,7 +3805,7 @@
       </c>
       <c r="H45" t="inlineStr">
         <is>
-          <t>Columna inclinada evaluar con inspector un corrimiento</t>
+          <t>Aplomar o cambiar</t>
         </is>
       </c>
       <c r="I45" t="n">
@@ -3823,14 +3823,14 @@
       </c>
       <c r="L45" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M45" t="n">
-        <v>-58.409579</v>
+        <v>-58.441049</v>
       </c>
       <c r="N45" t="n">
-        <v>-34.581134</v>
+        <v>-34.574625</v>
       </c>
       <c r="O45" t="inlineStr">
         <is>
@@ -3846,7 +3846,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>6230</t>
+          <t>6235</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
@@ -3856,17 +3856,17 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Santa maria de oro	2722</t>
+          <t>HUERGO 389</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>807763066</t>
+          <t>807763078</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
@@ -3903,10 +3903,10 @@
         </is>
       </c>
       <c r="M46" t="n">
-        <v>-58.422315</v>
+        <v>-58.432722</v>
       </c>
       <c r="N46" t="n">
-        <v>-34.576988</v>
+        <v>-34.572371</v>
       </c>
       <c r="O46" t="inlineStr">
         <is>
@@ -3922,17 +3922,17 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>6231</t>
+          <t>6295</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>6/24/2025</t>
+          <t>6/30/2025</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Ciudad de la Paz 275</t>
+          <t>SOLER 6017</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
@@ -3942,7 +3942,7 @@
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>807763070</t>
+          <t>807851636</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
@@ -3957,7 +3957,7 @@
       </c>
       <c r="H47" t="inlineStr">
         <is>
-          <t>Aplomar o cambiar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I47" t="n">
@@ -3975,14 +3975,14 @@
       </c>
       <c r="L47" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M47" t="n">
-        <v>-58.441049</v>
+        <v>-58.436808</v>
       </c>
       <c r="N47" t="n">
-        <v>-34.574625</v>
+        <v>-34.577464</v>
       </c>
       <c r="O47" t="inlineStr">
         <is>
@@ -3998,27 +3998,27 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>6235</t>
+          <t>6332</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>6/24/2025</t>
+          <t>7/3/2025</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>HUERGO 389</t>
+          <t>ARAOZ 2560</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>807763078</t>
+          <t>807965818</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
@@ -4055,10 +4055,10 @@
         </is>
       </c>
       <c r="M48" t="n">
-        <v>-58.432722</v>
+        <v>-58.414507</v>
       </c>
       <c r="N48" t="n">
-        <v>-34.572371</v>
+        <v>-34.585377</v>
       </c>
       <c r="O48" t="inlineStr">
         <is>
@@ -4074,27 +4074,27 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>6295</t>
+          <t>6363</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>6/30/2025</t>
+          <t>7/8/2025</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>SOLER 6017</t>
+          <t>MOLDES 3730</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>807851636</t>
+          <t>808099415</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
@@ -4109,7 +4109,7 @@
       </c>
       <c r="H49" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Poste inclinado</t>
         </is>
       </c>
       <c r="I49" t="n">
@@ -4117,7 +4117,7 @@
       </c>
       <c r="J49" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K49" t="inlineStr">
@@ -4127,50 +4127,50 @@
       </c>
       <c r="L49" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M49" t="n">
-        <v>-58.436808</v>
+        <v>-58.47192</v>
       </c>
       <c r="N49" t="n">
-        <v>-34.577464</v>
+        <v>-34.549398</v>
       </c>
       <c r="O49" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P49" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>6332</t>
+          <t>-503</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>7/3/2025</t>
+          <t>7/10/2025</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>ARAOZ 2560</t>
+          <t>Salguero 842</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>807965818</t>
+          <t>808148673</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
@@ -4185,7 +4185,7 @@
       </c>
       <c r="H50" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambiar columna picada en la base</t>
         </is>
       </c>
       <c r="I50" t="n">
@@ -4207,14 +4207,14 @@
         </is>
       </c>
       <c r="M50" t="n">
-        <v>-58.414507</v>
+        <v>-58.419166</v>
       </c>
       <c r="N50" t="n">
-        <v>-34.585377</v>
+        <v>-34.600265</v>
       </c>
       <c r="O50" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P50" t="inlineStr">
@@ -4226,27 +4226,27 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>6363</t>
+          <t>6506</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>7/8/2025</t>
+          <t>7/10/2025</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>MOLDES 3730</t>
+          <t>Ohiggins 1611</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>808099415</t>
+          <t>808148679</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
@@ -4261,7 +4261,7 @@
       </c>
       <c r="H51" t="inlineStr">
         <is>
-          <t>Poste inclinado</t>
+          <t>Columna podrida en la base</t>
         </is>
       </c>
       <c r="I51" t="n">
@@ -4269,28 +4269,28 @@
       </c>
       <c r="J51" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K51" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L51" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M51" t="n">
-        <v>-58.47192</v>
+        <v>-58.448993</v>
       </c>
       <c r="N51" t="n">
-        <v>-34.549398</v>
+        <v>-34.564383</v>
       </c>
       <c r="O51" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P51" t="inlineStr">
@@ -4302,27 +4302,27 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>-503</t>
+          <t>6437</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>7/10/2025</t>
+          <t>7/17/2025</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>Salguero 842</t>
+          <t>MILLER 4590</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>808148673</t>
+          <t>808400306</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
@@ -4337,7 +4337,7 @@
       </c>
       <c r="H52" t="inlineStr">
         <is>
-          <t>Cambiar columna picada en la base</t>
+          <t>Columna corroida</t>
         </is>
       </c>
       <c r="I52" t="n">
@@ -4359,46 +4359,46 @@
         </is>
       </c>
       <c r="M52" t="n">
-        <v>-58.419166</v>
+        <v>-58.495482</v>
       </c>
       <c r="N52" t="n">
-        <v>-34.600265</v>
+        <v>-34.552614</v>
       </c>
       <c r="O52" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P52" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>6506</t>
+          <t>-519</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>7/10/2025</t>
+          <t>7/17/2025</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>Ohiggins 1611</t>
+          <t>Vilela 2687</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>808148679</t>
+          <t>808400334</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
@@ -4413,7 +4413,7 @@
       </c>
       <c r="H53" t="inlineStr">
         <is>
-          <t>Columna podrida en la base</t>
+          <t>CAmbiar columna 114 picada en base</t>
         </is>
       </c>
       <c r="I53" t="n">
@@ -4426,7 +4426,7 @@
       </c>
       <c r="K53" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L53" t="inlineStr">
@@ -4435,14 +4435,14 @@
         </is>
       </c>
       <c r="M53" t="n">
-        <v>-58.448993</v>
+        <v>-58.472968</v>
       </c>
       <c r="N53" t="n">
-        <v>-34.564383</v>
+        <v>-34.546898</v>
       </c>
       <c r="O53" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P53" t="inlineStr">
@@ -4454,7 +4454,7 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>6437</t>
+          <t>6538</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
@@ -4464,7 +4464,7 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>MILLER 4590</t>
+          <t>Pedraza Manuela 4101</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
@@ -4474,7 +4474,7 @@
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>808400306</t>
+          <t>808400353</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
@@ -4489,7 +4489,7 @@
       </c>
       <c r="H54" t="inlineStr">
         <is>
-          <t>Columna corroida</t>
+          <t xml:space="preserve">Podrida en la base </t>
         </is>
       </c>
       <c r="I54" t="n">
@@ -4511,10 +4511,10 @@
         </is>
       </c>
       <c r="M54" t="n">
-        <v>-58.495482</v>
+        <v>-58.481569</v>
       </c>
       <c r="N54" t="n">
-        <v>-34.552614</v>
+        <v>-34.559853</v>
       </c>
       <c r="O54" t="inlineStr">
         <is>
@@ -4530,27 +4530,27 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>6447</t>
+          <t>-525</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>7/17/2025</t>
+          <t>7/22/2025</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>CIUDAD DE LA PAZ 1535</t>
+          <t>Zabala 3567</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>808400333</t>
+          <t>808480549</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
@@ -4565,7 +4565,7 @@
       </c>
       <c r="H55" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Corroida en base para recambio</t>
         </is>
       </c>
       <c r="I55" t="n">
@@ -4587,10 +4587,10 @@
         </is>
       </c>
       <c r="M55" t="n">
-        <v>-58.453124</v>
+        <v>-58.457492</v>
       </c>
       <c r="N55" t="n">
-        <v>-34.567382</v>
+        <v>-34.579336</v>
       </c>
       <c r="O55" t="inlineStr">
         <is>
@@ -4606,27 +4606,27 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>-519</t>
+          <t>6484</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>7/17/2025</t>
+          <t>7/24/2025</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>Vilela 2687</t>
+          <t>URIARTE 2396</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>808400334</t>
+          <t>808509373</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
@@ -4641,7 +4641,7 @@
       </c>
       <c r="H56" t="inlineStr">
         <is>
-          <t>CAmbiar columna 114 picada en base</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I56" t="n">
@@ -4663,46 +4663,46 @@
         </is>
       </c>
       <c r="M56" t="n">
-        <v>-58.472968</v>
+        <v>-58.423934</v>
       </c>
       <c r="N56" t="n">
-        <v>-34.546898</v>
+        <v>-34.581562</v>
       </c>
       <c r="O56" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P56" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>6538</t>
+          <t>6504</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>7/17/2025</t>
+          <t>7/25/2025</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>Pedraza Manuela 4101</t>
+          <t>CIUDAD DE LA PAZ 1278</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>808400353</t>
+          <t>808571974</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
@@ -4717,7 +4717,7 @@
       </c>
       <c r="H57" t="inlineStr">
         <is>
-          <t xml:space="preserve">Podrida en la base </t>
+          <t>Inclinada</t>
         </is>
       </c>
       <c r="I57" t="n">
@@ -4739,14 +4739,14 @@
         </is>
       </c>
       <c r="M57" t="n">
-        <v>-58.481569</v>
+        <v>-58.450753</v>
       </c>
       <c r="N57" t="n">
-        <v>-34.559853</v>
+        <v>-34.5688</v>
       </c>
       <c r="O57" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P57" t="inlineStr">
@@ -4758,27 +4758,27 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>-525</t>
+          <t>6512</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>7/22/2025</t>
+          <t>7/28/2025</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>Zabala 3567</t>
+          <t>GASCON 1195</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>808480549</t>
+          <t>808571975</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
@@ -4793,7 +4793,7 @@
       </c>
       <c r="H58" t="inlineStr">
         <is>
-          <t>Corroida en base para recambio</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I58" t="n">
@@ -4815,36 +4815,36 @@
         </is>
       </c>
       <c r="M58" t="n">
-        <v>-58.457492</v>
+        <v>-58.423127</v>
       </c>
       <c r="N58" t="n">
-        <v>-34.579336</v>
+        <v>-34.596476</v>
       </c>
       <c r="O58" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P58" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>6484</t>
+          <t>6513</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>7/24/2025</t>
+          <t>7/28/2025</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>URIARTE 2396</t>
+          <t>DORREGO 1925</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
@@ -4854,7 +4854,7 @@
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>808509373</t>
+          <t>808571976</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
@@ -4891,10 +4891,10 @@
         </is>
       </c>
       <c r="M59" t="n">
-        <v>-58.423934</v>
+        <v>-58.441281</v>
       </c>
       <c r="N59" t="n">
-        <v>-34.581562</v>
+        <v>-34.579867</v>
       </c>
       <c r="O59" t="inlineStr">
         <is>
@@ -4910,27 +4910,27 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>6502</t>
+          <t>6519</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>7/25/2025</t>
+          <t>7/28/2025</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>CIUDAD DE LA PAZ 1511</t>
+          <t>SALGUERO, JERONIMO 2874</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>808571972</t>
+          <t>808571977</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
@@ -4945,7 +4945,7 @@
       </c>
       <c r="H60" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Reparar rienda</t>
         </is>
       </c>
       <c r="I60" t="n">
@@ -4953,7 +4953,7 @@
       </c>
       <c r="J60" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Tensor</t>
         </is>
       </c>
       <c r="K60" t="inlineStr">
@@ -4963,50 +4963,50 @@
       </c>
       <c r="L60" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M60" t="n">
-        <v>-58.452907</v>
+        <v>-58.407256</v>
       </c>
       <c r="N60" t="n">
-        <v>-34.567508</v>
+        <v>-34.578976</v>
       </c>
       <c r="O60" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P60" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>6504</t>
+          <t>-536</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>7/25/2025</t>
+          <t>7/29/2025</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>CIUDAD DE LA PAZ 1278</t>
+          <t>Olof palme 4142</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>808571974</t>
+          <t xml:space="preserve">ICD30249764 </t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
@@ -5021,7 +5021,7 @@
       </c>
       <c r="H61" t="inlineStr">
         <is>
-          <t>Inclinada</t>
+          <t>Aplomar o desmontar poste</t>
         </is>
       </c>
       <c r="I61" t="n">
@@ -5029,7 +5029,7 @@
       </c>
       <c r="J61" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Desmonte</t>
         </is>
       </c>
       <c r="K61" t="inlineStr">
@@ -5039,18 +5039,18 @@
       </c>
       <c r="L61" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M61" t="n">
-        <v>-58.450753</v>
+        <v>-58.488239</v>
       </c>
       <c r="N61" t="n">
-        <v>-34.5688</v>
+        <v>-34.55341</v>
       </c>
       <c r="O61" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P61" t="inlineStr">
@@ -5062,27 +5062,27 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>6512</t>
+          <t>-538</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>7/28/2025</t>
+          <t>7/31/2025</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>GASCON 1195</t>
+          <t>Malabia 964</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>808571975</t>
+          <t>808609237</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
@@ -5097,7 +5097,7 @@
       </c>
       <c r="H62" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambiar poste mal estado por PRFV</t>
         </is>
       </c>
       <c r="I62" t="n">
@@ -5115,14 +5115,14 @@
       </c>
       <c r="L62" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M62" t="n">
-        <v>-58.423127</v>
+        <v>-58.433634</v>
       </c>
       <c r="N62" t="n">
-        <v>-34.596476</v>
+        <v>-34.595018</v>
       </c>
       <c r="O62" t="inlineStr">
         <is>
@@ -5132,382 +5132,6 @@
       <c r="P62" t="inlineStr">
         <is>
           <t>Capital Sur</t>
-        </is>
-      </c>
-    </row>
-    <row r="63">
-      <c r="A63" t="inlineStr">
-        <is>
-          <t>6513</t>
-        </is>
-      </c>
-      <c r="B63" t="inlineStr">
-        <is>
-          <t>7/28/2025</t>
-        </is>
-      </c>
-      <c r="C63" t="inlineStr">
-        <is>
-          <t>DORREGO 1925</t>
-        </is>
-      </c>
-      <c r="D63" t="inlineStr">
-        <is>
-          <t>14</t>
-        </is>
-      </c>
-      <c r="E63" t="inlineStr">
-        <is>
-          <t>808571976</t>
-        </is>
-      </c>
-      <c r="F63" t="inlineStr">
-        <is>
-          <t>NEW</t>
-        </is>
-      </c>
-      <c r="G63" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H63" t="inlineStr">
-        <is>
-          <t>Picada</t>
-        </is>
-      </c>
-      <c r="I63" t="n">
-        <v>1</v>
-      </c>
-      <c r="J63" t="inlineStr">
-        <is>
-          <t>Cambio</t>
-        </is>
-      </c>
-      <c r="K63" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L63" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
-      <c r="M63" t="n">
-        <v>-58.441281</v>
-      </c>
-      <c r="N63" t="n">
-        <v>-34.579867</v>
-      </c>
-      <c r="O63" t="inlineStr">
-        <is>
-          <t>Palermo</t>
-        </is>
-      </c>
-      <c r="P63" t="inlineStr">
-        <is>
-          <t>Capital Sur</t>
-        </is>
-      </c>
-    </row>
-    <row r="64">
-      <c r="A64" t="inlineStr">
-        <is>
-          <t>6519</t>
-        </is>
-      </c>
-      <c r="B64" t="inlineStr">
-        <is>
-          <t>7/28/2025</t>
-        </is>
-      </c>
-      <c r="C64" t="inlineStr">
-        <is>
-          <t>SALGUERO, JERONIMO 2874</t>
-        </is>
-      </c>
-      <c r="D64" t="inlineStr">
-        <is>
-          <t>14</t>
-        </is>
-      </c>
-      <c r="E64" t="inlineStr">
-        <is>
-          <t>808571977</t>
-        </is>
-      </c>
-      <c r="F64" t="inlineStr">
-        <is>
-          <t>NEW</t>
-        </is>
-      </c>
-      <c r="G64" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H64" t="inlineStr">
-        <is>
-          <t>Reparar rienda</t>
-        </is>
-      </c>
-      <c r="I64" t="n">
-        <v>1</v>
-      </c>
-      <c r="J64" t="inlineStr">
-        <is>
-          <t>Tensor</t>
-        </is>
-      </c>
-      <c r="K64" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L64" t="inlineStr">
-        <is>
-          <t>Terminal</t>
-        </is>
-      </c>
-      <c r="M64" t="n">
-        <v>-58.407256</v>
-      </c>
-      <c r="N64" t="n">
-        <v>-34.578976</v>
-      </c>
-      <c r="O64" t="inlineStr">
-        <is>
-          <t>Palermo</t>
-        </is>
-      </c>
-      <c r="P64" t="inlineStr">
-        <is>
-          <t>Capital Sur</t>
-        </is>
-      </c>
-    </row>
-    <row r="65">
-      <c r="A65" t="inlineStr">
-        <is>
-          <t>-536</t>
-        </is>
-      </c>
-      <c r="B65" t="inlineStr">
-        <is>
-          <t>7/29/2025</t>
-        </is>
-      </c>
-      <c r="C65" t="inlineStr">
-        <is>
-          <t>Olof palme 4142</t>
-        </is>
-      </c>
-      <c r="D65" t="inlineStr">
-        <is>
-          <t>12</t>
-        </is>
-      </c>
-      <c r="E65" t="inlineStr">
-        <is>
-          <t xml:space="preserve">ICD30249764 </t>
-        </is>
-      </c>
-      <c r="F65" t="inlineStr">
-        <is>
-          <t>NEW</t>
-        </is>
-      </c>
-      <c r="G65" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H65" t="inlineStr">
-        <is>
-          <t>Aplomar o desmontar poste</t>
-        </is>
-      </c>
-      <c r="I65" t="n">
-        <v>1</v>
-      </c>
-      <c r="J65" t="inlineStr">
-        <is>
-          <t>Desmonte</t>
-        </is>
-      </c>
-      <c r="K65" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L65" t="inlineStr">
-        <is>
-          <t>Poste</t>
-        </is>
-      </c>
-      <c r="M65" t="n">
-        <v>-58.488239</v>
-      </c>
-      <c r="N65" t="n">
-        <v>-34.55341</v>
-      </c>
-      <c r="O65" t="inlineStr">
-        <is>
-          <t>Saavedra</t>
-        </is>
-      </c>
-      <c r="P65" t="inlineStr">
-        <is>
-          <t>Capital Norte</t>
-        </is>
-      </c>
-    </row>
-    <row r="66">
-      <c r="A66" t="inlineStr">
-        <is>
-          <t>-538</t>
-        </is>
-      </c>
-      <c r="B66" t="inlineStr">
-        <is>
-          <t>7/31/2025</t>
-        </is>
-      </c>
-      <c r="C66" t="inlineStr">
-        <is>
-          <t>Malabia 964</t>
-        </is>
-      </c>
-      <c r="D66" t="inlineStr">
-        <is>
-          <t>15</t>
-        </is>
-      </c>
-      <c r="E66" t="inlineStr">
-        <is>
-          <t>808609237</t>
-        </is>
-      </c>
-      <c r="F66" t="inlineStr">
-        <is>
-          <t>NEW</t>
-        </is>
-      </c>
-      <c r="G66" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H66" t="inlineStr">
-        <is>
-          <t>Cambiar poste mal estado por PRFV</t>
-        </is>
-      </c>
-      <c r="I66" t="n">
-        <v>1</v>
-      </c>
-      <c r="J66" t="inlineStr">
-        <is>
-          <t>Cambio</t>
-        </is>
-      </c>
-      <c r="K66" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L66" t="inlineStr">
-        <is>
-          <t>Poste</t>
-        </is>
-      </c>
-      <c r="M66" t="n">
-        <v>-58.433634</v>
-      </c>
-      <c r="N66" t="n">
-        <v>-34.595018</v>
-      </c>
-      <c r="O66" t="inlineStr">
-        <is>
-          <t>Palermo</t>
-        </is>
-      </c>
-      <c r="P66" t="inlineStr">
-        <is>
-          <t>Capital Sur</t>
-        </is>
-      </c>
-    </row>
-    <row r="67">
-      <c r="A67" t="inlineStr">
-        <is>
-          <t>-543</t>
-        </is>
-      </c>
-      <c r="B67" t="inlineStr">
-        <is>
-          <t>8/1/2025</t>
-        </is>
-      </c>
-      <c r="C67" t="inlineStr">
-        <is>
-          <t>Pedro Ignacio Rivera 3258</t>
-        </is>
-      </c>
-      <c r="D67" t="inlineStr">
-        <is>
-          <t>13</t>
-        </is>
-      </c>
-      <c r="E67" t="inlineStr"/>
-      <c r="F67" t="inlineStr">
-        <is>
-          <t>NEW</t>
-        </is>
-      </c>
-      <c r="G67" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H67" t="inlineStr">
-        <is>
-          <t>Desmontar poste en desuso</t>
-        </is>
-      </c>
-      <c r="I67" t="n">
-        <v>1</v>
-      </c>
-      <c r="J67" t="inlineStr">
-        <is>
-          <t>Desmonte</t>
-        </is>
-      </c>
-      <c r="K67" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L67" t="inlineStr">
-        <is>
-          <t>Poste</t>
-        </is>
-      </c>
-      <c r="M67" t="n">
-        <v>-58.46967</v>
-      </c>
-      <c r="N67" t="n">
-        <v>-34.561676</v>
-      </c>
-      <c r="O67" t="inlineStr">
-        <is>
-          <t>Colegiales</t>
-        </is>
-      </c>
-      <c r="P67" t="inlineStr">
-        <is>
-          <t>Capital Norte</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-08-05 08:04:04)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_NEW.xlsx
+++ b/mapa_interactivo_NEW.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P62"/>
+  <dimension ref="A1:P60"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -822,17 +822,17 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>5589</t>
+          <t>4595</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>12/31/2023</t>
+          <t>1/15/2025</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>ARCOS 1520</t>
+          <t>PAROISSIEN 1806</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -842,7 +842,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>799540526</t>
+          <t>802747617</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -852,33 +852,41 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
+          <t>Pendiente</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Aplomar</t>
         </is>
       </c>
       <c r="I6" t="n">
-        <v>0</v>
-      </c>
-      <c r="J6" t="inlineStr"/>
-      <c r="K6" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>Aplomo</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M6" t="n">
-        <v>-58.449125</v>
+        <v>-58.464172</v>
       </c>
       <c r="N6" t="n">
-        <v>-34.565958</v>
+        <v>-34.543845</v>
       </c>
       <c r="O6" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P6" t="inlineStr">
@@ -890,27 +898,27 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>4595</t>
+          <t>4662</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>1/15/2025</t>
+          <t>1/21/2025</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>PAROISSIEN 1806</t>
+          <t>ALTOLAGUIRRE 2397</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>802747617</t>
+          <t>802823938</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -925,7 +933,7 @@
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>Aplomar</t>
+          <t>Inclinada</t>
         </is>
       </c>
       <c r="I7" t="n">
@@ -943,18 +951,18 @@
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M7" t="n">
-        <v>-58.464172</v>
+        <v>-58.490766</v>
       </c>
       <c r="N7" t="n">
-        <v>-34.543845</v>
+        <v>-34.576987</v>
       </c>
       <c r="O7" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P7" t="inlineStr">
@@ -966,27 +974,27 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>4662</t>
+          <t>6036</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>1/21/2025</t>
+          <t>2/24/2025</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>ALTOLAGUIRRE 2397</t>
+          <t>MEDRANO 1715</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>802823938</t>
+          <t>803608181</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -999,22 +1007,18 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H8" t="inlineStr">
-        <is>
-          <t>Inclinada</t>
-        </is>
-      </c>
+      <c r="H8" t="inlineStr"/>
       <c r="I8" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L8" t="inlineStr">
@@ -1023,46 +1027,46 @@
         </is>
       </c>
       <c r="M8" t="n">
-        <v>-58.490766</v>
+        <v>-58.418236</v>
       </c>
       <c r="N8" t="n">
-        <v>-34.576987</v>
+        <v>-34.589859</v>
       </c>
       <c r="O8" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P8" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>4862</t>
+          <t>803608480</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>1/23/2025</t>
+          <t>2/24/2025</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>ARCOS 2263</t>
+          <t>GUATEMALA /ALT/ 4415</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>802857379</t>
+          <t>803608480</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -1072,12 +1076,12 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
+          <t>Pendiente</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>picada</t>
+          <t xml:space="preserve">Guatemala 4415 </t>
         </is>
       </c>
       <c r="I9" t="n">
@@ -1090,7 +1094,7 @@
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L9" t="inlineStr">
@@ -1099,46 +1103,46 @@
         </is>
       </c>
       <c r="M9" t="n">
-        <v>-58.455082</v>
+        <v>-58.421661</v>
       </c>
       <c r="N9" t="n">
-        <v>-34.558883</v>
+        <v>-34.588428</v>
       </c>
       <c r="O9" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P9" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>6036</t>
+          <t>5053</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>2/24/2025</t>
+          <t>3/11/2025</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>MEDRANO 1715</t>
+          <t>MENDOZA 1153</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>803608181</t>
+          <t>803969314</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
@@ -1151,7 +1155,11 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H10" t="inlineStr"/>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>Poste</t>
+        </is>
+      </c>
       <c r="I10" t="n">
         <v>0</v>
       </c>
@@ -1162,55 +1170,55 @@
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L10" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M10" t="n">
-        <v>-58.418236</v>
+        <v>-58.44463</v>
       </c>
       <c r="N10" t="n">
-        <v>-34.589859</v>
+        <v>-34.553354</v>
       </c>
       <c r="O10" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P10" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>803608480</t>
+          <t>6071</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>2/24/2025</t>
+          <t>3/17/2025</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>GUATEMALA /ALT/ 4415</t>
+          <t>OSORIO 4994</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>803608480</t>
+          <t>804053324</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
@@ -1223,11 +1231,7 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H11" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Guatemala 4415 </t>
-        </is>
-      </c>
+      <c r="H11" t="inlineStr"/>
       <c r="I11" t="n">
         <v>0</v>
       </c>
@@ -1247,46 +1251,46 @@
         </is>
       </c>
       <c r="M11" t="n">
-        <v>-58.421661</v>
+        <v>-58.466241</v>
       </c>
       <c r="N11" t="n">
-        <v>-34.588428</v>
+        <v>-34.595741</v>
       </c>
       <c r="O11" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P11" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>5053</t>
+          <t>3348</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>3/11/2025</t>
+          <t>3/27/2025</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>MENDOZA 1153</t>
+          <t>ESTOMBA 2626</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>803969314</t>
+          <t>804309704</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
@@ -1301,15 +1305,15 @@
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I12" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Desmonte</t>
         </is>
       </c>
       <c r="K12" t="inlineStr">
@@ -1319,18 +1323,18 @@
       </c>
       <c r="L12" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M12" t="n">
-        <v>-58.44463</v>
+        <v>-58.47538</v>
       </c>
       <c r="N12" t="n">
-        <v>-34.553354</v>
+        <v>-34.566015</v>
       </c>
       <c r="O12" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P12" t="inlineStr">
@@ -1342,27 +1346,27 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>6071</t>
+          <t>-312</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>3/17/2025</t>
+          <t>3/29/2025</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>OSORIO 4994</t>
+          <t>MATIENZO BENJAMIN /ALT/ 1831</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>804053324</t>
+          <t>804333522</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
@@ -1375,7 +1379,11 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H13" t="inlineStr"/>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>Retirar columna ya traspasaron el nodo</t>
+        </is>
+      </c>
       <c r="I13" t="n">
         <v>0</v>
       </c>
@@ -1386,7 +1394,7 @@
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L13" t="inlineStr">
@@ -1395,36 +1403,36 @@
         </is>
       </c>
       <c r="M13" t="n">
-        <v>-58.466241</v>
+        <v>-58.434835</v>
       </c>
       <c r="N13" t="n">
-        <v>-34.595741</v>
+        <v>-34.569129</v>
       </c>
       <c r="O13" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P13" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>3348</t>
+          <t>3430</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>3/27/2025</t>
+          <t>4/1/2025</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>ESTOMBA 2626</t>
+          <t>MONROE 3838</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
@@ -1434,7 +1442,7 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>804309704</t>
+          <t>804468442</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
@@ -1449,7 +1457,7 @@
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Reparar rienda</t>
         </is>
       </c>
       <c r="I14" t="n">
@@ -1457,7 +1465,7 @@
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>Desmonte</t>
+          <t>Tensor</t>
         </is>
       </c>
       <c r="K14" t="inlineStr">
@@ -1467,14 +1475,14 @@
       </c>
       <c r="L14" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M14" t="n">
-        <v>-58.47538</v>
+        <v>-58.473659</v>
       </c>
       <c r="N14" t="n">
-        <v>-34.566015</v>
+        <v>-34.566979</v>
       </c>
       <c r="O14" t="inlineStr">
         <is>
@@ -1490,27 +1498,27 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>-312</t>
+          <t>5464</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>3/29/2025</t>
+          <t>4/4/2025</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>MATIENZO BENJAMIN /ALT/ 1831</t>
+          <t>SUCRE, ANTONIO JOSE DE, MCAL. 3100</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>804333522</t>
+          <t>804497880</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
@@ -1525,11 +1533,11 @@
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>Retirar columna ya traspasaron el nodo</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I15" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J15" t="inlineStr">
         <is>
@@ -1538,45 +1546,45 @@
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L15" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M15" t="n">
-        <v>-58.434835</v>
+        <v>-58.46161</v>
       </c>
       <c r="N15" t="n">
-        <v>-34.569129</v>
+        <v>-34.567849</v>
       </c>
       <c r="O15" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P15" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>3430</t>
+          <t>5469</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>4/1/2025</t>
+          <t>4/4/2025</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>MONROE 3838</t>
+          <t>ESTADO PLURINACIONAL DE BOLIVIA 5899</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
@@ -1586,7 +1594,7 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>804468442</t>
+          <t>804497887</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
@@ -1601,7 +1609,7 @@
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>Reparar rienda</t>
+          <t>Aplomar</t>
         </is>
       </c>
       <c r="I16" t="n">
@@ -1609,7 +1617,7 @@
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>Tensor</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K16" t="inlineStr">
@@ -1623,14 +1631,14 @@
         </is>
       </c>
       <c r="M16" t="n">
-        <v>-58.473659</v>
+        <v>-58.507746</v>
       </c>
       <c r="N16" t="n">
-        <v>-34.566979</v>
+        <v>-34.574217</v>
       </c>
       <c r="O16" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P16" t="inlineStr">
@@ -1642,7 +1650,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>5464</t>
+          <t>5492</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -1652,17 +1660,17 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>SUCRE, ANTONIO JOSE DE, MCAL. 3100</t>
+          <t>ESTADO PLURINACIONAL DE BOLIVIA 5920</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>804497880</t>
+          <t>804498035</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
@@ -1677,7 +1685,7 @@
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>aplomar</t>
         </is>
       </c>
       <c r="I17" t="n">
@@ -1685,7 +1693,7 @@
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K17" t="inlineStr">
@@ -1699,14 +1707,14 @@
         </is>
       </c>
       <c r="M17" t="n">
-        <v>-58.46161</v>
+        <v>-58.50751</v>
       </c>
       <c r="N17" t="n">
-        <v>-34.567849</v>
+        <v>-34.574543</v>
       </c>
       <c r="O17" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P17" t="inlineStr">
@@ -1718,17 +1726,17 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>5469</t>
+          <t>5599</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>4/4/2025</t>
+          <t>4/15/2025</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>ESTADO PLURINACIONAL DE BOLIVIA 5899</t>
+          <t>ESTOMBA 4052</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
@@ -1738,7 +1746,7 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>804497887</t>
+          <t>804732246</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
@@ -1753,7 +1761,7 @@
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>Aplomar</t>
+          <t>Columna PRFV quedo inclinada (la hicieron como estomba 4056)</t>
         </is>
       </c>
       <c r="I18" t="n">
@@ -1766,23 +1774,23 @@
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo TLC</t>
         </is>
       </c>
       <c r="L18" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M18" t="n">
-        <v>-58.507746</v>
+        <v>-58.485407</v>
       </c>
       <c r="N18" t="n">
-        <v>-34.574217</v>
+        <v>-34.552985</v>
       </c>
       <c r="O18" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P18" t="inlineStr">
@@ -1794,27 +1802,27 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>5492</t>
+          <t>5590</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>4/4/2025</t>
+          <t>4/15/2025</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>ESTADO PLURINACIONAL DE BOLIVIA 5920</t>
+          <t>O'HIGGINS 2441</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>804498035</t>
+          <t>804732275</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
@@ -1829,7 +1837,7 @@
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>aplomar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I19" t="n">
@@ -1837,7 +1845,7 @@
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K19" t="inlineStr">
@@ -1847,18 +1855,18 @@
       </c>
       <c r="L19" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M19" t="n">
-        <v>-58.50751</v>
+        <v>-58.45573</v>
       </c>
       <c r="N19" t="n">
-        <v>-34.574543</v>
+        <v>-34.556576</v>
       </c>
       <c r="O19" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P19" t="inlineStr">
@@ -1870,27 +1878,27 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>5599</t>
+          <t>804787368</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>4/15/2025</t>
+          <t>4/17/2025</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>ESTOMBA 4052</t>
+          <t>San Blas 2591</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>804732246</t>
+          <t>804787368</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
@@ -1905,7 +1913,7 @@
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>Columna PRFV quedo inclinada (la hicieron como estomba 4056)</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I20" t="n">
@@ -1913,12 +1921,12 @@
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>Nodo TLC</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L20" t="inlineStr">
@@ -1927,14 +1935,14 @@
         </is>
       </c>
       <c r="M20" t="n">
-        <v>-58.485407</v>
+        <v>-58.477427</v>
       </c>
       <c r="N20" t="n">
-        <v>-34.552985</v>
+        <v>-34.609261</v>
       </c>
       <c r="O20" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P20" t="inlineStr">
@@ -1946,17 +1954,17 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>5590</t>
+          <t>5624</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>4/15/2025</t>
+          <t>4/22/2025</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>O'HIGGINS 2441</t>
+          <t>PINO, VIRREY DEL 3456</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
@@ -1966,7 +1974,7 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>804732275</t>
+          <t>804876043</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
@@ -1981,7 +1989,7 @@
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Desmonte de poste</t>
         </is>
       </c>
       <c r="I21" t="n">
@@ -1989,7 +1997,7 @@
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Desmonte</t>
         </is>
       </c>
       <c r="K21" t="inlineStr">
@@ -1999,18 +2007,18 @@
       </c>
       <c r="L21" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M21" t="n">
-        <v>-58.45573</v>
+        <v>-58.464354</v>
       </c>
       <c r="N21" t="n">
-        <v>-34.556576</v>
+        <v>-34.572486</v>
       </c>
       <c r="O21" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P21" t="inlineStr">
@@ -2022,27 +2030,27 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>804787368</t>
+          <t>804922147</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>4/17/2025</t>
+          <t>4/24/2025</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>San Blas 2591</t>
+          <t>Av. Álvarez Thomas 1171</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>804787368</t>
+          <t>804922147</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
@@ -2061,7 +2069,7 @@
         </is>
       </c>
       <c r="I22" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J22" t="inlineStr">
         <is>
@@ -2079,14 +2087,14 @@
         </is>
       </c>
       <c r="M22" t="n">
-        <v>-58.477427</v>
+        <v>-58.45793</v>
       </c>
       <c r="N22" t="n">
-        <v>-34.609261</v>
+        <v>-34.578334</v>
       </c>
       <c r="O22" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P22" t="inlineStr">
@@ -2098,17 +2106,17 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>5624</t>
+          <t>804922171</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>4/22/2025</t>
+          <t>4/24/2025</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>PINO, VIRREY DEL 3456</t>
+          <t>Virrey Arredondo 3581</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
@@ -2118,7 +2126,7 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>804876043</t>
+          <t>804922171</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
@@ -2133,7 +2141,7 @@
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>Desmonte de poste</t>
+          <t>Aplomar</t>
         </is>
       </c>
       <c r="I23" t="n">
@@ -2141,7 +2149,7 @@
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>Desmonte</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K23" t="inlineStr">
@@ -2151,14 +2159,14 @@
       </c>
       <c r="L23" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M23" t="n">
-        <v>-58.464354</v>
+        <v>-58.459513</v>
       </c>
       <c r="N23" t="n">
-        <v>-34.572486</v>
+        <v>-34.578019</v>
       </c>
       <c r="O23" t="inlineStr">
         <is>
@@ -2174,7 +2182,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>804922147</t>
+          <t>5656</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -2184,17 +2192,17 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Av. Álvarez Thomas 1171</t>
+          <t>ECHEVERRIA 5893</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>804922147</t>
+          <t>804922184</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
@@ -2209,15 +2217,15 @@
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Poste con base quebrada</t>
         </is>
       </c>
       <c r="I24" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J24" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Desmonte</t>
         </is>
       </c>
       <c r="K24" t="inlineStr">
@@ -2227,18 +2235,18 @@
       </c>
       <c r="L24" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M24" t="n">
-        <v>-58.45793</v>
+        <v>-58.489627</v>
       </c>
       <c r="N24" t="n">
-        <v>-34.578334</v>
+        <v>-34.583761</v>
       </c>
       <c r="O24" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P24" t="inlineStr">
@@ -2250,27 +2258,27 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>804922171</t>
+          <t>6173</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>4/24/2025</t>
+          <t>4/29/2025</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Virrey Arredondo 3581</t>
+          <t>ARMENIA 2321</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>804922171</t>
+          <t>805507398</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
@@ -2285,7 +2293,7 @@
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>Aplomar</t>
+          <t>Picada volvio a entrar como caso 6325</t>
         </is>
       </c>
       <c r="I25" t="n">
@@ -2293,7 +2301,7 @@
       </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K25" t="inlineStr">
@@ -2303,40 +2311,40 @@
       </c>
       <c r="L25" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M25" t="n">
-        <v>-58.459513</v>
+        <v>-58.420549</v>
       </c>
       <c r="N25" t="n">
-        <v>-34.578019</v>
+        <v>-34.585103</v>
       </c>
       <c r="O25" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P25" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>5656</t>
+          <t>5715</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>4/24/2025</t>
+          <t>5/1/2025</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>ECHEVERRIA 5893</t>
+          <t>CUENCA 4690</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
@@ -2346,7 +2354,7 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>804922184</t>
+          <t>805579094</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
@@ -2361,7 +2369,7 @@
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>Poste con base quebrada</t>
+          <t>Aplomar poste</t>
         </is>
       </c>
       <c r="I26" t="n">
@@ -2369,7 +2377,7 @@
       </c>
       <c r="J26" t="inlineStr">
         <is>
-          <t>Desmonte</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K26" t="inlineStr">
@@ -2383,10 +2391,10 @@
         </is>
       </c>
       <c r="M26" t="n">
-        <v>-58.489627</v>
+        <v>-58.506061</v>
       </c>
       <c r="N26" t="n">
-        <v>-34.583761</v>
+        <v>-34.588887</v>
       </c>
       <c r="O26" t="inlineStr">
         <is>
@@ -2402,27 +2410,27 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>6173</t>
+          <t>5719</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>4/29/2025</t>
+          <t>5/1/2025</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>ARMENIA 2321</t>
+          <t>CABEZON, JOSE LEON 2440</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>805507398</t>
+          <t>805579157</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
@@ -2437,7 +2445,7 @@
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>Picada volvio a entrar como caso 6325</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I27" t="n">
@@ -2459,26 +2467,26 @@
         </is>
       </c>
       <c r="M27" t="n">
-        <v>-58.420549</v>
+        <v>-58.499967</v>
       </c>
       <c r="N27" t="n">
-        <v>-34.585103</v>
+        <v>-34.57974</v>
       </c>
       <c r="O27" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P27" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>5715</t>
+          <t>6333</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -2488,17 +2496,17 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>CUENCA 4690</t>
+          <t>ORTEGA Y GASSET 1816</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>805579094</t>
+          <t>805655342</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
@@ -2513,7 +2521,7 @@
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>Aplomar poste</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I28" t="n">
@@ -2521,7 +2529,7 @@
       </c>
       <c r="J28" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K28" t="inlineStr">
@@ -2531,50 +2539,50 @@
       </c>
       <c r="L28" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M28" t="n">
-        <v>-58.506061</v>
+        <v>-58.432556</v>
       </c>
       <c r="N28" t="n">
-        <v>-34.588887</v>
+        <v>-34.570279</v>
       </c>
       <c r="O28" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P28" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>5719</t>
+          <t>805707165</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>5/1/2025</t>
+          <t>5/7/2025</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>CABEZON, JOSE LEON 2440</t>
+          <t>Baez 793</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>805579157</t>
+          <t>805707165</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
@@ -2589,7 +2597,7 @@
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>DESMONTAR COLUMNA DE 7 MTS Y TRANSFERIR A COMUNITARIA</t>
         </is>
       </c>
       <c r="I29" t="n">
@@ -2607,50 +2615,50 @@
       </c>
       <c r="L29" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M29" t="n">
-        <v>-58.499967</v>
+        <v>-58.436165</v>
       </c>
       <c r="N29" t="n">
-        <v>-34.57974</v>
+        <v>-34.569081</v>
       </c>
       <c r="O29" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P29" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>6333</t>
+          <t>5847</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>5/1/2025</t>
+          <t>5/8/2025</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>ORTEGA Y GASSET 1816</t>
+          <t>JURAMENTO 5321</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>805655342</t>
+          <t>805791839</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
@@ -2687,36 +2695,36 @@
         </is>
       </c>
       <c r="M30" t="n">
-        <v>-58.432556</v>
+        <v>-58.485193</v>
       </c>
       <c r="N30" t="n">
-        <v>-34.570279</v>
+        <v>-34.579621</v>
       </c>
       <c r="O30" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P30" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>805707165</t>
+          <t>232</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>5/7/2025</t>
+          <t>5/9/2025</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Baez 793</t>
+          <t>Gorostiaga 2286</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
@@ -2726,7 +2734,7 @@
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>805707165</t>
+          <t>805791858</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
@@ -2741,7 +2749,7 @@
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>DESMONTAR COLUMNA DE 7 MTS Y TRANSFERIR A COMUNITARIA</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I31" t="n">
@@ -2759,14 +2767,14 @@
       </c>
       <c r="L31" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M31" t="n">
-        <v>-58.436165</v>
+        <v>-58.441563</v>
       </c>
       <c r="N31" t="n">
-        <v>-34.569081</v>
+        <v>-34.569743</v>
       </c>
       <c r="O31" t="inlineStr">
         <is>
@@ -2782,7 +2790,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>5847</t>
+          <t>-406</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
@@ -2792,7 +2800,7 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>JURAMENTO 5321</t>
+          <t>Olof palme 4144</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
@@ -2802,7 +2810,7 @@
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>805791839</t>
+          <t>805791925</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
@@ -2817,7 +2825,7 @@
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Tensar 2 riendas a pique columna 168</t>
         </is>
       </c>
       <c r="I32" t="n">
@@ -2825,7 +2833,7 @@
       </c>
       <c r="J32" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Tensor</t>
         </is>
       </c>
       <c r="K32" t="inlineStr">
@@ -2835,18 +2843,18 @@
       </c>
       <c r="L32" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M32" t="n">
-        <v>-58.485193</v>
+        <v>-58.488252</v>
       </c>
       <c r="N32" t="n">
-        <v>-34.579621</v>
+        <v>-34.553391</v>
       </c>
       <c r="O32" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P32" t="inlineStr">
@@ -2858,27 +2866,27 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>232</t>
+          <t>5826</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>5/9/2025</t>
+          <t>5/19/2025</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Gorostiaga 2286</t>
+          <t>ALBARELLOS AV. 3180</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>805791858</t>
+          <t>806926466</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
@@ -2893,7 +2901,7 @@
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Columna (metal) inclinada</t>
         </is>
       </c>
       <c r="I33" t="n">
@@ -2901,7 +2909,7 @@
       </c>
       <c r="J33" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K33" t="inlineStr">
@@ -2911,40 +2919,40 @@
       </c>
       <c r="L33" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M33" t="n">
-        <v>-58.441563</v>
+        <v>-58.513552</v>
       </c>
       <c r="N33" t="n">
-        <v>-34.569743</v>
+        <v>-34.579829</v>
       </c>
       <c r="O33" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P33" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>-406</t>
+          <t>5825</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>5/8/2025</t>
+          <t>5/19/2025</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Olof palme 4144</t>
+          <t>PAZ, GRAL. AV. 5602</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
@@ -2954,7 +2962,7 @@
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>805791925</t>
+          <t>806926472</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
@@ -2969,7 +2977,7 @@
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>Tensar 2 riendas a pique columna 168</t>
+          <t>reparar rienda cortada - ver foto no es la misma que albarellos</t>
         </is>
       </c>
       <c r="I34" t="n">
@@ -2991,14 +2999,14 @@
         </is>
       </c>
       <c r="M34" t="n">
-        <v>-58.488252</v>
+        <v>-58.513685</v>
       </c>
       <c r="N34" t="n">
-        <v>-34.553391</v>
+        <v>-34.579838</v>
       </c>
       <c r="O34" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P34" t="inlineStr">
@@ -3010,27 +3018,27 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>5826</t>
+          <t>807044192</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>5/19/2025</t>
+          <t>5/29/2025</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>ALBARELLOS AV. 3180</t>
+          <t>O'Higgins 4379</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>806926466</t>
+          <t>807044192</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
@@ -3045,7 +3053,7 @@
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>Columna (metal) inclinada</t>
+          <t xml:space="preserve">Poste </t>
         </is>
       </c>
       <c r="I35" t="n">
@@ -3053,7 +3061,7 @@
       </c>
       <c r="J35" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Desmonte</t>
         </is>
       </c>
       <c r="K35" t="inlineStr">
@@ -3063,18 +3071,18 @@
       </c>
       <c r="L35" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M35" t="n">
-        <v>-58.513552</v>
+        <v>-58.468425</v>
       </c>
       <c r="N35" t="n">
-        <v>-34.579829</v>
+        <v>-34.54124</v>
       </c>
       <c r="O35" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P35" t="inlineStr">
@@ -3086,27 +3094,27 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>5825</t>
+          <t>6020</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>5/19/2025</t>
+          <t>6/5/2025</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>PAZ, GRAL. AV. 5602</t>
+          <t>RAVIGNANI, EMILIO, DR. 2036</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>806926472</t>
+          <t>807215465</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
@@ -3121,7 +3129,7 @@
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>reparar rienda cortada - ver foto no es la misma que albarellos</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I36" t="n">
@@ -3129,7 +3137,7 @@
       </c>
       <c r="J36" t="inlineStr">
         <is>
-          <t>Tensor</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K36" t="inlineStr">
@@ -3139,50 +3147,50 @@
       </c>
       <c r="L36" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M36" t="n">
-        <v>-58.513685</v>
+        <v>-58.436298</v>
       </c>
       <c r="N36" t="n">
-        <v>-34.579838</v>
+        <v>-34.578972</v>
       </c>
       <c r="O36" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P36" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>807044192</t>
+          <t>6144</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>5/29/2025</t>
+          <t>6/11/2025</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>O'Higgins 4379</t>
+          <t>TURIN 2990</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>807044192</t>
+          <t>807458282</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
@@ -3197,7 +3205,7 @@
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t xml:space="preserve">Poste </t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I37" t="n">
@@ -3205,7 +3213,7 @@
       </c>
       <c r="J37" t="inlineStr">
         <is>
-          <t>Desmonte</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K37" t="inlineStr">
@@ -3215,18 +3223,18 @@
       </c>
       <c r="L37" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M37" t="n">
-        <v>-58.468425</v>
+        <v>-58.480925</v>
       </c>
       <c r="N37" t="n">
-        <v>-34.54124</v>
+        <v>-34.585471</v>
       </c>
       <c r="O37" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P37" t="inlineStr">
@@ -3238,27 +3246,27 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>6020</t>
+          <t>6143</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>6/5/2025</t>
+          <t>6/11/2025</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>RAVIGNANI, EMILIO, DR. 2036</t>
+          <t>SOLANO LOPEZ, F., MARISCAL 2845</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>807215465</t>
+          <t>807458296</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
@@ -3295,26 +3303,26 @@
         </is>
       </c>
       <c r="M38" t="n">
-        <v>-58.436298</v>
+        <v>-58.495071</v>
       </c>
       <c r="N38" t="n">
-        <v>-34.578972</v>
+        <v>-34.593122</v>
       </c>
       <c r="O38" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P38" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>6144</t>
+          <t>6141</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
@@ -3324,17 +3332,17 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>TURIN 2990</t>
+          <t>EL PAMPERO 2618</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>807458282</t>
+          <t>807458310</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
@@ -3371,10 +3379,10 @@
         </is>
       </c>
       <c r="M39" t="n">
-        <v>-58.480925</v>
+        <v>-58.481942</v>
       </c>
       <c r="N39" t="n">
-        <v>-34.585471</v>
+        <v>-34.602989</v>
       </c>
       <c r="O39" t="inlineStr">
         <is>
@@ -3390,27 +3398,27 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>6143</t>
+          <t>-478</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>6/11/2025</t>
+          <t>6/15/2025</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>SOLANO LOPEZ, F., MARISCAL 2845</t>
+          <t>Chivilcoy 4875</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>807458296</t>
+          <t>807508509</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
@@ -3425,7 +3433,7 @@
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Poste podrido</t>
         </is>
       </c>
       <c r="I40" t="n">
@@ -3443,14 +3451,14 @@
       </c>
       <c r="L40" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M40" t="n">
-        <v>-58.495071</v>
+        <v>-58.517389</v>
       </c>
       <c r="N40" t="n">
-        <v>-34.593122</v>
+        <v>-34.593541</v>
       </c>
       <c r="O40" t="inlineStr">
         <is>
@@ -3466,27 +3474,27 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>6141</t>
+          <t>6171</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>6/11/2025</t>
+          <t>6/18/2025</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>EL PAMPERO 2618</t>
+          <t>CABELLO 3486</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>807458310</t>
+          <t>807658640</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
@@ -3501,7 +3509,7 @@
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Columna inclinada evaluar con inspector un corrimiento</t>
         </is>
       </c>
       <c r="I41" t="n">
@@ -3523,46 +3531,46 @@
         </is>
       </c>
       <c r="M41" t="n">
-        <v>-58.481942</v>
+        <v>-58.409579</v>
       </c>
       <c r="N41" t="n">
-        <v>-34.602989</v>
+        <v>-34.581134</v>
       </c>
       <c r="O41" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P41" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>-478</t>
+          <t>6230</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>6/15/2025</t>
+          <t>6/24/2025</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Chivilcoy 4875</t>
+          <t>Santa maria de oro	2722</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>807508509</t>
+          <t>807763066</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
@@ -3577,7 +3585,7 @@
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>Poste podrido</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I42" t="n">
@@ -3595,40 +3603,40 @@
       </c>
       <c r="L42" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M42" t="n">
-        <v>-58.517389</v>
+        <v>-58.422315</v>
       </c>
       <c r="N42" t="n">
-        <v>-34.593541</v>
+        <v>-34.576988</v>
       </c>
       <c r="O42" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P42" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>6171</t>
+          <t>6231</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>6/18/2025</t>
+          <t>6/24/2025</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>CABELLO 3486</t>
+          <t>Ciudad de la Paz 275</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
@@ -3638,7 +3646,7 @@
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>807658640</t>
+          <t>807763070</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
@@ -3653,7 +3661,7 @@
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>Columna inclinada evaluar con inspector un corrimiento</t>
+          <t>Aplomar o cambiar</t>
         </is>
       </c>
       <c r="I43" t="n">
@@ -3671,14 +3679,14 @@
       </c>
       <c r="L43" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M43" t="n">
-        <v>-58.409579</v>
+        <v>-58.441049</v>
       </c>
       <c r="N43" t="n">
-        <v>-34.581134</v>
+        <v>-34.574625</v>
       </c>
       <c r="O43" t="inlineStr">
         <is>
@@ -3694,7 +3702,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>6230</t>
+          <t>6235</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
@@ -3704,17 +3712,17 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Santa maria de oro	2722</t>
+          <t>HUERGO 389</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>807763066</t>
+          <t>807763078</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
@@ -3751,10 +3759,10 @@
         </is>
       </c>
       <c r="M44" t="n">
-        <v>-58.422315</v>
+        <v>-58.432722</v>
       </c>
       <c r="N44" t="n">
-        <v>-34.576988</v>
+        <v>-34.572371</v>
       </c>
       <c r="O44" t="inlineStr">
         <is>
@@ -3770,17 +3778,17 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>6231</t>
+          <t>6295</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>6/24/2025</t>
+          <t>6/30/2025</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Ciudad de la Paz 275</t>
+          <t>SOLER 6017</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
@@ -3790,7 +3798,7 @@
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>807763070</t>
+          <t>807851636</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
@@ -3805,7 +3813,7 @@
       </c>
       <c r="H45" t="inlineStr">
         <is>
-          <t>Aplomar o cambiar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I45" t="n">
@@ -3823,14 +3831,14 @@
       </c>
       <c r="L45" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M45" t="n">
-        <v>-58.441049</v>
+        <v>-58.436808</v>
       </c>
       <c r="N45" t="n">
-        <v>-34.574625</v>
+        <v>-34.577464</v>
       </c>
       <c r="O45" t="inlineStr">
         <is>
@@ -3846,27 +3854,27 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>6235</t>
+          <t>6332</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>6/24/2025</t>
+          <t>7/3/2025</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>HUERGO 389</t>
+          <t>ARAOZ 2560</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>807763078</t>
+          <t>807965818</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
@@ -3903,10 +3911,10 @@
         </is>
       </c>
       <c r="M46" t="n">
-        <v>-58.432722</v>
+        <v>-58.414507</v>
       </c>
       <c r="N46" t="n">
-        <v>-34.572371</v>
+        <v>-34.585377</v>
       </c>
       <c r="O46" t="inlineStr">
         <is>
@@ -3922,27 +3930,27 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>6295</t>
+          <t>6363</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>6/30/2025</t>
+          <t>7/8/2025</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>SOLER 6017</t>
+          <t>MOLDES 3730</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>807851636</t>
+          <t>808099415</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
@@ -3957,7 +3965,7 @@
       </c>
       <c r="H47" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Poste inclinado</t>
         </is>
       </c>
       <c r="I47" t="n">
@@ -3965,7 +3973,7 @@
       </c>
       <c r="J47" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K47" t="inlineStr">
@@ -3975,50 +3983,50 @@
       </c>
       <c r="L47" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M47" t="n">
-        <v>-58.436808</v>
+        <v>-58.47192</v>
       </c>
       <c r="N47" t="n">
-        <v>-34.577464</v>
+        <v>-34.549398</v>
       </c>
       <c r="O47" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P47" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>6332</t>
+          <t>-503</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>7/3/2025</t>
+          <t>7/10/2025</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>ARAOZ 2560</t>
+          <t>Salguero 842</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>807965818</t>
+          <t>808148673</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
@@ -4033,7 +4041,7 @@
       </c>
       <c r="H48" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambiar columna picada en la base</t>
         </is>
       </c>
       <c r="I48" t="n">
@@ -4055,14 +4063,14 @@
         </is>
       </c>
       <c r="M48" t="n">
-        <v>-58.414507</v>
+        <v>-58.419166</v>
       </c>
       <c r="N48" t="n">
-        <v>-34.585377</v>
+        <v>-34.600265</v>
       </c>
       <c r="O48" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P48" t="inlineStr">
@@ -4074,27 +4082,27 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>6363</t>
+          <t>6506</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>7/8/2025</t>
+          <t>7/10/2025</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>MOLDES 3730</t>
+          <t>Ohiggins 1611</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>808099415</t>
+          <t>808148679</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
@@ -4109,7 +4117,7 @@
       </c>
       <c r="H49" t="inlineStr">
         <is>
-          <t>Poste inclinado</t>
+          <t>Columna podrida en la base</t>
         </is>
       </c>
       <c r="I49" t="n">
@@ -4117,28 +4125,28 @@
       </c>
       <c r="J49" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K49" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L49" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M49" t="n">
-        <v>-58.47192</v>
+        <v>-58.448993</v>
       </c>
       <c r="N49" t="n">
-        <v>-34.549398</v>
+        <v>-34.564383</v>
       </c>
       <c r="O49" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P49" t="inlineStr">
@@ -4150,27 +4158,27 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>-503</t>
+          <t>6437</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>7/10/2025</t>
+          <t>7/17/2025</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Salguero 842</t>
+          <t>MILLER 4590</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>808148673</t>
+          <t>808400306</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
@@ -4185,7 +4193,7 @@
       </c>
       <c r="H50" t="inlineStr">
         <is>
-          <t>Cambiar columna picada en la base</t>
+          <t>Columna corroida</t>
         </is>
       </c>
       <c r="I50" t="n">
@@ -4207,46 +4215,46 @@
         </is>
       </c>
       <c r="M50" t="n">
-        <v>-58.419166</v>
+        <v>-58.495482</v>
       </c>
       <c r="N50" t="n">
-        <v>-34.600265</v>
+        <v>-34.552614</v>
       </c>
       <c r="O50" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P50" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>6506</t>
+          <t>-519</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>7/10/2025</t>
+          <t>7/17/2025</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Ohiggins 1611</t>
+          <t>Vilela 2687</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>808148679</t>
+          <t>808400334</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
@@ -4261,7 +4269,7 @@
       </c>
       <c r="H51" t="inlineStr">
         <is>
-          <t>Columna podrida en la base</t>
+          <t>CAmbiar columna 114 picada en base</t>
         </is>
       </c>
       <c r="I51" t="n">
@@ -4274,7 +4282,7 @@
       </c>
       <c r="K51" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L51" t="inlineStr">
@@ -4283,14 +4291,14 @@
         </is>
       </c>
       <c r="M51" t="n">
-        <v>-58.448993</v>
+        <v>-58.472968</v>
       </c>
       <c r="N51" t="n">
-        <v>-34.564383</v>
+        <v>-34.546898</v>
       </c>
       <c r="O51" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P51" t="inlineStr">
@@ -4302,7 +4310,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>6437</t>
+          <t>6538</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
@@ -4312,7 +4320,7 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>MILLER 4590</t>
+          <t>Pedraza Manuela 4101</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
@@ -4322,7 +4330,7 @@
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>808400306</t>
+          <t>808400353</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
@@ -4337,7 +4345,7 @@
       </c>
       <c r="H52" t="inlineStr">
         <is>
-          <t>Columna corroida</t>
+          <t xml:space="preserve">Podrida en la base </t>
         </is>
       </c>
       <c r="I52" t="n">
@@ -4359,10 +4367,10 @@
         </is>
       </c>
       <c r="M52" t="n">
-        <v>-58.495482</v>
+        <v>-58.481569</v>
       </c>
       <c r="N52" t="n">
-        <v>-34.552614</v>
+        <v>-34.559853</v>
       </c>
       <c r="O52" t="inlineStr">
         <is>
@@ -4378,27 +4386,27 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>-519</t>
+          <t>-525</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>7/17/2025</t>
+          <t>7/22/2025</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>Vilela 2687</t>
+          <t>Zabala 3567</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>808400334</t>
+          <t>808480549</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
@@ -4413,7 +4421,7 @@
       </c>
       <c r="H53" t="inlineStr">
         <is>
-          <t>CAmbiar columna 114 picada en base</t>
+          <t>Corroida en base para recambio</t>
         </is>
       </c>
       <c r="I53" t="n">
@@ -4435,14 +4443,14 @@
         </is>
       </c>
       <c r="M53" t="n">
-        <v>-58.472968</v>
+        <v>-58.457492</v>
       </c>
       <c r="N53" t="n">
-        <v>-34.546898</v>
+        <v>-34.579336</v>
       </c>
       <c r="O53" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P53" t="inlineStr">
@@ -4454,27 +4462,27 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>6538</t>
+          <t>6484</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>7/17/2025</t>
+          <t>7/24/2025</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>Pedraza Manuela 4101</t>
+          <t>URIARTE 2396</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>808400353</t>
+          <t>808509373</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
@@ -4489,7 +4497,7 @@
       </c>
       <c r="H54" t="inlineStr">
         <is>
-          <t xml:space="preserve">Podrida en la base </t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I54" t="n">
@@ -4511,46 +4519,46 @@
         </is>
       </c>
       <c r="M54" t="n">
-        <v>-58.481569</v>
+        <v>-58.423934</v>
       </c>
       <c r="N54" t="n">
-        <v>-34.559853</v>
+        <v>-34.581562</v>
       </c>
       <c r="O54" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P54" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>-525</t>
+          <t>6512</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>7/22/2025</t>
+          <t>7/28/2025</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>Zabala 3567</t>
+          <t>GASCON 1195</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>808480549</t>
+          <t>808571975</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
@@ -4565,7 +4573,7 @@
       </c>
       <c r="H55" t="inlineStr">
         <is>
-          <t>Corroida en base para recambio</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I55" t="n">
@@ -4587,36 +4595,36 @@
         </is>
       </c>
       <c r="M55" t="n">
-        <v>-58.457492</v>
+        <v>-58.423127</v>
       </c>
       <c r="N55" t="n">
-        <v>-34.579336</v>
+        <v>-34.596476</v>
       </c>
       <c r="O55" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P55" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>6484</t>
+          <t>6513</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>7/24/2025</t>
+          <t>7/28/2025</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>URIARTE 2396</t>
+          <t>DORREGO 1925</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
@@ -4626,7 +4634,7 @@
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>808509373</t>
+          <t>808571976</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
@@ -4663,10 +4671,10 @@
         </is>
       </c>
       <c r="M56" t="n">
-        <v>-58.423934</v>
+        <v>-58.441281</v>
       </c>
       <c r="N56" t="n">
-        <v>-34.581562</v>
+        <v>-34.579867</v>
       </c>
       <c r="O56" t="inlineStr">
         <is>
@@ -4682,27 +4690,27 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>6504</t>
+          <t>6519</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>7/25/2025</t>
+          <t>7/28/2025</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>CIUDAD DE LA PAZ 1278</t>
+          <t>SALGUERO, JERONIMO 2874</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>808571974</t>
+          <t>808571977</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
@@ -4717,7 +4725,7 @@
       </c>
       <c r="H57" t="inlineStr">
         <is>
-          <t>Inclinada</t>
+          <t>Reparar rienda</t>
         </is>
       </c>
       <c r="I57" t="n">
@@ -4725,7 +4733,7 @@
       </c>
       <c r="J57" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Tensor</t>
         </is>
       </c>
       <c r="K57" t="inlineStr">
@@ -4735,50 +4743,50 @@
       </c>
       <c r="L57" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M57" t="n">
-        <v>-58.450753</v>
+        <v>-58.407256</v>
       </c>
       <c r="N57" t="n">
-        <v>-34.5688</v>
+        <v>-34.578976</v>
       </c>
       <c r="O57" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P57" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>6512</t>
+          <t>-536</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>7/28/2025</t>
+          <t>7/29/2025</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>GASCON 1195</t>
+          <t>Olof palme 4142</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>808571975</t>
+          <t xml:space="preserve">ICD30249764 </t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
@@ -4793,7 +4801,7 @@
       </c>
       <c r="H58" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Aplomar o desmontar poste</t>
         </is>
       </c>
       <c r="I58" t="n">
@@ -4801,7 +4809,7 @@
       </c>
       <c r="J58" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Desmonte</t>
         </is>
       </c>
       <c r="K58" t="inlineStr">
@@ -4811,50 +4819,50 @@
       </c>
       <c r="L58" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M58" t="n">
-        <v>-58.423127</v>
+        <v>-58.488239</v>
       </c>
       <c r="N58" t="n">
-        <v>-34.596476</v>
+        <v>-34.55341</v>
       </c>
       <c r="O58" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P58" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>6513</t>
+          <t>-538</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>7/28/2025</t>
+          <t>7/31/2025</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>DORREGO 1925</t>
+          <t>Malabia 964</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>808571976</t>
+          <t>808609237</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
@@ -4869,7 +4877,7 @@
       </c>
       <c r="H59" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambiar poste mal estado por PRFV</t>
         </is>
       </c>
       <c r="I59" t="n">
@@ -4887,14 +4895,14 @@
       </c>
       <c r="L59" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M59" t="n">
-        <v>-58.441281</v>
+        <v>-58.433634</v>
       </c>
       <c r="N59" t="n">
-        <v>-34.579867</v>
+        <v>-34.595018</v>
       </c>
       <c r="O59" t="inlineStr">
         <is>
@@ -4910,27 +4918,27 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>6519</t>
+          <t>6545</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>7/28/2025</t>
+          <t>8/4/2025</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>SALGUERO, JERONIMO 2874</t>
+          <t>SCALABRINI ORTIZ, RAUL AV. 708</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>808571977</t>
+          <t>808703864</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
@@ -4945,7 +4953,7 @@
       </c>
       <c r="H60" t="inlineStr">
         <is>
-          <t>Reparar rienda</t>
+          <t>Aplomar</t>
         </is>
       </c>
       <c r="I60" t="n">
@@ -4953,7 +4961,7 @@
       </c>
       <c r="J60" t="inlineStr">
         <is>
-          <t>Tensor</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K60" t="inlineStr">
@@ -4963,14 +4971,14 @@
       </c>
       <c r="L60" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M60" t="n">
-        <v>-58.407256</v>
+        <v>-58.434339</v>
       </c>
       <c r="N60" t="n">
-        <v>-34.578976</v>
+        <v>-34.59693</v>
       </c>
       <c r="O60" t="inlineStr">
         <is>
@@ -4978,158 +4986,6 @@
         </is>
       </c>
       <c r="P60" t="inlineStr">
-        <is>
-          <t>Capital Sur</t>
-        </is>
-      </c>
-    </row>
-    <row r="61">
-      <c r="A61" t="inlineStr">
-        <is>
-          <t>-536</t>
-        </is>
-      </c>
-      <c r="B61" t="inlineStr">
-        <is>
-          <t>7/29/2025</t>
-        </is>
-      </c>
-      <c r="C61" t="inlineStr">
-        <is>
-          <t>Olof palme 4142</t>
-        </is>
-      </c>
-      <c r="D61" t="inlineStr">
-        <is>
-          <t>12</t>
-        </is>
-      </c>
-      <c r="E61" t="inlineStr">
-        <is>
-          <t xml:space="preserve">ICD30249764 </t>
-        </is>
-      </c>
-      <c r="F61" t="inlineStr">
-        <is>
-          <t>NEW</t>
-        </is>
-      </c>
-      <c r="G61" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H61" t="inlineStr">
-        <is>
-          <t>Aplomar o desmontar poste</t>
-        </is>
-      </c>
-      <c r="I61" t="n">
-        <v>1</v>
-      </c>
-      <c r="J61" t="inlineStr">
-        <is>
-          <t>Desmonte</t>
-        </is>
-      </c>
-      <c r="K61" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L61" t="inlineStr">
-        <is>
-          <t>Poste</t>
-        </is>
-      </c>
-      <c r="M61" t="n">
-        <v>-58.488239</v>
-      </c>
-      <c r="N61" t="n">
-        <v>-34.55341</v>
-      </c>
-      <c r="O61" t="inlineStr">
-        <is>
-          <t>Saavedra</t>
-        </is>
-      </c>
-      <c r="P61" t="inlineStr">
-        <is>
-          <t>Capital Norte</t>
-        </is>
-      </c>
-    </row>
-    <row r="62">
-      <c r="A62" t="inlineStr">
-        <is>
-          <t>-538</t>
-        </is>
-      </c>
-      <c r="B62" t="inlineStr">
-        <is>
-          <t>7/31/2025</t>
-        </is>
-      </c>
-      <c r="C62" t="inlineStr">
-        <is>
-          <t>Malabia 964</t>
-        </is>
-      </c>
-      <c r="D62" t="inlineStr">
-        <is>
-          <t>15</t>
-        </is>
-      </c>
-      <c r="E62" t="inlineStr">
-        <is>
-          <t>808609237</t>
-        </is>
-      </c>
-      <c r="F62" t="inlineStr">
-        <is>
-          <t>NEW</t>
-        </is>
-      </c>
-      <c r="G62" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H62" t="inlineStr">
-        <is>
-          <t>Cambiar poste mal estado por PRFV</t>
-        </is>
-      </c>
-      <c r="I62" t="n">
-        <v>1</v>
-      </c>
-      <c r="J62" t="inlineStr">
-        <is>
-          <t>Cambio</t>
-        </is>
-      </c>
-      <c r="K62" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L62" t="inlineStr">
-        <is>
-          <t>Poste</t>
-        </is>
-      </c>
-      <c r="M62" t="n">
-        <v>-58.433634</v>
-      </c>
-      <c r="N62" t="n">
-        <v>-34.595018</v>
-      </c>
-      <c r="O62" t="inlineStr">
-        <is>
-          <t>Palermo</t>
-        </is>
-      </c>
-      <c r="P62" t="inlineStr">
         <is>
           <t>Capital Sur</t>
         </is>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-08-06 07:06:00)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_NEW.xlsx
+++ b/mapa_interactivo_NEW.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P60"/>
+  <dimension ref="A1:P62"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -822,17 +822,17 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>4595</t>
+          <t>5589</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>1/15/2025</t>
+          <t>12/31/2023</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>PAROISSIEN 1806</t>
+          <t>ARCOS 1520</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -842,7 +842,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>802747617</t>
+          <t>799540526</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -852,41 +852,33 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>Aplomar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I6" t="n">
-        <v>1</v>
-      </c>
-      <c r="J6" t="inlineStr">
-        <is>
-          <t>Aplomo</t>
-        </is>
-      </c>
-      <c r="K6" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="J6" t="inlineStr"/>
+      <c r="K6" t="inlineStr"/>
       <c r="L6" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M6" t="n">
-        <v>-58.464172</v>
+        <v>-58.449125</v>
       </c>
       <c r="N6" t="n">
-        <v>-34.543845</v>
+        <v>-34.565958</v>
       </c>
       <c r="O6" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P6" t="inlineStr">
@@ -898,27 +890,27 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>4662</t>
+          <t>4595</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>1/21/2025</t>
+          <t>1/15/2025</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>ALTOLAGUIRRE 2397</t>
+          <t>PAROISSIEN 1806</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>802823938</t>
+          <t>802747617</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -933,7 +925,7 @@
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>Inclinada</t>
+          <t>Aplomar</t>
         </is>
       </c>
       <c r="I7" t="n">
@@ -951,18 +943,18 @@
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M7" t="n">
-        <v>-58.490766</v>
+        <v>-58.464172</v>
       </c>
       <c r="N7" t="n">
-        <v>-34.576987</v>
+        <v>-34.543845</v>
       </c>
       <c r="O7" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P7" t="inlineStr">
@@ -974,27 +966,27 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>6036</t>
+          <t>4662</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>2/24/2025</t>
+          <t>1/21/2025</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>MEDRANO 1715</t>
+          <t>ALTOLAGUIRRE 2397</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>803608181</t>
+          <t>802823938</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -1007,18 +999,22 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H8" t="inlineStr"/>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>Inclinada</t>
+        </is>
+      </c>
       <c r="I8" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L8" t="inlineStr">
@@ -1027,46 +1023,46 @@
         </is>
       </c>
       <c r="M8" t="n">
-        <v>-58.418236</v>
+        <v>-58.490766</v>
       </c>
       <c r="N8" t="n">
-        <v>-34.589859</v>
+        <v>-34.576987</v>
       </c>
       <c r="O8" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P8" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>803608480</t>
+          <t>4862</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>2/24/2025</t>
+          <t>1/23/2025</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>GUATEMALA /ALT/ 4415</t>
+          <t>ARCOS 2263</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>803608480</t>
+          <t>802857379</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -1076,12 +1072,12 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t xml:space="preserve">Guatemala 4415 </t>
+          <t>picada</t>
         </is>
       </c>
       <c r="I9" t="n">
@@ -1094,7 +1090,7 @@
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L9" t="inlineStr">
@@ -1103,46 +1099,46 @@
         </is>
       </c>
       <c r="M9" t="n">
-        <v>-58.421661</v>
+        <v>-58.455082</v>
       </c>
       <c r="N9" t="n">
-        <v>-34.588428</v>
+        <v>-34.558883</v>
       </c>
       <c r="O9" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P9" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>5053</t>
+          <t>6036</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>3/11/2025</t>
+          <t>2/24/2025</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>MENDOZA 1153</t>
+          <t>MEDRANO 1715</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>803969314</t>
+          <t>803608181</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
@@ -1155,11 +1151,7 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H10" t="inlineStr">
-        <is>
-          <t>Poste</t>
-        </is>
-      </c>
+      <c r="H10" t="inlineStr"/>
       <c r="I10" t="n">
         <v>0</v>
       </c>
@@ -1170,55 +1162,55 @@
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L10" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M10" t="n">
-        <v>-58.44463</v>
+        <v>-58.418236</v>
       </c>
       <c r="N10" t="n">
-        <v>-34.553354</v>
+        <v>-34.589859</v>
       </c>
       <c r="O10" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P10" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>6071</t>
+          <t>803608480</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>3/17/2025</t>
+          <t>2/24/2025</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>OSORIO 4994</t>
+          <t>GUATEMALA /ALT/ 4415</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>804053324</t>
+          <t>803608480</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
@@ -1231,7 +1223,11 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H11" t="inlineStr"/>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Guatemala 4415 </t>
+        </is>
+      </c>
       <c r="I11" t="n">
         <v>0</v>
       </c>
@@ -1251,46 +1247,46 @@
         </is>
       </c>
       <c r="M11" t="n">
-        <v>-58.466241</v>
+        <v>-58.421661</v>
       </c>
       <c r="N11" t="n">
-        <v>-34.595741</v>
+        <v>-34.588428</v>
       </c>
       <c r="O11" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P11" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>3348</t>
+          <t>5053</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>3/27/2025</t>
+          <t>3/11/2025</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>ESTOMBA 2626</t>
+          <t>MENDOZA 1153</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>804309704</t>
+          <t>803969314</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
@@ -1305,15 +1301,15 @@
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="I12" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>Desmonte</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K12" t="inlineStr">
@@ -1323,18 +1319,18 @@
       </c>
       <c r="L12" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M12" t="n">
-        <v>-58.47538</v>
+        <v>-58.44463</v>
       </c>
       <c r="N12" t="n">
-        <v>-34.566015</v>
+        <v>-34.553354</v>
       </c>
       <c r="O12" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P12" t="inlineStr">
@@ -1346,27 +1342,27 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>-312</t>
+          <t>6071</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>3/29/2025</t>
+          <t>3/17/2025</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>MATIENZO BENJAMIN /ALT/ 1831</t>
+          <t>OSORIO 4994</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>804333522</t>
+          <t>804053324</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
@@ -1379,11 +1375,7 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H13" t="inlineStr">
-        <is>
-          <t>Retirar columna ya traspasaron el nodo</t>
-        </is>
-      </c>
+      <c r="H13" t="inlineStr"/>
       <c r="I13" t="n">
         <v>0</v>
       </c>
@@ -1394,7 +1386,7 @@
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L13" t="inlineStr">
@@ -1403,36 +1395,36 @@
         </is>
       </c>
       <c r="M13" t="n">
-        <v>-58.434835</v>
+        <v>-58.466241</v>
       </c>
       <c r="N13" t="n">
-        <v>-34.569129</v>
+        <v>-34.595741</v>
       </c>
       <c r="O13" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P13" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>3430</t>
+          <t>3348</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>4/1/2025</t>
+          <t>3/27/2025</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>MONROE 3838</t>
+          <t>ESTOMBA 2626</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
@@ -1442,7 +1434,7 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>804468442</t>
+          <t>804309704</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
@@ -1457,7 +1449,7 @@
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>Reparar rienda</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I14" t="n">
@@ -1465,7 +1457,7 @@
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>Tensor</t>
+          <t>Desmonte</t>
         </is>
       </c>
       <c r="K14" t="inlineStr">
@@ -1475,14 +1467,14 @@
       </c>
       <c r="L14" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M14" t="n">
-        <v>-58.473659</v>
+        <v>-58.47538</v>
       </c>
       <c r="N14" t="n">
-        <v>-34.566979</v>
+        <v>-34.566015</v>
       </c>
       <c r="O14" t="inlineStr">
         <is>
@@ -1498,27 +1490,27 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>5464</t>
+          <t>-312</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>4/4/2025</t>
+          <t>3/29/2025</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>SUCRE, ANTONIO JOSE DE, MCAL. 3100</t>
+          <t>MATIENZO BENJAMIN /ALT/ 1831</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>804497880</t>
+          <t>804333522</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
@@ -1533,11 +1525,11 @@
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Retirar columna ya traspasaron el nodo</t>
         </is>
       </c>
       <c r="I15" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J15" t="inlineStr">
         <is>
@@ -1546,45 +1538,45 @@
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L15" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M15" t="n">
-        <v>-58.46161</v>
+        <v>-58.434835</v>
       </c>
       <c r="N15" t="n">
-        <v>-34.567849</v>
+        <v>-34.569129</v>
       </c>
       <c r="O15" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P15" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>5469</t>
+          <t>3430</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>4/4/2025</t>
+          <t>4/1/2025</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>ESTADO PLURINACIONAL DE BOLIVIA 5899</t>
+          <t>MONROE 3838</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
@@ -1594,7 +1586,7 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>804497887</t>
+          <t>804468442</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
@@ -1609,7 +1601,7 @@
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>Aplomar</t>
+          <t>Reparar rienda</t>
         </is>
       </c>
       <c r="I16" t="n">
@@ -1617,7 +1609,7 @@
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Tensor</t>
         </is>
       </c>
       <c r="K16" t="inlineStr">
@@ -1631,14 +1623,14 @@
         </is>
       </c>
       <c r="M16" t="n">
-        <v>-58.507746</v>
+        <v>-58.473659</v>
       </c>
       <c r="N16" t="n">
-        <v>-34.574217</v>
+        <v>-34.566979</v>
       </c>
       <c r="O16" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P16" t="inlineStr">
@@ -1650,7 +1642,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>5492</t>
+          <t>5464</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -1660,17 +1652,17 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>ESTADO PLURINACIONAL DE BOLIVIA 5920</t>
+          <t>SUCRE, ANTONIO JOSE DE, MCAL. 3100</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>804498035</t>
+          <t>804497880</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
@@ -1685,7 +1677,7 @@
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>aplomar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I17" t="n">
@@ -1693,7 +1685,7 @@
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K17" t="inlineStr">
@@ -1707,14 +1699,14 @@
         </is>
       </c>
       <c r="M17" t="n">
-        <v>-58.50751</v>
+        <v>-58.46161</v>
       </c>
       <c r="N17" t="n">
-        <v>-34.574543</v>
+        <v>-34.567849</v>
       </c>
       <c r="O17" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P17" t="inlineStr">
@@ -1726,17 +1718,17 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>5599</t>
+          <t>5469</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>4/15/2025</t>
+          <t>4/4/2025</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>ESTOMBA 4052</t>
+          <t>ESTADO PLURINACIONAL DE BOLIVIA 5899</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
@@ -1746,7 +1738,7 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>804732246</t>
+          <t>804497887</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
@@ -1761,7 +1753,7 @@
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>Columna PRFV quedo inclinada (la hicieron como estomba 4056)</t>
+          <t>Aplomar</t>
         </is>
       </c>
       <c r="I18" t="n">
@@ -1774,23 +1766,23 @@
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>Nodo TLC</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L18" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M18" t="n">
-        <v>-58.485407</v>
+        <v>-58.507746</v>
       </c>
       <c r="N18" t="n">
-        <v>-34.552985</v>
+        <v>-34.574217</v>
       </c>
       <c r="O18" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P18" t="inlineStr">
@@ -1802,27 +1794,27 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>5590</t>
+          <t>5492</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>4/15/2025</t>
+          <t>4/4/2025</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>O'HIGGINS 2441</t>
+          <t>ESTADO PLURINACIONAL DE BOLIVIA 5920</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>804732275</t>
+          <t>804498035</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
@@ -1837,7 +1829,7 @@
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>aplomar</t>
         </is>
       </c>
       <c r="I19" t="n">
@@ -1845,7 +1837,7 @@
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K19" t="inlineStr">
@@ -1855,18 +1847,18 @@
       </c>
       <c r="L19" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M19" t="n">
-        <v>-58.45573</v>
+        <v>-58.50751</v>
       </c>
       <c r="N19" t="n">
-        <v>-34.556576</v>
+        <v>-34.574543</v>
       </c>
       <c r="O19" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P19" t="inlineStr">
@@ -1878,27 +1870,27 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>804787368</t>
+          <t>5599</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>4/17/2025</t>
+          <t>4/15/2025</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>San Blas 2591</t>
+          <t>ESTOMBA 4052</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>804787368</t>
+          <t>804732246</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
@@ -1913,7 +1905,7 @@
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Columna PRFV quedo inclinada (la hicieron como estomba 4056)</t>
         </is>
       </c>
       <c r="I20" t="n">
@@ -1921,12 +1913,12 @@
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo TLC</t>
         </is>
       </c>
       <c r="L20" t="inlineStr">
@@ -1935,14 +1927,14 @@
         </is>
       </c>
       <c r="M20" t="n">
-        <v>-58.477427</v>
+        <v>-58.485407</v>
       </c>
       <c r="N20" t="n">
-        <v>-34.609261</v>
+        <v>-34.552985</v>
       </c>
       <c r="O20" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P20" t="inlineStr">
@@ -1954,17 +1946,17 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>5624</t>
+          <t>5590</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>4/22/2025</t>
+          <t>4/15/2025</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>PINO, VIRREY DEL 3456</t>
+          <t>O'HIGGINS 2441</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
@@ -1974,7 +1966,7 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>804876043</t>
+          <t>804732275</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
@@ -1989,7 +1981,7 @@
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>Desmonte de poste</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I21" t="n">
@@ -1997,7 +1989,7 @@
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>Desmonte</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K21" t="inlineStr">
@@ -2007,18 +1999,18 @@
       </c>
       <c r="L21" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M21" t="n">
-        <v>-58.464354</v>
+        <v>-58.45573</v>
       </c>
       <c r="N21" t="n">
-        <v>-34.572486</v>
+        <v>-34.556576</v>
       </c>
       <c r="O21" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P21" t="inlineStr">
@@ -2030,27 +2022,27 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>804922147</t>
+          <t>804787368</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>4/24/2025</t>
+          <t>4/17/2025</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Av. Álvarez Thomas 1171</t>
+          <t>San Blas 2591</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>804922147</t>
+          <t>804787368</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
@@ -2069,7 +2061,7 @@
         </is>
       </c>
       <c r="I22" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J22" t="inlineStr">
         <is>
@@ -2087,14 +2079,14 @@
         </is>
       </c>
       <c r="M22" t="n">
-        <v>-58.45793</v>
+        <v>-58.477427</v>
       </c>
       <c r="N22" t="n">
-        <v>-34.578334</v>
+        <v>-34.609261</v>
       </c>
       <c r="O22" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P22" t="inlineStr">
@@ -2106,17 +2098,17 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>804922171</t>
+          <t>5624</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>4/24/2025</t>
+          <t>4/22/2025</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Virrey Arredondo 3581</t>
+          <t>PINO, VIRREY DEL 3456</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
@@ -2126,7 +2118,7 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>804922171</t>
+          <t>804876043</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
@@ -2141,7 +2133,7 @@
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>Aplomar</t>
+          <t>Desmonte de poste</t>
         </is>
       </c>
       <c r="I23" t="n">
@@ -2149,7 +2141,7 @@
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Desmonte</t>
         </is>
       </c>
       <c r="K23" t="inlineStr">
@@ -2159,14 +2151,14 @@
       </c>
       <c r="L23" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M23" t="n">
-        <v>-58.459513</v>
+        <v>-58.464354</v>
       </c>
       <c r="N23" t="n">
-        <v>-34.578019</v>
+        <v>-34.572486</v>
       </c>
       <c r="O23" t="inlineStr">
         <is>
@@ -2182,7 +2174,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>5656</t>
+          <t>804922147</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -2192,17 +2184,17 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>ECHEVERRIA 5893</t>
+          <t>Av. Álvarez Thomas 1171</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>804922184</t>
+          <t>804922147</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
@@ -2217,15 +2209,15 @@
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>Poste con base quebrada</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I24" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J24" t="inlineStr">
         <is>
-          <t>Desmonte</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K24" t="inlineStr">
@@ -2235,18 +2227,18 @@
       </c>
       <c r="L24" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M24" t="n">
-        <v>-58.489627</v>
+        <v>-58.45793</v>
       </c>
       <c r="N24" t="n">
-        <v>-34.583761</v>
+        <v>-34.578334</v>
       </c>
       <c r="O24" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P24" t="inlineStr">
@@ -2258,27 +2250,27 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>6173</t>
+          <t>804922171</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>4/29/2025</t>
+          <t>4/24/2025</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>ARMENIA 2321</t>
+          <t>Virrey Arredondo 3581</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>805507398</t>
+          <t>804922171</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
@@ -2293,7 +2285,7 @@
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>Picada volvio a entrar como caso 6325</t>
+          <t>Aplomar</t>
         </is>
       </c>
       <c r="I25" t="n">
@@ -2301,7 +2293,7 @@
       </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K25" t="inlineStr">
@@ -2311,40 +2303,40 @@
       </c>
       <c r="L25" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M25" t="n">
-        <v>-58.420549</v>
+        <v>-58.459513</v>
       </c>
       <c r="N25" t="n">
-        <v>-34.585103</v>
+        <v>-34.578019</v>
       </c>
       <c r="O25" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P25" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>5715</t>
+          <t>5656</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>5/1/2025</t>
+          <t>4/24/2025</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>CUENCA 4690</t>
+          <t>ECHEVERRIA 5893</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
@@ -2354,7 +2346,7 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>805579094</t>
+          <t>804922184</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
@@ -2369,7 +2361,7 @@
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>Aplomar poste</t>
+          <t>Poste con base quebrada</t>
         </is>
       </c>
       <c r="I26" t="n">
@@ -2377,7 +2369,7 @@
       </c>
       <c r="J26" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Desmonte</t>
         </is>
       </c>
       <c r="K26" t="inlineStr">
@@ -2391,10 +2383,10 @@
         </is>
       </c>
       <c r="M26" t="n">
-        <v>-58.506061</v>
+        <v>-58.489627</v>
       </c>
       <c r="N26" t="n">
-        <v>-34.588887</v>
+        <v>-34.583761</v>
       </c>
       <c r="O26" t="inlineStr">
         <is>
@@ -2410,27 +2402,27 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>5719</t>
+          <t>6173</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>5/1/2025</t>
+          <t>4/29/2025</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>CABEZON, JOSE LEON 2440</t>
+          <t>ARMENIA 2321</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>805579157</t>
+          <t>805507398</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
@@ -2445,7 +2437,7 @@
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Picada volvio a entrar como caso 6325</t>
         </is>
       </c>
       <c r="I27" t="n">
@@ -2467,26 +2459,26 @@
         </is>
       </c>
       <c r="M27" t="n">
-        <v>-58.499967</v>
+        <v>-58.420549</v>
       </c>
       <c r="N27" t="n">
-        <v>-34.57974</v>
+        <v>-34.585103</v>
       </c>
       <c r="O27" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P27" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>6333</t>
+          <t>5715</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -2496,17 +2488,17 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>ORTEGA Y GASSET 1816</t>
+          <t>CUENCA 4690</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>805655342</t>
+          <t>805579094</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
@@ -2521,7 +2513,7 @@
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Aplomar poste</t>
         </is>
       </c>
       <c r="I28" t="n">
@@ -2529,7 +2521,7 @@
       </c>
       <c r="J28" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K28" t="inlineStr">
@@ -2539,50 +2531,50 @@
       </c>
       <c r="L28" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M28" t="n">
-        <v>-58.432556</v>
+        <v>-58.506061</v>
       </c>
       <c r="N28" t="n">
-        <v>-34.570279</v>
+        <v>-34.588887</v>
       </c>
       <c r="O28" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P28" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>805707165</t>
+          <t>5719</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>5/7/2025</t>
+          <t>5/1/2025</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Baez 793</t>
+          <t>CABEZON, JOSE LEON 2440</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>805707165</t>
+          <t>805579157</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
@@ -2597,7 +2589,7 @@
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>DESMONTAR COLUMNA DE 7 MTS Y TRANSFERIR A COMUNITARIA</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I29" t="n">
@@ -2615,50 +2607,50 @@
       </c>
       <c r="L29" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M29" t="n">
-        <v>-58.436165</v>
+        <v>-58.499967</v>
       </c>
       <c r="N29" t="n">
-        <v>-34.569081</v>
+        <v>-34.57974</v>
       </c>
       <c r="O29" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P29" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>5847</t>
+          <t>6333</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>5/8/2025</t>
+          <t>5/1/2025</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>JURAMENTO 5321</t>
+          <t>ORTEGA Y GASSET 1816</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>805791839</t>
+          <t>805655342</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
@@ -2695,36 +2687,36 @@
         </is>
       </c>
       <c r="M30" t="n">
-        <v>-58.485193</v>
+        <v>-58.432556</v>
       </c>
       <c r="N30" t="n">
-        <v>-34.579621</v>
+        <v>-34.570279</v>
       </c>
       <c r="O30" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P30" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>232</t>
+          <t>805707165</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>5/9/2025</t>
+          <t>5/7/2025</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Gorostiaga 2286</t>
+          <t>Baez 793</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
@@ -2734,7 +2726,7 @@
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>805791858</t>
+          <t>805707165</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
@@ -2749,7 +2741,7 @@
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>DESMONTAR COLUMNA DE 7 MTS Y TRANSFERIR A COMUNITARIA</t>
         </is>
       </c>
       <c r="I31" t="n">
@@ -2767,14 +2759,14 @@
       </c>
       <c r="L31" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M31" t="n">
-        <v>-58.441563</v>
+        <v>-58.436165</v>
       </c>
       <c r="N31" t="n">
-        <v>-34.569743</v>
+        <v>-34.569081</v>
       </c>
       <c r="O31" t="inlineStr">
         <is>
@@ -2790,7 +2782,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>-406</t>
+          <t>5847</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
@@ -2800,7 +2792,7 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Olof palme 4144</t>
+          <t>JURAMENTO 5321</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
@@ -2810,7 +2802,7 @@
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>805791925</t>
+          <t>805791839</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
@@ -2825,7 +2817,7 @@
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>Tensar 2 riendas a pique columna 168</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I32" t="n">
@@ -2833,7 +2825,7 @@
       </c>
       <c r="J32" t="inlineStr">
         <is>
-          <t>Tensor</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K32" t="inlineStr">
@@ -2843,18 +2835,18 @@
       </c>
       <c r="L32" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M32" t="n">
-        <v>-58.488252</v>
+        <v>-58.485193</v>
       </c>
       <c r="N32" t="n">
-        <v>-34.553391</v>
+        <v>-34.579621</v>
       </c>
       <c r="O32" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P32" t="inlineStr">
@@ -2866,27 +2858,27 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>5826</t>
+          <t>232</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>5/19/2025</t>
+          <t>5/9/2025</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>ALBARELLOS AV. 3180</t>
+          <t>Gorostiaga 2286</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>806926466</t>
+          <t>805791858</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
@@ -2901,7 +2893,7 @@
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>Columna (metal) inclinada</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I33" t="n">
@@ -2909,7 +2901,7 @@
       </c>
       <c r="J33" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K33" t="inlineStr">
@@ -2919,40 +2911,40 @@
       </c>
       <c r="L33" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M33" t="n">
-        <v>-58.513552</v>
+        <v>-58.441563</v>
       </c>
       <c r="N33" t="n">
-        <v>-34.579829</v>
+        <v>-34.569743</v>
       </c>
       <c r="O33" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P33" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>5825</t>
+          <t>-406</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>5/19/2025</t>
+          <t>5/8/2025</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>PAZ, GRAL. AV. 5602</t>
+          <t>Olof palme 4144</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
@@ -2962,7 +2954,7 @@
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>806926472</t>
+          <t>805791925</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
@@ -2977,7 +2969,7 @@
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>reparar rienda cortada - ver foto no es la misma que albarellos</t>
+          <t>Tensar 2 riendas a pique columna 168</t>
         </is>
       </c>
       <c r="I34" t="n">
@@ -2999,14 +2991,14 @@
         </is>
       </c>
       <c r="M34" t="n">
-        <v>-58.513685</v>
+        <v>-58.488252</v>
       </c>
       <c r="N34" t="n">
-        <v>-34.579838</v>
+        <v>-34.553391</v>
       </c>
       <c r="O34" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P34" t="inlineStr">
@@ -3018,27 +3010,27 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>807044192</t>
+          <t>5826</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>5/29/2025</t>
+          <t>5/19/2025</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>O'Higgins 4379</t>
+          <t>ALBARELLOS AV. 3180</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>807044192</t>
+          <t>806926466</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
@@ -3053,7 +3045,7 @@
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t xml:space="preserve">Poste </t>
+          <t>Columna (metal) inclinada</t>
         </is>
       </c>
       <c r="I35" t="n">
@@ -3061,7 +3053,7 @@
       </c>
       <c r="J35" t="inlineStr">
         <is>
-          <t>Desmonte</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K35" t="inlineStr">
@@ -3071,18 +3063,18 @@
       </c>
       <c r="L35" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M35" t="n">
-        <v>-58.468425</v>
+        <v>-58.513552</v>
       </c>
       <c r="N35" t="n">
-        <v>-34.54124</v>
+        <v>-34.579829</v>
       </c>
       <c r="O35" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P35" t="inlineStr">
@@ -3094,27 +3086,27 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>6020</t>
+          <t>5825</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>6/5/2025</t>
+          <t>5/19/2025</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>RAVIGNANI, EMILIO, DR. 2036</t>
+          <t>PAZ, GRAL. AV. 5602</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>807215465</t>
+          <t>806926472</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
@@ -3129,7 +3121,7 @@
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>reparar rienda cortada - ver foto no es la misma que albarellos</t>
         </is>
       </c>
       <c r="I36" t="n">
@@ -3137,7 +3129,7 @@
       </c>
       <c r="J36" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Tensor</t>
         </is>
       </c>
       <c r="K36" t="inlineStr">
@@ -3147,50 +3139,50 @@
       </c>
       <c r="L36" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M36" t="n">
-        <v>-58.436298</v>
+        <v>-58.513685</v>
       </c>
       <c r="N36" t="n">
-        <v>-34.578972</v>
+        <v>-34.579838</v>
       </c>
       <c r="O36" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P36" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>6144</t>
+          <t>807044192</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>6/11/2025</t>
+          <t>5/29/2025</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>TURIN 2990</t>
+          <t>O'Higgins 4379</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>807458282</t>
+          <t>807044192</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
@@ -3205,7 +3197,7 @@
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t xml:space="preserve">Poste </t>
         </is>
       </c>
       <c r="I37" t="n">
@@ -3213,7 +3205,7 @@
       </c>
       <c r="J37" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Desmonte</t>
         </is>
       </c>
       <c r="K37" t="inlineStr">
@@ -3223,18 +3215,18 @@
       </c>
       <c r="L37" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M37" t="n">
-        <v>-58.480925</v>
+        <v>-58.468425</v>
       </c>
       <c r="N37" t="n">
-        <v>-34.585471</v>
+        <v>-34.54124</v>
       </c>
       <c r="O37" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P37" t="inlineStr">
@@ -3246,27 +3238,27 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>6143</t>
+          <t>6020</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>6/11/2025</t>
+          <t>6/5/2025</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>SOLANO LOPEZ, F., MARISCAL 2845</t>
+          <t>RAVIGNANI, EMILIO, DR. 2036</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>807458296</t>
+          <t>807215465</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
@@ -3303,26 +3295,26 @@
         </is>
       </c>
       <c r="M38" t="n">
-        <v>-58.495071</v>
+        <v>-58.436298</v>
       </c>
       <c r="N38" t="n">
-        <v>-34.593122</v>
+        <v>-34.578972</v>
       </c>
       <c r="O38" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P38" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>6141</t>
+          <t>6144</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
@@ -3332,17 +3324,17 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>EL PAMPERO 2618</t>
+          <t>TURIN 2990</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>807458310</t>
+          <t>807458282</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
@@ -3379,10 +3371,10 @@
         </is>
       </c>
       <c r="M39" t="n">
-        <v>-58.481942</v>
+        <v>-58.480925</v>
       </c>
       <c r="N39" t="n">
-        <v>-34.602989</v>
+        <v>-34.585471</v>
       </c>
       <c r="O39" t="inlineStr">
         <is>
@@ -3398,27 +3390,27 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>-478</t>
+          <t>6143</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>6/15/2025</t>
+          <t>6/11/2025</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Chivilcoy 4875</t>
+          <t>SOLANO LOPEZ, F., MARISCAL 2845</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>807508509</t>
+          <t>807458296</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
@@ -3433,7 +3425,7 @@
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t>Poste podrido</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I40" t="n">
@@ -3451,14 +3443,14 @@
       </c>
       <c r="L40" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M40" t="n">
-        <v>-58.517389</v>
+        <v>-58.495071</v>
       </c>
       <c r="N40" t="n">
-        <v>-34.593541</v>
+        <v>-34.593122</v>
       </c>
       <c r="O40" t="inlineStr">
         <is>
@@ -3474,27 +3466,27 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>6171</t>
+          <t>6141</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>6/18/2025</t>
+          <t>6/11/2025</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>CABELLO 3486</t>
+          <t>EL PAMPERO 2618</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>807658640</t>
+          <t>807458310</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
@@ -3509,7 +3501,7 @@
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>Columna inclinada evaluar con inspector un corrimiento</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I41" t="n">
@@ -3531,46 +3523,46 @@
         </is>
       </c>
       <c r="M41" t="n">
-        <v>-58.409579</v>
+        <v>-58.481942</v>
       </c>
       <c r="N41" t="n">
-        <v>-34.581134</v>
+        <v>-34.602989</v>
       </c>
       <c r="O41" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P41" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>6230</t>
+          <t>-478</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>6/24/2025</t>
+          <t>6/15/2025</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Santa maria de oro	2722</t>
+          <t>Chivilcoy 4875</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>807763066</t>
+          <t>807508509</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
@@ -3585,7 +3577,7 @@
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Poste podrido</t>
         </is>
       </c>
       <c r="I42" t="n">
@@ -3603,40 +3595,40 @@
       </c>
       <c r="L42" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M42" t="n">
-        <v>-58.422315</v>
+        <v>-58.517389</v>
       </c>
       <c r="N42" t="n">
-        <v>-34.576988</v>
+        <v>-34.593541</v>
       </c>
       <c r="O42" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P42" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>6231</t>
+          <t>6171</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>6/24/2025</t>
+          <t>6/18/2025</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Ciudad de la Paz 275</t>
+          <t>CABELLO 3486</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
@@ -3646,7 +3638,7 @@
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>807763070</t>
+          <t>807658640</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
@@ -3661,7 +3653,7 @@
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>Aplomar o cambiar</t>
+          <t>Columna inclinada evaluar con inspector un corrimiento</t>
         </is>
       </c>
       <c r="I43" t="n">
@@ -3679,14 +3671,14 @@
       </c>
       <c r="L43" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M43" t="n">
-        <v>-58.441049</v>
+        <v>-58.409579</v>
       </c>
       <c r="N43" t="n">
-        <v>-34.574625</v>
+        <v>-34.581134</v>
       </c>
       <c r="O43" t="inlineStr">
         <is>
@@ -3702,7 +3694,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>6235</t>
+          <t>6230</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
@@ -3712,17 +3704,17 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>HUERGO 389</t>
+          <t>Santa maria de oro	2722</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>807763078</t>
+          <t>807763066</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
@@ -3759,10 +3751,10 @@
         </is>
       </c>
       <c r="M44" t="n">
-        <v>-58.432722</v>
+        <v>-58.422315</v>
       </c>
       <c r="N44" t="n">
-        <v>-34.572371</v>
+        <v>-34.576988</v>
       </c>
       <c r="O44" t="inlineStr">
         <is>
@@ -3778,17 +3770,17 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>6295</t>
+          <t>6231</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>6/30/2025</t>
+          <t>6/24/2025</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>SOLER 6017</t>
+          <t>Ciudad de la Paz 275</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
@@ -3798,7 +3790,7 @@
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>807851636</t>
+          <t>807763070</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
@@ -3813,7 +3805,7 @@
       </c>
       <c r="H45" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Aplomar o cambiar</t>
         </is>
       </c>
       <c r="I45" t="n">
@@ -3831,14 +3823,14 @@
       </c>
       <c r="L45" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M45" t="n">
-        <v>-58.436808</v>
+        <v>-58.441049</v>
       </c>
       <c r="N45" t="n">
-        <v>-34.577464</v>
+        <v>-34.574625</v>
       </c>
       <c r="O45" t="inlineStr">
         <is>
@@ -3854,27 +3846,27 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>6332</t>
+          <t>6235</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>7/3/2025</t>
+          <t>6/24/2025</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>ARAOZ 2560</t>
+          <t>HUERGO 389</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>807965818</t>
+          <t>807763078</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
@@ -3911,10 +3903,10 @@
         </is>
       </c>
       <c r="M46" t="n">
-        <v>-58.414507</v>
+        <v>-58.432722</v>
       </c>
       <c r="N46" t="n">
-        <v>-34.585377</v>
+        <v>-34.572371</v>
       </c>
       <c r="O46" t="inlineStr">
         <is>
@@ -3930,27 +3922,27 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>6363</t>
+          <t>6295</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>7/8/2025</t>
+          <t>6/30/2025</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>MOLDES 3730</t>
+          <t>SOLER 6017</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>808099415</t>
+          <t>807851636</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
@@ -3965,7 +3957,7 @@
       </c>
       <c r="H47" t="inlineStr">
         <is>
-          <t>Poste inclinado</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I47" t="n">
@@ -3973,7 +3965,7 @@
       </c>
       <c r="J47" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K47" t="inlineStr">
@@ -3983,50 +3975,50 @@
       </c>
       <c r="L47" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M47" t="n">
-        <v>-58.47192</v>
+        <v>-58.436808</v>
       </c>
       <c r="N47" t="n">
-        <v>-34.549398</v>
+        <v>-34.577464</v>
       </c>
       <c r="O47" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P47" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>-503</t>
+          <t>6332</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>7/10/2025</t>
+          <t>7/3/2025</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Salguero 842</t>
+          <t>ARAOZ 2560</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>808148673</t>
+          <t>807965818</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
@@ -4041,7 +4033,7 @@
       </c>
       <c r="H48" t="inlineStr">
         <is>
-          <t>Cambiar columna picada en la base</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I48" t="n">
@@ -4063,14 +4055,14 @@
         </is>
       </c>
       <c r="M48" t="n">
-        <v>-58.419166</v>
+        <v>-58.414507</v>
       </c>
       <c r="N48" t="n">
-        <v>-34.600265</v>
+        <v>-34.585377</v>
       </c>
       <c r="O48" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P48" t="inlineStr">
@@ -4082,27 +4074,27 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>6506</t>
+          <t>6363</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>7/10/2025</t>
+          <t>7/8/2025</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Ohiggins 1611</t>
+          <t>MOLDES 3730</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>808148679</t>
+          <t>808099415</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
@@ -4117,7 +4109,7 @@
       </c>
       <c r="H49" t="inlineStr">
         <is>
-          <t>Columna podrida en la base</t>
+          <t>Poste inclinado</t>
         </is>
       </c>
       <c r="I49" t="n">
@@ -4125,28 +4117,28 @@
       </c>
       <c r="J49" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K49" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L49" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M49" t="n">
-        <v>-58.448993</v>
+        <v>-58.47192</v>
       </c>
       <c r="N49" t="n">
-        <v>-34.564383</v>
+        <v>-34.549398</v>
       </c>
       <c r="O49" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P49" t="inlineStr">
@@ -4158,27 +4150,27 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>6437</t>
+          <t>-503</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>7/17/2025</t>
+          <t>7/10/2025</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>MILLER 4590</t>
+          <t>Salguero 842</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>808400306</t>
+          <t>808148673</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
@@ -4193,7 +4185,7 @@
       </c>
       <c r="H50" t="inlineStr">
         <is>
-          <t>Columna corroida</t>
+          <t>Cambiar columna picada en la base</t>
         </is>
       </c>
       <c r="I50" t="n">
@@ -4215,46 +4207,46 @@
         </is>
       </c>
       <c r="M50" t="n">
-        <v>-58.495482</v>
+        <v>-58.419166</v>
       </c>
       <c r="N50" t="n">
-        <v>-34.552614</v>
+        <v>-34.600265</v>
       </c>
       <c r="O50" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P50" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>-519</t>
+          <t>6506</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>7/17/2025</t>
+          <t>7/10/2025</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Vilela 2687</t>
+          <t>Ohiggins 1611</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>808400334</t>
+          <t>808148679</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
@@ -4269,7 +4261,7 @@
       </c>
       <c r="H51" t="inlineStr">
         <is>
-          <t>CAmbiar columna 114 picada en base</t>
+          <t>Columna podrida en la base</t>
         </is>
       </c>
       <c r="I51" t="n">
@@ -4282,7 +4274,7 @@
       </c>
       <c r="K51" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L51" t="inlineStr">
@@ -4291,14 +4283,14 @@
         </is>
       </c>
       <c r="M51" t="n">
-        <v>-58.472968</v>
+        <v>-58.448993</v>
       </c>
       <c r="N51" t="n">
-        <v>-34.546898</v>
+        <v>-34.564383</v>
       </c>
       <c r="O51" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P51" t="inlineStr">
@@ -4310,7 +4302,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>6538</t>
+          <t>6437</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
@@ -4320,7 +4312,7 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>Pedraza Manuela 4101</t>
+          <t>MILLER 4590</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
@@ -4330,7 +4322,7 @@
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>808400353</t>
+          <t>808400306</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
@@ -4345,7 +4337,7 @@
       </c>
       <c r="H52" t="inlineStr">
         <is>
-          <t xml:space="preserve">Podrida en la base </t>
+          <t>Columna corroida</t>
         </is>
       </c>
       <c r="I52" t="n">
@@ -4367,10 +4359,10 @@
         </is>
       </c>
       <c r="M52" t="n">
-        <v>-58.481569</v>
+        <v>-58.495482</v>
       </c>
       <c r="N52" t="n">
-        <v>-34.559853</v>
+        <v>-34.552614</v>
       </c>
       <c r="O52" t="inlineStr">
         <is>
@@ -4386,27 +4378,27 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>-525</t>
+          <t>-519</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>7/22/2025</t>
+          <t>7/17/2025</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>Zabala 3567</t>
+          <t>Vilela 2687</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>808480549</t>
+          <t>808400334</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
@@ -4421,7 +4413,7 @@
       </c>
       <c r="H53" t="inlineStr">
         <is>
-          <t>Corroida en base para recambio</t>
+          <t>CAmbiar columna 114 picada en base</t>
         </is>
       </c>
       <c r="I53" t="n">
@@ -4443,14 +4435,14 @@
         </is>
       </c>
       <c r="M53" t="n">
-        <v>-58.457492</v>
+        <v>-58.472968</v>
       </c>
       <c r="N53" t="n">
-        <v>-34.579336</v>
+        <v>-34.546898</v>
       </c>
       <c r="O53" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P53" t="inlineStr">
@@ -4462,27 +4454,27 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>6484</t>
+          <t>6538</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>7/24/2025</t>
+          <t>7/17/2025</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>URIARTE 2396</t>
+          <t>Pedraza Manuela 4101</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>808509373</t>
+          <t>808400353</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
@@ -4497,7 +4489,7 @@
       </c>
       <c r="H54" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t xml:space="preserve">Podrida en la base </t>
         </is>
       </c>
       <c r="I54" t="n">
@@ -4519,46 +4511,46 @@
         </is>
       </c>
       <c r="M54" t="n">
-        <v>-58.423934</v>
+        <v>-58.481569</v>
       </c>
       <c r="N54" t="n">
-        <v>-34.581562</v>
+        <v>-34.559853</v>
       </c>
       <c r="O54" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P54" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>6512</t>
+          <t>-525</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>7/28/2025</t>
+          <t>7/22/2025</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>GASCON 1195</t>
+          <t>Zabala 3567</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>808571975</t>
+          <t>808480549</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
@@ -4573,7 +4565,7 @@
       </c>
       <c r="H55" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Corroida en base para recambio</t>
         </is>
       </c>
       <c r="I55" t="n">
@@ -4595,36 +4587,36 @@
         </is>
       </c>
       <c r="M55" t="n">
-        <v>-58.423127</v>
+        <v>-58.457492</v>
       </c>
       <c r="N55" t="n">
-        <v>-34.596476</v>
+        <v>-34.579336</v>
       </c>
       <c r="O55" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P55" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>6513</t>
+          <t>6484</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>7/28/2025</t>
+          <t>7/24/2025</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>DORREGO 1925</t>
+          <t>URIARTE 2396</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
@@ -4634,7 +4626,7 @@
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>808571976</t>
+          <t>808509373</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
@@ -4671,10 +4663,10 @@
         </is>
       </c>
       <c r="M56" t="n">
-        <v>-58.441281</v>
+        <v>-58.423934</v>
       </c>
       <c r="N56" t="n">
-        <v>-34.579867</v>
+        <v>-34.581562</v>
       </c>
       <c r="O56" t="inlineStr">
         <is>
@@ -4690,7 +4682,7 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>6519</t>
+          <t>6512</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
@@ -4700,7 +4692,7 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>SALGUERO, JERONIMO 2874</t>
+          <t>GASCON 1195</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
@@ -4710,7 +4702,7 @@
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>808571977</t>
+          <t>808571975</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
@@ -4725,7 +4717,7 @@
       </c>
       <c r="H57" t="inlineStr">
         <is>
-          <t>Reparar rienda</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I57" t="n">
@@ -4733,7 +4725,7 @@
       </c>
       <c r="J57" t="inlineStr">
         <is>
-          <t>Tensor</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K57" t="inlineStr">
@@ -4743,14 +4735,14 @@
       </c>
       <c r="L57" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M57" t="n">
-        <v>-58.407256</v>
+        <v>-58.423127</v>
       </c>
       <c r="N57" t="n">
-        <v>-34.578976</v>
+        <v>-34.596476</v>
       </c>
       <c r="O57" t="inlineStr">
         <is>
@@ -4766,27 +4758,27 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>-536</t>
+          <t>6513</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>7/29/2025</t>
+          <t>7/28/2025</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>Olof palme 4142</t>
+          <t>DORREGO 1925</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t xml:space="preserve">ICD30249764 </t>
+          <t>808571976</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
@@ -4801,7 +4793,7 @@
       </c>
       <c r="H58" t="inlineStr">
         <is>
-          <t>Aplomar o desmontar poste</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I58" t="n">
@@ -4809,7 +4801,7 @@
       </c>
       <c r="J58" t="inlineStr">
         <is>
-          <t>Desmonte</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K58" t="inlineStr">
@@ -4819,50 +4811,50 @@
       </c>
       <c r="L58" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M58" t="n">
-        <v>-58.488239</v>
+        <v>-58.441281</v>
       </c>
       <c r="N58" t="n">
-        <v>-34.55341</v>
+        <v>-34.579867</v>
       </c>
       <c r="O58" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P58" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>-538</t>
+          <t>6519</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>7/31/2025</t>
+          <t>7/28/2025</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>Malabia 964</t>
+          <t>SALGUERO, JERONIMO 2874</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>808609237</t>
+          <t>808571977</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
@@ -4877,7 +4869,7 @@
       </c>
       <c r="H59" t="inlineStr">
         <is>
-          <t>Cambiar poste mal estado por PRFV</t>
+          <t>Reparar rienda</t>
         </is>
       </c>
       <c r="I59" t="n">
@@ -4885,7 +4877,7 @@
       </c>
       <c r="J59" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Tensor</t>
         </is>
       </c>
       <c r="K59" t="inlineStr">
@@ -4895,14 +4887,14 @@
       </c>
       <c r="L59" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M59" t="n">
-        <v>-58.433634</v>
+        <v>-58.407256</v>
       </c>
       <c r="N59" t="n">
-        <v>-34.595018</v>
+        <v>-34.578976</v>
       </c>
       <c r="O59" t="inlineStr">
         <is>
@@ -4918,27 +4910,27 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>6545</t>
+          <t>-536</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>8/4/2025</t>
+          <t>7/29/2025</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>SCALABRINI ORTIZ, RAUL AV. 708</t>
+          <t>Olof palme 4142</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>808703864</t>
+          <t xml:space="preserve">ICD30249764 </t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
@@ -4953,7 +4945,7 @@
       </c>
       <c r="H60" t="inlineStr">
         <is>
-          <t>Aplomar</t>
+          <t>Aplomar o desmontar poste</t>
         </is>
       </c>
       <c r="I60" t="n">
@@ -4961,31 +4953,183 @@
       </c>
       <c r="J60" t="inlineStr">
         <is>
+          <t>Desmonte</t>
+        </is>
+      </c>
+      <c r="K60" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L60" t="inlineStr">
+        <is>
+          <t>Poste</t>
+        </is>
+      </c>
+      <c r="M60" t="n">
+        <v>-58.488239</v>
+      </c>
+      <c r="N60" t="n">
+        <v>-34.55341</v>
+      </c>
+      <c r="O60" t="inlineStr">
+        <is>
+          <t>Saavedra</t>
+        </is>
+      </c>
+      <c r="P60" t="inlineStr">
+        <is>
+          <t>Capital Norte</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>-538</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>7/31/2025</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>Malabia 964</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>808609237</t>
+        </is>
+      </c>
+      <c r="F61" t="inlineStr">
+        <is>
+          <t>NEW</t>
+        </is>
+      </c>
+      <c r="G61" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H61" t="inlineStr">
+        <is>
+          <t>Cambiar poste mal estado por PRFV</t>
+        </is>
+      </c>
+      <c r="I61" t="n">
+        <v>1</v>
+      </c>
+      <c r="J61" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K61" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L61" t="inlineStr">
+        <is>
+          <t>Poste</t>
+        </is>
+      </c>
+      <c r="M61" t="n">
+        <v>-58.433634</v>
+      </c>
+      <c r="N61" t="n">
+        <v>-34.595018</v>
+      </c>
+      <c r="O61" t="inlineStr">
+        <is>
+          <t>Palermo</t>
+        </is>
+      </c>
+      <c r="P61" t="inlineStr">
+        <is>
+          <t>Capital Sur</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>6545</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>8/4/2025</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>SCALABRINI ORTIZ, RAUL AV. 708</t>
+        </is>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="E62" t="inlineStr">
+        <is>
+          <t>808703864</t>
+        </is>
+      </c>
+      <c r="F62" t="inlineStr">
+        <is>
+          <t>NEW</t>
+        </is>
+      </c>
+      <c r="G62" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H62" t="inlineStr">
+        <is>
+          <t>Aplomar</t>
+        </is>
+      </c>
+      <c r="I62" t="n">
+        <v>1</v>
+      </c>
+      <c r="J62" t="inlineStr">
+        <is>
           <t>Aplomo</t>
         </is>
       </c>
-      <c r="K60" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L60" t="inlineStr">
+      <c r="K62" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L62" t="inlineStr">
         <is>
           <t>Pasante</t>
         </is>
       </c>
-      <c r="M60" t="n">
+      <c r="M62" t="n">
         <v>-58.434339</v>
       </c>
-      <c r="N60" t="n">
+      <c r="N62" t="n">
         <v>-34.59693</v>
       </c>
-      <c r="O60" t="inlineStr">
+      <c r="O62" t="inlineStr">
         <is>
           <t>Palermo</t>
         </is>
       </c>
-      <c r="P60" t="inlineStr">
+      <c r="P62" t="inlineStr">
         <is>
           <t>Capital Sur</t>
         </is>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-08-07 07:22:40)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_NEW.xlsx
+++ b/mapa_interactivo_NEW.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P62"/>
+  <dimension ref="A1:P60"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3162,27 +3162,27 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>807044192</t>
+          <t>6020</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>5/29/2025</t>
+          <t>6/5/2025</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>O'Higgins 4379</t>
+          <t>RAVIGNANI, EMILIO, DR. 2036</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>807044192</t>
+          <t>807215465</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
@@ -3197,7 +3197,7 @@
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t xml:space="preserve">Poste </t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I37" t="n">
@@ -3205,7 +3205,7 @@
       </c>
       <c r="J37" t="inlineStr">
         <is>
-          <t>Desmonte</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K37" t="inlineStr">
@@ -3215,50 +3215,50 @@
       </c>
       <c r="L37" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M37" t="n">
-        <v>-58.468425</v>
+        <v>-58.436298</v>
       </c>
       <c r="N37" t="n">
-        <v>-34.54124</v>
+        <v>-34.578972</v>
       </c>
       <c r="O37" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P37" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>6020</t>
+          <t>6144</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>6/5/2025</t>
+          <t>6/11/2025</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>RAVIGNANI, EMILIO, DR. 2036</t>
+          <t>TURIN 2990</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>807215465</t>
+          <t>807458282</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
@@ -3295,26 +3295,26 @@
         </is>
       </c>
       <c r="M38" t="n">
-        <v>-58.436298</v>
+        <v>-58.480925</v>
       </c>
       <c r="N38" t="n">
-        <v>-34.578972</v>
+        <v>-34.585471</v>
       </c>
       <c r="O38" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P38" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>6144</t>
+          <t>6143</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
@@ -3324,7 +3324,7 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>TURIN 2990</t>
+          <t>SOLANO LOPEZ, F., MARISCAL 2845</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
@@ -3334,7 +3334,7 @@
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>807458282</t>
+          <t>807458296</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
@@ -3371,10 +3371,10 @@
         </is>
       </c>
       <c r="M39" t="n">
-        <v>-58.480925</v>
+        <v>-58.495071</v>
       </c>
       <c r="N39" t="n">
-        <v>-34.585471</v>
+        <v>-34.593122</v>
       </c>
       <c r="O39" t="inlineStr">
         <is>
@@ -3390,7 +3390,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>6143</t>
+          <t>6141</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
@@ -3400,17 +3400,17 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>SOLANO LOPEZ, F., MARISCAL 2845</t>
+          <t>EL PAMPERO 2618</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>807458296</t>
+          <t>807458310</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
@@ -3447,10 +3447,10 @@
         </is>
       </c>
       <c r="M40" t="n">
-        <v>-58.495071</v>
+        <v>-58.481942</v>
       </c>
       <c r="N40" t="n">
-        <v>-34.593122</v>
+        <v>-34.602989</v>
       </c>
       <c r="O40" t="inlineStr">
         <is>
@@ -3466,17 +3466,17 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>6141</t>
+          <t>-478</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>6/11/2025</t>
+          <t>6/15/2025</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>EL PAMPERO 2618</t>
+          <t>Chivilcoy 4875</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
@@ -3486,7 +3486,7 @@
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>807458310</t>
+          <t>807508509</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
@@ -3501,7 +3501,7 @@
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Poste podrido</t>
         </is>
       </c>
       <c r="I41" t="n">
@@ -3519,14 +3519,14 @@
       </c>
       <c r="L41" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M41" t="n">
-        <v>-58.481942</v>
+        <v>-58.517389</v>
       </c>
       <c r="N41" t="n">
-        <v>-34.602989</v>
+        <v>-34.593541</v>
       </c>
       <c r="O41" t="inlineStr">
         <is>
@@ -3542,27 +3542,27 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>-478</t>
+          <t>6171</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>6/15/2025</t>
+          <t>6/18/2025</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Chivilcoy 4875</t>
+          <t>CABELLO 3486</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>807508509</t>
+          <t>807658640</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
@@ -3577,7 +3577,7 @@
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>Poste podrido</t>
+          <t>Columna inclinada evaluar con inspector un corrimiento</t>
         </is>
       </c>
       <c r="I42" t="n">
@@ -3595,40 +3595,40 @@
       </c>
       <c r="L42" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M42" t="n">
-        <v>-58.517389</v>
+        <v>-58.409579</v>
       </c>
       <c r="N42" t="n">
-        <v>-34.593541</v>
+        <v>-34.581134</v>
       </c>
       <c r="O42" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P42" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>6171</t>
+          <t>6230</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>6/18/2025</t>
+          <t>6/24/2025</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>CABELLO 3486</t>
+          <t>Santa maria de oro	2722</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
@@ -3638,7 +3638,7 @@
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>807658640</t>
+          <t>807763066</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
@@ -3653,7 +3653,7 @@
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>Columna inclinada evaluar con inspector un corrimiento</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I43" t="n">
@@ -3675,10 +3675,10 @@
         </is>
       </c>
       <c r="M43" t="n">
-        <v>-58.409579</v>
+        <v>-58.422315</v>
       </c>
       <c r="N43" t="n">
-        <v>-34.581134</v>
+        <v>-34.576988</v>
       </c>
       <c r="O43" t="inlineStr">
         <is>
@@ -3694,7 +3694,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>6230</t>
+          <t>6231</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
@@ -3704,7 +3704,7 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Santa maria de oro	2722</t>
+          <t>Ciudad de la Paz 275</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
@@ -3714,7 +3714,7 @@
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>807763066</t>
+          <t>807763070</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
@@ -3729,7 +3729,7 @@
       </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Aplomar o cambiar</t>
         </is>
       </c>
       <c r="I44" t="n">
@@ -3747,14 +3747,14 @@
       </c>
       <c r="L44" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M44" t="n">
-        <v>-58.422315</v>
+        <v>-58.441049</v>
       </c>
       <c r="N44" t="n">
-        <v>-34.576988</v>
+        <v>-34.574625</v>
       </c>
       <c r="O44" t="inlineStr">
         <is>
@@ -3770,7 +3770,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>6231</t>
+          <t>6235</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
@@ -3780,17 +3780,17 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Ciudad de la Paz 275</t>
+          <t>HUERGO 389</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>807763070</t>
+          <t>807763078</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
@@ -3805,7 +3805,7 @@
       </c>
       <c r="H45" t="inlineStr">
         <is>
-          <t>Aplomar o cambiar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I45" t="n">
@@ -3823,14 +3823,14 @@
       </c>
       <c r="L45" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M45" t="n">
-        <v>-58.441049</v>
+        <v>-58.432722</v>
       </c>
       <c r="N45" t="n">
-        <v>-34.574625</v>
+        <v>-34.572371</v>
       </c>
       <c r="O45" t="inlineStr">
         <is>
@@ -3846,27 +3846,27 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>6235</t>
+          <t>6295</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>6/24/2025</t>
+          <t>6/30/2025</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>HUERGO 389</t>
+          <t>SOLER 6017</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>807763078</t>
+          <t>807851636</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
@@ -3903,10 +3903,10 @@
         </is>
       </c>
       <c r="M46" t="n">
-        <v>-58.432722</v>
+        <v>-58.436808</v>
       </c>
       <c r="N46" t="n">
-        <v>-34.572371</v>
+        <v>-34.577464</v>
       </c>
       <c r="O46" t="inlineStr">
         <is>
@@ -3922,17 +3922,17 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>6295</t>
+          <t>6332</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>6/30/2025</t>
+          <t>7/3/2025</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>SOLER 6017</t>
+          <t>ARAOZ 2560</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
@@ -3942,7 +3942,7 @@
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>807851636</t>
+          <t>807965818</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
@@ -3979,10 +3979,10 @@
         </is>
       </c>
       <c r="M47" t="n">
-        <v>-58.436808</v>
+        <v>-58.414507</v>
       </c>
       <c r="N47" t="n">
-        <v>-34.577464</v>
+        <v>-34.585377</v>
       </c>
       <c r="O47" t="inlineStr">
         <is>
@@ -3998,27 +3998,27 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>6332</t>
+          <t>-503</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>7/3/2025</t>
+          <t>7/10/2025</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>ARAOZ 2560</t>
+          <t>Salguero 842</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>807965818</t>
+          <t>808148673</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
@@ -4033,7 +4033,7 @@
       </c>
       <c r="H48" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambiar columna picada en la base</t>
         </is>
       </c>
       <c r="I48" t="n">
@@ -4055,14 +4055,14 @@
         </is>
       </c>
       <c r="M48" t="n">
-        <v>-58.414507</v>
+        <v>-58.419166</v>
       </c>
       <c r="N48" t="n">
-        <v>-34.585377</v>
+        <v>-34.600265</v>
       </c>
       <c r="O48" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P48" t="inlineStr">
@@ -4074,27 +4074,27 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>6363</t>
+          <t>6506</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>7/8/2025</t>
+          <t>7/10/2025</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>MOLDES 3730</t>
+          <t>Ohiggins 1611</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>808099415</t>
+          <t>808148679</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
@@ -4109,7 +4109,7 @@
       </c>
       <c r="H49" t="inlineStr">
         <is>
-          <t>Poste inclinado</t>
+          <t>Columna podrida en la base</t>
         </is>
       </c>
       <c r="I49" t="n">
@@ -4117,28 +4117,28 @@
       </c>
       <c r="J49" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K49" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L49" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M49" t="n">
-        <v>-58.47192</v>
+        <v>-58.448993</v>
       </c>
       <c r="N49" t="n">
-        <v>-34.549398</v>
+        <v>-34.564383</v>
       </c>
       <c r="O49" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P49" t="inlineStr">
@@ -4150,27 +4150,27 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>-503</t>
+          <t>6437</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>7/10/2025</t>
+          <t>7/17/2025</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Salguero 842</t>
+          <t>MILLER 4590</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>808148673</t>
+          <t>808400306</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
@@ -4185,7 +4185,7 @@
       </c>
       <c r="H50" t="inlineStr">
         <is>
-          <t>Cambiar columna picada en la base</t>
+          <t>Columna corroida</t>
         </is>
       </c>
       <c r="I50" t="n">
@@ -4207,46 +4207,46 @@
         </is>
       </c>
       <c r="M50" t="n">
-        <v>-58.419166</v>
+        <v>-58.495482</v>
       </c>
       <c r="N50" t="n">
-        <v>-34.600265</v>
+        <v>-34.552614</v>
       </c>
       <c r="O50" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P50" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>6506</t>
+          <t>6538</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>7/10/2025</t>
+          <t>7/17/2025</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Ohiggins 1611</t>
+          <t>Pedraza Manuela 4101</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>808148679</t>
+          <t>808400353</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
@@ -4261,7 +4261,7 @@
       </c>
       <c r="H51" t="inlineStr">
         <is>
-          <t>Columna podrida en la base</t>
+          <t xml:space="preserve">Podrida en la base </t>
         </is>
       </c>
       <c r="I51" t="n">
@@ -4274,7 +4274,7 @@
       </c>
       <c r="K51" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L51" t="inlineStr">
@@ -4283,14 +4283,14 @@
         </is>
       </c>
       <c r="M51" t="n">
-        <v>-58.448993</v>
+        <v>-58.481569</v>
       </c>
       <c r="N51" t="n">
-        <v>-34.564383</v>
+        <v>-34.559853</v>
       </c>
       <c r="O51" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P51" t="inlineStr">
@@ -4302,27 +4302,27 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>6437</t>
+          <t>-525</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>7/17/2025</t>
+          <t>7/22/2025</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>MILLER 4590</t>
+          <t>Zabala 3567</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>808400306</t>
+          <t>808480549</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
@@ -4337,7 +4337,7 @@
       </c>
       <c r="H52" t="inlineStr">
         <is>
-          <t>Columna corroida</t>
+          <t>Corroida en base para recambio</t>
         </is>
       </c>
       <c r="I52" t="n">
@@ -4359,14 +4359,14 @@
         </is>
       </c>
       <c r="M52" t="n">
-        <v>-58.495482</v>
+        <v>-58.457492</v>
       </c>
       <c r="N52" t="n">
-        <v>-34.552614</v>
+        <v>-34.579336</v>
       </c>
       <c r="O52" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P52" t="inlineStr">
@@ -4378,27 +4378,27 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>-519</t>
+          <t>6484</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>7/17/2025</t>
+          <t>7/24/2025</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>Vilela 2687</t>
+          <t>URIARTE 2396</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>808400334</t>
+          <t>808509373</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
@@ -4413,7 +4413,7 @@
       </c>
       <c r="H53" t="inlineStr">
         <is>
-          <t>CAmbiar columna 114 picada en base</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I53" t="n">
@@ -4435,46 +4435,46 @@
         </is>
       </c>
       <c r="M53" t="n">
-        <v>-58.472968</v>
+        <v>-58.423934</v>
       </c>
       <c r="N53" t="n">
-        <v>-34.546898</v>
+        <v>-34.581562</v>
       </c>
       <c r="O53" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P53" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>6538</t>
+          <t>6512</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>7/17/2025</t>
+          <t>7/28/2025</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>Pedraza Manuela 4101</t>
+          <t>GASCON 1195</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>808400353</t>
+          <t>808571975</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
@@ -4489,7 +4489,7 @@
       </c>
       <c r="H54" t="inlineStr">
         <is>
-          <t xml:space="preserve">Podrida en la base </t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I54" t="n">
@@ -4511,46 +4511,46 @@
         </is>
       </c>
       <c r="M54" t="n">
-        <v>-58.481569</v>
+        <v>-58.423127</v>
       </c>
       <c r="N54" t="n">
-        <v>-34.559853</v>
+        <v>-34.596476</v>
       </c>
       <c r="O54" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P54" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>-525</t>
+          <t>6513</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>7/22/2025</t>
+          <t>7/28/2025</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>Zabala 3567</t>
+          <t>DORREGO 1925</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>808480549</t>
+          <t>808571976</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
@@ -4565,7 +4565,7 @@
       </c>
       <c r="H55" t="inlineStr">
         <is>
-          <t>Corroida en base para recambio</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I55" t="n">
@@ -4587,36 +4587,36 @@
         </is>
       </c>
       <c r="M55" t="n">
-        <v>-58.457492</v>
+        <v>-58.441281</v>
       </c>
       <c r="N55" t="n">
-        <v>-34.579336</v>
+        <v>-34.579867</v>
       </c>
       <c r="O55" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P55" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>6484</t>
+          <t>6519</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>7/24/2025</t>
+          <t>7/28/2025</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>URIARTE 2396</t>
+          <t>SALGUERO, JERONIMO 2874</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
@@ -4626,7 +4626,7 @@
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>808509373</t>
+          <t>808571977</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
@@ -4641,7 +4641,7 @@
       </c>
       <c r="H56" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Reparar rienda</t>
         </is>
       </c>
       <c r="I56" t="n">
@@ -4649,7 +4649,7 @@
       </c>
       <c r="J56" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Tensor</t>
         </is>
       </c>
       <c r="K56" t="inlineStr">
@@ -4659,14 +4659,14 @@
       </c>
       <c r="L56" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M56" t="n">
-        <v>-58.423934</v>
+        <v>-58.407256</v>
       </c>
       <c r="N56" t="n">
-        <v>-34.581562</v>
+        <v>-34.578976</v>
       </c>
       <c r="O56" t="inlineStr">
         <is>
@@ -4682,27 +4682,27 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>6512</t>
+          <t>-538</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>7/28/2025</t>
+          <t>7/31/2025</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>GASCON 1195</t>
+          <t>Malabia 964</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>808571975</t>
+          <t>808609237</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
@@ -4717,7 +4717,7 @@
       </c>
       <c r="H57" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambiar poste mal estado por PRFV</t>
         </is>
       </c>
       <c r="I57" t="n">
@@ -4735,14 +4735,14 @@
       </c>
       <c r="L57" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M57" t="n">
-        <v>-58.423127</v>
+        <v>-58.433634</v>
       </c>
       <c r="N57" t="n">
-        <v>-34.596476</v>
+        <v>-34.595018</v>
       </c>
       <c r="O57" t="inlineStr">
         <is>
@@ -4758,27 +4758,27 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>6513</t>
+          <t>6545</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>7/28/2025</t>
+          <t>8/4/2025</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>DORREGO 1925</t>
+          <t>SCALABRINI ORTIZ, RAUL AV. 708</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>808571976</t>
+          <t>808703864</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
@@ -4793,7 +4793,7 @@
       </c>
       <c r="H58" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Aplomar</t>
         </is>
       </c>
       <c r="I58" t="n">
@@ -4801,7 +4801,7 @@
       </c>
       <c r="J58" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K58" t="inlineStr">
@@ -4815,10 +4815,10 @@
         </is>
       </c>
       <c r="M58" t="n">
-        <v>-58.441281</v>
+        <v>-58.434339</v>
       </c>
       <c r="N58" t="n">
-        <v>-34.579867</v>
+        <v>-34.59693</v>
       </c>
       <c r="O58" t="inlineStr">
         <is>
@@ -4834,27 +4834,27 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>6519</t>
+          <t>6498</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>7/28/2025</t>
+          <t>8/6/2025</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>SALGUERO, JERONIMO 2874</t>
+          <t>BUCARELLI 2087</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>808571977</t>
+          <t>808733908</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
@@ -4869,7 +4869,7 @@
       </c>
       <c r="H59" t="inlineStr">
         <is>
-          <t>Reparar rienda</t>
+          <t>Base picada</t>
         </is>
       </c>
       <c r="I59" t="n">
@@ -4877,7 +4877,7 @@
       </c>
       <c r="J59" t="inlineStr">
         <is>
-          <t>Tensor</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K59" t="inlineStr">
@@ -4887,50 +4887,50 @@
       </c>
       <c r="L59" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M59" t="n">
-        <v>-58.407256</v>
+        <v>-58.485592</v>
       </c>
       <c r="N59" t="n">
-        <v>-34.578976</v>
+        <v>-34.578586</v>
       </c>
       <c r="O59" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P59" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>-536</t>
+          <t>-547</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>7/29/2025</t>
+          <t>8/6/2025</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>Olof palme 4142</t>
+          <t>Habana 4210</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t xml:space="preserve">ICD30249764 </t>
+          <t>808733921</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
@@ -4945,7 +4945,7 @@
       </c>
       <c r="H60" t="inlineStr">
         <is>
-          <t>Aplomar o desmontar poste</t>
+          <t>Cambiar poste dañado</t>
         </is>
       </c>
       <c r="I60" t="n">
@@ -4953,7 +4953,7 @@
       </c>
       <c r="J60" t="inlineStr">
         <is>
-          <t>Desmonte</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K60" t="inlineStr">
@@ -4967,171 +4967,19 @@
         </is>
       </c>
       <c r="M60" t="n">
-        <v>-58.488239</v>
+        <v>-58.515873</v>
       </c>
       <c r="N60" t="n">
-        <v>-34.55341</v>
+        <v>-34.599425</v>
       </c>
       <c r="O60" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P60" t="inlineStr">
         <is>
           <t>Capital Norte</t>
-        </is>
-      </c>
-    </row>
-    <row r="61">
-      <c r="A61" t="inlineStr">
-        <is>
-          <t>-538</t>
-        </is>
-      </c>
-      <c r="B61" t="inlineStr">
-        <is>
-          <t>7/31/2025</t>
-        </is>
-      </c>
-      <c r="C61" t="inlineStr">
-        <is>
-          <t>Malabia 964</t>
-        </is>
-      </c>
-      <c r="D61" t="inlineStr">
-        <is>
-          <t>15</t>
-        </is>
-      </c>
-      <c r="E61" t="inlineStr">
-        <is>
-          <t>808609237</t>
-        </is>
-      </c>
-      <c r="F61" t="inlineStr">
-        <is>
-          <t>NEW</t>
-        </is>
-      </c>
-      <c r="G61" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H61" t="inlineStr">
-        <is>
-          <t>Cambiar poste mal estado por PRFV</t>
-        </is>
-      </c>
-      <c r="I61" t="n">
-        <v>1</v>
-      </c>
-      <c r="J61" t="inlineStr">
-        <is>
-          <t>Cambio</t>
-        </is>
-      </c>
-      <c r="K61" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L61" t="inlineStr">
-        <is>
-          <t>Poste</t>
-        </is>
-      </c>
-      <c r="M61" t="n">
-        <v>-58.433634</v>
-      </c>
-      <c r="N61" t="n">
-        <v>-34.595018</v>
-      </c>
-      <c r="O61" t="inlineStr">
-        <is>
-          <t>Palermo</t>
-        </is>
-      </c>
-      <c r="P61" t="inlineStr">
-        <is>
-          <t>Capital Sur</t>
-        </is>
-      </c>
-    </row>
-    <row r="62">
-      <c r="A62" t="inlineStr">
-        <is>
-          <t>6545</t>
-        </is>
-      </c>
-      <c r="B62" t="inlineStr">
-        <is>
-          <t>8/4/2025</t>
-        </is>
-      </c>
-      <c r="C62" t="inlineStr">
-        <is>
-          <t>SCALABRINI ORTIZ, RAUL AV. 708</t>
-        </is>
-      </c>
-      <c r="D62" t="inlineStr">
-        <is>
-          <t>15</t>
-        </is>
-      </c>
-      <c r="E62" t="inlineStr">
-        <is>
-          <t>808703864</t>
-        </is>
-      </c>
-      <c r="F62" t="inlineStr">
-        <is>
-          <t>NEW</t>
-        </is>
-      </c>
-      <c r="G62" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H62" t="inlineStr">
-        <is>
-          <t>Aplomar</t>
-        </is>
-      </c>
-      <c r="I62" t="n">
-        <v>1</v>
-      </c>
-      <c r="J62" t="inlineStr">
-        <is>
-          <t>Aplomo</t>
-        </is>
-      </c>
-      <c r="K62" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L62" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
-      <c r="M62" t="n">
-        <v>-58.434339</v>
-      </c>
-      <c r="N62" t="n">
-        <v>-34.59693</v>
-      </c>
-      <c r="O62" t="inlineStr">
-        <is>
-          <t>Palermo</t>
-        </is>
-      </c>
-      <c r="P62" t="inlineStr">
-        <is>
-          <t>Capital Sur</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-08-07 14:26:25)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_NEW.xlsx
+++ b/mapa_interactivo_NEW.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P60"/>
+  <dimension ref="A1:P61"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4983,6 +4983,82 @@
         </is>
       </c>
     </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>6579</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>8/7/2025</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>RIVADAVIA MARTIN, COMODORO 1350</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>13</t>
+        </is>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>808749184</t>
+        </is>
+      </c>
+      <c r="F61" t="inlineStr">
+        <is>
+          <t>NEW</t>
+        </is>
+      </c>
+      <c r="G61" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H61" t="inlineStr">
+        <is>
+          <t>Poste inclinado</t>
+        </is>
+      </c>
+      <c r="I61" t="n">
+        <v>1</v>
+      </c>
+      <c r="J61" t="inlineStr">
+        <is>
+          <t>Aplomo</t>
+        </is>
+      </c>
+      <c r="K61" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L61" t="inlineStr">
+        <is>
+          <t>Poste</t>
+        </is>
+      </c>
+      <c r="M61" t="n">
+        <v>-58.461024</v>
+      </c>
+      <c r="N61" t="n">
+        <v>-34.539409</v>
+      </c>
+      <c r="O61" t="inlineStr">
+        <is>
+          <t>Saavedra</t>
+        </is>
+      </c>
+      <c r="P61" t="inlineStr">
+        <is>
+          <t>Capital Norte</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-08-08 07:21:14)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_NEW.xlsx
+++ b/mapa_interactivo_NEW.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P61"/>
+  <dimension ref="A1:P59"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -822,17 +822,17 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>5589</t>
+          <t>4595</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>12/31/2023</t>
+          <t>1/15/2025</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>ARCOS 1520</t>
+          <t>PAROISSIEN 1806</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -842,7 +842,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>799540526</t>
+          <t>802747617</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -852,33 +852,41 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
+          <t>Pendiente</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Aplomar</t>
         </is>
       </c>
       <c r="I6" t="n">
-        <v>0</v>
-      </c>
-      <c r="J6" t="inlineStr"/>
-      <c r="K6" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>Aplomo</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M6" t="n">
-        <v>-58.449125</v>
+        <v>-58.464172</v>
       </c>
       <c r="N6" t="n">
-        <v>-34.565958</v>
+        <v>-34.543845</v>
       </c>
       <c r="O6" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P6" t="inlineStr">
@@ -890,27 +898,27 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>4595</t>
+          <t>4662</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>1/15/2025</t>
+          <t>1/21/2025</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>PAROISSIEN 1806</t>
+          <t>ALTOLAGUIRRE 2397</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>802747617</t>
+          <t>802823938</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -925,7 +933,7 @@
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>Aplomar</t>
+          <t>Inclinada</t>
         </is>
       </c>
       <c r="I7" t="n">
@@ -943,18 +951,18 @@
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M7" t="n">
-        <v>-58.464172</v>
+        <v>-58.490766</v>
       </c>
       <c r="N7" t="n">
-        <v>-34.543845</v>
+        <v>-34.576987</v>
       </c>
       <c r="O7" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P7" t="inlineStr">
@@ -966,27 +974,27 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>4662</t>
+          <t>6036</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>1/21/2025</t>
+          <t>2/24/2025</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>ALTOLAGUIRRE 2397</t>
+          <t>MEDRANO 1715</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>802823938</t>
+          <t>803608181</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -999,22 +1007,18 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H8" t="inlineStr">
-        <is>
-          <t>Inclinada</t>
-        </is>
-      </c>
+      <c r="H8" t="inlineStr"/>
       <c r="I8" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L8" t="inlineStr">
@@ -1023,46 +1027,46 @@
         </is>
       </c>
       <c r="M8" t="n">
-        <v>-58.490766</v>
+        <v>-58.418236</v>
       </c>
       <c r="N8" t="n">
-        <v>-34.576987</v>
+        <v>-34.589859</v>
       </c>
       <c r="O8" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P8" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>4862</t>
+          <t>803608480</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>1/23/2025</t>
+          <t>2/24/2025</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>ARCOS 2263</t>
+          <t>GUATEMALA /ALT/ 4415</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>802857379</t>
+          <t>803608480</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -1072,12 +1076,12 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
+          <t>Pendiente</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>picada</t>
+          <t xml:space="preserve">Guatemala 4415 </t>
         </is>
       </c>
       <c r="I9" t="n">
@@ -1090,7 +1094,7 @@
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L9" t="inlineStr">
@@ -1099,46 +1103,46 @@
         </is>
       </c>
       <c r="M9" t="n">
-        <v>-58.455082</v>
+        <v>-58.421661</v>
       </c>
       <c r="N9" t="n">
-        <v>-34.558883</v>
+        <v>-34.588428</v>
       </c>
       <c r="O9" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P9" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>6036</t>
+          <t>5053</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>2/24/2025</t>
+          <t>3/11/2025</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>MEDRANO 1715</t>
+          <t>MENDOZA 1153</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>803608181</t>
+          <t>803969314</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
@@ -1151,7 +1155,11 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H10" t="inlineStr"/>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>Poste</t>
+        </is>
+      </c>
       <c r="I10" t="n">
         <v>0</v>
       </c>
@@ -1162,55 +1170,55 @@
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L10" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M10" t="n">
-        <v>-58.418236</v>
+        <v>-58.44463</v>
       </c>
       <c r="N10" t="n">
-        <v>-34.589859</v>
+        <v>-34.553354</v>
       </c>
       <c r="O10" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P10" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>803608480</t>
+          <t>6071</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>2/24/2025</t>
+          <t>3/17/2025</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>GUATEMALA /ALT/ 4415</t>
+          <t>OSORIO 4994</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>803608480</t>
+          <t>804053324</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
@@ -1223,11 +1231,7 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H11" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Guatemala 4415 </t>
-        </is>
-      </c>
+      <c r="H11" t="inlineStr"/>
       <c r="I11" t="n">
         <v>0</v>
       </c>
@@ -1247,46 +1251,46 @@
         </is>
       </c>
       <c r="M11" t="n">
-        <v>-58.421661</v>
+        <v>-58.466241</v>
       </c>
       <c r="N11" t="n">
-        <v>-34.588428</v>
+        <v>-34.595741</v>
       </c>
       <c r="O11" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P11" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>5053</t>
+          <t>3348</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>3/11/2025</t>
+          <t>3/27/2025</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>MENDOZA 1153</t>
+          <t>ESTOMBA 2626</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>803969314</t>
+          <t>804309704</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
@@ -1301,15 +1305,15 @@
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I12" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Desmonte</t>
         </is>
       </c>
       <c r="K12" t="inlineStr">
@@ -1319,18 +1323,18 @@
       </c>
       <c r="L12" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M12" t="n">
-        <v>-58.44463</v>
+        <v>-58.47538</v>
       </c>
       <c r="N12" t="n">
-        <v>-34.553354</v>
+        <v>-34.566015</v>
       </c>
       <c r="O12" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P12" t="inlineStr">
@@ -1342,27 +1346,27 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>6071</t>
+          <t>-312</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>3/17/2025</t>
+          <t>3/29/2025</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>OSORIO 4994</t>
+          <t>MATIENZO BENJAMIN /ALT/ 1831</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>804053324</t>
+          <t>804333522</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
@@ -1375,7 +1379,11 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H13" t="inlineStr"/>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>Retirar columna ya traspasaron el nodo</t>
+        </is>
+      </c>
       <c r="I13" t="n">
         <v>0</v>
       </c>
@@ -1386,7 +1394,7 @@
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L13" t="inlineStr">
@@ -1395,36 +1403,36 @@
         </is>
       </c>
       <c r="M13" t="n">
-        <v>-58.466241</v>
+        <v>-58.434835</v>
       </c>
       <c r="N13" t="n">
-        <v>-34.595741</v>
+        <v>-34.569129</v>
       </c>
       <c r="O13" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P13" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>3348</t>
+          <t>3430</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>3/27/2025</t>
+          <t>4/1/2025</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>ESTOMBA 2626</t>
+          <t>MONROE 3838</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
@@ -1434,7 +1442,7 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>804309704</t>
+          <t>804468442</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
@@ -1449,7 +1457,7 @@
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Reparar rienda</t>
         </is>
       </c>
       <c r="I14" t="n">
@@ -1457,7 +1465,7 @@
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>Desmonte</t>
+          <t>Tensor</t>
         </is>
       </c>
       <c r="K14" t="inlineStr">
@@ -1467,14 +1475,14 @@
       </c>
       <c r="L14" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M14" t="n">
-        <v>-58.47538</v>
+        <v>-58.473659</v>
       </c>
       <c r="N14" t="n">
-        <v>-34.566015</v>
+        <v>-34.566979</v>
       </c>
       <c r="O14" t="inlineStr">
         <is>
@@ -1490,27 +1498,27 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>-312</t>
+          <t>5464</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>3/29/2025</t>
+          <t>4/4/2025</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>MATIENZO BENJAMIN /ALT/ 1831</t>
+          <t>SUCRE, ANTONIO JOSE DE, MCAL. 3100</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>804333522</t>
+          <t>804497880</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
@@ -1525,11 +1533,11 @@
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>Retirar columna ya traspasaron el nodo</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I15" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J15" t="inlineStr">
         <is>
@@ -1538,45 +1546,45 @@
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L15" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M15" t="n">
-        <v>-58.434835</v>
+        <v>-58.46161</v>
       </c>
       <c r="N15" t="n">
-        <v>-34.569129</v>
+        <v>-34.567849</v>
       </c>
       <c r="O15" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P15" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>3430</t>
+          <t>5469</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>4/1/2025</t>
+          <t>4/4/2025</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>MONROE 3838</t>
+          <t>ESTADO PLURINACIONAL DE BOLIVIA 5899</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
@@ -1586,7 +1594,7 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>804468442</t>
+          <t>804497887</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
@@ -1601,7 +1609,7 @@
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>Reparar rienda</t>
+          <t>Aplomar</t>
         </is>
       </c>
       <c r="I16" t="n">
@@ -1609,7 +1617,7 @@
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>Tensor</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K16" t="inlineStr">
@@ -1623,14 +1631,14 @@
         </is>
       </c>
       <c r="M16" t="n">
-        <v>-58.473659</v>
+        <v>-58.507746</v>
       </c>
       <c r="N16" t="n">
-        <v>-34.566979</v>
+        <v>-34.574217</v>
       </c>
       <c r="O16" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P16" t="inlineStr">
@@ -1642,7 +1650,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>5464</t>
+          <t>5492</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -1652,17 +1660,17 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>SUCRE, ANTONIO JOSE DE, MCAL. 3100</t>
+          <t>ESTADO PLURINACIONAL DE BOLIVIA 5920</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>804497880</t>
+          <t>804498035</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
@@ -1677,7 +1685,7 @@
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>aplomar</t>
         </is>
       </c>
       <c r="I17" t="n">
@@ -1685,7 +1693,7 @@
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K17" t="inlineStr">
@@ -1699,14 +1707,14 @@
         </is>
       </c>
       <c r="M17" t="n">
-        <v>-58.46161</v>
+        <v>-58.50751</v>
       </c>
       <c r="N17" t="n">
-        <v>-34.567849</v>
+        <v>-34.574543</v>
       </c>
       <c r="O17" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P17" t="inlineStr">
@@ -1718,17 +1726,17 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>5469</t>
+          <t>5599</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>4/4/2025</t>
+          <t>4/15/2025</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>ESTADO PLURINACIONAL DE BOLIVIA 5899</t>
+          <t>ESTOMBA 4052</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
@@ -1738,7 +1746,7 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>804497887</t>
+          <t>804732246</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
@@ -1753,7 +1761,7 @@
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>Aplomar</t>
+          <t>Columna PRFV quedo inclinada (la hicieron como estomba 4056)</t>
         </is>
       </c>
       <c r="I18" t="n">
@@ -1766,23 +1774,23 @@
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo TLC</t>
         </is>
       </c>
       <c r="L18" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M18" t="n">
-        <v>-58.507746</v>
+        <v>-58.485407</v>
       </c>
       <c r="N18" t="n">
-        <v>-34.574217</v>
+        <v>-34.552985</v>
       </c>
       <c r="O18" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P18" t="inlineStr">
@@ -1794,27 +1802,27 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>5492</t>
+          <t>5590</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>4/4/2025</t>
+          <t>4/15/2025</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>ESTADO PLURINACIONAL DE BOLIVIA 5920</t>
+          <t>O'HIGGINS 2441</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>804498035</t>
+          <t>804732275</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
@@ -1829,7 +1837,7 @@
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>aplomar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I19" t="n">
@@ -1837,7 +1845,7 @@
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K19" t="inlineStr">
@@ -1847,18 +1855,18 @@
       </c>
       <c r="L19" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M19" t="n">
-        <v>-58.50751</v>
+        <v>-58.45573</v>
       </c>
       <c r="N19" t="n">
-        <v>-34.574543</v>
+        <v>-34.556576</v>
       </c>
       <c r="O19" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P19" t="inlineStr">
@@ -1870,27 +1878,27 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>5599</t>
+          <t>804787368</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>4/15/2025</t>
+          <t>4/17/2025</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>ESTOMBA 4052</t>
+          <t>San Blas 2591</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>804732246</t>
+          <t>804787368</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
@@ -1905,7 +1913,7 @@
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>Columna PRFV quedo inclinada (la hicieron como estomba 4056)</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I20" t="n">
@@ -1913,12 +1921,12 @@
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>Nodo TLC</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L20" t="inlineStr">
@@ -1927,14 +1935,14 @@
         </is>
       </c>
       <c r="M20" t="n">
-        <v>-58.485407</v>
+        <v>-58.477427</v>
       </c>
       <c r="N20" t="n">
-        <v>-34.552985</v>
+        <v>-34.609261</v>
       </c>
       <c r="O20" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P20" t="inlineStr">
@@ -1946,17 +1954,17 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>5590</t>
+          <t>5624</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>4/15/2025</t>
+          <t>4/22/2025</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>O'HIGGINS 2441</t>
+          <t>PINO, VIRREY DEL 3456</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
@@ -1966,7 +1974,7 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>804732275</t>
+          <t>804876043</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
@@ -1981,7 +1989,7 @@
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Desmonte de poste</t>
         </is>
       </c>
       <c r="I21" t="n">
@@ -1989,7 +1997,7 @@
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Desmonte</t>
         </is>
       </c>
       <c r="K21" t="inlineStr">
@@ -1999,18 +2007,18 @@
       </c>
       <c r="L21" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M21" t="n">
-        <v>-58.45573</v>
+        <v>-58.464354</v>
       </c>
       <c r="N21" t="n">
-        <v>-34.556576</v>
+        <v>-34.572486</v>
       </c>
       <c r="O21" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P21" t="inlineStr">
@@ -2022,27 +2030,27 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>804787368</t>
+          <t>804922147</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>4/17/2025</t>
+          <t>4/24/2025</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>San Blas 2591</t>
+          <t>Av. Álvarez Thomas 1171</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>804787368</t>
+          <t>804922147</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
@@ -2061,7 +2069,7 @@
         </is>
       </c>
       <c r="I22" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J22" t="inlineStr">
         <is>
@@ -2079,14 +2087,14 @@
         </is>
       </c>
       <c r="M22" t="n">
-        <v>-58.477427</v>
+        <v>-58.45793</v>
       </c>
       <c r="N22" t="n">
-        <v>-34.609261</v>
+        <v>-34.578334</v>
       </c>
       <c r="O22" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P22" t="inlineStr">
@@ -2098,17 +2106,17 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>5624</t>
+          <t>804922171</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>4/22/2025</t>
+          <t>4/24/2025</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>PINO, VIRREY DEL 3456</t>
+          <t>Virrey Arredondo 3581</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
@@ -2118,7 +2126,7 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>804876043</t>
+          <t>804922171</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
@@ -2133,7 +2141,7 @@
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>Desmonte de poste</t>
+          <t>Aplomar</t>
         </is>
       </c>
       <c r="I23" t="n">
@@ -2141,7 +2149,7 @@
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>Desmonte</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K23" t="inlineStr">
@@ -2151,14 +2159,14 @@
       </c>
       <c r="L23" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M23" t="n">
-        <v>-58.464354</v>
+        <v>-58.459513</v>
       </c>
       <c r="N23" t="n">
-        <v>-34.572486</v>
+        <v>-34.578019</v>
       </c>
       <c r="O23" t="inlineStr">
         <is>
@@ -2174,7 +2182,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>804922147</t>
+          <t>5656</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -2184,17 +2192,17 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Av. Álvarez Thomas 1171</t>
+          <t>ECHEVERRIA 5893</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>804922147</t>
+          <t>804922184</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
@@ -2209,15 +2217,15 @@
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Poste con base quebrada</t>
         </is>
       </c>
       <c r="I24" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J24" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Desmonte</t>
         </is>
       </c>
       <c r="K24" t="inlineStr">
@@ -2227,18 +2235,18 @@
       </c>
       <c r="L24" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M24" t="n">
-        <v>-58.45793</v>
+        <v>-58.489627</v>
       </c>
       <c r="N24" t="n">
-        <v>-34.578334</v>
+        <v>-34.583761</v>
       </c>
       <c r="O24" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P24" t="inlineStr">
@@ -2250,27 +2258,27 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>804922171</t>
+          <t>6173</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>4/24/2025</t>
+          <t>4/29/2025</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Virrey Arredondo 3581</t>
+          <t>ARMENIA 2321</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>804922171</t>
+          <t>805507398</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
@@ -2285,7 +2293,7 @@
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>Aplomar</t>
+          <t>Picada volvio a entrar como caso 6325</t>
         </is>
       </c>
       <c r="I25" t="n">
@@ -2293,7 +2301,7 @@
       </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K25" t="inlineStr">
@@ -2303,40 +2311,40 @@
       </c>
       <c r="L25" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M25" t="n">
-        <v>-58.459513</v>
+        <v>-58.420549</v>
       </c>
       <c r="N25" t="n">
-        <v>-34.578019</v>
+        <v>-34.585103</v>
       </c>
       <c r="O25" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P25" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>5656</t>
+          <t>5715</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>4/24/2025</t>
+          <t>5/1/2025</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>ECHEVERRIA 5893</t>
+          <t>CUENCA 4690</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
@@ -2346,7 +2354,7 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>804922184</t>
+          <t>805579094</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
@@ -2361,7 +2369,7 @@
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>Poste con base quebrada</t>
+          <t>Aplomar poste</t>
         </is>
       </c>
       <c r="I26" t="n">
@@ -2369,7 +2377,7 @@
       </c>
       <c r="J26" t="inlineStr">
         <is>
-          <t>Desmonte</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K26" t="inlineStr">
@@ -2383,10 +2391,10 @@
         </is>
       </c>
       <c r="M26" t="n">
-        <v>-58.489627</v>
+        <v>-58.506061</v>
       </c>
       <c r="N26" t="n">
-        <v>-34.583761</v>
+        <v>-34.588887</v>
       </c>
       <c r="O26" t="inlineStr">
         <is>
@@ -2402,27 +2410,27 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>6173</t>
+          <t>5719</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>4/29/2025</t>
+          <t>5/1/2025</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>ARMENIA 2321</t>
+          <t>CABEZON, JOSE LEON 2440</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>805507398</t>
+          <t>805579157</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
@@ -2437,7 +2445,7 @@
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>Picada volvio a entrar como caso 6325</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I27" t="n">
@@ -2459,26 +2467,26 @@
         </is>
       </c>
       <c r="M27" t="n">
-        <v>-58.420549</v>
+        <v>-58.499967</v>
       </c>
       <c r="N27" t="n">
-        <v>-34.585103</v>
+        <v>-34.57974</v>
       </c>
       <c r="O27" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P27" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>5715</t>
+          <t>6333</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -2488,17 +2496,17 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>CUENCA 4690</t>
+          <t>ORTEGA Y GASSET 1816</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>805579094</t>
+          <t>805655342</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
@@ -2513,7 +2521,7 @@
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>Aplomar poste</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I28" t="n">
@@ -2521,7 +2529,7 @@
       </c>
       <c r="J28" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K28" t="inlineStr">
@@ -2531,50 +2539,50 @@
       </c>
       <c r="L28" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M28" t="n">
-        <v>-58.506061</v>
+        <v>-58.432556</v>
       </c>
       <c r="N28" t="n">
-        <v>-34.588887</v>
+        <v>-34.570279</v>
       </c>
       <c r="O28" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P28" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>5719</t>
+          <t>805707165</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>5/1/2025</t>
+          <t>5/7/2025</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>CABEZON, JOSE LEON 2440</t>
+          <t>Baez 793</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>805579157</t>
+          <t>805707165</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
@@ -2589,7 +2597,7 @@
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>DESMONTAR COLUMNA DE 7 MTS Y TRANSFERIR A COMUNITARIA</t>
         </is>
       </c>
       <c r="I29" t="n">
@@ -2607,50 +2615,50 @@
       </c>
       <c r="L29" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M29" t="n">
-        <v>-58.499967</v>
+        <v>-58.436165</v>
       </c>
       <c r="N29" t="n">
-        <v>-34.57974</v>
+        <v>-34.569081</v>
       </c>
       <c r="O29" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P29" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>6333</t>
+          <t>5847</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>5/1/2025</t>
+          <t>5/8/2025</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>ORTEGA Y GASSET 1816</t>
+          <t>JURAMENTO 5321</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>805655342</t>
+          <t>805791839</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
@@ -2687,36 +2695,36 @@
         </is>
       </c>
       <c r="M30" t="n">
-        <v>-58.432556</v>
+        <v>-58.485193</v>
       </c>
       <c r="N30" t="n">
-        <v>-34.570279</v>
+        <v>-34.579621</v>
       </c>
       <c r="O30" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P30" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>805707165</t>
+          <t>232</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>5/7/2025</t>
+          <t>5/9/2025</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Baez 793</t>
+          <t>Gorostiaga 2286</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
@@ -2726,7 +2734,7 @@
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>805707165</t>
+          <t>805791858</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
@@ -2741,7 +2749,7 @@
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>DESMONTAR COLUMNA DE 7 MTS Y TRANSFERIR A COMUNITARIA</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I31" t="n">
@@ -2759,14 +2767,14 @@
       </c>
       <c r="L31" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M31" t="n">
-        <v>-58.436165</v>
+        <v>-58.441563</v>
       </c>
       <c r="N31" t="n">
-        <v>-34.569081</v>
+        <v>-34.569743</v>
       </c>
       <c r="O31" t="inlineStr">
         <is>
@@ -2782,7 +2790,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>5847</t>
+          <t>-406</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
@@ -2792,7 +2800,7 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>JURAMENTO 5321</t>
+          <t>Olof palme 4144</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
@@ -2802,7 +2810,7 @@
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>805791839</t>
+          <t>805791925</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
@@ -2817,7 +2825,7 @@
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Tensar 2 riendas a pique columna 168</t>
         </is>
       </c>
       <c r="I32" t="n">
@@ -2825,7 +2833,7 @@
       </c>
       <c r="J32" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Tensor</t>
         </is>
       </c>
       <c r="K32" t="inlineStr">
@@ -2835,18 +2843,18 @@
       </c>
       <c r="L32" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M32" t="n">
-        <v>-58.485193</v>
+        <v>-58.488252</v>
       </c>
       <c r="N32" t="n">
-        <v>-34.579621</v>
+        <v>-34.553391</v>
       </c>
       <c r="O32" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P32" t="inlineStr">
@@ -2858,27 +2866,27 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>232</t>
+          <t>5826</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>5/9/2025</t>
+          <t>5/19/2025</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Gorostiaga 2286</t>
+          <t>ALBARELLOS AV. 3180</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>805791858</t>
+          <t>806926466</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
@@ -2893,7 +2901,7 @@
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Columna (metal) inclinada</t>
         </is>
       </c>
       <c r="I33" t="n">
@@ -2901,7 +2909,7 @@
       </c>
       <c r="J33" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K33" t="inlineStr">
@@ -2911,40 +2919,40 @@
       </c>
       <c r="L33" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M33" t="n">
-        <v>-58.441563</v>
+        <v>-58.513552</v>
       </c>
       <c r="N33" t="n">
-        <v>-34.569743</v>
+        <v>-34.579829</v>
       </c>
       <c r="O33" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P33" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>-406</t>
+          <t>5825</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>5/8/2025</t>
+          <t>5/19/2025</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Olof palme 4144</t>
+          <t>PAZ, GRAL. AV. 5602</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
@@ -2954,7 +2962,7 @@
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>805791925</t>
+          <t>806926472</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
@@ -2969,7 +2977,7 @@
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>Tensar 2 riendas a pique columna 168</t>
+          <t>reparar rienda cortada - ver foto no es la misma que albarellos</t>
         </is>
       </c>
       <c r="I34" t="n">
@@ -2991,14 +2999,14 @@
         </is>
       </c>
       <c r="M34" t="n">
-        <v>-58.488252</v>
+        <v>-58.513685</v>
       </c>
       <c r="N34" t="n">
-        <v>-34.553391</v>
+        <v>-34.579838</v>
       </c>
       <c r="O34" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P34" t="inlineStr">
@@ -3010,27 +3018,27 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>5826</t>
+          <t>6020</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>5/19/2025</t>
+          <t>6/5/2025</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>ALBARELLOS AV. 3180</t>
+          <t>RAVIGNANI, EMILIO, DR. 2036</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>806926466</t>
+          <t>807215465</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
@@ -3045,7 +3053,7 @@
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>Columna (metal) inclinada</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I35" t="n">
@@ -3053,7 +3061,7 @@
       </c>
       <c r="J35" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K35" t="inlineStr">
@@ -3063,50 +3071,50 @@
       </c>
       <c r="L35" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M35" t="n">
-        <v>-58.513552</v>
+        <v>-58.436298</v>
       </c>
       <c r="N35" t="n">
-        <v>-34.579829</v>
+        <v>-34.578972</v>
       </c>
       <c r="O35" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P35" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>5825</t>
+          <t>6144</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>5/19/2025</t>
+          <t>6/11/2025</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>PAZ, GRAL. AV. 5602</t>
+          <t>TURIN 2990</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>806926472</t>
+          <t>807458282</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
@@ -3121,7 +3129,7 @@
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>reparar rienda cortada - ver foto no es la misma que albarellos</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I36" t="n">
@@ -3129,7 +3137,7 @@
       </c>
       <c r="J36" t="inlineStr">
         <is>
-          <t>Tensor</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K36" t="inlineStr">
@@ -3139,14 +3147,14 @@
       </c>
       <c r="L36" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M36" t="n">
-        <v>-58.513685</v>
+        <v>-58.480925</v>
       </c>
       <c r="N36" t="n">
-        <v>-34.579838</v>
+        <v>-34.585471</v>
       </c>
       <c r="O36" t="inlineStr">
         <is>
@@ -3162,27 +3170,27 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>6020</t>
+          <t>6143</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>6/5/2025</t>
+          <t>6/11/2025</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>RAVIGNANI, EMILIO, DR. 2036</t>
+          <t>SOLANO LOPEZ, F., MARISCAL 2845</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>807215465</t>
+          <t>807458296</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
@@ -3219,26 +3227,26 @@
         </is>
       </c>
       <c r="M37" t="n">
-        <v>-58.436298</v>
+        <v>-58.495071</v>
       </c>
       <c r="N37" t="n">
-        <v>-34.578972</v>
+        <v>-34.593122</v>
       </c>
       <c r="O37" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P37" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>6144</t>
+          <t>6141</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
@@ -3248,17 +3256,17 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>TURIN 2990</t>
+          <t>EL PAMPERO 2618</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>807458282</t>
+          <t>807458310</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
@@ -3295,10 +3303,10 @@
         </is>
       </c>
       <c r="M38" t="n">
-        <v>-58.480925</v>
+        <v>-58.481942</v>
       </c>
       <c r="N38" t="n">
-        <v>-34.585471</v>
+        <v>-34.602989</v>
       </c>
       <c r="O38" t="inlineStr">
         <is>
@@ -3314,27 +3322,27 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>6143</t>
+          <t>-478</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>6/11/2025</t>
+          <t>6/15/2025</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>SOLANO LOPEZ, F., MARISCAL 2845</t>
+          <t>Chivilcoy 4875</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>807458296</t>
+          <t>807508509</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
@@ -3349,7 +3357,7 @@
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Poste podrido</t>
         </is>
       </c>
       <c r="I39" t="n">
@@ -3367,14 +3375,14 @@
       </c>
       <c r="L39" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M39" t="n">
-        <v>-58.495071</v>
+        <v>-58.517389</v>
       </c>
       <c r="N39" t="n">
-        <v>-34.593122</v>
+        <v>-34.593541</v>
       </c>
       <c r="O39" t="inlineStr">
         <is>
@@ -3390,27 +3398,27 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>6141</t>
+          <t>6171</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>6/11/2025</t>
+          <t>6/18/2025</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>EL PAMPERO 2618</t>
+          <t>CABELLO 3486</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>807458310</t>
+          <t>807658640</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
@@ -3425,7 +3433,7 @@
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Columna inclinada evaluar con inspector un corrimiento</t>
         </is>
       </c>
       <c r="I40" t="n">
@@ -3447,46 +3455,46 @@
         </is>
       </c>
       <c r="M40" t="n">
-        <v>-58.481942</v>
+        <v>-58.409579</v>
       </c>
       <c r="N40" t="n">
-        <v>-34.602989</v>
+        <v>-34.581134</v>
       </c>
       <c r="O40" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P40" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>-478</t>
+          <t>6230</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>6/15/2025</t>
+          <t>6/24/2025</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Chivilcoy 4875</t>
+          <t>Santa maria de oro	2722</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>807508509</t>
+          <t>807763066</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
@@ -3501,7 +3509,7 @@
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>Poste podrido</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I41" t="n">
@@ -3519,40 +3527,40 @@
       </c>
       <c r="L41" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M41" t="n">
-        <v>-58.517389</v>
+        <v>-58.422315</v>
       </c>
       <c r="N41" t="n">
-        <v>-34.593541</v>
+        <v>-34.576988</v>
       </c>
       <c r="O41" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P41" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>6171</t>
+          <t>6231</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>6/18/2025</t>
+          <t>6/24/2025</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>CABELLO 3486</t>
+          <t>Ciudad de la Paz 275</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
@@ -3562,7 +3570,7 @@
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>807658640</t>
+          <t>807763070</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
@@ -3577,7 +3585,7 @@
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>Columna inclinada evaluar con inspector un corrimiento</t>
+          <t>Aplomar o cambiar</t>
         </is>
       </c>
       <c r="I42" t="n">
@@ -3595,14 +3603,14 @@
       </c>
       <c r="L42" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M42" t="n">
-        <v>-58.409579</v>
+        <v>-58.441049</v>
       </c>
       <c r="N42" t="n">
-        <v>-34.581134</v>
+        <v>-34.574625</v>
       </c>
       <c r="O42" t="inlineStr">
         <is>
@@ -3618,7 +3626,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>6230</t>
+          <t>6235</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
@@ -3628,17 +3636,17 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Santa maria de oro	2722</t>
+          <t>HUERGO 389</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>807763066</t>
+          <t>807763078</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
@@ -3675,10 +3683,10 @@
         </is>
       </c>
       <c r="M43" t="n">
-        <v>-58.422315</v>
+        <v>-58.432722</v>
       </c>
       <c r="N43" t="n">
-        <v>-34.576988</v>
+        <v>-34.572371</v>
       </c>
       <c r="O43" t="inlineStr">
         <is>
@@ -3694,17 +3702,17 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>6231</t>
+          <t>6295</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>6/24/2025</t>
+          <t>6/30/2025</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Ciudad de la Paz 275</t>
+          <t>SOLER 6017</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
@@ -3714,7 +3722,7 @@
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>807763070</t>
+          <t>807851636</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
@@ -3729,7 +3737,7 @@
       </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t>Aplomar o cambiar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I44" t="n">
@@ -3747,14 +3755,14 @@
       </c>
       <c r="L44" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M44" t="n">
-        <v>-58.441049</v>
+        <v>-58.436808</v>
       </c>
       <c r="N44" t="n">
-        <v>-34.574625</v>
+        <v>-34.577464</v>
       </c>
       <c r="O44" t="inlineStr">
         <is>
@@ -3770,27 +3778,27 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>6235</t>
+          <t>6332</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>6/24/2025</t>
+          <t>7/3/2025</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>HUERGO 389</t>
+          <t>ARAOZ 2560</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>807763078</t>
+          <t>807965818</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
@@ -3827,10 +3835,10 @@
         </is>
       </c>
       <c r="M45" t="n">
-        <v>-58.432722</v>
+        <v>-58.414507</v>
       </c>
       <c r="N45" t="n">
-        <v>-34.572371</v>
+        <v>-34.585377</v>
       </c>
       <c r="O45" t="inlineStr">
         <is>
@@ -3846,27 +3854,27 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>6295</t>
+          <t>-503</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>6/30/2025</t>
+          <t>7/10/2025</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>SOLER 6017</t>
+          <t>Salguero 842</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>807851636</t>
+          <t>808148673</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
@@ -3881,7 +3889,7 @@
       </c>
       <c r="H46" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambiar columna picada en la base</t>
         </is>
       </c>
       <c r="I46" t="n">
@@ -3903,14 +3911,14 @@
         </is>
       </c>
       <c r="M46" t="n">
-        <v>-58.436808</v>
+        <v>-58.419166</v>
       </c>
       <c r="N46" t="n">
-        <v>-34.577464</v>
+        <v>-34.600265</v>
       </c>
       <c r="O46" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P46" t="inlineStr">
@@ -3922,27 +3930,27 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>6332</t>
+          <t>6506</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>7/3/2025</t>
+          <t>7/10/2025</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>ARAOZ 2560</t>
+          <t>Ohiggins 1611</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>807965818</t>
+          <t>808148679</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
@@ -3957,7 +3965,7 @@
       </c>
       <c r="H47" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Columna podrida en la base</t>
         </is>
       </c>
       <c r="I47" t="n">
@@ -3970,7 +3978,7 @@
       </c>
       <c r="K47" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L47" t="inlineStr">
@@ -3979,46 +3987,46 @@
         </is>
       </c>
       <c r="M47" t="n">
-        <v>-58.414507</v>
+        <v>-58.448993</v>
       </c>
       <c r="N47" t="n">
-        <v>-34.585377</v>
+        <v>-34.564383</v>
       </c>
       <c r="O47" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P47" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>-503</t>
+          <t>6437</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>7/10/2025</t>
+          <t>7/17/2025</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Salguero 842</t>
+          <t>MILLER 4590</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>808148673</t>
+          <t>808400306</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
@@ -4033,7 +4041,7 @@
       </c>
       <c r="H48" t="inlineStr">
         <is>
-          <t>Cambiar columna picada en la base</t>
+          <t>Columna corroida</t>
         </is>
       </c>
       <c r="I48" t="n">
@@ -4055,46 +4063,46 @@
         </is>
       </c>
       <c r="M48" t="n">
-        <v>-58.419166</v>
+        <v>-58.495482</v>
       </c>
       <c r="N48" t="n">
-        <v>-34.600265</v>
+        <v>-34.552614</v>
       </c>
       <c r="O48" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P48" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>6506</t>
+          <t>6538</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>7/10/2025</t>
+          <t>7/17/2025</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Ohiggins 1611</t>
+          <t>Pedraza Manuela 4101</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>808148679</t>
+          <t>808400353</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
@@ -4109,7 +4117,7 @@
       </c>
       <c r="H49" t="inlineStr">
         <is>
-          <t>Columna podrida en la base</t>
+          <t xml:space="preserve">Podrida en la base </t>
         </is>
       </c>
       <c r="I49" t="n">
@@ -4122,7 +4130,7 @@
       </c>
       <c r="K49" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L49" t="inlineStr">
@@ -4131,14 +4139,14 @@
         </is>
       </c>
       <c r="M49" t="n">
-        <v>-58.448993</v>
+        <v>-58.481569</v>
       </c>
       <c r="N49" t="n">
-        <v>-34.564383</v>
+        <v>-34.559853</v>
       </c>
       <c r="O49" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P49" t="inlineStr">
@@ -4150,27 +4158,27 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>6437</t>
+          <t>-525</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>7/17/2025</t>
+          <t>7/22/2025</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>MILLER 4590</t>
+          <t>Zabala 3567</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>808400306</t>
+          <t>808480549</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
@@ -4185,7 +4193,7 @@
       </c>
       <c r="H50" t="inlineStr">
         <is>
-          <t>Columna corroida</t>
+          <t>Corroida en base para recambio</t>
         </is>
       </c>
       <c r="I50" t="n">
@@ -4207,14 +4215,14 @@
         </is>
       </c>
       <c r="M50" t="n">
-        <v>-58.495482</v>
+        <v>-58.457492</v>
       </c>
       <c r="N50" t="n">
-        <v>-34.552614</v>
+        <v>-34.579336</v>
       </c>
       <c r="O50" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P50" t="inlineStr">
@@ -4226,27 +4234,27 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>6538</t>
+          <t>6484</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>7/17/2025</t>
+          <t>7/24/2025</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Pedraza Manuela 4101</t>
+          <t>URIARTE 2396</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>808400353</t>
+          <t>808509373</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
@@ -4261,7 +4269,7 @@
       </c>
       <c r="H51" t="inlineStr">
         <is>
-          <t xml:space="preserve">Podrida en la base </t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I51" t="n">
@@ -4283,46 +4291,46 @@
         </is>
       </c>
       <c r="M51" t="n">
-        <v>-58.481569</v>
+        <v>-58.423934</v>
       </c>
       <c r="N51" t="n">
-        <v>-34.559853</v>
+        <v>-34.581562</v>
       </c>
       <c r="O51" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P51" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>-525</t>
+          <t>6512</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>7/22/2025</t>
+          <t>7/28/2025</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>Zabala 3567</t>
+          <t>GASCON 1195</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>808480549</t>
+          <t>808571975</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
@@ -4337,7 +4345,7 @@
       </c>
       <c r="H52" t="inlineStr">
         <is>
-          <t>Corroida en base para recambio</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I52" t="n">
@@ -4359,36 +4367,36 @@
         </is>
       </c>
       <c r="M52" t="n">
-        <v>-58.457492</v>
+        <v>-58.423127</v>
       </c>
       <c r="N52" t="n">
-        <v>-34.579336</v>
+        <v>-34.596476</v>
       </c>
       <c r="O52" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P52" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>6484</t>
+          <t>6513</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>7/24/2025</t>
+          <t>7/28/2025</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>URIARTE 2396</t>
+          <t>DORREGO 1925</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
@@ -4398,7 +4406,7 @@
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>808509373</t>
+          <t>808571976</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
@@ -4435,10 +4443,10 @@
         </is>
       </c>
       <c r="M53" t="n">
-        <v>-58.423934</v>
+        <v>-58.441281</v>
       </c>
       <c r="N53" t="n">
-        <v>-34.581562</v>
+        <v>-34.579867</v>
       </c>
       <c r="O53" t="inlineStr">
         <is>
@@ -4454,7 +4462,7 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>6512</t>
+          <t>6519</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
@@ -4464,7 +4472,7 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>GASCON 1195</t>
+          <t>SALGUERO, JERONIMO 2874</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
@@ -4474,7 +4482,7 @@
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>808571975</t>
+          <t>808571977</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
@@ -4489,7 +4497,7 @@
       </c>
       <c r="H54" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Reparar rienda</t>
         </is>
       </c>
       <c r="I54" t="n">
@@ -4497,7 +4505,7 @@
       </c>
       <c r="J54" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Tensor</t>
         </is>
       </c>
       <c r="K54" t="inlineStr">
@@ -4507,14 +4515,14 @@
       </c>
       <c r="L54" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M54" t="n">
-        <v>-58.423127</v>
+        <v>-58.407256</v>
       </c>
       <c r="N54" t="n">
-        <v>-34.596476</v>
+        <v>-34.578976</v>
       </c>
       <c r="O54" t="inlineStr">
         <is>
@@ -4530,27 +4538,27 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>6513</t>
+          <t>-538</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>7/28/2025</t>
+          <t>7/31/2025</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>DORREGO 1925</t>
+          <t>Malabia 964</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>808571976</t>
+          <t>808609237</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
@@ -4565,7 +4573,7 @@
       </c>
       <c r="H55" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambiar poste mal estado por PRFV</t>
         </is>
       </c>
       <c r="I55" t="n">
@@ -4583,14 +4591,14 @@
       </c>
       <c r="L55" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M55" t="n">
-        <v>-58.441281</v>
+        <v>-58.433634</v>
       </c>
       <c r="N55" t="n">
-        <v>-34.579867</v>
+        <v>-34.595018</v>
       </c>
       <c r="O55" t="inlineStr">
         <is>
@@ -4606,27 +4614,27 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>6519</t>
+          <t>6545</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>7/28/2025</t>
+          <t>8/4/2025</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>SALGUERO, JERONIMO 2874</t>
+          <t>SCALABRINI ORTIZ, RAUL AV. 708</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>808571977</t>
+          <t>808703864</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
@@ -4641,7 +4649,7 @@
       </c>
       <c r="H56" t="inlineStr">
         <is>
-          <t>Reparar rienda</t>
+          <t>Aplomar</t>
         </is>
       </c>
       <c r="I56" t="n">
@@ -4649,7 +4657,7 @@
       </c>
       <c r="J56" t="inlineStr">
         <is>
-          <t>Tensor</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K56" t="inlineStr">
@@ -4659,14 +4667,14 @@
       </c>
       <c r="L56" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M56" t="n">
-        <v>-58.407256</v>
+        <v>-58.434339</v>
       </c>
       <c r="N56" t="n">
-        <v>-34.578976</v>
+        <v>-34.59693</v>
       </c>
       <c r="O56" t="inlineStr">
         <is>
@@ -4682,27 +4690,27 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>-538</t>
+          <t>6498</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>7/31/2025</t>
+          <t>8/6/2025</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>Malabia 964</t>
+          <t>BUCARELLI 2087</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>808609237</t>
+          <t>808733908</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
@@ -4717,7 +4725,7 @@
       </c>
       <c r="H57" t="inlineStr">
         <is>
-          <t>Cambiar poste mal estado por PRFV</t>
+          <t>Base picada</t>
         </is>
       </c>
       <c r="I57" t="n">
@@ -4735,50 +4743,50 @@
       </c>
       <c r="L57" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M57" t="n">
-        <v>-58.433634</v>
+        <v>-58.485592</v>
       </c>
       <c r="N57" t="n">
-        <v>-34.595018</v>
+        <v>-34.578586</v>
       </c>
       <c r="O57" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P57" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>6545</t>
+          <t>-547</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>8/4/2025</t>
+          <t>8/6/2025</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>SCALABRINI ORTIZ, RAUL AV. 708</t>
+          <t>Habana 4210</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>808703864</t>
+          <t>808733921</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
@@ -4793,7 +4801,7 @@
       </c>
       <c r="H58" t="inlineStr">
         <is>
-          <t>Aplomar</t>
+          <t>Cambiar poste dañado</t>
         </is>
       </c>
       <c r="I58" t="n">
@@ -4801,7 +4809,7 @@
       </c>
       <c r="J58" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K58" t="inlineStr">
@@ -4811,50 +4819,50 @@
       </c>
       <c r="L58" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M58" t="n">
-        <v>-58.434339</v>
+        <v>-58.515873</v>
       </c>
       <c r="N58" t="n">
-        <v>-34.59693</v>
+        <v>-34.599425</v>
       </c>
       <c r="O58" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P58" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>6498</t>
+          <t>6579</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>8/6/2025</t>
+          <t>8/7/2025</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>BUCARELLI 2087</t>
+          <t>RIVADAVIA MARTIN, COMODORO 1350</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>808733908</t>
+          <t>808749184</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
@@ -4869,7 +4877,7 @@
       </c>
       <c r="H59" t="inlineStr">
         <is>
-          <t>Base picada</t>
+          <t>Poste inclinado</t>
         </is>
       </c>
       <c r="I59" t="n">
@@ -4877,7 +4885,7 @@
       </c>
       <c r="J59" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K59" t="inlineStr">
@@ -4887,173 +4895,21 @@
       </c>
       <c r="L59" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M59" t="n">
-        <v>-58.485592</v>
+        <v>-58.461024</v>
       </c>
       <c r="N59" t="n">
-        <v>-34.578586</v>
+        <v>-34.539409</v>
       </c>
       <c r="O59" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P59" t="inlineStr">
-        <is>
-          <t>Capital Norte</t>
-        </is>
-      </c>
-    </row>
-    <row r="60">
-      <c r="A60" t="inlineStr">
-        <is>
-          <t>-547</t>
-        </is>
-      </c>
-      <c r="B60" t="inlineStr">
-        <is>
-          <t>8/6/2025</t>
-        </is>
-      </c>
-      <c r="C60" t="inlineStr">
-        <is>
-          <t>Habana 4210</t>
-        </is>
-      </c>
-      <c r="D60" t="inlineStr">
-        <is>
-          <t>11</t>
-        </is>
-      </c>
-      <c r="E60" t="inlineStr">
-        <is>
-          <t>808733921</t>
-        </is>
-      </c>
-      <c r="F60" t="inlineStr">
-        <is>
-          <t>NEW</t>
-        </is>
-      </c>
-      <c r="G60" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H60" t="inlineStr">
-        <is>
-          <t>Cambiar poste dañado</t>
-        </is>
-      </c>
-      <c r="I60" t="n">
-        <v>1</v>
-      </c>
-      <c r="J60" t="inlineStr">
-        <is>
-          <t>Cambio</t>
-        </is>
-      </c>
-      <c r="K60" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L60" t="inlineStr">
-        <is>
-          <t>Poste</t>
-        </is>
-      </c>
-      <c r="M60" t="n">
-        <v>-58.515873</v>
-      </c>
-      <c r="N60" t="n">
-        <v>-34.599425</v>
-      </c>
-      <c r="O60" t="inlineStr">
-        <is>
-          <t>Paternal</t>
-        </is>
-      </c>
-      <c r="P60" t="inlineStr">
-        <is>
-          <t>Capital Norte</t>
-        </is>
-      </c>
-    </row>
-    <row r="61">
-      <c r="A61" t="inlineStr">
-        <is>
-          <t>6579</t>
-        </is>
-      </c>
-      <c r="B61" t="inlineStr">
-        <is>
-          <t>8/7/2025</t>
-        </is>
-      </c>
-      <c r="C61" t="inlineStr">
-        <is>
-          <t>RIVADAVIA MARTIN, COMODORO 1350</t>
-        </is>
-      </c>
-      <c r="D61" t="inlineStr">
-        <is>
-          <t>13</t>
-        </is>
-      </c>
-      <c r="E61" t="inlineStr">
-        <is>
-          <t>808749184</t>
-        </is>
-      </c>
-      <c r="F61" t="inlineStr">
-        <is>
-          <t>NEW</t>
-        </is>
-      </c>
-      <c r="G61" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H61" t="inlineStr">
-        <is>
-          <t>Poste inclinado</t>
-        </is>
-      </c>
-      <c r="I61" t="n">
-        <v>1</v>
-      </c>
-      <c r="J61" t="inlineStr">
-        <is>
-          <t>Aplomo</t>
-        </is>
-      </c>
-      <c r="K61" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L61" t="inlineStr">
-        <is>
-          <t>Poste</t>
-        </is>
-      </c>
-      <c r="M61" t="n">
-        <v>-58.461024</v>
-      </c>
-      <c r="N61" t="n">
-        <v>-34.539409</v>
-      </c>
-      <c r="O61" t="inlineStr">
-        <is>
-          <t>Saavedra</t>
-        </is>
-      </c>
-      <c r="P61" t="inlineStr">
         <is>
           <t>Capital Norte</t>
         </is>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-08-08 12:13:27)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_NEW.xlsx
+++ b/mapa_interactivo_NEW.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P59"/>
+  <dimension ref="A1:P61"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -822,17 +822,17 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>4595</t>
+          <t>5589</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>1/15/2025</t>
+          <t>12/31/2023</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>PAROISSIEN 1806</t>
+          <t>ARCOS 1520</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -842,7 +842,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>802747617</t>
+          <t>799540526</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -852,41 +852,33 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>Aplomar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I6" t="n">
-        <v>1</v>
-      </c>
-      <c r="J6" t="inlineStr">
-        <is>
-          <t>Aplomo</t>
-        </is>
-      </c>
-      <c r="K6" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="J6" t="inlineStr"/>
+      <c r="K6" t="inlineStr"/>
       <c r="L6" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M6" t="n">
-        <v>-58.464172</v>
+        <v>-58.449125</v>
       </c>
       <c r="N6" t="n">
-        <v>-34.543845</v>
+        <v>-34.565958</v>
       </c>
       <c r="O6" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P6" t="inlineStr">
@@ -898,27 +890,27 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>4662</t>
+          <t>4595</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>1/21/2025</t>
+          <t>1/15/2025</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>ALTOLAGUIRRE 2397</t>
+          <t>PAROISSIEN 1806</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>802823938</t>
+          <t>802747617</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -933,7 +925,7 @@
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>Inclinada</t>
+          <t>Aplomar</t>
         </is>
       </c>
       <c r="I7" t="n">
@@ -951,18 +943,18 @@
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M7" t="n">
-        <v>-58.490766</v>
+        <v>-58.464172</v>
       </c>
       <c r="N7" t="n">
-        <v>-34.576987</v>
+        <v>-34.543845</v>
       </c>
       <c r="O7" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P7" t="inlineStr">
@@ -974,27 +966,27 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>6036</t>
+          <t>4662</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>2/24/2025</t>
+          <t>1/21/2025</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>MEDRANO 1715</t>
+          <t>ALTOLAGUIRRE 2397</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>803608181</t>
+          <t>802823938</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -1007,18 +999,22 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H8" t="inlineStr"/>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>Inclinada</t>
+        </is>
+      </c>
       <c r="I8" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L8" t="inlineStr">
@@ -1027,46 +1023,46 @@
         </is>
       </c>
       <c r="M8" t="n">
-        <v>-58.418236</v>
+        <v>-58.490766</v>
       </c>
       <c r="N8" t="n">
-        <v>-34.589859</v>
+        <v>-34.576987</v>
       </c>
       <c r="O8" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P8" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>803608480</t>
+          <t>4862</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>2/24/2025</t>
+          <t>1/23/2025</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>GUATEMALA /ALT/ 4415</t>
+          <t>ARCOS 2263</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>803608480</t>
+          <t>802857379</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -1076,12 +1072,12 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t xml:space="preserve">Guatemala 4415 </t>
+          <t>picada</t>
         </is>
       </c>
       <c r="I9" t="n">
@@ -1094,7 +1090,7 @@
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L9" t="inlineStr">
@@ -1103,46 +1099,46 @@
         </is>
       </c>
       <c r="M9" t="n">
-        <v>-58.421661</v>
+        <v>-58.455082</v>
       </c>
       <c r="N9" t="n">
-        <v>-34.588428</v>
+        <v>-34.558883</v>
       </c>
       <c r="O9" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P9" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>5053</t>
+          <t>6036</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>3/11/2025</t>
+          <t>2/24/2025</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>MENDOZA 1153</t>
+          <t>MEDRANO 1715</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>803969314</t>
+          <t>803608181</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
@@ -1155,11 +1151,7 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H10" t="inlineStr">
-        <is>
-          <t>Poste</t>
-        </is>
-      </c>
+      <c r="H10" t="inlineStr"/>
       <c r="I10" t="n">
         <v>0</v>
       </c>
@@ -1170,55 +1162,55 @@
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L10" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M10" t="n">
-        <v>-58.44463</v>
+        <v>-58.418236</v>
       </c>
       <c r="N10" t="n">
-        <v>-34.553354</v>
+        <v>-34.589859</v>
       </c>
       <c r="O10" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P10" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>6071</t>
+          <t>803608480</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>3/17/2025</t>
+          <t>2/24/2025</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>OSORIO 4994</t>
+          <t>GUATEMALA /ALT/ 4415</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>804053324</t>
+          <t>803608480</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
@@ -1231,7 +1223,11 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H11" t="inlineStr"/>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Guatemala 4415 </t>
+        </is>
+      </c>
       <c r="I11" t="n">
         <v>0</v>
       </c>
@@ -1251,46 +1247,46 @@
         </is>
       </c>
       <c r="M11" t="n">
-        <v>-58.466241</v>
+        <v>-58.421661</v>
       </c>
       <c r="N11" t="n">
-        <v>-34.595741</v>
+        <v>-34.588428</v>
       </c>
       <c r="O11" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P11" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>3348</t>
+          <t>5053</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>3/27/2025</t>
+          <t>3/11/2025</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>ESTOMBA 2626</t>
+          <t>MENDOZA 1153</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>804309704</t>
+          <t>803969314</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
@@ -1305,15 +1301,15 @@
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="I12" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>Desmonte</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K12" t="inlineStr">
@@ -1323,18 +1319,18 @@
       </c>
       <c r="L12" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M12" t="n">
-        <v>-58.47538</v>
+        <v>-58.44463</v>
       </c>
       <c r="N12" t="n">
-        <v>-34.566015</v>
+        <v>-34.553354</v>
       </c>
       <c r="O12" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P12" t="inlineStr">
@@ -1346,27 +1342,27 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>-312</t>
+          <t>6071</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>3/29/2025</t>
+          <t>3/17/2025</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>MATIENZO BENJAMIN /ALT/ 1831</t>
+          <t>OSORIO 4994</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>804333522</t>
+          <t>804053324</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
@@ -1379,11 +1375,7 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H13" t="inlineStr">
-        <is>
-          <t>Retirar columna ya traspasaron el nodo</t>
-        </is>
-      </c>
+      <c r="H13" t="inlineStr"/>
       <c r="I13" t="n">
         <v>0</v>
       </c>
@@ -1394,7 +1386,7 @@
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L13" t="inlineStr">
@@ -1403,36 +1395,36 @@
         </is>
       </c>
       <c r="M13" t="n">
-        <v>-58.434835</v>
+        <v>-58.466241</v>
       </c>
       <c r="N13" t="n">
-        <v>-34.569129</v>
+        <v>-34.595741</v>
       </c>
       <c r="O13" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P13" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>3430</t>
+          <t>3348</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>4/1/2025</t>
+          <t>3/27/2025</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>MONROE 3838</t>
+          <t>ESTOMBA 2626</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
@@ -1442,7 +1434,7 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>804468442</t>
+          <t>804309704</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
@@ -1457,7 +1449,7 @@
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>Reparar rienda</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I14" t="n">
@@ -1465,7 +1457,7 @@
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>Tensor</t>
+          <t>Desmonte</t>
         </is>
       </c>
       <c r="K14" t="inlineStr">
@@ -1475,14 +1467,14 @@
       </c>
       <c r="L14" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M14" t="n">
-        <v>-58.473659</v>
+        <v>-58.47538</v>
       </c>
       <c r="N14" t="n">
-        <v>-34.566979</v>
+        <v>-34.566015</v>
       </c>
       <c r="O14" t="inlineStr">
         <is>
@@ -1498,27 +1490,27 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>5464</t>
+          <t>-312</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>4/4/2025</t>
+          <t>3/29/2025</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>SUCRE, ANTONIO JOSE DE, MCAL. 3100</t>
+          <t>MATIENZO BENJAMIN /ALT/ 1831</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>804497880</t>
+          <t>804333522</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
@@ -1533,11 +1525,11 @@
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Retirar columna ya traspasaron el nodo</t>
         </is>
       </c>
       <c r="I15" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J15" t="inlineStr">
         <is>
@@ -1546,45 +1538,45 @@
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L15" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M15" t="n">
-        <v>-58.46161</v>
+        <v>-58.434835</v>
       </c>
       <c r="N15" t="n">
-        <v>-34.567849</v>
+        <v>-34.569129</v>
       </c>
       <c r="O15" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P15" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>5469</t>
+          <t>3430</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>4/4/2025</t>
+          <t>4/1/2025</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>ESTADO PLURINACIONAL DE BOLIVIA 5899</t>
+          <t>MONROE 3838</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
@@ -1594,7 +1586,7 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>804497887</t>
+          <t>804468442</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
@@ -1609,7 +1601,7 @@
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>Aplomar</t>
+          <t>Reparar rienda</t>
         </is>
       </c>
       <c r="I16" t="n">
@@ -1617,7 +1609,7 @@
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Tensor</t>
         </is>
       </c>
       <c r="K16" t="inlineStr">
@@ -1631,14 +1623,14 @@
         </is>
       </c>
       <c r="M16" t="n">
-        <v>-58.507746</v>
+        <v>-58.473659</v>
       </c>
       <c r="N16" t="n">
-        <v>-34.574217</v>
+        <v>-34.566979</v>
       </c>
       <c r="O16" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P16" t="inlineStr">
@@ -1650,7 +1642,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>5492</t>
+          <t>5464</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -1660,17 +1652,17 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>ESTADO PLURINACIONAL DE BOLIVIA 5920</t>
+          <t>SUCRE, ANTONIO JOSE DE, MCAL. 3100</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>804498035</t>
+          <t>804497880</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
@@ -1685,7 +1677,7 @@
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>aplomar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I17" t="n">
@@ -1693,7 +1685,7 @@
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K17" t="inlineStr">
@@ -1707,14 +1699,14 @@
         </is>
       </c>
       <c r="M17" t="n">
-        <v>-58.50751</v>
+        <v>-58.46161</v>
       </c>
       <c r="N17" t="n">
-        <v>-34.574543</v>
+        <v>-34.567849</v>
       </c>
       <c r="O17" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P17" t="inlineStr">
@@ -1726,17 +1718,17 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>5599</t>
+          <t>5469</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>4/15/2025</t>
+          <t>4/4/2025</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>ESTOMBA 4052</t>
+          <t>ESTADO PLURINACIONAL DE BOLIVIA 5899</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
@@ -1746,7 +1738,7 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>804732246</t>
+          <t>804497887</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
@@ -1761,7 +1753,7 @@
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>Columna PRFV quedo inclinada (la hicieron como estomba 4056)</t>
+          <t>Aplomar</t>
         </is>
       </c>
       <c r="I18" t="n">
@@ -1774,23 +1766,23 @@
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>Nodo TLC</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L18" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M18" t="n">
-        <v>-58.485407</v>
+        <v>-58.507746</v>
       </c>
       <c r="N18" t="n">
-        <v>-34.552985</v>
+        <v>-34.574217</v>
       </c>
       <c r="O18" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P18" t="inlineStr">
@@ -1802,27 +1794,27 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>5590</t>
+          <t>5492</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>4/15/2025</t>
+          <t>4/4/2025</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>O'HIGGINS 2441</t>
+          <t>ESTADO PLURINACIONAL DE BOLIVIA 5920</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>804732275</t>
+          <t>804498035</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
@@ -1837,7 +1829,7 @@
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>aplomar</t>
         </is>
       </c>
       <c r="I19" t="n">
@@ -1845,7 +1837,7 @@
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K19" t="inlineStr">
@@ -1855,18 +1847,18 @@
       </c>
       <c r="L19" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M19" t="n">
-        <v>-58.45573</v>
+        <v>-58.50751</v>
       </c>
       <c r="N19" t="n">
-        <v>-34.556576</v>
+        <v>-34.574543</v>
       </c>
       <c r="O19" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P19" t="inlineStr">
@@ -1878,27 +1870,27 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>804787368</t>
+          <t>5599</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>4/17/2025</t>
+          <t>4/15/2025</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>San Blas 2591</t>
+          <t>ESTOMBA 4052</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>804787368</t>
+          <t>804732246</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
@@ -1913,7 +1905,7 @@
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Columna PRFV quedo inclinada (la hicieron como estomba 4056)</t>
         </is>
       </c>
       <c r="I20" t="n">
@@ -1921,12 +1913,12 @@
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo TLC</t>
         </is>
       </c>
       <c r="L20" t="inlineStr">
@@ -1935,14 +1927,14 @@
         </is>
       </c>
       <c r="M20" t="n">
-        <v>-58.477427</v>
+        <v>-58.485407</v>
       </c>
       <c r="N20" t="n">
-        <v>-34.609261</v>
+        <v>-34.552985</v>
       </c>
       <c r="O20" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P20" t="inlineStr">
@@ -1954,17 +1946,17 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>5624</t>
+          <t>5590</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>4/22/2025</t>
+          <t>4/15/2025</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>PINO, VIRREY DEL 3456</t>
+          <t>O'HIGGINS 2441</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
@@ -1974,7 +1966,7 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>804876043</t>
+          <t>804732275</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
@@ -1989,7 +1981,7 @@
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>Desmonte de poste</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I21" t="n">
@@ -1997,7 +1989,7 @@
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>Desmonte</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K21" t="inlineStr">
@@ -2007,18 +1999,18 @@
       </c>
       <c r="L21" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M21" t="n">
-        <v>-58.464354</v>
+        <v>-58.45573</v>
       </c>
       <c r="N21" t="n">
-        <v>-34.572486</v>
+        <v>-34.556576</v>
       </c>
       <c r="O21" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P21" t="inlineStr">
@@ -2030,27 +2022,27 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>804922147</t>
+          <t>804787368</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>4/24/2025</t>
+          <t>4/17/2025</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Av. Álvarez Thomas 1171</t>
+          <t>San Blas 2591</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>804922147</t>
+          <t>804787368</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
@@ -2069,7 +2061,7 @@
         </is>
       </c>
       <c r="I22" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J22" t="inlineStr">
         <is>
@@ -2087,14 +2079,14 @@
         </is>
       </c>
       <c r="M22" t="n">
-        <v>-58.45793</v>
+        <v>-58.477427</v>
       </c>
       <c r="N22" t="n">
-        <v>-34.578334</v>
+        <v>-34.609261</v>
       </c>
       <c r="O22" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P22" t="inlineStr">
@@ -2106,17 +2098,17 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>804922171</t>
+          <t>5624</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>4/24/2025</t>
+          <t>4/22/2025</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Virrey Arredondo 3581</t>
+          <t>PINO, VIRREY DEL 3456</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
@@ -2126,7 +2118,7 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>804922171</t>
+          <t>804876043</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
@@ -2141,7 +2133,7 @@
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>Aplomar</t>
+          <t>Desmonte de poste</t>
         </is>
       </c>
       <c r="I23" t="n">
@@ -2149,7 +2141,7 @@
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Desmonte</t>
         </is>
       </c>
       <c r="K23" t="inlineStr">
@@ -2159,14 +2151,14 @@
       </c>
       <c r="L23" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M23" t="n">
-        <v>-58.459513</v>
+        <v>-58.464354</v>
       </c>
       <c r="N23" t="n">
-        <v>-34.578019</v>
+        <v>-34.572486</v>
       </c>
       <c r="O23" t="inlineStr">
         <is>
@@ -2182,7 +2174,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>5656</t>
+          <t>804922147</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -2192,17 +2184,17 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>ECHEVERRIA 5893</t>
+          <t>Av. Álvarez Thomas 1171</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>804922184</t>
+          <t>804922147</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
@@ -2217,15 +2209,15 @@
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>Poste con base quebrada</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I24" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J24" t="inlineStr">
         <is>
-          <t>Desmonte</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K24" t="inlineStr">
@@ -2235,18 +2227,18 @@
       </c>
       <c r="L24" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M24" t="n">
-        <v>-58.489627</v>
+        <v>-58.45793</v>
       </c>
       <c r="N24" t="n">
-        <v>-34.583761</v>
+        <v>-34.578334</v>
       </c>
       <c r="O24" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P24" t="inlineStr">
@@ -2258,27 +2250,27 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>6173</t>
+          <t>804922171</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>4/29/2025</t>
+          <t>4/24/2025</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>ARMENIA 2321</t>
+          <t>Virrey Arredondo 3581</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>805507398</t>
+          <t>804922171</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
@@ -2293,7 +2285,7 @@
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>Picada volvio a entrar como caso 6325</t>
+          <t>Aplomar</t>
         </is>
       </c>
       <c r="I25" t="n">
@@ -2301,7 +2293,7 @@
       </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K25" t="inlineStr">
@@ -2311,40 +2303,40 @@
       </c>
       <c r="L25" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M25" t="n">
-        <v>-58.420549</v>
+        <v>-58.459513</v>
       </c>
       <c r="N25" t="n">
-        <v>-34.585103</v>
+        <v>-34.578019</v>
       </c>
       <c r="O25" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P25" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>5715</t>
+          <t>5656</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>5/1/2025</t>
+          <t>4/24/2025</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>CUENCA 4690</t>
+          <t>ECHEVERRIA 5893</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
@@ -2354,7 +2346,7 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>805579094</t>
+          <t>804922184</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
@@ -2369,7 +2361,7 @@
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>Aplomar poste</t>
+          <t>Poste con base quebrada</t>
         </is>
       </c>
       <c r="I26" t="n">
@@ -2377,7 +2369,7 @@
       </c>
       <c r="J26" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Desmonte</t>
         </is>
       </c>
       <c r="K26" t="inlineStr">
@@ -2391,10 +2383,10 @@
         </is>
       </c>
       <c r="M26" t="n">
-        <v>-58.506061</v>
+        <v>-58.489627</v>
       </c>
       <c r="N26" t="n">
-        <v>-34.588887</v>
+        <v>-34.583761</v>
       </c>
       <c r="O26" t="inlineStr">
         <is>
@@ -2410,27 +2402,27 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>5719</t>
+          <t>6173</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>5/1/2025</t>
+          <t>4/29/2025</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>CABEZON, JOSE LEON 2440</t>
+          <t>ARMENIA 2321</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>805579157</t>
+          <t>805507398</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
@@ -2445,7 +2437,7 @@
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Picada volvio a entrar como caso 6325</t>
         </is>
       </c>
       <c r="I27" t="n">
@@ -2467,26 +2459,26 @@
         </is>
       </c>
       <c r="M27" t="n">
-        <v>-58.499967</v>
+        <v>-58.420549</v>
       </c>
       <c r="N27" t="n">
-        <v>-34.57974</v>
+        <v>-34.585103</v>
       </c>
       <c r="O27" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P27" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>6333</t>
+          <t>5715</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -2496,17 +2488,17 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>ORTEGA Y GASSET 1816</t>
+          <t>CUENCA 4690</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>805655342</t>
+          <t>805579094</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
@@ -2521,7 +2513,7 @@
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Aplomar poste</t>
         </is>
       </c>
       <c r="I28" t="n">
@@ -2529,7 +2521,7 @@
       </c>
       <c r="J28" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K28" t="inlineStr">
@@ -2539,50 +2531,50 @@
       </c>
       <c r="L28" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M28" t="n">
-        <v>-58.432556</v>
+        <v>-58.506061</v>
       </c>
       <c r="N28" t="n">
-        <v>-34.570279</v>
+        <v>-34.588887</v>
       </c>
       <c r="O28" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P28" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>805707165</t>
+          <t>5719</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>5/7/2025</t>
+          <t>5/1/2025</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Baez 793</t>
+          <t>CABEZON, JOSE LEON 2440</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>805707165</t>
+          <t>805579157</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
@@ -2597,7 +2589,7 @@
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>DESMONTAR COLUMNA DE 7 MTS Y TRANSFERIR A COMUNITARIA</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I29" t="n">
@@ -2615,50 +2607,50 @@
       </c>
       <c r="L29" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M29" t="n">
-        <v>-58.436165</v>
+        <v>-58.499967</v>
       </c>
       <c r="N29" t="n">
-        <v>-34.569081</v>
+        <v>-34.57974</v>
       </c>
       <c r="O29" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P29" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>5847</t>
+          <t>6333</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>5/8/2025</t>
+          <t>5/1/2025</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>JURAMENTO 5321</t>
+          <t>ORTEGA Y GASSET 1816</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>805791839</t>
+          <t>805655342</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
@@ -2695,36 +2687,36 @@
         </is>
       </c>
       <c r="M30" t="n">
-        <v>-58.485193</v>
+        <v>-58.432556</v>
       </c>
       <c r="N30" t="n">
-        <v>-34.579621</v>
+        <v>-34.570279</v>
       </c>
       <c r="O30" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P30" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>232</t>
+          <t>805707165</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>5/9/2025</t>
+          <t>5/7/2025</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Gorostiaga 2286</t>
+          <t>Baez 793</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
@@ -2734,7 +2726,7 @@
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>805791858</t>
+          <t>805707165</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
@@ -2749,7 +2741,7 @@
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>DESMONTAR COLUMNA DE 7 MTS Y TRANSFERIR A COMUNITARIA</t>
         </is>
       </c>
       <c r="I31" t="n">
@@ -2767,14 +2759,14 @@
       </c>
       <c r="L31" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M31" t="n">
-        <v>-58.441563</v>
+        <v>-58.436165</v>
       </c>
       <c r="N31" t="n">
-        <v>-34.569743</v>
+        <v>-34.569081</v>
       </c>
       <c r="O31" t="inlineStr">
         <is>
@@ -2790,7 +2782,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>-406</t>
+          <t>5847</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
@@ -2800,7 +2792,7 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Olof palme 4144</t>
+          <t>JURAMENTO 5321</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
@@ -2810,7 +2802,7 @@
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>805791925</t>
+          <t>805791839</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
@@ -2825,7 +2817,7 @@
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>Tensar 2 riendas a pique columna 168</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I32" t="n">
@@ -2833,7 +2825,7 @@
       </c>
       <c r="J32" t="inlineStr">
         <is>
-          <t>Tensor</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K32" t="inlineStr">
@@ -2843,18 +2835,18 @@
       </c>
       <c r="L32" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M32" t="n">
-        <v>-58.488252</v>
+        <v>-58.485193</v>
       </c>
       <c r="N32" t="n">
-        <v>-34.553391</v>
+        <v>-34.579621</v>
       </c>
       <c r="O32" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P32" t="inlineStr">
@@ -2866,27 +2858,27 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>5826</t>
+          <t>232</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>5/19/2025</t>
+          <t>5/9/2025</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>ALBARELLOS AV. 3180</t>
+          <t>Gorostiaga 2286</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>806926466</t>
+          <t>805791858</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
@@ -2901,7 +2893,7 @@
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>Columna (metal) inclinada</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I33" t="n">
@@ -2909,7 +2901,7 @@
       </c>
       <c r="J33" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K33" t="inlineStr">
@@ -2919,40 +2911,40 @@
       </c>
       <c r="L33" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M33" t="n">
-        <v>-58.513552</v>
+        <v>-58.441563</v>
       </c>
       <c r="N33" t="n">
-        <v>-34.579829</v>
+        <v>-34.569743</v>
       </c>
       <c r="O33" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P33" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>5825</t>
+          <t>-406</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>5/19/2025</t>
+          <t>5/8/2025</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>PAZ, GRAL. AV. 5602</t>
+          <t>Olof palme 4144</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
@@ -2962,7 +2954,7 @@
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>806926472</t>
+          <t>805791925</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
@@ -2977,7 +2969,7 @@
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>reparar rienda cortada - ver foto no es la misma que albarellos</t>
+          <t>Tensar 2 riendas a pique columna 168</t>
         </is>
       </c>
       <c r="I34" t="n">
@@ -2999,14 +2991,14 @@
         </is>
       </c>
       <c r="M34" t="n">
-        <v>-58.513685</v>
+        <v>-58.488252</v>
       </c>
       <c r="N34" t="n">
-        <v>-34.579838</v>
+        <v>-34.553391</v>
       </c>
       <c r="O34" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P34" t="inlineStr">
@@ -3018,27 +3010,27 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>6020</t>
+          <t>5826</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>6/5/2025</t>
+          <t>5/19/2025</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>RAVIGNANI, EMILIO, DR. 2036</t>
+          <t>ALBARELLOS AV. 3180</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>807215465</t>
+          <t>806926466</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
@@ -3053,7 +3045,7 @@
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Columna (metal) inclinada</t>
         </is>
       </c>
       <c r="I35" t="n">
@@ -3061,7 +3053,7 @@
       </c>
       <c r="J35" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K35" t="inlineStr">
@@ -3071,50 +3063,50 @@
       </c>
       <c r="L35" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M35" t="n">
-        <v>-58.436298</v>
+        <v>-58.513552</v>
       </c>
       <c r="N35" t="n">
-        <v>-34.578972</v>
+        <v>-34.579829</v>
       </c>
       <c r="O35" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P35" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>6144</t>
+          <t>5825</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>6/11/2025</t>
+          <t>5/19/2025</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>TURIN 2990</t>
+          <t>PAZ, GRAL. AV. 5602</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>807458282</t>
+          <t>806926472</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
@@ -3129,7 +3121,7 @@
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>reparar rienda cortada - ver foto no es la misma que albarellos</t>
         </is>
       </c>
       <c r="I36" t="n">
@@ -3137,7 +3129,7 @@
       </c>
       <c r="J36" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Tensor</t>
         </is>
       </c>
       <c r="K36" t="inlineStr">
@@ -3147,14 +3139,14 @@
       </c>
       <c r="L36" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M36" t="n">
-        <v>-58.480925</v>
+        <v>-58.513685</v>
       </c>
       <c r="N36" t="n">
-        <v>-34.585471</v>
+        <v>-34.579838</v>
       </c>
       <c r="O36" t="inlineStr">
         <is>
@@ -3170,27 +3162,27 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>6143</t>
+          <t>6020</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>6/11/2025</t>
+          <t>6/5/2025</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>SOLANO LOPEZ, F., MARISCAL 2845</t>
+          <t>RAVIGNANI, EMILIO, DR. 2036</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>807458296</t>
+          <t>807215465</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
@@ -3227,26 +3219,26 @@
         </is>
       </c>
       <c r="M37" t="n">
-        <v>-58.495071</v>
+        <v>-58.436298</v>
       </c>
       <c r="N37" t="n">
-        <v>-34.593122</v>
+        <v>-34.578972</v>
       </c>
       <c r="O37" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P37" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>6141</t>
+          <t>6144</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
@@ -3256,17 +3248,17 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>EL PAMPERO 2618</t>
+          <t>TURIN 2990</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>807458310</t>
+          <t>807458282</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
@@ -3303,10 +3295,10 @@
         </is>
       </c>
       <c r="M38" t="n">
-        <v>-58.481942</v>
+        <v>-58.480925</v>
       </c>
       <c r="N38" t="n">
-        <v>-34.602989</v>
+        <v>-34.585471</v>
       </c>
       <c r="O38" t="inlineStr">
         <is>
@@ -3322,27 +3314,27 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>-478</t>
+          <t>6143</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>6/15/2025</t>
+          <t>6/11/2025</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Chivilcoy 4875</t>
+          <t>SOLANO LOPEZ, F., MARISCAL 2845</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>807508509</t>
+          <t>807458296</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
@@ -3357,7 +3349,7 @@
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>Poste podrido</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I39" t="n">
@@ -3375,14 +3367,14 @@
       </c>
       <c r="L39" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M39" t="n">
-        <v>-58.517389</v>
+        <v>-58.495071</v>
       </c>
       <c r="N39" t="n">
-        <v>-34.593541</v>
+        <v>-34.593122</v>
       </c>
       <c r="O39" t="inlineStr">
         <is>
@@ -3398,27 +3390,27 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>6171</t>
+          <t>6141</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>6/18/2025</t>
+          <t>6/11/2025</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>CABELLO 3486</t>
+          <t>EL PAMPERO 2618</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>807658640</t>
+          <t>807458310</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
@@ -3433,7 +3425,7 @@
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t>Columna inclinada evaluar con inspector un corrimiento</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I40" t="n">
@@ -3455,46 +3447,46 @@
         </is>
       </c>
       <c r="M40" t="n">
-        <v>-58.409579</v>
+        <v>-58.481942</v>
       </c>
       <c r="N40" t="n">
-        <v>-34.581134</v>
+        <v>-34.602989</v>
       </c>
       <c r="O40" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P40" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>6230</t>
+          <t>-478</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>6/24/2025</t>
+          <t>6/15/2025</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Santa maria de oro	2722</t>
+          <t>Chivilcoy 4875</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>807763066</t>
+          <t>807508509</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
@@ -3509,7 +3501,7 @@
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Poste podrido</t>
         </is>
       </c>
       <c r="I41" t="n">
@@ -3527,40 +3519,40 @@
       </c>
       <c r="L41" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M41" t="n">
-        <v>-58.422315</v>
+        <v>-58.517389</v>
       </c>
       <c r="N41" t="n">
-        <v>-34.576988</v>
+        <v>-34.593541</v>
       </c>
       <c r="O41" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P41" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>6231</t>
+          <t>6171</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>6/24/2025</t>
+          <t>6/18/2025</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Ciudad de la Paz 275</t>
+          <t>CABELLO 3486</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
@@ -3570,7 +3562,7 @@
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>807763070</t>
+          <t>807658640</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
@@ -3585,7 +3577,7 @@
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>Aplomar o cambiar</t>
+          <t>Columna inclinada evaluar con inspector un corrimiento</t>
         </is>
       </c>
       <c r="I42" t="n">
@@ -3603,14 +3595,14 @@
       </c>
       <c r="L42" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M42" t="n">
-        <v>-58.441049</v>
+        <v>-58.409579</v>
       </c>
       <c r="N42" t="n">
-        <v>-34.574625</v>
+        <v>-34.581134</v>
       </c>
       <c r="O42" t="inlineStr">
         <is>
@@ -3626,7 +3618,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>6235</t>
+          <t>6230</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
@@ -3636,17 +3628,17 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>HUERGO 389</t>
+          <t>Santa maria de oro	2722</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>807763078</t>
+          <t>807763066</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
@@ -3683,10 +3675,10 @@
         </is>
       </c>
       <c r="M43" t="n">
-        <v>-58.432722</v>
+        <v>-58.422315</v>
       </c>
       <c r="N43" t="n">
-        <v>-34.572371</v>
+        <v>-34.576988</v>
       </c>
       <c r="O43" t="inlineStr">
         <is>
@@ -3702,17 +3694,17 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>6295</t>
+          <t>6231</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>6/30/2025</t>
+          <t>6/24/2025</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>SOLER 6017</t>
+          <t>Ciudad de la Paz 275</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
@@ -3722,7 +3714,7 @@
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>807851636</t>
+          <t>807763070</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
@@ -3737,7 +3729,7 @@
       </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Aplomar o cambiar</t>
         </is>
       </c>
       <c r="I44" t="n">
@@ -3755,14 +3747,14 @@
       </c>
       <c r="L44" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M44" t="n">
-        <v>-58.436808</v>
+        <v>-58.441049</v>
       </c>
       <c r="N44" t="n">
-        <v>-34.577464</v>
+        <v>-34.574625</v>
       </c>
       <c r="O44" t="inlineStr">
         <is>
@@ -3778,27 +3770,27 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>6332</t>
+          <t>6235</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>7/3/2025</t>
+          <t>6/24/2025</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>ARAOZ 2560</t>
+          <t>HUERGO 389</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>807965818</t>
+          <t>807763078</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
@@ -3835,10 +3827,10 @@
         </is>
       </c>
       <c r="M45" t="n">
-        <v>-58.414507</v>
+        <v>-58.432722</v>
       </c>
       <c r="N45" t="n">
-        <v>-34.585377</v>
+        <v>-34.572371</v>
       </c>
       <c r="O45" t="inlineStr">
         <is>
@@ -3854,27 +3846,27 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>-503</t>
+          <t>6295</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>7/10/2025</t>
+          <t>6/30/2025</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Salguero 842</t>
+          <t>SOLER 6017</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>808148673</t>
+          <t>807851636</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
@@ -3889,7 +3881,7 @@
       </c>
       <c r="H46" t="inlineStr">
         <is>
-          <t>Cambiar columna picada en la base</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I46" t="n">
@@ -3911,14 +3903,14 @@
         </is>
       </c>
       <c r="M46" t="n">
-        <v>-58.419166</v>
+        <v>-58.436808</v>
       </c>
       <c r="N46" t="n">
-        <v>-34.600265</v>
+        <v>-34.577464</v>
       </c>
       <c r="O46" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P46" t="inlineStr">
@@ -3930,27 +3922,27 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>6506</t>
+          <t>6332</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>7/10/2025</t>
+          <t>7/3/2025</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Ohiggins 1611</t>
+          <t>ARAOZ 2560</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>808148679</t>
+          <t>807965818</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
@@ -3965,7 +3957,7 @@
       </c>
       <c r="H47" t="inlineStr">
         <is>
-          <t>Columna podrida en la base</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I47" t="n">
@@ -3978,7 +3970,7 @@
       </c>
       <c r="K47" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L47" t="inlineStr">
@@ -3987,46 +3979,46 @@
         </is>
       </c>
       <c r="M47" t="n">
-        <v>-58.448993</v>
+        <v>-58.414507</v>
       </c>
       <c r="N47" t="n">
-        <v>-34.564383</v>
+        <v>-34.585377</v>
       </c>
       <c r="O47" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P47" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>6437</t>
+          <t>-503</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>7/17/2025</t>
+          <t>7/10/2025</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>MILLER 4590</t>
+          <t>Salguero 842</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>808400306</t>
+          <t>808148673</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
@@ -4041,7 +4033,7 @@
       </c>
       <c r="H48" t="inlineStr">
         <is>
-          <t>Columna corroida</t>
+          <t>Cambiar columna picada en la base</t>
         </is>
       </c>
       <c r="I48" t="n">
@@ -4063,46 +4055,46 @@
         </is>
       </c>
       <c r="M48" t="n">
-        <v>-58.495482</v>
+        <v>-58.419166</v>
       </c>
       <c r="N48" t="n">
-        <v>-34.552614</v>
+        <v>-34.600265</v>
       </c>
       <c r="O48" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P48" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>6538</t>
+          <t>6506</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>7/17/2025</t>
+          <t>7/10/2025</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Pedraza Manuela 4101</t>
+          <t>Ohiggins 1611</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>808400353</t>
+          <t>808148679</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
@@ -4117,7 +4109,7 @@
       </c>
       <c r="H49" t="inlineStr">
         <is>
-          <t xml:space="preserve">Podrida en la base </t>
+          <t>Columna podrida en la base</t>
         </is>
       </c>
       <c r="I49" t="n">
@@ -4130,7 +4122,7 @@
       </c>
       <c r="K49" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L49" t="inlineStr">
@@ -4139,14 +4131,14 @@
         </is>
       </c>
       <c r="M49" t="n">
-        <v>-58.481569</v>
+        <v>-58.448993</v>
       </c>
       <c r="N49" t="n">
-        <v>-34.559853</v>
+        <v>-34.564383</v>
       </c>
       <c r="O49" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P49" t="inlineStr">
@@ -4158,27 +4150,27 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>-525</t>
+          <t>6437</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>7/22/2025</t>
+          <t>7/17/2025</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Zabala 3567</t>
+          <t>MILLER 4590</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>808480549</t>
+          <t>808400306</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
@@ -4193,7 +4185,7 @@
       </c>
       <c r="H50" t="inlineStr">
         <is>
-          <t>Corroida en base para recambio</t>
+          <t>Columna corroida</t>
         </is>
       </c>
       <c r="I50" t="n">
@@ -4215,14 +4207,14 @@
         </is>
       </c>
       <c r="M50" t="n">
-        <v>-58.457492</v>
+        <v>-58.495482</v>
       </c>
       <c r="N50" t="n">
-        <v>-34.579336</v>
+        <v>-34.552614</v>
       </c>
       <c r="O50" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P50" t="inlineStr">
@@ -4234,27 +4226,27 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>6484</t>
+          <t>6538</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>7/24/2025</t>
+          <t>7/17/2025</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>URIARTE 2396</t>
+          <t>Pedraza Manuela 4101</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>808509373</t>
+          <t>808400353</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
@@ -4269,7 +4261,7 @@
       </c>
       <c r="H51" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t xml:space="preserve">Podrida en la base </t>
         </is>
       </c>
       <c r="I51" t="n">
@@ -4291,46 +4283,46 @@
         </is>
       </c>
       <c r="M51" t="n">
-        <v>-58.423934</v>
+        <v>-58.481569</v>
       </c>
       <c r="N51" t="n">
-        <v>-34.581562</v>
+        <v>-34.559853</v>
       </c>
       <c r="O51" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P51" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>6512</t>
+          <t>-525</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>7/28/2025</t>
+          <t>7/22/2025</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>GASCON 1195</t>
+          <t>Zabala 3567</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>808571975</t>
+          <t>808480549</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
@@ -4345,7 +4337,7 @@
       </c>
       <c r="H52" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Corroida en base para recambio</t>
         </is>
       </c>
       <c r="I52" t="n">
@@ -4367,36 +4359,36 @@
         </is>
       </c>
       <c r="M52" t="n">
-        <v>-58.423127</v>
+        <v>-58.457492</v>
       </c>
       <c r="N52" t="n">
-        <v>-34.596476</v>
+        <v>-34.579336</v>
       </c>
       <c r="O52" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P52" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>6513</t>
+          <t>6484</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>7/28/2025</t>
+          <t>7/24/2025</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>DORREGO 1925</t>
+          <t>URIARTE 2396</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
@@ -4406,7 +4398,7 @@
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>808571976</t>
+          <t>808509373</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
@@ -4443,10 +4435,10 @@
         </is>
       </c>
       <c r="M53" t="n">
-        <v>-58.441281</v>
+        <v>-58.423934</v>
       </c>
       <c r="N53" t="n">
-        <v>-34.579867</v>
+        <v>-34.581562</v>
       </c>
       <c r="O53" t="inlineStr">
         <is>
@@ -4462,7 +4454,7 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>6519</t>
+          <t>6512</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
@@ -4472,7 +4464,7 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>SALGUERO, JERONIMO 2874</t>
+          <t>GASCON 1195</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
@@ -4482,7 +4474,7 @@
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>808571977</t>
+          <t>808571975</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
@@ -4497,7 +4489,7 @@
       </c>
       <c r="H54" t="inlineStr">
         <is>
-          <t>Reparar rienda</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I54" t="n">
@@ -4505,7 +4497,7 @@
       </c>
       <c r="J54" t="inlineStr">
         <is>
-          <t>Tensor</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K54" t="inlineStr">
@@ -4515,14 +4507,14 @@
       </c>
       <c r="L54" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M54" t="n">
-        <v>-58.407256</v>
+        <v>-58.423127</v>
       </c>
       <c r="N54" t="n">
-        <v>-34.578976</v>
+        <v>-34.596476</v>
       </c>
       <c r="O54" t="inlineStr">
         <is>
@@ -4538,27 +4530,27 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>-538</t>
+          <t>6513</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>7/31/2025</t>
+          <t>7/28/2025</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>Malabia 964</t>
+          <t>DORREGO 1925</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>808609237</t>
+          <t>808571976</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
@@ -4573,7 +4565,7 @@
       </c>
       <c r="H55" t="inlineStr">
         <is>
-          <t>Cambiar poste mal estado por PRFV</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I55" t="n">
@@ -4591,14 +4583,14 @@
       </c>
       <c r="L55" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M55" t="n">
-        <v>-58.433634</v>
+        <v>-58.441281</v>
       </c>
       <c r="N55" t="n">
-        <v>-34.595018</v>
+        <v>-34.579867</v>
       </c>
       <c r="O55" t="inlineStr">
         <is>
@@ -4614,27 +4606,27 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>6545</t>
+          <t>6519</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>8/4/2025</t>
+          <t>7/28/2025</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>SCALABRINI ORTIZ, RAUL AV. 708</t>
+          <t>SALGUERO, JERONIMO 2874</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>808703864</t>
+          <t>808571977</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
@@ -4649,7 +4641,7 @@
       </c>
       <c r="H56" t="inlineStr">
         <is>
-          <t>Aplomar</t>
+          <t>Reparar rienda</t>
         </is>
       </c>
       <c r="I56" t="n">
@@ -4657,7 +4649,7 @@
       </c>
       <c r="J56" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Tensor</t>
         </is>
       </c>
       <c r="K56" t="inlineStr">
@@ -4667,14 +4659,14 @@
       </c>
       <c r="L56" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M56" t="n">
-        <v>-58.434339</v>
+        <v>-58.407256</v>
       </c>
       <c r="N56" t="n">
-        <v>-34.59693</v>
+        <v>-34.578976</v>
       </c>
       <c r="O56" t="inlineStr">
         <is>
@@ -4690,27 +4682,27 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>6498</t>
+          <t>-538</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>8/6/2025</t>
+          <t>7/31/2025</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>BUCARELLI 2087</t>
+          <t>Malabia 964</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>808733908</t>
+          <t>808609237</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
@@ -4725,7 +4717,7 @@
       </c>
       <c r="H57" t="inlineStr">
         <is>
-          <t>Base picada</t>
+          <t>Cambiar poste mal estado por PRFV</t>
         </is>
       </c>
       <c r="I57" t="n">
@@ -4743,50 +4735,50 @@
       </c>
       <c r="L57" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M57" t="n">
-        <v>-58.485592</v>
+        <v>-58.433634</v>
       </c>
       <c r="N57" t="n">
-        <v>-34.578586</v>
+        <v>-34.595018</v>
       </c>
       <c r="O57" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P57" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>-547</t>
+          <t>6545</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>8/6/2025</t>
+          <t>8/4/2025</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>Habana 4210</t>
+          <t>SCALABRINI ORTIZ, RAUL AV. 708</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>808733921</t>
+          <t>808703864</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
@@ -4801,7 +4793,7 @@
       </c>
       <c r="H58" t="inlineStr">
         <is>
-          <t>Cambiar poste dañado</t>
+          <t>Aplomar</t>
         </is>
       </c>
       <c r="I58" t="n">
@@ -4809,7 +4801,7 @@
       </c>
       <c r="J58" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K58" t="inlineStr">
@@ -4819,50 +4811,50 @@
       </c>
       <c r="L58" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M58" t="n">
-        <v>-58.515873</v>
+        <v>-58.434339</v>
       </c>
       <c r="N58" t="n">
-        <v>-34.599425</v>
+        <v>-34.59693</v>
       </c>
       <c r="O58" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P58" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>6579</t>
+          <t>6498</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>8/7/2025</t>
+          <t>8/6/2025</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>RIVADAVIA MARTIN, COMODORO 1350</t>
+          <t>BUCARELLI 2087</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>808749184</t>
+          <t>808733908</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
@@ -4877,7 +4869,7 @@
       </c>
       <c r="H59" t="inlineStr">
         <is>
-          <t>Poste inclinado</t>
+          <t>Base picada</t>
         </is>
       </c>
       <c r="I59" t="n">
@@ -4885,31 +4877,183 @@
       </c>
       <c r="J59" t="inlineStr">
         <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K59" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L59" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M59" t="n">
+        <v>-58.485592</v>
+      </c>
+      <c r="N59" t="n">
+        <v>-34.578586</v>
+      </c>
+      <c r="O59" t="inlineStr">
+        <is>
+          <t>Paternal</t>
+        </is>
+      </c>
+      <c r="P59" t="inlineStr">
+        <is>
+          <t>Capital Norte</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>-547</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>8/6/2025</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>Habana 4210</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>808733921</t>
+        </is>
+      </c>
+      <c r="F60" t="inlineStr">
+        <is>
+          <t>NEW</t>
+        </is>
+      </c>
+      <c r="G60" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H60" t="inlineStr">
+        <is>
+          <t>Cambiar poste dañado</t>
+        </is>
+      </c>
+      <c r="I60" t="n">
+        <v>1</v>
+      </c>
+      <c r="J60" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K60" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L60" t="inlineStr">
+        <is>
+          <t>Poste</t>
+        </is>
+      </c>
+      <c r="M60" t="n">
+        <v>-58.515873</v>
+      </c>
+      <c r="N60" t="n">
+        <v>-34.599425</v>
+      </c>
+      <c r="O60" t="inlineStr">
+        <is>
+          <t>Paternal</t>
+        </is>
+      </c>
+      <c r="P60" t="inlineStr">
+        <is>
+          <t>Capital Norte</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>6579</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>8/7/2025</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>RIVADAVIA MARTIN, COMODORO 1350</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>13</t>
+        </is>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>808749184</t>
+        </is>
+      </c>
+      <c r="F61" t="inlineStr">
+        <is>
+          <t>NEW</t>
+        </is>
+      </c>
+      <c r="G61" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H61" t="inlineStr">
+        <is>
+          <t>Poste inclinado</t>
+        </is>
+      </c>
+      <c r="I61" t="n">
+        <v>1</v>
+      </c>
+      <c r="J61" t="inlineStr">
+        <is>
           <t>Aplomo</t>
         </is>
       </c>
-      <c r="K59" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L59" t="inlineStr">
+      <c r="K61" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L61" t="inlineStr">
         <is>
           <t>Poste</t>
         </is>
       </c>
-      <c r="M59" t="n">
+      <c r="M61" t="n">
         <v>-58.461024</v>
       </c>
-      <c r="N59" t="n">
+      <c r="N61" t="n">
         <v>-34.539409</v>
       </c>
-      <c r="O59" t="inlineStr">
+      <c r="O61" t="inlineStr">
         <is>
           <t>Saavedra</t>
         </is>
       </c>
-      <c r="P59" t="inlineStr">
+      <c r="P61" t="inlineStr">
         <is>
           <t>Capital Norte</t>
         </is>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-08-11 07:12:43)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_NEW.xlsx
+++ b/mapa_interactivo_NEW.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P61"/>
+  <dimension ref="A1:P60"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3086,27 +3086,27 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>5825</t>
+          <t>6020</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>5/19/2025</t>
+          <t>6/5/2025</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>PAZ, GRAL. AV. 5602</t>
+          <t>RAVIGNANI, EMILIO, DR. 2036</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>806926472</t>
+          <t>807215465</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
@@ -3121,7 +3121,7 @@
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>reparar rienda cortada - ver foto no es la misma que albarellos</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I36" t="n">
@@ -3129,7 +3129,7 @@
       </c>
       <c r="J36" t="inlineStr">
         <is>
-          <t>Tensor</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K36" t="inlineStr">
@@ -3139,50 +3139,50 @@
       </c>
       <c r="L36" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M36" t="n">
-        <v>-58.513685</v>
+        <v>-58.436298</v>
       </c>
       <c r="N36" t="n">
-        <v>-34.579838</v>
+        <v>-34.578972</v>
       </c>
       <c r="O36" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P36" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>6020</t>
+          <t>6144</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>6/5/2025</t>
+          <t>6/11/2025</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>RAVIGNANI, EMILIO, DR. 2036</t>
+          <t>TURIN 2990</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>807215465</t>
+          <t>807458282</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
@@ -3219,26 +3219,26 @@
         </is>
       </c>
       <c r="M37" t="n">
-        <v>-58.436298</v>
+        <v>-58.480925</v>
       </c>
       <c r="N37" t="n">
-        <v>-34.578972</v>
+        <v>-34.585471</v>
       </c>
       <c r="O37" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P37" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>6144</t>
+          <t>6143</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
@@ -3248,7 +3248,7 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>TURIN 2990</t>
+          <t>SOLANO LOPEZ, F., MARISCAL 2845</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
@@ -3258,7 +3258,7 @@
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>807458282</t>
+          <t>807458296</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
@@ -3295,10 +3295,10 @@
         </is>
       </c>
       <c r="M38" t="n">
-        <v>-58.480925</v>
+        <v>-58.495071</v>
       </c>
       <c r="N38" t="n">
-        <v>-34.585471</v>
+        <v>-34.593122</v>
       </c>
       <c r="O38" t="inlineStr">
         <is>
@@ -3314,7 +3314,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>6143</t>
+          <t>6141</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
@@ -3324,17 +3324,17 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>SOLANO LOPEZ, F., MARISCAL 2845</t>
+          <t>EL PAMPERO 2618</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>807458296</t>
+          <t>807458310</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
@@ -3371,10 +3371,10 @@
         </is>
       </c>
       <c r="M39" t="n">
-        <v>-58.495071</v>
+        <v>-58.481942</v>
       </c>
       <c r="N39" t="n">
-        <v>-34.593122</v>
+        <v>-34.602989</v>
       </c>
       <c r="O39" t="inlineStr">
         <is>
@@ -3390,17 +3390,17 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>6141</t>
+          <t>-478</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>6/11/2025</t>
+          <t>6/15/2025</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>EL PAMPERO 2618</t>
+          <t>Chivilcoy 4875</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
@@ -3410,7 +3410,7 @@
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>807458310</t>
+          <t>807508509</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
@@ -3425,7 +3425,7 @@
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Poste podrido</t>
         </is>
       </c>
       <c r="I40" t="n">
@@ -3443,14 +3443,14 @@
       </c>
       <c r="L40" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M40" t="n">
-        <v>-58.481942</v>
+        <v>-58.517389</v>
       </c>
       <c r="N40" t="n">
-        <v>-34.602989</v>
+        <v>-34.593541</v>
       </c>
       <c r="O40" t="inlineStr">
         <is>
@@ -3466,27 +3466,27 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>-478</t>
+          <t>6171</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>6/15/2025</t>
+          <t>6/18/2025</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Chivilcoy 4875</t>
+          <t>CABELLO 3486</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>807508509</t>
+          <t>807658640</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
@@ -3501,7 +3501,7 @@
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>Poste podrido</t>
+          <t>Columna inclinada evaluar con inspector un corrimiento</t>
         </is>
       </c>
       <c r="I41" t="n">
@@ -3519,40 +3519,40 @@
       </c>
       <c r="L41" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M41" t="n">
-        <v>-58.517389</v>
+        <v>-58.409579</v>
       </c>
       <c r="N41" t="n">
-        <v>-34.593541</v>
+        <v>-34.581134</v>
       </c>
       <c r="O41" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P41" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>6171</t>
+          <t>6230</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>6/18/2025</t>
+          <t>6/24/2025</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>CABELLO 3486</t>
+          <t>Santa maria de oro	2722</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
@@ -3562,7 +3562,7 @@
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>807658640</t>
+          <t>807763066</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
@@ -3577,7 +3577,7 @@
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>Columna inclinada evaluar con inspector un corrimiento</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I42" t="n">
@@ -3599,10 +3599,10 @@
         </is>
       </c>
       <c r="M42" t="n">
-        <v>-58.409579</v>
+        <v>-58.422315</v>
       </c>
       <c r="N42" t="n">
-        <v>-34.581134</v>
+        <v>-34.576988</v>
       </c>
       <c r="O42" t="inlineStr">
         <is>
@@ -3618,7 +3618,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>6230</t>
+          <t>6231</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
@@ -3628,7 +3628,7 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Santa maria de oro	2722</t>
+          <t>Ciudad de la Paz 275</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
@@ -3638,7 +3638,7 @@
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>807763066</t>
+          <t>807763070</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
@@ -3653,7 +3653,7 @@
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Aplomar o cambiar</t>
         </is>
       </c>
       <c r="I43" t="n">
@@ -3671,14 +3671,14 @@
       </c>
       <c r="L43" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M43" t="n">
-        <v>-58.422315</v>
+        <v>-58.441049</v>
       </c>
       <c r="N43" t="n">
-        <v>-34.576988</v>
+        <v>-34.574625</v>
       </c>
       <c r="O43" t="inlineStr">
         <is>
@@ -3694,7 +3694,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>6231</t>
+          <t>6235</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
@@ -3704,17 +3704,17 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Ciudad de la Paz 275</t>
+          <t>HUERGO 389</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>807763070</t>
+          <t>807763078</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
@@ -3729,7 +3729,7 @@
       </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t>Aplomar o cambiar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I44" t="n">
@@ -3747,14 +3747,14 @@
       </c>
       <c r="L44" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M44" t="n">
-        <v>-58.441049</v>
+        <v>-58.432722</v>
       </c>
       <c r="N44" t="n">
-        <v>-34.574625</v>
+        <v>-34.572371</v>
       </c>
       <c r="O44" t="inlineStr">
         <is>
@@ -3770,27 +3770,27 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>6235</t>
+          <t>6295</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>6/24/2025</t>
+          <t>6/30/2025</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>HUERGO 389</t>
+          <t>SOLER 6017</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>807763078</t>
+          <t>807851636</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
@@ -3827,10 +3827,10 @@
         </is>
       </c>
       <c r="M45" t="n">
-        <v>-58.432722</v>
+        <v>-58.436808</v>
       </c>
       <c r="N45" t="n">
-        <v>-34.572371</v>
+        <v>-34.577464</v>
       </c>
       <c r="O45" t="inlineStr">
         <is>
@@ -3846,17 +3846,17 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>6295</t>
+          <t>6332</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>6/30/2025</t>
+          <t>7/3/2025</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>SOLER 6017</t>
+          <t>ARAOZ 2560</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
@@ -3866,7 +3866,7 @@
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>807851636</t>
+          <t>807965818</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
@@ -3903,10 +3903,10 @@
         </is>
       </c>
       <c r="M46" t="n">
-        <v>-58.436808</v>
+        <v>-58.414507</v>
       </c>
       <c r="N46" t="n">
-        <v>-34.577464</v>
+        <v>-34.585377</v>
       </c>
       <c r="O46" t="inlineStr">
         <is>
@@ -3922,27 +3922,27 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>6332</t>
+          <t>-503</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>7/3/2025</t>
+          <t>7/10/2025</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>ARAOZ 2560</t>
+          <t>Salguero 842</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>807965818</t>
+          <t>808148673</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
@@ -3957,7 +3957,7 @@
       </c>
       <c r="H47" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambiar columna picada en la base</t>
         </is>
       </c>
       <c r="I47" t="n">
@@ -3979,14 +3979,14 @@
         </is>
       </c>
       <c r="M47" t="n">
-        <v>-58.414507</v>
+        <v>-58.419166</v>
       </c>
       <c r="N47" t="n">
-        <v>-34.585377</v>
+        <v>-34.600265</v>
       </c>
       <c r="O47" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P47" t="inlineStr">
@@ -3998,7 +3998,7 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>-503</t>
+          <t>6506</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
@@ -4008,17 +4008,17 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Salguero 842</t>
+          <t>Ohiggins 1611</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>808148673</t>
+          <t>808148679</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
@@ -4033,7 +4033,7 @@
       </c>
       <c r="H48" t="inlineStr">
         <is>
-          <t>Cambiar columna picada en la base</t>
+          <t>Columna podrida en la base</t>
         </is>
       </c>
       <c r="I48" t="n">
@@ -4046,7 +4046,7 @@
       </c>
       <c r="K48" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L48" t="inlineStr">
@@ -4055,46 +4055,46 @@
         </is>
       </c>
       <c r="M48" t="n">
-        <v>-58.419166</v>
+        <v>-58.448993</v>
       </c>
       <c r="N48" t="n">
-        <v>-34.600265</v>
+        <v>-34.564383</v>
       </c>
       <c r="O48" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P48" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>6506</t>
+          <t>6437</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>7/10/2025</t>
+          <t>7/17/2025</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Ohiggins 1611</t>
+          <t>MILLER 4590</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>808148679</t>
+          <t>808400306</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
@@ -4109,7 +4109,7 @@
       </c>
       <c r="H49" t="inlineStr">
         <is>
-          <t>Columna podrida en la base</t>
+          <t>Columna corroida</t>
         </is>
       </c>
       <c r="I49" t="n">
@@ -4122,7 +4122,7 @@
       </c>
       <c r="K49" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L49" t="inlineStr">
@@ -4131,14 +4131,14 @@
         </is>
       </c>
       <c r="M49" t="n">
-        <v>-58.448993</v>
+        <v>-58.495482</v>
       </c>
       <c r="N49" t="n">
-        <v>-34.564383</v>
+        <v>-34.552614</v>
       </c>
       <c r="O49" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P49" t="inlineStr">
@@ -4150,7 +4150,7 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>6437</t>
+          <t>6538</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
@@ -4160,7 +4160,7 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>MILLER 4590</t>
+          <t>Pedraza Manuela 4101</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
@@ -4170,7 +4170,7 @@
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>808400306</t>
+          <t>808400353</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
@@ -4185,7 +4185,7 @@
       </c>
       <c r="H50" t="inlineStr">
         <is>
-          <t>Columna corroida</t>
+          <t xml:space="preserve">Podrida en la base </t>
         </is>
       </c>
       <c r="I50" t="n">
@@ -4207,10 +4207,10 @@
         </is>
       </c>
       <c r="M50" t="n">
-        <v>-58.495482</v>
+        <v>-58.481569</v>
       </c>
       <c r="N50" t="n">
-        <v>-34.552614</v>
+        <v>-34.559853</v>
       </c>
       <c r="O50" t="inlineStr">
         <is>
@@ -4226,27 +4226,27 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>6538</t>
+          <t>-525</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>7/17/2025</t>
+          <t>7/22/2025</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Pedraza Manuela 4101</t>
+          <t>Zabala 3567</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>808400353</t>
+          <t>808480549</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
@@ -4261,7 +4261,7 @@
       </c>
       <c r="H51" t="inlineStr">
         <is>
-          <t xml:space="preserve">Podrida en la base </t>
+          <t>Corroida en base para recambio</t>
         </is>
       </c>
       <c r="I51" t="n">
@@ -4283,14 +4283,14 @@
         </is>
       </c>
       <c r="M51" t="n">
-        <v>-58.481569</v>
+        <v>-58.457492</v>
       </c>
       <c r="N51" t="n">
-        <v>-34.559853</v>
+        <v>-34.579336</v>
       </c>
       <c r="O51" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P51" t="inlineStr">
@@ -4302,27 +4302,27 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>-525</t>
+          <t>6484</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>7/22/2025</t>
+          <t>7/24/2025</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>Zabala 3567</t>
+          <t>URIARTE 2396</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>808480549</t>
+          <t>808509373</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
@@ -4337,7 +4337,7 @@
       </c>
       <c r="H52" t="inlineStr">
         <is>
-          <t>Corroida en base para recambio</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I52" t="n">
@@ -4359,36 +4359,36 @@
         </is>
       </c>
       <c r="M52" t="n">
-        <v>-58.457492</v>
+        <v>-58.423934</v>
       </c>
       <c r="N52" t="n">
-        <v>-34.579336</v>
+        <v>-34.581562</v>
       </c>
       <c r="O52" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P52" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>6484</t>
+          <t>6512</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>7/24/2025</t>
+          <t>7/28/2025</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>URIARTE 2396</t>
+          <t>GASCON 1195</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
@@ -4398,7 +4398,7 @@
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>808509373</t>
+          <t>808571975</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
@@ -4435,10 +4435,10 @@
         </is>
       </c>
       <c r="M53" t="n">
-        <v>-58.423934</v>
+        <v>-58.423127</v>
       </c>
       <c r="N53" t="n">
-        <v>-34.581562</v>
+        <v>-34.596476</v>
       </c>
       <c r="O53" t="inlineStr">
         <is>
@@ -4454,7 +4454,7 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>6512</t>
+          <t>6513</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
@@ -4464,7 +4464,7 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>GASCON 1195</t>
+          <t>DORREGO 1925</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
@@ -4474,7 +4474,7 @@
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>808571975</t>
+          <t>808571976</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
@@ -4511,10 +4511,10 @@
         </is>
       </c>
       <c r="M54" t="n">
-        <v>-58.423127</v>
+        <v>-58.441281</v>
       </c>
       <c r="N54" t="n">
-        <v>-34.596476</v>
+        <v>-34.579867</v>
       </c>
       <c r="O54" t="inlineStr">
         <is>
@@ -4530,7 +4530,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>6513</t>
+          <t>6519</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
@@ -4540,7 +4540,7 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>DORREGO 1925</t>
+          <t>SALGUERO, JERONIMO 2874</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
@@ -4550,7 +4550,7 @@
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>808571976</t>
+          <t>808571977</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
@@ -4565,7 +4565,7 @@
       </c>
       <c r="H55" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Reparar rienda</t>
         </is>
       </c>
       <c r="I55" t="n">
@@ -4573,7 +4573,7 @@
       </c>
       <c r="J55" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Tensor</t>
         </is>
       </c>
       <c r="K55" t="inlineStr">
@@ -4583,14 +4583,14 @@
       </c>
       <c r="L55" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M55" t="n">
-        <v>-58.441281</v>
+        <v>-58.407256</v>
       </c>
       <c r="N55" t="n">
-        <v>-34.579867</v>
+        <v>-34.578976</v>
       </c>
       <c r="O55" t="inlineStr">
         <is>
@@ -4606,27 +4606,27 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>6519</t>
+          <t>-538</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>7/28/2025</t>
+          <t>7/31/2025</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>SALGUERO, JERONIMO 2874</t>
+          <t>Malabia 964</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>808571977</t>
+          <t>808609237</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
@@ -4641,7 +4641,7 @@
       </c>
       <c r="H56" t="inlineStr">
         <is>
-          <t>Reparar rienda</t>
+          <t>Cambiar poste mal estado por PRFV</t>
         </is>
       </c>
       <c r="I56" t="n">
@@ -4649,7 +4649,7 @@
       </c>
       <c r="J56" t="inlineStr">
         <is>
-          <t>Tensor</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K56" t="inlineStr">
@@ -4659,14 +4659,14 @@
       </c>
       <c r="L56" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M56" t="n">
-        <v>-58.407256</v>
+        <v>-58.433634</v>
       </c>
       <c r="N56" t="n">
-        <v>-34.578976</v>
+        <v>-34.595018</v>
       </c>
       <c r="O56" t="inlineStr">
         <is>
@@ -4682,17 +4682,17 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>-538</t>
+          <t>6545</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>7/31/2025</t>
+          <t>8/4/2025</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>Malabia 964</t>
+          <t>SCALABRINI ORTIZ, RAUL AV. 708</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
@@ -4702,7 +4702,7 @@
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>808609237</t>
+          <t>808703864</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
@@ -4717,7 +4717,7 @@
       </c>
       <c r="H57" t="inlineStr">
         <is>
-          <t>Cambiar poste mal estado por PRFV</t>
+          <t>Aplomar</t>
         </is>
       </c>
       <c r="I57" t="n">
@@ -4725,7 +4725,7 @@
       </c>
       <c r="J57" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K57" t="inlineStr">
@@ -4735,14 +4735,14 @@
       </c>
       <c r="L57" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M57" t="n">
-        <v>-58.433634</v>
+        <v>-58.434339</v>
       </c>
       <c r="N57" t="n">
-        <v>-34.595018</v>
+        <v>-34.59693</v>
       </c>
       <c r="O57" t="inlineStr">
         <is>
@@ -4758,27 +4758,27 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>6545</t>
+          <t>6498</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>8/4/2025</t>
+          <t>8/6/2025</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>SCALABRINI ORTIZ, RAUL AV. 708</t>
+          <t>BUCARELLI 2087</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>808703864</t>
+          <t>808733908</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
@@ -4793,7 +4793,7 @@
       </c>
       <c r="H58" t="inlineStr">
         <is>
-          <t>Aplomar</t>
+          <t>Base picada</t>
         </is>
       </c>
       <c r="I58" t="n">
@@ -4801,7 +4801,7 @@
       </c>
       <c r="J58" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K58" t="inlineStr">
@@ -4815,26 +4815,26 @@
         </is>
       </c>
       <c r="M58" t="n">
-        <v>-58.434339</v>
+        <v>-58.485592</v>
       </c>
       <c r="N58" t="n">
-        <v>-34.59693</v>
+        <v>-34.578586</v>
       </c>
       <c r="O58" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P58" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>6498</t>
+          <t>-547</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
@@ -4844,17 +4844,17 @@
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>BUCARELLI 2087</t>
+          <t>Habana 4210</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>808733908</t>
+          <t>808733921</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
@@ -4869,7 +4869,7 @@
       </c>
       <c r="H59" t="inlineStr">
         <is>
-          <t>Base picada</t>
+          <t>Cambiar poste dañado</t>
         </is>
       </c>
       <c r="I59" t="n">
@@ -4887,14 +4887,14 @@
       </c>
       <c r="L59" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M59" t="n">
-        <v>-58.485592</v>
+        <v>-58.515873</v>
       </c>
       <c r="N59" t="n">
-        <v>-34.578586</v>
+        <v>-34.599425</v>
       </c>
       <c r="O59" t="inlineStr">
         <is>
@@ -4910,27 +4910,27 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>-547</t>
+          <t>6579</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>8/6/2025</t>
+          <t>8/7/2025</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>Habana 4210</t>
+          <t>RIVADAVIA MARTIN, COMODORO 1350</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>808733921</t>
+          <t>808749184</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
@@ -4945,7 +4945,7 @@
       </c>
       <c r="H60" t="inlineStr">
         <is>
-          <t>Cambiar poste dañado</t>
+          <t>Poste inclinado</t>
         </is>
       </c>
       <c r="I60" t="n">
@@ -4953,7 +4953,7 @@
       </c>
       <c r="J60" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K60" t="inlineStr">
@@ -4967,93 +4967,17 @@
         </is>
       </c>
       <c r="M60" t="n">
-        <v>-58.515873</v>
+        <v>-58.461024</v>
       </c>
       <c r="N60" t="n">
-        <v>-34.599425</v>
+        <v>-34.539409</v>
       </c>
       <c r="O60" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P60" t="inlineStr">
-        <is>
-          <t>Capital Norte</t>
-        </is>
-      </c>
-    </row>
-    <row r="61">
-      <c r="A61" t="inlineStr">
-        <is>
-          <t>6579</t>
-        </is>
-      </c>
-      <c r="B61" t="inlineStr">
-        <is>
-          <t>8/7/2025</t>
-        </is>
-      </c>
-      <c r="C61" t="inlineStr">
-        <is>
-          <t>RIVADAVIA MARTIN, COMODORO 1350</t>
-        </is>
-      </c>
-      <c r="D61" t="inlineStr">
-        <is>
-          <t>13</t>
-        </is>
-      </c>
-      <c r="E61" t="inlineStr">
-        <is>
-          <t>808749184</t>
-        </is>
-      </c>
-      <c r="F61" t="inlineStr">
-        <is>
-          <t>NEW</t>
-        </is>
-      </c>
-      <c r="G61" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H61" t="inlineStr">
-        <is>
-          <t>Poste inclinado</t>
-        </is>
-      </c>
-      <c r="I61" t="n">
-        <v>1</v>
-      </c>
-      <c r="J61" t="inlineStr">
-        <is>
-          <t>Aplomo</t>
-        </is>
-      </c>
-      <c r="K61" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L61" t="inlineStr">
-        <is>
-          <t>Poste</t>
-        </is>
-      </c>
-      <c r="M61" t="n">
-        <v>-58.461024</v>
-      </c>
-      <c r="N61" t="n">
-        <v>-34.539409</v>
-      </c>
-      <c r="O61" t="inlineStr">
-        <is>
-          <t>Saavedra</t>
-        </is>
-      </c>
-      <c r="P61" t="inlineStr">
         <is>
           <t>Capital Norte</t>
         </is>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-08-13 08:41:20)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_NEW.xlsx
+++ b/mapa_interactivo_NEW.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P60"/>
+  <dimension ref="A1:P65"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -518,17 +518,17 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2098</t>
+          <t>5589</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>5/24/2024</t>
+          <t>12/31/2023</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>AZURDUY JUANA 2449</t>
+          <t>ARCOS 1520</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -538,7 +538,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>788826017</t>
+          <t>799540526</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -548,41 +548,33 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>Terminal con rienda</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I2" t="n">
-        <v>1</v>
-      </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>Cambio</t>
-        </is>
-      </c>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="J2" t="inlineStr"/>
+      <c r="K2" t="inlineStr"/>
       <c r="L2" t="inlineStr">
         <is>
           <t>Pasante</t>
         </is>
       </c>
       <c r="M2" t="n">
-        <v>-58.467279</v>
+        <v>-58.449125</v>
       </c>
       <c r="N2" t="n">
-        <v>-34.551117</v>
+        <v>-34.565958</v>
       </c>
       <c r="O2" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P2" t="inlineStr">
@@ -594,27 +586,27 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>3299</t>
+          <t>4862</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>9/10/2024</t>
+          <t>1/23/2025</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>DIAZ COLODRERO 3309</t>
+          <t>ARCOS 2263</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>796186684</t>
+          <t>802857379</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -624,16 +616,16 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>Colocar columna para solicitar traspasos</t>
+          <t>picada</t>
         </is>
       </c>
       <c r="I3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J3" t="inlineStr">
         <is>
@@ -642,7 +634,7 @@
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>Nodo TLC</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L3" t="inlineStr">
@@ -651,14 +643,14 @@
         </is>
       </c>
       <c r="M3" t="n">
-        <v>-58.491722</v>
+        <v>-58.455082</v>
       </c>
       <c r="N3" t="n">
-        <v>-34.565845</v>
+        <v>-34.558883</v>
       </c>
       <c r="O3" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P3" t="inlineStr">
@@ -670,17 +662,17 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>3839</t>
+          <t>2098</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>10/23/2024</t>
+          <t>5/24/2024</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>PICO 1511</t>
+          <t>AZURDUY JUANA 2449</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -690,7 +682,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>798390296</t>
+          <t>788826017</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -705,7 +697,7 @@
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>Poste inclinado</t>
+          <t>Terminal con rienda</t>
         </is>
       </c>
       <c r="I4" t="n">
@@ -713,7 +705,7 @@
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
@@ -723,14 +715,14 @@
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M4" t="n">
-        <v>-58.465596</v>
+        <v>-58.467279</v>
       </c>
       <c r="N4" t="n">
-        <v>-34.53627</v>
+        <v>-34.551117</v>
       </c>
       <c r="O4" t="inlineStr">
         <is>
@@ -746,27 +738,27 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>801645368</t>
+          <t>3299</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>12/13/2024</t>
+          <t>9/10/2024</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>San Blas 1809</t>
+          <t>DIAZ COLODRERO 3309</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>801645368</t>
+          <t>796186684</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -781,11 +773,11 @@
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Colocar columna para solicitar traspasos</t>
         </is>
       </c>
       <c r="I5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J5" t="inlineStr">
         <is>
@@ -794,7 +786,7 @@
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo TLC</t>
         </is>
       </c>
       <c r="L5" t="inlineStr">
@@ -803,10 +795,10 @@
         </is>
       </c>
       <c r="M5" t="n">
-        <v>-58.467767</v>
+        <v>-58.491722</v>
       </c>
       <c r="N5" t="n">
-        <v>-34.604588</v>
+        <v>-34.565845</v>
       </c>
       <c r="O5" t="inlineStr">
         <is>
@@ -822,17 +814,17 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>5589</t>
+          <t>3839</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>12/31/2023</t>
+          <t>10/23/2024</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>ARCOS 1520</t>
+          <t>PICO 1511</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -842,7 +834,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>799540526</t>
+          <t>798390296</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -852,33 +844,41 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
+          <t>Pendiente</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Poste inclinado</t>
         </is>
       </c>
       <c r="I6" t="n">
-        <v>0</v>
-      </c>
-      <c r="J6" t="inlineStr"/>
-      <c r="K6" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>Aplomo</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M6" t="n">
-        <v>-58.449125</v>
+        <v>-58.465596</v>
       </c>
       <c r="N6" t="n">
-        <v>-34.565958</v>
+        <v>-34.53627</v>
       </c>
       <c r="O6" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P6" t="inlineStr">
@@ -890,27 +890,27 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>4595</t>
+          <t>801645368</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>1/15/2025</t>
+          <t>12/13/2024</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>PAROISSIEN 1806</t>
+          <t>San Blas 1809</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>802747617</t>
+          <t>801645368</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -925,15 +925,15 @@
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>Aplomar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I7" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K7" t="inlineStr">
@@ -943,18 +943,18 @@
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M7" t="n">
-        <v>-58.464172</v>
+        <v>-58.467767</v>
       </c>
       <c r="N7" t="n">
-        <v>-34.543845</v>
+        <v>-34.604588</v>
       </c>
       <c r="O7" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P7" t="inlineStr">
@@ -966,27 +966,27 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>4662</t>
+          <t>4595</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>1/21/2025</t>
+          <t>1/15/2025</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>ALTOLAGUIRRE 2397</t>
+          <t>PAROISSIEN 1806</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>802823938</t>
+          <t>802747617</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -1001,7 +1001,7 @@
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>Inclinada</t>
+          <t>Aplomar</t>
         </is>
       </c>
       <c r="I8" t="n">
@@ -1019,18 +1019,18 @@
       </c>
       <c r="L8" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M8" t="n">
-        <v>-58.490766</v>
+        <v>-58.464172</v>
       </c>
       <c r="N8" t="n">
-        <v>-34.576987</v>
+        <v>-34.543845</v>
       </c>
       <c r="O8" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P8" t="inlineStr">
@@ -1042,27 +1042,27 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>4862</t>
+          <t>4662</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>1/23/2025</t>
+          <t>1/21/2025</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>ARCOS 2263</t>
+          <t>ALTOLAGUIRRE 2397</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>802857379</t>
+          <t>802823938</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -1072,25 +1072,25 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
+          <t>Pendiente</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>picada</t>
+          <t>Inclinada</t>
         </is>
       </c>
       <c r="I9" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L9" t="inlineStr">
@@ -1099,14 +1099,14 @@
         </is>
       </c>
       <c r="M9" t="n">
-        <v>-58.455082</v>
+        <v>-58.490766</v>
       </c>
       <c r="N9" t="n">
-        <v>-34.558883</v>
+        <v>-34.576987</v>
       </c>
       <c r="O9" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P9" t="inlineStr">
@@ -3349,7 +3349,7 @@
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Picada info para cierre tambien entro como caso 6911</t>
         </is>
       </c>
       <c r="I39" t="n">
@@ -4978,6 +4978,386 @@
         </is>
       </c>
       <c r="P60" t="inlineStr">
+        <is>
+          <t>Capital Norte</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>6906</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>8/12/2025</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>MOSCONI GENERAL AV. 3163</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>808918685</t>
+        </is>
+      </c>
+      <c r="F61" t="inlineStr">
+        <is>
+          <t>NEW</t>
+        </is>
+      </c>
+      <c r="G61" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H61" t="inlineStr">
+        <is>
+          <t>Picada</t>
+        </is>
+      </c>
+      <c r="I61" t="n">
+        <v>1</v>
+      </c>
+      <c r="J61" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K61" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L61" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M61" t="n">
+        <v>-58.505731</v>
+      </c>
+      <c r="N61" t="n">
+        <v>-34.588316</v>
+      </c>
+      <c r="O61" t="inlineStr">
+        <is>
+          <t>Paternal</t>
+        </is>
+      </c>
+      <c r="P61" t="inlineStr">
+        <is>
+          <t>Capital Norte</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>6910</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>8/12/2025</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>RIVAS, GRAL. 2345</t>
+        </is>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
+      <c r="E62" t="inlineStr">
+        <is>
+          <t>808918698</t>
+        </is>
+      </c>
+      <c r="F62" t="inlineStr">
+        <is>
+          <t>NEW</t>
+        </is>
+      </c>
+      <c r="G62" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H62" t="inlineStr">
+        <is>
+          <t>Cambiar</t>
+        </is>
+      </c>
+      <c r="I62" t="n">
+        <v>1</v>
+      </c>
+      <c r="J62" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K62" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L62" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M62" t="n">
+        <v>-58.482497</v>
+      </c>
+      <c r="N62" t="n">
+        <v>-34.598714</v>
+      </c>
+      <c r="O62" t="inlineStr">
+        <is>
+          <t>Paternal</t>
+        </is>
+      </c>
+      <c r="P62" t="inlineStr">
+        <is>
+          <t>Capital Norte</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>6928</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>8/12/2025</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>ALBARELLOS AV. 3101</t>
+        </is>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="E63" t="inlineStr">
+        <is>
+          <t>808918710</t>
+        </is>
+      </c>
+      <c r="F63" t="inlineStr">
+        <is>
+          <t>NEW</t>
+        </is>
+      </c>
+      <c r="G63" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H63" t="inlineStr">
+        <is>
+          <t>Picada</t>
+        </is>
+      </c>
+      <c r="I63" t="n">
+        <v>1</v>
+      </c>
+      <c r="J63" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K63" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L63" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M63" t="n">
+        <v>-58.512623</v>
+      </c>
+      <c r="N63" t="n">
+        <v>-34.579137</v>
+      </c>
+      <c r="O63" t="inlineStr">
+        <is>
+          <t>Paternal</t>
+        </is>
+      </c>
+      <c r="P63" t="inlineStr">
+        <is>
+          <t>Capital Norte</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>6939</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>8/12/2025</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>ANDONAEGUI 1894</t>
+        </is>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="E64" t="inlineStr">
+        <is>
+          <t>808918715</t>
+        </is>
+      </c>
+      <c r="F64" t="inlineStr">
+        <is>
+          <t>NEW</t>
+        </is>
+      </c>
+      <c r="G64" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H64" t="inlineStr">
+        <is>
+          <t>Cambiar</t>
+        </is>
+      </c>
+      <c r="I64" t="n">
+        <v>1</v>
+      </c>
+      <c r="J64" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K64" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L64" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M64" t="n">
+        <v>-58.484848</v>
+      </c>
+      <c r="N64" t="n">
+        <v>-34.581325</v>
+      </c>
+      <c r="O64" t="inlineStr">
+        <is>
+          <t>Paternal</t>
+        </is>
+      </c>
+      <c r="P64" t="inlineStr">
+        <is>
+          <t>Capital Norte</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>-550</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>8/12/2025</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>Fitz roy 267</t>
+        </is>
+      </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="E65" t="inlineStr">
+        <is>
+          <t>808918720</t>
+        </is>
+      </c>
+      <c r="F65" t="inlineStr">
+        <is>
+          <t>NEW</t>
+        </is>
+      </c>
+      <c r="G65" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H65" t="inlineStr">
+        <is>
+          <t>Aplomar columna</t>
+        </is>
+      </c>
+      <c r="I65" t="n">
+        <v>1</v>
+      </c>
+      <c r="J65" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K65" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L65" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M65" t="n">
+        <v>-58.451378</v>
+      </c>
+      <c r="N65" t="n">
+        <v>-34.596195</v>
+      </c>
+      <c r="O65" t="inlineStr">
+        <is>
+          <t>Paternal</t>
+        </is>
+      </c>
+      <c r="P65" t="inlineStr">
         <is>
           <t>Capital Norte</t>
         </is>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-08-13 13:48:01)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_NEW.xlsx
+++ b/mapa_interactivo_NEW.xlsx
@@ -518,17 +518,17 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>5589</t>
+          <t>2098</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>12/31/2023</t>
+          <t>5/24/2024</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>ARCOS 1520</t>
+          <t>AZURDUY JUANA 2449</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -538,7 +538,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>799540526</t>
+          <t>788826017</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -548,33 +548,41 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
+          <t>Pendiente</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Terminal con rienda</t>
         </is>
       </c>
       <c r="I2" t="n">
-        <v>0</v>
-      </c>
-      <c r="J2" t="inlineStr"/>
-      <c r="K2" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
       <c r="L2" t="inlineStr">
         <is>
           <t>Pasante</t>
         </is>
       </c>
       <c r="M2" t="n">
-        <v>-58.449125</v>
+        <v>-58.467279</v>
       </c>
       <c r="N2" t="n">
-        <v>-34.565958</v>
+        <v>-34.551117</v>
       </c>
       <c r="O2" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P2" t="inlineStr">
@@ -586,27 +594,27 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>4862</t>
+          <t>3299</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>1/23/2025</t>
+          <t>9/10/2024</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>ARCOS 2263</t>
+          <t>DIAZ COLODRERO 3309</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>802857379</t>
+          <t>796186684</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -616,16 +624,16 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
+          <t>Pendiente</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>picada</t>
+          <t>Colocar columna para solicitar traspasos</t>
         </is>
       </c>
       <c r="I3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J3" t="inlineStr">
         <is>
@@ -634,7 +642,7 @@
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Nodo TLC</t>
         </is>
       </c>
       <c r="L3" t="inlineStr">
@@ -643,14 +651,14 @@
         </is>
       </c>
       <c r="M3" t="n">
-        <v>-58.455082</v>
+        <v>-58.491722</v>
       </c>
       <c r="N3" t="n">
-        <v>-34.558883</v>
+        <v>-34.565845</v>
       </c>
       <c r="O3" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P3" t="inlineStr">
@@ -662,17 +670,17 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2098</t>
+          <t>3839</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>5/24/2024</t>
+          <t>10/23/2024</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>AZURDUY JUANA 2449</t>
+          <t>PICO 1511</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -682,7 +690,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>788826017</t>
+          <t>798390296</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -697,7 +705,7 @@
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>Terminal con rienda</t>
+          <t>Poste inclinado</t>
         </is>
       </c>
       <c r="I4" t="n">
@@ -705,7 +713,7 @@
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
@@ -715,14 +723,14 @@
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M4" t="n">
-        <v>-58.467279</v>
+        <v>-58.465596</v>
       </c>
       <c r="N4" t="n">
-        <v>-34.551117</v>
+        <v>-34.53627</v>
       </c>
       <c r="O4" t="inlineStr">
         <is>
@@ -738,27 +746,27 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>3299</t>
+          <t>801645368</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>9/10/2024</t>
+          <t>12/13/2024</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>DIAZ COLODRERO 3309</t>
+          <t>San Blas 1809</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>796186684</t>
+          <t>801645368</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -773,11 +781,11 @@
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>Colocar columna para solicitar traspasos</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J5" t="inlineStr">
         <is>
@@ -786,7 +794,7 @@
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>Nodo TLC</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L5" t="inlineStr">
@@ -795,10 +803,10 @@
         </is>
       </c>
       <c r="M5" t="n">
-        <v>-58.491722</v>
+        <v>-58.467767</v>
       </c>
       <c r="N5" t="n">
-        <v>-34.565845</v>
+        <v>-34.604588</v>
       </c>
       <c r="O5" t="inlineStr">
         <is>
@@ -814,17 +822,17 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>3839</t>
+          <t>5589</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>10/23/2024</t>
+          <t>12/31/2023</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>PICO 1511</t>
+          <t>ARCOS 1520</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -834,7 +842,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>798390296</t>
+          <t>799540526</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -844,41 +852,41 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>Poste inclinado</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M6" t="n">
-        <v>-58.465596</v>
+        <v>-58.449125</v>
       </c>
       <c r="N6" t="n">
-        <v>-34.53627</v>
+        <v>-34.565958</v>
       </c>
       <c r="O6" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P6" t="inlineStr">
@@ -890,27 +898,27 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>801645368</t>
+          <t>4595</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>12/13/2024</t>
+          <t>1/15/2025</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>San Blas 1809</t>
+          <t>PAROISSIEN 1806</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>801645368</t>
+          <t>802747617</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -925,15 +933,15 @@
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Aplomar</t>
         </is>
       </c>
       <c r="I7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K7" t="inlineStr">
@@ -943,18 +951,18 @@
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M7" t="n">
-        <v>-58.467767</v>
+        <v>-58.464172</v>
       </c>
       <c r="N7" t="n">
-        <v>-34.604588</v>
+        <v>-34.543845</v>
       </c>
       <c r="O7" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P7" t="inlineStr">
@@ -966,27 +974,27 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>4595</t>
+          <t>4662</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>1/15/2025</t>
+          <t>1/21/2025</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>PAROISSIEN 1806</t>
+          <t>ALTOLAGUIRRE 2397</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>802747617</t>
+          <t>802823938</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -1001,7 +1009,7 @@
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>Aplomar</t>
+          <t>Inclinada</t>
         </is>
       </c>
       <c r="I8" t="n">
@@ -1019,18 +1027,18 @@
       </c>
       <c r="L8" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M8" t="n">
-        <v>-58.464172</v>
+        <v>-58.490766</v>
       </c>
       <c r="N8" t="n">
-        <v>-34.543845</v>
+        <v>-34.576987</v>
       </c>
       <c r="O8" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P8" t="inlineStr">
@@ -1042,27 +1050,27 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>4662</t>
+          <t>4862</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>1/21/2025</t>
+          <t>1/23/2025</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>ALTOLAGUIRRE 2397</t>
+          <t>ARCOS 2263</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>802823938</t>
+          <t>802857379</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -1072,25 +1080,25 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>Inclinada</t>
+          <t>picada</t>
         </is>
       </c>
       <c r="I9" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L9" t="inlineStr">
@@ -1099,14 +1107,14 @@
         </is>
       </c>
       <c r="M9" t="n">
-        <v>-58.490766</v>
+        <v>-58.455082</v>
       </c>
       <c r="N9" t="n">
-        <v>-34.576987</v>
+        <v>-34.558883</v>
       </c>
       <c r="O9" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P9" t="inlineStr">

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-08-15 11:42:25)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_NEW.xlsx
+++ b/mapa_interactivo_NEW.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P65"/>
+  <dimension ref="A1:P69"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5371,6 +5371,262 @@
         </is>
       </c>
     </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>6943</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>8/14/2025</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>SUPERI 1459</t>
+        </is>
+      </c>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>13</t>
+        </is>
+      </c>
+      <c r="E66" t="inlineStr">
+        <is>
+          <t>808972965</t>
+        </is>
+      </c>
+      <c r="F66" t="inlineStr">
+        <is>
+          <t>NEW</t>
+        </is>
+      </c>
+      <c r="G66" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H66" t="inlineStr">
+        <is>
+          <t>Poste con base quebrada ver si es posible desmonte</t>
+        </is>
+      </c>
+      <c r="I66" t="n">
+        <v>1</v>
+      </c>
+      <c r="J66" t="inlineStr">
+        <is>
+          <t>Desmonte</t>
+        </is>
+      </c>
+      <c r="K66" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L66" t="inlineStr">
+        <is>
+          <t>Poste</t>
+        </is>
+      </c>
+      <c r="M66" t="inlineStr"/>
+      <c r="N66" t="inlineStr"/>
+      <c r="O66" t="inlineStr"/>
+      <c r="P66" t="inlineStr"/>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>6944</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>8/14/2025</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>RAVIGNANI, EMILIO, DR. 2040</t>
+        </is>
+      </c>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>14</t>
+        </is>
+      </c>
+      <c r="E67" t="inlineStr">
+        <is>
+          <t>808972970</t>
+        </is>
+      </c>
+      <c r="F67" t="inlineStr">
+        <is>
+          <t>NEW</t>
+        </is>
+      </c>
+      <c r="G67" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H67" t="inlineStr">
+        <is>
+          <t>Picada</t>
+        </is>
+      </c>
+      <c r="I67" t="n">
+        <v>1</v>
+      </c>
+      <c r="J67" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K67" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L67" t="inlineStr">
+        <is>
+          <t>Terminal</t>
+        </is>
+      </c>
+      <c r="M67" t="inlineStr"/>
+      <c r="N67" t="inlineStr"/>
+      <c r="O67" t="inlineStr"/>
+      <c r="P67" t="inlineStr"/>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>6969</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>8/14/2025</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>CIUDAD DE LA PAZ 295</t>
+        </is>
+      </c>
+      <c r="D68" t="inlineStr">
+        <is>
+          <t>14</t>
+        </is>
+      </c>
+      <c r="E68" t="inlineStr">
+        <is>
+          <t>808972995</t>
+        </is>
+      </c>
+      <c r="F68" t="inlineStr">
+        <is>
+          <t>NEW</t>
+        </is>
+      </c>
+      <c r="G68" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H68" t="inlineStr">
+        <is>
+          <t>Cambiar</t>
+        </is>
+      </c>
+      <c r="I68" t="n">
+        <v>1</v>
+      </c>
+      <c r="J68" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K68" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L68" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M68" t="inlineStr"/>
+      <c r="N68" t="inlineStr"/>
+      <c r="O68" t="inlineStr"/>
+      <c r="P68" t="inlineStr"/>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>6971</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>8/14/2025</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>MAURE 1594</t>
+        </is>
+      </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>14</t>
+        </is>
+      </c>
+      <c r="E69" t="inlineStr">
+        <is>
+          <t>808973001</t>
+        </is>
+      </c>
+      <c r="F69" t="inlineStr">
+        <is>
+          <t>NEW</t>
+        </is>
+      </c>
+      <c r="G69" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H69" t="inlineStr">
+        <is>
+          <t>Ver de traspasar a telecentro y  desmontar ver con inspector</t>
+        </is>
+      </c>
+      <c r="I69" t="n">
+        <v>1</v>
+      </c>
+      <c r="J69" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K69" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L69" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M69" t="inlineStr"/>
+      <c r="N69" t="inlineStr"/>
+      <c r="O69" t="inlineStr"/>
+      <c r="P69" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-08-15 11:46:08)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_NEW.xlsx
+++ b/mapa_interactivo_NEW.xlsx
@@ -5430,10 +5430,22 @@
           <t>Poste</t>
         </is>
       </c>
-      <c r="M66" t="inlineStr"/>
-      <c r="N66" t="inlineStr"/>
-      <c r="O66" t="inlineStr"/>
-      <c r="P66" t="inlineStr"/>
+      <c r="M66" t="n">
+        <v>-58.460834</v>
+      </c>
+      <c r="N66" t="n">
+        <v>-34.573753</v>
+      </c>
+      <c r="O66" t="inlineStr">
+        <is>
+          <t>Colegiales</t>
+        </is>
+      </c>
+      <c r="P66" t="inlineStr">
+        <is>
+          <t>Capital Norte</t>
+        </is>
+      </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
@@ -5494,10 +5506,22 @@
           <t>Terminal</t>
         </is>
       </c>
-      <c r="M67" t="inlineStr"/>
-      <c r="N67" t="inlineStr"/>
-      <c r="O67" t="inlineStr"/>
-      <c r="P67" t="inlineStr"/>
+      <c r="M67" t="n">
+        <v>-58.436264</v>
+      </c>
+      <c r="N67" t="n">
+        <v>-34.578942</v>
+      </c>
+      <c r="O67" t="inlineStr">
+        <is>
+          <t>Palermo</t>
+        </is>
+      </c>
+      <c r="P67" t="inlineStr">
+        <is>
+          <t>Capital Sur</t>
+        </is>
+      </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
@@ -5558,10 +5582,22 @@
           <t>Pasante</t>
         </is>
       </c>
-      <c r="M68" t="inlineStr"/>
-      <c r="N68" t="inlineStr"/>
-      <c r="O68" t="inlineStr"/>
-      <c r="P68" t="inlineStr"/>
+      <c r="M68" t="n">
+        <v>-58.441171</v>
+      </c>
+      <c r="N68" t="n">
+        <v>-34.574547</v>
+      </c>
+      <c r="O68" t="inlineStr">
+        <is>
+          <t>Palermo</t>
+        </is>
+      </c>
+      <c r="P68" t="inlineStr">
+        <is>
+          <t>Capital Sur</t>
+        </is>
+      </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
@@ -5622,10 +5658,22 @@
           <t>Pasante</t>
         </is>
       </c>
-      <c r="M69" t="inlineStr"/>
-      <c r="N69" t="inlineStr"/>
-      <c r="O69" t="inlineStr"/>
-      <c r="P69" t="inlineStr"/>
+      <c r="M69" t="n">
+        <v>-58.435072</v>
+      </c>
+      <c r="N69" t="n">
+        <v>-34.565732</v>
+      </c>
+      <c r="O69" t="inlineStr">
+        <is>
+          <t>Palermo</t>
+        </is>
+      </c>
+      <c r="P69" t="inlineStr">
+        <is>
+          <t>Capital Sur</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-08-20 07:40:36)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_NEW.xlsx
+++ b/mapa_interactivo_NEW.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P69"/>
+  <dimension ref="A1:P68"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -518,27 +518,27 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2098</t>
+          <t>3299</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>5/24/2024</t>
+          <t>9/10/2024</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>AZURDUY JUANA 2449</t>
+          <t>DIAZ COLODRERO 3309</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>788826017</t>
+          <t>796186684</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -548,12 +548,12 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>Terminal con rienda</t>
+          <t>qap traspaso nodo TLC y Teco</t>
         </is>
       </c>
       <c r="I2" t="n">
@@ -566,7 +566,7 @@
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo TLC</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
@@ -575,14 +575,14 @@
         </is>
       </c>
       <c r="M2" t="n">
-        <v>-58.467279</v>
+        <v>-58.491722</v>
       </c>
       <c r="N2" t="n">
-        <v>-34.551117</v>
+        <v>-34.565845</v>
       </c>
       <c r="O2" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P2" t="inlineStr">
@@ -594,27 +594,27 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>3299</t>
+          <t>3839</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>9/10/2024</t>
+          <t>10/23/2024</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>DIAZ COLODRERO 3309</t>
+          <t>PICO 1511</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>796186684</t>
+          <t>798390296</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -629,7 +629,7 @@
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>Colocar columna para solicitar traspasos</t>
+          <t>Poste inclinado</t>
         </is>
       </c>
       <c r="I3" t="n">
@@ -637,28 +637,28 @@
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>Nodo TLC</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M3" t="n">
-        <v>-58.491722</v>
+        <v>-58.465596</v>
       </c>
       <c r="N3" t="n">
-        <v>-34.565845</v>
+        <v>-34.53627</v>
       </c>
       <c r="O3" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P3" t="inlineStr">
@@ -670,27 +670,27 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>3839</t>
+          <t>801645368</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>10/23/2024</t>
+          <t>12/13/2024</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>PICO 1511</t>
+          <t>San Blas 1809</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>798390296</t>
+          <t>801645368</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -705,15 +705,15 @@
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>Poste inclinado</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
@@ -723,18 +723,18 @@
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M4" t="n">
-        <v>-58.465596</v>
+        <v>-58.467767</v>
       </c>
       <c r="N4" t="n">
-        <v>-34.53627</v>
+        <v>-34.604588</v>
       </c>
       <c r="O4" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P4" t="inlineStr">
@@ -746,27 +746,27 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>801645368</t>
+          <t>5589</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>12/13/2024</t>
+          <t>12/31/2023</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>San Blas 1809</t>
+          <t>ARCOS 1520</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>801645368</t>
+          <t>799540526</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -776,7 +776,7 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
@@ -794,7 +794,7 @@
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L5" t="inlineStr">
@@ -803,14 +803,14 @@
         </is>
       </c>
       <c r="M5" t="n">
-        <v>-58.467767</v>
+        <v>-58.449125</v>
       </c>
       <c r="N5" t="n">
-        <v>-34.604588</v>
+        <v>-34.565958</v>
       </c>
       <c r="O5" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P5" t="inlineStr">
@@ -822,17 +822,17 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>5589</t>
+          <t>4595</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>12/31/2023</t>
+          <t>1/15/2025</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>ARCOS 1520</t>
+          <t>PAROISSIEN 1806</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -842,7 +842,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>799540526</t>
+          <t>802747617</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -852,41 +852,41 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
+          <t>Pendiente</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Aplomar</t>
         </is>
       </c>
       <c r="I6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M6" t="n">
-        <v>-58.449125</v>
+        <v>-58.464172</v>
       </c>
       <c r="N6" t="n">
-        <v>-34.565958</v>
+        <v>-34.543845</v>
       </c>
       <c r="O6" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P6" t="inlineStr">
@@ -898,27 +898,27 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>4595</t>
+          <t>4662</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>1/15/2025</t>
+          <t>1/21/2025</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>PAROISSIEN 1806</t>
+          <t>ALTOLAGUIRRE 2397</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>802747617</t>
+          <t>802823938</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -933,7 +933,7 @@
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>Aplomar</t>
+          <t>Inclinada</t>
         </is>
       </c>
       <c r="I7" t="n">
@@ -951,18 +951,18 @@
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M7" t="n">
-        <v>-58.464172</v>
+        <v>-58.490766</v>
       </c>
       <c r="N7" t="n">
-        <v>-34.543845</v>
+        <v>-34.576987</v>
       </c>
       <c r="O7" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P7" t="inlineStr">
@@ -974,27 +974,27 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>4662</t>
+          <t>4862</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>1/21/2025</t>
+          <t>1/23/2025</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>ALTOLAGUIRRE 2397</t>
+          <t>ARCOS 2263</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>802823938</t>
+          <t>802857379</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -1004,25 +1004,25 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>Inclinada</t>
+          <t>picada</t>
         </is>
       </c>
       <c r="I8" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L8" t="inlineStr">
@@ -1031,14 +1031,14 @@
         </is>
       </c>
       <c r="M8" t="n">
-        <v>-58.490766</v>
+        <v>-58.455082</v>
       </c>
       <c r="N8" t="n">
-        <v>-34.576987</v>
+        <v>-34.558883</v>
       </c>
       <c r="O8" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P8" t="inlineStr">
@@ -1050,27 +1050,27 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>4862</t>
+          <t>6036</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>1/23/2025</t>
+          <t>2/24/2025</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>ARCOS 2263</t>
+          <t>MEDRANO 1715</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>802857379</t>
+          <t>803608181</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -1080,14 +1080,10 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
-        </is>
-      </c>
-      <c r="H9" t="inlineStr">
-        <is>
-          <t>picada</t>
-        </is>
-      </c>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr"/>
       <c r="I9" t="n">
         <v>0</v>
       </c>
@@ -1107,26 +1103,26 @@
         </is>
       </c>
       <c r="M9" t="n">
-        <v>-58.455082</v>
+        <v>-58.418236</v>
       </c>
       <c r="N9" t="n">
-        <v>-34.558883</v>
+        <v>-34.589859</v>
       </c>
       <c r="O9" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P9" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>6036</t>
+          <t>803608480</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -1136,7 +1132,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>MEDRANO 1715</t>
+          <t>GUATEMALA /ALT/ 4415</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -1146,7 +1142,7 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>803608181</t>
+          <t>803608480</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
@@ -1159,7 +1155,11 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H10" t="inlineStr"/>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Guatemala 4415 </t>
+        </is>
+      </c>
       <c r="I10" t="n">
         <v>0</v>
       </c>
@@ -1170,7 +1170,7 @@
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L10" t="inlineStr">
@@ -1179,10 +1179,10 @@
         </is>
       </c>
       <c r="M10" t="n">
-        <v>-58.418236</v>
+        <v>-58.421661</v>
       </c>
       <c r="N10" t="n">
-        <v>-34.589859</v>
+        <v>-34.588428</v>
       </c>
       <c r="O10" t="inlineStr">
         <is>
@@ -1198,27 +1198,27 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>803608480</t>
+          <t>5053</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>2/24/2025</t>
+          <t>3/11/2025</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>GUATEMALA /ALT/ 4415</t>
+          <t>MENDOZA 1153</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>803608480</t>
+          <t>803969314</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
@@ -1233,7 +1233,7 @@
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t xml:space="preserve">Guatemala 4415 </t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="I11" t="n">
@@ -1251,50 +1251,50 @@
       </c>
       <c r="L11" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M11" t="n">
-        <v>-58.421661</v>
+        <v>-58.44463</v>
       </c>
       <c r="N11" t="n">
-        <v>-34.588428</v>
+        <v>-34.553354</v>
       </c>
       <c r="O11" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P11" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>5053</t>
+          <t>6071</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>3/11/2025</t>
+          <t>3/17/2025</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>MENDOZA 1153</t>
+          <t>OSORIO 4994</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>803969314</t>
+          <t>804053324</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
@@ -1307,11 +1307,7 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H12" t="inlineStr">
-        <is>
-          <t>Poste</t>
-        </is>
-      </c>
+      <c r="H12" t="inlineStr"/>
       <c r="I12" t="n">
         <v>0</v>
       </c>
@@ -1327,18 +1323,18 @@
       </c>
       <c r="L12" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M12" t="n">
-        <v>-58.44463</v>
+        <v>-58.466241</v>
       </c>
       <c r="N12" t="n">
-        <v>-34.553354</v>
+        <v>-34.595741</v>
       </c>
       <c r="O12" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P12" t="inlineStr">
@@ -1350,27 +1346,27 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>6071</t>
+          <t>3348</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>3/17/2025</t>
+          <t>3/27/2025</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>OSORIO 4994</t>
+          <t>ESTOMBA 2626</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>804053324</t>
+          <t>804309704</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
@@ -1383,13 +1379,17 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H13" t="inlineStr"/>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>Picada</t>
+        </is>
+      </c>
       <c r="I13" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Desmonte</t>
         </is>
       </c>
       <c r="K13" t="inlineStr">
@@ -1403,14 +1403,14 @@
         </is>
       </c>
       <c r="M13" t="n">
-        <v>-58.466241</v>
+        <v>-58.47538</v>
       </c>
       <c r="N13" t="n">
-        <v>-34.595741</v>
+        <v>-34.566015</v>
       </c>
       <c r="O13" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P13" t="inlineStr">
@@ -1422,27 +1422,27 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>3348</t>
+          <t>-312</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>3/27/2025</t>
+          <t>3/29/2025</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>ESTOMBA 2626</t>
+          <t>MATIENZO BENJAMIN /ALT/ 1831</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>804309704</t>
+          <t>804333522</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
@@ -1457,20 +1457,20 @@
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Retirar columna ya traspasaron el nodo</t>
         </is>
       </c>
       <c r="I14" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>Desmonte</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L14" t="inlineStr">
@@ -1479,46 +1479,46 @@
         </is>
       </c>
       <c r="M14" t="n">
-        <v>-58.47538</v>
+        <v>-58.434835</v>
       </c>
       <c r="N14" t="n">
-        <v>-34.566015</v>
+        <v>-34.569129</v>
       </c>
       <c r="O14" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P14" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>-312</t>
+          <t>3430</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>3/29/2025</t>
+          <t>4/1/2025</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>MATIENZO BENJAMIN /ALT/ 1831</t>
+          <t>MONROE 3838</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>804333522</t>
+          <t>804468442</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
@@ -1533,68 +1533,68 @@
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>Retirar columna ya traspasaron el nodo</t>
+          <t>Reparar rienda</t>
         </is>
       </c>
       <c r="I15" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Tensor</t>
         </is>
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L15" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M15" t="n">
-        <v>-58.434835</v>
+        <v>-58.473659</v>
       </c>
       <c r="N15" t="n">
-        <v>-34.569129</v>
+        <v>-34.566979</v>
       </c>
       <c r="O15" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P15" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>3430</t>
+          <t>5464</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>4/1/2025</t>
+          <t>4/4/2025</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>MONROE 3838</t>
+          <t>SUCRE, ANTONIO JOSE DE, MCAL. 3100</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>804468442</t>
+          <t>804497880</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
@@ -1609,7 +1609,7 @@
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>Reparar rienda</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I16" t="n">
@@ -1617,7 +1617,7 @@
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>Tensor</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K16" t="inlineStr">
@@ -1631,10 +1631,10 @@
         </is>
       </c>
       <c r="M16" t="n">
-        <v>-58.473659</v>
+        <v>-58.46161</v>
       </c>
       <c r="N16" t="n">
-        <v>-34.566979</v>
+        <v>-34.567849</v>
       </c>
       <c r="O16" t="inlineStr">
         <is>
@@ -1650,7 +1650,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>5464</t>
+          <t>5469</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -1660,17 +1660,17 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>SUCRE, ANTONIO JOSE DE, MCAL. 3100</t>
+          <t>ESTADO PLURINACIONAL DE BOLIVIA 5899</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>804497880</t>
+          <t>804497887</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
@@ -1685,7 +1685,7 @@
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Aplomar</t>
         </is>
       </c>
       <c r="I17" t="n">
@@ -1693,7 +1693,7 @@
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K17" t="inlineStr">
@@ -1707,14 +1707,14 @@
         </is>
       </c>
       <c r="M17" t="n">
-        <v>-58.46161</v>
+        <v>-58.507746</v>
       </c>
       <c r="N17" t="n">
-        <v>-34.567849</v>
+        <v>-34.574217</v>
       </c>
       <c r="O17" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P17" t="inlineStr">
@@ -1726,7 +1726,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>5469</t>
+          <t>5492</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -1736,7 +1736,7 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>ESTADO PLURINACIONAL DE BOLIVIA 5899</t>
+          <t>ESTADO PLURINACIONAL DE BOLIVIA 5920</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
@@ -1746,7 +1746,7 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>804497887</t>
+          <t>804498035</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
@@ -1761,7 +1761,7 @@
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>Aplomar</t>
+          <t>aplomar</t>
         </is>
       </c>
       <c r="I18" t="n">
@@ -1783,10 +1783,10 @@
         </is>
       </c>
       <c r="M18" t="n">
-        <v>-58.507746</v>
+        <v>-58.50751</v>
       </c>
       <c r="N18" t="n">
-        <v>-34.574217</v>
+        <v>-34.574543</v>
       </c>
       <c r="O18" t="inlineStr">
         <is>
@@ -1802,17 +1802,17 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>5492</t>
+          <t>5599</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>4/4/2025</t>
+          <t>4/15/2025</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>ESTADO PLURINACIONAL DE BOLIVIA 5920</t>
+          <t>ESTOMBA 4052</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
@@ -1822,7 +1822,7 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>804498035</t>
+          <t>804732246</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
@@ -1837,7 +1837,7 @@
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>aplomar</t>
+          <t>Columna PRFV quedo inclinada (la hicieron como estomba 4056)</t>
         </is>
       </c>
       <c r="I19" t="n">
@@ -1850,23 +1850,23 @@
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo TLC</t>
         </is>
       </c>
       <c r="L19" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M19" t="n">
-        <v>-58.50751</v>
+        <v>-58.485407</v>
       </c>
       <c r="N19" t="n">
-        <v>-34.574543</v>
+        <v>-34.552985</v>
       </c>
       <c r="O19" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P19" t="inlineStr">
@@ -1878,7 +1878,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>5599</t>
+          <t>5590</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -1888,17 +1888,17 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>ESTOMBA 4052</t>
+          <t>O'HIGGINS 2441</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>804732246</t>
+          <t>804732275</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
@@ -1913,7 +1913,7 @@
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>Columna PRFV quedo inclinada (la hicieron como estomba 4056)</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I20" t="n">
@@ -1921,12 +1921,12 @@
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>Nodo TLC</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L20" t="inlineStr">
@@ -1935,10 +1935,10 @@
         </is>
       </c>
       <c r="M20" t="n">
-        <v>-58.485407</v>
+        <v>-58.45573</v>
       </c>
       <c r="N20" t="n">
-        <v>-34.552985</v>
+        <v>-34.556576</v>
       </c>
       <c r="O20" t="inlineStr">
         <is>
@@ -1954,27 +1954,27 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>5590</t>
+          <t>804787368</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>4/15/2025</t>
+          <t>4/17/2025</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>O'HIGGINS 2441</t>
+          <t>San Blas 2591</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>804732275</t>
+          <t>804787368</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
@@ -2011,14 +2011,14 @@
         </is>
       </c>
       <c r="M21" t="n">
-        <v>-58.45573</v>
+        <v>-58.477427</v>
       </c>
       <c r="N21" t="n">
-        <v>-34.556576</v>
+        <v>-34.609261</v>
       </c>
       <c r="O21" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P21" t="inlineStr">
@@ -2030,27 +2030,27 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>804787368</t>
+          <t>5624</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>4/17/2025</t>
+          <t>4/22/2025</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>San Blas 2591</t>
+          <t>PINO, VIRREY DEL 3456</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>804787368</t>
+          <t>804876043</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
@@ -2065,7 +2065,7 @@
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Desmonte de poste</t>
         </is>
       </c>
       <c r="I22" t="n">
@@ -2073,7 +2073,7 @@
       </c>
       <c r="J22" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Desmonte</t>
         </is>
       </c>
       <c r="K22" t="inlineStr">
@@ -2083,18 +2083,18 @@
       </c>
       <c r="L22" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M22" t="n">
-        <v>-58.477427</v>
+        <v>-58.464354</v>
       </c>
       <c r="N22" t="n">
-        <v>-34.609261</v>
+        <v>-34.572486</v>
       </c>
       <c r="O22" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P22" t="inlineStr">
@@ -2106,17 +2106,17 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>5624</t>
+          <t>804922147</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>4/22/2025</t>
+          <t>4/24/2025</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>PINO, VIRREY DEL 3456</t>
+          <t>Av. Álvarez Thomas 1171</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
@@ -2126,7 +2126,7 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>804876043</t>
+          <t>804922147</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
@@ -2141,15 +2141,15 @@
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>Desmonte de poste</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I23" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>Desmonte</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K23" t="inlineStr">
@@ -2159,14 +2159,14 @@
       </c>
       <c r="L23" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M23" t="n">
-        <v>-58.464354</v>
+        <v>-58.45793</v>
       </c>
       <c r="N23" t="n">
-        <v>-34.572486</v>
+        <v>-34.578334</v>
       </c>
       <c r="O23" t="inlineStr">
         <is>
@@ -2182,7 +2182,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>804922147</t>
+          <t>804922171</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -2192,7 +2192,7 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Av. Álvarez Thomas 1171</t>
+          <t>Virrey Arredondo 3581</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
@@ -2202,7 +2202,7 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>804922147</t>
+          <t>804922171</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
@@ -2217,15 +2217,15 @@
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Aplomar</t>
         </is>
       </c>
       <c r="I24" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J24" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K24" t="inlineStr">
@@ -2235,14 +2235,14 @@
       </c>
       <c r="L24" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M24" t="n">
-        <v>-58.45793</v>
+        <v>-58.459513</v>
       </c>
       <c r="N24" t="n">
-        <v>-34.578334</v>
+        <v>-34.578019</v>
       </c>
       <c r="O24" t="inlineStr">
         <is>
@@ -2258,7 +2258,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>804922171</t>
+          <t>5656</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -2268,17 +2268,17 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Virrey Arredondo 3581</t>
+          <t>ECHEVERRIA 5893</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>804922171</t>
+          <t>804922184</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
@@ -2293,7 +2293,7 @@
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>Aplomar</t>
+          <t>Poste con base quebrada</t>
         </is>
       </c>
       <c r="I25" t="n">
@@ -2301,7 +2301,7 @@
       </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Desmonte</t>
         </is>
       </c>
       <c r="K25" t="inlineStr">
@@ -2311,18 +2311,18 @@
       </c>
       <c r="L25" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M25" t="n">
-        <v>-58.459513</v>
+        <v>-58.489627</v>
       </c>
       <c r="N25" t="n">
-        <v>-34.578019</v>
+        <v>-34.583761</v>
       </c>
       <c r="O25" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P25" t="inlineStr">
@@ -2334,27 +2334,27 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>5656</t>
+          <t>6173</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>4/24/2025</t>
+          <t>4/29/2025</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>ECHEVERRIA 5893</t>
+          <t>ARMENIA 2321</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>804922184</t>
+          <t>805507398</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
@@ -2369,7 +2369,7 @@
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>Poste con base quebrada</t>
+          <t>Picada volvio a entrar como caso 6325</t>
         </is>
       </c>
       <c r="I26" t="n">
@@ -2377,7 +2377,7 @@
       </c>
       <c r="J26" t="inlineStr">
         <is>
-          <t>Desmonte</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K26" t="inlineStr">
@@ -2387,50 +2387,50 @@
       </c>
       <c r="L26" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M26" t="n">
-        <v>-58.489627</v>
+        <v>-58.420549</v>
       </c>
       <c r="N26" t="n">
-        <v>-34.583761</v>
+        <v>-34.585103</v>
       </c>
       <c r="O26" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P26" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>6173</t>
+          <t>5715</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>4/29/2025</t>
+          <t>5/1/2025</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>ARMENIA 2321</t>
+          <t>CUENCA 4690</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>805507398</t>
+          <t>805579094</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
@@ -2445,7 +2445,7 @@
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>Picada volvio a entrar como caso 6325</t>
+          <t>Aplomar poste</t>
         </is>
       </c>
       <c r="I27" t="n">
@@ -2453,7 +2453,7 @@
       </c>
       <c r="J27" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K27" t="inlineStr">
@@ -2463,30 +2463,30 @@
       </c>
       <c r="L27" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M27" t="n">
-        <v>-58.420549</v>
+        <v>-58.506061</v>
       </c>
       <c r="N27" t="n">
-        <v>-34.585103</v>
+        <v>-34.588887</v>
       </c>
       <c r="O27" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P27" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>5715</t>
+          <t>5719</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -2496,7 +2496,7 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>CUENCA 4690</t>
+          <t>CABEZON, JOSE LEON 2440</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
@@ -2506,7 +2506,7 @@
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>805579094</t>
+          <t>805579157</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
@@ -2521,7 +2521,7 @@
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>Aplomar poste</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I28" t="n">
@@ -2529,7 +2529,7 @@
       </c>
       <c r="J28" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K28" t="inlineStr">
@@ -2539,14 +2539,14 @@
       </c>
       <c r="L28" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M28" t="n">
-        <v>-58.506061</v>
+        <v>-58.499967</v>
       </c>
       <c r="N28" t="n">
-        <v>-34.588887</v>
+        <v>-34.57974</v>
       </c>
       <c r="O28" t="inlineStr">
         <is>
@@ -2562,7 +2562,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>5719</t>
+          <t>6333</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -2572,17 +2572,17 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>CABEZON, JOSE LEON 2440</t>
+          <t>ORTEGA Y GASSET 1816</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>805579157</t>
+          <t>805655342</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
@@ -2619,36 +2619,36 @@
         </is>
       </c>
       <c r="M29" t="n">
-        <v>-58.499967</v>
+        <v>-58.432556</v>
       </c>
       <c r="N29" t="n">
-        <v>-34.57974</v>
+        <v>-34.570279</v>
       </c>
       <c r="O29" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P29" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>6333</t>
+          <t>805707165</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>5/1/2025</t>
+          <t>5/7/2025</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>ORTEGA Y GASSET 1816</t>
+          <t>Baez 793</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
@@ -2658,7 +2658,7 @@
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>805655342</t>
+          <t>805707165</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
@@ -2673,7 +2673,7 @@
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>DESMONTAR COLUMNA DE 7 MTS Y TRANSFERIR A COMUNITARIA</t>
         </is>
       </c>
       <c r="I30" t="n">
@@ -2691,14 +2691,14 @@
       </c>
       <c r="L30" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M30" t="n">
-        <v>-58.432556</v>
+        <v>-58.436165</v>
       </c>
       <c r="N30" t="n">
-        <v>-34.570279</v>
+        <v>-34.569081</v>
       </c>
       <c r="O30" t="inlineStr">
         <is>
@@ -2714,27 +2714,27 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>805707165</t>
+          <t>5847</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>5/7/2025</t>
+          <t>5/8/2025</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Baez 793</t>
+          <t>JURAMENTO 5321</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>805707165</t>
+          <t>805791839</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
@@ -2749,7 +2749,7 @@
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>DESMONTAR COLUMNA DE 7 MTS Y TRANSFERIR A COMUNITARIA</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I31" t="n">
@@ -2767,50 +2767,50 @@
       </c>
       <c r="L31" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M31" t="n">
-        <v>-58.436165</v>
+        <v>-58.485193</v>
       </c>
       <c r="N31" t="n">
-        <v>-34.569081</v>
+        <v>-34.579621</v>
       </c>
       <c r="O31" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P31" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>5847</t>
+          <t>232</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>5/8/2025</t>
+          <t>5/9/2025</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>JURAMENTO 5321</t>
+          <t>Gorostiaga 2286</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>805791839</t>
+          <t>805791858</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
@@ -2847,46 +2847,46 @@
         </is>
       </c>
       <c r="M32" t="n">
-        <v>-58.485193</v>
+        <v>-58.441563</v>
       </c>
       <c r="N32" t="n">
-        <v>-34.579621</v>
+        <v>-34.569743</v>
       </c>
       <c r="O32" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P32" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>232</t>
+          <t>-406</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>5/9/2025</t>
+          <t>5/8/2025</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Gorostiaga 2286</t>
+          <t>Olof palme 4144</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>805791858</t>
+          <t>805791925</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
@@ -2901,7 +2901,7 @@
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Tensar 2 riendas a pique columna 168</t>
         </is>
       </c>
       <c r="I33" t="n">
@@ -2909,7 +2909,7 @@
       </c>
       <c r="J33" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Tensor</t>
         </is>
       </c>
       <c r="K33" t="inlineStr">
@@ -2919,40 +2919,40 @@
       </c>
       <c r="L33" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M33" t="n">
-        <v>-58.441563</v>
+        <v>-58.488252</v>
       </c>
       <c r="N33" t="n">
-        <v>-34.569743</v>
+        <v>-34.553391</v>
       </c>
       <c r="O33" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P33" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>-406</t>
+          <t>5826</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>5/8/2025</t>
+          <t>5/19/2025</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Olof palme 4144</t>
+          <t>ALBARELLOS AV. 3180</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
@@ -2962,7 +2962,7 @@
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>805791925</t>
+          <t>806926466</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
@@ -2977,7 +2977,7 @@
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>Tensar 2 riendas a pique columna 168</t>
+          <t>Columna (metal) inclinada</t>
         </is>
       </c>
       <c r="I34" t="n">
@@ -2985,7 +2985,7 @@
       </c>
       <c r="J34" t="inlineStr">
         <is>
-          <t>Tensor</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K34" t="inlineStr">
@@ -2999,14 +2999,14 @@
         </is>
       </c>
       <c r="M34" t="n">
-        <v>-58.488252</v>
+        <v>-58.513552</v>
       </c>
       <c r="N34" t="n">
-        <v>-34.553391</v>
+        <v>-34.579829</v>
       </c>
       <c r="O34" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P34" t="inlineStr">
@@ -3018,27 +3018,27 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>5826</t>
+          <t>6020</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>5/19/2025</t>
+          <t>6/5/2025</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>ALBARELLOS AV. 3180</t>
+          <t>RAVIGNANI, EMILIO, DR. 2036</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>806926466</t>
+          <t>807215465</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
@@ -3053,7 +3053,7 @@
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>Columna (metal) inclinada</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I35" t="n">
@@ -3061,7 +3061,7 @@
       </c>
       <c r="J35" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K35" t="inlineStr">
@@ -3071,50 +3071,50 @@
       </c>
       <c r="L35" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M35" t="n">
-        <v>-58.513552</v>
+        <v>-58.436298</v>
       </c>
       <c r="N35" t="n">
-        <v>-34.579829</v>
+        <v>-34.578972</v>
       </c>
       <c r="O35" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P35" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>6020</t>
+          <t>6144</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>6/5/2025</t>
+          <t>6/11/2025</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>RAVIGNANI, EMILIO, DR. 2036</t>
+          <t>TURIN 2990</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>807215465</t>
+          <t>807458282</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
@@ -3151,26 +3151,26 @@
         </is>
       </c>
       <c r="M36" t="n">
-        <v>-58.436298</v>
+        <v>-58.480925</v>
       </c>
       <c r="N36" t="n">
-        <v>-34.578972</v>
+        <v>-34.585471</v>
       </c>
       <c r="O36" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P36" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>6144</t>
+          <t>6143</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
@@ -3180,7 +3180,7 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>TURIN 2990</t>
+          <t>SOLANO LOPEZ, F., MARISCAL 2845</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
@@ -3190,7 +3190,7 @@
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>807458282</t>
+          <t>807458296</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
@@ -3227,10 +3227,10 @@
         </is>
       </c>
       <c r="M37" t="n">
-        <v>-58.480925</v>
+        <v>-58.495071</v>
       </c>
       <c r="N37" t="n">
-        <v>-34.585471</v>
+        <v>-34.593122</v>
       </c>
       <c r="O37" t="inlineStr">
         <is>
@@ -3246,7 +3246,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>6143</t>
+          <t>6141</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
@@ -3256,17 +3256,17 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>SOLANO LOPEZ, F., MARISCAL 2845</t>
+          <t>EL PAMPERO 2618</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>807458296</t>
+          <t>807458310</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
@@ -3281,7 +3281,7 @@
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Picada info para cierre tambien entro como caso 6911</t>
         </is>
       </c>
       <c r="I38" t="n">
@@ -3303,10 +3303,10 @@
         </is>
       </c>
       <c r="M38" t="n">
-        <v>-58.495071</v>
+        <v>-58.481942</v>
       </c>
       <c r="N38" t="n">
-        <v>-34.593122</v>
+        <v>-34.602989</v>
       </c>
       <c r="O38" t="inlineStr">
         <is>
@@ -3322,17 +3322,17 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>6141</t>
+          <t>-478</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>6/11/2025</t>
+          <t>6/15/2025</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>EL PAMPERO 2618</t>
+          <t>Chivilcoy 4875</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
@@ -3342,7 +3342,7 @@
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>807458310</t>
+          <t>807508509</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
@@ -3357,7 +3357,7 @@
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>Picada info para cierre tambien entro como caso 6911</t>
+          <t>Poste podrido</t>
         </is>
       </c>
       <c r="I39" t="n">
@@ -3375,14 +3375,14 @@
       </c>
       <c r="L39" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M39" t="n">
-        <v>-58.481942</v>
+        <v>-58.517389</v>
       </c>
       <c r="N39" t="n">
-        <v>-34.602989</v>
+        <v>-34.593541</v>
       </c>
       <c r="O39" t="inlineStr">
         <is>
@@ -3398,27 +3398,27 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>-478</t>
+          <t>6171</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>6/15/2025</t>
+          <t>6/18/2025</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Chivilcoy 4875</t>
+          <t>CABELLO 3486</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>807508509</t>
+          <t>807658640</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
@@ -3433,7 +3433,7 @@
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t>Poste podrido</t>
+          <t>Columna inclinada evaluar con inspector un corrimiento</t>
         </is>
       </c>
       <c r="I40" t="n">
@@ -3451,40 +3451,40 @@
       </c>
       <c r="L40" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M40" t="n">
-        <v>-58.517389</v>
+        <v>-58.409579</v>
       </c>
       <c r="N40" t="n">
-        <v>-34.593541</v>
+        <v>-34.581134</v>
       </c>
       <c r="O40" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P40" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>6171</t>
+          <t>6230</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>6/18/2025</t>
+          <t>6/24/2025</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>CABELLO 3486</t>
+          <t>Santa maria de oro	2722</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
@@ -3494,7 +3494,7 @@
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>807658640</t>
+          <t>807763066</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
@@ -3509,7 +3509,7 @@
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>Columna inclinada evaluar con inspector un corrimiento</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I41" t="n">
@@ -3531,10 +3531,10 @@
         </is>
       </c>
       <c r="M41" t="n">
-        <v>-58.409579</v>
+        <v>-58.422315</v>
       </c>
       <c r="N41" t="n">
-        <v>-34.581134</v>
+        <v>-34.576988</v>
       </c>
       <c r="O41" t="inlineStr">
         <is>
@@ -3550,7 +3550,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>6230</t>
+          <t>6231</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
@@ -3560,7 +3560,7 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Santa maria de oro	2722</t>
+          <t>Ciudad de la Paz 275</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
@@ -3570,7 +3570,7 @@
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>807763066</t>
+          <t>807763070</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
@@ -3585,7 +3585,7 @@
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Aplomar o cambiar</t>
         </is>
       </c>
       <c r="I42" t="n">
@@ -3603,14 +3603,14 @@
       </c>
       <c r="L42" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M42" t="n">
-        <v>-58.422315</v>
+        <v>-58.441049</v>
       </c>
       <c r="N42" t="n">
-        <v>-34.576988</v>
+        <v>-34.574625</v>
       </c>
       <c r="O42" t="inlineStr">
         <is>
@@ -3626,7 +3626,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>6231</t>
+          <t>6235</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
@@ -3636,17 +3636,17 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Ciudad de la Paz 275</t>
+          <t>HUERGO 389</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>807763070</t>
+          <t>807763078</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
@@ -3661,7 +3661,7 @@
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>Aplomar o cambiar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I43" t="n">
@@ -3679,14 +3679,14 @@
       </c>
       <c r="L43" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M43" t="n">
-        <v>-58.441049</v>
+        <v>-58.432722</v>
       </c>
       <c r="N43" t="n">
-        <v>-34.574625</v>
+        <v>-34.572371</v>
       </c>
       <c r="O43" t="inlineStr">
         <is>
@@ -3702,27 +3702,27 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>6235</t>
+          <t>6295</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>6/24/2025</t>
+          <t>6/30/2025</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>HUERGO 389</t>
+          <t>SOLER 6017</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>807763078</t>
+          <t>807851636</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
@@ -3759,10 +3759,10 @@
         </is>
       </c>
       <c r="M44" t="n">
-        <v>-58.432722</v>
+        <v>-58.436808</v>
       </c>
       <c r="N44" t="n">
-        <v>-34.572371</v>
+        <v>-34.577464</v>
       </c>
       <c r="O44" t="inlineStr">
         <is>
@@ -3778,17 +3778,17 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>6295</t>
+          <t>6332</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>6/30/2025</t>
+          <t>7/3/2025</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>SOLER 6017</t>
+          <t>ARAOZ 2560</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
@@ -3798,7 +3798,7 @@
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>807851636</t>
+          <t>807965818</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
@@ -3835,10 +3835,10 @@
         </is>
       </c>
       <c r="M45" t="n">
-        <v>-58.436808</v>
+        <v>-58.414507</v>
       </c>
       <c r="N45" t="n">
-        <v>-34.577464</v>
+        <v>-34.585377</v>
       </c>
       <c r="O45" t="inlineStr">
         <is>
@@ -3854,27 +3854,27 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>6332</t>
+          <t>-503</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>7/3/2025</t>
+          <t>7/10/2025</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>ARAOZ 2560</t>
+          <t>Salguero 842</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>807965818</t>
+          <t>808148673</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
@@ -3889,7 +3889,7 @@
       </c>
       <c r="H46" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambiar columna picada en la base</t>
         </is>
       </c>
       <c r="I46" t="n">
@@ -3911,14 +3911,14 @@
         </is>
       </c>
       <c r="M46" t="n">
-        <v>-58.414507</v>
+        <v>-58.419166</v>
       </c>
       <c r="N46" t="n">
-        <v>-34.585377</v>
+        <v>-34.600265</v>
       </c>
       <c r="O46" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P46" t="inlineStr">
@@ -3930,7 +3930,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>-503</t>
+          <t>6506</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
@@ -3940,17 +3940,17 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Salguero 842</t>
+          <t>Ohiggins 1611</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>808148673</t>
+          <t>808148679</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
@@ -3965,7 +3965,7 @@
       </c>
       <c r="H47" t="inlineStr">
         <is>
-          <t>Cambiar columna picada en la base</t>
+          <t>Columna podrida en la base</t>
         </is>
       </c>
       <c r="I47" t="n">
@@ -3978,7 +3978,7 @@
       </c>
       <c r="K47" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L47" t="inlineStr">
@@ -3987,46 +3987,46 @@
         </is>
       </c>
       <c r="M47" t="n">
-        <v>-58.419166</v>
+        <v>-58.448993</v>
       </c>
       <c r="N47" t="n">
-        <v>-34.600265</v>
+        <v>-34.564383</v>
       </c>
       <c r="O47" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P47" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>6506</t>
+          <t>6437</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>7/10/2025</t>
+          <t>7/17/2025</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Ohiggins 1611</t>
+          <t>MILLER 4590</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>808148679</t>
+          <t>808400306</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
@@ -4041,7 +4041,7 @@
       </c>
       <c r="H48" t="inlineStr">
         <is>
-          <t>Columna podrida en la base</t>
+          <t>Columna corroida</t>
         </is>
       </c>
       <c r="I48" t="n">
@@ -4054,7 +4054,7 @@
       </c>
       <c r="K48" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L48" t="inlineStr">
@@ -4063,14 +4063,14 @@
         </is>
       </c>
       <c r="M48" t="n">
-        <v>-58.448993</v>
+        <v>-58.495482</v>
       </c>
       <c r="N48" t="n">
-        <v>-34.564383</v>
+        <v>-34.552614</v>
       </c>
       <c r="O48" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P48" t="inlineStr">
@@ -4082,7 +4082,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>6437</t>
+          <t>6538</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
@@ -4092,7 +4092,7 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>MILLER 4590</t>
+          <t>Pedraza Manuela 4101</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
@@ -4102,7 +4102,7 @@
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>808400306</t>
+          <t>808400353</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
@@ -4117,7 +4117,7 @@
       </c>
       <c r="H49" t="inlineStr">
         <is>
-          <t>Columna corroida</t>
+          <t xml:space="preserve">Podrida en la base </t>
         </is>
       </c>
       <c r="I49" t="n">
@@ -4139,10 +4139,10 @@
         </is>
       </c>
       <c r="M49" t="n">
-        <v>-58.495482</v>
+        <v>-58.481569</v>
       </c>
       <c r="N49" t="n">
-        <v>-34.552614</v>
+        <v>-34.559853</v>
       </c>
       <c r="O49" t="inlineStr">
         <is>
@@ -4158,27 +4158,27 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>6538</t>
+          <t>-525</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>7/17/2025</t>
+          <t>7/22/2025</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Pedraza Manuela 4101</t>
+          <t>Zabala 3567</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>808400353</t>
+          <t>808480549</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
@@ -4193,7 +4193,7 @@
       </c>
       <c r="H50" t="inlineStr">
         <is>
-          <t xml:space="preserve">Podrida en la base </t>
+          <t>Corroida en base para recambio</t>
         </is>
       </c>
       <c r="I50" t="n">
@@ -4215,14 +4215,14 @@
         </is>
       </c>
       <c r="M50" t="n">
-        <v>-58.481569</v>
+        <v>-58.457492</v>
       </c>
       <c r="N50" t="n">
-        <v>-34.559853</v>
+        <v>-34.579336</v>
       </c>
       <c r="O50" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P50" t="inlineStr">
@@ -4234,27 +4234,27 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>-525</t>
+          <t>6484</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>7/22/2025</t>
+          <t>7/24/2025</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Zabala 3567</t>
+          <t>URIARTE 2396</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>808480549</t>
+          <t>808509373</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
@@ -4269,7 +4269,7 @@
       </c>
       <c r="H51" t="inlineStr">
         <is>
-          <t>Corroida en base para recambio</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I51" t="n">
@@ -4291,36 +4291,36 @@
         </is>
       </c>
       <c r="M51" t="n">
-        <v>-58.457492</v>
+        <v>-58.423934</v>
       </c>
       <c r="N51" t="n">
-        <v>-34.579336</v>
+        <v>-34.581562</v>
       </c>
       <c r="O51" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P51" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>6484</t>
+          <t>6512</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>7/24/2025</t>
+          <t>7/28/2025</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>URIARTE 2396</t>
+          <t>GASCON 1195</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
@@ -4330,7 +4330,7 @@
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>808509373</t>
+          <t>808571975</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
@@ -4367,10 +4367,10 @@
         </is>
       </c>
       <c r="M52" t="n">
-        <v>-58.423934</v>
+        <v>-58.423127</v>
       </c>
       <c r="N52" t="n">
-        <v>-34.581562</v>
+        <v>-34.596476</v>
       </c>
       <c r="O52" t="inlineStr">
         <is>
@@ -4386,7 +4386,7 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>6512</t>
+          <t>6513</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
@@ -4396,7 +4396,7 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>GASCON 1195</t>
+          <t>DORREGO 1925</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
@@ -4406,7 +4406,7 @@
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>808571975</t>
+          <t>808571976</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
@@ -4443,10 +4443,10 @@
         </is>
       </c>
       <c r="M53" t="n">
-        <v>-58.423127</v>
+        <v>-58.441281</v>
       </c>
       <c r="N53" t="n">
-        <v>-34.596476</v>
+        <v>-34.579867</v>
       </c>
       <c r="O53" t="inlineStr">
         <is>
@@ -4462,7 +4462,7 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>6513</t>
+          <t>6519</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
@@ -4472,7 +4472,7 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>DORREGO 1925</t>
+          <t>SALGUERO, JERONIMO 2874</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
@@ -4482,7 +4482,7 @@
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>808571976</t>
+          <t>808571977</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
@@ -4497,7 +4497,7 @@
       </c>
       <c r="H54" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Reparar rienda</t>
         </is>
       </c>
       <c r="I54" t="n">
@@ -4505,7 +4505,7 @@
       </c>
       <c r="J54" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Tensor</t>
         </is>
       </c>
       <c r="K54" t="inlineStr">
@@ -4515,14 +4515,14 @@
       </c>
       <c r="L54" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M54" t="n">
-        <v>-58.441281</v>
+        <v>-58.407256</v>
       </c>
       <c r="N54" t="n">
-        <v>-34.579867</v>
+        <v>-34.578976</v>
       </c>
       <c r="O54" t="inlineStr">
         <is>
@@ -4538,27 +4538,27 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>6519</t>
+          <t>-538</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>7/28/2025</t>
+          <t>7/31/2025</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>SALGUERO, JERONIMO 2874</t>
+          <t>Malabia 964</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>808571977</t>
+          <t>808609237</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
@@ -4573,7 +4573,7 @@
       </c>
       <c r="H55" t="inlineStr">
         <is>
-          <t>Reparar rienda</t>
+          <t>Cambiar poste mal estado por PRFV</t>
         </is>
       </c>
       <c r="I55" t="n">
@@ -4581,7 +4581,7 @@
       </c>
       <c r="J55" t="inlineStr">
         <is>
-          <t>Tensor</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K55" t="inlineStr">
@@ -4591,14 +4591,14 @@
       </c>
       <c r="L55" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M55" t="n">
-        <v>-58.407256</v>
+        <v>-58.433634</v>
       </c>
       <c r="N55" t="n">
-        <v>-34.578976</v>
+        <v>-34.595018</v>
       </c>
       <c r="O55" t="inlineStr">
         <is>
@@ -4614,17 +4614,17 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>-538</t>
+          <t>6545</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>7/31/2025</t>
+          <t>8/4/2025</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>Malabia 964</t>
+          <t>SCALABRINI ORTIZ, RAUL AV. 708</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
@@ -4634,7 +4634,7 @@
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>808609237</t>
+          <t>808703864</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
@@ -4649,7 +4649,7 @@
       </c>
       <c r="H56" t="inlineStr">
         <is>
-          <t>Cambiar poste mal estado por PRFV</t>
+          <t>Aplomar</t>
         </is>
       </c>
       <c r="I56" t="n">
@@ -4657,7 +4657,7 @@
       </c>
       <c r="J56" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K56" t="inlineStr">
@@ -4667,14 +4667,14 @@
       </c>
       <c r="L56" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M56" t="n">
-        <v>-58.433634</v>
+        <v>-58.434339</v>
       </c>
       <c r="N56" t="n">
-        <v>-34.595018</v>
+        <v>-34.59693</v>
       </c>
       <c r="O56" t="inlineStr">
         <is>
@@ -4690,27 +4690,27 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>6545</t>
+          <t>6498</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>8/4/2025</t>
+          <t>8/6/2025</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>SCALABRINI ORTIZ, RAUL AV. 708</t>
+          <t>BUCARELLI 2087</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>808703864</t>
+          <t>808733908</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
@@ -4725,7 +4725,7 @@
       </c>
       <c r="H57" t="inlineStr">
         <is>
-          <t>Aplomar</t>
+          <t>Base picada</t>
         </is>
       </c>
       <c r="I57" t="n">
@@ -4733,7 +4733,7 @@
       </c>
       <c r="J57" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K57" t="inlineStr">
@@ -4747,26 +4747,26 @@
         </is>
       </c>
       <c r="M57" t="n">
-        <v>-58.434339</v>
+        <v>-58.485592</v>
       </c>
       <c r="N57" t="n">
-        <v>-34.59693</v>
+        <v>-34.578586</v>
       </c>
       <c r="O57" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P57" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>6498</t>
+          <t>-547</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
@@ -4776,17 +4776,17 @@
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>BUCARELLI 2087</t>
+          <t>Habana 4210</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>808733908</t>
+          <t>808733921</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
@@ -4801,7 +4801,7 @@
       </c>
       <c r="H58" t="inlineStr">
         <is>
-          <t>Base picada</t>
+          <t>Cambiar poste dañado</t>
         </is>
       </c>
       <c r="I58" t="n">
@@ -4819,14 +4819,14 @@
       </c>
       <c r="L58" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M58" t="n">
-        <v>-58.485592</v>
+        <v>-58.515873</v>
       </c>
       <c r="N58" t="n">
-        <v>-34.578586</v>
+        <v>-34.599425</v>
       </c>
       <c r="O58" t="inlineStr">
         <is>
@@ -4842,27 +4842,27 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>-547</t>
+          <t>6579</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>8/6/2025</t>
+          <t>8/7/2025</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>Habana 4210</t>
+          <t>RIVADAVIA MARTIN, COMODORO 1350</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>808733921</t>
+          <t>808749184</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
@@ -4877,7 +4877,7 @@
       </c>
       <c r="H59" t="inlineStr">
         <is>
-          <t>Cambiar poste dañado</t>
+          <t>Poste inclinado</t>
         </is>
       </c>
       <c r="I59" t="n">
@@ -4885,7 +4885,7 @@
       </c>
       <c r="J59" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K59" t="inlineStr">
@@ -4899,14 +4899,14 @@
         </is>
       </c>
       <c r="M59" t="n">
-        <v>-58.515873</v>
+        <v>-58.461024</v>
       </c>
       <c r="N59" t="n">
-        <v>-34.599425</v>
+        <v>-34.539409</v>
       </c>
       <c r="O59" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P59" t="inlineStr">
@@ -4918,27 +4918,27 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>6579</t>
+          <t>6906</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>8/7/2025</t>
+          <t>8/12/2025</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>RIVADAVIA MARTIN, COMODORO 1350</t>
+          <t>MOSCONI GENERAL AV. 3163</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>808749184</t>
+          <t>808918685</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
@@ -4953,7 +4953,7 @@
       </c>
       <c r="H60" t="inlineStr">
         <is>
-          <t>Poste inclinado</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I60" t="n">
@@ -4961,7 +4961,7 @@
       </c>
       <c r="J60" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K60" t="inlineStr">
@@ -4971,18 +4971,18 @@
       </c>
       <c r="L60" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M60" t="n">
-        <v>-58.461024</v>
+        <v>-58.505731</v>
       </c>
       <c r="N60" t="n">
-        <v>-34.539409</v>
+        <v>-34.588316</v>
       </c>
       <c r="O60" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P60" t="inlineStr">
@@ -4994,7 +4994,7 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>6906</t>
+          <t>6910</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
@@ -5004,17 +5004,17 @@
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>MOSCONI GENERAL AV. 3163</t>
+          <t>RIVAS, GRAL. 2345</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>808918685</t>
+          <t>808918698</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
@@ -5029,7 +5029,7 @@
       </c>
       <c r="H61" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I61" t="n">
@@ -5051,10 +5051,10 @@
         </is>
       </c>
       <c r="M61" t="n">
-        <v>-58.505731</v>
+        <v>-58.482497</v>
       </c>
       <c r="N61" t="n">
-        <v>-34.588316</v>
+        <v>-34.598714</v>
       </c>
       <c r="O61" t="inlineStr">
         <is>
@@ -5070,7 +5070,7 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>6910</t>
+          <t>6928</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
@@ -5080,17 +5080,17 @@
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>RIVAS, GRAL. 2345</t>
+          <t>ALBARELLOS AV. 3101</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>808918698</t>
+          <t>808918710</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
@@ -5105,7 +5105,7 @@
       </c>
       <c r="H62" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I62" t="n">
@@ -5127,10 +5127,10 @@
         </is>
       </c>
       <c r="M62" t="n">
-        <v>-58.482497</v>
+        <v>-58.512623</v>
       </c>
       <c r="N62" t="n">
-        <v>-34.598714</v>
+        <v>-34.579137</v>
       </c>
       <c r="O62" t="inlineStr">
         <is>
@@ -5146,7 +5146,7 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>6928</t>
+          <t>6939</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
@@ -5156,7 +5156,7 @@
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>ALBARELLOS AV. 3101</t>
+          <t>ANDONAEGUI 1894</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
@@ -5166,7 +5166,7 @@
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>808918710</t>
+          <t>808918715</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
@@ -5181,7 +5181,7 @@
       </c>
       <c r="H63" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I63" t="n">
@@ -5203,10 +5203,10 @@
         </is>
       </c>
       <c r="M63" t="n">
-        <v>-58.512623</v>
+        <v>-58.484848</v>
       </c>
       <c r="N63" t="n">
-        <v>-34.579137</v>
+        <v>-34.581325</v>
       </c>
       <c r="O63" t="inlineStr">
         <is>
@@ -5222,7 +5222,7 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>6939</t>
+          <t>-550</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
@@ -5232,17 +5232,17 @@
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>ANDONAEGUI 1894</t>
+          <t>Fitz roy 267</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>808918715</t>
+          <t>808918720</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
@@ -5257,7 +5257,7 @@
       </c>
       <c r="H64" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>Aplomar columna</t>
         </is>
       </c>
       <c r="I64" t="n">
@@ -5279,10 +5279,10 @@
         </is>
       </c>
       <c r="M64" t="n">
-        <v>-58.484848</v>
+        <v>-58.451378</v>
       </c>
       <c r="N64" t="n">
-        <v>-34.581325</v>
+        <v>-34.596195</v>
       </c>
       <c r="O64" t="inlineStr">
         <is>
@@ -5298,27 +5298,27 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>-550</t>
+          <t>6943</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>8/12/2025</t>
+          <t>8/14/2025</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>Fitz roy 267</t>
+          <t>SUPERI 1459</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>808918720</t>
+          <t>808972965</t>
         </is>
       </c>
       <c r="F65" t="inlineStr">
@@ -5333,7 +5333,7 @@
       </c>
       <c r="H65" t="inlineStr">
         <is>
-          <t>Aplomar columna</t>
+          <t>Poste con base quebrada ver si es posible desmonte</t>
         </is>
       </c>
       <c r="I65" t="n">
@@ -5341,7 +5341,7 @@
       </c>
       <c r="J65" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Desmonte</t>
         </is>
       </c>
       <c r="K65" t="inlineStr">
@@ -5351,18 +5351,18 @@
       </c>
       <c r="L65" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M65" t="n">
-        <v>-58.451378</v>
+        <v>-58.460834</v>
       </c>
       <c r="N65" t="n">
-        <v>-34.596195</v>
+        <v>-34.573753</v>
       </c>
       <c r="O65" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P65" t="inlineStr">
@@ -5374,7 +5374,7 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>6943</t>
+          <t>6944</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
@@ -5384,17 +5384,17 @@
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>SUPERI 1459</t>
+          <t>RAVIGNANI, EMILIO, DR. 2040</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>808972965</t>
+          <t>808972970</t>
         </is>
       </c>
       <c r="F66" t="inlineStr">
@@ -5409,7 +5409,7 @@
       </c>
       <c r="H66" t="inlineStr">
         <is>
-          <t>Poste con base quebrada ver si es posible desmonte</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I66" t="n">
@@ -5417,7 +5417,7 @@
       </c>
       <c r="J66" t="inlineStr">
         <is>
-          <t>Desmonte</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K66" t="inlineStr">
@@ -5427,30 +5427,30 @@
       </c>
       <c r="L66" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M66" t="n">
-        <v>-58.460834</v>
+        <v>-58.436264</v>
       </c>
       <c r="N66" t="n">
-        <v>-34.573753</v>
+        <v>-34.578942</v>
       </c>
       <c r="O66" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P66" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>6944</t>
+          <t>6969</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
@@ -5460,7 +5460,7 @@
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>RAVIGNANI, EMILIO, DR. 2040</t>
+          <t>CIUDAD DE LA PAZ 295</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
@@ -5470,7 +5470,7 @@
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>808972970</t>
+          <t>808972995</t>
         </is>
       </c>
       <c r="F67" t="inlineStr">
@@ -5485,7 +5485,7 @@
       </c>
       <c r="H67" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I67" t="n">
@@ -5503,14 +5503,14 @@
       </c>
       <c r="L67" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M67" t="n">
-        <v>-58.436264</v>
+        <v>-58.441171</v>
       </c>
       <c r="N67" t="n">
-        <v>-34.578942</v>
+        <v>-34.574547</v>
       </c>
       <c r="O67" t="inlineStr">
         <is>
@@ -5526,7 +5526,7 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>6969</t>
+          <t>6971</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
@@ -5536,7 +5536,7 @@
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>CIUDAD DE LA PAZ 295</t>
+          <t>MAURE 1594</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
@@ -5546,7 +5546,7 @@
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>808972995</t>
+          <t>808973001</t>
         </is>
       </c>
       <c r="F68" t="inlineStr">
@@ -5561,7 +5561,7 @@
       </c>
       <c r="H68" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>Ver de traspasar a telecentro y  desmontar ver con inspector</t>
         </is>
       </c>
       <c r="I68" t="n">
@@ -5583,10 +5583,10 @@
         </is>
       </c>
       <c r="M68" t="n">
-        <v>-58.441171</v>
+        <v>-58.435072</v>
       </c>
       <c r="N68" t="n">
-        <v>-34.574547</v>
+        <v>-34.565732</v>
       </c>
       <c r="O68" t="inlineStr">
         <is>
@@ -5594,82 +5594,6 @@
         </is>
       </c>
       <c r="P68" t="inlineStr">
-        <is>
-          <t>Capital Sur</t>
-        </is>
-      </c>
-    </row>
-    <row r="69">
-      <c r="A69" t="inlineStr">
-        <is>
-          <t>6971</t>
-        </is>
-      </c>
-      <c r="B69" t="inlineStr">
-        <is>
-          <t>8/14/2025</t>
-        </is>
-      </c>
-      <c r="C69" t="inlineStr">
-        <is>
-          <t>MAURE 1594</t>
-        </is>
-      </c>
-      <c r="D69" t="inlineStr">
-        <is>
-          <t>14</t>
-        </is>
-      </c>
-      <c r="E69" t="inlineStr">
-        <is>
-          <t>808973001</t>
-        </is>
-      </c>
-      <c r="F69" t="inlineStr">
-        <is>
-          <t>NEW</t>
-        </is>
-      </c>
-      <c r="G69" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H69" t="inlineStr">
-        <is>
-          <t>Ver de traspasar a telecentro y  desmontar ver con inspector</t>
-        </is>
-      </c>
-      <c r="I69" t="n">
-        <v>1</v>
-      </c>
-      <c r="J69" t="inlineStr">
-        <is>
-          <t>Cambio</t>
-        </is>
-      </c>
-      <c r="K69" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L69" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
-      <c r="M69" t="n">
-        <v>-58.435072</v>
-      </c>
-      <c r="N69" t="n">
-        <v>-34.565732</v>
-      </c>
-      <c r="O69" t="inlineStr">
-        <is>
-          <t>Palermo</t>
-        </is>
-      </c>
-      <c r="P69" t="inlineStr">
         <is>
           <t>Capital Sur</t>
         </is>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-08-21 08:06:57)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_NEW.xlsx
+++ b/mapa_interactivo_NEW.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P68"/>
+  <dimension ref="A1:P70"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -594,17 +594,17 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>3839</t>
+          <t>5589</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>10/23/2024</t>
+          <t>12/31/2023</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>PICO 1511</t>
+          <t>ARCOS 1520</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -614,7 +614,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>798390296</t>
+          <t>799540526</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -624,41 +624,41 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>Poste inclinado</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M3" t="n">
-        <v>-58.465596</v>
+        <v>-58.449125</v>
       </c>
       <c r="N3" t="n">
-        <v>-34.53627</v>
+        <v>-34.565958</v>
       </c>
       <c r="O3" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P3" t="inlineStr">
@@ -670,27 +670,27 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>801645368</t>
+          <t>4862</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>12/13/2024</t>
+          <t>1/23/2025</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>San Blas 1809</t>
+          <t>ARCOS 2263</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>801645368</t>
+          <t>802857379</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -700,12 +700,12 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>picada</t>
         </is>
       </c>
       <c r="I4" t="n">
@@ -718,7 +718,7 @@
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
@@ -727,14 +727,14 @@
         </is>
       </c>
       <c r="M4" t="n">
-        <v>-58.467767</v>
+        <v>-58.455082</v>
       </c>
       <c r="N4" t="n">
-        <v>-34.604588</v>
+        <v>-34.558883</v>
       </c>
       <c r="O4" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P4" t="inlineStr">
@@ -746,17 +746,17 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>5589</t>
+          <t>3839</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>12/31/2023</t>
+          <t>10/23/2024</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>ARCOS 1520</t>
+          <t>PICO 1511</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -766,7 +766,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>799540526</t>
+          <t>798390296</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -776,41 +776,41 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
+          <t>Pendiente</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Poste inclinado</t>
         </is>
       </c>
       <c r="I5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M5" t="n">
-        <v>-58.449125</v>
+        <v>-58.465596</v>
       </c>
       <c r="N5" t="n">
-        <v>-34.565958</v>
+        <v>-34.53627</v>
       </c>
       <c r="O5" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P5" t="inlineStr">
@@ -822,27 +822,27 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>4595</t>
+          <t>801645368</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>1/15/2025</t>
+          <t>12/13/2024</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>PAROISSIEN 1806</t>
+          <t>San Blas 1809</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>802747617</t>
+          <t>801645368</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -857,15 +857,15 @@
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>Aplomar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
@@ -875,18 +875,18 @@
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M6" t="n">
-        <v>-58.464172</v>
+        <v>-58.467767</v>
       </c>
       <c r="N6" t="n">
-        <v>-34.543845</v>
+        <v>-34.604588</v>
       </c>
       <c r="O6" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P6" t="inlineStr">
@@ -898,27 +898,27 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>4662</t>
+          <t>4595</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>1/21/2025</t>
+          <t>1/15/2025</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>ALTOLAGUIRRE 2397</t>
+          <t>PAROISSIEN 1806</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>802823938</t>
+          <t>802747617</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -933,7 +933,7 @@
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>Inclinada</t>
+          <t>Aplomar</t>
         </is>
       </c>
       <c r="I7" t="n">
@@ -951,18 +951,18 @@
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M7" t="n">
-        <v>-58.490766</v>
+        <v>-58.464172</v>
       </c>
       <c r="N7" t="n">
-        <v>-34.576987</v>
+        <v>-34.543845</v>
       </c>
       <c r="O7" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P7" t="inlineStr">
@@ -974,27 +974,27 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>4862</t>
+          <t>4662</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>1/23/2025</t>
+          <t>1/21/2025</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>ARCOS 2263</t>
+          <t>ALTOLAGUIRRE 2397</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>802857379</t>
+          <t>802823938</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -1004,25 +1004,25 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
+          <t>Pendiente</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>picada</t>
+          <t>Inclinada</t>
         </is>
       </c>
       <c r="I8" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L8" t="inlineStr">
@@ -1031,14 +1031,14 @@
         </is>
       </c>
       <c r="M8" t="n">
-        <v>-58.455082</v>
+        <v>-58.490766</v>
       </c>
       <c r="N8" t="n">
-        <v>-34.558883</v>
+        <v>-34.576987</v>
       </c>
       <c r="O8" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P8" t="inlineStr">
@@ -5596,6 +5596,158 @@
       <c r="P68" t="inlineStr">
         <is>
           <t>Capital Sur</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>7000</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>8/20/2025</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>SCALABRINI ORTIZ, RAUL AV. 2106</t>
+        </is>
+      </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>14</t>
+        </is>
+      </c>
+      <c r="E69" t="inlineStr">
+        <is>
+          <t>809065867</t>
+        </is>
+      </c>
+      <c r="F69" t="inlineStr">
+        <is>
+          <t>NEW</t>
+        </is>
+      </c>
+      <c r="G69" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H69" t="inlineStr">
+        <is>
+          <t>Picada</t>
+        </is>
+      </c>
+      <c r="I69" t="n">
+        <v>1</v>
+      </c>
+      <c r="J69" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K69" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L69" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M69" t="n">
+        <v>-58.420109</v>
+      </c>
+      <c r="N69" t="n">
+        <v>-34.58764</v>
+      </c>
+      <c r="O69" t="inlineStr">
+        <is>
+          <t>Palermo</t>
+        </is>
+      </c>
+      <c r="P69" t="inlineStr">
+        <is>
+          <t>Capital Sur</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>7003</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>8/20/2025</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>MELIAN AV. 2576</t>
+        </is>
+      </c>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="E70" t="inlineStr">
+        <is>
+          <t>809065874</t>
+        </is>
+      </c>
+      <c r="F70" t="inlineStr">
+        <is>
+          <t>NEW</t>
+        </is>
+      </c>
+      <c r="G70" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H70" t="inlineStr">
+        <is>
+          <t>Picada</t>
+        </is>
+      </c>
+      <c r="I70" t="n">
+        <v>1</v>
+      </c>
+      <c r="J70" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K70" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L70" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M70" t="n">
+        <v>-58.471943</v>
+      </c>
+      <c r="N70" t="n">
+        <v>-34.564948</v>
+      </c>
+      <c r="O70" t="inlineStr">
+        <is>
+          <t>Colegiales</t>
+        </is>
+      </c>
+      <c r="P70" t="inlineStr">
+        <is>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-08-22 08:55:17)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_NEW.xlsx
+++ b/mapa_interactivo_NEW.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P70"/>
+  <dimension ref="A1:P72"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -594,17 +594,17 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>5589</t>
+          <t>3839</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>12/31/2023</t>
+          <t>10/23/2024</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>ARCOS 1520</t>
+          <t>PICO 1511</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -614,7 +614,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>799540526</t>
+          <t>798390296</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -624,41 +624,41 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
+          <t>Pendiente</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Poste inclinado</t>
         </is>
       </c>
       <c r="I3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M3" t="n">
-        <v>-58.449125</v>
+        <v>-58.465596</v>
       </c>
       <c r="N3" t="n">
-        <v>-34.565958</v>
+        <v>-34.53627</v>
       </c>
       <c r="O3" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P3" t="inlineStr">
@@ -670,27 +670,27 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>4862</t>
+          <t>801645368</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>1/23/2025</t>
+          <t>12/13/2024</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>ARCOS 2263</t>
+          <t>San Blas 1809</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>802857379</t>
+          <t>801645368</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -700,12 +700,12 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
+          <t>Pendiente</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>picada</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I4" t="n">
@@ -718,7 +718,7 @@
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
@@ -727,14 +727,14 @@
         </is>
       </c>
       <c r="M4" t="n">
-        <v>-58.455082</v>
+        <v>-58.467767</v>
       </c>
       <c r="N4" t="n">
-        <v>-34.558883</v>
+        <v>-34.604588</v>
       </c>
       <c r="O4" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P4" t="inlineStr">
@@ -746,17 +746,17 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>3839</t>
+          <t>5589</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>10/23/2024</t>
+          <t>12/31/2023</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>PICO 1511</t>
+          <t>ARCOS 1520</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -766,7 +766,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>798390296</t>
+          <t>799540526</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -776,41 +776,41 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>Poste inclinado</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M5" t="n">
-        <v>-58.465596</v>
+        <v>-58.449125</v>
       </c>
       <c r="N5" t="n">
-        <v>-34.53627</v>
+        <v>-34.565958</v>
       </c>
       <c r="O5" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P5" t="inlineStr">
@@ -822,27 +822,27 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>801645368</t>
+          <t>4595</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>12/13/2024</t>
+          <t>1/15/2025</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>San Blas 1809</t>
+          <t>PAROISSIEN 1806</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>801645368</t>
+          <t>802747617</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -857,15 +857,15 @@
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Aplomar</t>
         </is>
       </c>
       <c r="I6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
@@ -875,18 +875,18 @@
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M6" t="n">
-        <v>-58.467767</v>
+        <v>-58.464172</v>
       </c>
       <c r="N6" t="n">
-        <v>-34.604588</v>
+        <v>-34.543845</v>
       </c>
       <c r="O6" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P6" t="inlineStr">
@@ -898,27 +898,27 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>4595</t>
+          <t>4662</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>1/15/2025</t>
+          <t>1/21/2025</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>PAROISSIEN 1806</t>
+          <t>ALTOLAGUIRRE 2397</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>802747617</t>
+          <t>802823938</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -933,7 +933,7 @@
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>Aplomar</t>
+          <t>Inclinada</t>
         </is>
       </c>
       <c r="I7" t="n">
@@ -951,18 +951,18 @@
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M7" t="n">
-        <v>-58.464172</v>
+        <v>-58.490766</v>
       </c>
       <c r="N7" t="n">
-        <v>-34.543845</v>
+        <v>-34.576987</v>
       </c>
       <c r="O7" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P7" t="inlineStr">
@@ -974,27 +974,27 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>4662</t>
+          <t>4862</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>1/21/2025</t>
+          <t>1/23/2025</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>ALTOLAGUIRRE 2397</t>
+          <t>ARCOS 2263</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>802823938</t>
+          <t>802857379</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -1004,25 +1004,25 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>Inclinada</t>
+          <t>picada</t>
         </is>
       </c>
       <c r="I8" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L8" t="inlineStr">
@@ -1031,14 +1031,14 @@
         </is>
       </c>
       <c r="M8" t="n">
-        <v>-58.490766</v>
+        <v>-58.455082</v>
       </c>
       <c r="N8" t="n">
-        <v>-34.576987</v>
+        <v>-34.558883</v>
       </c>
       <c r="O8" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P8" t="inlineStr">
@@ -5746,6 +5746,158 @@
         </is>
       </c>
       <c r="P70" t="inlineStr">
+        <is>
+          <t>Capital Norte</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>-558</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>8/21/2025</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>Blanco Encalada 4210</t>
+        </is>
+      </c>
+      <c r="D71" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="E71" t="inlineStr">
+        <is>
+          <t>Pendiente ADM</t>
+        </is>
+      </c>
+      <c r="F71" t="inlineStr">
+        <is>
+          <t>NEW</t>
+        </is>
+      </c>
+      <c r="G71" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H71" t="inlineStr">
+        <is>
+          <t>Colocar columna R400 para pedir taspaso de fuente telecom</t>
+        </is>
+      </c>
+      <c r="I71" t="n">
+        <v>1</v>
+      </c>
+      <c r="J71" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K71" t="inlineStr">
+        <is>
+          <t>Fuente Teco</t>
+        </is>
+      </c>
+      <c r="L71" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M71" t="n">
+        <v>-58.477593</v>
+      </c>
+      <c r="N71" t="n">
+        <v>-34.570321</v>
+      </c>
+      <c r="O71" t="inlineStr">
+        <is>
+          <t>Colegiales</t>
+        </is>
+      </c>
+      <c r="P71" t="inlineStr">
+        <is>
+          <t>Capital Norte</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>-559</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>8/21/2025</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>Av. Del Libertador 6736</t>
+        </is>
+      </c>
+      <c r="D72" t="inlineStr">
+        <is>
+          <t>13</t>
+        </is>
+      </c>
+      <c r="E72" t="inlineStr">
+        <is>
+          <t>809098713</t>
+        </is>
+      </c>
+      <c r="F72" t="inlineStr">
+        <is>
+          <t>NEW</t>
+        </is>
+      </c>
+      <c r="G72" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H72" t="inlineStr">
+        <is>
+          <t>Picada</t>
+        </is>
+      </c>
+      <c r="I72" t="n">
+        <v>1</v>
+      </c>
+      <c r="J72" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K72" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L72" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M72" t="n">
+        <v>-58.453398</v>
+      </c>
+      <c r="N72" t="n">
+        <v>-34.550238</v>
+      </c>
+      <c r="O72" t="inlineStr">
+        <is>
+          <t>Saavedra</t>
+        </is>
+      </c>
+      <c r="P72" t="inlineStr">
         <is>
           <t>Capital Norte</t>
         </is>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-08-25 08:01:30)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_NEW.xlsx
+++ b/mapa_interactivo_NEW.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P72"/>
+  <dimension ref="A1:P74"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5774,7 +5774,7 @@
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>Pendiente ADM</t>
+          <t>ICD30461848</t>
         </is>
       </c>
       <c r="F71" t="inlineStr">
@@ -5898,6 +5898,158 @@
         </is>
       </c>
       <c r="P72" t="inlineStr">
+        <is>
+          <t>Capital Norte</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>5467</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>8/22/2025</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>FRANCO 2515</t>
+        </is>
+      </c>
+      <c r="D73" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="E73" t="inlineStr">
+        <is>
+          <t>809102560</t>
+        </is>
+      </c>
+      <c r="F73" t="inlineStr">
+        <is>
+          <t>NEW</t>
+        </is>
+      </c>
+      <c r="G73" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H73" t="inlineStr">
+        <is>
+          <t>PIcada</t>
+        </is>
+      </c>
+      <c r="I73" t="n">
+        <v>1</v>
+      </c>
+      <c r="J73" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K73" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L73" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M73" t="n">
+        <v>-58.502342</v>
+      </c>
+      <c r="N73" t="n">
+        <v>-34.578839</v>
+      </c>
+      <c r="O73" t="inlineStr">
+        <is>
+          <t>Paternal</t>
+        </is>
+      </c>
+      <c r="P73" t="inlineStr">
+        <is>
+          <t>Capital Norte</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>5503</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>8/22/2025</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>CRAMER AV. 1771</t>
+        </is>
+      </c>
+      <c r="D74" t="inlineStr">
+        <is>
+          <t>13</t>
+        </is>
+      </c>
+      <c r="E74" t="inlineStr">
+        <is>
+          <t>809102564</t>
+        </is>
+      </c>
+      <c r="F74" t="inlineStr">
+        <is>
+          <t>NEW</t>
+        </is>
+      </c>
+      <c r="G74" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H74" t="inlineStr">
+        <is>
+          <t>PIcada</t>
+        </is>
+      </c>
+      <c r="I74" t="n">
+        <v>1</v>
+      </c>
+      <c r="J74" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K74" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L74" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M74" t="n">
+        <v>-58.458506</v>
+      </c>
+      <c r="N74" t="n">
+        <v>-34.56783</v>
+      </c>
+      <c r="O74" t="inlineStr">
+        <is>
+          <t>Colegiales</t>
+        </is>
+      </c>
+      <c r="P74" t="inlineStr">
         <is>
           <t>Capital Norte</t>
         </is>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-08-25 12:54:00)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_NEW.xlsx
+++ b/mapa_interactivo_NEW.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P74"/>
+  <dimension ref="A1:P75"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4158,7 +4158,7 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>-525</t>
+          <t>7023</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
@@ -4168,7 +4168,7 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Zabala 3567</t>
+          <t>ZABALA 3573</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
@@ -4215,10 +4215,10 @@
         </is>
       </c>
       <c r="M50" t="n">
-        <v>-58.457492</v>
+        <v>-58.457522</v>
       </c>
       <c r="N50" t="n">
-        <v>-34.579336</v>
+        <v>-34.579414</v>
       </c>
       <c r="O50" t="inlineStr">
         <is>
@@ -6052,6 +6052,82 @@
       <c r="P74" t="inlineStr">
         <is>
           <t>Capital Norte</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>7021</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>8/25/2025</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>VERA 445</t>
+        </is>
+      </c>
+      <c r="D75" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="E75" t="inlineStr">
+        <is>
+          <t>809155622</t>
+        </is>
+      </c>
+      <c r="F75" t="inlineStr">
+        <is>
+          <t>NEW</t>
+        </is>
+      </c>
+      <c r="G75" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H75" t="inlineStr">
+        <is>
+          <t>Picada</t>
+        </is>
+      </c>
+      <c r="I75" t="n">
+        <v>1</v>
+      </c>
+      <c r="J75" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K75" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L75" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M75" t="n">
+        <v>-58.437181</v>
+      </c>
+      <c r="N75" t="n">
+        <v>-34.5995</v>
+      </c>
+      <c r="O75" t="inlineStr">
+        <is>
+          <t>Palermo</t>
+        </is>
+      </c>
+      <c r="P75" t="inlineStr">
+        <is>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-08-26 10:32:58)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_NEW.xlsx
+++ b/mapa_interactivo_NEW.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P75"/>
+  <dimension ref="A1:P76"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6131,6 +6131,82 @@
         </is>
       </c>
     </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>-567</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>8/25/2025</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>Franco 2543</t>
+        </is>
+      </c>
+      <c r="D76" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="E76" t="inlineStr">
+        <is>
+          <t>809184735</t>
+        </is>
+      </c>
+      <c r="F76" t="inlineStr">
+        <is>
+          <t>NEW</t>
+        </is>
+      </c>
+      <c r="G76" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H76" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="I76" t="n">
+        <v>0</v>
+      </c>
+      <c r="J76" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K76" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L76" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M76" t="n">
+        <v>-58.502565</v>
+      </c>
+      <c r="N76" t="n">
+        <v>-34.578977</v>
+      </c>
+      <c r="O76" t="inlineStr">
+        <is>
+          <t>Paternal</t>
+        </is>
+      </c>
+      <c r="P76" t="inlineStr">
+        <is>
+          <t>Capital Norte</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-08-27 15:04:46)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_NEW.xlsx
+++ b/mapa_interactivo_NEW.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P76"/>
+  <dimension ref="A1:P72"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2486,7 +2486,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>5719</t>
+          <t>6333</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -2496,17 +2496,17 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>CABEZON, JOSE LEON 2440</t>
+          <t>ORTEGA Y GASSET 1816</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>805579157</t>
+          <t>805655342</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
@@ -2543,36 +2543,36 @@
         </is>
       </c>
       <c r="M28" t="n">
-        <v>-58.499967</v>
+        <v>-58.432556</v>
       </c>
       <c r="N28" t="n">
-        <v>-34.57974</v>
+        <v>-34.570279</v>
       </c>
       <c r="O28" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P28" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>6333</t>
+          <t>805707165</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>5/1/2025</t>
+          <t>5/7/2025</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>ORTEGA Y GASSET 1816</t>
+          <t>Baez 793</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
@@ -2582,7 +2582,7 @@
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>805655342</t>
+          <t>805707165</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
@@ -2597,7 +2597,7 @@
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>DESMONTAR COLUMNA DE 7 MTS Y TRANSFERIR A COMUNITARIA</t>
         </is>
       </c>
       <c r="I29" t="n">
@@ -2615,14 +2615,14 @@
       </c>
       <c r="L29" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M29" t="n">
-        <v>-58.432556</v>
+        <v>-58.436165</v>
       </c>
       <c r="N29" t="n">
-        <v>-34.570279</v>
+        <v>-34.569081</v>
       </c>
       <c r="O29" t="inlineStr">
         <is>
@@ -2638,27 +2638,27 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>805707165</t>
+          <t>5847</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>5/7/2025</t>
+          <t>5/8/2025</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Baez 793</t>
+          <t>JURAMENTO 5321</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>805707165</t>
+          <t>805791839</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
@@ -2673,7 +2673,7 @@
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>DESMONTAR COLUMNA DE 7 MTS Y TRANSFERIR A COMUNITARIA</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I30" t="n">
@@ -2691,50 +2691,50 @@
       </c>
       <c r="L30" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M30" t="n">
-        <v>-58.436165</v>
+        <v>-58.485193</v>
       </c>
       <c r="N30" t="n">
-        <v>-34.569081</v>
+        <v>-34.579621</v>
       </c>
       <c r="O30" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P30" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>5847</t>
+          <t>232</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>5/8/2025</t>
+          <t>5/9/2025</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>JURAMENTO 5321</t>
+          <t>Gorostiaga 2286</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>805791839</t>
+          <t>805791858</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
@@ -2771,46 +2771,46 @@
         </is>
       </c>
       <c r="M31" t="n">
-        <v>-58.485193</v>
+        <v>-58.441563</v>
       </c>
       <c r="N31" t="n">
-        <v>-34.579621</v>
+        <v>-34.569743</v>
       </c>
       <c r="O31" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P31" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>232</t>
+          <t>-406</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>5/9/2025</t>
+          <t>5/8/2025</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Gorostiaga 2286</t>
+          <t>Olof palme 4144</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>805791858</t>
+          <t>805791925</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
@@ -2825,7 +2825,7 @@
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Tensar 2 riendas a pique columna 168</t>
         </is>
       </c>
       <c r="I32" t="n">
@@ -2833,7 +2833,7 @@
       </c>
       <c r="J32" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Tensor</t>
         </is>
       </c>
       <c r="K32" t="inlineStr">
@@ -2843,40 +2843,40 @@
       </c>
       <c r="L32" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M32" t="n">
-        <v>-58.441563</v>
+        <v>-58.488252</v>
       </c>
       <c r="N32" t="n">
-        <v>-34.569743</v>
+        <v>-34.553391</v>
       </c>
       <c r="O32" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P32" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>-406</t>
+          <t>5826</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>5/8/2025</t>
+          <t>5/19/2025</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Olof palme 4144</t>
+          <t>ALBARELLOS AV. 3180</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
@@ -2886,7 +2886,7 @@
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>805791925</t>
+          <t>806926466</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
@@ -2901,7 +2901,7 @@
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>Tensar 2 riendas a pique columna 168</t>
+          <t>Columna (metal) inclinada</t>
         </is>
       </c>
       <c r="I33" t="n">
@@ -2909,7 +2909,7 @@
       </c>
       <c r="J33" t="inlineStr">
         <is>
-          <t>Tensor</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K33" t="inlineStr">
@@ -2923,14 +2923,14 @@
         </is>
       </c>
       <c r="M33" t="n">
-        <v>-58.488252</v>
+        <v>-58.513552</v>
       </c>
       <c r="N33" t="n">
-        <v>-34.553391</v>
+        <v>-34.579829</v>
       </c>
       <c r="O33" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P33" t="inlineStr">
@@ -2942,27 +2942,27 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>5826</t>
+          <t>6020</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>5/19/2025</t>
+          <t>6/5/2025</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>ALBARELLOS AV. 3180</t>
+          <t>RAVIGNANI, EMILIO, DR. 2036</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>806926466</t>
+          <t>807215465</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
@@ -2977,7 +2977,7 @@
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>Columna (metal) inclinada</t>
+          <t>Picada misma que 6260 y 6945</t>
         </is>
       </c>
       <c r="I34" t="n">
@@ -2985,7 +2985,7 @@
       </c>
       <c r="J34" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K34" t="inlineStr">
@@ -2995,50 +2995,50 @@
       </c>
       <c r="L34" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M34" t="n">
-        <v>-58.513552</v>
+        <v>-58.436298</v>
       </c>
       <c r="N34" t="n">
-        <v>-34.579829</v>
+        <v>-34.578972</v>
       </c>
       <c r="O34" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P34" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>6020</t>
+          <t>6144</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>6/5/2025</t>
+          <t>6/11/2025</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>RAVIGNANI, EMILIO, DR. 2036</t>
+          <t>TURIN 2990</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>807215465</t>
+          <t>807458282</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
@@ -3075,26 +3075,26 @@
         </is>
       </c>
       <c r="M35" t="n">
-        <v>-58.436298</v>
+        <v>-58.480925</v>
       </c>
       <c r="N35" t="n">
-        <v>-34.578972</v>
+        <v>-34.585471</v>
       </c>
       <c r="O35" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P35" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>6144</t>
+          <t>6143</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
@@ -3104,7 +3104,7 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>TURIN 2990</t>
+          <t>SOLANO LOPEZ, F., MARISCAL 2845</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
@@ -3114,7 +3114,7 @@
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>807458282</t>
+          <t>807458296</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
@@ -3151,10 +3151,10 @@
         </is>
       </c>
       <c r="M36" t="n">
-        <v>-58.480925</v>
+        <v>-58.495071</v>
       </c>
       <c r="N36" t="n">
-        <v>-34.585471</v>
+        <v>-34.593122</v>
       </c>
       <c r="O36" t="inlineStr">
         <is>
@@ -3170,7 +3170,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>6143</t>
+          <t>6141</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
@@ -3180,17 +3180,17 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>SOLANO LOPEZ, F., MARISCAL 2845</t>
+          <t>EL PAMPERO 2618</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>807458296</t>
+          <t>807458310</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
@@ -3205,7 +3205,7 @@
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Picada info para cierre tambien entro como caso 6911</t>
         </is>
       </c>
       <c r="I37" t="n">
@@ -3227,10 +3227,10 @@
         </is>
       </c>
       <c r="M37" t="n">
-        <v>-58.495071</v>
+        <v>-58.481942</v>
       </c>
       <c r="N37" t="n">
-        <v>-34.593122</v>
+        <v>-34.602989</v>
       </c>
       <c r="O37" t="inlineStr">
         <is>
@@ -3246,17 +3246,17 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>6141</t>
+          <t>-478</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>6/11/2025</t>
+          <t>6/15/2025</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>EL PAMPERO 2618</t>
+          <t>Chivilcoy 4875</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
@@ -3266,7 +3266,7 @@
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>807458310</t>
+          <t>807508509</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
@@ -3281,7 +3281,7 @@
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>Picada info para cierre tambien entro como caso 6911</t>
+          <t>Poste podrido</t>
         </is>
       </c>
       <c r="I38" t="n">
@@ -3299,14 +3299,14 @@
       </c>
       <c r="L38" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M38" t="n">
-        <v>-58.481942</v>
+        <v>-58.517389</v>
       </c>
       <c r="N38" t="n">
-        <v>-34.602989</v>
+        <v>-34.593541</v>
       </c>
       <c r="O38" t="inlineStr">
         <is>
@@ -3322,27 +3322,27 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>-478</t>
+          <t>6171</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>6/15/2025</t>
+          <t>6/18/2025</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Chivilcoy 4875</t>
+          <t>CABELLO 3486</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>807508509</t>
+          <t>807658640</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
@@ -3357,7 +3357,7 @@
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>Poste podrido</t>
+          <t>Columna inclinada evaluar con inspector un corrimiento</t>
         </is>
       </c>
       <c r="I39" t="n">
@@ -3375,40 +3375,40 @@
       </c>
       <c r="L39" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M39" t="n">
-        <v>-58.517389</v>
+        <v>-58.409579</v>
       </c>
       <c r="N39" t="n">
-        <v>-34.593541</v>
+        <v>-34.581134</v>
       </c>
       <c r="O39" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P39" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>6171</t>
+          <t>6230</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>6/18/2025</t>
+          <t>6/24/2025</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>CABELLO 3486</t>
+          <t>Santa maria de oro	2722</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
@@ -3418,7 +3418,7 @@
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>807658640</t>
+          <t>807763066</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
@@ -3433,7 +3433,7 @@
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t>Columna inclinada evaluar con inspector un corrimiento</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I40" t="n">
@@ -3455,10 +3455,10 @@
         </is>
       </c>
       <c r="M40" t="n">
-        <v>-58.409579</v>
+        <v>-58.422315</v>
       </c>
       <c r="N40" t="n">
-        <v>-34.581134</v>
+        <v>-34.576988</v>
       </c>
       <c r="O40" t="inlineStr">
         <is>
@@ -3474,7 +3474,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>6230</t>
+          <t>6231</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
@@ -3484,7 +3484,7 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Santa maria de oro	2722</t>
+          <t>Ciudad de la Paz 275</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
@@ -3494,7 +3494,7 @@
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>807763066</t>
+          <t>807763070</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
@@ -3509,7 +3509,7 @@
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Aplomar o cambiar</t>
         </is>
       </c>
       <c r="I41" t="n">
@@ -3527,14 +3527,14 @@
       </c>
       <c r="L41" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M41" t="n">
-        <v>-58.422315</v>
+        <v>-58.441049</v>
       </c>
       <c r="N41" t="n">
-        <v>-34.576988</v>
+        <v>-34.574625</v>
       </c>
       <c r="O41" t="inlineStr">
         <is>
@@ -3550,7 +3550,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>6231</t>
+          <t>6235</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
@@ -3560,17 +3560,17 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Ciudad de la Paz 275</t>
+          <t>HUERGO 389</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>807763070</t>
+          <t>807763078</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
@@ -3585,7 +3585,7 @@
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>Aplomar o cambiar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I42" t="n">
@@ -3603,14 +3603,14 @@
       </c>
       <c r="L42" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M42" t="n">
-        <v>-58.441049</v>
+        <v>-58.432722</v>
       </c>
       <c r="N42" t="n">
-        <v>-34.574625</v>
+        <v>-34.572371</v>
       </c>
       <c r="O42" t="inlineStr">
         <is>
@@ -3626,27 +3626,27 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>6235</t>
+          <t>6295</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>6/24/2025</t>
+          <t>6/30/2025</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>HUERGO 389</t>
+          <t>SOLER 6017</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>807763078</t>
+          <t>807851636</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
@@ -3683,10 +3683,10 @@
         </is>
       </c>
       <c r="M43" t="n">
-        <v>-58.432722</v>
+        <v>-58.436808</v>
       </c>
       <c r="N43" t="n">
-        <v>-34.572371</v>
+        <v>-34.577464</v>
       </c>
       <c r="O43" t="inlineStr">
         <is>
@@ -3702,17 +3702,17 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>6295</t>
+          <t>6332</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>6/30/2025</t>
+          <t>7/3/2025</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>SOLER 6017</t>
+          <t>ARAOZ 2560</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
@@ -3722,7 +3722,7 @@
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>807851636</t>
+          <t>807965818</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
@@ -3759,10 +3759,10 @@
         </is>
       </c>
       <c r="M44" t="n">
-        <v>-58.436808</v>
+        <v>-58.414507</v>
       </c>
       <c r="N44" t="n">
-        <v>-34.577464</v>
+        <v>-34.585377</v>
       </c>
       <c r="O44" t="inlineStr">
         <is>
@@ -3778,27 +3778,27 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>6332</t>
+          <t>-503</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>7/3/2025</t>
+          <t>7/10/2025</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>ARAOZ 2560</t>
+          <t>Salguero 842</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>807965818</t>
+          <t>808148673</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
@@ -3813,7 +3813,7 @@
       </c>
       <c r="H45" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambiar columna picada en la base</t>
         </is>
       </c>
       <c r="I45" t="n">
@@ -3835,14 +3835,14 @@
         </is>
       </c>
       <c r="M45" t="n">
-        <v>-58.414507</v>
+        <v>-58.419166</v>
       </c>
       <c r="N45" t="n">
-        <v>-34.585377</v>
+        <v>-34.600265</v>
       </c>
       <c r="O45" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P45" t="inlineStr">
@@ -3854,7 +3854,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>-503</t>
+          <t>6506</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
@@ -3864,17 +3864,17 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Salguero 842</t>
+          <t>Ohiggins 1611</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>808148673</t>
+          <t>808148679</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
@@ -3889,7 +3889,7 @@
       </c>
       <c r="H46" t="inlineStr">
         <is>
-          <t>Cambiar columna picada en la base</t>
+          <t>Columna podrida en la base</t>
         </is>
       </c>
       <c r="I46" t="n">
@@ -3902,7 +3902,7 @@
       </c>
       <c r="K46" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L46" t="inlineStr">
@@ -3911,46 +3911,46 @@
         </is>
       </c>
       <c r="M46" t="n">
-        <v>-58.419166</v>
+        <v>-58.448993</v>
       </c>
       <c r="N46" t="n">
-        <v>-34.600265</v>
+        <v>-34.564383</v>
       </c>
       <c r="O46" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P46" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>6506</t>
+          <t>6437</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>7/10/2025</t>
+          <t>7/17/2025</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Ohiggins 1611</t>
+          <t>MILLER 4590</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>808148679</t>
+          <t>808400306</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
@@ -3965,7 +3965,7 @@
       </c>
       <c r="H47" t="inlineStr">
         <is>
-          <t>Columna podrida en la base</t>
+          <t>Columna corroida</t>
         </is>
       </c>
       <c r="I47" t="n">
@@ -3978,7 +3978,7 @@
       </c>
       <c r="K47" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L47" t="inlineStr">
@@ -3987,14 +3987,14 @@
         </is>
       </c>
       <c r="M47" t="n">
-        <v>-58.448993</v>
+        <v>-58.495482</v>
       </c>
       <c r="N47" t="n">
-        <v>-34.564383</v>
+        <v>-34.552614</v>
       </c>
       <c r="O47" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P47" t="inlineStr">
@@ -4006,7 +4006,7 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>6437</t>
+          <t>6538</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
@@ -4016,7 +4016,7 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>MILLER 4590</t>
+          <t>Pedraza Manuela 4101</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
@@ -4026,7 +4026,7 @@
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>808400306</t>
+          <t>808400353</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
@@ -4041,7 +4041,7 @@
       </c>
       <c r="H48" t="inlineStr">
         <is>
-          <t>Columna corroida</t>
+          <t xml:space="preserve">Podrida en la base </t>
         </is>
       </c>
       <c r="I48" t="n">
@@ -4063,10 +4063,10 @@
         </is>
       </c>
       <c r="M48" t="n">
-        <v>-58.495482</v>
+        <v>-58.481569</v>
       </c>
       <c r="N48" t="n">
-        <v>-34.552614</v>
+        <v>-34.559853</v>
       </c>
       <c r="O48" t="inlineStr">
         <is>
@@ -4082,27 +4082,27 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>6538</t>
+          <t>7023</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>7/17/2025</t>
+          <t>7/22/2025</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Pedraza Manuela 4101</t>
+          <t>ZABALA 3573</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>808400353</t>
+          <t>808480549</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
@@ -4117,7 +4117,7 @@
       </c>
       <c r="H49" t="inlineStr">
         <is>
-          <t xml:space="preserve">Podrida en la base </t>
+          <t>Corroida en base para recambio</t>
         </is>
       </c>
       <c r="I49" t="n">
@@ -4139,14 +4139,14 @@
         </is>
       </c>
       <c r="M49" t="n">
-        <v>-58.481569</v>
+        <v>-58.457522</v>
       </c>
       <c r="N49" t="n">
-        <v>-34.559853</v>
+        <v>-34.579414</v>
       </c>
       <c r="O49" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P49" t="inlineStr">
@@ -4158,27 +4158,27 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>7023</t>
+          <t>6484</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>7/22/2025</t>
+          <t>7/24/2025</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>ZABALA 3573</t>
+          <t>URIARTE 2396</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>808480549</t>
+          <t>808509373</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
@@ -4193,7 +4193,7 @@
       </c>
       <c r="H50" t="inlineStr">
         <is>
-          <t>Corroida en base para recambio</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I50" t="n">
@@ -4215,36 +4215,36 @@
         </is>
       </c>
       <c r="M50" t="n">
-        <v>-58.457522</v>
+        <v>-58.423934</v>
       </c>
       <c r="N50" t="n">
-        <v>-34.579414</v>
+        <v>-34.581562</v>
       </c>
       <c r="O50" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P50" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>6484</t>
+          <t>6512</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>7/24/2025</t>
+          <t>7/28/2025</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>URIARTE 2396</t>
+          <t>GASCON 1195</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
@@ -4254,7 +4254,7 @@
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>808509373</t>
+          <t>808571975</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
@@ -4291,10 +4291,10 @@
         </is>
       </c>
       <c r="M51" t="n">
-        <v>-58.423934</v>
+        <v>-58.423127</v>
       </c>
       <c r="N51" t="n">
-        <v>-34.581562</v>
+        <v>-34.596476</v>
       </c>
       <c r="O51" t="inlineStr">
         <is>
@@ -4310,7 +4310,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>6512</t>
+          <t>6513</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
@@ -4320,7 +4320,7 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>GASCON 1195</t>
+          <t>DORREGO 1925</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
@@ -4330,7 +4330,7 @@
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>808571975</t>
+          <t>808571976</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
@@ -4367,10 +4367,10 @@
         </is>
       </c>
       <c r="M52" t="n">
-        <v>-58.423127</v>
+        <v>-58.441281</v>
       </c>
       <c r="N52" t="n">
-        <v>-34.596476</v>
+        <v>-34.579867</v>
       </c>
       <c r="O52" t="inlineStr">
         <is>
@@ -4386,7 +4386,7 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>6513</t>
+          <t>6519</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
@@ -4396,7 +4396,7 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>DORREGO 1925</t>
+          <t>SALGUERO, JERONIMO 2874</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
@@ -4406,7 +4406,7 @@
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>808571976</t>
+          <t>808571977</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
@@ -4421,7 +4421,7 @@
       </c>
       <c r="H53" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Reparar rienda</t>
         </is>
       </c>
       <c r="I53" t="n">
@@ -4429,7 +4429,7 @@
       </c>
       <c r="J53" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Tensor</t>
         </is>
       </c>
       <c r="K53" t="inlineStr">
@@ -4439,14 +4439,14 @@
       </c>
       <c r="L53" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M53" t="n">
-        <v>-58.441281</v>
+        <v>-58.407256</v>
       </c>
       <c r="N53" t="n">
-        <v>-34.579867</v>
+        <v>-34.578976</v>
       </c>
       <c r="O53" t="inlineStr">
         <is>
@@ -4462,27 +4462,27 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>6519</t>
+          <t>-538</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>7/28/2025</t>
+          <t>7/31/2025</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>SALGUERO, JERONIMO 2874</t>
+          <t>Malabia 964</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>808571977</t>
+          <t>808609237</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
@@ -4497,7 +4497,7 @@
       </c>
       <c r="H54" t="inlineStr">
         <is>
-          <t>Reparar rienda</t>
+          <t>Cambiar poste mal estado por PRFV</t>
         </is>
       </c>
       <c r="I54" t="n">
@@ -4505,7 +4505,7 @@
       </c>
       <c r="J54" t="inlineStr">
         <is>
-          <t>Tensor</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K54" t="inlineStr">
@@ -4515,14 +4515,14 @@
       </c>
       <c r="L54" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M54" t="n">
-        <v>-58.407256</v>
+        <v>-58.433634</v>
       </c>
       <c r="N54" t="n">
-        <v>-34.578976</v>
+        <v>-34.595018</v>
       </c>
       <c r="O54" t="inlineStr">
         <is>
@@ -4538,17 +4538,17 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>-538</t>
+          <t>6545</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>7/31/2025</t>
+          <t>8/4/2025</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>Malabia 964</t>
+          <t>SCALABRINI ORTIZ, RAUL AV. 708</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
@@ -4558,7 +4558,7 @@
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>808609237</t>
+          <t>808703864</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
@@ -4573,7 +4573,7 @@
       </c>
       <c r="H55" t="inlineStr">
         <is>
-          <t>Cambiar poste mal estado por PRFV</t>
+          <t>Aplomar</t>
         </is>
       </c>
       <c r="I55" t="n">
@@ -4581,7 +4581,7 @@
       </c>
       <c r="J55" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K55" t="inlineStr">
@@ -4591,14 +4591,14 @@
       </c>
       <c r="L55" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M55" t="n">
-        <v>-58.433634</v>
+        <v>-58.434339</v>
       </c>
       <c r="N55" t="n">
-        <v>-34.595018</v>
+        <v>-34.59693</v>
       </c>
       <c r="O55" t="inlineStr">
         <is>
@@ -4614,27 +4614,27 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>6545</t>
+          <t>6498</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>8/4/2025</t>
+          <t>8/6/2025</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>SCALABRINI ORTIZ, RAUL AV. 708</t>
+          <t>BUCARELLI 2087</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>808703864</t>
+          <t>808733908</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
@@ -4649,7 +4649,7 @@
       </c>
       <c r="H56" t="inlineStr">
         <is>
-          <t>Aplomar</t>
+          <t>Base picada</t>
         </is>
       </c>
       <c r="I56" t="n">
@@ -4657,7 +4657,7 @@
       </c>
       <c r="J56" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K56" t="inlineStr">
@@ -4671,26 +4671,26 @@
         </is>
       </c>
       <c r="M56" t="n">
-        <v>-58.434339</v>
+        <v>-58.485592</v>
       </c>
       <c r="N56" t="n">
-        <v>-34.59693</v>
+        <v>-34.578586</v>
       </c>
       <c r="O56" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P56" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>6498</t>
+          <t>-547</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
@@ -4700,17 +4700,17 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>BUCARELLI 2087</t>
+          <t>Habana 4210</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>808733908</t>
+          <t>808733921</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
@@ -4725,7 +4725,7 @@
       </c>
       <c r="H57" t="inlineStr">
         <is>
-          <t>Base picada</t>
+          <t>Cambiar poste dañado</t>
         </is>
       </c>
       <c r="I57" t="n">
@@ -4743,14 +4743,14 @@
       </c>
       <c r="L57" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M57" t="n">
-        <v>-58.485592</v>
+        <v>-58.515873</v>
       </c>
       <c r="N57" t="n">
-        <v>-34.578586</v>
+        <v>-34.599425</v>
       </c>
       <c r="O57" t="inlineStr">
         <is>
@@ -4766,27 +4766,27 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>-547</t>
+          <t>6579</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>8/6/2025</t>
+          <t>8/7/2025</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>Habana 4210</t>
+          <t>RIVADAVIA MARTIN, COMODORO 1350</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>808733921</t>
+          <t>808749184</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
@@ -4801,7 +4801,7 @@
       </c>
       <c r="H58" t="inlineStr">
         <is>
-          <t>Cambiar poste dañado</t>
+          <t>Poste inclinado</t>
         </is>
       </c>
       <c r="I58" t="n">
@@ -4809,7 +4809,7 @@
       </c>
       <c r="J58" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K58" t="inlineStr">
@@ -4823,14 +4823,14 @@
         </is>
       </c>
       <c r="M58" t="n">
-        <v>-58.515873</v>
+        <v>-58.461024</v>
       </c>
       <c r="N58" t="n">
-        <v>-34.599425</v>
+        <v>-34.539409</v>
       </c>
       <c r="O58" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P58" t="inlineStr">
@@ -4842,27 +4842,27 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>6579</t>
+          <t>6906</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>8/7/2025</t>
+          <t>8/12/2025</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>RIVADAVIA MARTIN, COMODORO 1350</t>
+          <t>MOSCONI GENERAL AV. 3163</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>808749184</t>
+          <t>808918685</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
@@ -4877,7 +4877,7 @@
       </c>
       <c r="H59" t="inlineStr">
         <is>
-          <t>Poste inclinado</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I59" t="n">
@@ -4885,7 +4885,7 @@
       </c>
       <c r="J59" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K59" t="inlineStr">
@@ -4895,18 +4895,18 @@
       </c>
       <c r="L59" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M59" t="n">
-        <v>-58.461024</v>
+        <v>-58.505731</v>
       </c>
       <c r="N59" t="n">
-        <v>-34.539409</v>
+        <v>-34.588316</v>
       </c>
       <c r="O59" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P59" t="inlineStr">
@@ -4918,7 +4918,7 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>6906</t>
+          <t>6910</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
@@ -4928,17 +4928,17 @@
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>MOSCONI GENERAL AV. 3163</t>
+          <t>RIVAS, GRAL. 2345</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>808918685</t>
+          <t>808918698</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
@@ -4953,7 +4953,7 @@
       </c>
       <c r="H60" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I60" t="n">
@@ -4975,10 +4975,10 @@
         </is>
       </c>
       <c r="M60" t="n">
-        <v>-58.505731</v>
+        <v>-58.482497</v>
       </c>
       <c r="N60" t="n">
-        <v>-34.588316</v>
+        <v>-34.598714</v>
       </c>
       <c r="O60" t="inlineStr">
         <is>
@@ -4994,7 +4994,7 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>6910</t>
+          <t>6928</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
@@ -5004,17 +5004,17 @@
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>RIVAS, GRAL. 2345</t>
+          <t>ALBARELLOS AV. 3101</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>808918698</t>
+          <t>808918710</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
@@ -5029,7 +5029,7 @@
       </c>
       <c r="H61" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I61" t="n">
@@ -5051,10 +5051,10 @@
         </is>
       </c>
       <c r="M61" t="n">
-        <v>-58.482497</v>
+        <v>-58.512623</v>
       </c>
       <c r="N61" t="n">
-        <v>-34.598714</v>
+        <v>-34.579137</v>
       </c>
       <c r="O61" t="inlineStr">
         <is>
@@ -5070,7 +5070,7 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>6928</t>
+          <t>6939</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
@@ -5080,7 +5080,7 @@
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>ALBARELLOS AV. 3101</t>
+          <t>ANDONAEGUI 1894</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
@@ -5090,7 +5090,7 @@
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>808918710</t>
+          <t>808918715</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
@@ -5105,7 +5105,7 @@
       </c>
       <c r="H62" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I62" t="n">
@@ -5127,10 +5127,10 @@
         </is>
       </c>
       <c r="M62" t="n">
-        <v>-58.512623</v>
+        <v>-58.484848</v>
       </c>
       <c r="N62" t="n">
-        <v>-34.579137</v>
+        <v>-34.581325</v>
       </c>
       <c r="O62" t="inlineStr">
         <is>
@@ -5146,7 +5146,7 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>6939</t>
+          <t>-550</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
@@ -5156,17 +5156,17 @@
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>ANDONAEGUI 1894</t>
+          <t>Fitz roy 267</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>808918715</t>
+          <t>808918720</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
@@ -5181,7 +5181,7 @@
       </c>
       <c r="H63" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>Aplomar columna</t>
         </is>
       </c>
       <c r="I63" t="n">
@@ -5203,10 +5203,10 @@
         </is>
       </c>
       <c r="M63" t="n">
-        <v>-58.484848</v>
+        <v>-58.451378</v>
       </c>
       <c r="N63" t="n">
-        <v>-34.581325</v>
+        <v>-34.596195</v>
       </c>
       <c r="O63" t="inlineStr">
         <is>
@@ -5222,27 +5222,27 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>-550</t>
+          <t>6943</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>8/12/2025</t>
+          <t>8/14/2025</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>Fitz roy 267</t>
+          <t>SUPERI 1459</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>808918720</t>
+          <t>808972965</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
@@ -5257,7 +5257,7 @@
       </c>
       <c r="H64" t="inlineStr">
         <is>
-          <t>Aplomar columna</t>
+          <t>Poste con base quebrada ver si es posible desmonte</t>
         </is>
       </c>
       <c r="I64" t="n">
@@ -5265,7 +5265,7 @@
       </c>
       <c r="J64" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Desmonte</t>
         </is>
       </c>
       <c r="K64" t="inlineStr">
@@ -5275,18 +5275,18 @@
       </c>
       <c r="L64" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M64" t="n">
-        <v>-58.451378</v>
+        <v>-58.460834</v>
       </c>
       <c r="N64" t="n">
-        <v>-34.596195</v>
+        <v>-34.573753</v>
       </c>
       <c r="O64" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P64" t="inlineStr">
@@ -5298,7 +5298,7 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>6943</t>
+          <t>6969</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
@@ -5308,17 +5308,17 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>SUPERI 1459</t>
+          <t>CIUDAD DE LA PAZ 295</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>808972965</t>
+          <t>808972995</t>
         </is>
       </c>
       <c r="F65" t="inlineStr">
@@ -5333,7 +5333,7 @@
       </c>
       <c r="H65" t="inlineStr">
         <is>
-          <t>Poste con base quebrada ver si es posible desmonte</t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I65" t="n">
@@ -5341,7 +5341,7 @@
       </c>
       <c r="J65" t="inlineStr">
         <is>
-          <t>Desmonte</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K65" t="inlineStr">
@@ -5351,30 +5351,30 @@
       </c>
       <c r="L65" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M65" t="n">
-        <v>-58.460834</v>
+        <v>-58.441171</v>
       </c>
       <c r="N65" t="n">
-        <v>-34.573753</v>
+        <v>-34.574547</v>
       </c>
       <c r="O65" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P65" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>6944</t>
+          <t>6971</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
@@ -5384,7 +5384,7 @@
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>RAVIGNANI, EMILIO, DR. 2040</t>
+          <t>MAURE 1594</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
@@ -5394,7 +5394,7 @@
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>808972970</t>
+          <t>808973001</t>
         </is>
       </c>
       <c r="F66" t="inlineStr">
@@ -5409,7 +5409,7 @@
       </c>
       <c r="H66" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Ver de traspasar a telecentro y  desmontar ver con inspector</t>
         </is>
       </c>
       <c r="I66" t="n">
@@ -5427,14 +5427,14 @@
       </c>
       <c r="L66" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M66" t="n">
-        <v>-58.436264</v>
+        <v>-58.435072</v>
       </c>
       <c r="N66" t="n">
-        <v>-34.578942</v>
+        <v>-34.565732</v>
       </c>
       <c r="O66" t="inlineStr">
         <is>
@@ -5450,17 +5450,17 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>6969</t>
+          <t>7000</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>8/14/2025</t>
+          <t>8/20/2025</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>CIUDAD DE LA PAZ 295</t>
+          <t>SCALABRINI ORTIZ, RAUL AV. 2106</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
@@ -5470,7 +5470,7 @@
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>808972995</t>
+          <t>809065867</t>
         </is>
       </c>
       <c r="F67" t="inlineStr">
@@ -5485,7 +5485,7 @@
       </c>
       <c r="H67" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I67" t="n">
@@ -5507,10 +5507,10 @@
         </is>
       </c>
       <c r="M67" t="n">
-        <v>-58.441171</v>
+        <v>-58.420109</v>
       </c>
       <c r="N67" t="n">
-        <v>-34.574547</v>
+        <v>-34.58764</v>
       </c>
       <c r="O67" t="inlineStr">
         <is>
@@ -5526,27 +5526,27 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>6971</t>
+          <t>7003</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>8/14/2025</t>
+          <t>8/20/2025</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>MAURE 1594</t>
+          <t>MELIAN AV. 2576</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>808973001</t>
+          <t>809065874</t>
         </is>
       </c>
       <c r="F68" t="inlineStr">
@@ -5561,7 +5561,7 @@
       </c>
       <c r="H68" t="inlineStr">
         <is>
-          <t>Ver de traspasar a telecentro y  desmontar ver con inspector</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I68" t="n">
@@ -5583,46 +5583,46 @@
         </is>
       </c>
       <c r="M68" t="n">
-        <v>-58.435072</v>
+        <v>-58.471943</v>
       </c>
       <c r="N68" t="n">
-        <v>-34.565732</v>
+        <v>-34.564948</v>
       </c>
       <c r="O68" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P68" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>7000</t>
+          <t>-558</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>8/20/2025</t>
+          <t>8/21/2025</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>SCALABRINI ORTIZ, RAUL AV. 2106</t>
+          <t>Blanco Encalada 4210</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>809065867</t>
+          <t>ICD30461848</t>
         </is>
       </c>
       <c r="F69" t="inlineStr">
@@ -5637,7 +5637,7 @@
       </c>
       <c r="H69" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Colocar columna R400 para pedir taspaso de fuente telecom</t>
         </is>
       </c>
       <c r="I69" t="n">
@@ -5650,7 +5650,7 @@
       </c>
       <c r="K69" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Fuente Teco</t>
         </is>
       </c>
       <c r="L69" t="inlineStr">
@@ -5659,46 +5659,46 @@
         </is>
       </c>
       <c r="M69" t="n">
-        <v>-58.420109</v>
+        <v>-58.477593</v>
       </c>
       <c r="N69" t="n">
-        <v>-34.58764</v>
+        <v>-34.570321</v>
       </c>
       <c r="O69" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P69" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>7003</t>
+          <t>-559</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>8/20/2025</t>
+          <t>8/21/2025</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>MELIAN AV. 2576</t>
+          <t>Av. Del Libertador 6736</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>809065874</t>
+          <t>809098713</t>
         </is>
       </c>
       <c r="F70" t="inlineStr">
@@ -5735,14 +5735,14 @@
         </is>
       </c>
       <c r="M70" t="n">
-        <v>-58.471943</v>
+        <v>-58.453398</v>
       </c>
       <c r="N70" t="n">
-        <v>-34.564948</v>
+        <v>-34.550238</v>
       </c>
       <c r="O70" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P70" t="inlineStr">
@@ -5754,27 +5754,27 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>-558</t>
+          <t>5503</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>8/21/2025</t>
+          <t>8/22/2025</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>Blanco Encalada 4210</t>
+          <t>CRAMER AV. 1771</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>ICD30461848</t>
+          <t>809102564</t>
         </is>
       </c>
       <c r="F71" t="inlineStr">
@@ -5789,7 +5789,7 @@
       </c>
       <c r="H71" t="inlineStr">
         <is>
-          <t>Colocar columna R400 para pedir taspaso de fuente telecom</t>
+          <t>PIcada</t>
         </is>
       </c>
       <c r="I71" t="n">
@@ -5802,7 +5802,7 @@
       </c>
       <c r="K71" t="inlineStr">
         <is>
-          <t>Fuente Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L71" t="inlineStr">
@@ -5811,10 +5811,10 @@
         </is>
       </c>
       <c r="M71" t="n">
-        <v>-58.477593</v>
+        <v>-58.458506</v>
       </c>
       <c r="N71" t="n">
-        <v>-34.570321</v>
+        <v>-34.56783</v>
       </c>
       <c r="O71" t="inlineStr">
         <is>
@@ -5830,27 +5830,27 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>-559</t>
+          <t>7021</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>8/21/2025</t>
+          <t>8/25/2025</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>Av. Del Libertador 6736</t>
+          <t>VERA 445</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>809098713</t>
+          <t>809155622</t>
         </is>
       </c>
       <c r="F72" t="inlineStr">
@@ -5865,7 +5865,7 @@
       </c>
       <c r="H72" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Picada entro tambien como caso 7044</t>
         </is>
       </c>
       <c r="I72" t="n">
@@ -5887,323 +5887,19 @@
         </is>
       </c>
       <c r="M72" t="n">
-        <v>-58.453398</v>
+        <v>-58.437181</v>
       </c>
       <c r="N72" t="n">
-        <v>-34.550238</v>
+        <v>-34.5995</v>
       </c>
       <c r="O72" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P72" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
-        </is>
-      </c>
-    </row>
-    <row r="73">
-      <c r="A73" t="inlineStr">
-        <is>
-          <t>5467</t>
-        </is>
-      </c>
-      <c r="B73" t="inlineStr">
-        <is>
-          <t>8/22/2025</t>
-        </is>
-      </c>
-      <c r="C73" t="inlineStr">
-        <is>
-          <t>FRANCO 2515</t>
-        </is>
-      </c>
-      <c r="D73" t="inlineStr">
-        <is>
-          <t>12</t>
-        </is>
-      </c>
-      <c r="E73" t="inlineStr">
-        <is>
-          <t>809102560</t>
-        </is>
-      </c>
-      <c r="F73" t="inlineStr">
-        <is>
-          <t>NEW</t>
-        </is>
-      </c>
-      <c r="G73" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H73" t="inlineStr">
-        <is>
-          <t>PIcada</t>
-        </is>
-      </c>
-      <c r="I73" t="n">
-        <v>1</v>
-      </c>
-      <c r="J73" t="inlineStr">
-        <is>
-          <t>Cambio</t>
-        </is>
-      </c>
-      <c r="K73" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L73" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
-      <c r="M73" t="n">
-        <v>-58.502342</v>
-      </c>
-      <c r="N73" t="n">
-        <v>-34.578839</v>
-      </c>
-      <c r="O73" t="inlineStr">
-        <is>
-          <t>Paternal</t>
-        </is>
-      </c>
-      <c r="P73" t="inlineStr">
-        <is>
-          <t>Capital Norte</t>
-        </is>
-      </c>
-    </row>
-    <row r="74">
-      <c r="A74" t="inlineStr">
-        <is>
-          <t>5503</t>
-        </is>
-      </c>
-      <c r="B74" t="inlineStr">
-        <is>
-          <t>8/22/2025</t>
-        </is>
-      </c>
-      <c r="C74" t="inlineStr">
-        <is>
-          <t>CRAMER AV. 1771</t>
-        </is>
-      </c>
-      <c r="D74" t="inlineStr">
-        <is>
-          <t>13</t>
-        </is>
-      </c>
-      <c r="E74" t="inlineStr">
-        <is>
-          <t>809102564</t>
-        </is>
-      </c>
-      <c r="F74" t="inlineStr">
-        <is>
-          <t>NEW</t>
-        </is>
-      </c>
-      <c r="G74" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H74" t="inlineStr">
-        <is>
-          <t>PIcada</t>
-        </is>
-      </c>
-      <c r="I74" t="n">
-        <v>1</v>
-      </c>
-      <c r="J74" t="inlineStr">
-        <is>
-          <t>Cambio</t>
-        </is>
-      </c>
-      <c r="K74" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L74" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
-      <c r="M74" t="n">
-        <v>-58.458506</v>
-      </c>
-      <c r="N74" t="n">
-        <v>-34.56783</v>
-      </c>
-      <c r="O74" t="inlineStr">
-        <is>
-          <t>Colegiales</t>
-        </is>
-      </c>
-      <c r="P74" t="inlineStr">
-        <is>
-          <t>Capital Norte</t>
-        </is>
-      </c>
-    </row>
-    <row r="75">
-      <c r="A75" t="inlineStr">
-        <is>
-          <t>7021</t>
-        </is>
-      </c>
-      <c r="B75" t="inlineStr">
-        <is>
-          <t>8/25/2025</t>
-        </is>
-      </c>
-      <c r="C75" t="inlineStr">
-        <is>
-          <t>VERA 445</t>
-        </is>
-      </c>
-      <c r="D75" t="inlineStr">
-        <is>
-          <t>15</t>
-        </is>
-      </c>
-      <c r="E75" t="inlineStr">
-        <is>
-          <t>809155622</t>
-        </is>
-      </c>
-      <c r="F75" t="inlineStr">
-        <is>
-          <t>NEW</t>
-        </is>
-      </c>
-      <c r="G75" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H75" t="inlineStr">
-        <is>
-          <t>Picada entro tambien como caso 7044</t>
-        </is>
-      </c>
-      <c r="I75" t="n">
-        <v>1</v>
-      </c>
-      <c r="J75" t="inlineStr">
-        <is>
-          <t>Cambio</t>
-        </is>
-      </c>
-      <c r="K75" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L75" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
-      <c r="M75" t="n">
-        <v>-58.437181</v>
-      </c>
-      <c r="N75" t="n">
-        <v>-34.5995</v>
-      </c>
-      <c r="O75" t="inlineStr">
-        <is>
-          <t>Palermo</t>
-        </is>
-      </c>
-      <c r="P75" t="inlineStr">
-        <is>
           <t>Capital Sur</t>
-        </is>
-      </c>
-    </row>
-    <row r="76">
-      <c r="A76" t="inlineStr">
-        <is>
-          <t>-567</t>
-        </is>
-      </c>
-      <c r="B76" t="inlineStr">
-        <is>
-          <t>8/25/2025</t>
-        </is>
-      </c>
-      <c r="C76" t="inlineStr">
-        <is>
-          <t>Franco 2543</t>
-        </is>
-      </c>
-      <c r="D76" t="inlineStr">
-        <is>
-          <t>12</t>
-        </is>
-      </c>
-      <c r="E76" t="inlineStr">
-        <is>
-          <t>809184735</t>
-        </is>
-      </c>
-      <c r="F76" t="inlineStr">
-        <is>
-          <t>NEW</t>
-        </is>
-      </c>
-      <c r="G76" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H76" t="inlineStr">
-        <is>
-          <t>Cambio</t>
-        </is>
-      </c>
-      <c r="I76" t="n">
-        <v>0</v>
-      </c>
-      <c r="J76" t="inlineStr">
-        <is>
-          <t>Cambio</t>
-        </is>
-      </c>
-      <c r="K76" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L76" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
-      <c r="M76" t="n">
-        <v>-58.502565</v>
-      </c>
-      <c r="N76" t="n">
-        <v>-34.578977</v>
-      </c>
-      <c r="O76" t="inlineStr">
-        <is>
-          <t>Paternal</t>
-        </is>
-      </c>
-      <c r="P76" t="inlineStr">
-        <is>
-          <t>Capital Norte</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-08-29 08:11:50)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_NEW.xlsx
+++ b/mapa_interactivo_NEW.xlsx
@@ -1802,27 +1802,27 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>5599</t>
+          <t>5507</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>4/15/2025</t>
+          <t>4/7/2025</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>ESTOMBA 4052</t>
+          <t>CONGRESO 1927</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>804732246</t>
+          <t>804568921</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
@@ -1832,12 +1832,12 @@
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Transito</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>Columna PRFV quedo inclinada (la hicieron como estomba 4056)</t>
+          <t>No se puede trabajar queda QAP entro tambien como caso 7032</t>
         </is>
       </c>
       <c r="I19" t="n">
@@ -1845,12 +1845,12 @@
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>Nodo TLC</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L19" t="inlineStr">
@@ -1859,10 +1859,10 @@
         </is>
       </c>
       <c r="M19" t="n">
-        <v>-58.485407</v>
+        <v>-58.457701</v>
       </c>
       <c r="N19" t="n">
-        <v>-34.552985</v>
+        <v>-34.552844</v>
       </c>
       <c r="O19" t="inlineStr">
         <is>
@@ -1878,7 +1878,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>5590</t>
+          <t>5599</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -1888,17 +1888,17 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>O'HIGGINS 2441</t>
+          <t>ESTOMBA 4052</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>804732275</t>
+          <t>804732246</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
@@ -1913,7 +1913,7 @@
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Columna PRFV quedo inclinada (la hicieron como estomba 4056)</t>
         </is>
       </c>
       <c r="I20" t="n">
@@ -1921,12 +1921,12 @@
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo TLC</t>
         </is>
       </c>
       <c r="L20" t="inlineStr">
@@ -1935,10 +1935,10 @@
         </is>
       </c>
       <c r="M20" t="n">
-        <v>-58.45573</v>
+        <v>-58.485407</v>
       </c>
       <c r="N20" t="n">
-        <v>-34.556576</v>
+        <v>-34.552985</v>
       </c>
       <c r="O20" t="inlineStr">
         <is>
@@ -1954,27 +1954,27 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>804787368</t>
+          <t>5590</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>4/17/2025</t>
+          <t>4/15/2025</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>San Blas 2591</t>
+          <t>O'HIGGINS 2441</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>804787368</t>
+          <t>804732275</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
@@ -2011,14 +2011,14 @@
         </is>
       </c>
       <c r="M21" t="n">
-        <v>-58.477427</v>
+        <v>-58.45573</v>
       </c>
       <c r="N21" t="n">
-        <v>-34.609261</v>
+        <v>-34.556576</v>
       </c>
       <c r="O21" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P21" t="inlineStr">
@@ -2030,27 +2030,27 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>5624</t>
+          <t>804787368</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>4/22/2025</t>
+          <t>4/17/2025</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>PINO, VIRREY DEL 3456</t>
+          <t>San Blas 2591</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>804876043</t>
+          <t>804787368</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
@@ -2065,7 +2065,7 @@
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>Desmonte de poste</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I22" t="n">
@@ -2073,7 +2073,7 @@
       </c>
       <c r="J22" t="inlineStr">
         <is>
-          <t>Desmonte</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K22" t="inlineStr">
@@ -2083,18 +2083,18 @@
       </c>
       <c r="L22" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M22" t="n">
-        <v>-58.464354</v>
+        <v>-58.477427</v>
       </c>
       <c r="N22" t="n">
-        <v>-34.572486</v>
+        <v>-34.609261</v>
       </c>
       <c r="O22" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P22" t="inlineStr">
@@ -2106,17 +2106,17 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>804922147</t>
+          <t>5624</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>4/24/2025</t>
+          <t>4/22/2025</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Av. Álvarez Thomas 1171</t>
+          <t>PINO, VIRREY DEL 3456</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
@@ -2126,7 +2126,7 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>804922147</t>
+          <t>804876043</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
@@ -2141,15 +2141,15 @@
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Desmonte de poste</t>
         </is>
       </c>
       <c r="I23" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Desmonte</t>
         </is>
       </c>
       <c r="K23" t="inlineStr">
@@ -2159,14 +2159,14 @@
       </c>
       <c r="L23" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M23" t="n">
-        <v>-58.45793</v>
+        <v>-58.464354</v>
       </c>
       <c r="N23" t="n">
-        <v>-34.578334</v>
+        <v>-34.572486</v>
       </c>
       <c r="O23" t="inlineStr">
         <is>
@@ -2182,7 +2182,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>804922171</t>
+          <t>804922147</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -2192,7 +2192,7 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Virrey Arredondo 3581</t>
+          <t>Av. Álvarez Thomas 1171</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
@@ -2202,7 +2202,7 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>804922171</t>
+          <t>804922147</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
@@ -2217,15 +2217,15 @@
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>Aplomar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I24" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J24" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K24" t="inlineStr">
@@ -2235,14 +2235,14 @@
       </c>
       <c r="L24" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M24" t="n">
-        <v>-58.459513</v>
+        <v>-58.45793</v>
       </c>
       <c r="N24" t="n">
-        <v>-34.578019</v>
+        <v>-34.578334</v>
       </c>
       <c r="O24" t="inlineStr">
         <is>
@@ -2258,7 +2258,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>5656</t>
+          <t>804922171</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -2268,17 +2268,17 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>ECHEVERRIA 5893</t>
+          <t>Virrey Arredondo 3581</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>804922184</t>
+          <t>804922171</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
@@ -2293,7 +2293,7 @@
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>Poste con base quebrada</t>
+          <t>Aplomar</t>
         </is>
       </c>
       <c r="I25" t="n">
@@ -2301,7 +2301,7 @@
       </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t>Desmonte</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K25" t="inlineStr">
@@ -2311,18 +2311,18 @@
       </c>
       <c r="L25" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M25" t="n">
-        <v>-58.489627</v>
+        <v>-58.459513</v>
       </c>
       <c r="N25" t="n">
-        <v>-34.583761</v>
+        <v>-34.578019</v>
       </c>
       <c r="O25" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P25" t="inlineStr">
@@ -2334,27 +2334,27 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>6173</t>
+          <t>5656</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>4/29/2025</t>
+          <t>4/24/2025</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>ARMENIA 2321</t>
+          <t>ECHEVERRIA 5893</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>805507398</t>
+          <t>804922184</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
@@ -2369,7 +2369,7 @@
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>Picada volvio a entrar como caso 6325</t>
+          <t>Poste con base quebrada</t>
         </is>
       </c>
       <c r="I26" t="n">
@@ -2377,7 +2377,7 @@
       </c>
       <c r="J26" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Desmonte</t>
         </is>
       </c>
       <c r="K26" t="inlineStr">
@@ -2387,50 +2387,50 @@
       </c>
       <c r="L26" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M26" t="n">
-        <v>-58.420549</v>
+        <v>-58.489627</v>
       </c>
       <c r="N26" t="n">
-        <v>-34.585103</v>
+        <v>-34.583761</v>
       </c>
       <c r="O26" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P26" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>5715</t>
+          <t>6173</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>5/1/2025</t>
+          <t>4/29/2025</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>CUENCA 4690</t>
+          <t>ARMENIA 2321</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>805579094</t>
+          <t>805507398</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
@@ -2445,7 +2445,7 @@
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>Aplomar poste</t>
+          <t>Picada volvio a entrar como caso 6325</t>
         </is>
       </c>
       <c r="I27" t="n">
@@ -2453,7 +2453,7 @@
       </c>
       <c r="J27" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K27" t="inlineStr">
@@ -2463,30 +2463,30 @@
       </c>
       <c r="L27" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M27" t="n">
-        <v>-58.506061</v>
+        <v>-58.420549</v>
       </c>
       <c r="N27" t="n">
-        <v>-34.588887</v>
+        <v>-34.585103</v>
       </c>
       <c r="O27" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P27" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>6333</t>
+          <t>5715</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -2496,17 +2496,17 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>ORTEGA Y GASSET 1816</t>
+          <t>CUENCA 4690</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>805655342</t>
+          <t>805579094</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
@@ -2521,7 +2521,7 @@
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Aplomar poste</t>
         </is>
       </c>
       <c r="I28" t="n">
@@ -2529,7 +2529,7 @@
       </c>
       <c r="J28" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K28" t="inlineStr">
@@ -2539,40 +2539,40 @@
       </c>
       <c r="L28" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M28" t="n">
-        <v>-58.432556</v>
+        <v>-58.506061</v>
       </c>
       <c r="N28" t="n">
-        <v>-34.570279</v>
+        <v>-34.588887</v>
       </c>
       <c r="O28" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P28" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>805707165</t>
+          <t>6333</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>5/7/2025</t>
+          <t>5/1/2025</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Baez 793</t>
+          <t>ORTEGA Y GASSET 1816</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
@@ -2582,7 +2582,7 @@
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>805707165</t>
+          <t>805655342</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
@@ -2597,7 +2597,7 @@
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>DESMONTAR COLUMNA DE 7 MTS Y TRANSFERIR A COMUNITARIA</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I29" t="n">
@@ -2615,14 +2615,14 @@
       </c>
       <c r="L29" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M29" t="n">
-        <v>-58.436165</v>
+        <v>-58.432556</v>
       </c>
       <c r="N29" t="n">
-        <v>-34.569081</v>
+        <v>-34.570279</v>
       </c>
       <c r="O29" t="inlineStr">
         <is>
@@ -2638,27 +2638,27 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>5847</t>
+          <t>805707165</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>5/8/2025</t>
+          <t>5/7/2025</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>JURAMENTO 5321</t>
+          <t>Baez 793</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>805791839</t>
+          <t>805707165</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
@@ -2673,7 +2673,7 @@
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>DESMONTAR COLUMNA DE 7 MTS Y TRANSFERIR A COMUNITARIA</t>
         </is>
       </c>
       <c r="I30" t="n">
@@ -2691,50 +2691,50 @@
       </c>
       <c r="L30" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M30" t="n">
-        <v>-58.485193</v>
+        <v>-58.436165</v>
       </c>
       <c r="N30" t="n">
-        <v>-34.579621</v>
+        <v>-34.569081</v>
       </c>
       <c r="O30" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P30" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>232</t>
+          <t>5847</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>5/9/2025</t>
+          <t>5/8/2025</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Gorostiaga 2286</t>
+          <t>JURAMENTO 5321</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>805791858</t>
+          <t>805791839</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
@@ -2771,46 +2771,46 @@
         </is>
       </c>
       <c r="M31" t="n">
-        <v>-58.441563</v>
+        <v>-58.485193</v>
       </c>
       <c r="N31" t="n">
-        <v>-34.569743</v>
+        <v>-34.579621</v>
       </c>
       <c r="O31" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P31" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>-406</t>
+          <t>232</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>5/8/2025</t>
+          <t>5/9/2025</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Olof palme 4144</t>
+          <t>Gorostiaga 2286</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>805791925</t>
+          <t>805791858</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
@@ -2825,7 +2825,7 @@
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>Tensar 2 riendas a pique columna 168</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I32" t="n">
@@ -2833,7 +2833,7 @@
       </c>
       <c r="J32" t="inlineStr">
         <is>
-          <t>Tensor</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K32" t="inlineStr">
@@ -2843,40 +2843,40 @@
       </c>
       <c r="L32" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M32" t="n">
-        <v>-58.488252</v>
+        <v>-58.441563</v>
       </c>
       <c r="N32" t="n">
-        <v>-34.553391</v>
+        <v>-34.569743</v>
       </c>
       <c r="O32" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P32" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>5826</t>
+          <t>-406</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>5/19/2025</t>
+          <t>5/8/2025</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>ALBARELLOS AV. 3180</t>
+          <t>Olof palme 4144</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
@@ -2886,7 +2886,7 @@
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>806926466</t>
+          <t>805791925</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
@@ -2901,7 +2901,7 @@
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>Columna (metal) inclinada</t>
+          <t>Tensar 2 riendas a pique columna 168</t>
         </is>
       </c>
       <c r="I33" t="n">
@@ -2909,7 +2909,7 @@
       </c>
       <c r="J33" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Tensor</t>
         </is>
       </c>
       <c r="K33" t="inlineStr">
@@ -2923,14 +2923,14 @@
         </is>
       </c>
       <c r="M33" t="n">
-        <v>-58.513552</v>
+        <v>-58.488252</v>
       </c>
       <c r="N33" t="n">
-        <v>-34.579829</v>
+        <v>-34.553391</v>
       </c>
       <c r="O33" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P33" t="inlineStr">
@@ -2942,27 +2942,27 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>6020</t>
+          <t>5826</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>6/5/2025</t>
+          <t>5/19/2025</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>RAVIGNANI, EMILIO, DR. 2036</t>
+          <t>ALBARELLOS AV. 3180</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>807215465</t>
+          <t>806926466</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
@@ -2977,7 +2977,7 @@
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>Picada misma que 6260 y 6945</t>
+          <t>Columna (metal) inclinada</t>
         </is>
       </c>
       <c r="I34" t="n">
@@ -2985,7 +2985,7 @@
       </c>
       <c r="J34" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K34" t="inlineStr">
@@ -2995,50 +2995,50 @@
       </c>
       <c r="L34" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M34" t="n">
-        <v>-58.436298</v>
+        <v>-58.513552</v>
       </c>
       <c r="N34" t="n">
-        <v>-34.578972</v>
+        <v>-34.579829</v>
       </c>
       <c r="O34" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P34" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>6144</t>
+          <t>6020</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>6/11/2025</t>
+          <t>6/5/2025</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>TURIN 2990</t>
+          <t>RAVIGNANI, EMILIO, DR. 2036</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>807458282</t>
+          <t>807215465</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
@@ -3053,7 +3053,7 @@
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Picada misma que 6260 y 6945</t>
         </is>
       </c>
       <c r="I35" t="n">
@@ -3075,26 +3075,26 @@
         </is>
       </c>
       <c r="M35" t="n">
-        <v>-58.480925</v>
+        <v>-58.436298</v>
       </c>
       <c r="N35" t="n">
-        <v>-34.585471</v>
+        <v>-34.578972</v>
       </c>
       <c r="O35" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P35" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>6143</t>
+          <t>6144</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
@@ -3104,7 +3104,7 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>SOLANO LOPEZ, F., MARISCAL 2845</t>
+          <t>TURIN 2990</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
@@ -3114,7 +3114,7 @@
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>807458296</t>
+          <t>807458282</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
@@ -3151,10 +3151,10 @@
         </is>
       </c>
       <c r="M36" t="n">
-        <v>-58.495071</v>
+        <v>-58.480925</v>
       </c>
       <c r="N36" t="n">
-        <v>-34.593122</v>
+        <v>-34.585471</v>
       </c>
       <c r="O36" t="inlineStr">
         <is>
@@ -3170,7 +3170,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>6141</t>
+          <t>6143</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
@@ -3180,17 +3180,17 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>EL PAMPERO 2618</t>
+          <t>SOLANO LOPEZ, F., MARISCAL 2845</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>807458310</t>
+          <t>807458296</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
@@ -3205,7 +3205,7 @@
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>Picada info para cierre tambien entro como caso 6911</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I37" t="n">
@@ -3227,10 +3227,10 @@
         </is>
       </c>
       <c r="M37" t="n">
-        <v>-58.481942</v>
+        <v>-58.495071</v>
       </c>
       <c r="N37" t="n">
-        <v>-34.602989</v>
+        <v>-34.593122</v>
       </c>
       <c r="O37" t="inlineStr">
         <is>
@@ -3246,17 +3246,17 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>-478</t>
+          <t>6141</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>6/15/2025</t>
+          <t>6/11/2025</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Chivilcoy 4875</t>
+          <t>EL PAMPERO 2618</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
@@ -3266,7 +3266,7 @@
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>807508509</t>
+          <t>807458310</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
@@ -3281,7 +3281,7 @@
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>Poste podrido</t>
+          <t>Picada info para cierre tambien entro como caso 6911</t>
         </is>
       </c>
       <c r="I38" t="n">
@@ -3299,14 +3299,14 @@
       </c>
       <c r="L38" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M38" t="n">
-        <v>-58.517389</v>
+        <v>-58.481942</v>
       </c>
       <c r="N38" t="n">
-        <v>-34.593541</v>
+        <v>-34.602989</v>
       </c>
       <c r="O38" t="inlineStr">
         <is>
@@ -3322,27 +3322,27 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>6171</t>
+          <t>-478</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>6/18/2025</t>
+          <t>6/15/2025</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>CABELLO 3486</t>
+          <t>Chivilcoy 4875</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>807658640</t>
+          <t>807508509</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
@@ -3357,7 +3357,7 @@
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>Columna inclinada evaluar con inspector un corrimiento</t>
+          <t>Poste podrido</t>
         </is>
       </c>
       <c r="I39" t="n">
@@ -3375,40 +3375,40 @@
       </c>
       <c r="L39" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M39" t="n">
-        <v>-58.409579</v>
+        <v>-58.517389</v>
       </c>
       <c r="N39" t="n">
-        <v>-34.581134</v>
+        <v>-34.593541</v>
       </c>
       <c r="O39" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P39" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>6230</t>
+          <t>6171</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>6/24/2025</t>
+          <t>6/18/2025</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Santa maria de oro	2722</t>
+          <t>CABELLO 3486</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
@@ -3418,7 +3418,7 @@
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>807763066</t>
+          <t>807658640</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
@@ -3433,7 +3433,7 @@
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Columna inclinada evaluar con inspector un corrimiento</t>
         </is>
       </c>
       <c r="I40" t="n">
@@ -3455,10 +3455,10 @@
         </is>
       </c>
       <c r="M40" t="n">
-        <v>-58.422315</v>
+        <v>-58.409579</v>
       </c>
       <c r="N40" t="n">
-        <v>-34.576988</v>
+        <v>-34.581134</v>
       </c>
       <c r="O40" t="inlineStr">
         <is>
@@ -3474,7 +3474,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>6231</t>
+          <t>6230</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
@@ -3484,7 +3484,7 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Ciudad de la Paz 275</t>
+          <t>Santa maria de oro	2722</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
@@ -3494,7 +3494,7 @@
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>807763070</t>
+          <t>807763066</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
@@ -3509,7 +3509,7 @@
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>Aplomar o cambiar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I41" t="n">
@@ -3527,14 +3527,14 @@
       </c>
       <c r="L41" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M41" t="n">
-        <v>-58.441049</v>
+        <v>-58.422315</v>
       </c>
       <c r="N41" t="n">
-        <v>-34.574625</v>
+        <v>-34.576988</v>
       </c>
       <c r="O41" t="inlineStr">
         <is>
@@ -3550,7 +3550,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>6235</t>
+          <t>6231</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
@@ -3560,17 +3560,17 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>HUERGO 389</t>
+          <t>Ciudad de la Paz 275</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>807763078</t>
+          <t>807763070</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
@@ -3585,7 +3585,7 @@
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Aplomar o cambiar</t>
         </is>
       </c>
       <c r="I42" t="n">
@@ -3603,14 +3603,14 @@
       </c>
       <c r="L42" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M42" t="n">
-        <v>-58.432722</v>
+        <v>-58.441049</v>
       </c>
       <c r="N42" t="n">
-        <v>-34.572371</v>
+        <v>-34.574625</v>
       </c>
       <c r="O42" t="inlineStr">
         <is>
@@ -3626,27 +3626,27 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>6295</t>
+          <t>6235</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>6/30/2025</t>
+          <t>6/24/2025</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>SOLER 6017</t>
+          <t>HUERGO 389</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>807851636</t>
+          <t>807763078</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
@@ -3683,10 +3683,10 @@
         </is>
       </c>
       <c r="M43" t="n">
-        <v>-58.436808</v>
+        <v>-58.432722</v>
       </c>
       <c r="N43" t="n">
-        <v>-34.577464</v>
+        <v>-34.572371</v>
       </c>
       <c r="O43" t="inlineStr">
         <is>
@@ -3702,17 +3702,17 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>6332</t>
+          <t>6295</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>7/3/2025</t>
+          <t>6/30/2025</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>ARAOZ 2560</t>
+          <t>SOLER 6017</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
@@ -3722,7 +3722,7 @@
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>807965818</t>
+          <t>807851636</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
@@ -3759,10 +3759,10 @@
         </is>
       </c>
       <c r="M44" t="n">
-        <v>-58.414507</v>
+        <v>-58.436808</v>
       </c>
       <c r="N44" t="n">
-        <v>-34.585377</v>
+        <v>-34.577464</v>
       </c>
       <c r="O44" t="inlineStr">
         <is>
@@ -3778,27 +3778,27 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>-503</t>
+          <t>6332</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>7/10/2025</t>
+          <t>7/3/2025</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Salguero 842</t>
+          <t>ARAOZ 2560</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>808148673</t>
+          <t>807965818</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
@@ -3813,7 +3813,7 @@
       </c>
       <c r="H45" t="inlineStr">
         <is>
-          <t>Cambiar columna picada en la base</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I45" t="n">
@@ -3835,14 +3835,14 @@
         </is>
       </c>
       <c r="M45" t="n">
-        <v>-58.419166</v>
+        <v>-58.414507</v>
       </c>
       <c r="N45" t="n">
-        <v>-34.600265</v>
+        <v>-34.585377</v>
       </c>
       <c r="O45" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P45" t="inlineStr">
@@ -4538,27 +4538,27 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>6545</t>
+          <t>6498</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>8/4/2025</t>
+          <t>8/6/2025</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>SCALABRINI ORTIZ, RAUL AV. 708</t>
+          <t>BUCARELLI 2087</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>808703864</t>
+          <t>808733908</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
@@ -4573,7 +4573,7 @@
       </c>
       <c r="H55" t="inlineStr">
         <is>
-          <t>Aplomar</t>
+          <t>Base picada</t>
         </is>
       </c>
       <c r="I55" t="n">
@@ -4581,7 +4581,7 @@
       </c>
       <c r="J55" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K55" t="inlineStr">
@@ -4595,26 +4595,26 @@
         </is>
       </c>
       <c r="M55" t="n">
-        <v>-58.434339</v>
+        <v>-58.485592</v>
       </c>
       <c r="N55" t="n">
-        <v>-34.59693</v>
+        <v>-34.578586</v>
       </c>
       <c r="O55" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P55" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>6498</t>
+          <t>-547</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
@@ -4624,17 +4624,17 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>BUCARELLI 2087</t>
+          <t>Habana 4210</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>808733908</t>
+          <t>808733921</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
@@ -4649,7 +4649,7 @@
       </c>
       <c r="H56" t="inlineStr">
         <is>
-          <t>Base picada</t>
+          <t>Cambiar poste dañado</t>
         </is>
       </c>
       <c r="I56" t="n">
@@ -4667,14 +4667,14 @@
       </c>
       <c r="L56" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M56" t="n">
-        <v>-58.485592</v>
+        <v>-58.515873</v>
       </c>
       <c r="N56" t="n">
-        <v>-34.578586</v>
+        <v>-34.599425</v>
       </c>
       <c r="O56" t="inlineStr">
         <is>
@@ -4690,27 +4690,27 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>-547</t>
+          <t>6579</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>8/6/2025</t>
+          <t>8/7/2025</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>Habana 4210</t>
+          <t>RIVADAVIA MARTIN, COMODORO 1350</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>808733921</t>
+          <t>808749184</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
@@ -4725,7 +4725,7 @@
       </c>
       <c r="H57" t="inlineStr">
         <is>
-          <t>Cambiar poste dañado</t>
+          <t>Poste inclinado</t>
         </is>
       </c>
       <c r="I57" t="n">
@@ -4733,7 +4733,7 @@
       </c>
       <c r="J57" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K57" t="inlineStr">
@@ -4747,14 +4747,14 @@
         </is>
       </c>
       <c r="M57" t="n">
-        <v>-58.515873</v>
+        <v>-58.461024</v>
       </c>
       <c r="N57" t="n">
-        <v>-34.599425</v>
+        <v>-34.539409</v>
       </c>
       <c r="O57" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P57" t="inlineStr">
@@ -4766,27 +4766,27 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>6579</t>
+          <t>6906</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>8/7/2025</t>
+          <t>8/12/2025</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>RIVADAVIA MARTIN, COMODORO 1350</t>
+          <t>MOSCONI GENERAL AV. 3163</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>808749184</t>
+          <t>808918685</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
@@ -4801,7 +4801,7 @@
       </c>
       <c r="H58" t="inlineStr">
         <is>
-          <t>Poste inclinado</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I58" t="n">
@@ -4809,7 +4809,7 @@
       </c>
       <c r="J58" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K58" t="inlineStr">
@@ -4819,18 +4819,18 @@
       </c>
       <c r="L58" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M58" t="n">
-        <v>-58.461024</v>
+        <v>-58.505731</v>
       </c>
       <c r="N58" t="n">
-        <v>-34.539409</v>
+        <v>-34.588316</v>
       </c>
       <c r="O58" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P58" t="inlineStr">
@@ -4842,7 +4842,7 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>6906</t>
+          <t>6910</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
@@ -4852,17 +4852,17 @@
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>MOSCONI GENERAL AV. 3163</t>
+          <t>RIVAS, GRAL. 2345</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>808918685</t>
+          <t>808918698</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
@@ -4877,7 +4877,7 @@
       </c>
       <c r="H59" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I59" t="n">
@@ -4899,10 +4899,10 @@
         </is>
       </c>
       <c r="M59" t="n">
-        <v>-58.505731</v>
+        <v>-58.482497</v>
       </c>
       <c r="N59" t="n">
-        <v>-34.588316</v>
+        <v>-34.598714</v>
       </c>
       <c r="O59" t="inlineStr">
         <is>
@@ -4918,7 +4918,7 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>6910</t>
+          <t>6928</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
@@ -4928,17 +4928,17 @@
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>RIVAS, GRAL. 2345</t>
+          <t>ALBARELLOS AV. 3101</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>808918698</t>
+          <t>808918710</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
@@ -4953,7 +4953,7 @@
       </c>
       <c r="H60" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I60" t="n">
@@ -4975,10 +4975,10 @@
         </is>
       </c>
       <c r="M60" t="n">
-        <v>-58.482497</v>
+        <v>-58.512623</v>
       </c>
       <c r="N60" t="n">
-        <v>-34.598714</v>
+        <v>-34.579137</v>
       </c>
       <c r="O60" t="inlineStr">
         <is>
@@ -4994,7 +4994,7 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>6928</t>
+          <t>6939</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
@@ -5004,7 +5004,7 @@
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>ALBARELLOS AV. 3101</t>
+          <t>ANDONAEGUI 1894</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
@@ -5014,7 +5014,7 @@
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>808918710</t>
+          <t>808918715</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
@@ -5029,7 +5029,7 @@
       </c>
       <c r="H61" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I61" t="n">
@@ -5051,10 +5051,10 @@
         </is>
       </c>
       <c r="M61" t="n">
-        <v>-58.512623</v>
+        <v>-58.484848</v>
       </c>
       <c r="N61" t="n">
-        <v>-34.579137</v>
+        <v>-34.581325</v>
       </c>
       <c r="O61" t="inlineStr">
         <is>
@@ -5070,7 +5070,7 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>6939</t>
+          <t>-550</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
@@ -5080,17 +5080,17 @@
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>ANDONAEGUI 1894</t>
+          <t>Fitz roy 267</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>808918715</t>
+          <t>808918720</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
@@ -5105,7 +5105,7 @@
       </c>
       <c r="H62" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>Aplomar columna</t>
         </is>
       </c>
       <c r="I62" t="n">
@@ -5127,10 +5127,10 @@
         </is>
       </c>
       <c r="M62" t="n">
-        <v>-58.484848</v>
+        <v>-58.451378</v>
       </c>
       <c r="N62" t="n">
-        <v>-34.581325</v>
+        <v>-34.596195</v>
       </c>
       <c r="O62" t="inlineStr">
         <is>
@@ -5146,27 +5146,27 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>-550</t>
+          <t>6943</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>8/12/2025</t>
+          <t>8/14/2025</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>Fitz roy 267</t>
+          <t>SUPERI 1459</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>808918720</t>
+          <t>808972965</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
@@ -5181,7 +5181,7 @@
       </c>
       <c r="H63" t="inlineStr">
         <is>
-          <t>Aplomar columna</t>
+          <t>Poste con base quebrada ver si es posible desmonte</t>
         </is>
       </c>
       <c r="I63" t="n">
@@ -5189,7 +5189,7 @@
       </c>
       <c r="J63" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Desmonte</t>
         </is>
       </c>
       <c r="K63" t="inlineStr">
@@ -5199,18 +5199,18 @@
       </c>
       <c r="L63" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M63" t="n">
-        <v>-58.451378</v>
+        <v>-58.460834</v>
       </c>
       <c r="N63" t="n">
-        <v>-34.596195</v>
+        <v>-34.573753</v>
       </c>
       <c r="O63" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P63" t="inlineStr">
@@ -5222,7 +5222,7 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>6943</t>
+          <t>6969</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
@@ -5232,17 +5232,17 @@
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>SUPERI 1459</t>
+          <t>CIUDAD DE LA PAZ 295</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>808972965</t>
+          <t>808972995</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
@@ -5257,7 +5257,7 @@
       </c>
       <c r="H64" t="inlineStr">
         <is>
-          <t>Poste con base quebrada ver si es posible desmonte</t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I64" t="n">
@@ -5265,7 +5265,7 @@
       </c>
       <c r="J64" t="inlineStr">
         <is>
-          <t>Desmonte</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K64" t="inlineStr">
@@ -5275,30 +5275,30 @@
       </c>
       <c r="L64" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M64" t="n">
-        <v>-58.460834</v>
+        <v>-58.441171</v>
       </c>
       <c r="N64" t="n">
-        <v>-34.573753</v>
+        <v>-34.574547</v>
       </c>
       <c r="O64" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P64" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>6969</t>
+          <t>6971</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
@@ -5308,7 +5308,7 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>CIUDAD DE LA PAZ 295</t>
+          <t>MAURE 1594</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
@@ -5318,7 +5318,7 @@
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>808972995</t>
+          <t>808973001</t>
         </is>
       </c>
       <c r="F65" t="inlineStr">
@@ -5333,7 +5333,7 @@
       </c>
       <c r="H65" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>Ver de traspasar a telecentro y  desmontar ver con inspector</t>
         </is>
       </c>
       <c r="I65" t="n">
@@ -5355,10 +5355,10 @@
         </is>
       </c>
       <c r="M65" t="n">
-        <v>-58.441171</v>
+        <v>-58.435072</v>
       </c>
       <c r="N65" t="n">
-        <v>-34.574547</v>
+        <v>-34.565732</v>
       </c>
       <c r="O65" t="inlineStr">
         <is>
@@ -5374,17 +5374,17 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>6971</t>
+          <t>7000</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>8/14/2025</t>
+          <t>8/20/2025</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>MAURE 1594</t>
+          <t>SCALABRINI ORTIZ, RAUL AV. 2106</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
@@ -5394,7 +5394,7 @@
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>808973001</t>
+          <t>809065867</t>
         </is>
       </c>
       <c r="F66" t="inlineStr">
@@ -5409,7 +5409,7 @@
       </c>
       <c r="H66" t="inlineStr">
         <is>
-          <t>Ver de traspasar a telecentro y  desmontar ver con inspector</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I66" t="n">
@@ -5431,10 +5431,10 @@
         </is>
       </c>
       <c r="M66" t="n">
-        <v>-58.435072</v>
+        <v>-58.420109</v>
       </c>
       <c r="N66" t="n">
-        <v>-34.565732</v>
+        <v>-34.58764</v>
       </c>
       <c r="O66" t="inlineStr">
         <is>
@@ -5450,7 +5450,7 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>7000</t>
+          <t>7003</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
@@ -5460,17 +5460,17 @@
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>SCALABRINI ORTIZ, RAUL AV. 2106</t>
+          <t>MELIAN AV. 2576</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>809065867</t>
+          <t>809065874</t>
         </is>
       </c>
       <c r="F67" t="inlineStr">
@@ -5507,36 +5507,36 @@
         </is>
       </c>
       <c r="M67" t="n">
-        <v>-58.420109</v>
+        <v>-58.471943</v>
       </c>
       <c r="N67" t="n">
-        <v>-34.58764</v>
+        <v>-34.564948</v>
       </c>
       <c r="O67" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P67" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>7003</t>
+          <t>-558</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>8/20/2025</t>
+          <t>8/21/2025</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>MELIAN AV. 2576</t>
+          <t>Blanco Encalada 4210</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
@@ -5546,7 +5546,7 @@
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>809065874</t>
+          <t>ICD30461848</t>
         </is>
       </c>
       <c r="F68" t="inlineStr">
@@ -5561,7 +5561,7 @@
       </c>
       <c r="H68" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Colocar columna R400 para pedir taspaso de fuente telecom</t>
         </is>
       </c>
       <c r="I68" t="n">
@@ -5574,7 +5574,7 @@
       </c>
       <c r="K68" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Fuente Teco</t>
         </is>
       </c>
       <c r="L68" t="inlineStr">
@@ -5583,10 +5583,10 @@
         </is>
       </c>
       <c r="M68" t="n">
-        <v>-58.471943</v>
+        <v>-58.477593</v>
       </c>
       <c r="N68" t="n">
-        <v>-34.564948</v>
+        <v>-34.570321</v>
       </c>
       <c r="O68" t="inlineStr">
         <is>
@@ -5602,7 +5602,7 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>-558</t>
+          <t>-559</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
@@ -5612,17 +5612,17 @@
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>Blanco Encalada 4210</t>
+          <t>Av. Del Libertador 6736</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>ICD30461848</t>
+          <t>809098713</t>
         </is>
       </c>
       <c r="F69" t="inlineStr">
@@ -5637,7 +5637,7 @@
       </c>
       <c r="H69" t="inlineStr">
         <is>
-          <t>Colocar columna R400 para pedir taspaso de fuente telecom</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I69" t="n">
@@ -5650,7 +5650,7 @@
       </c>
       <c r="K69" t="inlineStr">
         <is>
-          <t>Fuente Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L69" t="inlineStr">
@@ -5659,14 +5659,14 @@
         </is>
       </c>
       <c r="M69" t="n">
-        <v>-58.477593</v>
+        <v>-58.453398</v>
       </c>
       <c r="N69" t="n">
-        <v>-34.570321</v>
+        <v>-34.550238</v>
       </c>
       <c r="O69" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P69" t="inlineStr">
@@ -5678,17 +5678,17 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>-559</t>
+          <t>5503</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>8/21/2025</t>
+          <t>8/22/2025</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>Av. Del Libertador 6736</t>
+          <t>CRAMER AV. 1771</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
@@ -5698,7 +5698,7 @@
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>809098713</t>
+          <t>809102564</t>
         </is>
       </c>
       <c r="F70" t="inlineStr">
@@ -5713,7 +5713,7 @@
       </c>
       <c r="H70" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>PIcada</t>
         </is>
       </c>
       <c r="I70" t="n">
@@ -5735,14 +5735,14 @@
         </is>
       </c>
       <c r="M70" t="n">
-        <v>-58.453398</v>
+        <v>-58.458506</v>
       </c>
       <c r="N70" t="n">
-        <v>-34.550238</v>
+        <v>-34.56783</v>
       </c>
       <c r="O70" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P70" t="inlineStr">
@@ -5754,17 +5754,17 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>5503</t>
+          <t>7080</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>8/22/2025</t>
+          <t>8/25/2025</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>CRAMER AV. 1771</t>
+          <t>UGARTE, MANUEL 2196</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
@@ -5774,7 +5774,7 @@
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>809102564</t>
+          <t>809125906</t>
         </is>
       </c>
       <c r="F71" t="inlineStr">
@@ -5789,7 +5789,7 @@
       </c>
       <c r="H71" t="inlineStr">
         <is>
-          <t>PIcada</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I71" t="n">
@@ -5811,14 +5811,14 @@
         </is>
       </c>
       <c r="M71" t="n">
-        <v>-58.458506</v>
+        <v>-58.459402</v>
       </c>
       <c r="N71" t="n">
-        <v>-34.56783</v>
+        <v>-34.555262</v>
       </c>
       <c r="O71" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P71" t="inlineStr">
@@ -5830,7 +5830,7 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>7080</t>
+          <t>7021</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
@@ -5840,17 +5840,17 @@
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>UGARTE, MANUEL 2196</t>
+          <t>VERA 445</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>809125906</t>
+          <t>809155622</t>
         </is>
       </c>
       <c r="F72" t="inlineStr">
@@ -5865,7 +5865,7 @@
       </c>
       <c r="H72" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Correrla para sacarla del cantero</t>
         </is>
       </c>
       <c r="I72" t="n">
@@ -5887,19 +5887,19 @@
         </is>
       </c>
       <c r="M72" t="n">
-        <v>-58.459402</v>
+        <v>-58.437181</v>
       </c>
       <c r="N72" t="n">
-        <v>-34.555262</v>
+        <v>-34.5995</v>
       </c>
       <c r="O72" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P72" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-08-30 08:22:25)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_NEW.xlsx
+++ b/mapa_interactivo_NEW.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P74"/>
+  <dimension ref="A1:P77"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1802,27 +1802,27 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>5507</t>
+          <t>5599</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>4/7/2025</t>
+          <t>4/15/2025</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>CONGRESO 1927</t>
+          <t>ESTOMBA 4052</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>804568921</t>
+          <t>804732246</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
@@ -1832,12 +1832,12 @@
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>Pendiente de Transito</t>
+          <t>Pendiente</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>No se puede trabajar queda QAP entro tambien como caso 7032</t>
+          <t>Columna PRFV quedo inclinada (la hicieron como estomba 4056)</t>
         </is>
       </c>
       <c r="I19" t="n">
@@ -1845,12 +1845,12 @@
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo TLC</t>
         </is>
       </c>
       <c r="L19" t="inlineStr">
@@ -1859,10 +1859,10 @@
         </is>
       </c>
       <c r="M19" t="n">
-        <v>-58.457701</v>
+        <v>-58.485407</v>
       </c>
       <c r="N19" t="n">
-        <v>-34.552844</v>
+        <v>-34.552985</v>
       </c>
       <c r="O19" t="inlineStr">
         <is>
@@ -1878,7 +1878,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>5599</t>
+          <t>5590</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -1888,17 +1888,17 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>ESTOMBA 4052</t>
+          <t>O'HIGGINS 2441</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>804732246</t>
+          <t>804732275</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
@@ -1913,7 +1913,7 @@
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>Columna PRFV quedo inclinada (la hicieron como estomba 4056)</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I20" t="n">
@@ -1921,12 +1921,12 @@
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>Nodo TLC</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L20" t="inlineStr">
@@ -1935,10 +1935,10 @@
         </is>
       </c>
       <c r="M20" t="n">
-        <v>-58.485407</v>
+        <v>-58.45573</v>
       </c>
       <c r="N20" t="n">
-        <v>-34.552985</v>
+        <v>-34.556576</v>
       </c>
       <c r="O20" t="inlineStr">
         <is>
@@ -1954,27 +1954,27 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>5590</t>
+          <t>804787368</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>4/15/2025</t>
+          <t>4/17/2025</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>O'HIGGINS 2441</t>
+          <t>San Blas 2591</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>804732275</t>
+          <t>804787368</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
@@ -2011,14 +2011,14 @@
         </is>
       </c>
       <c r="M21" t="n">
-        <v>-58.45573</v>
+        <v>-58.477427</v>
       </c>
       <c r="N21" t="n">
-        <v>-34.556576</v>
+        <v>-34.609261</v>
       </c>
       <c r="O21" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P21" t="inlineStr">
@@ -2030,27 +2030,27 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>804787368</t>
+          <t>5624</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>4/17/2025</t>
+          <t>4/22/2025</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>San Blas 2591</t>
+          <t>PINO, VIRREY DEL 3456</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>804787368</t>
+          <t>804876043</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
@@ -2065,7 +2065,7 @@
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Desmonte de poste</t>
         </is>
       </c>
       <c r="I22" t="n">
@@ -2073,7 +2073,7 @@
       </c>
       <c r="J22" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Desmonte</t>
         </is>
       </c>
       <c r="K22" t="inlineStr">
@@ -2083,18 +2083,18 @@
       </c>
       <c r="L22" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M22" t="n">
-        <v>-58.477427</v>
+        <v>-58.464354</v>
       </c>
       <c r="N22" t="n">
-        <v>-34.609261</v>
+        <v>-34.572486</v>
       </c>
       <c r="O22" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P22" t="inlineStr">
@@ -2106,17 +2106,17 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>5624</t>
+          <t>804922147</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>4/22/2025</t>
+          <t>4/24/2025</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>PINO, VIRREY DEL 3456</t>
+          <t>Av. Álvarez Thomas 1171</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
@@ -2126,7 +2126,7 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>804876043</t>
+          <t>804922147</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
@@ -2141,15 +2141,15 @@
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>Desmonte de poste</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I23" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>Desmonte</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K23" t="inlineStr">
@@ -2159,14 +2159,14 @@
       </c>
       <c r="L23" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M23" t="n">
-        <v>-58.464354</v>
+        <v>-58.45793</v>
       </c>
       <c r="N23" t="n">
-        <v>-34.572486</v>
+        <v>-34.578334</v>
       </c>
       <c r="O23" t="inlineStr">
         <is>
@@ -2182,7 +2182,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>804922147</t>
+          <t>804922171</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -2192,7 +2192,7 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Av. Álvarez Thomas 1171</t>
+          <t>Virrey Arredondo 3581</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
@@ -2202,7 +2202,7 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>804922147</t>
+          <t>804922171</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
@@ -2217,15 +2217,15 @@
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Aplomar</t>
         </is>
       </c>
       <c r="I24" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J24" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K24" t="inlineStr">
@@ -2235,14 +2235,14 @@
       </c>
       <c r="L24" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M24" t="n">
-        <v>-58.45793</v>
+        <v>-58.459513</v>
       </c>
       <c r="N24" t="n">
-        <v>-34.578334</v>
+        <v>-34.578019</v>
       </c>
       <c r="O24" t="inlineStr">
         <is>
@@ -2258,7 +2258,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>804922171</t>
+          <t>5656</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -2268,17 +2268,17 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Virrey Arredondo 3581</t>
+          <t>ECHEVERRIA 5893</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>804922171</t>
+          <t>804922184</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
@@ -2293,7 +2293,7 @@
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>Aplomar</t>
+          <t>Poste con base quebrada</t>
         </is>
       </c>
       <c r="I25" t="n">
@@ -2301,7 +2301,7 @@
       </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Desmonte</t>
         </is>
       </c>
       <c r="K25" t="inlineStr">
@@ -2311,18 +2311,18 @@
       </c>
       <c r="L25" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M25" t="n">
-        <v>-58.459513</v>
+        <v>-58.489627</v>
       </c>
       <c r="N25" t="n">
-        <v>-34.578019</v>
+        <v>-34.583761</v>
       </c>
       <c r="O25" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P25" t="inlineStr">
@@ -2334,27 +2334,27 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>5656</t>
+          <t>6173</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>4/24/2025</t>
+          <t>4/29/2025</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>ECHEVERRIA 5893</t>
+          <t>ARMENIA 2321</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>804922184</t>
+          <t>805507398</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
@@ -2369,7 +2369,7 @@
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>Poste con base quebrada</t>
+          <t>Picada volvio a entrar como caso 6325</t>
         </is>
       </c>
       <c r="I26" t="n">
@@ -2377,7 +2377,7 @@
       </c>
       <c r="J26" t="inlineStr">
         <is>
-          <t>Desmonte</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K26" t="inlineStr">
@@ -2387,50 +2387,50 @@
       </c>
       <c r="L26" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M26" t="n">
-        <v>-58.489627</v>
+        <v>-58.420549</v>
       </c>
       <c r="N26" t="n">
-        <v>-34.583761</v>
+        <v>-34.585103</v>
       </c>
       <c r="O26" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P26" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>6173</t>
+          <t>5715</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>4/29/2025</t>
+          <t>5/1/2025</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>ARMENIA 2321</t>
+          <t>CUENCA 4690</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>805507398</t>
+          <t>805579094</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
@@ -2445,7 +2445,7 @@
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>Picada volvio a entrar como caso 6325</t>
+          <t>Aplomar poste</t>
         </is>
       </c>
       <c r="I27" t="n">
@@ -2453,7 +2453,7 @@
       </c>
       <c r="J27" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K27" t="inlineStr">
@@ -2463,30 +2463,30 @@
       </c>
       <c r="L27" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M27" t="n">
-        <v>-58.420549</v>
+        <v>-58.506061</v>
       </c>
       <c r="N27" t="n">
-        <v>-34.585103</v>
+        <v>-34.588887</v>
       </c>
       <c r="O27" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P27" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>5715</t>
+          <t>6333</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -2496,17 +2496,17 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>CUENCA 4690</t>
+          <t>ORTEGA Y GASSET 1816</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>805579094</t>
+          <t>805655342</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
@@ -2521,7 +2521,7 @@
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>Aplomar poste</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I28" t="n">
@@ -2529,7 +2529,7 @@
       </c>
       <c r="J28" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K28" t="inlineStr">
@@ -2539,40 +2539,40 @@
       </c>
       <c r="L28" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M28" t="n">
-        <v>-58.506061</v>
+        <v>-58.432556</v>
       </c>
       <c r="N28" t="n">
-        <v>-34.588887</v>
+        <v>-34.570279</v>
       </c>
       <c r="O28" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P28" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>6333</t>
+          <t>805707165</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>5/1/2025</t>
+          <t>5/7/2025</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>ORTEGA Y GASSET 1816</t>
+          <t>Baez 793</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
@@ -2582,7 +2582,7 @@
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>805655342</t>
+          <t>805707165</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
@@ -2597,7 +2597,7 @@
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>DESMONTAR COLUMNA DE 7 MTS Y TRANSFERIR A COMUNITARIA</t>
         </is>
       </c>
       <c r="I29" t="n">
@@ -2615,14 +2615,14 @@
       </c>
       <c r="L29" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M29" t="n">
-        <v>-58.432556</v>
+        <v>-58.436165</v>
       </c>
       <c r="N29" t="n">
-        <v>-34.570279</v>
+        <v>-34.569081</v>
       </c>
       <c r="O29" t="inlineStr">
         <is>
@@ -2638,27 +2638,27 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>805707165</t>
+          <t>5847</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>5/7/2025</t>
+          <t>5/8/2025</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Baez 793</t>
+          <t>JURAMENTO 5321</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>805707165</t>
+          <t>805791839</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
@@ -2673,7 +2673,7 @@
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>DESMONTAR COLUMNA DE 7 MTS Y TRANSFERIR A COMUNITARIA</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I30" t="n">
@@ -2691,50 +2691,50 @@
       </c>
       <c r="L30" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M30" t="n">
-        <v>-58.436165</v>
+        <v>-58.485193</v>
       </c>
       <c r="N30" t="n">
-        <v>-34.569081</v>
+        <v>-34.579621</v>
       </c>
       <c r="O30" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P30" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>5847</t>
+          <t>232</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>5/8/2025</t>
+          <t>5/9/2025</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>JURAMENTO 5321</t>
+          <t>Gorostiaga 2286</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>805791839</t>
+          <t>805791858</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
@@ -2771,46 +2771,46 @@
         </is>
       </c>
       <c r="M31" t="n">
-        <v>-58.485193</v>
+        <v>-58.441563</v>
       </c>
       <c r="N31" t="n">
-        <v>-34.579621</v>
+        <v>-34.569743</v>
       </c>
       <c r="O31" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P31" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>232</t>
+          <t>-404</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>5/9/2025</t>
+          <t>5/8/2025</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Gorostiaga 2286</t>
+          <t>Amenabar 3048</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>805791858</t>
+          <t>805791896</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
@@ -2825,7 +2825,7 @@
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Aplomar columna 114</t>
         </is>
       </c>
       <c r="I32" t="n">
@@ -2833,7 +2833,7 @@
       </c>
       <c r="J32" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K32" t="inlineStr">
@@ -2847,19 +2847,19 @@
         </is>
       </c>
       <c r="M32" t="n">
-        <v>-58.441563</v>
+        <v>-58.46579</v>
       </c>
       <c r="N32" t="n">
-        <v>-34.569743</v>
+        <v>-34.555012</v>
       </c>
       <c r="O32" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P32" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
@@ -3246,17 +3246,17 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>6141</t>
+          <t>-478</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>6/11/2025</t>
+          <t>6/15/2025</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>EL PAMPERO 2618</t>
+          <t>Chivilcoy 4875</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
@@ -3266,7 +3266,7 @@
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>807458310</t>
+          <t>807508509</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
@@ -3281,7 +3281,7 @@
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>Picada info para cierre tambien entro como caso 6911</t>
+          <t>Poste podrido</t>
         </is>
       </c>
       <c r="I38" t="n">
@@ -3299,14 +3299,14 @@
       </c>
       <c r="L38" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M38" t="n">
-        <v>-58.481942</v>
+        <v>-58.517389</v>
       </c>
       <c r="N38" t="n">
-        <v>-34.602989</v>
+        <v>-34.593541</v>
       </c>
       <c r="O38" t="inlineStr">
         <is>
@@ -3322,27 +3322,27 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>-478</t>
+          <t>6171</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>6/15/2025</t>
+          <t>6/18/2025</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Chivilcoy 4875</t>
+          <t>CABELLO 3486</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>807508509</t>
+          <t>807658640</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
@@ -3357,7 +3357,7 @@
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>Poste podrido</t>
+          <t>Columna inclinada evaluar con inspector un corrimiento</t>
         </is>
       </c>
       <c r="I39" t="n">
@@ -3375,40 +3375,40 @@
       </c>
       <c r="L39" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M39" t="n">
-        <v>-58.517389</v>
+        <v>-58.409579</v>
       </c>
       <c r="N39" t="n">
-        <v>-34.593541</v>
+        <v>-34.581134</v>
       </c>
       <c r="O39" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P39" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>6171</t>
+          <t>6230</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>6/18/2025</t>
+          <t>6/24/2025</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>CABELLO 3486</t>
+          <t>Santa maria de oro	2722</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
@@ -3418,7 +3418,7 @@
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>807658640</t>
+          <t>807763066</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
@@ -3433,7 +3433,7 @@
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t>Columna inclinada evaluar con inspector un corrimiento</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I40" t="n">
@@ -3455,10 +3455,10 @@
         </is>
       </c>
       <c r="M40" t="n">
-        <v>-58.409579</v>
+        <v>-58.422315</v>
       </c>
       <c r="N40" t="n">
-        <v>-34.581134</v>
+        <v>-34.576988</v>
       </c>
       <c r="O40" t="inlineStr">
         <is>
@@ -3474,7 +3474,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>6230</t>
+          <t>6231</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
@@ -3484,7 +3484,7 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Santa maria de oro	2722</t>
+          <t>Ciudad de la Paz 275</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
@@ -3494,7 +3494,7 @@
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>807763066</t>
+          <t>807763070</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
@@ -3509,7 +3509,7 @@
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Aplomar o cambiar</t>
         </is>
       </c>
       <c r="I41" t="n">
@@ -3527,14 +3527,14 @@
       </c>
       <c r="L41" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M41" t="n">
-        <v>-58.422315</v>
+        <v>-58.441049</v>
       </c>
       <c r="N41" t="n">
-        <v>-34.576988</v>
+        <v>-34.574625</v>
       </c>
       <c r="O41" t="inlineStr">
         <is>
@@ -3550,7 +3550,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>6231</t>
+          <t>6235</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
@@ -3560,17 +3560,17 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Ciudad de la Paz 275</t>
+          <t>HUERGO 389</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>807763070</t>
+          <t>807763078</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
@@ -3585,7 +3585,7 @@
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>Aplomar o cambiar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I42" t="n">
@@ -3603,14 +3603,14 @@
       </c>
       <c r="L42" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M42" t="n">
-        <v>-58.441049</v>
+        <v>-58.432722</v>
       </c>
       <c r="N42" t="n">
-        <v>-34.574625</v>
+        <v>-34.572371</v>
       </c>
       <c r="O42" t="inlineStr">
         <is>
@@ -3626,27 +3626,27 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>6235</t>
+          <t>6295</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>6/24/2025</t>
+          <t>6/30/2025</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>HUERGO 389</t>
+          <t>SOLER 6017</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>807763078</t>
+          <t>807851636</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
@@ -3683,10 +3683,10 @@
         </is>
       </c>
       <c r="M43" t="n">
-        <v>-58.432722</v>
+        <v>-58.436808</v>
       </c>
       <c r="N43" t="n">
-        <v>-34.572371</v>
+        <v>-34.577464</v>
       </c>
       <c r="O43" t="inlineStr">
         <is>
@@ -3702,17 +3702,17 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>6295</t>
+          <t>6332</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>6/30/2025</t>
+          <t>7/3/2025</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>SOLER 6017</t>
+          <t>ARAOZ 2560</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
@@ -3722,7 +3722,7 @@
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>807851636</t>
+          <t>807965818</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
@@ -3759,10 +3759,10 @@
         </is>
       </c>
       <c r="M44" t="n">
-        <v>-58.436808</v>
+        <v>-58.414507</v>
       </c>
       <c r="N44" t="n">
-        <v>-34.577464</v>
+        <v>-34.585377</v>
       </c>
       <c r="O44" t="inlineStr">
         <is>
@@ -3778,27 +3778,27 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>6332</t>
+          <t>6506</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>7/3/2025</t>
+          <t>7/10/2025</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>ARAOZ 2560</t>
+          <t>Ohiggins 1611</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>807965818</t>
+          <t>808148679</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
@@ -3813,7 +3813,7 @@
       </c>
       <c r="H45" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Columna podrida en la base</t>
         </is>
       </c>
       <c r="I45" t="n">
@@ -3826,7 +3826,7 @@
       </c>
       <c r="K45" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L45" t="inlineStr">
@@ -3835,46 +3835,46 @@
         </is>
       </c>
       <c r="M45" t="n">
-        <v>-58.414507</v>
+        <v>-58.448993</v>
       </c>
       <c r="N45" t="n">
-        <v>-34.585377</v>
+        <v>-34.564383</v>
       </c>
       <c r="O45" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P45" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>6506</t>
+          <t>6437</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>7/10/2025</t>
+          <t>7/17/2025</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Ohiggins 1611</t>
+          <t>MILLER 4590</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>808148679</t>
+          <t>808400306</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
@@ -3889,7 +3889,7 @@
       </c>
       <c r="H46" t="inlineStr">
         <is>
-          <t>Columna podrida en la base</t>
+          <t>Columna corroida</t>
         </is>
       </c>
       <c r="I46" t="n">
@@ -3902,7 +3902,7 @@
       </c>
       <c r="K46" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L46" t="inlineStr">
@@ -3911,14 +3911,14 @@
         </is>
       </c>
       <c r="M46" t="n">
-        <v>-58.448993</v>
+        <v>-58.495482</v>
       </c>
       <c r="N46" t="n">
-        <v>-34.564383</v>
+        <v>-34.552614</v>
       </c>
       <c r="O46" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P46" t="inlineStr">
@@ -3930,7 +3930,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>6437</t>
+          <t>6538</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
@@ -3940,7 +3940,7 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>MILLER 4590</t>
+          <t>Pedraza Manuela 4101</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
@@ -3950,7 +3950,7 @@
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>808400306</t>
+          <t>808400353</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
@@ -3965,7 +3965,7 @@
       </c>
       <c r="H47" t="inlineStr">
         <is>
-          <t>Columna corroida</t>
+          <t xml:space="preserve">Podrida en la base </t>
         </is>
       </c>
       <c r="I47" t="n">
@@ -3987,10 +3987,10 @@
         </is>
       </c>
       <c r="M47" t="n">
-        <v>-58.495482</v>
+        <v>-58.481569</v>
       </c>
       <c r="N47" t="n">
-        <v>-34.552614</v>
+        <v>-34.559853</v>
       </c>
       <c r="O47" t="inlineStr">
         <is>
@@ -4006,27 +4006,27 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>6538</t>
+          <t>7023</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>7/17/2025</t>
+          <t>7/22/2025</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Pedraza Manuela 4101</t>
+          <t>ZABALA 3573</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>808400353</t>
+          <t>808480549</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
@@ -4041,7 +4041,7 @@
       </c>
       <c r="H48" t="inlineStr">
         <is>
-          <t xml:space="preserve">Podrida en la base </t>
+          <t>Corroida en base para recambio</t>
         </is>
       </c>
       <c r="I48" t="n">
@@ -4063,14 +4063,14 @@
         </is>
       </c>
       <c r="M48" t="n">
-        <v>-58.481569</v>
+        <v>-58.457522</v>
       </c>
       <c r="N48" t="n">
-        <v>-34.559853</v>
+        <v>-34.579414</v>
       </c>
       <c r="O48" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P48" t="inlineStr">
@@ -4082,27 +4082,27 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>7023</t>
+          <t>6484</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>7/22/2025</t>
+          <t>7/24/2025</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>ZABALA 3573</t>
+          <t>URIARTE 2396</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>808480549</t>
+          <t>808509373</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
@@ -4117,7 +4117,7 @@
       </c>
       <c r="H49" t="inlineStr">
         <is>
-          <t>Corroida en base para recambio</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I49" t="n">
@@ -4139,36 +4139,36 @@
         </is>
       </c>
       <c r="M49" t="n">
-        <v>-58.457522</v>
+        <v>-58.423934</v>
       </c>
       <c r="N49" t="n">
-        <v>-34.579414</v>
+        <v>-34.581562</v>
       </c>
       <c r="O49" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P49" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>6484</t>
+          <t>6512</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>7/24/2025</t>
+          <t>7/28/2025</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>URIARTE 2396</t>
+          <t>GASCON 1195</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
@@ -4178,7 +4178,7 @@
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>808509373</t>
+          <t>808571975</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
@@ -4215,10 +4215,10 @@
         </is>
       </c>
       <c r="M50" t="n">
-        <v>-58.423934</v>
+        <v>-58.423127</v>
       </c>
       <c r="N50" t="n">
-        <v>-34.581562</v>
+        <v>-34.596476</v>
       </c>
       <c r="O50" t="inlineStr">
         <is>
@@ -4234,7 +4234,7 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>6512</t>
+          <t>6513</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
@@ -4244,7 +4244,7 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>GASCON 1195</t>
+          <t>DORREGO 1925</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
@@ -4254,7 +4254,7 @@
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>808571975</t>
+          <t>808571976</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
@@ -4291,10 +4291,10 @@
         </is>
       </c>
       <c r="M51" t="n">
-        <v>-58.423127</v>
+        <v>-58.441281</v>
       </c>
       <c r="N51" t="n">
-        <v>-34.596476</v>
+        <v>-34.579867</v>
       </c>
       <c r="O51" t="inlineStr">
         <is>
@@ -4310,7 +4310,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>6513</t>
+          <t>6519</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
@@ -4320,7 +4320,7 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>DORREGO 1925</t>
+          <t>SALGUERO, JERONIMO 2874</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
@@ -4330,7 +4330,7 @@
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>808571976</t>
+          <t>808571977</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
@@ -4345,7 +4345,7 @@
       </c>
       <c r="H52" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Reparar rienda</t>
         </is>
       </c>
       <c r="I52" t="n">
@@ -4353,7 +4353,7 @@
       </c>
       <c r="J52" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Tensor</t>
         </is>
       </c>
       <c r="K52" t="inlineStr">
@@ -4363,14 +4363,14 @@
       </c>
       <c r="L52" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M52" t="n">
-        <v>-58.441281</v>
+        <v>-58.407256</v>
       </c>
       <c r="N52" t="n">
-        <v>-34.579867</v>
+        <v>-34.578976</v>
       </c>
       <c r="O52" t="inlineStr">
         <is>
@@ -4386,27 +4386,27 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>6519</t>
+          <t>-538</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>7/28/2025</t>
+          <t>7/31/2025</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>SALGUERO, JERONIMO 2874</t>
+          <t>Malabia 964</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>808571977</t>
+          <t>808609237</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
@@ -4421,7 +4421,7 @@
       </c>
       <c r="H53" t="inlineStr">
         <is>
-          <t>Reparar rienda</t>
+          <t>Cambiar poste mal estado por PRFV</t>
         </is>
       </c>
       <c r="I53" t="n">
@@ -4429,7 +4429,7 @@
       </c>
       <c r="J53" t="inlineStr">
         <is>
-          <t>Tensor</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K53" t="inlineStr">
@@ -4439,14 +4439,14 @@
       </c>
       <c r="L53" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M53" t="n">
-        <v>-58.407256</v>
+        <v>-58.433634</v>
       </c>
       <c r="N53" t="n">
-        <v>-34.578976</v>
+        <v>-34.595018</v>
       </c>
       <c r="O53" t="inlineStr">
         <is>
@@ -4462,27 +4462,27 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>-538</t>
+          <t>6498</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>7/31/2025</t>
+          <t>8/6/2025</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>Malabia 964</t>
+          <t>BUCARELLI 2087</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>808609237</t>
+          <t>808733908</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
@@ -4497,7 +4497,7 @@
       </c>
       <c r="H54" t="inlineStr">
         <is>
-          <t>Cambiar poste mal estado por PRFV</t>
+          <t>Base picada</t>
         </is>
       </c>
       <c r="I54" t="n">
@@ -4515,30 +4515,30 @@
       </c>
       <c r="L54" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M54" t="n">
-        <v>-58.433634</v>
+        <v>-58.485592</v>
       </c>
       <c r="N54" t="n">
-        <v>-34.595018</v>
+        <v>-34.578586</v>
       </c>
       <c r="O54" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P54" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>6498</t>
+          <t>-547</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
@@ -4548,17 +4548,17 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>BUCARELLI 2087</t>
+          <t>Habana 4210</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>808733908</t>
+          <t>808733921</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
@@ -4573,7 +4573,7 @@
       </c>
       <c r="H55" t="inlineStr">
         <is>
-          <t>Base picada</t>
+          <t>Cambiar poste dañado</t>
         </is>
       </c>
       <c r="I55" t="n">
@@ -4591,14 +4591,14 @@
       </c>
       <c r="L55" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M55" t="n">
-        <v>-58.485592</v>
+        <v>-58.515873</v>
       </c>
       <c r="N55" t="n">
-        <v>-34.578586</v>
+        <v>-34.599425</v>
       </c>
       <c r="O55" t="inlineStr">
         <is>
@@ -4614,27 +4614,27 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>-547</t>
+          <t>6579</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>8/6/2025</t>
+          <t>8/7/2025</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>Habana 4210</t>
+          <t>RIVADAVIA MARTIN, COMODORO 1350</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>808733921</t>
+          <t>808749184</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
@@ -4649,7 +4649,7 @@
       </c>
       <c r="H56" t="inlineStr">
         <is>
-          <t>Cambiar poste dañado</t>
+          <t>Poste inclinado</t>
         </is>
       </c>
       <c r="I56" t="n">
@@ -4657,7 +4657,7 @@
       </c>
       <c r="J56" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K56" t="inlineStr">
@@ -4671,14 +4671,14 @@
         </is>
       </c>
       <c r="M56" t="n">
-        <v>-58.515873</v>
+        <v>-58.461024</v>
       </c>
       <c r="N56" t="n">
-        <v>-34.599425</v>
+        <v>-34.539409</v>
       </c>
       <c r="O56" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P56" t="inlineStr">
@@ -4690,27 +4690,27 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>6579</t>
+          <t>6906</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>8/7/2025</t>
+          <t>8/12/2025</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>RIVADAVIA MARTIN, COMODORO 1350</t>
+          <t>MOSCONI GENERAL AV. 3163</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>808749184</t>
+          <t>808918685</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
@@ -4725,7 +4725,7 @@
       </c>
       <c r="H57" t="inlineStr">
         <is>
-          <t>Poste inclinado</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I57" t="n">
@@ -4733,7 +4733,7 @@
       </c>
       <c r="J57" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K57" t="inlineStr">
@@ -4743,18 +4743,18 @@
       </c>
       <c r="L57" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M57" t="n">
-        <v>-58.461024</v>
+        <v>-58.505731</v>
       </c>
       <c r="N57" t="n">
-        <v>-34.539409</v>
+        <v>-34.588316</v>
       </c>
       <c r="O57" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P57" t="inlineStr">
@@ -4766,7 +4766,7 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>6906</t>
+          <t>6910</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
@@ -4776,17 +4776,17 @@
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>MOSCONI GENERAL AV. 3163</t>
+          <t>RIVAS, GRAL. 2345</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>808918685</t>
+          <t>808918698</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
@@ -4801,7 +4801,7 @@
       </c>
       <c r="H58" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I58" t="n">
@@ -4823,10 +4823,10 @@
         </is>
       </c>
       <c r="M58" t="n">
-        <v>-58.505731</v>
+        <v>-58.482497</v>
       </c>
       <c r="N58" t="n">
-        <v>-34.588316</v>
+        <v>-34.598714</v>
       </c>
       <c r="O58" t="inlineStr">
         <is>
@@ -4842,7 +4842,7 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>6910</t>
+          <t>6928</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
@@ -4852,17 +4852,17 @@
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>RIVAS, GRAL. 2345</t>
+          <t>ALBARELLOS AV. 3101</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>808918698</t>
+          <t>808918710</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
@@ -4877,7 +4877,7 @@
       </c>
       <c r="H59" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I59" t="n">
@@ -4899,10 +4899,10 @@
         </is>
       </c>
       <c r="M59" t="n">
-        <v>-58.482497</v>
+        <v>-58.512623</v>
       </c>
       <c r="N59" t="n">
-        <v>-34.598714</v>
+        <v>-34.579137</v>
       </c>
       <c r="O59" t="inlineStr">
         <is>
@@ -4918,7 +4918,7 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>6928</t>
+          <t>6939</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
@@ -4928,7 +4928,7 @@
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>ALBARELLOS AV. 3101</t>
+          <t>ANDONAEGUI 1894</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
@@ -4938,7 +4938,7 @@
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>808918710</t>
+          <t>808918715</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
@@ -4953,7 +4953,7 @@
       </c>
       <c r="H60" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I60" t="n">
@@ -4975,10 +4975,10 @@
         </is>
       </c>
       <c r="M60" t="n">
-        <v>-58.512623</v>
+        <v>-58.484848</v>
       </c>
       <c r="N60" t="n">
-        <v>-34.579137</v>
+        <v>-34.581325</v>
       </c>
       <c r="O60" t="inlineStr">
         <is>
@@ -4994,7 +4994,7 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>6939</t>
+          <t>-550</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
@@ -5004,17 +5004,17 @@
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>ANDONAEGUI 1894</t>
+          <t>Fitz roy 267</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>808918715</t>
+          <t>808918720</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
@@ -5029,7 +5029,7 @@
       </c>
       <c r="H61" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>Aplomar columna</t>
         </is>
       </c>
       <c r="I61" t="n">
@@ -5051,10 +5051,10 @@
         </is>
       </c>
       <c r="M61" t="n">
-        <v>-58.484848</v>
+        <v>-58.451378</v>
       </c>
       <c r="N61" t="n">
-        <v>-34.581325</v>
+        <v>-34.596195</v>
       </c>
       <c r="O61" t="inlineStr">
         <is>
@@ -5070,27 +5070,27 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>-550</t>
+          <t>6943</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>8/12/2025</t>
+          <t>8/14/2025</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>Fitz roy 267</t>
+          <t>SUPERI 1459</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>808918720</t>
+          <t>808972965</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
@@ -5105,7 +5105,7 @@
       </c>
       <c r="H62" t="inlineStr">
         <is>
-          <t>Aplomar columna</t>
+          <t>Poste con base quebrada ver si es posible desmonte</t>
         </is>
       </c>
       <c r="I62" t="n">
@@ -5113,7 +5113,7 @@
       </c>
       <c r="J62" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Desmonte</t>
         </is>
       </c>
       <c r="K62" t="inlineStr">
@@ -5123,18 +5123,18 @@
       </c>
       <c r="L62" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M62" t="n">
-        <v>-58.451378</v>
+        <v>-58.460834</v>
       </c>
       <c r="N62" t="n">
-        <v>-34.596195</v>
+        <v>-34.573753</v>
       </c>
       <c r="O62" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P62" t="inlineStr">
@@ -5146,7 +5146,7 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>6943</t>
+          <t>6969</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
@@ -5156,17 +5156,17 @@
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>SUPERI 1459</t>
+          <t>CIUDAD DE LA PAZ 295</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>808972965</t>
+          <t>808972995</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
@@ -5181,7 +5181,7 @@
       </c>
       <c r="H63" t="inlineStr">
         <is>
-          <t>Poste con base quebrada ver si es posible desmonte</t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I63" t="n">
@@ -5189,7 +5189,7 @@
       </c>
       <c r="J63" t="inlineStr">
         <is>
-          <t>Desmonte</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K63" t="inlineStr">
@@ -5199,30 +5199,30 @@
       </c>
       <c r="L63" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M63" t="n">
-        <v>-58.460834</v>
+        <v>-58.441171</v>
       </c>
       <c r="N63" t="n">
-        <v>-34.573753</v>
+        <v>-34.574547</v>
       </c>
       <c r="O63" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P63" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>6969</t>
+          <t>6971</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
@@ -5232,7 +5232,7 @@
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>CIUDAD DE LA PAZ 295</t>
+          <t>MAURE 1594</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
@@ -5242,7 +5242,7 @@
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>808972995</t>
+          <t>808973001</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
@@ -5257,7 +5257,7 @@
       </c>
       <c r="H64" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>Ver de traspasar a telecentro y  desmontar ver con inspector</t>
         </is>
       </c>
       <c r="I64" t="n">
@@ -5279,10 +5279,10 @@
         </is>
       </c>
       <c r="M64" t="n">
-        <v>-58.441171</v>
+        <v>-58.435072</v>
       </c>
       <c r="N64" t="n">
-        <v>-34.574547</v>
+        <v>-34.565732</v>
       </c>
       <c r="O64" t="inlineStr">
         <is>
@@ -5298,17 +5298,17 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>6971</t>
+          <t>7000</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>8/14/2025</t>
+          <t>8/20/2025</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>MAURE 1594</t>
+          <t>SCALABRINI ORTIZ, RAUL AV. 2106</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
@@ -5318,7 +5318,7 @@
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>808973001</t>
+          <t>809065867</t>
         </is>
       </c>
       <c r="F65" t="inlineStr">
@@ -5333,7 +5333,7 @@
       </c>
       <c r="H65" t="inlineStr">
         <is>
-          <t>Ver de traspasar a telecentro y  desmontar ver con inspector</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I65" t="n">
@@ -5355,10 +5355,10 @@
         </is>
       </c>
       <c r="M65" t="n">
-        <v>-58.435072</v>
+        <v>-58.420109</v>
       </c>
       <c r="N65" t="n">
-        <v>-34.565732</v>
+        <v>-34.58764</v>
       </c>
       <c r="O65" t="inlineStr">
         <is>
@@ -5374,7 +5374,7 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>7000</t>
+          <t>7003</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
@@ -5384,17 +5384,17 @@
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>SCALABRINI ORTIZ, RAUL AV. 2106</t>
+          <t>MELIAN AV. 2576</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>809065867</t>
+          <t>809065874</t>
         </is>
       </c>
       <c r="F66" t="inlineStr">
@@ -5431,36 +5431,36 @@
         </is>
       </c>
       <c r="M66" t="n">
-        <v>-58.420109</v>
+        <v>-58.471943</v>
       </c>
       <c r="N66" t="n">
-        <v>-34.58764</v>
+        <v>-34.564948</v>
       </c>
       <c r="O66" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P66" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>7003</t>
+          <t>-558</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>8/20/2025</t>
+          <t>8/21/2025</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>MELIAN AV. 2576</t>
+          <t>Blanco Encalada 4210</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
@@ -5470,7 +5470,7 @@
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>809065874</t>
+          <t>ICD30461848</t>
         </is>
       </c>
       <c r="F67" t="inlineStr">
@@ -5485,7 +5485,7 @@
       </c>
       <c r="H67" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Colocar columna R400 para pedir taspaso de fuente telecom</t>
         </is>
       </c>
       <c r="I67" t="n">
@@ -5498,7 +5498,7 @@
       </c>
       <c r="K67" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Fuente Teco</t>
         </is>
       </c>
       <c r="L67" t="inlineStr">
@@ -5507,10 +5507,10 @@
         </is>
       </c>
       <c r="M67" t="n">
-        <v>-58.471943</v>
+        <v>-58.477593</v>
       </c>
       <c r="N67" t="n">
-        <v>-34.564948</v>
+        <v>-34.570321</v>
       </c>
       <c r="O67" t="inlineStr">
         <is>
@@ -5526,7 +5526,7 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>-558</t>
+          <t>-559</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
@@ -5536,17 +5536,17 @@
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>Blanco Encalada 4210</t>
+          <t>Av. Del Libertador 6736</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>ICD30461848</t>
+          <t>809098713</t>
         </is>
       </c>
       <c r="F68" t="inlineStr">
@@ -5561,7 +5561,7 @@
       </c>
       <c r="H68" t="inlineStr">
         <is>
-          <t>Colocar columna R400 para pedir taspaso de fuente telecom</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I68" t="n">
@@ -5574,7 +5574,7 @@
       </c>
       <c r="K68" t="inlineStr">
         <is>
-          <t>Fuente Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L68" t="inlineStr">
@@ -5583,14 +5583,14 @@
         </is>
       </c>
       <c r="M68" t="n">
-        <v>-58.477593</v>
+        <v>-58.453398</v>
       </c>
       <c r="N68" t="n">
-        <v>-34.570321</v>
+        <v>-34.550238</v>
       </c>
       <c r="O68" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P68" t="inlineStr">
@@ -5602,17 +5602,17 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>-559</t>
+          <t>5503</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>8/21/2025</t>
+          <t>8/22/2025</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>Av. Del Libertador 6736</t>
+          <t>CRAMER AV. 1771</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
@@ -5622,7 +5622,7 @@
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>809098713</t>
+          <t>809102564</t>
         </is>
       </c>
       <c r="F69" t="inlineStr">
@@ -5637,7 +5637,7 @@
       </c>
       <c r="H69" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>PIcada</t>
         </is>
       </c>
       <c r="I69" t="n">
@@ -5659,14 +5659,14 @@
         </is>
       </c>
       <c r="M69" t="n">
-        <v>-58.453398</v>
+        <v>-58.458506</v>
       </c>
       <c r="N69" t="n">
-        <v>-34.550238</v>
+        <v>-34.56783</v>
       </c>
       <c r="O69" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P69" t="inlineStr">
@@ -5678,27 +5678,27 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>5503</t>
+          <t>7098</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>8/22/2025</t>
+          <t>8/25/2025</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>CRAMER AV. 1771</t>
+          <t>UGARTE, MANUEL 3484</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>809102564</t>
+          <t>809126236</t>
         </is>
       </c>
       <c r="F70" t="inlineStr">
@@ -5713,7 +5713,7 @@
       </c>
       <c r="H70" t="inlineStr">
         <is>
-          <t>PIcada</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I70" t="n">
@@ -5735,10 +5735,10 @@
         </is>
       </c>
       <c r="M70" t="n">
-        <v>-58.458506</v>
+        <v>-58.472869</v>
       </c>
       <c r="N70" t="n">
-        <v>-34.56783</v>
+        <v>-34.562</v>
       </c>
       <c r="O70" t="inlineStr">
         <is>
@@ -6050,6 +6050,234 @@
         </is>
       </c>
       <c r="P74" t="inlineStr">
+        <is>
+          <t>Capital Norte</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>-575</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>8/28/2025</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>Amenabar 3064</t>
+        </is>
+      </c>
+      <c r="D75" t="inlineStr">
+        <is>
+          <t>13</t>
+        </is>
+      </c>
+      <c r="E75" t="inlineStr">
+        <is>
+          <t>809281299</t>
+        </is>
+      </c>
+      <c r="F75" t="inlineStr">
+        <is>
+          <t>NEW</t>
+        </is>
+      </c>
+      <c r="G75" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H75" t="inlineStr">
+        <is>
+          <t>Picada</t>
+        </is>
+      </c>
+      <c r="I75" t="n">
+        <v>1</v>
+      </c>
+      <c r="J75" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K75" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L75" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M75" t="n">
+        <v>-58.465984</v>
+      </c>
+      <c r="N75" t="n">
+        <v>-34.554869</v>
+      </c>
+      <c r="O75" t="inlineStr">
+        <is>
+          <t>Saavedra</t>
+        </is>
+      </c>
+      <c r="P75" t="inlineStr">
+        <is>
+          <t>Capital Norte</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>4166</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>8/29/2025</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>ALTOLAGUIRRE 2201</t>
+        </is>
+      </c>
+      <c r="D76" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="E76" t="inlineStr">
+        <is>
+          <t>809309591</t>
+        </is>
+      </c>
+      <c r="F76" t="inlineStr">
+        <is>
+          <t>NEW</t>
+        </is>
+      </c>
+      <c r="G76" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H76" t="inlineStr">
+        <is>
+          <t>Cambiar</t>
+        </is>
+      </c>
+      <c r="I76" t="n">
+        <v>1</v>
+      </c>
+      <c r="J76" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K76" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L76" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M76" t="n">
+        <v>-58.489622</v>
+      </c>
+      <c r="N76" t="n">
+        <v>-34.578426</v>
+      </c>
+      <c r="O76" t="inlineStr">
+        <is>
+          <t>Paternal</t>
+        </is>
+      </c>
+      <c r="P76" t="inlineStr">
+        <is>
+          <t>Capital Norte</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>-576</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>8/29/2025</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>Av. Boyacá 2030</t>
+        </is>
+      </c>
+      <c r="D77" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
+      <c r="E77" t="inlineStr">
+        <is>
+          <t>809309606</t>
+        </is>
+      </c>
+      <c r="F77" t="inlineStr">
+        <is>
+          <t>NEW</t>
+        </is>
+      </c>
+      <c r="G77" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H77" t="inlineStr">
+        <is>
+          <t>Picada</t>
+        </is>
+      </c>
+      <c r="I77" t="n">
+        <v>1</v>
+      </c>
+      <c r="J77" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K77" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L77" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M77" t="n">
+        <v>-58.471173</v>
+      </c>
+      <c r="N77" t="n">
+        <v>-34.60704</v>
+      </c>
+      <c r="O77" t="inlineStr">
+        <is>
+          <t>Paternal</t>
+        </is>
+      </c>
+      <c r="P77" t="inlineStr">
         <is>
           <t>Capital Norte</t>
         </is>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-09-01 14:41:13)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_NEW.xlsx
+++ b/mapa_interactivo_NEW.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P77"/>
+  <dimension ref="A1:P78"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6283,6 +6283,82 @@
         </is>
       </c>
     </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>7111</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>9/1/2025</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>VILELA 3699</t>
+        </is>
+      </c>
+      <c r="D78" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="E78" t="inlineStr">
+        <is>
+          <t>809371823</t>
+        </is>
+      </c>
+      <c r="F78" t="inlineStr">
+        <is>
+          <t>NEW</t>
+        </is>
+      </c>
+      <c r="G78" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H78" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Cambiar </t>
+        </is>
+      </c>
+      <c r="I78" t="n">
+        <v>1</v>
+      </c>
+      <c r="J78" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K78" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L78" t="inlineStr">
+        <is>
+          <t>Terminal</t>
+        </is>
+      </c>
+      <c r="M78" t="n">
+        <v>-58.482817</v>
+      </c>
+      <c r="N78" t="n">
+        <v>-34.550845</v>
+      </c>
+      <c r="O78" t="inlineStr">
+        <is>
+          <t>Saavedra</t>
+        </is>
+      </c>
+      <c r="P78" t="inlineStr">
+        <is>
+          <t>Capital Norte</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-09-02 18:47:54)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_NEW.xlsx
+++ b/mapa_interactivo_NEW.xlsx
@@ -2638,27 +2638,27 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>5847</t>
+          <t>232</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>5/8/2025</t>
+          <t>5/9/2025</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>JURAMENTO 5321</t>
+          <t>Gorostiaga 2286</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>805791839</t>
+          <t>805791858</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
@@ -2695,46 +2695,46 @@
         </is>
       </c>
       <c r="M30" t="n">
-        <v>-58.485193</v>
+        <v>-58.441563</v>
       </c>
       <c r="N30" t="n">
-        <v>-34.579621</v>
+        <v>-34.569743</v>
       </c>
       <c r="O30" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P30" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>232</t>
+          <t>-404</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>5/9/2025</t>
+          <t>5/8/2025</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Gorostiaga 2286</t>
+          <t>Amenabar 3048</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>805791858</t>
+          <t>805791896</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
@@ -2749,7 +2749,7 @@
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Aplomar columna 114</t>
         </is>
       </c>
       <c r="I31" t="n">
@@ -2757,7 +2757,7 @@
       </c>
       <c r="J31" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K31" t="inlineStr">
@@ -2771,26 +2771,26 @@
         </is>
       </c>
       <c r="M31" t="n">
-        <v>-58.441563</v>
+        <v>-58.46579</v>
       </c>
       <c r="N31" t="n">
-        <v>-34.569743</v>
+        <v>-34.555012</v>
       </c>
       <c r="O31" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P31" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>-404</t>
+          <t>-406</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
@@ -2800,17 +2800,17 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Amenabar 3048</t>
+          <t>Olof palme 4144</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>805791896</t>
+          <t>805791925</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
@@ -2825,7 +2825,7 @@
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>Aplomar columna 114</t>
+          <t>Tensar 2 riendas a pique columna 168</t>
         </is>
       </c>
       <c r="I32" t="n">
@@ -2833,7 +2833,7 @@
       </c>
       <c r="J32" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Tensor</t>
         </is>
       </c>
       <c r="K32" t="inlineStr">
@@ -2843,14 +2843,14 @@
       </c>
       <c r="L32" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M32" t="n">
-        <v>-58.46579</v>
+        <v>-58.488252</v>
       </c>
       <c r="N32" t="n">
-        <v>-34.555012</v>
+        <v>-34.553391</v>
       </c>
       <c r="O32" t="inlineStr">
         <is>
@@ -2866,17 +2866,17 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>-406</t>
+          <t>5826</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>5/8/2025</t>
+          <t>5/19/2025</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Olof palme 4144</t>
+          <t>ALBARELLOS AV. 3180</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
@@ -2886,7 +2886,7 @@
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>805791925</t>
+          <t>806926466</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
@@ -2901,7 +2901,7 @@
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>Tensar 2 riendas a pique columna 168</t>
+          <t>Columna (metal) inclinada</t>
         </is>
       </c>
       <c r="I33" t="n">
@@ -2909,7 +2909,7 @@
       </c>
       <c r="J33" t="inlineStr">
         <is>
-          <t>Tensor</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K33" t="inlineStr">
@@ -2923,14 +2923,14 @@
         </is>
       </c>
       <c r="M33" t="n">
-        <v>-58.488252</v>
+        <v>-58.513552</v>
       </c>
       <c r="N33" t="n">
-        <v>-34.553391</v>
+        <v>-34.579829</v>
       </c>
       <c r="O33" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P33" t="inlineStr">
@@ -2942,27 +2942,27 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>5826</t>
+          <t>6020</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>5/19/2025</t>
+          <t>6/5/2025</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>ALBARELLOS AV. 3180</t>
+          <t>RAVIGNANI, EMILIO, DR. 2036</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>806926466</t>
+          <t>807215465</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
@@ -2977,7 +2977,7 @@
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>Columna (metal) inclinada</t>
+          <t>Picada misma que 6260 y 6945</t>
         </is>
       </c>
       <c r="I34" t="n">
@@ -2985,7 +2985,7 @@
       </c>
       <c r="J34" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K34" t="inlineStr">
@@ -2995,50 +2995,50 @@
       </c>
       <c r="L34" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M34" t="n">
-        <v>-58.513552</v>
+        <v>-58.436298</v>
       </c>
       <c r="N34" t="n">
-        <v>-34.579829</v>
+        <v>-34.578972</v>
       </c>
       <c r="O34" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P34" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>6020</t>
+          <t>6144</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>6/5/2025</t>
+          <t>6/11/2025</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>RAVIGNANI, EMILIO, DR. 2036</t>
+          <t>TURIN 2990</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>807215465</t>
+          <t>807458282</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
@@ -3053,7 +3053,7 @@
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>Picada misma que 6260 y 6945</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I35" t="n">
@@ -3075,26 +3075,26 @@
         </is>
       </c>
       <c r="M35" t="n">
-        <v>-58.436298</v>
+        <v>-58.480925</v>
       </c>
       <c r="N35" t="n">
-        <v>-34.578972</v>
+        <v>-34.585471</v>
       </c>
       <c r="O35" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P35" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>6144</t>
+          <t>6143</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
@@ -3104,7 +3104,7 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>TURIN 2990</t>
+          <t>SOLANO LOPEZ, F., MARISCAL 2845</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
@@ -3114,7 +3114,7 @@
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>807458282</t>
+          <t>807458296</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
@@ -3151,10 +3151,10 @@
         </is>
       </c>
       <c r="M36" t="n">
-        <v>-58.480925</v>
+        <v>-58.495071</v>
       </c>
       <c r="N36" t="n">
-        <v>-34.585471</v>
+        <v>-34.593122</v>
       </c>
       <c r="O36" t="inlineStr">
         <is>
@@ -3170,27 +3170,27 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>6143</t>
+          <t>-478</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>6/11/2025</t>
+          <t>6/15/2025</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>SOLANO LOPEZ, F., MARISCAL 2845</t>
+          <t>Chivilcoy 4875</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>807458296</t>
+          <t>807508509</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
@@ -3205,7 +3205,7 @@
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Poste podrido</t>
         </is>
       </c>
       <c r="I37" t="n">
@@ -3223,14 +3223,14 @@
       </c>
       <c r="L37" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M37" t="n">
-        <v>-58.495071</v>
+        <v>-58.517389</v>
       </c>
       <c r="N37" t="n">
-        <v>-34.593122</v>
+        <v>-34.593541</v>
       </c>
       <c r="O37" t="inlineStr">
         <is>
@@ -3246,27 +3246,27 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>-478</t>
+          <t>6171</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>6/15/2025</t>
+          <t>6/18/2025</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Chivilcoy 4875</t>
+          <t>CABELLO 3486</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>807508509</t>
+          <t>807658640</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
@@ -3281,7 +3281,7 @@
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>Poste podrido</t>
+          <t>Columna inclinada evaluar con inspector un corrimiento</t>
         </is>
       </c>
       <c r="I38" t="n">
@@ -3299,40 +3299,40 @@
       </c>
       <c r="L38" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M38" t="n">
-        <v>-58.517389</v>
+        <v>-58.409579</v>
       </c>
       <c r="N38" t="n">
-        <v>-34.593541</v>
+        <v>-34.581134</v>
       </c>
       <c r="O38" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P38" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>6171</t>
+          <t>6230</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>6/18/2025</t>
+          <t>6/24/2025</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>CABELLO 3486</t>
+          <t>Santa maria de oro	2722</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
@@ -3342,7 +3342,7 @@
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>807658640</t>
+          <t>807763066</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
@@ -3357,7 +3357,7 @@
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>Columna inclinada evaluar con inspector un corrimiento</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I39" t="n">
@@ -3379,10 +3379,10 @@
         </is>
       </c>
       <c r="M39" t="n">
-        <v>-58.409579</v>
+        <v>-58.422315</v>
       </c>
       <c r="N39" t="n">
-        <v>-34.581134</v>
+        <v>-34.576988</v>
       </c>
       <c r="O39" t="inlineStr">
         <is>
@@ -3398,7 +3398,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>6230</t>
+          <t>6231</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
@@ -3408,7 +3408,7 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Santa maria de oro	2722</t>
+          <t>Ciudad de la Paz 275</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
@@ -3418,7 +3418,7 @@
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>807763066</t>
+          <t>807763070</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
@@ -3433,7 +3433,7 @@
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Aplomar o cambiar</t>
         </is>
       </c>
       <c r="I40" t="n">
@@ -3451,14 +3451,14 @@
       </c>
       <c r="L40" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M40" t="n">
-        <v>-58.422315</v>
+        <v>-58.441049</v>
       </c>
       <c r="N40" t="n">
-        <v>-34.576988</v>
+        <v>-34.574625</v>
       </c>
       <c r="O40" t="inlineStr">
         <is>
@@ -3474,7 +3474,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>6231</t>
+          <t>6235</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
@@ -3484,17 +3484,17 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Ciudad de la Paz 275</t>
+          <t>HUERGO 389</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>807763070</t>
+          <t>807763078</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
@@ -3509,7 +3509,7 @@
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>Aplomar o cambiar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I41" t="n">
@@ -3527,14 +3527,14 @@
       </c>
       <c r="L41" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M41" t="n">
-        <v>-58.441049</v>
+        <v>-58.432722</v>
       </c>
       <c r="N41" t="n">
-        <v>-34.574625</v>
+        <v>-34.572371</v>
       </c>
       <c r="O41" t="inlineStr">
         <is>
@@ -3550,27 +3550,27 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>6235</t>
+          <t>6295</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>6/24/2025</t>
+          <t>6/30/2025</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>HUERGO 389</t>
+          <t>SOLER 6017</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>807763078</t>
+          <t>807851636</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
@@ -3607,10 +3607,10 @@
         </is>
       </c>
       <c r="M42" t="n">
-        <v>-58.432722</v>
+        <v>-58.436808</v>
       </c>
       <c r="N42" t="n">
-        <v>-34.572371</v>
+        <v>-34.577464</v>
       </c>
       <c r="O42" t="inlineStr">
         <is>
@@ -3626,17 +3626,17 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>6295</t>
+          <t>6332</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>6/30/2025</t>
+          <t>7/3/2025</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>SOLER 6017</t>
+          <t>ARAOZ 2560</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
@@ -3646,7 +3646,7 @@
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>807851636</t>
+          <t>807965818</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
@@ -3683,10 +3683,10 @@
         </is>
       </c>
       <c r="M43" t="n">
-        <v>-58.436808</v>
+        <v>-58.414507</v>
       </c>
       <c r="N43" t="n">
-        <v>-34.577464</v>
+        <v>-34.585377</v>
       </c>
       <c r="O43" t="inlineStr">
         <is>
@@ -3702,27 +3702,27 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>6332</t>
+          <t>6506</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>7/3/2025</t>
+          <t>7/10/2025</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>ARAOZ 2560</t>
+          <t>Ohiggins 1611</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>807965818</t>
+          <t>808148679</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
@@ -3737,7 +3737,7 @@
       </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Columna podrida en la base</t>
         </is>
       </c>
       <c r="I44" t="n">
@@ -3750,7 +3750,7 @@
       </c>
       <c r="K44" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L44" t="inlineStr">
@@ -3759,46 +3759,46 @@
         </is>
       </c>
       <c r="M44" t="n">
-        <v>-58.414507</v>
+        <v>-58.448993</v>
       </c>
       <c r="N44" t="n">
-        <v>-34.585377</v>
+        <v>-34.564383</v>
       </c>
       <c r="O44" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P44" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>6506</t>
+          <t>6437</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>7/10/2025</t>
+          <t>7/17/2025</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Ohiggins 1611</t>
+          <t>MILLER 4590</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>808148679</t>
+          <t>808400306</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
@@ -3813,7 +3813,7 @@
       </c>
       <c r="H45" t="inlineStr">
         <is>
-          <t>Columna podrida en la base</t>
+          <t>Columna corroida</t>
         </is>
       </c>
       <c r="I45" t="n">
@@ -3826,7 +3826,7 @@
       </c>
       <c r="K45" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L45" t="inlineStr">
@@ -3835,14 +3835,14 @@
         </is>
       </c>
       <c r="M45" t="n">
-        <v>-58.448993</v>
+        <v>-58.495482</v>
       </c>
       <c r="N45" t="n">
-        <v>-34.564383</v>
+        <v>-34.552614</v>
       </c>
       <c r="O45" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P45" t="inlineStr">
@@ -3854,7 +3854,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>6437</t>
+          <t>6538</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
@@ -3864,7 +3864,7 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>MILLER 4590</t>
+          <t>Pedraza Manuela 4101</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
@@ -3874,7 +3874,7 @@
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>808400306</t>
+          <t>808400353</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
@@ -3889,7 +3889,7 @@
       </c>
       <c r="H46" t="inlineStr">
         <is>
-          <t>Columna corroida</t>
+          <t xml:space="preserve">Podrida en la base </t>
         </is>
       </c>
       <c r="I46" t="n">
@@ -3911,10 +3911,10 @@
         </is>
       </c>
       <c r="M46" t="n">
-        <v>-58.495482</v>
+        <v>-58.481569</v>
       </c>
       <c r="N46" t="n">
-        <v>-34.552614</v>
+        <v>-34.559853</v>
       </c>
       <c r="O46" t="inlineStr">
         <is>
@@ -3930,27 +3930,27 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>6538</t>
+          <t>7023</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>7/17/2025</t>
+          <t>7/22/2025</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Pedraza Manuela 4101</t>
+          <t>ZABALA 3573</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>808400353</t>
+          <t>808480549</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
@@ -3965,7 +3965,7 @@
       </c>
       <c r="H47" t="inlineStr">
         <is>
-          <t xml:space="preserve">Podrida en la base </t>
+          <t>Corroida en base para recambio</t>
         </is>
       </c>
       <c r="I47" t="n">
@@ -3987,14 +3987,14 @@
         </is>
       </c>
       <c r="M47" t="n">
-        <v>-58.481569</v>
+        <v>-58.457522</v>
       </c>
       <c r="N47" t="n">
-        <v>-34.559853</v>
+        <v>-34.579414</v>
       </c>
       <c r="O47" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P47" t="inlineStr">
@@ -4006,27 +4006,27 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>7023</t>
+          <t>6484</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>7/22/2025</t>
+          <t>7/24/2025</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>ZABALA 3573</t>
+          <t>URIARTE 2396</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>808480549</t>
+          <t>808509373</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
@@ -4041,7 +4041,7 @@
       </c>
       <c r="H48" t="inlineStr">
         <is>
-          <t>Corroida en base para recambio</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I48" t="n">
@@ -4063,36 +4063,36 @@
         </is>
       </c>
       <c r="M48" t="n">
-        <v>-58.457522</v>
+        <v>-58.423934</v>
       </c>
       <c r="N48" t="n">
-        <v>-34.579414</v>
+        <v>-34.581562</v>
       </c>
       <c r="O48" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P48" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>6484</t>
+          <t>6512</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>7/24/2025</t>
+          <t>7/28/2025</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>URIARTE 2396</t>
+          <t>GASCON 1195</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
@@ -4102,7 +4102,7 @@
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>808509373</t>
+          <t>808571975</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
@@ -4139,10 +4139,10 @@
         </is>
       </c>
       <c r="M49" t="n">
-        <v>-58.423934</v>
+        <v>-58.423127</v>
       </c>
       <c r="N49" t="n">
-        <v>-34.581562</v>
+        <v>-34.596476</v>
       </c>
       <c r="O49" t="inlineStr">
         <is>
@@ -4158,7 +4158,7 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>6512</t>
+          <t>6513</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
@@ -4168,7 +4168,7 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>GASCON 1195</t>
+          <t>DORREGO 1925</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
@@ -4178,7 +4178,7 @@
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>808571975</t>
+          <t>808571976</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
@@ -4215,10 +4215,10 @@
         </is>
       </c>
       <c r="M50" t="n">
-        <v>-58.423127</v>
+        <v>-58.441281</v>
       </c>
       <c r="N50" t="n">
-        <v>-34.596476</v>
+        <v>-34.579867</v>
       </c>
       <c r="O50" t="inlineStr">
         <is>
@@ -4234,7 +4234,7 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>6513</t>
+          <t>6519</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
@@ -4244,7 +4244,7 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>DORREGO 1925</t>
+          <t>SALGUERO, JERONIMO 2874</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
@@ -4254,7 +4254,7 @@
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>808571976</t>
+          <t>808571977</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
@@ -4269,7 +4269,7 @@
       </c>
       <c r="H51" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Reparar rienda</t>
         </is>
       </c>
       <c r="I51" t="n">
@@ -4277,7 +4277,7 @@
       </c>
       <c r="J51" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Tensor</t>
         </is>
       </c>
       <c r="K51" t="inlineStr">
@@ -4287,14 +4287,14 @@
       </c>
       <c r="L51" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M51" t="n">
-        <v>-58.441281</v>
+        <v>-58.407256</v>
       </c>
       <c r="N51" t="n">
-        <v>-34.579867</v>
+        <v>-34.578976</v>
       </c>
       <c r="O51" t="inlineStr">
         <is>
@@ -4310,27 +4310,27 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>6519</t>
+          <t>-538</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>7/28/2025</t>
+          <t>7/31/2025</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>SALGUERO, JERONIMO 2874</t>
+          <t>Malabia 964</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>808571977</t>
+          <t>808609237</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
@@ -4345,7 +4345,7 @@
       </c>
       <c r="H52" t="inlineStr">
         <is>
-          <t>Reparar rienda</t>
+          <t>Cambiar poste mal estado por PRFV</t>
         </is>
       </c>
       <c r="I52" t="n">
@@ -4353,7 +4353,7 @@
       </c>
       <c r="J52" t="inlineStr">
         <is>
-          <t>Tensor</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K52" t="inlineStr">
@@ -4363,14 +4363,14 @@
       </c>
       <c r="L52" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M52" t="n">
-        <v>-58.407256</v>
+        <v>-58.433634</v>
       </c>
       <c r="N52" t="n">
-        <v>-34.578976</v>
+        <v>-34.595018</v>
       </c>
       <c r="O52" t="inlineStr">
         <is>
@@ -4386,27 +4386,27 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>-538</t>
+          <t>-547</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>7/31/2025</t>
+          <t>8/6/2025</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>Malabia 964</t>
+          <t>Habana 4210</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>808609237</t>
+          <t>808733921</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
@@ -4421,7 +4421,7 @@
       </c>
       <c r="H53" t="inlineStr">
         <is>
-          <t>Cambiar poste mal estado por PRFV</t>
+          <t>Cambiar poste dañado</t>
         </is>
       </c>
       <c r="I53" t="n">
@@ -4443,46 +4443,46 @@
         </is>
       </c>
       <c r="M53" t="n">
-        <v>-58.433634</v>
+        <v>-58.515873</v>
       </c>
       <c r="N53" t="n">
-        <v>-34.595018</v>
+        <v>-34.599425</v>
       </c>
       <c r="O53" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P53" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>6498</t>
+          <t>6579</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>8/6/2025</t>
+          <t>8/7/2025</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>BUCARELLI 2087</t>
+          <t>RIVADAVIA MARTIN, COMODORO 1350</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>808733908</t>
+          <t>808749184</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
@@ -4497,7 +4497,7 @@
       </c>
       <c r="H54" t="inlineStr">
         <is>
-          <t>Base picada</t>
+          <t>Poste inclinado</t>
         </is>
       </c>
       <c r="I54" t="n">
@@ -4505,7 +4505,7 @@
       </c>
       <c r="J54" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K54" t="inlineStr">
@@ -4515,18 +4515,18 @@
       </c>
       <c r="L54" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M54" t="n">
-        <v>-58.485592</v>
+        <v>-58.461024</v>
       </c>
       <c r="N54" t="n">
-        <v>-34.578586</v>
+        <v>-34.539409</v>
       </c>
       <c r="O54" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P54" t="inlineStr">
@@ -4538,27 +4538,27 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>-547</t>
+          <t>6906</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>8/6/2025</t>
+          <t>8/12/2025</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>Habana 4210</t>
+          <t>MOSCONI GENERAL AV. 3163</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>808733921</t>
+          <t>808918685</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
@@ -4573,7 +4573,7 @@
       </c>
       <c r="H55" t="inlineStr">
         <is>
-          <t>Cambiar poste dañado</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I55" t="n">
@@ -4591,14 +4591,14 @@
       </c>
       <c r="L55" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M55" t="n">
-        <v>-58.515873</v>
+        <v>-58.505731</v>
       </c>
       <c r="N55" t="n">
-        <v>-34.599425</v>
+        <v>-34.588316</v>
       </c>
       <c r="O55" t="inlineStr">
         <is>
@@ -4614,27 +4614,27 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>6579</t>
+          <t>6910</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>8/7/2025</t>
+          <t>8/12/2025</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>RIVADAVIA MARTIN, COMODORO 1350</t>
+          <t>RIVAS, GRAL. 2345</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>808749184</t>
+          <t>808918698</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
@@ -4649,7 +4649,7 @@
       </c>
       <c r="H56" t="inlineStr">
         <is>
-          <t>Poste inclinado</t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I56" t="n">
@@ -4657,7 +4657,7 @@
       </c>
       <c r="J56" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K56" t="inlineStr">
@@ -4667,18 +4667,18 @@
       </c>
       <c r="L56" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M56" t="n">
-        <v>-58.461024</v>
+        <v>-58.482497</v>
       </c>
       <c r="N56" t="n">
-        <v>-34.539409</v>
+        <v>-34.598714</v>
       </c>
       <c r="O56" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P56" t="inlineStr">
@@ -4690,7 +4690,7 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>6906</t>
+          <t>6928</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
@@ -4700,7 +4700,7 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>MOSCONI GENERAL AV. 3163</t>
+          <t>ALBARELLOS AV. 3101</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
@@ -4710,7 +4710,7 @@
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>808918685</t>
+          <t>808918710</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
@@ -4747,10 +4747,10 @@
         </is>
       </c>
       <c r="M57" t="n">
-        <v>-58.505731</v>
+        <v>-58.512623</v>
       </c>
       <c r="N57" t="n">
-        <v>-34.588316</v>
+        <v>-34.579137</v>
       </c>
       <c r="O57" t="inlineStr">
         <is>
@@ -4766,7 +4766,7 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>6910</t>
+          <t>-550</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
@@ -4776,17 +4776,17 @@
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>RIVAS, GRAL. 2345</t>
+          <t>Fitz roy 267</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>808918698</t>
+          <t>808918720</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
@@ -4801,7 +4801,7 @@
       </c>
       <c r="H58" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>Aplomar columna</t>
         </is>
       </c>
       <c r="I58" t="n">
@@ -4823,10 +4823,10 @@
         </is>
       </c>
       <c r="M58" t="n">
-        <v>-58.482497</v>
+        <v>-58.451378</v>
       </c>
       <c r="N58" t="n">
-        <v>-34.598714</v>
+        <v>-34.596195</v>
       </c>
       <c r="O58" t="inlineStr">
         <is>
@@ -4842,27 +4842,27 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>6928</t>
+          <t>6943</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>8/12/2025</t>
+          <t>8/14/2025</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>ALBARELLOS AV. 3101</t>
+          <t>SUPERI 1459</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>808918710</t>
+          <t>808972965</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
@@ -4877,7 +4877,7 @@
       </c>
       <c r="H59" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Poste con base quebrada ver si es posible desmonte</t>
         </is>
       </c>
       <c r="I59" t="n">
@@ -4885,7 +4885,7 @@
       </c>
       <c r="J59" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Desmonte</t>
         </is>
       </c>
       <c r="K59" t="inlineStr">
@@ -4895,18 +4895,18 @@
       </c>
       <c r="L59" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M59" t="n">
-        <v>-58.512623</v>
+        <v>-58.460834</v>
       </c>
       <c r="N59" t="n">
-        <v>-34.579137</v>
+        <v>-34.573753</v>
       </c>
       <c r="O59" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P59" t="inlineStr">
@@ -4918,27 +4918,27 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>6939</t>
+          <t>6969</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>8/12/2025</t>
+          <t>8/14/2025</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>ANDONAEGUI 1894</t>
+          <t>CIUDAD DE LA PAZ 295</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>808918715</t>
+          <t>808972995</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
@@ -4975,46 +4975,46 @@
         </is>
       </c>
       <c r="M60" t="n">
-        <v>-58.484848</v>
+        <v>-58.441171</v>
       </c>
       <c r="N60" t="n">
-        <v>-34.581325</v>
+        <v>-34.574547</v>
       </c>
       <c r="O60" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P60" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>-550</t>
+          <t>6971</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>8/12/2025</t>
+          <t>8/14/2025</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>Fitz roy 267</t>
+          <t>MAURE 1594</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>808918720</t>
+          <t>808973001</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
@@ -5029,7 +5029,7 @@
       </c>
       <c r="H61" t="inlineStr">
         <is>
-          <t>Aplomar columna</t>
+          <t>Ver de traspasar a telecentro y  desmontar ver con inspector</t>
         </is>
       </c>
       <c r="I61" t="n">
@@ -5051,46 +5051,46 @@
         </is>
       </c>
       <c r="M61" t="n">
-        <v>-58.451378</v>
+        <v>-58.435072</v>
       </c>
       <c r="N61" t="n">
-        <v>-34.596195</v>
+        <v>-34.565732</v>
       </c>
       <c r="O61" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P61" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>6943</t>
+          <t>7000</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>8/14/2025</t>
+          <t>8/20/2025</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>SUPERI 1459</t>
+          <t>SCALABRINI ORTIZ, RAUL AV. 2106</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>808972965</t>
+          <t>809065867</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
@@ -5105,7 +5105,7 @@
       </c>
       <c r="H62" t="inlineStr">
         <is>
-          <t>Poste con base quebrada ver si es posible desmonte</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I62" t="n">
@@ -5113,7 +5113,7 @@
       </c>
       <c r="J62" t="inlineStr">
         <is>
-          <t>Desmonte</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K62" t="inlineStr">
@@ -5123,50 +5123,50 @@
       </c>
       <c r="L62" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M62" t="n">
-        <v>-58.460834</v>
+        <v>-58.420109</v>
       </c>
       <c r="N62" t="n">
-        <v>-34.573753</v>
+        <v>-34.58764</v>
       </c>
       <c r="O62" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P62" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>6969</t>
+          <t>7003</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>8/14/2025</t>
+          <t>8/20/2025</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>CIUDAD DE LA PAZ 295</t>
+          <t>MELIAN AV. 2576</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>808972995</t>
+          <t>809065874</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
@@ -5181,7 +5181,7 @@
       </c>
       <c r="H63" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I63" t="n">
@@ -5203,46 +5203,46 @@
         </is>
       </c>
       <c r="M63" t="n">
-        <v>-58.441171</v>
+        <v>-58.471943</v>
       </c>
       <c r="N63" t="n">
-        <v>-34.574547</v>
+        <v>-34.564948</v>
       </c>
       <c r="O63" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P63" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>6971</t>
+          <t>-559</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>8/14/2025</t>
+          <t>8/21/2025</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>MAURE 1594</t>
+          <t>Av. Del Libertador 6736</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>808973001</t>
+          <t>809098713</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
@@ -5257,7 +5257,7 @@
       </c>
       <c r="H64" t="inlineStr">
         <is>
-          <t>Ver de traspasar a telecentro y  desmontar ver con inspector</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I64" t="n">
@@ -5279,46 +5279,46 @@
         </is>
       </c>
       <c r="M64" t="n">
-        <v>-58.435072</v>
+        <v>-58.453398</v>
       </c>
       <c r="N64" t="n">
-        <v>-34.565732</v>
+        <v>-34.550238</v>
       </c>
       <c r="O64" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P64" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>7000</t>
+          <t>5503</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>8/20/2025</t>
+          <t>8/22/2025</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>SCALABRINI ORTIZ, RAUL AV. 2106</t>
+          <t>CRAMER AV. 1771</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>809065867</t>
+          <t>809102564</t>
         </is>
       </c>
       <c r="F65" t="inlineStr">
@@ -5333,7 +5333,7 @@
       </c>
       <c r="H65" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>PIcada</t>
         </is>
       </c>
       <c r="I65" t="n">
@@ -5355,36 +5355,36 @@
         </is>
       </c>
       <c r="M65" t="n">
-        <v>-58.420109</v>
+        <v>-58.458506</v>
       </c>
       <c r="N65" t="n">
-        <v>-34.58764</v>
+        <v>-34.56783</v>
       </c>
       <c r="O65" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P65" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>7003</t>
+          <t>7098</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>8/20/2025</t>
+          <t>8/25/2025</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>MELIAN AV. 2576</t>
+          <t>UGARTE, MANUEL 3484</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
@@ -5394,7 +5394,7 @@
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>809065874</t>
+          <t>809126236</t>
         </is>
       </c>
       <c r="F66" t="inlineStr">
@@ -5431,10 +5431,10 @@
         </is>
       </c>
       <c r="M66" t="n">
-        <v>-58.471943</v>
+        <v>-58.472869</v>
       </c>
       <c r="N66" t="n">
-        <v>-34.564948</v>
+        <v>-34.562</v>
       </c>
       <c r="O66" t="inlineStr">
         <is>
@@ -5450,27 +5450,27 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>-558</t>
+          <t>7080</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>8/21/2025</t>
+          <t>8/25/2025</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>Blanco Encalada 4210</t>
+          <t>UGARTE, MANUEL 2196</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>ICD30461848</t>
+          <t>809125906</t>
         </is>
       </c>
       <c r="F67" t="inlineStr">
@@ -5485,7 +5485,7 @@
       </c>
       <c r="H67" t="inlineStr">
         <is>
-          <t>Colocar columna R400 para pedir taspaso de fuente telecom</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I67" t="n">
@@ -5498,7 +5498,7 @@
       </c>
       <c r="K67" t="inlineStr">
         <is>
-          <t>Fuente Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L67" t="inlineStr">
@@ -5507,14 +5507,14 @@
         </is>
       </c>
       <c r="M67" t="n">
-        <v>-58.477593</v>
+        <v>-58.459402</v>
       </c>
       <c r="N67" t="n">
-        <v>-34.570321</v>
+        <v>-34.555262</v>
       </c>
       <c r="O67" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P67" t="inlineStr">
@@ -5526,27 +5526,27 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>-559</t>
+          <t>7021</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>8/21/2025</t>
+          <t>8/25/2025</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>Av. Del Libertador 6736</t>
+          <t>VERA 445</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>809098713</t>
+          <t>809155622</t>
         </is>
       </c>
       <c r="F68" t="inlineStr">
@@ -5561,7 +5561,7 @@
       </c>
       <c r="H68" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Correrla para sacarla del cantero</t>
         </is>
       </c>
       <c r="I68" t="n">
@@ -5583,46 +5583,46 @@
         </is>
       </c>
       <c r="M68" t="n">
-        <v>-58.453398</v>
+        <v>-58.437181</v>
       </c>
       <c r="N68" t="n">
-        <v>-34.550238</v>
+        <v>-34.5995</v>
       </c>
       <c r="O68" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P68" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>5503</t>
+          <t>6465</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>8/22/2025</t>
+          <t>8/28/2025</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>CRAMER AV. 1771</t>
+          <t>AGUIRRE 368</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>809102564</t>
+          <t>809268249</t>
         </is>
       </c>
       <c r="F69" t="inlineStr">
@@ -5637,7 +5637,7 @@
       </c>
       <c r="H69" t="inlineStr">
         <is>
-          <t>PIcada</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I69" t="n">
@@ -5659,46 +5659,46 @@
         </is>
       </c>
       <c r="M69" t="n">
-        <v>-58.458506</v>
+        <v>-58.434651</v>
       </c>
       <c r="N69" t="n">
-        <v>-34.56783</v>
+        <v>-34.598814</v>
       </c>
       <c r="O69" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P69" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>7098</t>
+          <t>7095</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>8/25/2025</t>
+          <t>8/28/2025</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>UGARTE, MANUEL 3484</t>
+          <t>SAN MARTIN AV. 4515</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>809126236</t>
+          <t>809268240</t>
         </is>
       </c>
       <c r="F70" t="inlineStr">
@@ -5713,7 +5713,7 @@
       </c>
       <c r="H70" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Columna chocada</t>
         </is>
       </c>
       <c r="I70" t="n">
@@ -5731,18 +5731,18 @@
       </c>
       <c r="L70" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M70" t="n">
-        <v>-58.472869</v>
+        <v>-58.483415</v>
       </c>
       <c r="N70" t="n">
-        <v>-34.562</v>
+        <v>-34.597663</v>
       </c>
       <c r="O70" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P70" t="inlineStr">
@@ -5754,17 +5754,17 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>7080</t>
+          <t>-575</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>8/25/2025</t>
+          <t>8/28/2025</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>UGARTE, MANUEL 2196</t>
+          <t>Amenabar 3064</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
@@ -5774,7 +5774,7 @@
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>809125906</t>
+          <t>809281299</t>
         </is>
       </c>
       <c r="F71" t="inlineStr">
@@ -5811,10 +5811,10 @@
         </is>
       </c>
       <c r="M71" t="n">
-        <v>-58.459402</v>
+        <v>-58.465984</v>
       </c>
       <c r="N71" t="n">
-        <v>-34.555262</v>
+        <v>-34.554869</v>
       </c>
       <c r="O71" t="inlineStr">
         <is>
@@ -5830,27 +5830,27 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>7021</t>
+          <t>4166</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>8/25/2025</t>
+          <t>8/29/2025</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>VERA 445</t>
+          <t>ALTOLAGUIRRE 2201</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>809155622</t>
+          <t>809309591</t>
         </is>
       </c>
       <c r="F72" t="inlineStr">
@@ -5865,7 +5865,7 @@
       </c>
       <c r="H72" t="inlineStr">
         <is>
-          <t>Correrla para sacarla del cantero</t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I72" t="n">
@@ -5887,46 +5887,46 @@
         </is>
       </c>
       <c r="M72" t="n">
-        <v>-58.437181</v>
+        <v>-58.489622</v>
       </c>
       <c r="N72" t="n">
-        <v>-34.5995</v>
+        <v>-34.578426</v>
       </c>
       <c r="O72" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P72" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>6465</t>
+          <t>-576</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>8/28/2025</t>
+          <t>8/29/2025</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>AGUIRRE 368</t>
+          <t>Av. Boyacá 2030</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>809268249</t>
+          <t>809309606</t>
         </is>
       </c>
       <c r="F73" t="inlineStr">
@@ -5963,46 +5963,46 @@
         </is>
       </c>
       <c r="M73" t="n">
-        <v>-58.434651</v>
+        <v>-58.471173</v>
       </c>
       <c r="N73" t="n">
-        <v>-34.598814</v>
+        <v>-34.60704</v>
       </c>
       <c r="O73" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P73" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>7095</t>
+          <t>7111</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>8/28/2025</t>
+          <t>9/1/2025</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>SAN MARTIN AV. 4515</t>
+          <t>VILELA 3699</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>809268240</t>
+          <t>809371823</t>
         </is>
       </c>
       <c r="F74" t="inlineStr">
@@ -6017,7 +6017,7 @@
       </c>
       <c r="H74" t="inlineStr">
         <is>
-          <t>Columna chocada</t>
+          <t xml:space="preserve">Cambiar </t>
         </is>
       </c>
       <c r="I74" t="n">
@@ -6039,14 +6039,14 @@
         </is>
       </c>
       <c r="M74" t="n">
-        <v>-58.483415</v>
+        <v>-58.482817</v>
       </c>
       <c r="N74" t="n">
-        <v>-34.597663</v>
+        <v>-34.550845</v>
       </c>
       <c r="O74" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P74" t="inlineStr">
@@ -6058,27 +6058,27 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>-575</t>
+          <t>7118</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>8/28/2025</t>
+          <t>9/2/2025</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>Amenabar 3064</t>
+          <t>CUBAS, JOSE 2211</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>809281299</t>
+          <t>809406168</t>
         </is>
       </c>
       <c r="F75" t="inlineStr">
@@ -6115,14 +6115,14 @@
         </is>
       </c>
       <c r="M75" t="n">
-        <v>-58.465984</v>
+        <v>-58.492448</v>
       </c>
       <c r="N75" t="n">
-        <v>-34.554869</v>
+        <v>-34.58372</v>
       </c>
       <c r="O75" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P75" t="inlineStr">
@@ -6134,27 +6134,27 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>4166</t>
+          <t>-577</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>8/29/2025</t>
+          <t>9/2/2025</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>ALTOLAGUIRRE 2201</t>
+          <t>Manuel Ugarte 2318</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>809309591</t>
+          <t>809406177</t>
         </is>
       </c>
       <c r="F76" t="inlineStr">
@@ -6169,7 +6169,7 @@
       </c>
       <c r="H76" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I76" t="n">
@@ -6191,14 +6191,14 @@
         </is>
       </c>
       <c r="M76" t="n">
-        <v>-58.489622</v>
+        <v>-58.460635</v>
       </c>
       <c r="N76" t="n">
-        <v>-34.578426</v>
+        <v>-34.555932</v>
       </c>
       <c r="O76" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P76" t="inlineStr">
@@ -6210,27 +6210,27 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>-576</t>
+          <t>-578</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>8/29/2025</t>
+          <t>9/2/2025</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>Av. Boyacá 2030</t>
+          <t>Pedro I Rivera 2536</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>809309606</t>
+          <t>809406189</t>
         </is>
       </c>
       <c r="F77" t="inlineStr">
@@ -6267,14 +6267,14 @@
         </is>
       </c>
       <c r="M77" t="n">
-        <v>-58.471173</v>
+        <v>-58.462327</v>
       </c>
       <c r="N77" t="n">
-        <v>-34.60704</v>
+        <v>-34.557565</v>
       </c>
       <c r="O77" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P77" t="inlineStr">
@@ -6286,27 +6286,27 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>7111</t>
+          <t>-579</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>9/1/2025</t>
+          <t>9/2/2025</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>VILELA 3699</t>
+          <t>Pedro Rivera 2546</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>809371823</t>
+          <t>Pendiente ADM</t>
         </is>
       </c>
       <c r="F78" t="inlineStr">
@@ -6321,7 +6321,7 @@
       </c>
       <c r="H78" t="inlineStr">
         <is>
-          <t xml:space="preserve">Cambiar </t>
+          <t>Colocar R200 para pedir traspaso de equipos</t>
         </is>
       </c>
       <c r="I78" t="n">
@@ -6334,19 +6334,19 @@
       </c>
       <c r="K78" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L78" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M78" t="n">
-        <v>-58.482817</v>
+        <v>-58.462479</v>
       </c>
       <c r="N78" t="n">
-        <v>-34.550845</v>
+        <v>-34.55765</v>
       </c>
       <c r="O78" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-09-02 19:33:57)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_NEW.xlsx
+++ b/mapa_interactivo_NEW.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P78"/>
+  <dimension ref="A1:P76"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -898,27 +898,27 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>4662</t>
+          <t>4862</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>1/21/2025</t>
+          <t>1/23/2025</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>ALTOLAGUIRRE 2397</t>
+          <t>ARCOS 2263</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>802823938</t>
+          <t>802857379</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -928,25 +928,25 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>Inclinada</t>
+          <t>picada</t>
         </is>
       </c>
       <c r="I7" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L7" t="inlineStr">
@@ -955,14 +955,14 @@
         </is>
       </c>
       <c r="M7" t="n">
-        <v>-58.490766</v>
+        <v>-58.455082</v>
       </c>
       <c r="N7" t="n">
-        <v>-34.576987</v>
+        <v>-34.558883</v>
       </c>
       <c r="O7" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P7" t="inlineStr">
@@ -974,27 +974,27 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>4862</t>
+          <t>6036</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>1/23/2025</t>
+          <t>2/24/2025</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>ARCOS 2263</t>
+          <t>MEDRANO 1715</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>802857379</t>
+          <t>803608181</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -1004,14 +1004,10 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
-        </is>
-      </c>
-      <c r="H8" t="inlineStr">
-        <is>
-          <t>picada</t>
-        </is>
-      </c>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr"/>
       <c r="I8" t="n">
         <v>0</v>
       </c>
@@ -1031,26 +1027,26 @@
         </is>
       </c>
       <c r="M8" t="n">
-        <v>-58.455082</v>
+        <v>-58.418236</v>
       </c>
       <c r="N8" t="n">
-        <v>-34.558883</v>
+        <v>-34.589859</v>
       </c>
       <c r="O8" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P8" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>6036</t>
+          <t>803608480</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -1060,7 +1056,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>MEDRANO 1715</t>
+          <t>GUATEMALA /ALT/ 4415</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -1070,7 +1066,7 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>803608181</t>
+          <t>803608480</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -1083,7 +1079,11 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H9" t="inlineStr"/>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Guatemala 4415 </t>
+        </is>
+      </c>
       <c r="I9" t="n">
         <v>0</v>
       </c>
@@ -1094,7 +1094,7 @@
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L9" t="inlineStr">
@@ -1103,10 +1103,10 @@
         </is>
       </c>
       <c r="M9" t="n">
-        <v>-58.418236</v>
+        <v>-58.421661</v>
       </c>
       <c r="N9" t="n">
-        <v>-34.589859</v>
+        <v>-34.588428</v>
       </c>
       <c r="O9" t="inlineStr">
         <is>
@@ -1122,27 +1122,27 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>803608480</t>
+          <t>5053</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>2/24/2025</t>
+          <t>3/11/2025</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>GUATEMALA /ALT/ 4415</t>
+          <t>MENDOZA 1153</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>803608480</t>
+          <t>803969314</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
@@ -1157,7 +1157,7 @@
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t xml:space="preserve">Guatemala 4415 </t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="I10" t="n">
@@ -1175,50 +1175,50 @@
       </c>
       <c r="L10" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M10" t="n">
-        <v>-58.421661</v>
+        <v>-58.44463</v>
       </c>
       <c r="N10" t="n">
-        <v>-34.588428</v>
+        <v>-34.553354</v>
       </c>
       <c r="O10" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P10" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>5053</t>
+          <t>6071</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>3/11/2025</t>
+          <t>3/17/2025</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>MENDOZA 1153</t>
+          <t>OSORIO 4994</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>803969314</t>
+          <t>804053324</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
@@ -1231,11 +1231,7 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H11" t="inlineStr">
-        <is>
-          <t>Poste</t>
-        </is>
-      </c>
+      <c r="H11" t="inlineStr"/>
       <c r="I11" t="n">
         <v>0</v>
       </c>
@@ -1251,18 +1247,18 @@
       </c>
       <c r="L11" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M11" t="n">
-        <v>-58.44463</v>
+        <v>-58.466241</v>
       </c>
       <c r="N11" t="n">
-        <v>-34.553354</v>
+        <v>-34.595741</v>
       </c>
       <c r="O11" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P11" t="inlineStr">
@@ -1274,27 +1270,27 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>6071</t>
+          <t>3348</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>3/17/2025</t>
+          <t>3/27/2025</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>OSORIO 4994</t>
+          <t>ESTOMBA 2626</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>804053324</t>
+          <t>804309704</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
@@ -1307,13 +1303,17 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H12" t="inlineStr"/>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>Picada</t>
+        </is>
+      </c>
       <c r="I12" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Desmonte</t>
         </is>
       </c>
       <c r="K12" t="inlineStr">
@@ -1327,14 +1327,14 @@
         </is>
       </c>
       <c r="M12" t="n">
-        <v>-58.466241</v>
+        <v>-58.47538</v>
       </c>
       <c r="N12" t="n">
-        <v>-34.595741</v>
+        <v>-34.566015</v>
       </c>
       <c r="O12" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P12" t="inlineStr">
@@ -1346,27 +1346,27 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>3348</t>
+          <t>-312</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>3/27/2025</t>
+          <t>3/29/2025</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>ESTOMBA 2626</t>
+          <t>MATIENZO BENJAMIN /ALT/ 1831</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>804309704</t>
+          <t>804333522</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
@@ -1381,20 +1381,20 @@
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Retirar columna ya traspasaron el nodo</t>
         </is>
       </c>
       <c r="I13" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>Desmonte</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L13" t="inlineStr">
@@ -1403,46 +1403,46 @@
         </is>
       </c>
       <c r="M13" t="n">
-        <v>-58.47538</v>
+        <v>-58.434835</v>
       </c>
       <c r="N13" t="n">
-        <v>-34.566015</v>
+        <v>-34.569129</v>
       </c>
       <c r="O13" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P13" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>-312</t>
+          <t>3430</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>3/29/2025</t>
+          <t>4/1/2025</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>MATIENZO BENJAMIN /ALT/ 1831</t>
+          <t>MONROE 3838</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>804333522</t>
+          <t>804468442</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
@@ -1457,68 +1457,68 @@
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>Retirar columna ya traspasaron el nodo</t>
+          <t>Reparar rienda</t>
         </is>
       </c>
       <c r="I14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Tensor</t>
         </is>
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L14" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M14" t="n">
-        <v>-58.434835</v>
+        <v>-58.473659</v>
       </c>
       <c r="N14" t="n">
-        <v>-34.569129</v>
+        <v>-34.566979</v>
       </c>
       <c r="O14" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P14" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>3430</t>
+          <t>5464</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>4/1/2025</t>
+          <t>4/4/2025</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>MONROE 3838</t>
+          <t>SUCRE, ANTONIO JOSE DE, MCAL. 3100</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>804468442</t>
+          <t>804497880</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
@@ -1533,7 +1533,7 @@
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>Reparar rienda</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I15" t="n">
@@ -1541,7 +1541,7 @@
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>Tensor</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K15" t="inlineStr">
@@ -1555,10 +1555,10 @@
         </is>
       </c>
       <c r="M15" t="n">
-        <v>-58.473659</v>
+        <v>-58.46161</v>
       </c>
       <c r="N15" t="n">
-        <v>-34.566979</v>
+        <v>-34.567849</v>
       </c>
       <c r="O15" t="inlineStr">
         <is>
@@ -1574,7 +1574,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>5464</t>
+          <t>5469</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -1584,17 +1584,17 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>SUCRE, ANTONIO JOSE DE, MCAL. 3100</t>
+          <t>ESTADO PLURINACIONAL DE BOLIVIA 5899</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>804497880</t>
+          <t>804497887</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
@@ -1609,7 +1609,7 @@
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Aplomar</t>
         </is>
       </c>
       <c r="I16" t="n">
@@ -1617,7 +1617,7 @@
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K16" t="inlineStr">
@@ -1631,14 +1631,14 @@
         </is>
       </c>
       <c r="M16" t="n">
-        <v>-58.46161</v>
+        <v>-58.507746</v>
       </c>
       <c r="N16" t="n">
-        <v>-34.567849</v>
+        <v>-34.574217</v>
       </c>
       <c r="O16" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P16" t="inlineStr">
@@ -1650,7 +1650,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>5469</t>
+          <t>5492</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -1660,7 +1660,7 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>ESTADO PLURINACIONAL DE BOLIVIA 5899</t>
+          <t>ESTADO PLURINACIONAL DE BOLIVIA 5920</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
@@ -1670,7 +1670,7 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>804497887</t>
+          <t>804498035</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
@@ -1685,7 +1685,7 @@
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>Aplomar</t>
+          <t>aplomar</t>
         </is>
       </c>
       <c r="I17" t="n">
@@ -1707,10 +1707,10 @@
         </is>
       </c>
       <c r="M17" t="n">
-        <v>-58.507746</v>
+        <v>-58.50751</v>
       </c>
       <c r="N17" t="n">
-        <v>-34.574217</v>
+        <v>-34.574543</v>
       </c>
       <c r="O17" t="inlineStr">
         <is>
@@ -1726,17 +1726,17 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>5492</t>
+          <t>5599</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>4/4/2025</t>
+          <t>4/15/2025</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>ESTADO PLURINACIONAL DE BOLIVIA 5920</t>
+          <t>ESTOMBA 4052</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
@@ -1746,7 +1746,7 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>804498035</t>
+          <t>804732246</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
@@ -1761,7 +1761,7 @@
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>aplomar</t>
+          <t>Columna PRFV quedo inclinada (la hicieron como estomba 4056)</t>
         </is>
       </c>
       <c r="I18" t="n">
@@ -1774,23 +1774,23 @@
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo TLC</t>
         </is>
       </c>
       <c r="L18" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M18" t="n">
-        <v>-58.50751</v>
+        <v>-58.485407</v>
       </c>
       <c r="N18" t="n">
-        <v>-34.574543</v>
+        <v>-34.552985</v>
       </c>
       <c r="O18" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P18" t="inlineStr">
@@ -1802,7 +1802,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>5599</t>
+          <t>5590</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -1812,17 +1812,17 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>ESTOMBA 4052</t>
+          <t>O'HIGGINS 2441</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>804732246</t>
+          <t>804732275</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
@@ -1837,7 +1837,7 @@
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>Columna PRFV quedo inclinada (la hicieron como estomba 4056)</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I19" t="n">
@@ -1845,12 +1845,12 @@
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>Nodo TLC</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L19" t="inlineStr">
@@ -1859,10 +1859,10 @@
         </is>
       </c>
       <c r="M19" t="n">
-        <v>-58.485407</v>
+        <v>-58.45573</v>
       </c>
       <c r="N19" t="n">
-        <v>-34.552985</v>
+        <v>-34.556576</v>
       </c>
       <c r="O19" t="inlineStr">
         <is>
@@ -1878,27 +1878,27 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>5590</t>
+          <t>804787368</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>4/15/2025</t>
+          <t>4/17/2025</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>O'HIGGINS 2441</t>
+          <t>San Blas 2591</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>804732275</t>
+          <t>804787368</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
@@ -1935,14 +1935,14 @@
         </is>
       </c>
       <c r="M20" t="n">
-        <v>-58.45573</v>
+        <v>-58.477427</v>
       </c>
       <c r="N20" t="n">
-        <v>-34.556576</v>
+        <v>-34.609261</v>
       </c>
       <c r="O20" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P20" t="inlineStr">
@@ -1954,27 +1954,27 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>804787368</t>
+          <t>5624</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>4/17/2025</t>
+          <t>4/22/2025</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>San Blas 2591</t>
+          <t>PINO, VIRREY DEL 3456</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>804787368</t>
+          <t>804876043</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
@@ -1989,7 +1989,7 @@
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Desmonte de poste</t>
         </is>
       </c>
       <c r="I21" t="n">
@@ -1997,7 +1997,7 @@
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Desmonte</t>
         </is>
       </c>
       <c r="K21" t="inlineStr">
@@ -2007,18 +2007,18 @@
       </c>
       <c r="L21" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M21" t="n">
-        <v>-58.477427</v>
+        <v>-58.464354</v>
       </c>
       <c r="N21" t="n">
-        <v>-34.609261</v>
+        <v>-34.572486</v>
       </c>
       <c r="O21" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P21" t="inlineStr">
@@ -2030,17 +2030,17 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>5624</t>
+          <t>804922147</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>4/22/2025</t>
+          <t>4/24/2025</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>PINO, VIRREY DEL 3456</t>
+          <t>Av. Álvarez Thomas 1171</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
@@ -2050,7 +2050,7 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>804876043</t>
+          <t>804922147</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
@@ -2065,15 +2065,15 @@
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>Desmonte de poste</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I22" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J22" t="inlineStr">
         <is>
-          <t>Desmonte</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K22" t="inlineStr">
@@ -2083,14 +2083,14 @@
       </c>
       <c r="L22" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M22" t="n">
-        <v>-58.464354</v>
+        <v>-58.45793</v>
       </c>
       <c r="N22" t="n">
-        <v>-34.572486</v>
+        <v>-34.578334</v>
       </c>
       <c r="O22" t="inlineStr">
         <is>
@@ -2106,7 +2106,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>804922147</t>
+          <t>804922171</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -2116,7 +2116,7 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Av. Álvarez Thomas 1171</t>
+          <t>Virrey Arredondo 3581</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
@@ -2126,7 +2126,7 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>804922147</t>
+          <t>804922171</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
@@ -2141,15 +2141,15 @@
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Aplomar</t>
         </is>
       </c>
       <c r="I23" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K23" t="inlineStr">
@@ -2159,14 +2159,14 @@
       </c>
       <c r="L23" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M23" t="n">
-        <v>-58.45793</v>
+        <v>-58.459513</v>
       </c>
       <c r="N23" t="n">
-        <v>-34.578334</v>
+        <v>-34.578019</v>
       </c>
       <c r="O23" t="inlineStr">
         <is>
@@ -2182,7 +2182,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>804922171</t>
+          <t>5656</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -2192,17 +2192,17 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Virrey Arredondo 3581</t>
+          <t>ECHEVERRIA 5893</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>804922171</t>
+          <t>804922184</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
@@ -2217,7 +2217,7 @@
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>Aplomar</t>
+          <t>Poste con base quebrada</t>
         </is>
       </c>
       <c r="I24" t="n">
@@ -2225,7 +2225,7 @@
       </c>
       <c r="J24" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Desmonte</t>
         </is>
       </c>
       <c r="K24" t="inlineStr">
@@ -2235,18 +2235,18 @@
       </c>
       <c r="L24" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M24" t="n">
-        <v>-58.459513</v>
+        <v>-58.489627</v>
       </c>
       <c r="N24" t="n">
-        <v>-34.578019</v>
+        <v>-34.583761</v>
       </c>
       <c r="O24" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P24" t="inlineStr">
@@ -2258,27 +2258,27 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>5656</t>
+          <t>6173</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>4/24/2025</t>
+          <t>4/29/2025</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>ECHEVERRIA 5893</t>
+          <t>ARMENIA 2321</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>804922184</t>
+          <t>805507398</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
@@ -2293,7 +2293,7 @@
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>Poste con base quebrada</t>
+          <t>Picada volvio a entrar como caso 6325</t>
         </is>
       </c>
       <c r="I25" t="n">
@@ -2301,7 +2301,7 @@
       </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t>Desmonte</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K25" t="inlineStr">
@@ -2311,50 +2311,50 @@
       </c>
       <c r="L25" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M25" t="n">
-        <v>-58.489627</v>
+        <v>-58.420549</v>
       </c>
       <c r="N25" t="n">
-        <v>-34.583761</v>
+        <v>-34.585103</v>
       </c>
       <c r="O25" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P25" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>6173</t>
+          <t>5715</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>4/29/2025</t>
+          <t>5/1/2025</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>ARMENIA 2321</t>
+          <t>CUENCA 4690</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>805507398</t>
+          <t>805579094</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
@@ -2369,7 +2369,7 @@
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>Picada volvio a entrar como caso 6325</t>
+          <t>Aplomar poste</t>
         </is>
       </c>
       <c r="I26" t="n">
@@ -2377,7 +2377,7 @@
       </c>
       <c r="J26" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K26" t="inlineStr">
@@ -2387,30 +2387,30 @@
       </c>
       <c r="L26" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M26" t="n">
-        <v>-58.420549</v>
+        <v>-58.506061</v>
       </c>
       <c r="N26" t="n">
-        <v>-34.585103</v>
+        <v>-34.588887</v>
       </c>
       <c r="O26" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P26" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>5715</t>
+          <t>6333</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -2420,17 +2420,17 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>CUENCA 4690</t>
+          <t>ORTEGA Y GASSET 1816</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>805579094</t>
+          <t>805655342</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
@@ -2445,7 +2445,7 @@
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>Aplomar poste</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I27" t="n">
@@ -2453,7 +2453,7 @@
       </c>
       <c r="J27" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K27" t="inlineStr">
@@ -2463,40 +2463,40 @@
       </c>
       <c r="L27" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M27" t="n">
-        <v>-58.506061</v>
+        <v>-58.432556</v>
       </c>
       <c r="N27" t="n">
-        <v>-34.588887</v>
+        <v>-34.570279</v>
       </c>
       <c r="O27" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P27" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>6333</t>
+          <t>805707165</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>5/1/2025</t>
+          <t>5/7/2025</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>ORTEGA Y GASSET 1816</t>
+          <t>Baez 793</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
@@ -2506,7 +2506,7 @@
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>805655342</t>
+          <t>ICD30592749</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
@@ -2521,7 +2521,7 @@
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>DESMONTAR COLUMNA DE 7 MTS Y TRANSFERIR A COMUNITARIA</t>
         </is>
       </c>
       <c r="I28" t="n">
@@ -2539,14 +2539,14 @@
       </c>
       <c r="L28" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M28" t="n">
-        <v>-58.432556</v>
+        <v>-58.436165</v>
       </c>
       <c r="N28" t="n">
-        <v>-34.570279</v>
+        <v>-34.569081</v>
       </c>
       <c r="O28" t="inlineStr">
         <is>
@@ -2562,17 +2562,17 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>805707165</t>
+          <t>232</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>5/7/2025</t>
+          <t>5/9/2025</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Baez 793</t>
+          <t>Gorostiaga 2286</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
@@ -2582,7 +2582,7 @@
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>ICD30592749</t>
+          <t>805791858</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
@@ -2597,7 +2597,7 @@
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>DESMONTAR COLUMNA DE 7 MTS Y TRANSFERIR A COMUNITARIA</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I29" t="n">
@@ -2615,14 +2615,14 @@
       </c>
       <c r="L29" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M29" t="n">
-        <v>-58.436165</v>
+        <v>-58.441563</v>
       </c>
       <c r="N29" t="n">
-        <v>-34.569081</v>
+        <v>-34.569743</v>
       </c>
       <c r="O29" t="inlineStr">
         <is>
@@ -2638,27 +2638,27 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>232</t>
+          <t>-404</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>5/9/2025</t>
+          <t>5/8/2025</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Gorostiaga 2286</t>
+          <t>Amenabar 3048</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>805791858</t>
+          <t>805791896</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
@@ -2673,7 +2673,7 @@
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Aplomar columna 114</t>
         </is>
       </c>
       <c r="I30" t="n">
@@ -2681,7 +2681,7 @@
       </c>
       <c r="J30" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K30" t="inlineStr">
@@ -2695,26 +2695,26 @@
         </is>
       </c>
       <c r="M30" t="n">
-        <v>-58.441563</v>
+        <v>-58.46579</v>
       </c>
       <c r="N30" t="n">
-        <v>-34.569743</v>
+        <v>-34.555012</v>
       </c>
       <c r="O30" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P30" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>-404</t>
+          <t>-406</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
@@ -2724,17 +2724,17 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Amenabar 3048</t>
+          <t>Olof palme 4144</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>805791896</t>
+          <t>805791925</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
@@ -2749,7 +2749,7 @@
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>Aplomar columna 114</t>
+          <t>Tensar 2 riendas a pique columna 168</t>
         </is>
       </c>
       <c r="I31" t="n">
@@ -2757,7 +2757,7 @@
       </c>
       <c r="J31" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Tensor</t>
         </is>
       </c>
       <c r="K31" t="inlineStr">
@@ -2767,14 +2767,14 @@
       </c>
       <c r="L31" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M31" t="n">
-        <v>-58.46579</v>
+        <v>-58.488252</v>
       </c>
       <c r="N31" t="n">
-        <v>-34.555012</v>
+        <v>-34.553391</v>
       </c>
       <c r="O31" t="inlineStr">
         <is>
@@ -2790,17 +2790,17 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>-406</t>
+          <t>5826</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>5/8/2025</t>
+          <t>5/19/2025</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Olof palme 4144</t>
+          <t>ALBARELLOS AV. 3180</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
@@ -2810,7 +2810,7 @@
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>805791925</t>
+          <t>806926466</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
@@ -2825,7 +2825,7 @@
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>Tensar 2 riendas a pique columna 168</t>
+          <t>Columna (metal) inclinada</t>
         </is>
       </c>
       <c r="I32" t="n">
@@ -2833,7 +2833,7 @@
       </c>
       <c r="J32" t="inlineStr">
         <is>
-          <t>Tensor</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K32" t="inlineStr">
@@ -2847,14 +2847,14 @@
         </is>
       </c>
       <c r="M32" t="n">
-        <v>-58.488252</v>
+        <v>-58.513552</v>
       </c>
       <c r="N32" t="n">
-        <v>-34.553391</v>
+        <v>-34.579829</v>
       </c>
       <c r="O32" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P32" t="inlineStr">
@@ -2866,27 +2866,27 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>5826</t>
+          <t>6020</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>5/19/2025</t>
+          <t>6/5/2025</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>ALBARELLOS AV. 3180</t>
+          <t>RAVIGNANI, EMILIO, DR. 2036</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>806926466</t>
+          <t>807215465</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
@@ -2901,7 +2901,7 @@
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>Columna (metal) inclinada</t>
+          <t>Picada misma que 6260 y 6945</t>
         </is>
       </c>
       <c r="I33" t="n">
@@ -2909,7 +2909,7 @@
       </c>
       <c r="J33" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K33" t="inlineStr">
@@ -2919,50 +2919,50 @@
       </c>
       <c r="L33" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M33" t="n">
-        <v>-58.513552</v>
+        <v>-58.436298</v>
       </c>
       <c r="N33" t="n">
-        <v>-34.579829</v>
+        <v>-34.578972</v>
       </c>
       <c r="O33" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P33" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>6020</t>
+          <t>6144</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>6/5/2025</t>
+          <t>6/11/2025</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>RAVIGNANI, EMILIO, DR. 2036</t>
+          <t>TURIN 2990</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>807215465</t>
+          <t>807458282</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
@@ -2977,7 +2977,7 @@
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>Picada misma que 6260 y 6945</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I34" t="n">
@@ -2999,26 +2999,26 @@
         </is>
       </c>
       <c r="M34" t="n">
-        <v>-58.436298</v>
+        <v>-58.480925</v>
       </c>
       <c r="N34" t="n">
-        <v>-34.578972</v>
+        <v>-34.585471</v>
       </c>
       <c r="O34" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P34" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>6144</t>
+          <t>6143</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
@@ -3028,7 +3028,7 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>TURIN 2990</t>
+          <t>SOLANO LOPEZ, F., MARISCAL 2845</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
@@ -3038,7 +3038,7 @@
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>807458282</t>
+          <t>807458296</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
@@ -3075,10 +3075,10 @@
         </is>
       </c>
       <c r="M35" t="n">
-        <v>-58.480925</v>
+        <v>-58.495071</v>
       </c>
       <c r="N35" t="n">
-        <v>-34.585471</v>
+        <v>-34.593122</v>
       </c>
       <c r="O35" t="inlineStr">
         <is>
@@ -3094,27 +3094,27 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>6143</t>
+          <t>-478</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>6/11/2025</t>
+          <t>6/15/2025</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>SOLANO LOPEZ, F., MARISCAL 2845</t>
+          <t>Chivilcoy 4875</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>807458296</t>
+          <t>807508509</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
@@ -3129,7 +3129,7 @@
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Poste podrido</t>
         </is>
       </c>
       <c r="I36" t="n">
@@ -3147,14 +3147,14 @@
       </c>
       <c r="L36" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M36" t="n">
-        <v>-58.495071</v>
+        <v>-58.517389</v>
       </c>
       <c r="N36" t="n">
-        <v>-34.593122</v>
+        <v>-34.593541</v>
       </c>
       <c r="O36" t="inlineStr">
         <is>
@@ -3170,27 +3170,27 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>-478</t>
+          <t>6171</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>6/15/2025</t>
+          <t>6/18/2025</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Chivilcoy 4875</t>
+          <t>CABELLO 3486</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>807508509</t>
+          <t>807658640</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
@@ -3205,7 +3205,7 @@
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>Poste podrido</t>
+          <t>Columna inclinada evaluar con inspector un corrimiento</t>
         </is>
       </c>
       <c r="I37" t="n">
@@ -3223,40 +3223,40 @@
       </c>
       <c r="L37" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M37" t="n">
-        <v>-58.517389</v>
+        <v>-58.409579</v>
       </c>
       <c r="N37" t="n">
-        <v>-34.593541</v>
+        <v>-34.581134</v>
       </c>
       <c r="O37" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P37" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>6171</t>
+          <t>6230</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>6/18/2025</t>
+          <t>6/24/2025</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>CABELLO 3486</t>
+          <t>Santa maria de oro	2722</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
@@ -3266,7 +3266,7 @@
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>807658640</t>
+          <t>807763066</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
@@ -3281,7 +3281,7 @@
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>Columna inclinada evaluar con inspector un corrimiento</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I38" t="n">
@@ -3303,10 +3303,10 @@
         </is>
       </c>
       <c r="M38" t="n">
-        <v>-58.409579</v>
+        <v>-58.422315</v>
       </c>
       <c r="N38" t="n">
-        <v>-34.581134</v>
+        <v>-34.576988</v>
       </c>
       <c r="O38" t="inlineStr">
         <is>
@@ -3322,7 +3322,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>6230</t>
+          <t>6231</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
@@ -3332,7 +3332,7 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Santa maria de oro	2722</t>
+          <t>Ciudad de la Paz 275</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
@@ -3342,7 +3342,7 @@
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>807763066</t>
+          <t>807763070</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
@@ -3357,7 +3357,7 @@
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Aplomar o cambiar</t>
         </is>
       </c>
       <c r="I39" t="n">
@@ -3375,14 +3375,14 @@
       </c>
       <c r="L39" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M39" t="n">
-        <v>-58.422315</v>
+        <v>-58.441049</v>
       </c>
       <c r="N39" t="n">
-        <v>-34.576988</v>
+        <v>-34.574625</v>
       </c>
       <c r="O39" t="inlineStr">
         <is>
@@ -3398,7 +3398,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>6231</t>
+          <t>6235</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
@@ -3408,17 +3408,17 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Ciudad de la Paz 275</t>
+          <t>HUERGO 389</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>807763070</t>
+          <t>807763078</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
@@ -3433,7 +3433,7 @@
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t>Aplomar o cambiar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I40" t="n">
@@ -3451,14 +3451,14 @@
       </c>
       <c r="L40" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M40" t="n">
-        <v>-58.441049</v>
+        <v>-58.432722</v>
       </c>
       <c r="N40" t="n">
-        <v>-34.574625</v>
+        <v>-34.572371</v>
       </c>
       <c r="O40" t="inlineStr">
         <is>
@@ -3474,27 +3474,27 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>6235</t>
+          <t>6295</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>6/24/2025</t>
+          <t>6/30/2025</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>HUERGO 389</t>
+          <t>SOLER 6017</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>807763078</t>
+          <t>807851636</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
@@ -3531,10 +3531,10 @@
         </is>
       </c>
       <c r="M41" t="n">
-        <v>-58.432722</v>
+        <v>-58.436808</v>
       </c>
       <c r="N41" t="n">
-        <v>-34.572371</v>
+        <v>-34.577464</v>
       </c>
       <c r="O41" t="inlineStr">
         <is>
@@ -3550,17 +3550,17 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>6295</t>
+          <t>6332</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>6/30/2025</t>
+          <t>7/3/2025</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>SOLER 6017</t>
+          <t>ARAOZ 2560</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
@@ -3570,7 +3570,7 @@
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>807851636</t>
+          <t>807965818</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
@@ -3607,10 +3607,10 @@
         </is>
       </c>
       <c r="M42" t="n">
-        <v>-58.436808</v>
+        <v>-58.414507</v>
       </c>
       <c r="N42" t="n">
-        <v>-34.577464</v>
+        <v>-34.585377</v>
       </c>
       <c r="O42" t="inlineStr">
         <is>
@@ -3626,27 +3626,27 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>6332</t>
+          <t>6506</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>7/3/2025</t>
+          <t>7/10/2025</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>ARAOZ 2560</t>
+          <t>Ohiggins 1611</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>807965818</t>
+          <t>808148679</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
@@ -3661,7 +3661,7 @@
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Columna podrida en la base</t>
         </is>
       </c>
       <c r="I43" t="n">
@@ -3674,7 +3674,7 @@
       </c>
       <c r="K43" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L43" t="inlineStr">
@@ -3683,46 +3683,46 @@
         </is>
       </c>
       <c r="M43" t="n">
-        <v>-58.414507</v>
+        <v>-58.448993</v>
       </c>
       <c r="N43" t="n">
-        <v>-34.585377</v>
+        <v>-34.564383</v>
       </c>
       <c r="O43" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P43" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>6506</t>
+          <t>6437</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>7/10/2025</t>
+          <t>7/17/2025</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Ohiggins 1611</t>
+          <t>MILLER 4590</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>808148679</t>
+          <t>808400306</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
@@ -3737,7 +3737,7 @@
       </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t>Columna podrida en la base</t>
+          <t>Columna corroida</t>
         </is>
       </c>
       <c r="I44" t="n">
@@ -3750,7 +3750,7 @@
       </c>
       <c r="K44" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L44" t="inlineStr">
@@ -3759,14 +3759,14 @@
         </is>
       </c>
       <c r="M44" t="n">
-        <v>-58.448993</v>
+        <v>-58.495482</v>
       </c>
       <c r="N44" t="n">
-        <v>-34.564383</v>
+        <v>-34.552614</v>
       </c>
       <c r="O44" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P44" t="inlineStr">
@@ -3778,7 +3778,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>6437</t>
+          <t>6538</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
@@ -3788,7 +3788,7 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>MILLER 4590</t>
+          <t>Pedraza Manuela 4101</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
@@ -3798,7 +3798,7 @@
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>808400306</t>
+          <t>808400353</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
@@ -3813,7 +3813,7 @@
       </c>
       <c r="H45" t="inlineStr">
         <is>
-          <t>Columna corroida</t>
+          <t xml:space="preserve">Podrida en la base </t>
         </is>
       </c>
       <c r="I45" t="n">
@@ -3835,10 +3835,10 @@
         </is>
       </c>
       <c r="M45" t="n">
-        <v>-58.495482</v>
+        <v>-58.481569</v>
       </c>
       <c r="N45" t="n">
-        <v>-34.552614</v>
+        <v>-34.559853</v>
       </c>
       <c r="O45" t="inlineStr">
         <is>
@@ -3854,27 +3854,27 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>6538</t>
+          <t>7023</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>7/17/2025</t>
+          <t>7/22/2025</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Pedraza Manuela 4101</t>
+          <t>ZABALA 3573</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>808400353</t>
+          <t>808480549</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
@@ -3889,7 +3889,7 @@
       </c>
       <c r="H46" t="inlineStr">
         <is>
-          <t xml:space="preserve">Podrida en la base </t>
+          <t>Corroida en base para recambio</t>
         </is>
       </c>
       <c r="I46" t="n">
@@ -3911,14 +3911,14 @@
         </is>
       </c>
       <c r="M46" t="n">
-        <v>-58.481569</v>
+        <v>-58.457522</v>
       </c>
       <c r="N46" t="n">
-        <v>-34.559853</v>
+        <v>-34.579414</v>
       </c>
       <c r="O46" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P46" t="inlineStr">
@@ -3930,27 +3930,27 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>7023</t>
+          <t>6484</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>7/22/2025</t>
+          <t>7/24/2025</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>ZABALA 3573</t>
+          <t>URIARTE 2396</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>808480549</t>
+          <t>808509373</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
@@ -3965,7 +3965,7 @@
       </c>
       <c r="H47" t="inlineStr">
         <is>
-          <t>Corroida en base para recambio</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I47" t="n">
@@ -3987,36 +3987,36 @@
         </is>
       </c>
       <c r="M47" t="n">
-        <v>-58.457522</v>
+        <v>-58.423934</v>
       </c>
       <c r="N47" t="n">
-        <v>-34.579414</v>
+        <v>-34.581562</v>
       </c>
       <c r="O47" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P47" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>6484</t>
+          <t>6512</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>7/24/2025</t>
+          <t>7/28/2025</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>URIARTE 2396</t>
+          <t>GASCON 1195</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
@@ -4026,7 +4026,7 @@
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>808509373</t>
+          <t>808571975</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
@@ -4063,10 +4063,10 @@
         </is>
       </c>
       <c r="M48" t="n">
-        <v>-58.423934</v>
+        <v>-58.423127</v>
       </c>
       <c r="N48" t="n">
-        <v>-34.581562</v>
+        <v>-34.596476</v>
       </c>
       <c r="O48" t="inlineStr">
         <is>
@@ -4082,7 +4082,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>6512</t>
+          <t>6513</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
@@ -4092,7 +4092,7 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>GASCON 1195</t>
+          <t>DORREGO 1925</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
@@ -4102,7 +4102,7 @@
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>808571975</t>
+          <t>808571976</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
@@ -4139,10 +4139,10 @@
         </is>
       </c>
       <c r="M49" t="n">
-        <v>-58.423127</v>
+        <v>-58.441281</v>
       </c>
       <c r="N49" t="n">
-        <v>-34.596476</v>
+        <v>-34.579867</v>
       </c>
       <c r="O49" t="inlineStr">
         <is>
@@ -4158,7 +4158,7 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>6513</t>
+          <t>6519</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
@@ -4168,7 +4168,7 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>DORREGO 1925</t>
+          <t>SALGUERO, JERONIMO 2874</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
@@ -4178,7 +4178,7 @@
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>808571976</t>
+          <t>808571977</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
@@ -4193,7 +4193,7 @@
       </c>
       <c r="H50" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Reparar rienda</t>
         </is>
       </c>
       <c r="I50" t="n">
@@ -4201,7 +4201,7 @@
       </c>
       <c r="J50" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Tensor</t>
         </is>
       </c>
       <c r="K50" t="inlineStr">
@@ -4211,14 +4211,14 @@
       </c>
       <c r="L50" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M50" t="n">
-        <v>-58.441281</v>
+        <v>-58.407256</v>
       </c>
       <c r="N50" t="n">
-        <v>-34.579867</v>
+        <v>-34.578976</v>
       </c>
       <c r="O50" t="inlineStr">
         <is>
@@ -4234,27 +4234,27 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>6519</t>
+          <t>-538</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>7/28/2025</t>
+          <t>7/31/2025</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>SALGUERO, JERONIMO 2874</t>
+          <t>Malabia 964</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>808571977</t>
+          <t>808609237</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
@@ -4269,7 +4269,7 @@
       </c>
       <c r="H51" t="inlineStr">
         <is>
-          <t>Reparar rienda</t>
+          <t>Cambiar poste mal estado por PRFV</t>
         </is>
       </c>
       <c r="I51" t="n">
@@ -4277,7 +4277,7 @@
       </c>
       <c r="J51" t="inlineStr">
         <is>
-          <t>Tensor</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K51" t="inlineStr">
@@ -4287,14 +4287,14 @@
       </c>
       <c r="L51" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M51" t="n">
-        <v>-58.407256</v>
+        <v>-58.433634</v>
       </c>
       <c r="N51" t="n">
-        <v>-34.578976</v>
+        <v>-34.595018</v>
       </c>
       <c r="O51" t="inlineStr">
         <is>
@@ -4310,27 +4310,27 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>-538</t>
+          <t>-547</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>7/31/2025</t>
+          <t>8/6/2025</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>Malabia 964</t>
+          <t>Habana 4210</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>808609237</t>
+          <t>808733921</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
@@ -4345,7 +4345,7 @@
       </c>
       <c r="H52" t="inlineStr">
         <is>
-          <t>Cambiar poste mal estado por PRFV</t>
+          <t>Cambiar poste dañado</t>
         </is>
       </c>
       <c r="I52" t="n">
@@ -4367,46 +4367,46 @@
         </is>
       </c>
       <c r="M52" t="n">
-        <v>-58.433634</v>
+        <v>-58.515873</v>
       </c>
       <c r="N52" t="n">
-        <v>-34.595018</v>
+        <v>-34.599425</v>
       </c>
       <c r="O52" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P52" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>-547</t>
+          <t>6579</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>8/6/2025</t>
+          <t>8/7/2025</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>Habana 4210</t>
+          <t>RIVADAVIA MARTIN, COMODORO 1350</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>808733921</t>
+          <t>808749184</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
@@ -4421,7 +4421,7 @@
       </c>
       <c r="H53" t="inlineStr">
         <is>
-          <t>Cambiar poste dañado</t>
+          <t>Poste inclinado</t>
         </is>
       </c>
       <c r="I53" t="n">
@@ -4429,7 +4429,7 @@
       </c>
       <c r="J53" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K53" t="inlineStr">
@@ -4443,14 +4443,14 @@
         </is>
       </c>
       <c r="M53" t="n">
-        <v>-58.515873</v>
+        <v>-58.461024</v>
       </c>
       <c r="N53" t="n">
-        <v>-34.599425</v>
+        <v>-34.539409</v>
       </c>
       <c r="O53" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P53" t="inlineStr">
@@ -4462,27 +4462,27 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>6579</t>
+          <t>6906</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>8/7/2025</t>
+          <t>8/12/2025</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>RIVADAVIA MARTIN, COMODORO 1350</t>
+          <t>MOSCONI GENERAL AV. 3163</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>808749184</t>
+          <t>808918685</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
@@ -4497,7 +4497,7 @@
       </c>
       <c r="H54" t="inlineStr">
         <is>
-          <t>Poste inclinado</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I54" t="n">
@@ -4505,7 +4505,7 @@
       </c>
       <c r="J54" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K54" t="inlineStr">
@@ -4515,18 +4515,18 @@
       </c>
       <c r="L54" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M54" t="n">
-        <v>-58.461024</v>
+        <v>-58.505731</v>
       </c>
       <c r="N54" t="n">
-        <v>-34.539409</v>
+        <v>-34.588316</v>
       </c>
       <c r="O54" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P54" t="inlineStr">
@@ -4538,7 +4538,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>6906</t>
+          <t>6910</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
@@ -4548,17 +4548,17 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>MOSCONI GENERAL AV. 3163</t>
+          <t>RIVAS, GRAL. 2345</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>808918685</t>
+          <t>808918698</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
@@ -4573,7 +4573,7 @@
       </c>
       <c r="H55" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I55" t="n">
@@ -4595,10 +4595,10 @@
         </is>
       </c>
       <c r="M55" t="n">
-        <v>-58.505731</v>
+        <v>-58.482497</v>
       </c>
       <c r="N55" t="n">
-        <v>-34.588316</v>
+        <v>-34.598714</v>
       </c>
       <c r="O55" t="inlineStr">
         <is>
@@ -4614,7 +4614,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>6910</t>
+          <t>6928</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
@@ -4624,17 +4624,17 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>RIVAS, GRAL. 2345</t>
+          <t>ALBARELLOS AV. 3101</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>808918698</t>
+          <t>808918710</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
@@ -4649,7 +4649,7 @@
       </c>
       <c r="H56" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I56" t="n">
@@ -4671,10 +4671,10 @@
         </is>
       </c>
       <c r="M56" t="n">
-        <v>-58.482497</v>
+        <v>-58.512623</v>
       </c>
       <c r="N56" t="n">
-        <v>-34.598714</v>
+        <v>-34.579137</v>
       </c>
       <c r="O56" t="inlineStr">
         <is>
@@ -4690,7 +4690,7 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>6928</t>
+          <t>-550</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
@@ -4700,17 +4700,17 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>ALBARELLOS AV. 3101</t>
+          <t>Fitz roy 267</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>808918710</t>
+          <t>808918720</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
@@ -4725,7 +4725,7 @@
       </c>
       <c r="H57" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Aplomar columna</t>
         </is>
       </c>
       <c r="I57" t="n">
@@ -4747,10 +4747,10 @@
         </is>
       </c>
       <c r="M57" t="n">
-        <v>-58.512623</v>
+        <v>-58.451378</v>
       </c>
       <c r="N57" t="n">
-        <v>-34.579137</v>
+        <v>-34.596195</v>
       </c>
       <c r="O57" t="inlineStr">
         <is>
@@ -4766,27 +4766,27 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>-550</t>
+          <t>6943</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>8/12/2025</t>
+          <t>8/14/2025</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>Fitz roy 267</t>
+          <t>SUPERI 1459</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>808918720</t>
+          <t>808972965</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
@@ -4801,7 +4801,7 @@
       </c>
       <c r="H58" t="inlineStr">
         <is>
-          <t>Aplomar columna</t>
+          <t>Poste con base quebrada ver si es posible desmonte</t>
         </is>
       </c>
       <c r="I58" t="n">
@@ -4809,7 +4809,7 @@
       </c>
       <c r="J58" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Desmonte</t>
         </is>
       </c>
       <c r="K58" t="inlineStr">
@@ -4819,18 +4819,18 @@
       </c>
       <c r="L58" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M58" t="n">
-        <v>-58.451378</v>
+        <v>-58.460834</v>
       </c>
       <c r="N58" t="n">
-        <v>-34.596195</v>
+        <v>-34.573753</v>
       </c>
       <c r="O58" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P58" t="inlineStr">
@@ -4842,7 +4842,7 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>6943</t>
+          <t>6969</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
@@ -4852,17 +4852,17 @@
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>SUPERI 1459</t>
+          <t>CIUDAD DE LA PAZ 295</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>808972965</t>
+          <t>808972995</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
@@ -4877,7 +4877,7 @@
       </c>
       <c r="H59" t="inlineStr">
         <is>
-          <t>Poste con base quebrada ver si es posible desmonte</t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I59" t="n">
@@ -4885,7 +4885,7 @@
       </c>
       <c r="J59" t="inlineStr">
         <is>
-          <t>Desmonte</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K59" t="inlineStr">
@@ -4895,30 +4895,30 @@
       </c>
       <c r="L59" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M59" t="n">
-        <v>-58.460834</v>
+        <v>-58.441171</v>
       </c>
       <c r="N59" t="n">
-        <v>-34.573753</v>
+        <v>-34.574547</v>
       </c>
       <c r="O59" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P59" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>6969</t>
+          <t>6971</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
@@ -4928,7 +4928,7 @@
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>CIUDAD DE LA PAZ 295</t>
+          <t>MAURE 1594</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
@@ -4938,7 +4938,7 @@
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>808972995</t>
+          <t>808973001</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
@@ -4953,7 +4953,7 @@
       </c>
       <c r="H60" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>Ver de traspasar a telecentro y  desmontar ver con inspector</t>
         </is>
       </c>
       <c r="I60" t="n">
@@ -4975,10 +4975,10 @@
         </is>
       </c>
       <c r="M60" t="n">
-        <v>-58.441171</v>
+        <v>-58.435072</v>
       </c>
       <c r="N60" t="n">
-        <v>-34.574547</v>
+        <v>-34.565732</v>
       </c>
       <c r="O60" t="inlineStr">
         <is>
@@ -4994,17 +4994,17 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>6971</t>
+          <t>7000</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>8/14/2025</t>
+          <t>8/20/2025</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>MAURE 1594</t>
+          <t>SCALABRINI ORTIZ, RAUL AV. 2106</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
@@ -5014,7 +5014,7 @@
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>808973001</t>
+          <t>809065867</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
@@ -5029,7 +5029,7 @@
       </c>
       <c r="H61" t="inlineStr">
         <is>
-          <t>Ver de traspasar a telecentro y  desmontar ver con inspector</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I61" t="n">
@@ -5051,10 +5051,10 @@
         </is>
       </c>
       <c r="M61" t="n">
-        <v>-58.435072</v>
+        <v>-58.420109</v>
       </c>
       <c r="N61" t="n">
-        <v>-34.565732</v>
+        <v>-34.58764</v>
       </c>
       <c r="O61" t="inlineStr">
         <is>
@@ -5070,7 +5070,7 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>7000</t>
+          <t>7003</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
@@ -5080,17 +5080,17 @@
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>SCALABRINI ORTIZ, RAUL AV. 2106</t>
+          <t>MELIAN AV. 2576</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>809065867</t>
+          <t>809065874</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
@@ -5127,46 +5127,46 @@
         </is>
       </c>
       <c r="M62" t="n">
-        <v>-58.420109</v>
+        <v>-58.471943</v>
       </c>
       <c r="N62" t="n">
-        <v>-34.58764</v>
+        <v>-34.564948</v>
       </c>
       <c r="O62" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P62" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>7003</t>
+          <t>-559</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>8/20/2025</t>
+          <t>8/21/2025</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>MELIAN AV. 2576</t>
+          <t>Av. Del Libertador 6736</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>809065874</t>
+          <t>809098713</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
@@ -5203,14 +5203,14 @@
         </is>
       </c>
       <c r="M63" t="n">
-        <v>-58.471943</v>
+        <v>-58.453398</v>
       </c>
       <c r="N63" t="n">
-        <v>-34.564948</v>
+        <v>-34.550238</v>
       </c>
       <c r="O63" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P63" t="inlineStr">
@@ -5222,17 +5222,17 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>-559</t>
+          <t>5503</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>8/21/2025</t>
+          <t>8/22/2025</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>Av. Del Libertador 6736</t>
+          <t>CRAMER AV. 1771</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
@@ -5242,7 +5242,7 @@
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>809098713</t>
+          <t>809102564</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
@@ -5257,7 +5257,7 @@
       </c>
       <c r="H64" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>PIcada</t>
         </is>
       </c>
       <c r="I64" t="n">
@@ -5279,14 +5279,14 @@
         </is>
       </c>
       <c r="M64" t="n">
-        <v>-58.453398</v>
+        <v>-58.458506</v>
       </c>
       <c r="N64" t="n">
-        <v>-34.550238</v>
+        <v>-34.56783</v>
       </c>
       <c r="O64" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P64" t="inlineStr">
@@ -5298,27 +5298,27 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>5503</t>
+          <t>7098</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>8/22/2025</t>
+          <t>8/25/2025</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>CRAMER AV. 1771</t>
+          <t>UGARTE, MANUEL 3484</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>809102564</t>
+          <t>809126236</t>
         </is>
       </c>
       <c r="F65" t="inlineStr">
@@ -5333,7 +5333,7 @@
       </c>
       <c r="H65" t="inlineStr">
         <is>
-          <t>PIcada</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I65" t="n">
@@ -5355,10 +5355,10 @@
         </is>
       </c>
       <c r="M65" t="n">
-        <v>-58.458506</v>
+        <v>-58.472869</v>
       </c>
       <c r="N65" t="n">
-        <v>-34.56783</v>
+        <v>-34.562</v>
       </c>
       <c r="O65" t="inlineStr">
         <is>
@@ -5374,7 +5374,7 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>7098</t>
+          <t>7080</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
@@ -5384,17 +5384,17 @@
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>UGARTE, MANUEL 3484</t>
+          <t>UGARTE, MANUEL 2196</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>809126236</t>
+          <t>809125906</t>
         </is>
       </c>
       <c r="F66" t="inlineStr">
@@ -5431,14 +5431,14 @@
         </is>
       </c>
       <c r="M66" t="n">
-        <v>-58.472869</v>
+        <v>-58.459402</v>
       </c>
       <c r="N66" t="n">
-        <v>-34.562</v>
+        <v>-34.555262</v>
       </c>
       <c r="O66" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P66" t="inlineStr">
@@ -5450,7 +5450,7 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>7080</t>
+          <t>7021</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
@@ -5460,17 +5460,17 @@
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>UGARTE, MANUEL 2196</t>
+          <t>VERA 445</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>809125906</t>
+          <t>809155622</t>
         </is>
       </c>
       <c r="F67" t="inlineStr">
@@ -5485,7 +5485,7 @@
       </c>
       <c r="H67" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Correrla para sacarla del cantero</t>
         </is>
       </c>
       <c r="I67" t="n">
@@ -5507,36 +5507,36 @@
         </is>
       </c>
       <c r="M67" t="n">
-        <v>-58.459402</v>
+        <v>-58.437181</v>
       </c>
       <c r="N67" t="n">
-        <v>-34.555262</v>
+        <v>-34.5995</v>
       </c>
       <c r="O67" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P67" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>7021</t>
+          <t>6465</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>8/25/2025</t>
+          <t>8/28/2025</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>VERA 445</t>
+          <t>AGUIRRE 368</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
@@ -5546,7 +5546,7 @@
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>809155622</t>
+          <t>809268249</t>
         </is>
       </c>
       <c r="F68" t="inlineStr">
@@ -5561,7 +5561,7 @@
       </c>
       <c r="H68" t="inlineStr">
         <is>
-          <t>Correrla para sacarla del cantero</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I68" t="n">
@@ -5583,10 +5583,10 @@
         </is>
       </c>
       <c r="M68" t="n">
-        <v>-58.437181</v>
+        <v>-58.434651</v>
       </c>
       <c r="N68" t="n">
-        <v>-34.5995</v>
+        <v>-34.598814</v>
       </c>
       <c r="O68" t="inlineStr">
         <is>
@@ -5602,7 +5602,7 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>6465</t>
+          <t>7095</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
@@ -5612,7 +5612,7 @@
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>AGUIRRE 368</t>
+          <t>SAN MARTIN AV. 4515</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
@@ -5622,7 +5622,7 @@
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>809268249</t>
+          <t>809268240</t>
         </is>
       </c>
       <c r="F69" t="inlineStr">
@@ -5637,7 +5637,7 @@
       </c>
       <c r="H69" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Columna chocada</t>
         </is>
       </c>
       <c r="I69" t="n">
@@ -5655,30 +5655,30 @@
       </c>
       <c r="L69" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M69" t="n">
-        <v>-58.434651</v>
+        <v>-58.483415</v>
       </c>
       <c r="N69" t="n">
-        <v>-34.598814</v>
+        <v>-34.597663</v>
       </c>
       <c r="O69" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P69" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>7095</t>
+          <t>-575</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
@@ -5688,17 +5688,17 @@
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>SAN MARTIN AV. 4515</t>
+          <t>Amenabar 3064</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>809268240</t>
+          <t>809281299</t>
         </is>
       </c>
       <c r="F70" t="inlineStr">
@@ -5713,7 +5713,7 @@
       </c>
       <c r="H70" t="inlineStr">
         <is>
-          <t>Columna chocada</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I70" t="n">
@@ -5731,18 +5731,18 @@
       </c>
       <c r="L70" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M70" t="n">
-        <v>-58.483415</v>
+        <v>-58.465984</v>
       </c>
       <c r="N70" t="n">
-        <v>-34.597663</v>
+        <v>-34.554869</v>
       </c>
       <c r="O70" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P70" t="inlineStr">
@@ -5754,27 +5754,27 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>-575</t>
+          <t>-576</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>8/28/2025</t>
+          <t>8/29/2025</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>Amenabar 3064</t>
+          <t>Av. Boyacá 2030</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>809281299</t>
+          <t>809309606</t>
         </is>
       </c>
       <c r="F71" t="inlineStr">
@@ -5811,14 +5811,14 @@
         </is>
       </c>
       <c r="M71" t="n">
-        <v>-58.465984</v>
+        <v>-58.471173</v>
       </c>
       <c r="N71" t="n">
-        <v>-34.554869</v>
+        <v>-34.60704</v>
       </c>
       <c r="O71" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P71" t="inlineStr">
@@ -5830,17 +5830,17 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>4166</t>
+          <t>7111</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>8/29/2025</t>
+          <t>9/1/2025</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>ALTOLAGUIRRE 2201</t>
+          <t>VILELA 3699</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
@@ -5850,7 +5850,7 @@
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>809309591</t>
+          <t>809371823</t>
         </is>
       </c>
       <c r="F72" t="inlineStr">
@@ -5865,7 +5865,7 @@
       </c>
       <c r="H72" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t xml:space="preserve">Cambiar </t>
         </is>
       </c>
       <c r="I72" t="n">
@@ -5883,18 +5883,18 @@
       </c>
       <c r="L72" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M72" t="n">
-        <v>-58.489622</v>
+        <v>-58.482817</v>
       </c>
       <c r="N72" t="n">
-        <v>-34.578426</v>
+        <v>-34.550845</v>
       </c>
       <c r="O72" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P72" t="inlineStr">
@@ -5906,27 +5906,27 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>-576</t>
+          <t>7118</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>8/29/2025</t>
+          <t>9/2/2025</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>Av. Boyacá 2030</t>
+          <t>CUBAS, JOSE 2211</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>809309606</t>
+          <t>809406168</t>
         </is>
       </c>
       <c r="F73" t="inlineStr">
@@ -5963,10 +5963,10 @@
         </is>
       </c>
       <c r="M73" t="n">
-        <v>-58.471173</v>
+        <v>-58.492448</v>
       </c>
       <c r="N73" t="n">
-        <v>-34.60704</v>
+        <v>-34.58372</v>
       </c>
       <c r="O73" t="inlineStr">
         <is>
@@ -5982,27 +5982,27 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>7111</t>
+          <t>-577</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>9/1/2025</t>
+          <t>9/2/2025</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>VILELA 3699</t>
+          <t>Manuel Ugarte 2318</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>809371823</t>
+          <t>809406177</t>
         </is>
       </c>
       <c r="F74" t="inlineStr">
@@ -6017,7 +6017,7 @@
       </c>
       <c r="H74" t="inlineStr">
         <is>
-          <t xml:space="preserve">Cambiar </t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I74" t="n">
@@ -6035,14 +6035,14 @@
       </c>
       <c r="L74" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M74" t="n">
-        <v>-58.482817</v>
+        <v>-58.460635</v>
       </c>
       <c r="N74" t="n">
-        <v>-34.550845</v>
+        <v>-34.555932</v>
       </c>
       <c r="O74" t="inlineStr">
         <is>
@@ -6058,7 +6058,7 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>7118</t>
+          <t>-578</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
@@ -6068,17 +6068,17 @@
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>CUBAS, JOSE 2211</t>
+          <t>Pedro I Rivera 2536</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>809406168</t>
+          <t>809406189</t>
         </is>
       </c>
       <c r="F75" t="inlineStr">
@@ -6115,14 +6115,14 @@
         </is>
       </c>
       <c r="M75" t="n">
-        <v>-58.492448</v>
+        <v>-58.462327</v>
       </c>
       <c r="N75" t="n">
-        <v>-34.58372</v>
+        <v>-34.557565</v>
       </c>
       <c r="O75" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P75" t="inlineStr">
@@ -6134,7 +6134,7 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>-577</t>
+          <t>-579</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
@@ -6144,7 +6144,7 @@
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>Manuel Ugarte 2318</t>
+          <t>Pedro Rivera 2546</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
@@ -6154,7 +6154,7 @@
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>809406177</t>
+          <t>Pendiente ADM</t>
         </is>
       </c>
       <c r="F76" t="inlineStr">
@@ -6169,7 +6169,7 @@
       </c>
       <c r="H76" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Colocar R200 para pedir traspaso de equipos</t>
         </is>
       </c>
       <c r="I76" t="n">
@@ -6182,7 +6182,7 @@
       </c>
       <c r="K76" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L76" t="inlineStr">
@@ -6191,10 +6191,10 @@
         </is>
       </c>
       <c r="M76" t="n">
-        <v>-58.460635</v>
+        <v>-58.462479</v>
       </c>
       <c r="N76" t="n">
-        <v>-34.555932</v>
+        <v>-34.55765</v>
       </c>
       <c r="O76" t="inlineStr">
         <is>
@@ -6202,158 +6202,6 @@
         </is>
       </c>
       <c r="P76" t="inlineStr">
-        <is>
-          <t>Capital Norte</t>
-        </is>
-      </c>
-    </row>
-    <row r="77">
-      <c r="A77" t="inlineStr">
-        <is>
-          <t>-578</t>
-        </is>
-      </c>
-      <c r="B77" t="inlineStr">
-        <is>
-          <t>9/2/2025</t>
-        </is>
-      </c>
-      <c r="C77" t="inlineStr">
-        <is>
-          <t>Pedro I Rivera 2536</t>
-        </is>
-      </c>
-      <c r="D77" t="inlineStr">
-        <is>
-          <t>13</t>
-        </is>
-      </c>
-      <c r="E77" t="inlineStr">
-        <is>
-          <t>809406189</t>
-        </is>
-      </c>
-      <c r="F77" t="inlineStr">
-        <is>
-          <t>NEW</t>
-        </is>
-      </c>
-      <c r="G77" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H77" t="inlineStr">
-        <is>
-          <t>Picada</t>
-        </is>
-      </c>
-      <c r="I77" t="n">
-        <v>1</v>
-      </c>
-      <c r="J77" t="inlineStr">
-        <is>
-          <t>Cambio</t>
-        </is>
-      </c>
-      <c r="K77" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L77" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
-      <c r="M77" t="n">
-        <v>-58.462327</v>
-      </c>
-      <c r="N77" t="n">
-        <v>-34.557565</v>
-      </c>
-      <c r="O77" t="inlineStr">
-        <is>
-          <t>Saavedra</t>
-        </is>
-      </c>
-      <c r="P77" t="inlineStr">
-        <is>
-          <t>Capital Norte</t>
-        </is>
-      </c>
-    </row>
-    <row r="78">
-      <c r="A78" t="inlineStr">
-        <is>
-          <t>-579</t>
-        </is>
-      </c>
-      <c r="B78" t="inlineStr">
-        <is>
-          <t>9/2/2025</t>
-        </is>
-      </c>
-      <c r="C78" t="inlineStr">
-        <is>
-          <t>Pedro Rivera 2546</t>
-        </is>
-      </c>
-      <c r="D78" t="inlineStr">
-        <is>
-          <t>13</t>
-        </is>
-      </c>
-      <c r="E78" t="inlineStr">
-        <is>
-          <t>Pendiente ADM</t>
-        </is>
-      </c>
-      <c r="F78" t="inlineStr">
-        <is>
-          <t>NEW</t>
-        </is>
-      </c>
-      <c r="G78" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H78" t="inlineStr">
-        <is>
-          <t>Colocar R200 para pedir traspaso de equipos</t>
-        </is>
-      </c>
-      <c r="I78" t="n">
-        <v>1</v>
-      </c>
-      <c r="J78" t="inlineStr">
-        <is>
-          <t>Cambio</t>
-        </is>
-      </c>
-      <c r="K78" t="inlineStr">
-        <is>
-          <t>Nodo Teco</t>
-        </is>
-      </c>
-      <c r="L78" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
-      <c r="M78" t="n">
-        <v>-58.462479</v>
-      </c>
-      <c r="N78" t="n">
-        <v>-34.55765</v>
-      </c>
-      <c r="O78" t="inlineStr">
-        <is>
-          <t>Saavedra</t>
-        </is>
-      </c>
-      <c r="P78" t="inlineStr">
         <is>
           <t>Capital Norte</t>
         </is>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-09-04 18:55:26)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_NEW.xlsx
+++ b/mapa_interactivo_NEW.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P76"/>
+  <dimension ref="A1:P77"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4538,7 +4538,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>6910</t>
+          <t>6002</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
@@ -4548,17 +4548,17 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>RIVAS, GRAL. 2345</t>
+          <t>LA PLATA AV. 832</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>808918698</t>
+          <t>808918694</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
@@ -4573,7 +4573,7 @@
       </c>
       <c r="H55" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I55" t="n">
@@ -4595,26 +4595,26 @@
         </is>
       </c>
       <c r="M55" t="n">
-        <v>-58.482497</v>
+        <v>-58.426947</v>
       </c>
       <c r="N55" t="n">
-        <v>-34.598714</v>
+        <v>-34.625698</v>
       </c>
       <c r="O55" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P55" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>6928</t>
+          <t>6910</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
@@ -4624,17 +4624,17 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>ALBARELLOS AV. 3101</t>
+          <t>RIVAS, GRAL. 2345</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>808918710</t>
+          <t>808918698</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
@@ -4649,7 +4649,7 @@
       </c>
       <c r="H56" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I56" t="n">
@@ -4671,10 +4671,10 @@
         </is>
       </c>
       <c r="M56" t="n">
-        <v>-58.512623</v>
+        <v>-58.482497</v>
       </c>
       <c r="N56" t="n">
-        <v>-34.579137</v>
+        <v>-34.598714</v>
       </c>
       <c r="O56" t="inlineStr">
         <is>
@@ -4690,7 +4690,7 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>-550</t>
+          <t>6928</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
@@ -4700,17 +4700,17 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>Fitz roy 267</t>
+          <t>ALBARELLOS AV. 3101</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>808918720</t>
+          <t>808918710</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
@@ -4725,7 +4725,7 @@
       </c>
       <c r="H57" t="inlineStr">
         <is>
-          <t>Aplomar columna</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I57" t="n">
@@ -4747,10 +4747,10 @@
         </is>
       </c>
       <c r="M57" t="n">
-        <v>-58.451378</v>
+        <v>-58.512623</v>
       </c>
       <c r="N57" t="n">
-        <v>-34.596195</v>
+        <v>-34.579137</v>
       </c>
       <c r="O57" t="inlineStr">
         <is>
@@ -4766,27 +4766,27 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>6943</t>
+          <t>-550</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>8/14/2025</t>
+          <t>8/12/2025</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>SUPERI 1459</t>
+          <t>Fitz roy 267</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>808972965</t>
+          <t>808918720</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
@@ -4801,7 +4801,7 @@
       </c>
       <c r="H58" t="inlineStr">
         <is>
-          <t>Poste con base quebrada ver si es posible desmonte</t>
+          <t>Aplomar columna</t>
         </is>
       </c>
       <c r="I58" t="n">
@@ -4809,7 +4809,7 @@
       </c>
       <c r="J58" t="inlineStr">
         <is>
-          <t>Desmonte</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K58" t="inlineStr">
@@ -4819,18 +4819,18 @@
       </c>
       <c r="L58" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M58" t="n">
-        <v>-58.460834</v>
+        <v>-58.451378</v>
       </c>
       <c r="N58" t="n">
-        <v>-34.573753</v>
+        <v>-34.596195</v>
       </c>
       <c r="O58" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P58" t="inlineStr">
@@ -4842,7 +4842,7 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>6969</t>
+          <t>6943</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
@@ -4852,17 +4852,17 @@
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>CIUDAD DE LA PAZ 295</t>
+          <t>SUPERI 1459</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>808972995</t>
+          <t>808972965</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
@@ -4877,7 +4877,7 @@
       </c>
       <c r="H59" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>Poste con base quebrada ver si es posible desmonte</t>
         </is>
       </c>
       <c r="I59" t="n">
@@ -4885,7 +4885,7 @@
       </c>
       <c r="J59" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Desmonte</t>
         </is>
       </c>
       <c r="K59" t="inlineStr">
@@ -4895,30 +4895,30 @@
       </c>
       <c r="L59" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M59" t="n">
-        <v>-58.441171</v>
+        <v>-58.460834</v>
       </c>
       <c r="N59" t="n">
-        <v>-34.574547</v>
+        <v>-34.573753</v>
       </c>
       <c r="O59" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P59" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>6971</t>
+          <t>6969</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
@@ -4928,7 +4928,7 @@
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>MAURE 1594</t>
+          <t>CIUDAD DE LA PAZ 295</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
@@ -4938,7 +4938,7 @@
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>808973001</t>
+          <t>808972995</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
@@ -4953,7 +4953,7 @@
       </c>
       <c r="H60" t="inlineStr">
         <is>
-          <t>Ver de traspasar a telecentro y  desmontar ver con inspector</t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I60" t="n">
@@ -4975,10 +4975,10 @@
         </is>
       </c>
       <c r="M60" t="n">
-        <v>-58.435072</v>
+        <v>-58.441171</v>
       </c>
       <c r="N60" t="n">
-        <v>-34.565732</v>
+        <v>-34.574547</v>
       </c>
       <c r="O60" t="inlineStr">
         <is>
@@ -4994,17 +4994,17 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>7000</t>
+          <t>6971</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>8/20/2025</t>
+          <t>8/14/2025</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>SCALABRINI ORTIZ, RAUL AV. 2106</t>
+          <t>MAURE 1594</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
@@ -5014,7 +5014,7 @@
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>809065867</t>
+          <t>808973001</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
@@ -5029,7 +5029,7 @@
       </c>
       <c r="H61" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Ver de traspasar a telecentro y  desmontar ver con inspector</t>
         </is>
       </c>
       <c r="I61" t="n">
@@ -5051,10 +5051,10 @@
         </is>
       </c>
       <c r="M61" t="n">
-        <v>-58.420109</v>
+        <v>-58.435072</v>
       </c>
       <c r="N61" t="n">
-        <v>-34.58764</v>
+        <v>-34.565732</v>
       </c>
       <c r="O61" t="inlineStr">
         <is>
@@ -5070,7 +5070,7 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>7003</t>
+          <t>7000</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
@@ -5080,17 +5080,17 @@
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>MELIAN AV. 2576</t>
+          <t>SCALABRINI ORTIZ, RAUL AV. 2106</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>809065874</t>
+          <t>809065867</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
@@ -5127,46 +5127,46 @@
         </is>
       </c>
       <c r="M62" t="n">
-        <v>-58.471943</v>
+        <v>-58.420109</v>
       </c>
       <c r="N62" t="n">
-        <v>-34.564948</v>
+        <v>-34.58764</v>
       </c>
       <c r="O62" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P62" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>-559</t>
+          <t>7003</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>8/21/2025</t>
+          <t>8/20/2025</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>Av. Del Libertador 6736</t>
+          <t>MELIAN AV. 2576</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>809098713</t>
+          <t>809065874</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
@@ -5203,14 +5203,14 @@
         </is>
       </c>
       <c r="M63" t="n">
-        <v>-58.453398</v>
+        <v>-58.471943</v>
       </c>
       <c r="N63" t="n">
-        <v>-34.550238</v>
+        <v>-34.564948</v>
       </c>
       <c r="O63" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P63" t="inlineStr">
@@ -5222,17 +5222,17 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>5503</t>
+          <t>-559</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>8/22/2025</t>
+          <t>8/21/2025</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>CRAMER AV. 1771</t>
+          <t>Av. Del Libertador 6736</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
@@ -5242,7 +5242,7 @@
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>809102564</t>
+          <t>809098713</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
@@ -5257,7 +5257,7 @@
       </c>
       <c r="H64" t="inlineStr">
         <is>
-          <t>PIcada</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I64" t="n">
@@ -5279,14 +5279,14 @@
         </is>
       </c>
       <c r="M64" t="n">
-        <v>-58.458506</v>
+        <v>-58.453398</v>
       </c>
       <c r="N64" t="n">
-        <v>-34.56783</v>
+        <v>-34.550238</v>
       </c>
       <c r="O64" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P64" t="inlineStr">
@@ -5298,27 +5298,27 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>7098</t>
+          <t>5503</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>8/25/2025</t>
+          <t>8/22/2025</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>UGARTE, MANUEL 3484</t>
+          <t>CRAMER AV. 1771</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>809126236</t>
+          <t>809102564</t>
         </is>
       </c>
       <c r="F65" t="inlineStr">
@@ -5333,7 +5333,7 @@
       </c>
       <c r="H65" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>PIcada</t>
         </is>
       </c>
       <c r="I65" t="n">
@@ -5355,10 +5355,10 @@
         </is>
       </c>
       <c r="M65" t="n">
-        <v>-58.472869</v>
+        <v>-58.458506</v>
       </c>
       <c r="N65" t="n">
-        <v>-34.562</v>
+        <v>-34.56783</v>
       </c>
       <c r="O65" t="inlineStr">
         <is>
@@ -5374,7 +5374,7 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>7080</t>
+          <t>7098</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
@@ -5384,17 +5384,17 @@
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>UGARTE, MANUEL 2196</t>
+          <t>UGARTE, MANUEL 3484</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>809125906</t>
+          <t>809126236</t>
         </is>
       </c>
       <c r="F66" t="inlineStr">
@@ -5431,14 +5431,14 @@
         </is>
       </c>
       <c r="M66" t="n">
-        <v>-58.459402</v>
+        <v>-58.472869</v>
       </c>
       <c r="N66" t="n">
-        <v>-34.555262</v>
+        <v>-34.562</v>
       </c>
       <c r="O66" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P66" t="inlineStr">
@@ -5450,7 +5450,7 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>7021</t>
+          <t>7080</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
@@ -5460,17 +5460,17 @@
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>VERA 445</t>
+          <t>UGARTE, MANUEL 2196</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>809155622</t>
+          <t>809125906</t>
         </is>
       </c>
       <c r="F67" t="inlineStr">
@@ -5485,7 +5485,7 @@
       </c>
       <c r="H67" t="inlineStr">
         <is>
-          <t>Correrla para sacarla del cantero</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I67" t="n">
@@ -5507,36 +5507,36 @@
         </is>
       </c>
       <c r="M67" t="n">
-        <v>-58.437181</v>
+        <v>-58.459402</v>
       </c>
       <c r="N67" t="n">
-        <v>-34.5995</v>
+        <v>-34.555262</v>
       </c>
       <c r="O67" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P67" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>6465</t>
+          <t>7021</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>8/28/2025</t>
+          <t>8/25/2025</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>AGUIRRE 368</t>
+          <t>VERA 445</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
@@ -5546,7 +5546,7 @@
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>809268249</t>
+          <t>809155622</t>
         </is>
       </c>
       <c r="F68" t="inlineStr">
@@ -5561,7 +5561,7 @@
       </c>
       <c r="H68" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Correrla para sacarla del cantero</t>
         </is>
       </c>
       <c r="I68" t="n">
@@ -5583,10 +5583,10 @@
         </is>
       </c>
       <c r="M68" t="n">
-        <v>-58.434651</v>
+        <v>-58.437181</v>
       </c>
       <c r="N68" t="n">
-        <v>-34.598814</v>
+        <v>-34.5995</v>
       </c>
       <c r="O68" t="inlineStr">
         <is>
@@ -5602,7 +5602,7 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>7095</t>
+          <t>6465</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
@@ -5612,7 +5612,7 @@
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>SAN MARTIN AV. 4515</t>
+          <t>AGUIRRE 368</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
@@ -5622,7 +5622,7 @@
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>809268240</t>
+          <t>809268249</t>
         </is>
       </c>
       <c r="F69" t="inlineStr">
@@ -5637,7 +5637,7 @@
       </c>
       <c r="H69" t="inlineStr">
         <is>
-          <t>Columna chocada</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I69" t="n">
@@ -5655,30 +5655,30 @@
       </c>
       <c r="L69" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M69" t="n">
-        <v>-58.483415</v>
+        <v>-58.434651</v>
       </c>
       <c r="N69" t="n">
-        <v>-34.597663</v>
+        <v>-34.598814</v>
       </c>
       <c r="O69" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P69" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>-575</t>
+          <t>7095</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
@@ -5688,17 +5688,17 @@
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>Amenabar 3064</t>
+          <t>SAN MARTIN AV. 4515</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>809281299</t>
+          <t>809268240</t>
         </is>
       </c>
       <c r="F70" t="inlineStr">
@@ -5713,7 +5713,7 @@
       </c>
       <c r="H70" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Columna chocada</t>
         </is>
       </c>
       <c r="I70" t="n">
@@ -5731,18 +5731,18 @@
       </c>
       <c r="L70" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M70" t="n">
-        <v>-58.465984</v>
+        <v>-58.483415</v>
       </c>
       <c r="N70" t="n">
-        <v>-34.554869</v>
+        <v>-34.597663</v>
       </c>
       <c r="O70" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P70" t="inlineStr">
@@ -5754,27 +5754,27 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>-576</t>
+          <t>-575</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>8/29/2025</t>
+          <t>8/28/2025</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>Av. Boyacá 2030</t>
+          <t>Amenabar 3064</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>809309606</t>
+          <t>809281299</t>
         </is>
       </c>
       <c r="F71" t="inlineStr">
@@ -5811,14 +5811,14 @@
         </is>
       </c>
       <c r="M71" t="n">
-        <v>-58.471173</v>
+        <v>-58.465984</v>
       </c>
       <c r="N71" t="n">
-        <v>-34.60704</v>
+        <v>-34.554869</v>
       </c>
       <c r="O71" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P71" t="inlineStr">
@@ -5830,27 +5830,27 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>7111</t>
+          <t>-576</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>9/1/2025</t>
+          <t>8/29/2025</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>VILELA 3699</t>
+          <t>Av. Boyacá 2030</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>809371823</t>
+          <t>809309606</t>
         </is>
       </c>
       <c r="F72" t="inlineStr">
@@ -5865,7 +5865,7 @@
       </c>
       <c r="H72" t="inlineStr">
         <is>
-          <t xml:space="preserve">Cambiar </t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I72" t="n">
@@ -5883,18 +5883,18 @@
       </c>
       <c r="L72" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M72" t="n">
-        <v>-58.482817</v>
+        <v>-58.471173</v>
       </c>
       <c r="N72" t="n">
-        <v>-34.550845</v>
+        <v>-34.60704</v>
       </c>
       <c r="O72" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P72" t="inlineStr">
@@ -5906,17 +5906,17 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>7118</t>
+          <t>7111</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>9/2/2025</t>
+          <t>9/1/2025</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>CUBAS, JOSE 2211</t>
+          <t>VILELA 3699</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
@@ -5926,7 +5926,7 @@
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>809406168</t>
+          <t>809371823</t>
         </is>
       </c>
       <c r="F73" t="inlineStr">
@@ -5941,7 +5941,7 @@
       </c>
       <c r="H73" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t xml:space="preserve">Cambiar </t>
         </is>
       </c>
       <c r="I73" t="n">
@@ -5959,18 +5959,18 @@
       </c>
       <c r="L73" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M73" t="n">
-        <v>-58.492448</v>
+        <v>-58.482817</v>
       </c>
       <c r="N73" t="n">
-        <v>-34.58372</v>
+        <v>-34.550845</v>
       </c>
       <c r="O73" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P73" t="inlineStr">
@@ -5982,7 +5982,7 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>-577</t>
+          <t>7118</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
@@ -5992,17 +5992,17 @@
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>Manuel Ugarte 2318</t>
+          <t>CUBAS, JOSE 2211</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>809406177</t>
+          <t>809406168</t>
         </is>
       </c>
       <c r="F74" t="inlineStr">
@@ -6039,14 +6039,14 @@
         </is>
       </c>
       <c r="M74" t="n">
-        <v>-58.460635</v>
+        <v>-58.492448</v>
       </c>
       <c r="N74" t="n">
-        <v>-34.555932</v>
+        <v>-34.58372</v>
       </c>
       <c r="O74" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P74" t="inlineStr">
@@ -6058,7 +6058,7 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>-578</t>
+          <t>-577</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
@@ -6068,7 +6068,7 @@
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>Pedro I Rivera 2536</t>
+          <t>Manuel Ugarte 2318</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
@@ -6078,7 +6078,7 @@
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>809406189</t>
+          <t>809406177</t>
         </is>
       </c>
       <c r="F75" t="inlineStr">
@@ -6115,10 +6115,10 @@
         </is>
       </c>
       <c r="M75" t="n">
-        <v>-58.462327</v>
+        <v>-58.460635</v>
       </c>
       <c r="N75" t="n">
-        <v>-34.557565</v>
+        <v>-34.555932</v>
       </c>
       <c r="O75" t="inlineStr">
         <is>
@@ -6134,74 +6134,150 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
+          <t>-578</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>9/2/2025</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>Pedro I Rivera 2536</t>
+        </is>
+      </c>
+      <c r="D76" t="inlineStr">
+        <is>
+          <t>13</t>
+        </is>
+      </c>
+      <c r="E76" t="inlineStr">
+        <is>
+          <t>809406189</t>
+        </is>
+      </c>
+      <c r="F76" t="inlineStr">
+        <is>
+          <t>NEW</t>
+        </is>
+      </c>
+      <c r="G76" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H76" t="inlineStr">
+        <is>
+          <t>Picada</t>
+        </is>
+      </c>
+      <c r="I76" t="n">
+        <v>1</v>
+      </c>
+      <c r="J76" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K76" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L76" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M76" t="n">
+        <v>-58.462327</v>
+      </c>
+      <c r="N76" t="n">
+        <v>-34.557565</v>
+      </c>
+      <c r="O76" t="inlineStr">
+        <is>
+          <t>Saavedra</t>
+        </is>
+      </c>
+      <c r="P76" t="inlineStr">
+        <is>
+          <t>Capital Norte</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
           <t>-579</t>
         </is>
       </c>
-      <c r="B76" t="inlineStr">
+      <c r="B77" t="inlineStr">
         <is>
           <t>9/2/2025</t>
         </is>
       </c>
-      <c r="C76" t="inlineStr">
+      <c r="C77" t="inlineStr">
         <is>
           <t>Pedro Rivera 2546</t>
         </is>
       </c>
-      <c r="D76" t="inlineStr">
+      <c r="D77" t="inlineStr">
         <is>
           <t>13</t>
         </is>
       </c>
-      <c r="E76" t="inlineStr">
+      <c r="E77" t="inlineStr">
         <is>
           <t>ICD30612785</t>
         </is>
       </c>
-      <c r="F76" t="inlineStr">
-        <is>
-          <t>NEW</t>
-        </is>
-      </c>
-      <c r="G76" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H76" t="inlineStr">
+      <c r="F77" t="inlineStr">
+        <is>
+          <t>NEW</t>
+        </is>
+      </c>
+      <c r="G77" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H77" t="inlineStr">
         <is>
           <t>Colocar R200 para pedir traspaso de equipos</t>
         </is>
       </c>
-      <c r="I76" t="n">
-        <v>1</v>
-      </c>
-      <c r="J76" t="inlineStr">
+      <c r="I77" t="n">
+        <v>1</v>
+      </c>
+      <c r="J77" t="inlineStr">
         <is>
           <t>Cambio</t>
         </is>
       </c>
-      <c r="K76" t="inlineStr">
+      <c r="K77" t="inlineStr">
         <is>
           <t>Nodo Teco</t>
         </is>
       </c>
-      <c r="L76" t="inlineStr">
+      <c r="L77" t="inlineStr">
         <is>
           <t>Pasante</t>
         </is>
       </c>
-      <c r="M76" t="n">
+      <c r="M77" t="n">
         <v>-58.462479</v>
       </c>
-      <c r="N76" t="n">
+      <c r="N77" t="n">
         <v>-34.55765</v>
       </c>
-      <c r="O76" t="inlineStr">
+      <c r="O77" t="inlineStr">
         <is>
           <t>Saavedra</t>
         </is>
       </c>
-      <c r="P76" t="inlineStr">
+      <c r="P77" t="inlineStr">
         <is>
           <t>Capital Norte</t>
         </is>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-09-04 21:00:47)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_NEW.xlsx
+++ b/mapa_interactivo_NEW.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P77"/>
+  <dimension ref="A1:P79"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -898,27 +898,27 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>4862</t>
+          <t>4528</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>1/23/2025</t>
+          <t>1/16/2025</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>ARCOS 2263</t>
+          <t>BARCO CENTENERA DEL 545</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>802857379</t>
+          <t>802774521</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -928,16 +928,16 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
+          <t>Pendiente</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>picada</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J7" t="inlineStr">
         <is>
@@ -946,7 +946,7 @@
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L7" t="inlineStr">
@@ -955,46 +955,46 @@
         </is>
       </c>
       <c r="M7" t="n">
-        <v>-58.455082</v>
+        <v>-58.440625</v>
       </c>
       <c r="N7" t="n">
-        <v>-34.558883</v>
+        <v>-34.625499</v>
       </c>
       <c r="O7" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P7" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>6036</t>
+          <t>4862</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>2/24/2025</t>
+          <t>1/23/2025</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>MEDRANO 1715</t>
+          <t>ARCOS 2263</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>803608181</t>
+          <t>802857379</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -1004,10 +1004,14 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H8" t="inlineStr"/>
+          <t>Pendiente de Traspaso PROPIO</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>picada</t>
+        </is>
+      </c>
       <c r="I8" t="n">
         <v>0</v>
       </c>
@@ -1027,26 +1031,26 @@
         </is>
       </c>
       <c r="M8" t="n">
-        <v>-58.418236</v>
+        <v>-58.455082</v>
       </c>
       <c r="N8" t="n">
-        <v>-34.589859</v>
+        <v>-34.558883</v>
       </c>
       <c r="O8" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P8" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>803608480</t>
+          <t>6036</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -1056,7 +1060,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>GUATEMALA /ALT/ 4415</t>
+          <t>MEDRANO 1715</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -1066,7 +1070,7 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>803608480</t>
+          <t>803608181</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -1079,11 +1083,7 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H9" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Guatemala 4415 </t>
-        </is>
-      </c>
+      <c r="H9" t="inlineStr"/>
       <c r="I9" t="n">
         <v>0</v>
       </c>
@@ -1094,7 +1094,7 @@
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L9" t="inlineStr">
@@ -1103,10 +1103,10 @@
         </is>
       </c>
       <c r="M9" t="n">
-        <v>-58.421661</v>
+        <v>-58.418236</v>
       </c>
       <c r="N9" t="n">
-        <v>-34.588428</v>
+        <v>-34.589859</v>
       </c>
       <c r="O9" t="inlineStr">
         <is>
@@ -1122,27 +1122,27 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>5053</t>
+          <t>803608480</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>3/11/2025</t>
+          <t>2/24/2025</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>MENDOZA 1153</t>
+          <t>GUATEMALA /ALT/ 4415</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>803969314</t>
+          <t>803608480</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
@@ -1157,7 +1157,7 @@
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t xml:space="preserve">Guatemala 4415 </t>
         </is>
       </c>
       <c r="I10" t="n">
@@ -1175,50 +1175,50 @@
       </c>
       <c r="L10" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M10" t="n">
-        <v>-58.44463</v>
+        <v>-58.421661</v>
       </c>
       <c r="N10" t="n">
-        <v>-34.553354</v>
+        <v>-34.588428</v>
       </c>
       <c r="O10" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P10" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>6071</t>
+          <t>5053</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>3/17/2025</t>
+          <t>3/11/2025</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>OSORIO 4994</t>
+          <t>MENDOZA 1153</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>804053324</t>
+          <t>803969314</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
@@ -1231,7 +1231,11 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H11" t="inlineStr"/>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>Poste</t>
+        </is>
+      </c>
       <c r="I11" t="n">
         <v>0</v>
       </c>
@@ -1247,18 +1251,18 @@
       </c>
       <c r="L11" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M11" t="n">
-        <v>-58.466241</v>
+        <v>-58.44463</v>
       </c>
       <c r="N11" t="n">
-        <v>-34.595741</v>
+        <v>-34.553354</v>
       </c>
       <c r="O11" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P11" t="inlineStr">
@@ -1270,27 +1274,27 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>3348</t>
+          <t>6071</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>3/27/2025</t>
+          <t>3/17/2025</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>ESTOMBA 2626</t>
+          <t>OSORIO 4994</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>804309704</t>
+          <t>804053324</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
@@ -1303,17 +1307,13 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H12" t="inlineStr">
-        <is>
-          <t>Picada</t>
-        </is>
-      </c>
+      <c r="H12" t="inlineStr"/>
       <c r="I12" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>Desmonte</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K12" t="inlineStr">
@@ -1327,14 +1327,14 @@
         </is>
       </c>
       <c r="M12" t="n">
-        <v>-58.47538</v>
+        <v>-58.466241</v>
       </c>
       <c r="N12" t="n">
-        <v>-34.566015</v>
+        <v>-34.595741</v>
       </c>
       <c r="O12" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P12" t="inlineStr">
@@ -1346,27 +1346,27 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>-312</t>
+          <t>2485</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>3/29/2025</t>
+          <t>3/26/2025</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>MATIENZO BENJAMIN /ALT/ 1831</t>
+          <t>LA PLATA AV. 1095</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>804333522</t>
+          <t>804302893</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
@@ -1381,36 +1381,36 @@
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>Retirar columna ya traspasaron el nodo</t>
+          <t>Sacar ancla de rienda vieja y cementar vereda</t>
         </is>
       </c>
       <c r="I13" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Tensor</t>
         </is>
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L13" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M13" t="n">
-        <v>-58.434835</v>
+        <v>-58.426593</v>
       </c>
       <c r="N13" t="n">
-        <v>-34.569129</v>
+        <v>-34.628211</v>
       </c>
       <c r="O13" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P13" t="inlineStr">
@@ -1422,17 +1422,17 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>3430</t>
+          <t>3348</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>4/1/2025</t>
+          <t>3/27/2025</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>MONROE 3838</t>
+          <t>ESTOMBA 2626</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
@@ -1442,7 +1442,7 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>804468442</t>
+          <t>804309704</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
@@ -1457,7 +1457,7 @@
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>Reparar rienda</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I14" t="n">
@@ -1465,7 +1465,7 @@
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>Tensor</t>
+          <t>Desmonte</t>
         </is>
       </c>
       <c r="K14" t="inlineStr">
@@ -1475,14 +1475,14 @@
       </c>
       <c r="L14" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M14" t="n">
-        <v>-58.473659</v>
+        <v>-58.47538</v>
       </c>
       <c r="N14" t="n">
-        <v>-34.566979</v>
+        <v>-34.566015</v>
       </c>
       <c r="O14" t="inlineStr">
         <is>
@@ -1498,27 +1498,27 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>5464</t>
+          <t>-312</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>4/4/2025</t>
+          <t>3/29/2025</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>SUCRE, ANTONIO JOSE DE, MCAL. 3100</t>
+          <t>MATIENZO BENJAMIN /ALT/ 1831</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>804497880</t>
+          <t>804333522</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
@@ -1533,11 +1533,11 @@
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Retirar columna ya traspasaron el nodo</t>
         </is>
       </c>
       <c r="I15" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J15" t="inlineStr">
         <is>
@@ -1546,45 +1546,45 @@
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L15" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M15" t="n">
-        <v>-58.46161</v>
+        <v>-58.434835</v>
       </c>
       <c r="N15" t="n">
-        <v>-34.567849</v>
+        <v>-34.569129</v>
       </c>
       <c r="O15" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P15" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>5469</t>
+          <t>3430</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>4/4/2025</t>
+          <t>4/1/2025</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>ESTADO PLURINACIONAL DE BOLIVIA 5899</t>
+          <t>MONROE 3838</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
@@ -1594,7 +1594,7 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>804497887</t>
+          <t>804468442</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
@@ -1609,7 +1609,7 @@
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>Aplomar</t>
+          <t>Reparar rienda</t>
         </is>
       </c>
       <c r="I16" t="n">
@@ -1617,7 +1617,7 @@
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Tensor</t>
         </is>
       </c>
       <c r="K16" t="inlineStr">
@@ -1631,14 +1631,14 @@
         </is>
       </c>
       <c r="M16" t="n">
-        <v>-58.507746</v>
+        <v>-58.473659</v>
       </c>
       <c r="N16" t="n">
-        <v>-34.574217</v>
+        <v>-34.566979</v>
       </c>
       <c r="O16" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P16" t="inlineStr">
@@ -1650,7 +1650,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>5492</t>
+          <t>5464</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -1660,17 +1660,17 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>ESTADO PLURINACIONAL DE BOLIVIA 5920</t>
+          <t>SUCRE, ANTONIO JOSE DE, MCAL. 3100</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>804498035</t>
+          <t>804497880</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
@@ -1685,7 +1685,7 @@
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>aplomar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I17" t="n">
@@ -1693,7 +1693,7 @@
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K17" t="inlineStr">
@@ -1707,14 +1707,14 @@
         </is>
       </c>
       <c r="M17" t="n">
-        <v>-58.50751</v>
+        <v>-58.46161</v>
       </c>
       <c r="N17" t="n">
-        <v>-34.574543</v>
+        <v>-34.567849</v>
       </c>
       <c r="O17" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P17" t="inlineStr">
@@ -1726,17 +1726,17 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>5599</t>
+          <t>5469</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>4/15/2025</t>
+          <t>4/4/2025</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>ESTOMBA 4052</t>
+          <t>ESTADO PLURINACIONAL DE BOLIVIA 5899</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
@@ -1746,7 +1746,7 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>804732246</t>
+          <t>804497887</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
@@ -1761,7 +1761,7 @@
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>Columna PRFV quedo inclinada (la hicieron como estomba 4056)</t>
+          <t>Aplomar</t>
         </is>
       </c>
       <c r="I18" t="n">
@@ -1774,23 +1774,23 @@
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>Nodo TLC</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L18" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M18" t="n">
-        <v>-58.485407</v>
+        <v>-58.507746</v>
       </c>
       <c r="N18" t="n">
-        <v>-34.552985</v>
+        <v>-34.574217</v>
       </c>
       <c r="O18" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P18" t="inlineStr">
@@ -1802,27 +1802,27 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>5590</t>
+          <t>5492</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>4/15/2025</t>
+          <t>4/4/2025</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>O'HIGGINS 2441</t>
+          <t>ESTADO PLURINACIONAL DE BOLIVIA 5920</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>804732275</t>
+          <t>804498035</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
@@ -1837,7 +1837,7 @@
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>aplomar</t>
         </is>
       </c>
       <c r="I19" t="n">
@@ -1845,7 +1845,7 @@
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K19" t="inlineStr">
@@ -1855,18 +1855,18 @@
       </c>
       <c r="L19" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M19" t="n">
-        <v>-58.45573</v>
+        <v>-58.50751</v>
       </c>
       <c r="N19" t="n">
-        <v>-34.556576</v>
+        <v>-34.574543</v>
       </c>
       <c r="O19" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P19" t="inlineStr">
@@ -1878,27 +1878,27 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>804787368</t>
+          <t>5599</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>4/17/2025</t>
+          <t>4/15/2025</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>San Blas 2591</t>
+          <t>ESTOMBA 4052</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>804787368</t>
+          <t>804732246</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
@@ -1913,7 +1913,7 @@
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Columna PRFV quedo inclinada (la hicieron como estomba 4056)</t>
         </is>
       </c>
       <c r="I20" t="n">
@@ -1921,12 +1921,12 @@
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo TLC</t>
         </is>
       </c>
       <c r="L20" t="inlineStr">
@@ -1935,14 +1935,14 @@
         </is>
       </c>
       <c r="M20" t="n">
-        <v>-58.477427</v>
+        <v>-58.485407</v>
       </c>
       <c r="N20" t="n">
-        <v>-34.609261</v>
+        <v>-34.552985</v>
       </c>
       <c r="O20" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P20" t="inlineStr">
@@ -1954,17 +1954,17 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>5624</t>
+          <t>5590</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>4/22/2025</t>
+          <t>4/15/2025</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>PINO, VIRREY DEL 3456</t>
+          <t>O'HIGGINS 2441</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
@@ -1974,7 +1974,7 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>804876043</t>
+          <t>804732275</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
@@ -1989,7 +1989,7 @@
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>Desmonte de poste</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I21" t="n">
@@ -1997,7 +1997,7 @@
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>Desmonte</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K21" t="inlineStr">
@@ -2007,18 +2007,18 @@
       </c>
       <c r="L21" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M21" t="n">
-        <v>-58.464354</v>
+        <v>-58.45573</v>
       </c>
       <c r="N21" t="n">
-        <v>-34.572486</v>
+        <v>-34.556576</v>
       </c>
       <c r="O21" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P21" t="inlineStr">
@@ -2030,27 +2030,27 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>804922147</t>
+          <t>804787368</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>4/24/2025</t>
+          <t>4/17/2025</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Av. Álvarez Thomas 1171</t>
+          <t>San Blas 2591</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>804922147</t>
+          <t>804787368</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
@@ -2069,7 +2069,7 @@
         </is>
       </c>
       <c r="I22" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J22" t="inlineStr">
         <is>
@@ -2087,14 +2087,14 @@
         </is>
       </c>
       <c r="M22" t="n">
-        <v>-58.45793</v>
+        <v>-58.477427</v>
       </c>
       <c r="N22" t="n">
-        <v>-34.578334</v>
+        <v>-34.609261</v>
       </c>
       <c r="O22" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P22" t="inlineStr">
@@ -2106,17 +2106,17 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>804922171</t>
+          <t>5624</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>4/24/2025</t>
+          <t>4/22/2025</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Virrey Arredondo 3581</t>
+          <t>PINO, VIRREY DEL 3456</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
@@ -2126,7 +2126,7 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>804922171</t>
+          <t>804876043</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
@@ -2141,7 +2141,7 @@
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>Aplomar</t>
+          <t>Desmonte de poste</t>
         </is>
       </c>
       <c r="I23" t="n">
@@ -2149,7 +2149,7 @@
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Desmonte</t>
         </is>
       </c>
       <c r="K23" t="inlineStr">
@@ -2159,14 +2159,14 @@
       </c>
       <c r="L23" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M23" t="n">
-        <v>-58.459513</v>
+        <v>-58.464354</v>
       </c>
       <c r="N23" t="n">
-        <v>-34.578019</v>
+        <v>-34.572486</v>
       </c>
       <c r="O23" t="inlineStr">
         <is>
@@ -2182,7 +2182,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>5656</t>
+          <t>804922147</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -2192,17 +2192,17 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>ECHEVERRIA 5893</t>
+          <t>Av. Álvarez Thomas 1171</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>804922184</t>
+          <t>804922147</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
@@ -2217,15 +2217,15 @@
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>Poste con base quebrada</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I24" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J24" t="inlineStr">
         <is>
-          <t>Desmonte</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K24" t="inlineStr">
@@ -2235,18 +2235,18 @@
       </c>
       <c r="L24" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M24" t="n">
-        <v>-58.489627</v>
+        <v>-58.45793</v>
       </c>
       <c r="N24" t="n">
-        <v>-34.583761</v>
+        <v>-34.578334</v>
       </c>
       <c r="O24" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P24" t="inlineStr">
@@ -2258,27 +2258,27 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>6173</t>
+          <t>804922171</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>4/29/2025</t>
+          <t>4/24/2025</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>ARMENIA 2321</t>
+          <t>Virrey Arredondo 3581</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>805507398</t>
+          <t>804922171</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
@@ -2293,7 +2293,7 @@
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>Picada volvio a entrar como caso 6325</t>
+          <t>Aplomar</t>
         </is>
       </c>
       <c r="I25" t="n">
@@ -2301,7 +2301,7 @@
       </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K25" t="inlineStr">
@@ -2311,40 +2311,40 @@
       </c>
       <c r="L25" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M25" t="n">
-        <v>-58.420549</v>
+        <v>-58.459513</v>
       </c>
       <c r="N25" t="n">
-        <v>-34.585103</v>
+        <v>-34.578019</v>
       </c>
       <c r="O25" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P25" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>5715</t>
+          <t>5656</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>5/1/2025</t>
+          <t>4/24/2025</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>CUENCA 4690</t>
+          <t>ECHEVERRIA 5893</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
@@ -2354,7 +2354,7 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>805579094</t>
+          <t>804922184</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
@@ -2369,7 +2369,7 @@
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>Aplomar poste</t>
+          <t>Poste con base quebrada</t>
         </is>
       </c>
       <c r="I26" t="n">
@@ -2377,7 +2377,7 @@
       </c>
       <c r="J26" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Desmonte</t>
         </is>
       </c>
       <c r="K26" t="inlineStr">
@@ -2391,10 +2391,10 @@
         </is>
       </c>
       <c r="M26" t="n">
-        <v>-58.506061</v>
+        <v>-58.489627</v>
       </c>
       <c r="N26" t="n">
-        <v>-34.588887</v>
+        <v>-34.583761</v>
       </c>
       <c r="O26" t="inlineStr">
         <is>
@@ -2410,17 +2410,17 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>6333</t>
+          <t>6173</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>5/1/2025</t>
+          <t>4/29/2025</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>ORTEGA Y GASSET 1816</t>
+          <t>ARMENIA 2321</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
@@ -2430,7 +2430,7 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>805655342</t>
+          <t>805507398</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
@@ -2445,7 +2445,7 @@
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Picada volvio a entrar como caso 6325</t>
         </is>
       </c>
       <c r="I27" t="n">
@@ -2467,10 +2467,10 @@
         </is>
       </c>
       <c r="M27" t="n">
-        <v>-58.432556</v>
+        <v>-58.420549</v>
       </c>
       <c r="N27" t="n">
-        <v>-34.570279</v>
+        <v>-34.585103</v>
       </c>
       <c r="O27" t="inlineStr">
         <is>
@@ -2486,27 +2486,27 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>805707165</t>
+          <t>5715</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>5/7/2025</t>
+          <t>5/1/2025</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Baez 793</t>
+          <t>CUENCA 4690</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>ICD30592749</t>
+          <t>805579094</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
@@ -2521,7 +2521,7 @@
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>DESMONTAR COLUMNA DE 7 MTS Y TRANSFERIR A COMUNITARIA</t>
+          <t>Aplomar poste</t>
         </is>
       </c>
       <c r="I28" t="n">
@@ -2529,7 +2529,7 @@
       </c>
       <c r="J28" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K28" t="inlineStr">
@@ -2539,40 +2539,40 @@
       </c>
       <c r="L28" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M28" t="n">
-        <v>-58.436165</v>
+        <v>-58.506061</v>
       </c>
       <c r="N28" t="n">
-        <v>-34.569081</v>
+        <v>-34.588887</v>
       </c>
       <c r="O28" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P28" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>232</t>
+          <t>6333</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>5/9/2025</t>
+          <t>5/1/2025</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Gorostiaga 2286</t>
+          <t>ORTEGA Y GASSET 1816</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
@@ -2582,7 +2582,7 @@
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>805791858</t>
+          <t>805655342</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
@@ -2619,10 +2619,10 @@
         </is>
       </c>
       <c r="M29" t="n">
-        <v>-58.441563</v>
+        <v>-58.432556</v>
       </c>
       <c r="N29" t="n">
-        <v>-34.569743</v>
+        <v>-34.570279</v>
       </c>
       <c r="O29" t="inlineStr">
         <is>
@@ -2638,27 +2638,27 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>-404</t>
+          <t>805707165</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>5/8/2025</t>
+          <t>5/7/2025</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Amenabar 3048</t>
+          <t>Baez 793</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>805791896</t>
+          <t>ICD30592749</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
@@ -2673,7 +2673,7 @@
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>Aplomar columna 114</t>
+          <t>DESMONTAR COLUMNA DE 7 MTS Y TRANSFERIR A COMUNITARIA</t>
         </is>
       </c>
       <c r="I30" t="n">
@@ -2681,7 +2681,7 @@
       </c>
       <c r="J30" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K30" t="inlineStr">
@@ -2691,50 +2691,50 @@
       </c>
       <c r="L30" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M30" t="n">
-        <v>-58.46579</v>
+        <v>-58.436165</v>
       </c>
       <c r="N30" t="n">
-        <v>-34.555012</v>
+        <v>-34.569081</v>
       </c>
       <c r="O30" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P30" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>-406</t>
+          <t>232</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>5/8/2025</t>
+          <t>5/9/2025</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Olof palme 4144</t>
+          <t>Gorostiaga 2286</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>805791925</t>
+          <t>805791858</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
@@ -2749,7 +2749,7 @@
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>Tensar 2 riendas a pique columna 168</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I31" t="n">
@@ -2757,7 +2757,7 @@
       </c>
       <c r="J31" t="inlineStr">
         <is>
-          <t>Tensor</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K31" t="inlineStr">
@@ -2767,50 +2767,50 @@
       </c>
       <c r="L31" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M31" t="n">
-        <v>-58.488252</v>
+        <v>-58.441563</v>
       </c>
       <c r="N31" t="n">
-        <v>-34.553391</v>
+        <v>-34.569743</v>
       </c>
       <c r="O31" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P31" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>5826</t>
+          <t>-404</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>5/19/2025</t>
+          <t>5/8/2025</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>ALBARELLOS AV. 3180</t>
+          <t>Amenabar 3048</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>806926466</t>
+          <t>805791896</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
@@ -2825,7 +2825,7 @@
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>Columna (metal) inclinada</t>
+          <t>Aplomar columna 114</t>
         </is>
       </c>
       <c r="I32" t="n">
@@ -2843,18 +2843,18 @@
       </c>
       <c r="L32" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M32" t="n">
-        <v>-58.513552</v>
+        <v>-58.46579</v>
       </c>
       <c r="N32" t="n">
-        <v>-34.579829</v>
+        <v>-34.555012</v>
       </c>
       <c r="O32" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P32" t="inlineStr">
@@ -2866,27 +2866,27 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>6020</t>
+          <t>-406</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>6/5/2025</t>
+          <t>5/8/2025</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>RAVIGNANI, EMILIO, DR. 2036</t>
+          <t>Olof palme 4144</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>807215465</t>
+          <t>805791925</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
@@ -2901,7 +2901,7 @@
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>Picada misma que 6260 y 6945</t>
+          <t>Tensar 2 riendas a pique columna 168</t>
         </is>
       </c>
       <c r="I33" t="n">
@@ -2909,7 +2909,7 @@
       </c>
       <c r="J33" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Tensor</t>
         </is>
       </c>
       <c r="K33" t="inlineStr">
@@ -2919,50 +2919,50 @@
       </c>
       <c r="L33" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M33" t="n">
-        <v>-58.436298</v>
+        <v>-58.488252</v>
       </c>
       <c r="N33" t="n">
-        <v>-34.578972</v>
+        <v>-34.553391</v>
       </c>
       <c r="O33" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P33" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>6144</t>
+          <t>5826</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>6/11/2025</t>
+          <t>5/19/2025</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>TURIN 2990</t>
+          <t>ALBARELLOS AV. 3180</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>807458282</t>
+          <t>806926466</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
@@ -2977,7 +2977,7 @@
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Columna (metal) inclinada</t>
         </is>
       </c>
       <c r="I34" t="n">
@@ -2985,7 +2985,7 @@
       </c>
       <c r="J34" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K34" t="inlineStr">
@@ -2995,14 +2995,14 @@
       </c>
       <c r="L34" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M34" t="n">
-        <v>-58.480925</v>
+        <v>-58.513552</v>
       </c>
       <c r="N34" t="n">
-        <v>-34.585471</v>
+        <v>-34.579829</v>
       </c>
       <c r="O34" t="inlineStr">
         <is>
@@ -3018,7 +3018,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>6143</t>
+          <t>6144</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
@@ -3028,7 +3028,7 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>SOLANO LOPEZ, F., MARISCAL 2845</t>
+          <t>TURIN 2990</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
@@ -3038,7 +3038,7 @@
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>807458296</t>
+          <t>807458282</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
@@ -3075,10 +3075,10 @@
         </is>
       </c>
       <c r="M35" t="n">
-        <v>-58.495071</v>
+        <v>-58.480925</v>
       </c>
       <c r="N35" t="n">
-        <v>-34.593122</v>
+        <v>-34.585471</v>
       </c>
       <c r="O35" t="inlineStr">
         <is>
@@ -3094,27 +3094,27 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>-478</t>
+          <t>6143</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>6/15/2025</t>
+          <t>6/11/2025</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Chivilcoy 4875</t>
+          <t>SOLANO LOPEZ, F., MARISCAL 2845</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>807508509</t>
+          <t>807458296</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
@@ -3129,7 +3129,7 @@
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>Poste podrido</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I36" t="n">
@@ -3147,14 +3147,14 @@
       </c>
       <c r="L36" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M36" t="n">
-        <v>-58.517389</v>
+        <v>-58.495071</v>
       </c>
       <c r="N36" t="n">
-        <v>-34.593541</v>
+        <v>-34.593122</v>
       </c>
       <c r="O36" t="inlineStr">
         <is>
@@ -3170,27 +3170,27 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>6171</t>
+          <t>-478</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>6/18/2025</t>
+          <t>6/15/2025</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>CABELLO 3486</t>
+          <t>Chivilcoy 4875</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>807658640</t>
+          <t>807508509</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
@@ -3205,7 +3205,7 @@
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>Columna inclinada evaluar con inspector un corrimiento</t>
+          <t>Poste podrido</t>
         </is>
       </c>
       <c r="I37" t="n">
@@ -3223,40 +3223,40 @@
       </c>
       <c r="L37" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M37" t="n">
-        <v>-58.409579</v>
+        <v>-58.517389</v>
       </c>
       <c r="N37" t="n">
-        <v>-34.581134</v>
+        <v>-34.593541</v>
       </c>
       <c r="O37" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P37" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>6230</t>
+          <t>6171</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>6/24/2025</t>
+          <t>6/18/2025</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Santa maria de oro	2722</t>
+          <t>CABELLO 3486</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
@@ -3266,7 +3266,7 @@
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>807763066</t>
+          <t>807658640</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
@@ -3281,7 +3281,7 @@
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Columna inclinada evaluar con inspector un corrimiento</t>
         </is>
       </c>
       <c r="I38" t="n">
@@ -3303,10 +3303,10 @@
         </is>
       </c>
       <c r="M38" t="n">
-        <v>-58.422315</v>
+        <v>-58.409579</v>
       </c>
       <c r="N38" t="n">
-        <v>-34.576988</v>
+        <v>-34.581134</v>
       </c>
       <c r="O38" t="inlineStr">
         <is>
@@ -3322,7 +3322,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>6231</t>
+          <t>6230</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
@@ -3332,7 +3332,7 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Ciudad de la Paz 275</t>
+          <t>Santa maria de oro	2722</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
@@ -3342,7 +3342,7 @@
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>807763070</t>
+          <t>807763066</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
@@ -3357,7 +3357,7 @@
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>Aplomar o cambiar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I39" t="n">
@@ -3375,14 +3375,14 @@
       </c>
       <c r="L39" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M39" t="n">
-        <v>-58.441049</v>
+        <v>-58.422315</v>
       </c>
       <c r="N39" t="n">
-        <v>-34.574625</v>
+        <v>-34.576988</v>
       </c>
       <c r="O39" t="inlineStr">
         <is>
@@ -3398,7 +3398,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>6235</t>
+          <t>6231</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
@@ -3408,17 +3408,17 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>HUERGO 389</t>
+          <t>Ciudad de la Paz 275</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>807763078</t>
+          <t>807763070</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
@@ -3433,7 +3433,7 @@
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Aplomar o cambiar</t>
         </is>
       </c>
       <c r="I40" t="n">
@@ -3451,14 +3451,14 @@
       </c>
       <c r="L40" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M40" t="n">
-        <v>-58.432722</v>
+        <v>-58.441049</v>
       </c>
       <c r="N40" t="n">
-        <v>-34.572371</v>
+        <v>-34.574625</v>
       </c>
       <c r="O40" t="inlineStr">
         <is>
@@ -3474,27 +3474,27 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>6295</t>
+          <t>6235</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>6/30/2025</t>
+          <t>6/24/2025</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>SOLER 6017</t>
+          <t>HUERGO 389</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>807851636</t>
+          <t>807763078</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
@@ -3531,10 +3531,10 @@
         </is>
       </c>
       <c r="M41" t="n">
-        <v>-58.436808</v>
+        <v>-58.432722</v>
       </c>
       <c r="N41" t="n">
-        <v>-34.577464</v>
+        <v>-34.572371</v>
       </c>
       <c r="O41" t="inlineStr">
         <is>
@@ -3550,17 +3550,17 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>6332</t>
+          <t>6295</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>7/3/2025</t>
+          <t>6/30/2025</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>ARAOZ 2560</t>
+          <t>SOLER 6017</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
@@ -3570,7 +3570,7 @@
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>807965818</t>
+          <t>807851636</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
@@ -3607,10 +3607,10 @@
         </is>
       </c>
       <c r="M42" t="n">
-        <v>-58.414507</v>
+        <v>-58.436808</v>
       </c>
       <c r="N42" t="n">
-        <v>-34.585377</v>
+        <v>-34.577464</v>
       </c>
       <c r="O42" t="inlineStr">
         <is>
@@ -3626,27 +3626,27 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>6506</t>
+          <t>6308</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>7/10/2025</t>
+          <t>7/1/2025</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Ohiggins 1611</t>
+          <t>Guayaquil 637</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>808148679</t>
+          <t>807896343</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
@@ -3661,7 +3661,7 @@
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>Columna podrida en la base</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I43" t="n">
@@ -3674,7 +3674,7 @@
       </c>
       <c r="K43" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L43" t="inlineStr">
@@ -3683,46 +3683,46 @@
         </is>
       </c>
       <c r="M43" t="n">
-        <v>-58.448993</v>
+        <v>-58.437378</v>
       </c>
       <c r="N43" t="n">
-        <v>-34.564383</v>
+        <v>-34.62116</v>
       </c>
       <c r="O43" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P43" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>6437</t>
+          <t>6332</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>7/17/2025</t>
+          <t>7/3/2025</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>MILLER 4590</t>
+          <t>ARAOZ 2560</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>808400306</t>
+          <t>807965818</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
@@ -3737,7 +3737,7 @@
       </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t>Columna corroida</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I44" t="n">
@@ -3759,46 +3759,46 @@
         </is>
       </c>
       <c r="M44" t="n">
-        <v>-58.495482</v>
+        <v>-58.414507</v>
       </c>
       <c r="N44" t="n">
-        <v>-34.552614</v>
+        <v>-34.585377</v>
       </c>
       <c r="O44" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P44" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>6538</t>
+          <t>6383</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>7/17/2025</t>
+          <t>7/8/2025</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Pedraza Manuela 4101</t>
+          <t>FALCON, RAMON L.,CNEL. 1411</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>808400353</t>
+          <t>808099320</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
@@ -3813,7 +3813,7 @@
       </c>
       <c r="H45" t="inlineStr">
         <is>
-          <t xml:space="preserve">Podrida en la base </t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I45" t="n">
@@ -3835,46 +3835,46 @@
         </is>
       </c>
       <c r="M45" t="n">
-        <v>-58.481569</v>
+        <v>-58.448523</v>
       </c>
       <c r="N45" t="n">
-        <v>-34.559853</v>
+        <v>-34.62452</v>
       </c>
       <c r="O45" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P45" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>7023</t>
+          <t>6506</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>7/22/2025</t>
+          <t>7/10/2025</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>ZABALA 3573</t>
+          <t>Ohiggins 1611</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>808480549</t>
+          <t>808148679</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
@@ -3889,7 +3889,7 @@
       </c>
       <c r="H46" t="inlineStr">
         <is>
-          <t>Corroida en base para recambio</t>
+          <t>Columna podrida en la base</t>
         </is>
       </c>
       <c r="I46" t="n">
@@ -3902,7 +3902,7 @@
       </c>
       <c r="K46" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L46" t="inlineStr">
@@ -3911,10 +3911,10 @@
         </is>
       </c>
       <c r="M46" t="n">
-        <v>-58.457522</v>
+        <v>-58.448993</v>
       </c>
       <c r="N46" t="n">
-        <v>-34.579414</v>
+        <v>-34.564383</v>
       </c>
       <c r="O46" t="inlineStr">
         <is>
@@ -3930,27 +3930,27 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>6484</t>
+          <t>6437</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>7/24/2025</t>
+          <t>7/17/2025</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>URIARTE 2396</t>
+          <t>MILLER 4590</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>808509373</t>
+          <t>808400306</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
@@ -3965,7 +3965,7 @@
       </c>
       <c r="H47" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Columna corroida</t>
         </is>
       </c>
       <c r="I47" t="n">
@@ -3987,46 +3987,46 @@
         </is>
       </c>
       <c r="M47" t="n">
-        <v>-58.423934</v>
+        <v>-58.495482</v>
       </c>
       <c r="N47" t="n">
-        <v>-34.581562</v>
+        <v>-34.552614</v>
       </c>
       <c r="O47" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P47" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>6512</t>
+          <t>6538</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>7/28/2025</t>
+          <t>7/17/2025</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>GASCON 1195</t>
+          <t>Pedraza Manuela 4101</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>808571975</t>
+          <t>808400353</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
@@ -4041,7 +4041,7 @@
       </c>
       <c r="H48" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t xml:space="preserve">Podrida en la base </t>
         </is>
       </c>
       <c r="I48" t="n">
@@ -4063,46 +4063,46 @@
         </is>
       </c>
       <c r="M48" t="n">
-        <v>-58.423127</v>
+        <v>-58.481569</v>
       </c>
       <c r="N48" t="n">
-        <v>-34.596476</v>
+        <v>-34.559853</v>
       </c>
       <c r="O48" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P48" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>6513</t>
+          <t>7023</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>7/28/2025</t>
+          <t>7/22/2025</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>DORREGO 1925</t>
+          <t>ZABALA 3573</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>808571976</t>
+          <t>808480549</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
@@ -4117,7 +4117,7 @@
       </c>
       <c r="H49" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Corroida en base para recambio</t>
         </is>
       </c>
       <c r="I49" t="n">
@@ -4139,36 +4139,36 @@
         </is>
       </c>
       <c r="M49" t="n">
-        <v>-58.441281</v>
+        <v>-58.457522</v>
       </c>
       <c r="N49" t="n">
-        <v>-34.579867</v>
+        <v>-34.579414</v>
       </c>
       <c r="O49" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P49" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>6519</t>
+          <t>6484</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>7/28/2025</t>
+          <t>7/24/2025</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>SALGUERO, JERONIMO 2874</t>
+          <t>URIARTE 2396</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
@@ -4178,7 +4178,7 @@
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>808571977</t>
+          <t>808509373</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
@@ -4193,7 +4193,7 @@
       </c>
       <c r="H50" t="inlineStr">
         <is>
-          <t>Reparar rienda</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I50" t="n">
@@ -4201,7 +4201,7 @@
       </c>
       <c r="J50" t="inlineStr">
         <is>
-          <t>Tensor</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K50" t="inlineStr">
@@ -4211,14 +4211,14 @@
       </c>
       <c r="L50" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M50" t="n">
-        <v>-58.407256</v>
+        <v>-58.423934</v>
       </c>
       <c r="N50" t="n">
-        <v>-34.578976</v>
+        <v>-34.581562</v>
       </c>
       <c r="O50" t="inlineStr">
         <is>
@@ -4234,27 +4234,27 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>-538</t>
+          <t>6512</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>7/31/2025</t>
+          <t>7/28/2025</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Malabia 964</t>
+          <t>GASCON 1195</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>808609237</t>
+          <t>808571975</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
@@ -4269,7 +4269,7 @@
       </c>
       <c r="H51" t="inlineStr">
         <is>
-          <t>Cambiar poste mal estado por PRFV</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I51" t="n">
@@ -4287,14 +4287,14 @@
       </c>
       <c r="L51" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M51" t="n">
-        <v>-58.433634</v>
+        <v>-58.423127</v>
       </c>
       <c r="N51" t="n">
-        <v>-34.595018</v>
+        <v>-34.596476</v>
       </c>
       <c r="O51" t="inlineStr">
         <is>
@@ -4310,27 +4310,27 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>-547</t>
+          <t>6519</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>8/6/2025</t>
+          <t>7/28/2025</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>Habana 4210</t>
+          <t>SALGUERO, JERONIMO 2874</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>808733921</t>
+          <t>808571977</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
@@ -4345,7 +4345,7 @@
       </c>
       <c r="H52" t="inlineStr">
         <is>
-          <t>Cambiar poste dañado</t>
+          <t>Reparar rienda</t>
         </is>
       </c>
       <c r="I52" t="n">
@@ -4353,7 +4353,7 @@
       </c>
       <c r="J52" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Tensor</t>
         </is>
       </c>
       <c r="K52" t="inlineStr">
@@ -4363,50 +4363,50 @@
       </c>
       <c r="L52" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M52" t="n">
-        <v>-58.515873</v>
+        <v>-58.407256</v>
       </c>
       <c r="N52" t="n">
-        <v>-34.599425</v>
+        <v>-34.578976</v>
       </c>
       <c r="O52" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P52" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>6579</t>
+          <t>-538</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>8/7/2025</t>
+          <t>7/31/2025</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>RIVADAVIA MARTIN, COMODORO 1350</t>
+          <t>Malabia 964</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>808749184</t>
+          <t>808609237</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
@@ -4421,7 +4421,7 @@
       </c>
       <c r="H53" t="inlineStr">
         <is>
-          <t>Poste inclinado</t>
+          <t>Cambiar poste mal estado por PRFV</t>
         </is>
       </c>
       <c r="I53" t="n">
@@ -4429,7 +4429,7 @@
       </c>
       <c r="J53" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K53" t="inlineStr">
@@ -4443,46 +4443,46 @@
         </is>
       </c>
       <c r="M53" t="n">
-        <v>-58.461024</v>
+        <v>-58.433634</v>
       </c>
       <c r="N53" t="n">
-        <v>-34.539409</v>
+        <v>-34.595018</v>
       </c>
       <c r="O53" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P53" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>6906</t>
+          <t>-547</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>8/12/2025</t>
+          <t>8/6/2025</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>MOSCONI GENERAL AV. 3163</t>
+          <t>Habana 4210</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>808918685</t>
+          <t>808733921</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
@@ -4497,7 +4497,7 @@
       </c>
       <c r="H54" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambiar poste dañado</t>
         </is>
       </c>
       <c r="I54" t="n">
@@ -4515,14 +4515,14 @@
       </c>
       <c r="L54" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M54" t="n">
-        <v>-58.505731</v>
+        <v>-58.515873</v>
       </c>
       <c r="N54" t="n">
-        <v>-34.588316</v>
+        <v>-34.599425</v>
       </c>
       <c r="O54" t="inlineStr">
         <is>
@@ -4538,27 +4538,27 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>6002</t>
+          <t>6579</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>8/12/2025</t>
+          <t>8/7/2025</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>LA PLATA AV. 832</t>
+          <t>RIVADAVIA MARTIN, COMODORO 1350</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>808918694</t>
+          <t>808749184</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
@@ -4573,7 +4573,7 @@
       </c>
       <c r="H55" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Poste inclinado</t>
         </is>
       </c>
       <c r="I55" t="n">
@@ -4581,7 +4581,7 @@
       </c>
       <c r="J55" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K55" t="inlineStr">
@@ -4591,30 +4591,30 @@
       </c>
       <c r="L55" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M55" t="n">
-        <v>-58.426947</v>
+        <v>-58.461024</v>
       </c>
       <c r="N55" t="n">
-        <v>-34.625698</v>
+        <v>-34.539409</v>
       </c>
       <c r="O55" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P55" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>6910</t>
+          <t>6906</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
@@ -4624,17 +4624,17 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>RIVAS, GRAL. 2345</t>
+          <t>MOSCONI GENERAL AV. 3163</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>808918698</t>
+          <t>808918685</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
@@ -4649,7 +4649,7 @@
       </c>
       <c r="H56" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I56" t="n">
@@ -4671,10 +4671,10 @@
         </is>
       </c>
       <c r="M56" t="n">
-        <v>-58.482497</v>
+        <v>-58.505731</v>
       </c>
       <c r="N56" t="n">
-        <v>-34.598714</v>
+        <v>-34.588316</v>
       </c>
       <c r="O56" t="inlineStr">
         <is>
@@ -4690,7 +4690,7 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>6928</t>
+          <t>6002</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
@@ -4700,17 +4700,17 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>ALBARELLOS AV. 3101</t>
+          <t>LA PLATA AV. 832</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>808918710</t>
+          <t>808918694</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
@@ -4747,26 +4747,26 @@
         </is>
       </c>
       <c r="M57" t="n">
-        <v>-58.512623</v>
+        <v>-58.426947</v>
       </c>
       <c r="N57" t="n">
-        <v>-34.579137</v>
+        <v>-34.625698</v>
       </c>
       <c r="O57" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P57" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>-550</t>
+          <t>6910</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
@@ -4776,17 +4776,17 @@
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>Fitz roy 267</t>
+          <t>RIVAS, GRAL. 2345</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>808918720</t>
+          <t>808918698</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
@@ -4801,7 +4801,7 @@
       </c>
       <c r="H58" t="inlineStr">
         <is>
-          <t>Aplomar columna</t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I58" t="n">
@@ -4823,10 +4823,10 @@
         </is>
       </c>
       <c r="M58" t="n">
-        <v>-58.451378</v>
+        <v>-58.482497</v>
       </c>
       <c r="N58" t="n">
-        <v>-34.596195</v>
+        <v>-34.598714</v>
       </c>
       <c r="O58" t="inlineStr">
         <is>
@@ -4842,27 +4842,27 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>6943</t>
+          <t>6928</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>8/14/2025</t>
+          <t>8/12/2025</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>SUPERI 1459</t>
+          <t>ALBARELLOS AV. 3101</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>808972965</t>
+          <t>808918710</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
@@ -4877,7 +4877,7 @@
       </c>
       <c r="H59" t="inlineStr">
         <is>
-          <t>Poste con base quebrada ver si es posible desmonte</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I59" t="n">
@@ -4885,7 +4885,7 @@
       </c>
       <c r="J59" t="inlineStr">
         <is>
-          <t>Desmonte</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K59" t="inlineStr">
@@ -4895,18 +4895,18 @@
       </c>
       <c r="L59" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M59" t="n">
-        <v>-58.460834</v>
+        <v>-58.512623</v>
       </c>
       <c r="N59" t="n">
-        <v>-34.573753</v>
+        <v>-34.579137</v>
       </c>
       <c r="O59" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P59" t="inlineStr">
@@ -4918,27 +4918,27 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>6969</t>
+          <t>-550</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>8/14/2025</t>
+          <t>8/12/2025</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>CIUDAD DE LA PAZ 295</t>
+          <t>Fitz roy 267</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>808972995</t>
+          <t>808918720</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
@@ -4953,7 +4953,7 @@
       </c>
       <c r="H60" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>Aplomar columna</t>
         </is>
       </c>
       <c r="I60" t="n">
@@ -4975,26 +4975,26 @@
         </is>
       </c>
       <c r="M60" t="n">
-        <v>-58.441171</v>
+        <v>-58.451378</v>
       </c>
       <c r="N60" t="n">
-        <v>-34.574547</v>
+        <v>-34.596195</v>
       </c>
       <c r="O60" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P60" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>6971</t>
+          <t>6943</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
@@ -5004,17 +5004,17 @@
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>MAURE 1594</t>
+          <t>SUPERI 1459</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>808973001</t>
+          <t>808972965</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
@@ -5029,7 +5029,7 @@
       </c>
       <c r="H61" t="inlineStr">
         <is>
-          <t>Ver de traspasar a telecentro y  desmontar ver con inspector</t>
+          <t>Poste con base quebrada ver si es posible desmonte</t>
         </is>
       </c>
       <c r="I61" t="n">
@@ -5037,7 +5037,7 @@
       </c>
       <c r="J61" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Desmonte</t>
         </is>
       </c>
       <c r="K61" t="inlineStr">
@@ -5047,40 +5047,40 @@
       </c>
       <c r="L61" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M61" t="n">
-        <v>-58.435072</v>
+        <v>-58.460834</v>
       </c>
       <c r="N61" t="n">
-        <v>-34.565732</v>
+        <v>-34.573753</v>
       </c>
       <c r="O61" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P61" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>7000</t>
+          <t>6969</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>8/20/2025</t>
+          <t>8/14/2025</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>SCALABRINI ORTIZ, RAUL AV. 2106</t>
+          <t>CIUDAD DE LA PAZ 295</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
@@ -5090,7 +5090,7 @@
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>809065867</t>
+          <t>808972995</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
@@ -5105,7 +5105,7 @@
       </c>
       <c r="H62" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I62" t="n">
@@ -5127,10 +5127,10 @@
         </is>
       </c>
       <c r="M62" t="n">
-        <v>-58.420109</v>
+        <v>-58.441171</v>
       </c>
       <c r="N62" t="n">
-        <v>-34.58764</v>
+        <v>-34.574547</v>
       </c>
       <c r="O62" t="inlineStr">
         <is>
@@ -5146,27 +5146,27 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>7003</t>
+          <t>6971</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>8/20/2025</t>
+          <t>8/14/2025</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>MELIAN AV. 2576</t>
+          <t>MAURE 1594</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>809065874</t>
+          <t>808973001</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
@@ -5181,7 +5181,7 @@
       </c>
       <c r="H63" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Ver de traspasar a telecentro y  desmontar ver con inspector</t>
         </is>
       </c>
       <c r="I63" t="n">
@@ -5203,46 +5203,46 @@
         </is>
       </c>
       <c r="M63" t="n">
-        <v>-58.471943</v>
+        <v>-58.435072</v>
       </c>
       <c r="N63" t="n">
-        <v>-34.564948</v>
+        <v>-34.565732</v>
       </c>
       <c r="O63" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P63" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>-559</t>
+          <t>7000</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>8/21/2025</t>
+          <t>8/20/2025</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>Av. Del Libertador 6736</t>
+          <t>SCALABRINI ORTIZ, RAUL AV. 2106</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>809098713</t>
+          <t>809065867</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
@@ -5279,46 +5279,46 @@
         </is>
       </c>
       <c r="M64" t="n">
-        <v>-58.453398</v>
+        <v>-58.420109</v>
       </c>
       <c r="N64" t="n">
-        <v>-34.550238</v>
+        <v>-34.58764</v>
       </c>
       <c r="O64" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P64" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>5503</t>
+          <t>7003</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>8/22/2025</t>
+          <t>8/20/2025</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>CRAMER AV. 1771</t>
+          <t>MELIAN AV. 2576</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>809102564</t>
+          <t>809065874</t>
         </is>
       </c>
       <c r="F65" t="inlineStr">
@@ -5333,7 +5333,7 @@
       </c>
       <c r="H65" t="inlineStr">
         <is>
-          <t>PIcada</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I65" t="n">
@@ -5355,10 +5355,10 @@
         </is>
       </c>
       <c r="M65" t="n">
-        <v>-58.458506</v>
+        <v>-58.471943</v>
       </c>
       <c r="N65" t="n">
-        <v>-34.56783</v>
+        <v>-34.564948</v>
       </c>
       <c r="O65" t="inlineStr">
         <is>
@@ -5374,27 +5374,27 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>7098</t>
+          <t>-559</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>8/25/2025</t>
+          <t>8/21/2025</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>UGARTE, MANUEL 3484</t>
+          <t>Av. Del Libertador 6736</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>809126236</t>
+          <t>809098713</t>
         </is>
       </c>
       <c r="F66" t="inlineStr">
@@ -5431,14 +5431,14 @@
         </is>
       </c>
       <c r="M66" t="n">
-        <v>-58.472869</v>
+        <v>-58.453398</v>
       </c>
       <c r="N66" t="n">
-        <v>-34.562</v>
+        <v>-34.550238</v>
       </c>
       <c r="O66" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P66" t="inlineStr">
@@ -5450,17 +5450,17 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>7080</t>
+          <t>5503</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>8/25/2025</t>
+          <t>8/22/2025</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>UGARTE, MANUEL 2196</t>
+          <t>CRAMER AV. 1771</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
@@ -5470,7 +5470,7 @@
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>809125906</t>
+          <t>809102564</t>
         </is>
       </c>
       <c r="F67" t="inlineStr">
@@ -5485,7 +5485,7 @@
       </c>
       <c r="H67" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>PIcada</t>
         </is>
       </c>
       <c r="I67" t="n">
@@ -5507,14 +5507,14 @@
         </is>
       </c>
       <c r="M67" t="n">
-        <v>-58.459402</v>
+        <v>-58.458506</v>
       </c>
       <c r="N67" t="n">
-        <v>-34.555262</v>
+        <v>-34.56783</v>
       </c>
       <c r="O67" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P67" t="inlineStr">
@@ -5526,7 +5526,7 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>7021</t>
+          <t>7098</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
@@ -5536,17 +5536,17 @@
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>VERA 445</t>
+          <t>UGARTE, MANUEL 3484</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>809155622</t>
+          <t>809126236</t>
         </is>
       </c>
       <c r="F68" t="inlineStr">
@@ -5561,7 +5561,7 @@
       </c>
       <c r="H68" t="inlineStr">
         <is>
-          <t>Correrla para sacarla del cantero</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I68" t="n">
@@ -5583,46 +5583,46 @@
         </is>
       </c>
       <c r="M68" t="n">
-        <v>-58.437181</v>
+        <v>-58.472869</v>
       </c>
       <c r="N68" t="n">
-        <v>-34.5995</v>
+        <v>-34.562</v>
       </c>
       <c r="O68" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P68" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>6465</t>
+          <t>7080</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>8/28/2025</t>
+          <t>8/25/2025</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>AGUIRRE 368</t>
+          <t>UGARTE, MANUEL 2196</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>809268249</t>
+          <t>809125906</t>
         </is>
       </c>
       <c r="F69" t="inlineStr">
@@ -5659,36 +5659,36 @@
         </is>
       </c>
       <c r="M69" t="n">
-        <v>-58.434651</v>
+        <v>-58.459402</v>
       </c>
       <c r="N69" t="n">
-        <v>-34.598814</v>
+        <v>-34.555262</v>
       </c>
       <c r="O69" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P69" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>7095</t>
+          <t>7021</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>8/28/2025</t>
+          <t>8/25/2025</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>SAN MARTIN AV. 4515</t>
+          <t>VERA 445</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
@@ -5698,7 +5698,7 @@
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>809268240</t>
+          <t>809155622</t>
         </is>
       </c>
       <c r="F70" t="inlineStr">
@@ -5713,7 +5713,7 @@
       </c>
       <c r="H70" t="inlineStr">
         <is>
-          <t>Columna chocada</t>
+          <t>Correrla para sacarla del cantero</t>
         </is>
       </c>
       <c r="I70" t="n">
@@ -5731,30 +5731,30 @@
       </c>
       <c r="L70" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M70" t="n">
-        <v>-58.483415</v>
+        <v>-58.437181</v>
       </c>
       <c r="N70" t="n">
-        <v>-34.597663</v>
+        <v>-34.5995</v>
       </c>
       <c r="O70" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P70" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>-575</t>
+          <t>6465</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
@@ -5764,17 +5764,17 @@
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>Amenabar 3064</t>
+          <t>AGUIRRE 368</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>809281299</t>
+          <t>809268249</t>
         </is>
       </c>
       <c r="F71" t="inlineStr">
@@ -5811,46 +5811,46 @@
         </is>
       </c>
       <c r="M71" t="n">
-        <v>-58.465984</v>
+        <v>-58.434651</v>
       </c>
       <c r="N71" t="n">
-        <v>-34.554869</v>
+        <v>-34.598814</v>
       </c>
       <c r="O71" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P71" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>-576</t>
+          <t>7095</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>8/29/2025</t>
+          <t>8/28/2025</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>Av. Boyacá 2030</t>
+          <t>SAN MARTIN AV. 4515</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>809309606</t>
+          <t>809268240</t>
         </is>
       </c>
       <c r="F72" t="inlineStr">
@@ -5865,7 +5865,7 @@
       </c>
       <c r="H72" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Columna chocada</t>
         </is>
       </c>
       <c r="I72" t="n">
@@ -5883,14 +5883,14 @@
       </c>
       <c r="L72" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M72" t="n">
-        <v>-58.471173</v>
+        <v>-58.483415</v>
       </c>
       <c r="N72" t="n">
-        <v>-34.60704</v>
+        <v>-34.597663</v>
       </c>
       <c r="O72" t="inlineStr">
         <is>
@@ -5906,27 +5906,27 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>7111</t>
+          <t>-575</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>9/1/2025</t>
+          <t>8/28/2025</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>VILELA 3699</t>
+          <t>Amenabar 3064</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>809371823</t>
+          <t>809281299</t>
         </is>
       </c>
       <c r="F73" t="inlineStr">
@@ -5941,7 +5941,7 @@
       </c>
       <c r="H73" t="inlineStr">
         <is>
-          <t xml:space="preserve">Cambiar </t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I73" t="n">
@@ -5959,14 +5959,14 @@
       </c>
       <c r="L73" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M73" t="n">
-        <v>-58.482817</v>
+        <v>-58.465984</v>
       </c>
       <c r="N73" t="n">
-        <v>-34.550845</v>
+        <v>-34.554869</v>
       </c>
       <c r="O73" t="inlineStr">
         <is>
@@ -5982,27 +5982,27 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>7118</t>
+          <t>-576</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>9/2/2025</t>
+          <t>8/29/2025</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>CUBAS, JOSE 2211</t>
+          <t>Av. Boyacá 2030</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>809406168</t>
+          <t>809309606</t>
         </is>
       </c>
       <c r="F74" t="inlineStr">
@@ -6039,10 +6039,10 @@
         </is>
       </c>
       <c r="M74" t="n">
-        <v>-58.492448</v>
+        <v>-58.471173</v>
       </c>
       <c r="N74" t="n">
-        <v>-34.58372</v>
+        <v>-34.60704</v>
       </c>
       <c r="O74" t="inlineStr">
         <is>
@@ -6058,27 +6058,27 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>-577</t>
+          <t>7111</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>9/2/2025</t>
+          <t>9/1/2025</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>Manuel Ugarte 2318</t>
+          <t>VILELA 3699</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>809406177</t>
+          <t>809371823</t>
         </is>
       </c>
       <c r="F75" t="inlineStr">
@@ -6093,7 +6093,7 @@
       </c>
       <c r="H75" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t xml:space="preserve">Cambiar </t>
         </is>
       </c>
       <c r="I75" t="n">
@@ -6111,14 +6111,14 @@
       </c>
       <c r="L75" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M75" t="n">
-        <v>-58.460635</v>
+        <v>-58.482817</v>
       </c>
       <c r="N75" t="n">
-        <v>-34.555932</v>
+        <v>-34.550845</v>
       </c>
       <c r="O75" t="inlineStr">
         <is>
@@ -6134,7 +6134,7 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>-578</t>
+          <t>7118</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
@@ -6144,17 +6144,17 @@
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>Pedro I Rivera 2536</t>
+          <t>CUBAS, JOSE 2211</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>809406189</t>
+          <t>809406168</t>
         </is>
       </c>
       <c r="F76" t="inlineStr">
@@ -6191,14 +6191,14 @@
         </is>
       </c>
       <c r="M76" t="n">
-        <v>-58.462327</v>
+        <v>-58.492448</v>
       </c>
       <c r="N76" t="n">
-        <v>-34.557565</v>
+        <v>-34.58372</v>
       </c>
       <c r="O76" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P76" t="inlineStr">
@@ -6210,74 +6210,226 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
+          <t>-577</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>9/2/2025</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>Manuel Ugarte 2318</t>
+        </is>
+      </c>
+      <c r="D77" t="inlineStr">
+        <is>
+          <t>13</t>
+        </is>
+      </c>
+      <c r="E77" t="inlineStr">
+        <is>
+          <t>809406177</t>
+        </is>
+      </c>
+      <c r="F77" t="inlineStr">
+        <is>
+          <t>NEW</t>
+        </is>
+      </c>
+      <c r="G77" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H77" t="inlineStr">
+        <is>
+          <t>Picada</t>
+        </is>
+      </c>
+      <c r="I77" t="n">
+        <v>1</v>
+      </c>
+      <c r="J77" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K77" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L77" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M77" t="n">
+        <v>-58.460635</v>
+      </c>
+      <c r="N77" t="n">
+        <v>-34.555932</v>
+      </c>
+      <c r="O77" t="inlineStr">
+        <is>
+          <t>Saavedra</t>
+        </is>
+      </c>
+      <c r="P77" t="inlineStr">
+        <is>
+          <t>Capital Norte</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>-578</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>9/2/2025</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>Pedro I Rivera 2536</t>
+        </is>
+      </c>
+      <c r="D78" t="inlineStr">
+        <is>
+          <t>13</t>
+        </is>
+      </c>
+      <c r="E78" t="inlineStr">
+        <is>
+          <t>809406189</t>
+        </is>
+      </c>
+      <c r="F78" t="inlineStr">
+        <is>
+          <t>NEW</t>
+        </is>
+      </c>
+      <c r="G78" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H78" t="inlineStr">
+        <is>
+          <t>Picada</t>
+        </is>
+      </c>
+      <c r="I78" t="n">
+        <v>1</v>
+      </c>
+      <c r="J78" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K78" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L78" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M78" t="n">
+        <v>-58.462327</v>
+      </c>
+      <c r="N78" t="n">
+        <v>-34.557565</v>
+      </c>
+      <c r="O78" t="inlineStr">
+        <is>
+          <t>Saavedra</t>
+        </is>
+      </c>
+      <c r="P78" t="inlineStr">
+        <is>
+          <t>Capital Norte</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
           <t>-579</t>
         </is>
       </c>
-      <c r="B77" t="inlineStr">
+      <c r="B79" t="inlineStr">
         <is>
           <t>9/2/2025</t>
         </is>
       </c>
-      <c r="C77" t="inlineStr">
+      <c r="C79" t="inlineStr">
         <is>
           <t>Pedro Rivera 2546</t>
         </is>
       </c>
-      <c r="D77" t="inlineStr">
+      <c r="D79" t="inlineStr">
         <is>
           <t>13</t>
         </is>
       </c>
-      <c r="E77" t="inlineStr">
+      <c r="E79" t="inlineStr">
         <is>
           <t>ICD30612785</t>
         </is>
       </c>
-      <c r="F77" t="inlineStr">
-        <is>
-          <t>NEW</t>
-        </is>
-      </c>
-      <c r="G77" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H77" t="inlineStr">
+      <c r="F79" t="inlineStr">
+        <is>
+          <t>NEW</t>
+        </is>
+      </c>
+      <c r="G79" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H79" t="inlineStr">
         <is>
           <t>Colocar R200 para pedir traspaso de equipos</t>
         </is>
       </c>
-      <c r="I77" t="n">
-        <v>1</v>
-      </c>
-      <c r="J77" t="inlineStr">
+      <c r="I79" t="n">
+        <v>1</v>
+      </c>
+      <c r="J79" t="inlineStr">
         <is>
           <t>Cambio</t>
         </is>
       </c>
-      <c r="K77" t="inlineStr">
+      <c r="K79" t="inlineStr">
         <is>
           <t>Nodo Teco</t>
         </is>
       </c>
-      <c r="L77" t="inlineStr">
+      <c r="L79" t="inlineStr">
         <is>
           <t>Pasante</t>
         </is>
       </c>
-      <c r="M77" t="n">
+      <c r="M79" t="n">
         <v>-58.462479</v>
       </c>
-      <c r="N77" t="n">
+      <c r="N79" t="n">
         <v>-34.55765</v>
       </c>
-      <c r="O77" t="inlineStr">
+      <c r="O79" t="inlineStr">
         <is>
           <t>Saavedra</t>
         </is>
       </c>
-      <c r="P77" t="inlineStr">
+      <c r="P79" t="inlineStr">
         <is>
           <t>Capital Norte</t>
         </is>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-09-05 06:59:25)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_NEW.xlsx
+++ b/mapa_interactivo_NEW.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P79"/>
+  <dimension ref="A1:P80"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6435,6 +6435,82 @@
         </is>
       </c>
     </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>-582</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>9/4/2025</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>Vilela 4019</t>
+        </is>
+      </c>
+      <c r="D80" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="E80" t="inlineStr">
+        <is>
+          <t>809454353</t>
+        </is>
+      </c>
+      <c r="F80" t="inlineStr">
+        <is>
+          <t>NEW</t>
+        </is>
+      </c>
+      <c r="G80" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H80" t="inlineStr">
+        <is>
+          <t>Poste telefonico propio quebrado en base</t>
+        </is>
+      </c>
+      <c r="I80" t="n">
+        <v>1</v>
+      </c>
+      <c r="J80" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K80" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L80" t="inlineStr">
+        <is>
+          <t>Poste</t>
+        </is>
+      </c>
+      <c r="M80" t="n">
+        <v>-58.485872</v>
+      </c>
+      <c r="N80" t="n">
+        <v>-34.552645</v>
+      </c>
+      <c r="O80" t="inlineStr">
+        <is>
+          <t>Saavedra</t>
+        </is>
+      </c>
+      <c r="P80" t="inlineStr">
+        <is>
+          <t>Capital Norte</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-09-08 07:30:22)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_NEW.xlsx
+++ b/mapa_interactivo_NEW.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P80"/>
+  <dimension ref="A1:P78"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4690,7 +4690,7 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>6002</t>
+          <t>6910</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
@@ -4700,17 +4700,17 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>LA PLATA AV. 832</t>
+          <t>RIVAS, GRAL. 2345</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>808918694</t>
+          <t>808918698</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
@@ -4725,7 +4725,7 @@
       </c>
       <c r="H57" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I57" t="n">
@@ -4747,26 +4747,26 @@
         </is>
       </c>
       <c r="M57" t="n">
-        <v>-58.426947</v>
+        <v>-58.482497</v>
       </c>
       <c r="N57" t="n">
-        <v>-34.625698</v>
+        <v>-34.598714</v>
       </c>
       <c r="O57" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P57" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>6910</t>
+          <t>6928</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
@@ -4776,17 +4776,17 @@
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>RIVAS, GRAL. 2345</t>
+          <t>ALBARELLOS AV. 3101</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>808918698</t>
+          <t>808918710</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
@@ -4801,7 +4801,7 @@
       </c>
       <c r="H58" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I58" t="n">
@@ -4823,10 +4823,10 @@
         </is>
       </c>
       <c r="M58" t="n">
-        <v>-58.482497</v>
+        <v>-58.512623</v>
       </c>
       <c r="N58" t="n">
-        <v>-34.598714</v>
+        <v>-34.579137</v>
       </c>
       <c r="O58" t="inlineStr">
         <is>
@@ -4842,7 +4842,7 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>6928</t>
+          <t>-550</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
@@ -4852,17 +4852,17 @@
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>ALBARELLOS AV. 3101</t>
+          <t>Fitz roy 267</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>808918710</t>
+          <t>808918720</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
@@ -4877,7 +4877,7 @@
       </c>
       <c r="H59" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Aplomar columna</t>
         </is>
       </c>
       <c r="I59" t="n">
@@ -4899,10 +4899,10 @@
         </is>
       </c>
       <c r="M59" t="n">
-        <v>-58.512623</v>
+        <v>-58.451378</v>
       </c>
       <c r="N59" t="n">
-        <v>-34.579137</v>
+        <v>-34.596195</v>
       </c>
       <c r="O59" t="inlineStr">
         <is>
@@ -4918,27 +4918,27 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>-550</t>
+          <t>6943</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>8/12/2025</t>
+          <t>8/14/2025</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>Fitz roy 267</t>
+          <t>SUPERI 1459</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>808918720</t>
+          <t>808972965</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
@@ -4953,7 +4953,7 @@
       </c>
       <c r="H60" t="inlineStr">
         <is>
-          <t>Aplomar columna</t>
+          <t>Poste con base quebrada ver si es posible desmonte</t>
         </is>
       </c>
       <c r="I60" t="n">
@@ -4961,7 +4961,7 @@
       </c>
       <c r="J60" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Desmonte</t>
         </is>
       </c>
       <c r="K60" t="inlineStr">
@@ -4971,18 +4971,18 @@
       </c>
       <c r="L60" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M60" t="n">
-        <v>-58.451378</v>
+        <v>-58.460834</v>
       </c>
       <c r="N60" t="n">
-        <v>-34.596195</v>
+        <v>-34.573753</v>
       </c>
       <c r="O60" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P60" t="inlineStr">
@@ -4994,7 +4994,7 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>6943</t>
+          <t>6969</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
@@ -5004,17 +5004,17 @@
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>SUPERI 1459</t>
+          <t>CIUDAD DE LA PAZ 295</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>808972965</t>
+          <t>808972995</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
@@ -5029,7 +5029,7 @@
       </c>
       <c r="H61" t="inlineStr">
         <is>
-          <t>Poste con base quebrada ver si es posible desmonte</t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I61" t="n">
@@ -5037,7 +5037,7 @@
       </c>
       <c r="J61" t="inlineStr">
         <is>
-          <t>Desmonte</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K61" t="inlineStr">
@@ -5047,30 +5047,30 @@
       </c>
       <c r="L61" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M61" t="n">
-        <v>-58.460834</v>
+        <v>-58.441171</v>
       </c>
       <c r="N61" t="n">
-        <v>-34.573753</v>
+        <v>-34.574547</v>
       </c>
       <c r="O61" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P61" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>6969</t>
+          <t>6971</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
@@ -5080,7 +5080,7 @@
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>CIUDAD DE LA PAZ 295</t>
+          <t>MAURE 1594</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
@@ -5090,7 +5090,7 @@
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>808972995</t>
+          <t>808973001</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
@@ -5105,7 +5105,7 @@
       </c>
       <c r="H62" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>Ver de traspasar a telecentro y  desmontar ver con inspector</t>
         </is>
       </c>
       <c r="I62" t="n">
@@ -5127,10 +5127,10 @@
         </is>
       </c>
       <c r="M62" t="n">
-        <v>-58.441171</v>
+        <v>-58.435072</v>
       </c>
       <c r="N62" t="n">
-        <v>-34.574547</v>
+        <v>-34.565732</v>
       </c>
       <c r="O62" t="inlineStr">
         <is>
@@ -5146,17 +5146,17 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>6971</t>
+          <t>7000</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>8/14/2025</t>
+          <t>8/20/2025</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>MAURE 1594</t>
+          <t>SCALABRINI ORTIZ, RAUL AV. 2106</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
@@ -5166,7 +5166,7 @@
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>808973001</t>
+          <t>809065867</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
@@ -5181,7 +5181,7 @@
       </c>
       <c r="H63" t="inlineStr">
         <is>
-          <t>Ver de traspasar a telecentro y  desmontar ver con inspector</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I63" t="n">
@@ -5203,10 +5203,10 @@
         </is>
       </c>
       <c r="M63" t="n">
-        <v>-58.435072</v>
+        <v>-58.420109</v>
       </c>
       <c r="N63" t="n">
-        <v>-34.565732</v>
+        <v>-34.58764</v>
       </c>
       <c r="O63" t="inlineStr">
         <is>
@@ -5222,7 +5222,7 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>7000</t>
+          <t>7003</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
@@ -5232,17 +5232,17 @@
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>SCALABRINI ORTIZ, RAUL AV. 2106</t>
+          <t>MELIAN AV. 2576</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>809065867</t>
+          <t>809065874</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
@@ -5279,46 +5279,46 @@
         </is>
       </c>
       <c r="M64" t="n">
-        <v>-58.420109</v>
+        <v>-58.471943</v>
       </c>
       <c r="N64" t="n">
-        <v>-34.58764</v>
+        <v>-34.564948</v>
       </c>
       <c r="O64" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P64" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>7003</t>
+          <t>-559</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>8/20/2025</t>
+          <t>8/21/2025</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>MELIAN AV. 2576</t>
+          <t>Av. Del Libertador 6736</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>809065874</t>
+          <t>809098713</t>
         </is>
       </c>
       <c r="F65" t="inlineStr">
@@ -5355,14 +5355,14 @@
         </is>
       </c>
       <c r="M65" t="n">
-        <v>-58.471943</v>
+        <v>-58.453398</v>
       </c>
       <c r="N65" t="n">
-        <v>-34.564948</v>
+        <v>-34.550238</v>
       </c>
       <c r="O65" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P65" t="inlineStr">
@@ -5374,17 +5374,17 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>-559</t>
+          <t>5503</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>8/21/2025</t>
+          <t>8/22/2025</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>Av. Del Libertador 6736</t>
+          <t>CRAMER AV. 1771</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
@@ -5394,7 +5394,7 @@
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>809098713</t>
+          <t>809102564</t>
         </is>
       </c>
       <c r="F66" t="inlineStr">
@@ -5409,7 +5409,7 @@
       </c>
       <c r="H66" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>PIcada</t>
         </is>
       </c>
       <c r="I66" t="n">
@@ -5431,14 +5431,14 @@
         </is>
       </c>
       <c r="M66" t="n">
-        <v>-58.453398</v>
+        <v>-58.458506</v>
       </c>
       <c r="N66" t="n">
-        <v>-34.550238</v>
+        <v>-34.56783</v>
       </c>
       <c r="O66" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P66" t="inlineStr">
@@ -5450,27 +5450,27 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>5503</t>
+          <t>7098</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>8/22/2025</t>
+          <t>8/25/2025</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>CRAMER AV. 1771</t>
+          <t>UGARTE, MANUEL 3484</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>809102564</t>
+          <t>809126236</t>
         </is>
       </c>
       <c r="F67" t="inlineStr">
@@ -5485,7 +5485,7 @@
       </c>
       <c r="H67" t="inlineStr">
         <is>
-          <t>PIcada</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I67" t="n">
@@ -5507,10 +5507,10 @@
         </is>
       </c>
       <c r="M67" t="n">
-        <v>-58.458506</v>
+        <v>-58.472869</v>
       </c>
       <c r="N67" t="n">
-        <v>-34.56783</v>
+        <v>-34.562</v>
       </c>
       <c r="O67" t="inlineStr">
         <is>
@@ -5526,7 +5526,7 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>7098</t>
+          <t>7080</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
@@ -5536,17 +5536,17 @@
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>UGARTE, MANUEL 3484</t>
+          <t>UGARTE, MANUEL 2196</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>809126236</t>
+          <t>809125906</t>
         </is>
       </c>
       <c r="F68" t="inlineStr">
@@ -5583,14 +5583,14 @@
         </is>
       </c>
       <c r="M68" t="n">
-        <v>-58.472869</v>
+        <v>-58.459402</v>
       </c>
       <c r="N68" t="n">
-        <v>-34.562</v>
+        <v>-34.555262</v>
       </c>
       <c r="O68" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P68" t="inlineStr">
@@ -5602,7 +5602,7 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>7080</t>
+          <t>7021</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
@@ -5612,17 +5612,17 @@
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>UGARTE, MANUEL 2196</t>
+          <t>VERA 445</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>809125906</t>
+          <t>809155622</t>
         </is>
       </c>
       <c r="F69" t="inlineStr">
@@ -5637,7 +5637,7 @@
       </c>
       <c r="H69" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Correrla para sacarla del cantero</t>
         </is>
       </c>
       <c r="I69" t="n">
@@ -5659,36 +5659,36 @@
         </is>
       </c>
       <c r="M69" t="n">
-        <v>-58.459402</v>
+        <v>-58.437181</v>
       </c>
       <c r="N69" t="n">
-        <v>-34.555262</v>
+        <v>-34.5995</v>
       </c>
       <c r="O69" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P69" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>7021</t>
+          <t>6465</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>8/25/2025</t>
+          <t>8/28/2025</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>VERA 445</t>
+          <t>AGUIRRE 368</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
@@ -5698,7 +5698,7 @@
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>809155622</t>
+          <t>809268249</t>
         </is>
       </c>
       <c r="F70" t="inlineStr">
@@ -5713,7 +5713,7 @@
       </c>
       <c r="H70" t="inlineStr">
         <is>
-          <t>Correrla para sacarla del cantero</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I70" t="n">
@@ -5735,10 +5735,10 @@
         </is>
       </c>
       <c r="M70" t="n">
-        <v>-58.437181</v>
+        <v>-58.434651</v>
       </c>
       <c r="N70" t="n">
-        <v>-34.5995</v>
+        <v>-34.598814</v>
       </c>
       <c r="O70" t="inlineStr">
         <is>
@@ -5754,7 +5754,7 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>6465</t>
+          <t>7095</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
@@ -5764,7 +5764,7 @@
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>AGUIRRE 368</t>
+          <t>SAN MARTIN AV. 4515</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
@@ -5774,7 +5774,7 @@
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>809268249</t>
+          <t>809268240</t>
         </is>
       </c>
       <c r="F71" t="inlineStr">
@@ -5789,7 +5789,7 @@
       </c>
       <c r="H71" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Columna chocada</t>
         </is>
       </c>
       <c r="I71" t="n">
@@ -5807,30 +5807,30 @@
       </c>
       <c r="L71" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M71" t="n">
-        <v>-58.434651</v>
+        <v>-58.483415</v>
       </c>
       <c r="N71" t="n">
-        <v>-34.598814</v>
+        <v>-34.597663</v>
       </c>
       <c r="O71" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P71" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>7095</t>
+          <t>-575</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
@@ -5840,17 +5840,17 @@
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>SAN MARTIN AV. 4515</t>
+          <t>Amenabar 3064</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>809268240</t>
+          <t>809281299</t>
         </is>
       </c>
       <c r="F72" t="inlineStr">
@@ -5865,7 +5865,7 @@
       </c>
       <c r="H72" t="inlineStr">
         <is>
-          <t>Columna chocada</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I72" t="n">
@@ -5883,18 +5883,18 @@
       </c>
       <c r="L72" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M72" t="n">
-        <v>-58.483415</v>
+        <v>-58.465984</v>
       </c>
       <c r="N72" t="n">
-        <v>-34.597663</v>
+        <v>-34.554869</v>
       </c>
       <c r="O72" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P72" t="inlineStr">
@@ -5906,27 +5906,27 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>-575</t>
+          <t>-576</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>8/28/2025</t>
+          <t>8/29/2025</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>Amenabar 3064</t>
+          <t>Av. Boyacá 2030</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>809281299</t>
+          <t>809309606</t>
         </is>
       </c>
       <c r="F73" t="inlineStr">
@@ -5963,14 +5963,14 @@
         </is>
       </c>
       <c r="M73" t="n">
-        <v>-58.465984</v>
+        <v>-58.471173</v>
       </c>
       <c r="N73" t="n">
-        <v>-34.554869</v>
+        <v>-34.60704</v>
       </c>
       <c r="O73" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P73" t="inlineStr">
@@ -5982,27 +5982,27 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>-576</t>
+          <t>7111</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>8/29/2025</t>
+          <t>9/1/2025</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>Av. Boyacá 2030</t>
+          <t>VILELA 3699</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>809309606</t>
+          <t>809371823</t>
         </is>
       </c>
       <c r="F74" t="inlineStr">
@@ -6017,7 +6017,7 @@
       </c>
       <c r="H74" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t xml:space="preserve">Cambiar </t>
         </is>
       </c>
       <c r="I74" t="n">
@@ -6035,18 +6035,18 @@
       </c>
       <c r="L74" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M74" t="n">
-        <v>-58.471173</v>
+        <v>-58.482817</v>
       </c>
       <c r="N74" t="n">
-        <v>-34.60704</v>
+        <v>-34.550845</v>
       </c>
       <c r="O74" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P74" t="inlineStr">
@@ -6058,17 +6058,17 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>7111</t>
+          <t>7118</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>9/1/2025</t>
+          <t>9/2/2025</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>VILELA 3699</t>
+          <t>CUBAS, JOSE 2211</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
@@ -6078,7 +6078,7 @@
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>809371823</t>
+          <t>809406168</t>
         </is>
       </c>
       <c r="F75" t="inlineStr">
@@ -6093,7 +6093,7 @@
       </c>
       <c r="H75" t="inlineStr">
         <is>
-          <t xml:space="preserve">Cambiar </t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I75" t="n">
@@ -6111,18 +6111,18 @@
       </c>
       <c r="L75" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M75" t="n">
-        <v>-58.482817</v>
+        <v>-58.492448</v>
       </c>
       <c r="N75" t="n">
-        <v>-34.550845</v>
+        <v>-34.58372</v>
       </c>
       <c r="O75" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P75" t="inlineStr">
@@ -6134,7 +6134,7 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>7118</t>
+          <t>-577</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
@@ -6144,17 +6144,17 @@
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>CUBAS, JOSE 2211</t>
+          <t>Manuel Ugarte 2318</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>809406168</t>
+          <t>809406177</t>
         </is>
       </c>
       <c r="F76" t="inlineStr">
@@ -6191,14 +6191,14 @@
         </is>
       </c>
       <c r="M76" t="n">
-        <v>-58.492448</v>
+        <v>-58.460635</v>
       </c>
       <c r="N76" t="n">
-        <v>-34.58372</v>
+        <v>-34.555932</v>
       </c>
       <c r="O76" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P76" t="inlineStr">
@@ -6210,7 +6210,7 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>-577</t>
+          <t>-578</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
@@ -6220,7 +6220,7 @@
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>Manuel Ugarte 2318</t>
+          <t>Pedro I Rivera 2536</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
@@ -6230,7 +6230,7 @@
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>809406177</t>
+          <t>809406189</t>
         </is>
       </c>
       <c r="F77" t="inlineStr">
@@ -6267,10 +6267,10 @@
         </is>
       </c>
       <c r="M77" t="n">
-        <v>-58.460635</v>
+        <v>-58.462327</v>
       </c>
       <c r="N77" t="n">
-        <v>-34.555932</v>
+        <v>-34.557565</v>
       </c>
       <c r="O77" t="inlineStr">
         <is>
@@ -6286,7 +6286,7 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>-578</t>
+          <t>-579</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
@@ -6296,7 +6296,7 @@
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>Pedro I Rivera 2536</t>
+          <t>Pedro Rivera 2546</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
@@ -6306,7 +6306,7 @@
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>809406189</t>
+          <t>ICD30612785</t>
         </is>
       </c>
       <c r="F78" t="inlineStr">
@@ -6321,7 +6321,7 @@
       </c>
       <c r="H78" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Colocar R200 para pedir traspaso de equipos</t>
         </is>
       </c>
       <c r="I78" t="n">
@@ -6334,7 +6334,7 @@
       </c>
       <c r="K78" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L78" t="inlineStr">
@@ -6343,10 +6343,10 @@
         </is>
       </c>
       <c r="M78" t="n">
-        <v>-58.462327</v>
+        <v>-58.462479</v>
       </c>
       <c r="N78" t="n">
-        <v>-34.557565</v>
+        <v>-34.55765</v>
       </c>
       <c r="O78" t="inlineStr">
         <is>
@@ -6354,158 +6354,6 @@
         </is>
       </c>
       <c r="P78" t="inlineStr">
-        <is>
-          <t>Capital Norte</t>
-        </is>
-      </c>
-    </row>
-    <row r="79">
-      <c r="A79" t="inlineStr">
-        <is>
-          <t>-579</t>
-        </is>
-      </c>
-      <c r="B79" t="inlineStr">
-        <is>
-          <t>9/2/2025</t>
-        </is>
-      </c>
-      <c r="C79" t="inlineStr">
-        <is>
-          <t>Pedro Rivera 2546</t>
-        </is>
-      </c>
-      <c r="D79" t="inlineStr">
-        <is>
-          <t>13</t>
-        </is>
-      </c>
-      <c r="E79" t="inlineStr">
-        <is>
-          <t>ICD30612785</t>
-        </is>
-      </c>
-      <c r="F79" t="inlineStr">
-        <is>
-          <t>NEW</t>
-        </is>
-      </c>
-      <c r="G79" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H79" t="inlineStr">
-        <is>
-          <t>Colocar R200 para pedir traspaso de equipos</t>
-        </is>
-      </c>
-      <c r="I79" t="n">
-        <v>1</v>
-      </c>
-      <c r="J79" t="inlineStr">
-        <is>
-          <t>Cambio</t>
-        </is>
-      </c>
-      <c r="K79" t="inlineStr">
-        <is>
-          <t>Nodo Teco</t>
-        </is>
-      </c>
-      <c r="L79" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
-      <c r="M79" t="n">
-        <v>-58.462479</v>
-      </c>
-      <c r="N79" t="n">
-        <v>-34.55765</v>
-      </c>
-      <c r="O79" t="inlineStr">
-        <is>
-          <t>Saavedra</t>
-        </is>
-      </c>
-      <c r="P79" t="inlineStr">
-        <is>
-          <t>Capital Norte</t>
-        </is>
-      </c>
-    </row>
-    <row r="80">
-      <c r="A80" t="inlineStr">
-        <is>
-          <t>-582</t>
-        </is>
-      </c>
-      <c r="B80" t="inlineStr">
-        <is>
-          <t>9/4/2025</t>
-        </is>
-      </c>
-      <c r="C80" t="inlineStr">
-        <is>
-          <t>Vilela 4019</t>
-        </is>
-      </c>
-      <c r="D80" t="inlineStr">
-        <is>
-          <t>12</t>
-        </is>
-      </c>
-      <c r="E80" t="inlineStr">
-        <is>
-          <t>809454353</t>
-        </is>
-      </c>
-      <c r="F80" t="inlineStr">
-        <is>
-          <t>NEW</t>
-        </is>
-      </c>
-      <c r="G80" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H80" t="inlineStr">
-        <is>
-          <t>Poste telefonico propio quebrado en base</t>
-        </is>
-      </c>
-      <c r="I80" t="n">
-        <v>1</v>
-      </c>
-      <c r="J80" t="inlineStr">
-        <is>
-          <t>Cambio</t>
-        </is>
-      </c>
-      <c r="K80" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L80" t="inlineStr">
-        <is>
-          <t>Poste</t>
-        </is>
-      </c>
-      <c r="M80" t="n">
-        <v>-58.485872</v>
-      </c>
-      <c r="N80" t="n">
-        <v>-34.552645</v>
-      </c>
-      <c r="O80" t="inlineStr">
-        <is>
-          <t>Saavedra</t>
-        </is>
-      </c>
-      <c r="P80" t="inlineStr">
         <is>
           <t>Capital Norte</t>
         </is>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-09-09 09:00:22)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_NEW.xlsx
+++ b/mapa_interactivo_NEW.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P73"/>
+  <dimension ref="A1:P74"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -518,17 +518,17 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>7118</t>
+          <t>3299</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>9/2/2025</t>
+          <t>9/10/2024</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>CUBAS, JOSE 2211</t>
+          <t>DIAZ COLODRERO 3309</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -538,7 +538,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>809406168</t>
+          <t>796186684</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -548,12 +548,12 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>qap traspaso nodo TLC y Teco</t>
         </is>
       </c>
       <c r="I2" t="n">
@@ -566,7 +566,7 @@
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo TLC</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
@@ -575,10 +575,10 @@
         </is>
       </c>
       <c r="M2" t="n">
-        <v>-58.492448</v>
+        <v>-58.491722</v>
       </c>
       <c r="N2" t="n">
-        <v>-34.58372</v>
+        <v>-34.565845</v>
       </c>
       <c r="O2" t="inlineStr">
         <is>
@@ -594,27 +594,27 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>7111</t>
+          <t>3839</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>9/1/2025</t>
+          <t>10/23/2024</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>VILELA 3699</t>
+          <t>PICO 1511</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>809371823</t>
+          <t>798390296</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -629,7 +629,7 @@
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Cambiar </t>
+          <t>Poste inclinado</t>
         </is>
       </c>
       <c r="I3" t="n">
@@ -637,7 +637,7 @@
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
@@ -647,14 +647,14 @@
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M3" t="n">
-        <v>-58.482817</v>
+        <v>-58.465596</v>
       </c>
       <c r="N3" t="n">
-        <v>-34.550845</v>
+        <v>-34.53627</v>
       </c>
       <c r="O3" t="inlineStr">
         <is>
@@ -670,27 +670,27 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>7098</t>
+          <t>5589</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>8/25/2025</t>
+          <t>12/31/2023</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>UGARTE, MANUEL 3484</t>
+          <t>ARCOS 1520</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>809126236</t>
+          <t>799540526</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -700,7 +700,7 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
@@ -709,7 +709,7 @@
         </is>
       </c>
       <c r="I4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J4" t="inlineStr">
         <is>
@@ -718,7 +718,7 @@
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
@@ -727,10 +727,10 @@
         </is>
       </c>
       <c r="M4" t="n">
-        <v>-58.472869</v>
+        <v>-58.449125</v>
       </c>
       <c r="N4" t="n">
-        <v>-34.562</v>
+        <v>-34.565958</v>
       </c>
       <c r="O4" t="inlineStr">
         <is>
@@ -746,27 +746,27 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>7095</t>
+          <t>4595</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>8/28/2025</t>
+          <t>1/15/2025</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>SAN MARTIN AV. 4515</t>
+          <t>PAROISSIEN 1806</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>809268240</t>
+          <t>802747617</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -781,7 +781,7 @@
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>Columna chocada</t>
+          <t>Aplomar</t>
         </is>
       </c>
       <c r="I5" t="n">
@@ -789,7 +789,7 @@
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
@@ -803,14 +803,14 @@
         </is>
       </c>
       <c r="M5" t="n">
-        <v>-58.483415</v>
+        <v>-58.464172</v>
       </c>
       <c r="N5" t="n">
-        <v>-34.597663</v>
+        <v>-34.543845</v>
       </c>
       <c r="O5" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P5" t="inlineStr">
@@ -822,27 +822,27 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>7080</t>
+          <t>4528</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>8/25/2025</t>
+          <t>1/16/2025</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>UGARTE, MANUEL 2196</t>
+          <t>BARCO CENTENERA DEL 545</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>809125906</t>
+          <t>802774521</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -879,46 +879,46 @@
         </is>
       </c>
       <c r="M6" t="n">
-        <v>-58.459402</v>
+        <v>-58.440625</v>
       </c>
       <c r="N6" t="n">
-        <v>-34.555262</v>
+        <v>-34.625499</v>
       </c>
       <c r="O6" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P6" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>7023</t>
+          <t>4862</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>7/22/2025</t>
+          <t>1/23/2025</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>ZABALA 3573</t>
+          <t>ARCOS 2263</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>808480549</t>
+          <t>802857379</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -928,16 +928,16 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>Corroida en base para recambio entro tambien como caso 3575</t>
+          <t>picada</t>
         </is>
       </c>
       <c r="I7" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J7" t="inlineStr">
         <is>
@@ -946,7 +946,7 @@
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L7" t="inlineStr">
@@ -955,14 +955,14 @@
         </is>
       </c>
       <c r="M7" t="n">
-        <v>-58.457522</v>
+        <v>-58.455082</v>
       </c>
       <c r="N7" t="n">
-        <v>-34.579414</v>
+        <v>-34.558883</v>
       </c>
       <c r="O7" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P7" t="inlineStr">
@@ -974,27 +974,27 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>7021</t>
+          <t>6036</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>8/25/2025</t>
+          <t>2/24/2025</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>VERA 445</t>
+          <t>MEDRANO 1715</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>809155622</t>
+          <t>803608181</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -1007,13 +1007,9 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H8" t="inlineStr">
-        <is>
-          <t>Correrla para sacarla del cantero</t>
-        </is>
-      </c>
+      <c r="H8" t="inlineStr"/>
       <c r="I8" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J8" t="inlineStr">
         <is>
@@ -1022,7 +1018,7 @@
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L8" t="inlineStr">
@@ -1031,10 +1027,10 @@
         </is>
       </c>
       <c r="M8" t="n">
-        <v>-58.437181</v>
+        <v>-58.418236</v>
       </c>
       <c r="N8" t="n">
-        <v>-34.5995</v>
+        <v>-34.589859</v>
       </c>
       <c r="O8" t="inlineStr">
         <is>
@@ -1050,27 +1046,27 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>7003</t>
+          <t>5053</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>8/20/2025</t>
+          <t>3/11/2025</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>MELIAN AV. 2576</t>
+          <t>MENDOZA 1153</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>809065874</t>
+          <t>803969314</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -1085,11 +1081,11 @@
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="I9" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J9" t="inlineStr">
         <is>
@@ -1103,18 +1099,18 @@
       </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M9" t="n">
-        <v>-58.471943</v>
+        <v>-58.44463</v>
       </c>
       <c r="N9" t="n">
-        <v>-34.564948</v>
+        <v>-34.553354</v>
       </c>
       <c r="O9" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P9" t="inlineStr">
@@ -1126,27 +1122,27 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>7000</t>
+          <t>6071</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>8/20/2025</t>
+          <t>3/17/2025</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>SCALABRINI ORTIZ, RAUL AV. 2106</t>
+          <t>OSORIO 4994</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>809065867</t>
+          <t>804053324</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
@@ -1159,13 +1155,9 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H10" t="inlineStr">
-        <is>
-          <t>Picada</t>
-        </is>
-      </c>
+      <c r="H10" t="inlineStr"/>
       <c r="I10" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J10" t="inlineStr">
         <is>
@@ -1183,46 +1175,46 @@
         </is>
       </c>
       <c r="M10" t="n">
-        <v>-58.420109</v>
+        <v>-58.466241</v>
       </c>
       <c r="N10" t="n">
-        <v>-34.58764</v>
+        <v>-34.595741</v>
       </c>
       <c r="O10" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P10" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>6971</t>
+          <t>2485</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>8/14/2025</t>
+          <t>3/26/2025</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>MAURE 1594</t>
+          <t>LA PLATA AV. 1095</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>808973001</t>
+          <t>804302893</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
@@ -1237,7 +1229,7 @@
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>Ver de traspasar a telecentro y  desmontar ver con inspector</t>
+          <t>Sacar ancla de rienda vieja y cementar vereda</t>
         </is>
       </c>
       <c r="I11" t="n">
@@ -1245,7 +1237,7 @@
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Tensor</t>
         </is>
       </c>
       <c r="K11" t="inlineStr">
@@ -1255,18 +1247,18 @@
       </c>
       <c r="L11" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M11" t="n">
-        <v>-58.435072</v>
+        <v>-58.426593</v>
       </c>
       <c r="N11" t="n">
-        <v>-34.565732</v>
+        <v>-34.628211</v>
       </c>
       <c r="O11" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P11" t="inlineStr">
@@ -1278,27 +1270,27 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>6969</t>
+          <t>3348</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>8/14/2025</t>
+          <t>3/27/2025</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>CIUDAD DE LA PAZ 295</t>
+          <t>ESTOMBA 2626</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>808972995</t>
+          <t>804309704</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
@@ -1313,7 +1305,7 @@
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I12" t="n">
@@ -1321,7 +1313,7 @@
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Desmonte</t>
         </is>
       </c>
       <c r="K12" t="inlineStr">
@@ -1335,46 +1327,46 @@
         </is>
       </c>
       <c r="M12" t="n">
-        <v>-58.441171</v>
+        <v>-58.47538</v>
       </c>
       <c r="N12" t="n">
-        <v>-34.574547</v>
+        <v>-34.566015</v>
       </c>
       <c r="O12" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P12" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>6943</t>
+          <t>-312</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>8/14/2025</t>
+          <t>3/29/2025</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>SUPERI 1459</t>
+          <t>MATIENZO BENJAMIN /ALT/ 1831</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>808972965</t>
+          <t>804333522</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
@@ -1389,58 +1381,58 @@
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>Poste con base quebrada ver si es posible desmonte</t>
+          <t>Retirar columna ya traspasaron el nodo</t>
         </is>
       </c>
       <c r="I13" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>Desmonte</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L13" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M13" t="n">
-        <v>-58.460834</v>
+        <v>-58.434835</v>
       </c>
       <c r="N13" t="n">
-        <v>-34.573753</v>
+        <v>-34.569129</v>
       </c>
       <c r="O13" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P13" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>6928</t>
+          <t>3430</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>8/12/2025</t>
+          <t>4/1/2025</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>ALBARELLOS AV. 3101</t>
+          <t>MONROE 3838</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
@@ -1450,7 +1442,7 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>808918710</t>
+          <t>804468442</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
@@ -1465,7 +1457,7 @@
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Reparar rienda</t>
         </is>
       </c>
       <c r="I14" t="n">
@@ -1473,7 +1465,7 @@
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Tensor</t>
         </is>
       </c>
       <c r="K14" t="inlineStr">
@@ -1483,18 +1475,18 @@
       </c>
       <c r="L14" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M14" t="n">
-        <v>-58.512623</v>
+        <v>-58.473659</v>
       </c>
       <c r="N14" t="n">
-        <v>-34.579137</v>
+        <v>-34.566979</v>
       </c>
       <c r="O14" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P14" t="inlineStr">
@@ -1506,27 +1498,27 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>6910</t>
+          <t>5464</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>8/12/2025</t>
+          <t>4/4/2025</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>RIVAS, GRAL. 2345</t>
+          <t>SUCRE, ANTONIO JOSE DE, MCAL. 3100</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>808918698</t>
+          <t>804497880</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
@@ -1541,7 +1533,7 @@
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I15" t="n">
@@ -1559,18 +1551,18 @@
       </c>
       <c r="L15" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M15" t="n">
-        <v>-58.482497</v>
+        <v>-58.46161</v>
       </c>
       <c r="N15" t="n">
-        <v>-34.598714</v>
+        <v>-34.567849</v>
       </c>
       <c r="O15" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P15" t="inlineStr">
@@ -1582,17 +1574,17 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>6906</t>
+          <t>5469</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>8/12/2025</t>
+          <t>4/4/2025</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>MOSCONI GENERAL AV. 3163</t>
+          <t>ESTADO PLURINACIONAL DE BOLIVIA 5899</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
@@ -1602,7 +1594,7 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>808918685</t>
+          <t>804497887</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
@@ -1617,7 +1609,7 @@
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Aplomar</t>
         </is>
       </c>
       <c r="I16" t="n">
@@ -1625,7 +1617,7 @@
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K16" t="inlineStr">
@@ -1635,14 +1627,14 @@
       </c>
       <c r="L16" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M16" t="n">
-        <v>-58.505731</v>
+        <v>-58.507746</v>
       </c>
       <c r="N16" t="n">
-        <v>-34.588316</v>
+        <v>-34.574217</v>
       </c>
       <c r="O16" t="inlineStr">
         <is>
@@ -1658,27 +1650,27 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>6579</t>
+          <t>5492</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>8/7/2025</t>
+          <t>4/4/2025</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>RIVADAVIA MARTIN, COMODORO 1350</t>
+          <t>ESTADO PLURINACIONAL DE BOLIVIA 5920</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>808749184</t>
+          <t>804498035</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
@@ -1693,7 +1685,7 @@
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>Poste inclinado</t>
+          <t>aplomar</t>
         </is>
       </c>
       <c r="I17" t="n">
@@ -1711,18 +1703,18 @@
       </c>
       <c r="L17" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M17" t="n">
-        <v>-58.461024</v>
+        <v>-58.50751</v>
       </c>
       <c r="N17" t="n">
-        <v>-34.539409</v>
+        <v>-34.574543</v>
       </c>
       <c r="O17" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P17" t="inlineStr">
@@ -1734,17 +1726,17 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>6538</t>
+          <t>5599</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>7/17/2025</t>
+          <t>4/15/2025</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Pedraza Manuela 4101</t>
+          <t>ESTOMBA 4052</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
@@ -1754,7 +1746,7 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>808400353</t>
+          <t>804732246</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
@@ -1769,7 +1761,7 @@
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t xml:space="preserve">Podrida en la base </t>
+          <t>Columna PRFV quedo inclinada (la hicieron como estomba 4056)</t>
         </is>
       </c>
       <c r="I18" t="n">
@@ -1777,12 +1769,12 @@
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo TLC</t>
         </is>
       </c>
       <c r="L18" t="inlineStr">
@@ -1791,10 +1783,10 @@
         </is>
       </c>
       <c r="M18" t="n">
-        <v>-58.481569</v>
+        <v>-58.485407</v>
       </c>
       <c r="N18" t="n">
-        <v>-34.559853</v>
+        <v>-34.552985</v>
       </c>
       <c r="O18" t="inlineStr">
         <is>
@@ -1810,27 +1802,27 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>6519</t>
+          <t>5590</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>7/28/2025</t>
+          <t>4/15/2025</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>SALGUERO, JERONIMO 2874</t>
+          <t>O'HIGGINS 2441</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>808571977</t>
+          <t>804732275</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
@@ -1845,7 +1837,7 @@
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>Reparar rienda</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I19" t="n">
@@ -1853,7 +1845,7 @@
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>Tensor</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K19" t="inlineStr">
@@ -1863,50 +1855,50 @@
       </c>
       <c r="L19" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M19" t="n">
-        <v>-58.407256</v>
+        <v>-58.45573</v>
       </c>
       <c r="N19" t="n">
-        <v>-34.578976</v>
+        <v>-34.556576</v>
       </c>
       <c r="O19" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P19" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>6512</t>
+          <t>5624</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>7/28/2025</t>
+          <t>4/22/2025</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>GASCON 1195</t>
+          <t>PINO, VIRREY DEL 3456</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>808571975</t>
+          <t>804876043</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
@@ -1921,7 +1913,7 @@
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Desmonte de poste</t>
         </is>
       </c>
       <c r="I20" t="n">
@@ -1929,7 +1921,7 @@
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Desmonte</t>
         </is>
       </c>
       <c r="K20" t="inlineStr">
@@ -1939,50 +1931,50 @@
       </c>
       <c r="L20" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M20" t="n">
-        <v>-58.423127</v>
+        <v>-58.464354</v>
       </c>
       <c r="N20" t="n">
-        <v>-34.596476</v>
+        <v>-34.572486</v>
       </c>
       <c r="O20" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P20" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>6506</t>
+          <t>5656</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>7/10/2025</t>
+          <t>4/24/2025</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Ohiggins 1611</t>
+          <t>ECHEVERRIA 5893</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>808148679</t>
+          <t>804922184</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
@@ -1997,7 +1989,7 @@
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>Columna podrida en la base</t>
+          <t>Poste con base quebrada</t>
         </is>
       </c>
       <c r="I21" t="n">
@@ -2005,28 +1997,28 @@
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Desmonte</t>
         </is>
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L21" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M21" t="n">
-        <v>-58.448993</v>
+        <v>-58.489627</v>
       </c>
       <c r="N21" t="n">
-        <v>-34.564383</v>
+        <v>-34.583761</v>
       </c>
       <c r="O21" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P21" t="inlineStr">
@@ -2038,17 +2030,17 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>6484</t>
+          <t>6173</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>7/24/2025</t>
+          <t>4/29/2025</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>URIARTE 2396</t>
+          <t>ARMENIA 2321</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
@@ -2058,7 +2050,7 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>808509373</t>
+          <t>805507398</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
@@ -2073,7 +2065,7 @@
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Picada volvio a entrar como caso 6325</t>
         </is>
       </c>
       <c r="I22" t="n">
@@ -2095,10 +2087,10 @@
         </is>
       </c>
       <c r="M22" t="n">
-        <v>-58.423934</v>
+        <v>-58.420549</v>
       </c>
       <c r="N22" t="n">
-        <v>-34.581562</v>
+        <v>-34.585103</v>
       </c>
       <c r="O22" t="inlineStr">
         <is>
@@ -2114,27 +2106,27 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>6465</t>
+          <t>5715</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>8/28/2025</t>
+          <t>5/1/2025</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>AGUIRRE 368</t>
+          <t>CUENCA 4690</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>809268249</t>
+          <t>805579094</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
@@ -2149,7 +2141,7 @@
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Aplomar poste</t>
         </is>
       </c>
       <c r="I23" t="n">
@@ -2157,7 +2149,7 @@
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K23" t="inlineStr">
@@ -2167,50 +2159,50 @@
       </c>
       <c r="L23" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M23" t="n">
-        <v>-58.434651</v>
+        <v>-58.506061</v>
       </c>
       <c r="N23" t="n">
-        <v>-34.598814</v>
+        <v>-34.588887</v>
       </c>
       <c r="O23" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P23" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>6437</t>
+          <t>6333</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>7/17/2025</t>
+          <t>5/1/2025</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>MILLER 4590</t>
+          <t>ORTEGA Y GASSET 1816</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>808400306</t>
+          <t>805655342</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
@@ -2225,7 +2217,7 @@
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>Columna corroida</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I24" t="n">
@@ -2247,46 +2239,46 @@
         </is>
       </c>
       <c r="M24" t="n">
-        <v>-58.495482</v>
+        <v>-58.432556</v>
       </c>
       <c r="N24" t="n">
-        <v>-34.552614</v>
+        <v>-34.570279</v>
       </c>
       <c r="O24" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P24" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>6383</t>
+          <t>232</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>7/8/2025</t>
+          <t>5/9/2025</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>FALCON, RAMON L.,CNEL. 1411</t>
+          <t>Gorostiaga 2286</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>808099320</t>
+          <t>805791858</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
@@ -2323,14 +2315,14 @@
         </is>
       </c>
       <c r="M25" t="n">
-        <v>-58.448523</v>
+        <v>-58.441563</v>
       </c>
       <c r="N25" t="n">
-        <v>-34.62452</v>
+        <v>-34.569743</v>
       </c>
       <c r="O25" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P25" t="inlineStr">
@@ -2342,27 +2334,27 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>6333</t>
+          <t>-404</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>5/1/2025</t>
+          <t>5/8/2025</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>ORTEGA Y GASSET 1816</t>
+          <t>Amenabar 3048</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>805655342</t>
+          <t>805791896</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
@@ -2377,7 +2369,7 @@
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Aplomar columna 114</t>
         </is>
       </c>
       <c r="I26" t="n">
@@ -2385,7 +2377,7 @@
       </c>
       <c r="J26" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K26" t="inlineStr">
@@ -2399,46 +2391,46 @@
         </is>
       </c>
       <c r="M26" t="n">
-        <v>-58.432556</v>
+        <v>-58.46579</v>
       </c>
       <c r="N26" t="n">
-        <v>-34.570279</v>
+        <v>-34.555012</v>
       </c>
       <c r="O26" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P26" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>6332</t>
+          <t>-406</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>7/3/2025</t>
+          <t>5/8/2025</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>ARAOZ 2560</t>
+          <t>Olof palme 4144</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>807965818</t>
+          <t>805791925</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
@@ -2453,7 +2445,7 @@
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Tensar 2 riendas a pique columna 168</t>
         </is>
       </c>
       <c r="I27" t="n">
@@ -2461,7 +2453,7 @@
       </c>
       <c r="J27" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Tensor</t>
         </is>
       </c>
       <c r="K27" t="inlineStr">
@@ -2471,50 +2463,50 @@
       </c>
       <c r="L27" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M27" t="n">
-        <v>-58.414507</v>
+        <v>-58.488252</v>
       </c>
       <c r="N27" t="n">
-        <v>-34.585377</v>
+        <v>-34.553391</v>
       </c>
       <c r="O27" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P27" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>6308</t>
+          <t>5826</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>7/1/2025</t>
+          <t>5/19/2025</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Guayaquil 637</t>
+          <t>ALBARELLOS AV. 3180</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>807896343</t>
+          <t>806926466</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
@@ -2529,7 +2521,7 @@
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Columna (metal) inclinada</t>
         </is>
       </c>
       <c r="I28" t="n">
@@ -2537,7 +2529,7 @@
       </c>
       <c r="J28" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K28" t="inlineStr">
@@ -2547,50 +2539,50 @@
       </c>
       <c r="L28" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M28" t="n">
-        <v>-58.437378</v>
+        <v>-58.513552</v>
       </c>
       <c r="N28" t="n">
-        <v>-34.62116</v>
+        <v>-34.579829</v>
       </c>
       <c r="O28" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P28" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>6295</t>
+          <t>6144</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>6/30/2025</t>
+          <t>6/11/2025</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>SOLER 6017</t>
+          <t>TURIN 2990</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>807851636</t>
+          <t>807458282</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
@@ -2627,46 +2619,46 @@
         </is>
       </c>
       <c r="M29" t="n">
-        <v>-58.436808</v>
+        <v>-58.480925</v>
       </c>
       <c r="N29" t="n">
-        <v>-34.577464</v>
+        <v>-34.585471</v>
       </c>
       <c r="O29" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P29" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>6235</t>
+          <t>6143</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>6/24/2025</t>
+          <t>6/11/2025</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>HUERGO 389</t>
+          <t>SOLANO LOPEZ, F., MARISCAL 2845</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>807763078</t>
+          <t>807458296</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
@@ -2703,46 +2695,46 @@
         </is>
       </c>
       <c r="M30" t="n">
-        <v>-58.432722</v>
+        <v>-58.495071</v>
       </c>
       <c r="N30" t="n">
-        <v>-34.572371</v>
+        <v>-34.593122</v>
       </c>
       <c r="O30" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P30" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>6231</t>
+          <t>-478</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>6/24/2025</t>
+          <t>6/15/2025</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Ciudad de la Paz 275</t>
+          <t>Chivilcoy 4875</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>807763070</t>
+          <t>807508509</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
@@ -2757,7 +2749,7 @@
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>Aplomar o cambiar</t>
+          <t>Poste podrido</t>
         </is>
       </c>
       <c r="I31" t="n">
@@ -2775,40 +2767,40 @@
       </c>
       <c r="L31" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M31" t="n">
-        <v>-58.441049</v>
+        <v>-58.517389</v>
       </c>
       <c r="N31" t="n">
-        <v>-34.574625</v>
+        <v>-34.593541</v>
       </c>
       <c r="O31" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P31" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>6230</t>
+          <t>6171</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>6/24/2025</t>
+          <t>6/18/2025</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Santa maria de oro	2722</t>
+          <t>CABELLO 3486</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
@@ -2818,7 +2810,7 @@
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>807763066</t>
+          <t>807658640</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
@@ -2833,7 +2825,7 @@
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Columna inclinada evaluar con inspector un corrimiento</t>
         </is>
       </c>
       <c r="I32" t="n">
@@ -2855,10 +2847,10 @@
         </is>
       </c>
       <c r="M32" t="n">
-        <v>-58.422315</v>
+        <v>-58.409579</v>
       </c>
       <c r="N32" t="n">
-        <v>-34.576988</v>
+        <v>-34.581134</v>
       </c>
       <c r="O32" t="inlineStr">
         <is>
@@ -2874,17 +2866,17 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>6173</t>
+          <t>6230</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>4/29/2025</t>
+          <t>6/24/2025</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>ARMENIA 2321</t>
+          <t>Santa maria de oro	2722</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
@@ -2894,7 +2886,7 @@
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>805507398</t>
+          <t>807763066</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
@@ -2909,7 +2901,7 @@
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>Picada volvio a entrar como caso 6325</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I33" t="n">
@@ -2931,10 +2923,10 @@
         </is>
       </c>
       <c r="M33" t="n">
-        <v>-58.420549</v>
+        <v>-58.422315</v>
       </c>
       <c r="N33" t="n">
-        <v>-34.585103</v>
+        <v>-34.576988</v>
       </c>
       <c r="O33" t="inlineStr">
         <is>
@@ -2950,17 +2942,17 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>6171</t>
+          <t>6231</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>6/18/2025</t>
+          <t>6/24/2025</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>CABELLO 3486</t>
+          <t>Ciudad de la Paz 275</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
@@ -2970,7 +2962,7 @@
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>807658640</t>
+          <t>807763070</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
@@ -2985,7 +2977,7 @@
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>Columna inclinada evaluar con inspector un corrimiento</t>
+          <t>Aplomar o cambiar</t>
         </is>
       </c>
       <c r="I34" t="n">
@@ -3003,14 +2995,14 @@
       </c>
       <c r="L34" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M34" t="n">
-        <v>-58.409579</v>
+        <v>-58.441049</v>
       </c>
       <c r="N34" t="n">
-        <v>-34.581134</v>
+        <v>-34.574625</v>
       </c>
       <c r="O34" t="inlineStr">
         <is>
@@ -3026,27 +3018,27 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>6144</t>
+          <t>6235</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>6/11/2025</t>
+          <t>6/24/2025</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>TURIN 2990</t>
+          <t>HUERGO 389</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>807458282</t>
+          <t>807763078</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
@@ -3083,46 +3075,46 @@
         </is>
       </c>
       <c r="M35" t="n">
-        <v>-58.480925</v>
+        <v>-58.432722</v>
       </c>
       <c r="N35" t="n">
-        <v>-34.585471</v>
+        <v>-34.572371</v>
       </c>
       <c r="O35" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P35" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>6143</t>
+          <t>6295</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>6/11/2025</t>
+          <t>6/30/2025</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>SOLANO LOPEZ, F., MARISCAL 2845</t>
+          <t>SOLER 6017</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>807458296</t>
+          <t>807851636</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
@@ -3159,46 +3151,46 @@
         </is>
       </c>
       <c r="M36" t="n">
-        <v>-58.495071</v>
+        <v>-58.436808</v>
       </c>
       <c r="N36" t="n">
-        <v>-34.593122</v>
+        <v>-34.577464</v>
       </c>
       <c r="O36" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P36" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>6071</t>
+          <t>6308</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>3/17/2025</t>
+          <t>7/1/2025</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>OSORIO 4994</t>
+          <t>Guayaquil 637</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>804053324</t>
+          <t>807896343</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
@@ -3211,9 +3203,13 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H37" t="inlineStr"/>
+      <c r="H37" t="inlineStr">
+        <is>
+          <t>Picada</t>
+        </is>
+      </c>
       <c r="I37" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J37" t="inlineStr">
         <is>
@@ -3231,36 +3227,36 @@
         </is>
       </c>
       <c r="M37" t="n">
-        <v>-58.466241</v>
+        <v>-58.437378</v>
       </c>
       <c r="N37" t="n">
-        <v>-34.595741</v>
+        <v>-34.62116</v>
       </c>
       <c r="O37" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P37" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>6036</t>
+          <t>6332</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>2/24/2025</t>
+          <t>7/3/2025</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>MEDRANO 1715</t>
+          <t>ARAOZ 2560</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
@@ -3270,7 +3266,7 @@
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>803608181</t>
+          <t>807965818</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
@@ -3283,9 +3279,13 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H38" t="inlineStr"/>
+      <c r="H38" t="inlineStr">
+        <is>
+          <t>Picada</t>
+        </is>
+      </c>
       <c r="I38" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J38" t="inlineStr">
         <is>
@@ -3294,7 +3294,7 @@
       </c>
       <c r="K38" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L38" t="inlineStr">
@@ -3303,10 +3303,10 @@
         </is>
       </c>
       <c r="M38" t="n">
-        <v>-58.418236</v>
+        <v>-58.414507</v>
       </c>
       <c r="N38" t="n">
-        <v>-34.589859</v>
+        <v>-34.585377</v>
       </c>
       <c r="O38" t="inlineStr">
         <is>
@@ -3322,27 +3322,27 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>-587</t>
+          <t>6383</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>9/8/2025</t>
+          <t>7/8/2025</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>ARIAS 4048</t>
+          <t>FALCON, RAMON L.,CNEL. 1411</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>809526164</t>
+          <t>808099320</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
@@ -3357,7 +3357,7 @@
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>Cambiar 114 picada</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I39" t="n">
@@ -3379,46 +3379,46 @@
         </is>
       </c>
       <c r="M39" t="n">
-        <v>-58.488936</v>
+        <v>-58.448523</v>
       </c>
       <c r="N39" t="n">
-        <v>-34.549005</v>
+        <v>-34.62452</v>
       </c>
       <c r="O39" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P39" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>5826</t>
+          <t>6506</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>5/19/2025</t>
+          <t>7/10/2025</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>ALBARELLOS AV. 3180</t>
+          <t>Ohiggins 1611</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>806926466</t>
+          <t>808148679</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
@@ -3433,7 +3433,7 @@
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t>Columna (metal) inclinada</t>
+          <t>Columna podrida en la base</t>
         </is>
       </c>
       <c r="I40" t="n">
@@ -3441,28 +3441,28 @@
       </c>
       <c r="J40" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K40" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L40" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M40" t="n">
-        <v>-58.513552</v>
+        <v>-58.448993</v>
       </c>
       <c r="N40" t="n">
-        <v>-34.579829</v>
+        <v>-34.564383</v>
       </c>
       <c r="O40" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P40" t="inlineStr">
@@ -3474,27 +3474,27 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>-579</t>
+          <t>6437</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>9/2/2025</t>
+          <t>7/17/2025</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Pedro Rivera 2546</t>
+          <t>MILLER 4590</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>ICD30612785</t>
+          <t>808400306</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
@@ -3509,7 +3509,7 @@
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>Colocar R200 para pedir traspaso de equipos</t>
+          <t>Columna corroida</t>
         </is>
       </c>
       <c r="I41" t="n">
@@ -3522,7 +3522,7 @@
       </c>
       <c r="K41" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L41" t="inlineStr">
@@ -3531,10 +3531,10 @@
         </is>
       </c>
       <c r="M41" t="n">
-        <v>-58.462479</v>
+        <v>-58.495482</v>
       </c>
       <c r="N41" t="n">
-        <v>-34.55765</v>
+        <v>-34.552614</v>
       </c>
       <c r="O41" t="inlineStr">
         <is>
@@ -3550,27 +3550,27 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>-578</t>
+          <t>6538</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>9/2/2025</t>
+          <t>7/17/2025</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Pedro I Rivera 2536</t>
+          <t>Pedraza Manuela 4101</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>809406189</t>
+          <t>808400353</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
@@ -3585,7 +3585,7 @@
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t xml:space="preserve">Podrida en la base </t>
         </is>
       </c>
       <c r="I42" t="n">
@@ -3607,10 +3607,10 @@
         </is>
       </c>
       <c r="M42" t="n">
-        <v>-58.462327</v>
+        <v>-58.481569</v>
       </c>
       <c r="N42" t="n">
-        <v>-34.557565</v>
+        <v>-34.559853</v>
       </c>
       <c r="O42" t="inlineStr">
         <is>
@@ -3626,27 +3626,27 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>-577</t>
+          <t>7023</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>9/2/2025</t>
+          <t>7/22/2025</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Manuel Ugarte 2318</t>
+          <t>ZABALA 3573</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>809406177</t>
+          <t>808480549</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
@@ -3661,7 +3661,7 @@
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Corroida en base para recambio entro tambien como caso 3575</t>
         </is>
       </c>
       <c r="I43" t="n">
@@ -3683,14 +3683,14 @@
         </is>
       </c>
       <c r="M43" t="n">
-        <v>-58.460635</v>
+        <v>-58.457522</v>
       </c>
       <c r="N43" t="n">
-        <v>-34.555932</v>
+        <v>-34.579414</v>
       </c>
       <c r="O43" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P43" t="inlineStr">
@@ -3702,27 +3702,27 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>-576</t>
+          <t>6484</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>8/29/2025</t>
+          <t>7/24/2025</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Av. Boyacá 2030</t>
+          <t>URIARTE 2396</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>809309606</t>
+          <t>808509373</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
@@ -3759,46 +3759,46 @@
         </is>
       </c>
       <c r="M44" t="n">
-        <v>-58.471173</v>
+        <v>-58.423934</v>
       </c>
       <c r="N44" t="n">
-        <v>-34.60704</v>
+        <v>-34.581562</v>
       </c>
       <c r="O44" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P44" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>-575</t>
+          <t>6512</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>8/28/2025</t>
+          <t>7/28/2025</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Amenabar 3064</t>
+          <t>GASCON 1195</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>809281299</t>
+          <t>808571975</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
@@ -3835,46 +3835,46 @@
         </is>
       </c>
       <c r="M45" t="n">
-        <v>-58.465984</v>
+        <v>-58.423127</v>
       </c>
       <c r="N45" t="n">
-        <v>-34.554869</v>
+        <v>-34.596476</v>
       </c>
       <c r="O45" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P45" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>5715</t>
+          <t>6519</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>5/1/2025</t>
+          <t>7/28/2025</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>CUENCA 4690</t>
+          <t>SALGUERO, JERONIMO 2874</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>805579094</t>
+          <t>808571977</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
@@ -3889,7 +3889,7 @@
       </c>
       <c r="H46" t="inlineStr">
         <is>
-          <t>Aplomar poste</t>
+          <t>Reparar rienda</t>
         </is>
       </c>
       <c r="I46" t="n">
@@ -3897,7 +3897,7 @@
       </c>
       <c r="J46" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Tensor</t>
         </is>
       </c>
       <c r="K46" t="inlineStr">
@@ -3907,50 +3907,50 @@
       </c>
       <c r="L46" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M46" t="n">
-        <v>-58.506061</v>
+        <v>-58.407256</v>
       </c>
       <c r="N46" t="n">
-        <v>-34.588887</v>
+        <v>-34.578976</v>
       </c>
       <c r="O46" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P46" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>5656</t>
+          <t>-538</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>4/24/2025</t>
+          <t>7/31/2025</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>ECHEVERRIA 5893</t>
+          <t>Malabia 964</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>804922184</t>
+          <t>808609237</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
@@ -3965,7 +3965,7 @@
       </c>
       <c r="H47" t="inlineStr">
         <is>
-          <t>Poste con base quebrada</t>
+          <t>Cambiar poste mal estado por PRFV</t>
         </is>
       </c>
       <c r="I47" t="n">
@@ -3973,7 +3973,7 @@
       </c>
       <c r="J47" t="inlineStr">
         <is>
-          <t>Desmonte</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K47" t="inlineStr">
@@ -3987,46 +3987,46 @@
         </is>
       </c>
       <c r="M47" t="n">
-        <v>-58.489627</v>
+        <v>-58.433634</v>
       </c>
       <c r="N47" t="n">
-        <v>-34.583761</v>
+        <v>-34.595018</v>
       </c>
       <c r="O47" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P47" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>5624</t>
+          <t>-547</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>4/22/2025</t>
+          <t>8/6/2025</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>PINO, VIRREY DEL 3456</t>
+          <t>Habana 4210</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>804876043</t>
+          <t>808733921</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
@@ -4041,7 +4041,7 @@
       </c>
       <c r="H48" t="inlineStr">
         <is>
-          <t>Desmonte de poste</t>
+          <t>Cambiar poste dañado</t>
         </is>
       </c>
       <c r="I48" t="n">
@@ -4049,7 +4049,7 @@
       </c>
       <c r="J48" t="inlineStr">
         <is>
-          <t>Desmonte</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K48" t="inlineStr">
@@ -4063,14 +4063,14 @@
         </is>
       </c>
       <c r="M48" t="n">
-        <v>-58.464354</v>
+        <v>-58.515873</v>
       </c>
       <c r="N48" t="n">
-        <v>-34.572486</v>
+        <v>-34.599425</v>
       </c>
       <c r="O48" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P48" t="inlineStr">
@@ -4082,27 +4082,27 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>5599</t>
+          <t>6579</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>4/15/2025</t>
+          <t>8/7/2025</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>ESTOMBA 4052</t>
+          <t>RIVADAVIA MARTIN, COMODORO 1350</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>804732246</t>
+          <t>808749184</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
@@ -4117,7 +4117,7 @@
       </c>
       <c r="H49" t="inlineStr">
         <is>
-          <t>Columna PRFV quedo inclinada (la hicieron como estomba 4056)</t>
+          <t>Poste inclinado</t>
         </is>
       </c>
       <c r="I49" t="n">
@@ -4130,19 +4130,19 @@
       </c>
       <c r="K49" t="inlineStr">
         <is>
-          <t>Nodo TLC</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L49" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M49" t="n">
-        <v>-58.485407</v>
+        <v>-58.461024</v>
       </c>
       <c r="N49" t="n">
-        <v>-34.552985</v>
+        <v>-34.539409</v>
       </c>
       <c r="O49" t="inlineStr">
         <is>
@@ -4158,27 +4158,27 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>5590</t>
+          <t>6906</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>4/15/2025</t>
+          <t>8/12/2025</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>O'HIGGINS 2441</t>
+          <t>MOSCONI GENERAL AV. 3163</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>804732275</t>
+          <t>808918685</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
@@ -4215,14 +4215,14 @@
         </is>
       </c>
       <c r="M50" t="n">
-        <v>-58.45573</v>
+        <v>-58.505731</v>
       </c>
       <c r="N50" t="n">
-        <v>-34.556576</v>
+        <v>-34.588316</v>
       </c>
       <c r="O50" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P50" t="inlineStr">
@@ -4234,27 +4234,27 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>-559</t>
+          <t>6910</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>8/21/2025</t>
+          <t>8/12/2025</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Av. Del Libertador 6736</t>
+          <t>RIVAS, GRAL. 2345</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>809098713</t>
+          <t>808918698</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
@@ -4269,7 +4269,7 @@
       </c>
       <c r="H51" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I51" t="n">
@@ -4291,14 +4291,14 @@
         </is>
       </c>
       <c r="M51" t="n">
-        <v>-58.453398</v>
+        <v>-58.482497</v>
       </c>
       <c r="N51" t="n">
-        <v>-34.550238</v>
+        <v>-34.598714</v>
       </c>
       <c r="O51" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P51" t="inlineStr">
@@ -4310,27 +4310,27 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>5589</t>
+          <t>6928</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>12/31/2023</t>
+          <t>8/12/2025</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>ARCOS 1520</t>
+          <t>ALBARELLOS AV. 3101</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>799540526</t>
+          <t>808918710</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
@@ -4340,7 +4340,7 @@
       </c>
       <c r="G52" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
+          <t>Pendiente</t>
         </is>
       </c>
       <c r="H52" t="inlineStr">
@@ -4349,7 +4349,7 @@
         </is>
       </c>
       <c r="I52" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J52" t="inlineStr">
         <is>
@@ -4358,7 +4358,7 @@
       </c>
       <c r="K52" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L52" t="inlineStr">
@@ -4367,14 +4367,14 @@
         </is>
       </c>
       <c r="M52" t="n">
-        <v>-58.449125</v>
+        <v>-58.512623</v>
       </c>
       <c r="N52" t="n">
-        <v>-34.565958</v>
+        <v>-34.579137</v>
       </c>
       <c r="O52" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P52" t="inlineStr">
@@ -4386,27 +4386,27 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>5503</t>
+          <t>-550</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>8/22/2025</t>
+          <t>8/12/2025</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>CRAMER AV. 1771</t>
+          <t>Fitz roy 267</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>809102564</t>
+          <t>808918720</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
@@ -4421,7 +4421,7 @@
       </c>
       <c r="H53" t="inlineStr">
         <is>
-          <t>PIcada</t>
+          <t>Aplomar columna</t>
         </is>
       </c>
       <c r="I53" t="n">
@@ -4443,14 +4443,14 @@
         </is>
       </c>
       <c r="M53" t="n">
-        <v>-58.458506</v>
+        <v>-58.451378</v>
       </c>
       <c r="N53" t="n">
-        <v>-34.56783</v>
+        <v>-34.596195</v>
       </c>
       <c r="O53" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P53" t="inlineStr">
@@ -4462,27 +4462,27 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>-550</t>
+          <t>6943</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>8/12/2025</t>
+          <t>8/14/2025</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>Fitz roy 267</t>
+          <t>SUPERI 1459</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>808918720</t>
+          <t>808972965</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
@@ -4497,7 +4497,7 @@
       </c>
       <c r="H54" t="inlineStr">
         <is>
-          <t>Aplomar columna</t>
+          <t>Poste con base quebrada ver si es posible desmonte</t>
         </is>
       </c>
       <c r="I54" t="n">
@@ -4505,7 +4505,7 @@
       </c>
       <c r="J54" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Desmonte</t>
         </is>
       </c>
       <c r="K54" t="inlineStr">
@@ -4515,18 +4515,18 @@
       </c>
       <c r="L54" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M54" t="n">
-        <v>-58.451378</v>
+        <v>-58.460834</v>
       </c>
       <c r="N54" t="n">
-        <v>-34.596195</v>
+        <v>-34.573753</v>
       </c>
       <c r="O54" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P54" t="inlineStr">
@@ -4538,27 +4538,27 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>5492</t>
+          <t>6969</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>4/4/2025</t>
+          <t>8/14/2025</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>ESTADO PLURINACIONAL DE BOLIVIA 5920</t>
+          <t>CIUDAD DE LA PAZ 295</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>804498035</t>
+          <t>808972995</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
@@ -4573,7 +4573,7 @@
       </c>
       <c r="H55" t="inlineStr">
         <is>
-          <t>aplomar</t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I55" t="n">
@@ -4581,7 +4581,7 @@
       </c>
       <c r="J55" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K55" t="inlineStr">
@@ -4591,50 +4591,50 @@
       </c>
       <c r="L55" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M55" t="n">
-        <v>-58.50751</v>
+        <v>-58.441171</v>
       </c>
       <c r="N55" t="n">
-        <v>-34.574543</v>
+        <v>-34.574547</v>
       </c>
       <c r="O55" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P55" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>-547</t>
+          <t>6971</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>8/6/2025</t>
+          <t>8/14/2025</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>Habana 4210</t>
+          <t>MAURE 1594</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>808733921</t>
+          <t>808973001</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
@@ -4649,7 +4649,7 @@
       </c>
       <c r="H56" t="inlineStr">
         <is>
-          <t>Cambiar poste dañado</t>
+          <t>Ver de traspasar a telecentro y  desmontar ver con inspector</t>
         </is>
       </c>
       <c r="I56" t="n">
@@ -4667,50 +4667,50 @@
       </c>
       <c r="L56" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M56" t="n">
-        <v>-58.515873</v>
+        <v>-58.435072</v>
       </c>
       <c r="N56" t="n">
-        <v>-34.599425</v>
+        <v>-34.565732</v>
       </c>
       <c r="O56" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P56" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>5469</t>
+          <t>7000</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>4/4/2025</t>
+          <t>8/20/2025</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>ESTADO PLURINACIONAL DE BOLIVIA 5899</t>
+          <t>SCALABRINI ORTIZ, RAUL AV. 2106</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>804497887</t>
+          <t>809065867</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
@@ -4725,7 +4725,7 @@
       </c>
       <c r="H57" t="inlineStr">
         <is>
-          <t>Aplomar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I57" t="n">
@@ -4733,7 +4733,7 @@
       </c>
       <c r="J57" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K57" t="inlineStr">
@@ -4743,50 +4743,50 @@
       </c>
       <c r="L57" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M57" t="n">
-        <v>-58.507746</v>
+        <v>-58.420109</v>
       </c>
       <c r="N57" t="n">
-        <v>-34.574217</v>
+        <v>-34.58764</v>
       </c>
       <c r="O57" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P57" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>5464</t>
+          <t>7003</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>4/4/2025</t>
+          <t>8/20/2025</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>SUCRE, ANTONIO JOSE DE, MCAL. 3100</t>
+          <t>MELIAN AV. 2576</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>804497880</t>
+          <t>809065874</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
@@ -4819,14 +4819,14 @@
       </c>
       <c r="L58" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M58" t="n">
-        <v>-58.46161</v>
+        <v>-58.471943</v>
       </c>
       <c r="N58" t="n">
-        <v>-34.567849</v>
+        <v>-34.564948</v>
       </c>
       <c r="O58" t="inlineStr">
         <is>
@@ -4842,27 +4842,27 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>-538</t>
+          <t>-559</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>7/31/2025</t>
+          <t>8/21/2025</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>Malabia 964</t>
+          <t>Av. Del Libertador 6736</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>808609237</t>
+          <t>809098713</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
@@ -4877,7 +4877,7 @@
       </c>
       <c r="H59" t="inlineStr">
         <is>
-          <t>Cambiar poste mal estado por PRFV</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I59" t="n">
@@ -4895,40 +4895,40 @@
       </c>
       <c r="L59" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M59" t="n">
-        <v>-58.433634</v>
+        <v>-58.453398</v>
       </c>
       <c r="N59" t="n">
-        <v>-34.595018</v>
+        <v>-34.550238</v>
       </c>
       <c r="O59" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P59" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>5053</t>
+          <t>5503</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>3/11/2025</t>
+          <t>8/22/2025</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>MENDOZA 1153</t>
+          <t>CRAMER AV. 1771</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
@@ -4938,7 +4938,7 @@
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>803969314</t>
+          <t>809102564</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
@@ -4953,11 +4953,11 @@
       </c>
       <c r="H60" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>PIcada</t>
         </is>
       </c>
       <c r="I60" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J60" t="inlineStr">
         <is>
@@ -4971,18 +4971,18 @@
       </c>
       <c r="L60" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M60" t="n">
-        <v>-58.44463</v>
+        <v>-58.458506</v>
       </c>
       <c r="N60" t="n">
-        <v>-34.553354</v>
+        <v>-34.56783</v>
       </c>
       <c r="O60" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P60" t="inlineStr">
@@ -4994,27 +4994,27 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>4862</t>
+          <t>7098</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>1/23/2025</t>
+          <t>8/25/2025</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>ARCOS 2263</t>
+          <t>UGARTE, MANUEL 3484</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>802857379</t>
+          <t>809126236</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
@@ -5024,16 +5024,16 @@
       </c>
       <c r="G61" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
+          <t>Pendiente</t>
         </is>
       </c>
       <c r="H61" t="inlineStr">
         <is>
-          <t>picada</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I61" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J61" t="inlineStr">
         <is>
@@ -5042,7 +5042,7 @@
       </c>
       <c r="K61" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L61" t="inlineStr">
@@ -5051,14 +5051,14 @@
         </is>
       </c>
       <c r="M61" t="n">
-        <v>-58.455082</v>
+        <v>-58.472869</v>
       </c>
       <c r="N61" t="n">
-        <v>-34.558883</v>
+        <v>-34.562</v>
       </c>
       <c r="O61" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P61" t="inlineStr">
@@ -5070,27 +5070,27 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>-478</t>
+          <t>7080</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>6/15/2025</t>
+          <t>8/25/2025</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>Chivilcoy 4875</t>
+          <t>UGARTE, MANUEL 2196</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>807508509</t>
+          <t>809125906</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
@@ -5105,7 +5105,7 @@
       </c>
       <c r="H62" t="inlineStr">
         <is>
-          <t>Poste podrido</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I62" t="n">
@@ -5123,18 +5123,18 @@
       </c>
       <c r="L62" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M62" t="n">
-        <v>-58.517389</v>
+        <v>-58.459402</v>
       </c>
       <c r="N62" t="n">
-        <v>-34.593541</v>
+        <v>-34.555262</v>
       </c>
       <c r="O62" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P62" t="inlineStr">
@@ -5146,27 +5146,27 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>4595</t>
+          <t>7021</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>1/15/2025</t>
+          <t>8/25/2025</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>PAROISSIEN 1806</t>
+          <t>VERA 445</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>802747617</t>
+          <t>809155622</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
@@ -5181,7 +5181,7 @@
       </c>
       <c r="H63" t="inlineStr">
         <is>
-          <t>Aplomar</t>
+          <t>Correrla para sacarla del cantero</t>
         </is>
       </c>
       <c r="I63" t="n">
@@ -5189,7 +5189,7 @@
       </c>
       <c r="J63" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K63" t="inlineStr">
@@ -5199,50 +5199,50 @@
       </c>
       <c r="L63" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M63" t="n">
-        <v>-58.464172</v>
+        <v>-58.437181</v>
       </c>
       <c r="N63" t="n">
-        <v>-34.543845</v>
+        <v>-34.5995</v>
       </c>
       <c r="O63" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P63" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>4528</t>
+          <t>-569</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>1/16/2025</t>
+          <t>8/27/2025</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>BARCO CENTENERA DEL 545</t>
+          <t>Palpa 2862</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>802774521</t>
+          <t>809257759</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
@@ -5279,46 +5279,46 @@
         </is>
       </c>
       <c r="M64" t="n">
-        <v>-58.440625</v>
+        <v>-58.449512</v>
       </c>
       <c r="N64" t="n">
-        <v>-34.625499</v>
+        <v>-34.573404</v>
       </c>
       <c r="O64" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P64" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>-406</t>
+          <t>6465</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>5/8/2025</t>
+          <t>8/28/2025</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>Olof palme 4144</t>
+          <t>AGUIRRE 368</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>805791925</t>
+          <t>809268249</t>
         </is>
       </c>
       <c r="F65" t="inlineStr">
@@ -5333,7 +5333,7 @@
       </c>
       <c r="H65" t="inlineStr">
         <is>
-          <t>Tensar 2 riendas a pique columna 168</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I65" t="n">
@@ -5341,7 +5341,7 @@
       </c>
       <c r="J65" t="inlineStr">
         <is>
-          <t>Tensor</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K65" t="inlineStr">
@@ -5351,50 +5351,50 @@
       </c>
       <c r="L65" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M65" t="n">
-        <v>-58.488252</v>
+        <v>-58.434651</v>
       </c>
       <c r="N65" t="n">
-        <v>-34.553391</v>
+        <v>-34.598814</v>
       </c>
       <c r="O65" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P65" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>-404</t>
+          <t>7095</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>5/8/2025</t>
+          <t>8/28/2025</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>Amenabar 3048</t>
+          <t>SAN MARTIN AV. 4515</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>805791896</t>
+          <t>809268240</t>
         </is>
       </c>
       <c r="F66" t="inlineStr">
@@ -5409,7 +5409,7 @@
       </c>
       <c r="H66" t="inlineStr">
         <is>
-          <t>Aplomar columna 114</t>
+          <t>Columna chocada</t>
         </is>
       </c>
       <c r="I66" t="n">
@@ -5417,7 +5417,7 @@
       </c>
       <c r="J66" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K66" t="inlineStr">
@@ -5427,18 +5427,18 @@
       </c>
       <c r="L66" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M66" t="n">
-        <v>-58.46579</v>
+        <v>-58.483415</v>
       </c>
       <c r="N66" t="n">
-        <v>-34.555012</v>
+        <v>-34.597663</v>
       </c>
       <c r="O66" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P66" t="inlineStr">
@@ -5450,17 +5450,17 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>3839</t>
+          <t>-575</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>10/23/2024</t>
+          <t>8/28/2025</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>PICO 1511</t>
+          <t>Amenabar 3064</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
@@ -5470,7 +5470,7 @@
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>798390296</t>
+          <t>809281299</t>
         </is>
       </c>
       <c r="F67" t="inlineStr">
@@ -5485,7 +5485,7 @@
       </c>
       <c r="H67" t="inlineStr">
         <is>
-          <t>Poste inclinado</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I67" t="n">
@@ -5493,7 +5493,7 @@
       </c>
       <c r="J67" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K67" t="inlineStr">
@@ -5503,14 +5503,14 @@
       </c>
       <c r="L67" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M67" t="n">
-        <v>-58.465596</v>
+        <v>-58.465984</v>
       </c>
       <c r="N67" t="n">
-        <v>-34.53627</v>
+        <v>-34.554869</v>
       </c>
       <c r="O67" t="inlineStr">
         <is>
@@ -5526,27 +5526,27 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>3430</t>
+          <t>-576</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>4/1/2025</t>
+          <t>8/29/2025</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>MONROE 3838</t>
+          <t>Av. Boyacá 2030</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>804468442</t>
+          <t>809309606</t>
         </is>
       </c>
       <c r="F68" t="inlineStr">
@@ -5561,7 +5561,7 @@
       </c>
       <c r="H68" t="inlineStr">
         <is>
-          <t>Reparar rienda</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I68" t="n">
@@ -5569,7 +5569,7 @@
       </c>
       <c r="J68" t="inlineStr">
         <is>
-          <t>Tensor</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K68" t="inlineStr">
@@ -5579,18 +5579,18 @@
       </c>
       <c r="L68" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M68" t="n">
-        <v>-58.473659</v>
+        <v>-58.471173</v>
       </c>
       <c r="N68" t="n">
-        <v>-34.566979</v>
+        <v>-34.60704</v>
       </c>
       <c r="O68" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P68" t="inlineStr">
@@ -5602,17 +5602,17 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>3348</t>
+          <t>7111</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>3/27/2025</t>
+          <t>9/1/2025</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>ESTOMBA 2626</t>
+          <t>VILELA 3699</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
@@ -5622,7 +5622,7 @@
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>804309704</t>
+          <t>809371823</t>
         </is>
       </c>
       <c r="F69" t="inlineStr">
@@ -5637,7 +5637,7 @@
       </c>
       <c r="H69" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t xml:space="preserve">Cambiar </t>
         </is>
       </c>
       <c r="I69" t="n">
@@ -5645,7 +5645,7 @@
       </c>
       <c r="J69" t="inlineStr">
         <is>
-          <t>Desmonte</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K69" t="inlineStr">
@@ -5655,18 +5655,18 @@
       </c>
       <c r="L69" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M69" t="n">
-        <v>-58.47538</v>
+        <v>-58.482817</v>
       </c>
       <c r="N69" t="n">
-        <v>-34.566015</v>
+        <v>-34.550845</v>
       </c>
       <c r="O69" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P69" t="inlineStr">
@@ -5678,17 +5678,17 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>3299</t>
+          <t>7118</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>9/10/2024</t>
+          <t>9/2/2025</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>DIAZ COLODRERO 3309</t>
+          <t>CUBAS, JOSE 2211</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
@@ -5698,7 +5698,7 @@
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>796186684</t>
+          <t>809406168</t>
         </is>
       </c>
       <c r="F70" t="inlineStr">
@@ -5708,12 +5708,12 @@
       </c>
       <c r="G70" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
+          <t>Pendiente</t>
         </is>
       </c>
       <c r="H70" t="inlineStr">
         <is>
-          <t>qap traspaso nodo TLC y Teco</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I70" t="n">
@@ -5726,7 +5726,7 @@
       </c>
       <c r="K70" t="inlineStr">
         <is>
-          <t>Nodo TLC</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L70" t="inlineStr">
@@ -5735,10 +5735,10 @@
         </is>
       </c>
       <c r="M70" t="n">
-        <v>-58.491722</v>
+        <v>-58.492448</v>
       </c>
       <c r="N70" t="n">
-        <v>-34.565845</v>
+        <v>-34.58372</v>
       </c>
       <c r="O70" t="inlineStr">
         <is>
@@ -5754,27 +5754,27 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>-312</t>
+          <t>-577</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>3/29/2025</t>
+          <t>9/2/2025</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>MATIENZO BENJAMIN /ALT/ 1831</t>
+          <t>Manuel Ugarte 2318</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>804333522</t>
+          <t>809406177</t>
         </is>
       </c>
       <c r="F71" t="inlineStr">
@@ -5789,11 +5789,11 @@
       </c>
       <c r="H71" t="inlineStr">
         <is>
-          <t>Retirar columna ya traspasaron el nodo</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I71" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J71" t="inlineStr">
         <is>
@@ -5802,7 +5802,7 @@
       </c>
       <c r="K71" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L71" t="inlineStr">
@@ -5811,46 +5811,46 @@
         </is>
       </c>
       <c r="M71" t="n">
-        <v>-58.434835</v>
+        <v>-58.460635</v>
       </c>
       <c r="N71" t="n">
-        <v>-34.569129</v>
+        <v>-34.555932</v>
       </c>
       <c r="O71" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P71" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>2485</t>
+          <t>-578</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>3/26/2025</t>
+          <t>9/2/2025</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>LA PLATA AV. 1095</t>
+          <t>Pedro I Rivera 2536</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>804302893</t>
+          <t>809406189</t>
         </is>
       </c>
       <c r="F72" t="inlineStr">
@@ -5865,7 +5865,7 @@
       </c>
       <c r="H72" t="inlineStr">
         <is>
-          <t>Sacar ancla de rienda vieja y cementar vereda</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I72" t="n">
@@ -5873,7 +5873,7 @@
       </c>
       <c r="J72" t="inlineStr">
         <is>
-          <t>Tensor</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K72" t="inlineStr">
@@ -5883,50 +5883,50 @@
       </c>
       <c r="L72" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M72" t="n">
-        <v>-58.426593</v>
+        <v>-58.462327</v>
       </c>
       <c r="N72" t="n">
-        <v>-34.628211</v>
+        <v>-34.557565</v>
       </c>
       <c r="O72" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P72" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>232</t>
+          <t>-579</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>5/9/2025</t>
+          <t>9/2/2025</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>Gorostiaga 2286</t>
+          <t>Pedro Rivera 2546</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>805791858</t>
+          <t>ICD30612785</t>
         </is>
       </c>
       <c r="F73" t="inlineStr">
@@ -5941,7 +5941,7 @@
       </c>
       <c r="H73" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Colocar R200 para pedir traspaso de equipos</t>
         </is>
       </c>
       <c r="I73" t="n">
@@ -5954,7 +5954,7 @@
       </c>
       <c r="K73" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L73" t="inlineStr">
@@ -5963,19 +5963,95 @@
         </is>
       </c>
       <c r="M73" t="n">
-        <v>-58.441563</v>
+        <v>-58.462479</v>
       </c>
       <c r="N73" t="n">
-        <v>-34.569743</v>
+        <v>-34.55765</v>
       </c>
       <c r="O73" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P73" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>-587</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>9/8/2025</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>ARIAS 4048</t>
+        </is>
+      </c>
+      <c r="D74" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="E74" t="inlineStr">
+        <is>
+          <t>809526164</t>
+        </is>
+      </c>
+      <c r="F74" t="inlineStr">
+        <is>
+          <t>NEW</t>
+        </is>
+      </c>
+      <c r="G74" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H74" t="inlineStr">
+        <is>
+          <t>Cambiar 114 picada</t>
+        </is>
+      </c>
+      <c r="I74" t="n">
+        <v>1</v>
+      </c>
+      <c r="J74" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K74" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L74" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M74" t="n">
+        <v>-58.488936</v>
+      </c>
+      <c r="N74" t="n">
+        <v>-34.549005</v>
+      </c>
+      <c r="O74" t="inlineStr">
+        <is>
+          <t>Saavedra</t>
+        </is>
+      </c>
+      <c r="P74" t="inlineStr">
+        <is>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-09-11 07:49:43)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_NEW.xlsx
+++ b/mapa_interactivo_NEW.xlsx
@@ -5754,7 +5754,7 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>-577</t>
+          <t>7211</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
@@ -5764,7 +5764,7 @@
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>Manuel Ugarte 2318</t>
+          <t>UGARTE, MANUEL 2318</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
@@ -5830,7 +5830,7 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>-578</t>
+          <t>7210</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
@@ -5840,7 +5840,7 @@
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>Pedro I Rivera 2536</t>
+          <t>RIVERA, PEDRO I., Dr. 2536</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-09-15 07:09:38)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_NEW.xlsx
+++ b/mapa_interactivo_NEW.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P74"/>
+  <dimension ref="A1:P73"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -518,27 +518,27 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>3299</t>
+          <t>7211</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>9/10/2024</t>
+          <t>9/2/2025</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>DIAZ COLODRERO 3309</t>
+          <t>UGARTE, MANUEL 2318</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>796186684</t>
+          <t>809406177</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -548,12 +548,12 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
+          <t>Pendiente</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>qap traspaso nodo TLC y Teco</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I2" t="n">
@@ -566,7 +566,7 @@
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>Nodo TLC</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
@@ -575,14 +575,14 @@
         </is>
       </c>
       <c r="M2" t="n">
-        <v>-58.491722</v>
+        <v>-58.460635</v>
       </c>
       <c r="N2" t="n">
-        <v>-34.565845</v>
+        <v>-34.555932</v>
       </c>
       <c r="O2" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P2" t="inlineStr">
@@ -594,17 +594,17 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>3839</t>
+          <t>7210</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>10/23/2024</t>
+          <t>9/2/2025</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>PICO 1511</t>
+          <t>RIVERA, PEDRO I., Dr. 2536</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -614,7 +614,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>798390296</t>
+          <t>809406189</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -629,7 +629,7 @@
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>Poste inclinado</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I3" t="n">
@@ -637,7 +637,7 @@
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
@@ -647,14 +647,14 @@
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M3" t="n">
-        <v>-58.465596</v>
+        <v>-58.462327</v>
       </c>
       <c r="N3" t="n">
-        <v>-34.53627</v>
+        <v>-34.557565</v>
       </c>
       <c r="O3" t="inlineStr">
         <is>
@@ -670,27 +670,27 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>5589</t>
+          <t>7118</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>12/31/2023</t>
+          <t>9/2/2025</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>ARCOS 1520</t>
+          <t>CUBAS, JOSE 2211</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>799540526</t>
+          <t>809406168</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -700,7 +700,7 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
+          <t>Pendiente</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
@@ -709,7 +709,7 @@
         </is>
       </c>
       <c r="I4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J4" t="inlineStr">
         <is>
@@ -718,7 +718,7 @@
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
@@ -727,14 +727,14 @@
         </is>
       </c>
       <c r="M4" t="n">
-        <v>-58.449125</v>
+        <v>-58.492448</v>
       </c>
       <c r="N4" t="n">
-        <v>-34.565958</v>
+        <v>-34.58372</v>
       </c>
       <c r="O4" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P4" t="inlineStr">
@@ -746,27 +746,27 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>4595</t>
+          <t>7111</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>1/15/2025</t>
+          <t>9/1/2025</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>PAROISSIEN 1806</t>
+          <t>VILELA 3699</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>802747617</t>
+          <t>809371823</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -781,7 +781,7 @@
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>Aplomar</t>
+          <t xml:space="preserve">Cambiar </t>
         </is>
       </c>
       <c r="I5" t="n">
@@ -789,7 +789,7 @@
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
@@ -803,10 +803,10 @@
         </is>
       </c>
       <c r="M5" t="n">
-        <v>-58.464172</v>
+        <v>-58.482817</v>
       </c>
       <c r="N5" t="n">
-        <v>-34.543845</v>
+        <v>-34.550845</v>
       </c>
       <c r="O5" t="inlineStr">
         <is>
@@ -822,27 +822,27 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>4528</t>
+          <t>7098</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>1/16/2025</t>
+          <t>8/25/2025</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>BARCO CENTENERA DEL 545</t>
+          <t>UGARTE, MANUEL 3484</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>802774521</t>
+          <t>809126236</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -879,46 +879,46 @@
         </is>
       </c>
       <c r="M6" t="n">
-        <v>-58.440625</v>
+        <v>-58.472869</v>
       </c>
       <c r="N6" t="n">
-        <v>-34.625499</v>
+        <v>-34.562</v>
       </c>
       <c r="O6" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P6" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>4862</t>
+          <t>7095</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>1/23/2025</t>
+          <t>8/28/2025</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>ARCOS 2263</t>
+          <t>SAN MARTIN AV. 4515</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>802857379</t>
+          <t>809268240</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -928,16 +928,16 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
+          <t>Pendiente</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>picada</t>
+          <t>Columna chocada</t>
         </is>
       </c>
       <c r="I7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J7" t="inlineStr">
         <is>
@@ -946,23 +946,23 @@
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M7" t="n">
-        <v>-58.455082</v>
+        <v>-58.483415</v>
       </c>
       <c r="N7" t="n">
-        <v>-34.558883</v>
+        <v>-34.597663</v>
       </c>
       <c r="O7" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P7" t="inlineStr">
@@ -974,27 +974,27 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>6036</t>
+          <t>7080</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>2/24/2025</t>
+          <t>8/25/2025</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>MEDRANO 1715</t>
+          <t>UGARTE, MANUEL 2196</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>803608181</t>
+          <t>809125906</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -1007,9 +1007,13 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H8" t="inlineStr"/>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>Picada</t>
+        </is>
+      </c>
       <c r="I8" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J8" t="inlineStr">
         <is>
@@ -1018,7 +1022,7 @@
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L8" t="inlineStr">
@@ -1027,46 +1031,46 @@
         </is>
       </c>
       <c r="M8" t="n">
-        <v>-58.418236</v>
+        <v>-58.459402</v>
       </c>
       <c r="N8" t="n">
-        <v>-34.589859</v>
+        <v>-34.555262</v>
       </c>
       <c r="O8" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P8" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>5053</t>
+          <t>7023</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>3/11/2025</t>
+          <t>7/22/2025</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>MENDOZA 1153</t>
+          <t>ZABALA 3573</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>803969314</t>
+          <t>808480549</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -1081,11 +1085,11 @@
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Corroida en base para recambio entro tambien como caso 3575</t>
         </is>
       </c>
       <c r="I9" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J9" t="inlineStr">
         <is>
@@ -1099,18 +1103,18 @@
       </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M9" t="n">
-        <v>-58.44463</v>
+        <v>-58.457522</v>
       </c>
       <c r="N9" t="n">
-        <v>-34.553354</v>
+        <v>-34.579414</v>
       </c>
       <c r="O9" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P9" t="inlineStr">
@@ -1122,17 +1126,17 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>6071</t>
+          <t>7021</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>3/17/2025</t>
+          <t>8/25/2025</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>OSORIO 4994</t>
+          <t>VERA 445</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -1142,7 +1146,7 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>804053324</t>
+          <t>809155622</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
@@ -1155,9 +1159,13 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H10" t="inlineStr"/>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>Correrla para sacarla del cantero</t>
+        </is>
+      </c>
       <c r="I10" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J10" t="inlineStr">
         <is>
@@ -1175,46 +1183,46 @@
         </is>
       </c>
       <c r="M10" t="n">
-        <v>-58.466241</v>
+        <v>-58.437181</v>
       </c>
       <c r="N10" t="n">
-        <v>-34.595741</v>
+        <v>-34.5995</v>
       </c>
       <c r="O10" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P10" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2485</t>
+          <t>7003</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>3/26/2025</t>
+          <t>8/20/2025</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>LA PLATA AV. 1095</t>
+          <t>MELIAN AV. 2576</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>804302893</t>
+          <t>809065874</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
@@ -1229,7 +1237,7 @@
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>Sacar ancla de rienda vieja y cementar vereda</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I11" t="n">
@@ -1237,7 +1245,7 @@
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>Tensor</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K11" t="inlineStr">
@@ -1247,50 +1255,50 @@
       </c>
       <c r="L11" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M11" t="n">
-        <v>-58.426593</v>
+        <v>-58.471943</v>
       </c>
       <c r="N11" t="n">
-        <v>-34.628211</v>
+        <v>-34.564948</v>
       </c>
       <c r="O11" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P11" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>3348</t>
+          <t>7000</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>3/27/2025</t>
+          <t>8/20/2025</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>ESTOMBA 2626</t>
+          <t>SCALABRINI ORTIZ, RAUL AV. 2106</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>804309704</t>
+          <t>809065867</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
@@ -1313,7 +1321,7 @@
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>Desmonte</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K12" t="inlineStr">
@@ -1327,36 +1335,36 @@
         </is>
       </c>
       <c r="M12" t="n">
-        <v>-58.47538</v>
+        <v>-58.420109</v>
       </c>
       <c r="N12" t="n">
-        <v>-34.566015</v>
+        <v>-34.58764</v>
       </c>
       <c r="O12" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P12" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>-312</t>
+          <t>6971</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>3/29/2025</t>
+          <t>8/14/2025</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>MATIENZO BENJAMIN /ALT/ 1831</t>
+          <t>MAURE 1594</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -1366,7 +1374,7 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>804333522</t>
+          <t>ICD30754530</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
@@ -1381,11 +1389,11 @@
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>Retirar columna ya traspasaron el nodo</t>
+          <t>Desmontar columna</t>
         </is>
       </c>
       <c r="I13" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J13" t="inlineStr">
         <is>
@@ -1394,7 +1402,7 @@
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L13" t="inlineStr">
@@ -1403,10 +1411,10 @@
         </is>
       </c>
       <c r="M13" t="n">
-        <v>-58.434835</v>
+        <v>-58.435072</v>
       </c>
       <c r="N13" t="n">
-        <v>-34.569129</v>
+        <v>-34.565732</v>
       </c>
       <c r="O13" t="inlineStr">
         <is>
@@ -1422,27 +1430,27 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>3430</t>
+          <t>6943</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>4/1/2025</t>
+          <t>8/14/2025</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>MONROE 3838</t>
+          <t>SUPERI 1459</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>804468442</t>
+          <t>808972965</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
@@ -1457,7 +1465,7 @@
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>Reparar rienda</t>
+          <t>Poste con base quebrada ver si es posible desmonte</t>
         </is>
       </c>
       <c r="I14" t="n">
@@ -1465,7 +1473,7 @@
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>Tensor</t>
+          <t>Desmonte</t>
         </is>
       </c>
       <c r="K14" t="inlineStr">
@@ -1475,14 +1483,14 @@
       </c>
       <c r="L14" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M14" t="n">
-        <v>-58.473659</v>
+        <v>-58.460834</v>
       </c>
       <c r="N14" t="n">
-        <v>-34.566979</v>
+        <v>-34.573753</v>
       </c>
       <c r="O14" t="inlineStr">
         <is>
@@ -1498,27 +1506,27 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>5464</t>
+          <t>6928</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>4/4/2025</t>
+          <t>8/12/2025</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>SUCRE, ANTONIO JOSE DE, MCAL. 3100</t>
+          <t>ALBARELLOS AV. 3101</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>804497880</t>
+          <t>808918710</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
@@ -1551,18 +1559,18 @@
       </c>
       <c r="L15" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M15" t="n">
-        <v>-58.46161</v>
+        <v>-58.512623</v>
       </c>
       <c r="N15" t="n">
-        <v>-34.567849</v>
+        <v>-34.579137</v>
       </c>
       <c r="O15" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P15" t="inlineStr">
@@ -1574,27 +1582,27 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>5469</t>
+          <t>6910</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>4/4/2025</t>
+          <t>8/12/2025</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>ESTADO PLURINACIONAL DE BOLIVIA 5899</t>
+          <t>RIVAS, GRAL. 2345</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>804497887</t>
+          <t>808918698</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
@@ -1609,7 +1617,7 @@
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>Aplomar</t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I16" t="n">
@@ -1617,7 +1625,7 @@
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K16" t="inlineStr">
@@ -1627,14 +1635,14 @@
       </c>
       <c r="L16" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M16" t="n">
-        <v>-58.507746</v>
+        <v>-58.482497</v>
       </c>
       <c r="N16" t="n">
-        <v>-34.574217</v>
+        <v>-34.598714</v>
       </c>
       <c r="O16" t="inlineStr">
         <is>
@@ -1650,17 +1658,17 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>5492</t>
+          <t>6906</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>4/4/2025</t>
+          <t>8/12/2025</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>ESTADO PLURINACIONAL DE BOLIVIA 5920</t>
+          <t>MOSCONI GENERAL AV. 3163</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
@@ -1670,7 +1678,7 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>804498035</t>
+          <t>808918685</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
@@ -1685,7 +1693,7 @@
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>aplomar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I17" t="n">
@@ -1693,7 +1701,7 @@
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K17" t="inlineStr">
@@ -1703,14 +1711,14 @@
       </c>
       <c r="L17" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M17" t="n">
-        <v>-58.50751</v>
+        <v>-58.505731</v>
       </c>
       <c r="N17" t="n">
-        <v>-34.574543</v>
+        <v>-34.588316</v>
       </c>
       <c r="O17" t="inlineStr">
         <is>
@@ -1726,27 +1734,27 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>5599</t>
+          <t>6579</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>4/15/2025</t>
+          <t>8/7/2025</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>ESTOMBA 4052</t>
+          <t>RIVADAVIA MARTIN, COMODORO 1350</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>804732246</t>
+          <t>808749184</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
@@ -1761,7 +1769,7 @@
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>Columna PRFV quedo inclinada (la hicieron como estomba 4056)</t>
+          <t>Poste inclinado</t>
         </is>
       </c>
       <c r="I18" t="n">
@@ -1774,19 +1782,19 @@
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>Nodo TLC</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L18" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M18" t="n">
-        <v>-58.485407</v>
+        <v>-58.461024</v>
       </c>
       <c r="N18" t="n">
-        <v>-34.552985</v>
+        <v>-34.539409</v>
       </c>
       <c r="O18" t="inlineStr">
         <is>
@@ -1802,27 +1810,27 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>5590</t>
+          <t>6538</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>4/15/2025</t>
+          <t>7/17/2025</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>O'HIGGINS 2441</t>
+          <t>Pedraza Manuela 4101</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>804732275</t>
+          <t>808400353</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
@@ -1837,7 +1845,7 @@
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t xml:space="preserve">Podrida en la base </t>
         </is>
       </c>
       <c r="I19" t="n">
@@ -1859,10 +1867,10 @@
         </is>
       </c>
       <c r="M19" t="n">
-        <v>-58.45573</v>
+        <v>-58.481569</v>
       </c>
       <c r="N19" t="n">
-        <v>-34.556576</v>
+        <v>-34.559853</v>
       </c>
       <c r="O19" t="inlineStr">
         <is>
@@ -1878,27 +1886,27 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>5624</t>
+          <t>6519</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>4/22/2025</t>
+          <t>7/28/2025</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>PINO, VIRREY DEL 3456</t>
+          <t>SALGUERO, JERONIMO 2874</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>804876043</t>
+          <t>808571977</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
@@ -1913,7 +1921,7 @@
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>Desmonte de poste</t>
+          <t>Reparar rienda</t>
         </is>
       </c>
       <c r="I20" t="n">
@@ -1921,7 +1929,7 @@
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>Desmonte</t>
+          <t>Tensor</t>
         </is>
       </c>
       <c r="K20" t="inlineStr">
@@ -1931,50 +1939,50 @@
       </c>
       <c r="L20" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M20" t="n">
-        <v>-58.464354</v>
+        <v>-58.407256</v>
       </c>
       <c r="N20" t="n">
-        <v>-34.572486</v>
+        <v>-34.578976</v>
       </c>
       <c r="O20" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P20" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>5656</t>
+          <t>6512</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>4/24/2025</t>
+          <t>7/28/2025</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>ECHEVERRIA 5893</t>
+          <t>GASCON 1195</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>804922184</t>
+          <t>808571975</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
@@ -1989,7 +1997,7 @@
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>Poste con base quebrada</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I21" t="n">
@@ -1997,7 +2005,7 @@
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>Desmonte</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K21" t="inlineStr">
@@ -2007,50 +2015,50 @@
       </c>
       <c r="L21" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M21" t="n">
-        <v>-58.489627</v>
+        <v>-58.423127</v>
       </c>
       <c r="N21" t="n">
-        <v>-34.583761</v>
+        <v>-34.596476</v>
       </c>
       <c r="O21" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P21" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>6173</t>
+          <t>6506</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>4/29/2025</t>
+          <t>7/10/2025</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>ARMENIA 2321</t>
+          <t>Ohiggins 1611</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>805507398</t>
+          <t>808148679</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
@@ -2065,7 +2073,7 @@
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>Picada volvio a entrar como caso 6325</t>
+          <t>Columna podrida en la base</t>
         </is>
       </c>
       <c r="I22" t="n">
@@ -2078,7 +2086,7 @@
       </c>
       <c r="K22" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L22" t="inlineStr">
@@ -2087,46 +2095,46 @@
         </is>
       </c>
       <c r="M22" t="n">
-        <v>-58.420549</v>
+        <v>-58.448993</v>
       </c>
       <c r="N22" t="n">
-        <v>-34.585103</v>
+        <v>-34.564383</v>
       </c>
       <c r="O22" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P22" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>5715</t>
+          <t>6484</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>5/1/2025</t>
+          <t>7/24/2025</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>CUENCA 4690</t>
+          <t>URIARTE 2396</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>805579094</t>
+          <t>808509373</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
@@ -2141,7 +2149,7 @@
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>Aplomar poste</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I23" t="n">
@@ -2149,7 +2157,7 @@
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K23" t="inlineStr">
@@ -2159,50 +2167,50 @@
       </c>
       <c r="L23" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M23" t="n">
-        <v>-58.506061</v>
+        <v>-58.423934</v>
       </c>
       <c r="N23" t="n">
-        <v>-34.588887</v>
+        <v>-34.581562</v>
       </c>
       <c r="O23" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P23" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>6333</t>
+          <t>6465</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>5/1/2025</t>
+          <t>8/28/2025</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>ORTEGA Y GASSET 1816</t>
+          <t>AGUIRRE 368</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>805655342</t>
+          <t>809268249</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
@@ -2239,10 +2247,10 @@
         </is>
       </c>
       <c r="M24" t="n">
-        <v>-58.432556</v>
+        <v>-58.434651</v>
       </c>
       <c r="N24" t="n">
-        <v>-34.570279</v>
+        <v>-34.598814</v>
       </c>
       <c r="O24" t="inlineStr">
         <is>
@@ -2258,27 +2266,27 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>232</t>
+          <t>6437</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>5/9/2025</t>
+          <t>7/17/2025</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Gorostiaga 2286</t>
+          <t>MILLER 4590</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>805791858</t>
+          <t>808400306</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
@@ -2293,7 +2301,7 @@
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Columna corroida</t>
         </is>
       </c>
       <c r="I25" t="n">
@@ -2315,46 +2323,46 @@
         </is>
       </c>
       <c r="M25" t="n">
-        <v>-58.441563</v>
+        <v>-58.495482</v>
       </c>
       <c r="N25" t="n">
-        <v>-34.569743</v>
+        <v>-34.552614</v>
       </c>
       <c r="O25" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P25" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>-404</t>
+          <t>6383</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>5/8/2025</t>
+          <t>7/8/2025</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Amenabar 3048</t>
+          <t>FALCON, RAMON L.,CNEL. 1411</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>805791896</t>
+          <t>808099320</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
@@ -2369,7 +2377,7 @@
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>Aplomar columna 114</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I26" t="n">
@@ -2377,7 +2385,7 @@
       </c>
       <c r="J26" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K26" t="inlineStr">
@@ -2391,46 +2399,46 @@
         </is>
       </c>
       <c r="M26" t="n">
-        <v>-58.46579</v>
+        <v>-58.448523</v>
       </c>
       <c r="N26" t="n">
-        <v>-34.555012</v>
+        <v>-34.62452</v>
       </c>
       <c r="O26" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P26" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>-406</t>
+          <t>6333</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>5/8/2025</t>
+          <t>5/1/2025</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Olof palme 4144</t>
+          <t>ORTEGA Y GASSET 1816</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>805791925</t>
+          <t>805655342</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
@@ -2445,7 +2453,7 @@
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>Tensar 2 riendas a pique columna 168</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I27" t="n">
@@ -2453,7 +2461,7 @@
       </c>
       <c r="J27" t="inlineStr">
         <is>
-          <t>Tensor</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K27" t="inlineStr">
@@ -2463,50 +2471,50 @@
       </c>
       <c r="L27" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M27" t="n">
-        <v>-58.488252</v>
+        <v>-58.432556</v>
       </c>
       <c r="N27" t="n">
-        <v>-34.553391</v>
+        <v>-34.570279</v>
       </c>
       <c r="O27" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P27" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>5826</t>
+          <t>6332</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>5/19/2025</t>
+          <t>7/3/2025</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>ALBARELLOS AV. 3180</t>
+          <t>ARAOZ 2560</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>806926466</t>
+          <t>807965818</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
@@ -2521,7 +2529,7 @@
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>Columna (metal) inclinada</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I28" t="n">
@@ -2529,7 +2537,7 @@
       </c>
       <c r="J28" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K28" t="inlineStr">
@@ -2539,50 +2547,50 @@
       </c>
       <c r="L28" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M28" t="n">
-        <v>-58.513552</v>
+        <v>-58.414507</v>
       </c>
       <c r="N28" t="n">
-        <v>-34.579829</v>
+        <v>-34.585377</v>
       </c>
       <c r="O28" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P28" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>6144</t>
+          <t>6308</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>6/11/2025</t>
+          <t>7/1/2025</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>TURIN 2990</t>
+          <t>Guayaquil 637</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>807458282</t>
+          <t>807896343</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
@@ -2619,46 +2627,46 @@
         </is>
       </c>
       <c r="M29" t="n">
-        <v>-58.480925</v>
+        <v>-58.437378</v>
       </c>
       <c r="N29" t="n">
-        <v>-34.585471</v>
+        <v>-34.62116</v>
       </c>
       <c r="O29" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P29" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>6143</t>
+          <t>6295</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>6/11/2025</t>
+          <t>6/30/2025</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>SOLANO LOPEZ, F., MARISCAL 2845</t>
+          <t>SOLER 6017</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>807458296</t>
+          <t>807851636</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
@@ -2695,36 +2703,36 @@
         </is>
       </c>
       <c r="M30" t="n">
-        <v>-58.495071</v>
+        <v>-58.436808</v>
       </c>
       <c r="N30" t="n">
-        <v>-34.593122</v>
+        <v>-34.577464</v>
       </c>
       <c r="O30" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P30" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>-478</t>
+          <t>6235</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>6/15/2025</t>
+          <t>6/24/2025</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Chivilcoy 4875</t>
+          <t>HUERGO 389</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
@@ -2734,7 +2742,7 @@
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>807508509</t>
+          <t>807763078</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
@@ -2749,7 +2757,7 @@
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>Poste podrido</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I31" t="n">
@@ -2767,40 +2775,40 @@
       </c>
       <c r="L31" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M31" t="n">
-        <v>-58.517389</v>
+        <v>-58.432722</v>
       </c>
       <c r="N31" t="n">
-        <v>-34.593541</v>
+        <v>-34.572371</v>
       </c>
       <c r="O31" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P31" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>6171</t>
+          <t>6231</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>6/18/2025</t>
+          <t>6/24/2025</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>CABELLO 3486</t>
+          <t>Ciudad de la Paz 275</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
@@ -2810,7 +2818,7 @@
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>807658640</t>
+          <t>807763070</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
@@ -2825,7 +2833,7 @@
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>Columna inclinada evaluar con inspector un corrimiento</t>
+          <t>Aplomar o cambiar</t>
         </is>
       </c>
       <c r="I32" t="n">
@@ -2843,14 +2851,14 @@
       </c>
       <c r="L32" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M32" t="n">
-        <v>-58.409579</v>
+        <v>-58.441049</v>
       </c>
       <c r="N32" t="n">
-        <v>-34.581134</v>
+        <v>-34.574625</v>
       </c>
       <c r="O32" t="inlineStr">
         <is>
@@ -2942,17 +2950,17 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>6231</t>
+          <t>6173</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>6/24/2025</t>
+          <t>4/29/2025</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Ciudad de la Paz 275</t>
+          <t>ARMENIA 2321</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
@@ -2962,7 +2970,7 @@
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>807763070</t>
+          <t>805507398</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
@@ -2977,7 +2985,7 @@
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>Aplomar o cambiar</t>
+          <t>Picada volvio a entrar como caso 6325</t>
         </is>
       </c>
       <c r="I34" t="n">
@@ -2995,14 +3003,14 @@
       </c>
       <c r="L34" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M34" t="n">
-        <v>-58.441049</v>
+        <v>-58.420549</v>
       </c>
       <c r="N34" t="n">
-        <v>-34.574625</v>
+        <v>-34.585103</v>
       </c>
       <c r="O34" t="inlineStr">
         <is>
@@ -3018,27 +3026,27 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>6235</t>
+          <t>6171</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>6/24/2025</t>
+          <t>6/18/2025</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>HUERGO 389</t>
+          <t>CABELLO 3486</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>807763078</t>
+          <t>807658640</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
@@ -3053,7 +3061,7 @@
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Columna inclinada evaluar con inspector un corrimiento</t>
         </is>
       </c>
       <c r="I35" t="n">
@@ -3075,10 +3083,10 @@
         </is>
       </c>
       <c r="M35" t="n">
-        <v>-58.432722</v>
+        <v>-58.409579</v>
       </c>
       <c r="N35" t="n">
-        <v>-34.572371</v>
+        <v>-34.581134</v>
       </c>
       <c r="O35" t="inlineStr">
         <is>
@@ -3094,27 +3102,27 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>6295</t>
+          <t>6144</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>6/30/2025</t>
+          <t>6/11/2025</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>SOLER 6017</t>
+          <t>TURIN 2990</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>807851636</t>
+          <t>807458282</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
@@ -3151,46 +3159,46 @@
         </is>
       </c>
       <c r="M36" t="n">
-        <v>-58.436808</v>
+        <v>-58.480925</v>
       </c>
       <c r="N36" t="n">
-        <v>-34.577464</v>
+        <v>-34.585471</v>
       </c>
       <c r="O36" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P36" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>6308</t>
+          <t>6143</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>7/1/2025</t>
+          <t>6/11/2025</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Guayaquil 637</t>
+          <t>SOLANO LOPEZ, F., MARISCAL 2845</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>807896343</t>
+          <t>807458296</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
@@ -3227,46 +3235,46 @@
         </is>
       </c>
       <c r="M37" t="n">
-        <v>-58.437378</v>
+        <v>-58.495071</v>
       </c>
       <c r="N37" t="n">
-        <v>-34.62116</v>
+        <v>-34.593122</v>
       </c>
       <c r="O37" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P37" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>6332</t>
+          <t>6071</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>7/3/2025</t>
+          <t>3/17/2025</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>ARAOZ 2560</t>
+          <t>OSORIO 4994</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>807965818</t>
+          <t>804053324</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
@@ -3279,13 +3287,9 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H38" t="inlineStr">
-        <is>
-          <t>Picada</t>
-        </is>
-      </c>
+      <c r="H38" t="inlineStr"/>
       <c r="I38" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J38" t="inlineStr">
         <is>
@@ -3303,46 +3307,46 @@
         </is>
       </c>
       <c r="M38" t="n">
-        <v>-58.414507</v>
+        <v>-58.466241</v>
       </c>
       <c r="N38" t="n">
-        <v>-34.585377</v>
+        <v>-34.595741</v>
       </c>
       <c r="O38" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P38" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>6383</t>
+          <t>6036</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>7/8/2025</t>
+          <t>2/24/2025</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>FALCON, RAMON L.,CNEL. 1411</t>
+          <t>MEDRANO 1715</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>808099320</t>
+          <t>803608181</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
@@ -3355,13 +3359,9 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H39" t="inlineStr">
-        <is>
-          <t>Picada</t>
-        </is>
-      </c>
+      <c r="H39" t="inlineStr"/>
       <c r="I39" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J39" t="inlineStr">
         <is>
@@ -3370,7 +3370,7 @@
       </c>
       <c r="K39" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L39" t="inlineStr">
@@ -3379,14 +3379,14 @@
         </is>
       </c>
       <c r="M39" t="n">
-        <v>-58.448523</v>
+        <v>-58.418236</v>
       </c>
       <c r="N39" t="n">
-        <v>-34.62452</v>
+        <v>-34.589859</v>
       </c>
       <c r="O39" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P39" t="inlineStr">
@@ -3398,27 +3398,27 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>6506</t>
+          <t>-587</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>7/10/2025</t>
+          <t>9/8/2025</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Ohiggins 1611</t>
+          <t>ARIAS 4048</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>808148679</t>
+          <t>809526164</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
@@ -3433,7 +3433,7 @@
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t>Columna podrida en la base</t>
+          <t>Cambiar 114 picada</t>
         </is>
       </c>
       <c r="I40" t="n">
@@ -3446,7 +3446,7 @@
       </c>
       <c r="K40" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L40" t="inlineStr">
@@ -3455,14 +3455,14 @@
         </is>
       </c>
       <c r="M40" t="n">
-        <v>-58.448993</v>
+        <v>-58.488936</v>
       </c>
       <c r="N40" t="n">
-        <v>-34.564383</v>
+        <v>-34.549005</v>
       </c>
       <c r="O40" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P40" t="inlineStr">
@@ -3474,17 +3474,17 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>6437</t>
+          <t>5826</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>7/17/2025</t>
+          <t>5/19/2025</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>MILLER 4590</t>
+          <t>ALBARELLOS AV. 3180</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
@@ -3494,7 +3494,7 @@
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>808400306</t>
+          <t>806926466</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
@@ -3509,7 +3509,7 @@
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>Columna corroida</t>
+          <t>Columna (metal) inclinada</t>
         </is>
       </c>
       <c r="I41" t="n">
@@ -3517,7 +3517,7 @@
       </c>
       <c r="J41" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K41" t="inlineStr">
@@ -3527,18 +3527,18 @@
       </c>
       <c r="L41" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M41" t="n">
-        <v>-58.495482</v>
+        <v>-58.513552</v>
       </c>
       <c r="N41" t="n">
-        <v>-34.552614</v>
+        <v>-34.579829</v>
       </c>
       <c r="O41" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P41" t="inlineStr">
@@ -3550,27 +3550,27 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>6538</t>
+          <t>-579</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>7/17/2025</t>
+          <t>9/2/2025</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Pedraza Manuela 4101</t>
+          <t>Pedro Rivera 2546</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>808400353</t>
+          <t>ICD30612785</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
@@ -3585,7 +3585,7 @@
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t xml:space="preserve">Podrida en la base </t>
+          <t>Colocar R200 para pedir traspaso de equipos</t>
         </is>
       </c>
       <c r="I42" t="n">
@@ -3598,7 +3598,7 @@
       </c>
       <c r="K42" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L42" t="inlineStr">
@@ -3607,10 +3607,10 @@
         </is>
       </c>
       <c r="M42" t="n">
-        <v>-58.481569</v>
+        <v>-58.462479</v>
       </c>
       <c r="N42" t="n">
-        <v>-34.559853</v>
+        <v>-34.55765</v>
       </c>
       <c r="O42" t="inlineStr">
         <is>
@@ -3626,27 +3626,27 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>7023</t>
+          <t>-576</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>7/22/2025</t>
+          <t>8/29/2025</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>ZABALA 3573</t>
+          <t>Av. Boyacá 2030</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>808480549</t>
+          <t>809309606</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
@@ -3661,7 +3661,7 @@
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>Corroida en base para recambio entro tambien como caso 3575</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I43" t="n">
@@ -3683,14 +3683,14 @@
         </is>
       </c>
       <c r="M43" t="n">
-        <v>-58.457522</v>
+        <v>-58.471173</v>
       </c>
       <c r="N43" t="n">
-        <v>-34.579414</v>
+        <v>-34.60704</v>
       </c>
       <c r="O43" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P43" t="inlineStr">
@@ -3702,27 +3702,27 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>6484</t>
+          <t>-575</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>7/24/2025</t>
+          <t>8/28/2025</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>URIARTE 2396</t>
+          <t>Amenabar 3064</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>808509373</t>
+          <t>809281299</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
@@ -3759,46 +3759,46 @@
         </is>
       </c>
       <c r="M44" t="n">
-        <v>-58.423934</v>
+        <v>-58.465984</v>
       </c>
       <c r="N44" t="n">
-        <v>-34.581562</v>
+        <v>-34.554869</v>
       </c>
       <c r="O44" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P44" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>6512</t>
+          <t>5715</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>7/28/2025</t>
+          <t>5/1/2025</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>GASCON 1195</t>
+          <t>CUENCA 4690</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>808571975</t>
+          <t>805579094</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
@@ -3813,7 +3813,7 @@
       </c>
       <c r="H45" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Aplomar poste</t>
         </is>
       </c>
       <c r="I45" t="n">
@@ -3821,7 +3821,7 @@
       </c>
       <c r="J45" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K45" t="inlineStr">
@@ -3831,50 +3831,50 @@
       </c>
       <c r="L45" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M45" t="n">
-        <v>-58.423127</v>
+        <v>-58.506061</v>
       </c>
       <c r="N45" t="n">
-        <v>-34.596476</v>
+        <v>-34.588887</v>
       </c>
       <c r="O45" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P45" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>6519</t>
+          <t>-569</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>7/28/2025</t>
+          <t>8/27/2025</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>SALGUERO, JERONIMO 2874</t>
+          <t>Palpa 2862</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>808571977</t>
+          <t>809257759</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
@@ -3889,7 +3889,7 @@
       </c>
       <c r="H46" t="inlineStr">
         <is>
-          <t>Reparar rienda</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I46" t="n">
@@ -3897,7 +3897,7 @@
       </c>
       <c r="J46" t="inlineStr">
         <is>
-          <t>Tensor</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K46" t="inlineStr">
@@ -3907,50 +3907,50 @@
       </c>
       <c r="L46" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M46" t="n">
-        <v>-58.407256</v>
+        <v>-58.449512</v>
       </c>
       <c r="N46" t="n">
-        <v>-34.578976</v>
+        <v>-34.573404</v>
       </c>
       <c r="O46" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P46" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>-538</t>
+          <t>5656</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>7/31/2025</t>
+          <t>4/24/2025</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Malabia 964</t>
+          <t>ECHEVERRIA 5893</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>808609237</t>
+          <t>804922184</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
@@ -3965,7 +3965,7 @@
       </c>
       <c r="H47" t="inlineStr">
         <is>
-          <t>Cambiar poste mal estado por PRFV</t>
+          <t>Poste con base quebrada</t>
         </is>
       </c>
       <c r="I47" t="n">
@@ -3973,7 +3973,7 @@
       </c>
       <c r="J47" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Desmonte</t>
         </is>
       </c>
       <c r="K47" t="inlineStr">
@@ -3987,46 +3987,46 @@
         </is>
       </c>
       <c r="M47" t="n">
-        <v>-58.433634</v>
+        <v>-58.489627</v>
       </c>
       <c r="N47" t="n">
-        <v>-34.595018</v>
+        <v>-34.583761</v>
       </c>
       <c r="O47" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P47" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>-547</t>
+          <t>5624</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>8/6/2025</t>
+          <t>4/22/2025</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Habana 4210</t>
+          <t>PINO, VIRREY DEL 3456</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>808733921</t>
+          <t>804876043</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
@@ -4041,7 +4041,7 @@
       </c>
       <c r="H48" t="inlineStr">
         <is>
-          <t>Cambiar poste dañado</t>
+          <t>Desmonte de poste</t>
         </is>
       </c>
       <c r="I48" t="n">
@@ -4049,7 +4049,7 @@
       </c>
       <c r="J48" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Desmonte</t>
         </is>
       </c>
       <c r="K48" t="inlineStr">
@@ -4063,14 +4063,14 @@
         </is>
       </c>
       <c r="M48" t="n">
-        <v>-58.515873</v>
+        <v>-58.464354</v>
       </c>
       <c r="N48" t="n">
-        <v>-34.599425</v>
+        <v>-34.572486</v>
       </c>
       <c r="O48" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P48" t="inlineStr">
@@ -4082,27 +4082,27 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>6579</t>
+          <t>5599</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>8/7/2025</t>
+          <t>4/15/2025</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>RIVADAVIA MARTIN, COMODORO 1350</t>
+          <t>ESTOMBA 4052</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>808749184</t>
+          <t>804732246</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
@@ -4117,7 +4117,7 @@
       </c>
       <c r="H49" t="inlineStr">
         <is>
-          <t>Poste inclinado</t>
+          <t>Columna PRFV quedo inclinada (la hicieron como estomba 4056)</t>
         </is>
       </c>
       <c r="I49" t="n">
@@ -4130,19 +4130,19 @@
       </c>
       <c r="K49" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo TLC</t>
         </is>
       </c>
       <c r="L49" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M49" t="n">
-        <v>-58.461024</v>
+        <v>-58.485407</v>
       </c>
       <c r="N49" t="n">
-        <v>-34.539409</v>
+        <v>-34.552985</v>
       </c>
       <c r="O49" t="inlineStr">
         <is>
@@ -4158,27 +4158,27 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>6906</t>
+          <t>5590</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>8/12/2025</t>
+          <t>4/15/2025</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>MOSCONI GENERAL AV. 3163</t>
+          <t>O'HIGGINS 2441</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>808918685</t>
+          <t>804732275</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
@@ -4215,14 +4215,14 @@
         </is>
       </c>
       <c r="M50" t="n">
-        <v>-58.505731</v>
+        <v>-58.45573</v>
       </c>
       <c r="N50" t="n">
-        <v>-34.588316</v>
+        <v>-34.556576</v>
       </c>
       <c r="O50" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P50" t="inlineStr">
@@ -4234,27 +4234,27 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>6910</t>
+          <t>-559</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>8/12/2025</t>
+          <t>8/21/2025</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>RIVAS, GRAL. 2345</t>
+          <t>Av. Del Libertador 6736</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>808918698</t>
+          <t>809098713</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
@@ -4269,7 +4269,7 @@
       </c>
       <c r="H51" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I51" t="n">
@@ -4291,14 +4291,14 @@
         </is>
       </c>
       <c r="M51" t="n">
-        <v>-58.482497</v>
+        <v>-58.453398</v>
       </c>
       <c r="N51" t="n">
-        <v>-34.598714</v>
+        <v>-34.550238</v>
       </c>
       <c r="O51" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P51" t="inlineStr">
@@ -4310,27 +4310,27 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>6928</t>
+          <t>5589</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>8/12/2025</t>
+          <t>12/31/2023</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>ALBARELLOS AV. 3101</t>
+          <t>ARCOS 1520</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>808918710</t>
+          <t>799540526</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
@@ -4340,7 +4340,7 @@
       </c>
       <c r="G52" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H52" t="inlineStr">
@@ -4349,7 +4349,7 @@
         </is>
       </c>
       <c r="I52" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J52" t="inlineStr">
         <is>
@@ -4358,7 +4358,7 @@
       </c>
       <c r="K52" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L52" t="inlineStr">
@@ -4367,14 +4367,14 @@
         </is>
       </c>
       <c r="M52" t="n">
-        <v>-58.512623</v>
+        <v>-58.449125</v>
       </c>
       <c r="N52" t="n">
-        <v>-34.579137</v>
+        <v>-34.565958</v>
       </c>
       <c r="O52" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P52" t="inlineStr">
@@ -4386,27 +4386,27 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>-550</t>
+          <t>5503</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>8/12/2025</t>
+          <t>8/22/2025</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>Fitz roy 267</t>
+          <t>CRAMER AV. 1771</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>808918720</t>
+          <t>809102564</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
@@ -4421,7 +4421,7 @@
       </c>
       <c r="H53" t="inlineStr">
         <is>
-          <t>Aplomar columna</t>
+          <t>PIcada</t>
         </is>
       </c>
       <c r="I53" t="n">
@@ -4443,14 +4443,14 @@
         </is>
       </c>
       <c r="M53" t="n">
-        <v>-58.451378</v>
+        <v>-58.458506</v>
       </c>
       <c r="N53" t="n">
-        <v>-34.596195</v>
+        <v>-34.56783</v>
       </c>
       <c r="O53" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P53" t="inlineStr">
@@ -4462,27 +4462,27 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>6943</t>
+          <t>-550</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>8/14/2025</t>
+          <t>8/12/2025</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>SUPERI 1459</t>
+          <t>Fitz roy 267</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>808972965</t>
+          <t>808918720</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
@@ -4497,7 +4497,7 @@
       </c>
       <c r="H54" t="inlineStr">
         <is>
-          <t>Poste con base quebrada ver si es posible desmonte</t>
+          <t>Aplomar columna</t>
         </is>
       </c>
       <c r="I54" t="n">
@@ -4505,7 +4505,7 @@
       </c>
       <c r="J54" t="inlineStr">
         <is>
-          <t>Desmonte</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K54" t="inlineStr">
@@ -4515,18 +4515,18 @@
       </c>
       <c r="L54" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M54" t="n">
-        <v>-58.460834</v>
+        <v>-58.451378</v>
       </c>
       <c r="N54" t="n">
-        <v>-34.573753</v>
+        <v>-34.596195</v>
       </c>
       <c r="O54" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P54" t="inlineStr">
@@ -4538,27 +4538,27 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>6969</t>
+          <t>5492</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>8/14/2025</t>
+          <t>4/4/2025</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>CIUDAD DE LA PAZ 295</t>
+          <t>ESTADO PLURINACIONAL DE BOLIVIA 5920</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>808972995</t>
+          <t>804498035</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
@@ -4573,7 +4573,7 @@
       </c>
       <c r="H55" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>aplomar</t>
         </is>
       </c>
       <c r="I55" t="n">
@@ -4581,7 +4581,7 @@
       </c>
       <c r="J55" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K55" t="inlineStr">
@@ -4591,50 +4591,50 @@
       </c>
       <c r="L55" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M55" t="n">
-        <v>-58.441171</v>
+        <v>-58.50751</v>
       </c>
       <c r="N55" t="n">
-        <v>-34.574547</v>
+        <v>-34.574543</v>
       </c>
       <c r="O55" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P55" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>6971</t>
+          <t>-547</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>8/14/2025</t>
+          <t>8/6/2025</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>MAURE 1594</t>
+          <t>Habana 4210</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>808973001</t>
+          <t>808733921</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
@@ -4649,7 +4649,7 @@
       </c>
       <c r="H56" t="inlineStr">
         <is>
-          <t>Ver de traspasar a telecentro y  desmontar ver con inspector</t>
+          <t>Cambiar poste dañado</t>
         </is>
       </c>
       <c r="I56" t="n">
@@ -4667,50 +4667,50 @@
       </c>
       <c r="L56" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M56" t="n">
-        <v>-58.435072</v>
+        <v>-58.515873</v>
       </c>
       <c r="N56" t="n">
-        <v>-34.565732</v>
+        <v>-34.599425</v>
       </c>
       <c r="O56" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P56" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>7000</t>
+          <t>5469</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>8/20/2025</t>
+          <t>4/4/2025</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>SCALABRINI ORTIZ, RAUL AV. 2106</t>
+          <t>ESTADO PLURINACIONAL DE BOLIVIA 5899</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>809065867</t>
+          <t>804497887</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
@@ -4725,7 +4725,7 @@
       </c>
       <c r="H57" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Aplomar</t>
         </is>
       </c>
       <c r="I57" t="n">
@@ -4733,7 +4733,7 @@
       </c>
       <c r="J57" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K57" t="inlineStr">
@@ -4743,50 +4743,50 @@
       </c>
       <c r="L57" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M57" t="n">
-        <v>-58.420109</v>
+        <v>-58.507746</v>
       </c>
       <c r="N57" t="n">
-        <v>-34.58764</v>
+        <v>-34.574217</v>
       </c>
       <c r="O57" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P57" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>7003</t>
+          <t>5464</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>8/20/2025</t>
+          <t>4/4/2025</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>MELIAN AV. 2576</t>
+          <t>SUCRE, ANTONIO JOSE DE, MCAL. 3100</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>809065874</t>
+          <t>804497880</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
@@ -4819,14 +4819,14 @@
       </c>
       <c r="L58" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M58" t="n">
-        <v>-58.471943</v>
+        <v>-58.46161</v>
       </c>
       <c r="N58" t="n">
-        <v>-34.564948</v>
+        <v>-34.567849</v>
       </c>
       <c r="O58" t="inlineStr">
         <is>
@@ -4842,27 +4842,27 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>-559</t>
+          <t>-538</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>8/21/2025</t>
+          <t>7/31/2025</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>Av. Del Libertador 6736</t>
+          <t>Malabia 964</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>809098713</t>
+          <t>808609237</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
@@ -4877,7 +4877,7 @@
       </c>
       <c r="H59" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambiar poste mal estado por PRFV</t>
         </is>
       </c>
       <c r="I59" t="n">
@@ -4895,40 +4895,40 @@
       </c>
       <c r="L59" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M59" t="n">
-        <v>-58.453398</v>
+        <v>-58.433634</v>
       </c>
       <c r="N59" t="n">
-        <v>-34.550238</v>
+        <v>-34.595018</v>
       </c>
       <c r="O59" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P59" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>5503</t>
+          <t>5053</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>8/22/2025</t>
+          <t>3/11/2025</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>CRAMER AV. 1771</t>
+          <t>MENDOZA 1153</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
@@ -4938,7 +4938,7 @@
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>809102564</t>
+          <t>803969314</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
@@ -4953,11 +4953,11 @@
       </c>
       <c r="H60" t="inlineStr">
         <is>
-          <t>PIcada</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="I60" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J60" t="inlineStr">
         <is>
@@ -4971,18 +4971,18 @@
       </c>
       <c r="L60" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M60" t="n">
-        <v>-58.458506</v>
+        <v>-58.44463</v>
       </c>
       <c r="N60" t="n">
-        <v>-34.56783</v>
+        <v>-34.553354</v>
       </c>
       <c r="O60" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P60" t="inlineStr">
@@ -4994,27 +4994,27 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>7098</t>
+          <t>4862</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>8/25/2025</t>
+          <t>1/23/2025</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>UGARTE, MANUEL 3484</t>
+          <t>ARCOS 2263</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>809126236</t>
+          <t>802857379</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
@@ -5024,16 +5024,16 @@
       </c>
       <c r="G61" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H61" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>picada</t>
         </is>
       </c>
       <c r="I61" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J61" t="inlineStr">
         <is>
@@ -5042,7 +5042,7 @@
       </c>
       <c r="K61" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L61" t="inlineStr">
@@ -5051,14 +5051,14 @@
         </is>
       </c>
       <c r="M61" t="n">
-        <v>-58.472869</v>
+        <v>-58.455082</v>
       </c>
       <c r="N61" t="n">
-        <v>-34.562</v>
+        <v>-34.558883</v>
       </c>
       <c r="O61" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P61" t="inlineStr">
@@ -5070,27 +5070,27 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>7080</t>
+          <t>-478</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>8/25/2025</t>
+          <t>6/15/2025</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>UGARTE, MANUEL 2196</t>
+          <t>Chivilcoy 4875</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>809125906</t>
+          <t>807508509</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
@@ -5105,7 +5105,7 @@
       </c>
       <c r="H62" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Poste podrido</t>
         </is>
       </c>
       <c r="I62" t="n">
@@ -5123,18 +5123,18 @@
       </c>
       <c r="L62" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M62" t="n">
-        <v>-58.459402</v>
+        <v>-58.517389</v>
       </c>
       <c r="N62" t="n">
-        <v>-34.555262</v>
+        <v>-34.593541</v>
       </c>
       <c r="O62" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P62" t="inlineStr">
@@ -5146,27 +5146,27 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>7021</t>
+          <t>4595</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>8/25/2025</t>
+          <t>1/15/2025</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>VERA 445</t>
+          <t>PAROISSIEN 1806</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>809155622</t>
+          <t>802747617</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
@@ -5181,7 +5181,7 @@
       </c>
       <c r="H63" t="inlineStr">
         <is>
-          <t>Correrla para sacarla del cantero</t>
+          <t>Aplomar</t>
         </is>
       </c>
       <c r="I63" t="n">
@@ -5189,7 +5189,7 @@
       </c>
       <c r="J63" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K63" t="inlineStr">
@@ -5199,50 +5199,50 @@
       </c>
       <c r="L63" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M63" t="n">
-        <v>-58.437181</v>
+        <v>-58.464172</v>
       </c>
       <c r="N63" t="n">
-        <v>-34.5995</v>
+        <v>-34.543845</v>
       </c>
       <c r="O63" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P63" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>-569</t>
+          <t>4528</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>8/27/2025</t>
+          <t>1/16/2025</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>Palpa 2862</t>
+          <t>BARCO CENTENERA DEL 545</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>809257759</t>
+          <t>802774521</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
@@ -5279,46 +5279,46 @@
         </is>
       </c>
       <c r="M64" t="n">
-        <v>-58.449512</v>
+        <v>-58.440625</v>
       </c>
       <c r="N64" t="n">
-        <v>-34.573404</v>
+        <v>-34.625499</v>
       </c>
       <c r="O64" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P64" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>6465</t>
+          <t>-406</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>8/28/2025</t>
+          <t>5/8/2025</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>AGUIRRE 368</t>
+          <t>Olof palme 4144</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>809268249</t>
+          <t>805791925</t>
         </is>
       </c>
       <c r="F65" t="inlineStr">
@@ -5333,7 +5333,7 @@
       </c>
       <c r="H65" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Tensar 2 riendas a pique columna 168</t>
         </is>
       </c>
       <c r="I65" t="n">
@@ -5341,7 +5341,7 @@
       </c>
       <c r="J65" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Tensor</t>
         </is>
       </c>
       <c r="K65" t="inlineStr">
@@ -5351,50 +5351,50 @@
       </c>
       <c r="L65" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M65" t="n">
-        <v>-58.434651</v>
+        <v>-58.488252</v>
       </c>
       <c r="N65" t="n">
-        <v>-34.598814</v>
+        <v>-34.553391</v>
       </c>
       <c r="O65" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P65" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>7095</t>
+          <t>-404</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>8/28/2025</t>
+          <t>5/8/2025</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>SAN MARTIN AV. 4515</t>
+          <t>Amenabar 3048</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>809268240</t>
+          <t>805791896</t>
         </is>
       </c>
       <c r="F66" t="inlineStr">
@@ -5409,7 +5409,7 @@
       </c>
       <c r="H66" t="inlineStr">
         <is>
-          <t>Columna chocada</t>
+          <t>Aplomar columna 114</t>
         </is>
       </c>
       <c r="I66" t="n">
@@ -5417,7 +5417,7 @@
       </c>
       <c r="J66" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K66" t="inlineStr">
@@ -5427,18 +5427,18 @@
       </c>
       <c r="L66" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M66" t="n">
-        <v>-58.483415</v>
+        <v>-58.46579</v>
       </c>
       <c r="N66" t="n">
-        <v>-34.597663</v>
+        <v>-34.555012</v>
       </c>
       <c r="O66" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P66" t="inlineStr">
@@ -5450,17 +5450,17 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>-575</t>
+          <t>3839</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>8/28/2025</t>
+          <t>10/23/2024</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>Amenabar 3064</t>
+          <t>PICO 1511</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
@@ -5470,7 +5470,7 @@
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>809281299</t>
+          <t>798390296</t>
         </is>
       </c>
       <c r="F67" t="inlineStr">
@@ -5485,7 +5485,7 @@
       </c>
       <c r="H67" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Poste inclinado</t>
         </is>
       </c>
       <c r="I67" t="n">
@@ -5493,7 +5493,7 @@
       </c>
       <c r="J67" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K67" t="inlineStr">
@@ -5503,14 +5503,14 @@
       </c>
       <c r="L67" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M67" t="n">
-        <v>-58.465984</v>
+        <v>-58.465596</v>
       </c>
       <c r="N67" t="n">
-        <v>-34.554869</v>
+        <v>-34.53627</v>
       </c>
       <c r="O67" t="inlineStr">
         <is>
@@ -5526,27 +5526,27 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>-576</t>
+          <t>3430</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>8/29/2025</t>
+          <t>4/1/2025</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>Av. Boyacá 2030</t>
+          <t>MONROE 3838</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>809309606</t>
+          <t>804468442</t>
         </is>
       </c>
       <c r="F68" t="inlineStr">
@@ -5561,7 +5561,7 @@
       </c>
       <c r="H68" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Reparar rienda</t>
         </is>
       </c>
       <c r="I68" t="n">
@@ -5569,7 +5569,7 @@
       </c>
       <c r="J68" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Tensor</t>
         </is>
       </c>
       <c r="K68" t="inlineStr">
@@ -5579,18 +5579,18 @@
       </c>
       <c r="L68" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M68" t="n">
-        <v>-58.471173</v>
+        <v>-58.473659</v>
       </c>
       <c r="N68" t="n">
-        <v>-34.60704</v>
+        <v>-34.566979</v>
       </c>
       <c r="O68" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P68" t="inlineStr">
@@ -5602,17 +5602,17 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>7111</t>
+          <t>3348</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>9/1/2025</t>
+          <t>3/27/2025</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>VILELA 3699</t>
+          <t>ESTOMBA 2626</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
@@ -5622,7 +5622,7 @@
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>809371823</t>
+          <t>804309704</t>
         </is>
       </c>
       <c r="F69" t="inlineStr">
@@ -5637,7 +5637,7 @@
       </c>
       <c r="H69" t="inlineStr">
         <is>
-          <t xml:space="preserve">Cambiar </t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I69" t="n">
@@ -5645,7 +5645,7 @@
       </c>
       <c r="J69" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Desmonte</t>
         </is>
       </c>
       <c r="K69" t="inlineStr">
@@ -5655,18 +5655,18 @@
       </c>
       <c r="L69" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M69" t="n">
-        <v>-58.482817</v>
+        <v>-58.47538</v>
       </c>
       <c r="N69" t="n">
-        <v>-34.550845</v>
+        <v>-34.566015</v>
       </c>
       <c r="O69" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P69" t="inlineStr">
@@ -5678,17 +5678,17 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>7118</t>
+          <t>3299</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>9/2/2025</t>
+          <t>9/10/2024</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>CUBAS, JOSE 2211</t>
+          <t>DIAZ COLODRERO 3309</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
@@ -5698,7 +5698,7 @@
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>809406168</t>
+          <t>796186684</t>
         </is>
       </c>
       <c r="F70" t="inlineStr">
@@ -5708,12 +5708,12 @@
       </c>
       <c r="G70" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H70" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>qap traspaso nodo TLC y Teco</t>
         </is>
       </c>
       <c r="I70" t="n">
@@ -5726,7 +5726,7 @@
       </c>
       <c r="K70" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo TLC</t>
         </is>
       </c>
       <c r="L70" t="inlineStr">
@@ -5735,10 +5735,10 @@
         </is>
       </c>
       <c r="M70" t="n">
-        <v>-58.492448</v>
+        <v>-58.491722</v>
       </c>
       <c r="N70" t="n">
-        <v>-34.58372</v>
+        <v>-34.565845</v>
       </c>
       <c r="O70" t="inlineStr">
         <is>
@@ -5754,27 +5754,27 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>7211</t>
+          <t>-312</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>9/2/2025</t>
+          <t>3/29/2025</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>UGARTE, MANUEL 2318</t>
+          <t>MATIENZO BENJAMIN /ALT/ 1831</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>809406177</t>
+          <t>804333522</t>
         </is>
       </c>
       <c r="F71" t="inlineStr">
@@ -5789,11 +5789,11 @@
       </c>
       <c r="H71" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Retirar columna ya traspasaron el nodo</t>
         </is>
       </c>
       <c r="I71" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J71" t="inlineStr">
         <is>
@@ -5802,7 +5802,7 @@
       </c>
       <c r="K71" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L71" t="inlineStr">
@@ -5811,46 +5811,46 @@
         </is>
       </c>
       <c r="M71" t="n">
-        <v>-58.460635</v>
+        <v>-58.434835</v>
       </c>
       <c r="N71" t="n">
-        <v>-34.555932</v>
+        <v>-34.569129</v>
       </c>
       <c r="O71" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P71" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>7210</t>
+          <t>2485</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>9/2/2025</t>
+          <t>3/26/2025</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>RIVERA, PEDRO I., Dr. 2536</t>
+          <t>LA PLATA AV. 1095</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>809406189</t>
+          <t>804302893</t>
         </is>
       </c>
       <c r="F72" t="inlineStr">
@@ -5865,7 +5865,7 @@
       </c>
       <c r="H72" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Sacar ancla de rienda vieja y cementar vereda</t>
         </is>
       </c>
       <c r="I72" t="n">
@@ -5873,7 +5873,7 @@
       </c>
       <c r="J72" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Tensor</t>
         </is>
       </c>
       <c r="K72" t="inlineStr">
@@ -5883,50 +5883,50 @@
       </c>
       <c r="L72" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M72" t="n">
-        <v>-58.462327</v>
+        <v>-58.426593</v>
       </c>
       <c r="N72" t="n">
-        <v>-34.557565</v>
+        <v>-34.628211</v>
       </c>
       <c r="O72" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P72" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>-579</t>
+          <t>232</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>9/2/2025</t>
+          <t>5/9/2025</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>Pedro Rivera 2546</t>
+          <t>Gorostiaga 2286</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>ICD30612785</t>
+          <t>805791858</t>
         </is>
       </c>
       <c r="F73" t="inlineStr">
@@ -5941,7 +5941,7 @@
       </c>
       <c r="H73" t="inlineStr">
         <is>
-          <t>Colocar R200 para pedir traspaso de equipos</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I73" t="n">
@@ -5954,7 +5954,7 @@
       </c>
       <c r="K73" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L73" t="inlineStr">
@@ -5963,95 +5963,19 @@
         </is>
       </c>
       <c r="M73" t="n">
-        <v>-58.462479</v>
+        <v>-58.441563</v>
       </c>
       <c r="N73" t="n">
-        <v>-34.55765</v>
+        <v>-34.569743</v>
       </c>
       <c r="O73" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P73" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
-        </is>
-      </c>
-    </row>
-    <row r="74">
-      <c r="A74" t="inlineStr">
-        <is>
-          <t>-587</t>
-        </is>
-      </c>
-      <c r="B74" t="inlineStr">
-        <is>
-          <t>9/8/2025</t>
-        </is>
-      </c>
-      <c r="C74" t="inlineStr">
-        <is>
-          <t>ARIAS 4048</t>
-        </is>
-      </c>
-      <c r="D74" t="inlineStr">
-        <is>
-          <t>12</t>
-        </is>
-      </c>
-      <c r="E74" t="inlineStr">
-        <is>
-          <t>809526164</t>
-        </is>
-      </c>
-      <c r="F74" t="inlineStr">
-        <is>
-          <t>NEW</t>
-        </is>
-      </c>
-      <c r="G74" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H74" t="inlineStr">
-        <is>
-          <t>Cambiar 114 picada</t>
-        </is>
-      </c>
-      <c r="I74" t="n">
-        <v>1</v>
-      </c>
-      <c r="J74" t="inlineStr">
-        <is>
-          <t>Cambio</t>
-        </is>
-      </c>
-      <c r="K74" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L74" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
-      <c r="M74" t="n">
-        <v>-58.488936</v>
-      </c>
-      <c r="N74" t="n">
-        <v>-34.549005</v>
-      </c>
-      <c r="O74" t="inlineStr">
-        <is>
-          <t>Saavedra</t>
-        </is>
-      </c>
-      <c r="P74" t="inlineStr">
-        <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-09-15 11:59:37)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_NEW.xlsx
+++ b/mapa_interactivo_NEW.xlsx
@@ -518,27 +518,27 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>7211</t>
+          <t>3299</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>9/2/2025</t>
+          <t>9/10/2024</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>UGARTE, MANUEL 2318</t>
+          <t>DIAZ COLODRERO 3309</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>809406177</t>
+          <t>796186684</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -548,12 +548,12 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>qap traspaso nodo TLC y Teco</t>
         </is>
       </c>
       <c r="I2" t="n">
@@ -566,7 +566,7 @@
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo TLC</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
@@ -575,14 +575,14 @@
         </is>
       </c>
       <c r="M2" t="n">
-        <v>-58.460635</v>
+        <v>-58.491722</v>
       </c>
       <c r="N2" t="n">
-        <v>-34.555932</v>
+        <v>-34.565845</v>
       </c>
       <c r="O2" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P2" t="inlineStr">
@@ -594,17 +594,17 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>7210</t>
+          <t>3839</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>9/2/2025</t>
+          <t>10/23/2024</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>RIVERA, PEDRO I., Dr. 2536</t>
+          <t>PICO 1511</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -614,7 +614,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>809406189</t>
+          <t>798390296</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -629,7 +629,7 @@
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Poste inclinado</t>
         </is>
       </c>
       <c r="I3" t="n">
@@ -637,7 +637,7 @@
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
@@ -647,14 +647,14 @@
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M3" t="n">
-        <v>-58.462327</v>
+        <v>-58.465596</v>
       </c>
       <c r="N3" t="n">
-        <v>-34.557565</v>
+        <v>-34.53627</v>
       </c>
       <c r="O3" t="inlineStr">
         <is>
@@ -670,27 +670,27 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>7118</t>
+          <t>5589</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>9/2/2025</t>
+          <t>12/31/2023</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>CUBAS, JOSE 2211</t>
+          <t>ARCOS 1520</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>809406168</t>
+          <t>799540526</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -700,7 +700,7 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
@@ -709,7 +709,7 @@
         </is>
       </c>
       <c r="I4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J4" t="inlineStr">
         <is>
@@ -718,7 +718,7 @@
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
@@ -727,14 +727,14 @@
         </is>
       </c>
       <c r="M4" t="n">
-        <v>-58.492448</v>
+        <v>-58.449125</v>
       </c>
       <c r="N4" t="n">
-        <v>-34.58372</v>
+        <v>-34.565958</v>
       </c>
       <c r="O4" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P4" t="inlineStr">
@@ -746,27 +746,27 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>7111</t>
+          <t>4595</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>9/1/2025</t>
+          <t>1/15/2025</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>VILELA 3699</t>
+          <t>PAROISSIEN 1806</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>809371823</t>
+          <t>802747617</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -781,7 +781,7 @@
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t xml:space="preserve">Cambiar </t>
+          <t>Aplomar</t>
         </is>
       </c>
       <c r="I5" t="n">
@@ -789,7 +789,7 @@
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
@@ -803,10 +803,10 @@
         </is>
       </c>
       <c r="M5" t="n">
-        <v>-58.482817</v>
+        <v>-58.464172</v>
       </c>
       <c r="N5" t="n">
-        <v>-34.550845</v>
+        <v>-34.543845</v>
       </c>
       <c r="O5" t="inlineStr">
         <is>
@@ -822,27 +822,27 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>7098</t>
+          <t>4528</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>8/25/2025</t>
+          <t>1/16/2025</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>UGARTE, MANUEL 3484</t>
+          <t>BARCO CENTENERA DEL 545</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>809126236</t>
+          <t>802774521</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -879,46 +879,46 @@
         </is>
       </c>
       <c r="M6" t="n">
-        <v>-58.472869</v>
+        <v>-58.440625</v>
       </c>
       <c r="N6" t="n">
-        <v>-34.562</v>
+        <v>-34.625499</v>
       </c>
       <c r="O6" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P6" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>7095</t>
+          <t>4862</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>8/28/2025</t>
+          <t>1/23/2025</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>SAN MARTIN AV. 4515</t>
+          <t>ARCOS 2263</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>809268240</t>
+          <t>802857379</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -928,16 +928,16 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>Columna chocada</t>
+          <t>picada</t>
         </is>
       </c>
       <c r="I7" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J7" t="inlineStr">
         <is>
@@ -946,23 +946,23 @@
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M7" t="n">
-        <v>-58.483415</v>
+        <v>-58.455082</v>
       </c>
       <c r="N7" t="n">
-        <v>-34.597663</v>
+        <v>-34.558883</v>
       </c>
       <c r="O7" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P7" t="inlineStr">
@@ -974,27 +974,27 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>7080</t>
+          <t>6036</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>8/25/2025</t>
+          <t>2/24/2025</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>UGARTE, MANUEL 2196</t>
+          <t>MEDRANO 1715</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>809125906</t>
+          <t>803608181</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -1007,13 +1007,9 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H8" t="inlineStr">
-        <is>
-          <t>Picada</t>
-        </is>
-      </c>
+      <c r="H8" t="inlineStr"/>
       <c r="I8" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J8" t="inlineStr">
         <is>
@@ -1022,7 +1018,7 @@
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L8" t="inlineStr">
@@ -1031,46 +1027,46 @@
         </is>
       </c>
       <c r="M8" t="n">
-        <v>-58.459402</v>
+        <v>-58.418236</v>
       </c>
       <c r="N8" t="n">
-        <v>-34.555262</v>
+        <v>-34.589859</v>
       </c>
       <c r="O8" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P8" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>7023</t>
+          <t>5053</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>7/22/2025</t>
+          <t>3/11/2025</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>ZABALA 3573</t>
+          <t>MENDOZA 1153</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>808480549</t>
+          <t>803969314</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -1085,11 +1081,11 @@
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>Corroida en base para recambio entro tambien como caso 3575</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="I9" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J9" t="inlineStr">
         <is>
@@ -1103,18 +1099,18 @@
       </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M9" t="n">
-        <v>-58.457522</v>
+        <v>-58.44463</v>
       </c>
       <c r="N9" t="n">
-        <v>-34.579414</v>
+        <v>-34.553354</v>
       </c>
       <c r="O9" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P9" t="inlineStr">
@@ -1126,17 +1122,17 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>7021</t>
+          <t>6071</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>8/25/2025</t>
+          <t>3/17/2025</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>VERA 445</t>
+          <t>OSORIO 4994</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -1146,7 +1142,7 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>809155622</t>
+          <t>804053324</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
@@ -1159,13 +1155,9 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H10" t="inlineStr">
-        <is>
-          <t>Correrla para sacarla del cantero</t>
-        </is>
-      </c>
+      <c r="H10" t="inlineStr"/>
       <c r="I10" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J10" t="inlineStr">
         <is>
@@ -1183,46 +1175,46 @@
         </is>
       </c>
       <c r="M10" t="n">
-        <v>-58.437181</v>
+        <v>-58.466241</v>
       </c>
       <c r="N10" t="n">
-        <v>-34.5995</v>
+        <v>-34.595741</v>
       </c>
       <c r="O10" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P10" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>7003</t>
+          <t>2485</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>8/20/2025</t>
+          <t>3/26/2025</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>MELIAN AV. 2576</t>
+          <t>LA PLATA AV. 1095</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>809065874</t>
+          <t>804302893</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
@@ -1237,7 +1229,7 @@
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Sacar ancla de rienda vieja y cementar vereda</t>
         </is>
       </c>
       <c r="I11" t="n">
@@ -1245,7 +1237,7 @@
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Tensor</t>
         </is>
       </c>
       <c r="K11" t="inlineStr">
@@ -1255,50 +1247,50 @@
       </c>
       <c r="L11" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M11" t="n">
-        <v>-58.471943</v>
+        <v>-58.426593</v>
       </c>
       <c r="N11" t="n">
-        <v>-34.564948</v>
+        <v>-34.628211</v>
       </c>
       <c r="O11" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P11" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>7000</t>
+          <t>3348</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>8/20/2025</t>
+          <t>3/27/2025</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>SCALABRINI ORTIZ, RAUL AV. 2106</t>
+          <t>ESTOMBA 2626</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>809065867</t>
+          <t>804309704</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
@@ -1321,7 +1313,7 @@
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Desmonte</t>
         </is>
       </c>
       <c r="K12" t="inlineStr">
@@ -1335,36 +1327,36 @@
         </is>
       </c>
       <c r="M12" t="n">
-        <v>-58.420109</v>
+        <v>-58.47538</v>
       </c>
       <c r="N12" t="n">
-        <v>-34.58764</v>
+        <v>-34.566015</v>
       </c>
       <c r="O12" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P12" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>6971</t>
+          <t>-312</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>8/14/2025</t>
+          <t>3/29/2025</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>MAURE 1594</t>
+          <t>MATIENZO BENJAMIN /ALT/ 1831</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -1374,7 +1366,7 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>ICD30754530</t>
+          <t>804333522</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
@@ -1389,11 +1381,11 @@
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>Desmontar columna</t>
+          <t>Retirar columna ya traspasaron el nodo</t>
         </is>
       </c>
       <c r="I13" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J13" t="inlineStr">
         <is>
@@ -1402,7 +1394,7 @@
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L13" t="inlineStr">
@@ -1411,10 +1403,10 @@
         </is>
       </c>
       <c r="M13" t="n">
-        <v>-58.435072</v>
+        <v>-58.434835</v>
       </c>
       <c r="N13" t="n">
-        <v>-34.565732</v>
+        <v>-34.569129</v>
       </c>
       <c r="O13" t="inlineStr">
         <is>
@@ -1430,27 +1422,27 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>6943</t>
+          <t>3430</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>8/14/2025</t>
+          <t>4/1/2025</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>SUPERI 1459</t>
+          <t>MONROE 3838</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>808972965</t>
+          <t>804468442</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
@@ -1465,7 +1457,7 @@
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>Poste con base quebrada ver si es posible desmonte</t>
+          <t>Reparar rienda</t>
         </is>
       </c>
       <c r="I14" t="n">
@@ -1473,7 +1465,7 @@
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>Desmonte</t>
+          <t>Tensor</t>
         </is>
       </c>
       <c r="K14" t="inlineStr">
@@ -1483,14 +1475,14 @@
       </c>
       <c r="L14" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M14" t="n">
-        <v>-58.460834</v>
+        <v>-58.473659</v>
       </c>
       <c r="N14" t="n">
-        <v>-34.573753</v>
+        <v>-34.566979</v>
       </c>
       <c r="O14" t="inlineStr">
         <is>
@@ -1506,27 +1498,27 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>6928</t>
+          <t>5464</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>8/12/2025</t>
+          <t>4/4/2025</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>ALBARELLOS AV. 3101</t>
+          <t>SUCRE, ANTONIO JOSE DE, MCAL. 3100</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>808918710</t>
+          <t>804497880</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
@@ -1559,18 +1551,18 @@
       </c>
       <c r="L15" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M15" t="n">
-        <v>-58.512623</v>
+        <v>-58.46161</v>
       </c>
       <c r="N15" t="n">
-        <v>-34.579137</v>
+        <v>-34.567849</v>
       </c>
       <c r="O15" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P15" t="inlineStr">
@@ -1582,27 +1574,27 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>6910</t>
+          <t>5469</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>8/12/2025</t>
+          <t>4/4/2025</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>RIVAS, GRAL. 2345</t>
+          <t>ESTADO PLURINACIONAL DE BOLIVIA 5899</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>808918698</t>
+          <t>804497887</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
@@ -1617,7 +1609,7 @@
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>Aplomar</t>
         </is>
       </c>
       <c r="I16" t="n">
@@ -1625,7 +1617,7 @@
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K16" t="inlineStr">
@@ -1635,14 +1627,14 @@
       </c>
       <c r="L16" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M16" t="n">
-        <v>-58.482497</v>
+        <v>-58.507746</v>
       </c>
       <c r="N16" t="n">
-        <v>-34.598714</v>
+        <v>-34.574217</v>
       </c>
       <c r="O16" t="inlineStr">
         <is>
@@ -1658,17 +1650,17 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>6906</t>
+          <t>5492</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>8/12/2025</t>
+          <t>4/4/2025</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>MOSCONI GENERAL AV. 3163</t>
+          <t>ESTADO PLURINACIONAL DE BOLIVIA 5920</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
@@ -1678,7 +1670,7 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>808918685</t>
+          <t>804498035</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
@@ -1693,7 +1685,7 @@
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>aplomar</t>
         </is>
       </c>
       <c r="I17" t="n">
@@ -1701,7 +1693,7 @@
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K17" t="inlineStr">
@@ -1711,14 +1703,14 @@
       </c>
       <c r="L17" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M17" t="n">
-        <v>-58.505731</v>
+        <v>-58.50751</v>
       </c>
       <c r="N17" t="n">
-        <v>-34.588316</v>
+        <v>-34.574543</v>
       </c>
       <c r="O17" t="inlineStr">
         <is>
@@ -1734,27 +1726,27 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>6579</t>
+          <t>5599</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>8/7/2025</t>
+          <t>4/15/2025</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>RIVADAVIA MARTIN, COMODORO 1350</t>
+          <t>ESTOMBA 4052</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>808749184</t>
+          <t>804732246</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
@@ -1769,7 +1761,7 @@
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>Poste inclinado</t>
+          <t>Columna PRFV quedo inclinada (la hicieron como estomba 4056)</t>
         </is>
       </c>
       <c r="I18" t="n">
@@ -1782,19 +1774,19 @@
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo TLC</t>
         </is>
       </c>
       <c r="L18" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M18" t="n">
-        <v>-58.461024</v>
+        <v>-58.485407</v>
       </c>
       <c r="N18" t="n">
-        <v>-34.539409</v>
+        <v>-34.552985</v>
       </c>
       <c r="O18" t="inlineStr">
         <is>
@@ -1810,27 +1802,27 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>6538</t>
+          <t>5590</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>7/17/2025</t>
+          <t>4/15/2025</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Pedraza Manuela 4101</t>
+          <t>O'HIGGINS 2441</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>808400353</t>
+          <t>804732275</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
@@ -1845,7 +1837,7 @@
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t xml:space="preserve">Podrida en la base </t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I19" t="n">
@@ -1867,10 +1859,10 @@
         </is>
       </c>
       <c r="M19" t="n">
-        <v>-58.481569</v>
+        <v>-58.45573</v>
       </c>
       <c r="N19" t="n">
-        <v>-34.559853</v>
+        <v>-34.556576</v>
       </c>
       <c r="O19" t="inlineStr">
         <is>
@@ -1886,27 +1878,27 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>6519</t>
+          <t>5624</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>7/28/2025</t>
+          <t>4/22/2025</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>SALGUERO, JERONIMO 2874</t>
+          <t>PINO, VIRREY DEL 3456</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>808571977</t>
+          <t>804876043</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
@@ -1921,7 +1913,7 @@
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>Reparar rienda</t>
+          <t>Desmonte de poste</t>
         </is>
       </c>
       <c r="I20" t="n">
@@ -1929,7 +1921,7 @@
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>Tensor</t>
+          <t>Desmonte</t>
         </is>
       </c>
       <c r="K20" t="inlineStr">
@@ -1939,50 +1931,50 @@
       </c>
       <c r="L20" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M20" t="n">
-        <v>-58.407256</v>
+        <v>-58.464354</v>
       </c>
       <c r="N20" t="n">
-        <v>-34.578976</v>
+        <v>-34.572486</v>
       </c>
       <c r="O20" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P20" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>6512</t>
+          <t>5656</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>7/28/2025</t>
+          <t>4/24/2025</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>GASCON 1195</t>
+          <t>ECHEVERRIA 5893</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>808571975</t>
+          <t>804922184</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
@@ -1997,7 +1989,7 @@
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Poste con base quebrada</t>
         </is>
       </c>
       <c r="I21" t="n">
@@ -2005,7 +1997,7 @@
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Desmonte</t>
         </is>
       </c>
       <c r="K21" t="inlineStr">
@@ -2015,50 +2007,50 @@
       </c>
       <c r="L21" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M21" t="n">
-        <v>-58.423127</v>
+        <v>-58.489627</v>
       </c>
       <c r="N21" t="n">
-        <v>-34.596476</v>
+        <v>-34.583761</v>
       </c>
       <c r="O21" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P21" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>6506</t>
+          <t>6173</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>7/10/2025</t>
+          <t>4/29/2025</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Ohiggins 1611</t>
+          <t>ARMENIA 2321</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>808148679</t>
+          <t>805507398</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
@@ -2073,7 +2065,7 @@
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>Columna podrida en la base</t>
+          <t>Picada volvio a entrar como caso 6325</t>
         </is>
       </c>
       <c r="I22" t="n">
@@ -2086,7 +2078,7 @@
       </c>
       <c r="K22" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L22" t="inlineStr">
@@ -2095,46 +2087,46 @@
         </is>
       </c>
       <c r="M22" t="n">
-        <v>-58.448993</v>
+        <v>-58.420549</v>
       </c>
       <c r="N22" t="n">
-        <v>-34.564383</v>
+        <v>-34.585103</v>
       </c>
       <c r="O22" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P22" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>6484</t>
+          <t>5715</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>7/24/2025</t>
+          <t>5/1/2025</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>URIARTE 2396</t>
+          <t>CUENCA 4690</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>808509373</t>
+          <t>805579094</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
@@ -2149,7 +2141,7 @@
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Aplomar poste</t>
         </is>
       </c>
       <c r="I23" t="n">
@@ -2157,7 +2149,7 @@
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K23" t="inlineStr">
@@ -2167,50 +2159,50 @@
       </c>
       <c r="L23" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M23" t="n">
-        <v>-58.423934</v>
+        <v>-58.506061</v>
       </c>
       <c r="N23" t="n">
-        <v>-34.581562</v>
+        <v>-34.588887</v>
       </c>
       <c r="O23" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P23" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>6465</t>
+          <t>6333</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>8/28/2025</t>
+          <t>5/1/2025</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>AGUIRRE 368</t>
+          <t>ORTEGA Y GASSET 1816</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>809268249</t>
+          <t>805655342</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
@@ -2247,10 +2239,10 @@
         </is>
       </c>
       <c r="M24" t="n">
-        <v>-58.434651</v>
+        <v>-58.432556</v>
       </c>
       <c r="N24" t="n">
-        <v>-34.598814</v>
+        <v>-34.570279</v>
       </c>
       <c r="O24" t="inlineStr">
         <is>
@@ -2266,27 +2258,27 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>6437</t>
+          <t>232</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>7/17/2025</t>
+          <t>5/9/2025</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>MILLER 4590</t>
+          <t>Gorostiaga 2286</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>808400306</t>
+          <t>805791858</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
@@ -2301,7 +2293,7 @@
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>Columna corroida</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I25" t="n">
@@ -2323,46 +2315,46 @@
         </is>
       </c>
       <c r="M25" t="n">
-        <v>-58.495482</v>
+        <v>-58.441563</v>
       </c>
       <c r="N25" t="n">
-        <v>-34.552614</v>
+        <v>-34.569743</v>
       </c>
       <c r="O25" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P25" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>6383</t>
+          <t>-404</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>7/8/2025</t>
+          <t>5/8/2025</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>FALCON, RAMON L.,CNEL. 1411</t>
+          <t>Amenabar 3048</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>808099320</t>
+          <t>805791896</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
@@ -2377,7 +2369,7 @@
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Aplomar columna 114</t>
         </is>
       </c>
       <c r="I26" t="n">
@@ -2385,7 +2377,7 @@
       </c>
       <c r="J26" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K26" t="inlineStr">
@@ -2399,46 +2391,46 @@
         </is>
       </c>
       <c r="M26" t="n">
-        <v>-58.448523</v>
+        <v>-58.46579</v>
       </c>
       <c r="N26" t="n">
-        <v>-34.62452</v>
+        <v>-34.555012</v>
       </c>
       <c r="O26" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P26" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>6333</t>
+          <t>-406</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>5/1/2025</t>
+          <t>5/8/2025</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>ORTEGA Y GASSET 1816</t>
+          <t>Olof palme 4144</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>805655342</t>
+          <t>805791925</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
@@ -2453,7 +2445,7 @@
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Tensar 2 riendas a pique columna 168</t>
         </is>
       </c>
       <c r="I27" t="n">
@@ -2461,7 +2453,7 @@
       </c>
       <c r="J27" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Tensor</t>
         </is>
       </c>
       <c r="K27" t="inlineStr">
@@ -2471,50 +2463,50 @@
       </c>
       <c r="L27" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M27" t="n">
-        <v>-58.432556</v>
+        <v>-58.488252</v>
       </c>
       <c r="N27" t="n">
-        <v>-34.570279</v>
+        <v>-34.553391</v>
       </c>
       <c r="O27" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P27" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>6332</t>
+          <t>5826</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>7/3/2025</t>
+          <t>5/19/2025</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>ARAOZ 2560</t>
+          <t>ALBARELLOS AV. 3180</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>807965818</t>
+          <t>806926466</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
@@ -2529,7 +2521,7 @@
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Columna (metal) inclinada</t>
         </is>
       </c>
       <c r="I28" t="n">
@@ -2537,7 +2529,7 @@
       </c>
       <c r="J28" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K28" t="inlineStr">
@@ -2547,50 +2539,50 @@
       </c>
       <c r="L28" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M28" t="n">
-        <v>-58.414507</v>
+        <v>-58.513552</v>
       </c>
       <c r="N28" t="n">
-        <v>-34.585377</v>
+        <v>-34.579829</v>
       </c>
       <c r="O28" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P28" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>6308</t>
+          <t>6144</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>7/1/2025</t>
+          <t>6/11/2025</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Guayaquil 637</t>
+          <t>TURIN 2990</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>807896343</t>
+          <t>807458282</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
@@ -2627,46 +2619,46 @@
         </is>
       </c>
       <c r="M29" t="n">
-        <v>-58.437378</v>
+        <v>-58.480925</v>
       </c>
       <c r="N29" t="n">
-        <v>-34.62116</v>
+        <v>-34.585471</v>
       </c>
       <c r="O29" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P29" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>6295</t>
+          <t>6143</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>6/30/2025</t>
+          <t>6/11/2025</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>SOLER 6017</t>
+          <t>SOLANO LOPEZ, F., MARISCAL 2845</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>807851636</t>
+          <t>807458296</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
@@ -2703,36 +2695,36 @@
         </is>
       </c>
       <c r="M30" t="n">
-        <v>-58.436808</v>
+        <v>-58.495071</v>
       </c>
       <c r="N30" t="n">
-        <v>-34.577464</v>
+        <v>-34.593122</v>
       </c>
       <c r="O30" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P30" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>6235</t>
+          <t>-478</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>6/24/2025</t>
+          <t>6/15/2025</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>HUERGO 389</t>
+          <t>Chivilcoy 4875</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
@@ -2742,7 +2734,7 @@
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>807763078</t>
+          <t>807508509</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
@@ -2757,7 +2749,7 @@
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Poste podrido</t>
         </is>
       </c>
       <c r="I31" t="n">
@@ -2775,40 +2767,40 @@
       </c>
       <c r="L31" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M31" t="n">
-        <v>-58.432722</v>
+        <v>-58.517389</v>
       </c>
       <c r="N31" t="n">
-        <v>-34.572371</v>
+        <v>-34.593541</v>
       </c>
       <c r="O31" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P31" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>6231</t>
+          <t>6171</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>6/24/2025</t>
+          <t>6/18/2025</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Ciudad de la Paz 275</t>
+          <t>CABELLO 3486</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
@@ -2818,7 +2810,7 @@
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>807763070</t>
+          <t>807658640</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
@@ -2833,7 +2825,7 @@
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>Aplomar o cambiar</t>
+          <t>Columna inclinada evaluar con inspector un corrimiento</t>
         </is>
       </c>
       <c r="I32" t="n">
@@ -2851,14 +2843,14 @@
       </c>
       <c r="L32" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M32" t="n">
-        <v>-58.441049</v>
+        <v>-58.409579</v>
       </c>
       <c r="N32" t="n">
-        <v>-34.574625</v>
+        <v>-34.581134</v>
       </c>
       <c r="O32" t="inlineStr">
         <is>
@@ -2950,17 +2942,17 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>6173</t>
+          <t>6231</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>4/29/2025</t>
+          <t>6/24/2025</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>ARMENIA 2321</t>
+          <t>Ciudad de la Paz 275</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
@@ -2970,7 +2962,7 @@
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>805507398</t>
+          <t>807763070</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
@@ -2985,7 +2977,7 @@
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>Picada volvio a entrar como caso 6325</t>
+          <t>Aplomar o cambiar</t>
         </is>
       </c>
       <c r="I34" t="n">
@@ -3003,14 +2995,14 @@
       </c>
       <c r="L34" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M34" t="n">
-        <v>-58.420549</v>
+        <v>-58.441049</v>
       </c>
       <c r="N34" t="n">
-        <v>-34.585103</v>
+        <v>-34.574625</v>
       </c>
       <c r="O34" t="inlineStr">
         <is>
@@ -3026,27 +3018,27 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>6171</t>
+          <t>6235</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>6/18/2025</t>
+          <t>6/24/2025</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>CABELLO 3486</t>
+          <t>HUERGO 389</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>807658640</t>
+          <t>807763078</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
@@ -3061,7 +3053,7 @@
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>Columna inclinada evaluar con inspector un corrimiento</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I35" t="n">
@@ -3083,10 +3075,10 @@
         </is>
       </c>
       <c r="M35" t="n">
-        <v>-58.409579</v>
+        <v>-58.432722</v>
       </c>
       <c r="N35" t="n">
-        <v>-34.581134</v>
+        <v>-34.572371</v>
       </c>
       <c r="O35" t="inlineStr">
         <is>
@@ -3102,27 +3094,27 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>6144</t>
+          <t>6295</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>6/11/2025</t>
+          <t>6/30/2025</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>TURIN 2990</t>
+          <t>SOLER 6017</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>807458282</t>
+          <t>807851636</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
@@ -3159,46 +3151,46 @@
         </is>
       </c>
       <c r="M36" t="n">
-        <v>-58.480925</v>
+        <v>-58.436808</v>
       </c>
       <c r="N36" t="n">
-        <v>-34.585471</v>
+        <v>-34.577464</v>
       </c>
       <c r="O36" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P36" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>6143</t>
+          <t>6308</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>6/11/2025</t>
+          <t>7/1/2025</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>SOLANO LOPEZ, F., MARISCAL 2845</t>
+          <t>Guayaquil 637</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>807458296</t>
+          <t>807896343</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
@@ -3235,46 +3227,46 @@
         </is>
       </c>
       <c r="M37" t="n">
-        <v>-58.495071</v>
+        <v>-58.437378</v>
       </c>
       <c r="N37" t="n">
-        <v>-34.593122</v>
+        <v>-34.62116</v>
       </c>
       <c r="O37" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P37" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>6071</t>
+          <t>6332</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>3/17/2025</t>
+          <t>7/3/2025</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>OSORIO 4994</t>
+          <t>ARAOZ 2560</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>804053324</t>
+          <t>807965818</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
@@ -3287,9 +3279,13 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H38" t="inlineStr"/>
+      <c r="H38" t="inlineStr">
+        <is>
+          <t>Picada</t>
+        </is>
+      </c>
       <c r="I38" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J38" t="inlineStr">
         <is>
@@ -3307,46 +3303,46 @@
         </is>
       </c>
       <c r="M38" t="n">
-        <v>-58.466241</v>
+        <v>-58.414507</v>
       </c>
       <c r="N38" t="n">
-        <v>-34.595741</v>
+        <v>-34.585377</v>
       </c>
       <c r="O38" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P38" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>6036</t>
+          <t>6383</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>2/24/2025</t>
+          <t>7/8/2025</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>MEDRANO 1715</t>
+          <t>FALCON, RAMON L.,CNEL. 1411</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>803608181</t>
+          <t>808099320</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
@@ -3359,9 +3355,13 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H39" t="inlineStr"/>
+      <c r="H39" t="inlineStr">
+        <is>
+          <t>Picada</t>
+        </is>
+      </c>
       <c r="I39" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J39" t="inlineStr">
         <is>
@@ -3370,7 +3370,7 @@
       </c>
       <c r="K39" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L39" t="inlineStr">
@@ -3379,14 +3379,14 @@
         </is>
       </c>
       <c r="M39" t="n">
-        <v>-58.418236</v>
+        <v>-58.448523</v>
       </c>
       <c r="N39" t="n">
-        <v>-34.589859</v>
+        <v>-34.62452</v>
       </c>
       <c r="O39" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P39" t="inlineStr">
@@ -3398,27 +3398,27 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>-587</t>
+          <t>6506</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>9/8/2025</t>
+          <t>7/10/2025</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>ARIAS 4048</t>
+          <t>Ohiggins 1611</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>809526164</t>
+          <t>808148679</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
@@ -3433,7 +3433,7 @@
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t>Cambiar 114 picada</t>
+          <t>Columna podrida en la base</t>
         </is>
       </c>
       <c r="I40" t="n">
@@ -3446,7 +3446,7 @@
       </c>
       <c r="K40" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L40" t="inlineStr">
@@ -3455,14 +3455,14 @@
         </is>
       </c>
       <c r="M40" t="n">
-        <v>-58.488936</v>
+        <v>-58.448993</v>
       </c>
       <c r="N40" t="n">
-        <v>-34.549005</v>
+        <v>-34.564383</v>
       </c>
       <c r="O40" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P40" t="inlineStr">
@@ -3474,17 +3474,17 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>5826</t>
+          <t>6437</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>5/19/2025</t>
+          <t>7/17/2025</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>ALBARELLOS AV. 3180</t>
+          <t>MILLER 4590</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
@@ -3494,7 +3494,7 @@
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>806926466</t>
+          <t>808400306</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
@@ -3509,7 +3509,7 @@
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>Columna (metal) inclinada</t>
+          <t>Columna corroida</t>
         </is>
       </c>
       <c r="I41" t="n">
@@ -3517,7 +3517,7 @@
       </c>
       <c r="J41" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K41" t="inlineStr">
@@ -3527,18 +3527,18 @@
       </c>
       <c r="L41" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M41" t="n">
-        <v>-58.513552</v>
+        <v>-58.495482</v>
       </c>
       <c r="N41" t="n">
-        <v>-34.579829</v>
+        <v>-34.552614</v>
       </c>
       <c r="O41" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P41" t="inlineStr">
@@ -3550,27 +3550,27 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>-579</t>
+          <t>6538</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>9/2/2025</t>
+          <t>7/17/2025</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Pedro Rivera 2546</t>
+          <t>Pedraza Manuela 4101</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>ICD30612785</t>
+          <t>808400353</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
@@ -3585,7 +3585,7 @@
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>Colocar R200 para pedir traspaso de equipos</t>
+          <t xml:space="preserve">Podrida en la base </t>
         </is>
       </c>
       <c r="I42" t="n">
@@ -3598,7 +3598,7 @@
       </c>
       <c r="K42" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L42" t="inlineStr">
@@ -3607,10 +3607,10 @@
         </is>
       </c>
       <c r="M42" t="n">
-        <v>-58.462479</v>
+        <v>-58.481569</v>
       </c>
       <c r="N42" t="n">
-        <v>-34.55765</v>
+        <v>-34.559853</v>
       </c>
       <c r="O42" t="inlineStr">
         <is>
@@ -3626,27 +3626,27 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>-576</t>
+          <t>7023</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>8/29/2025</t>
+          <t>7/22/2025</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Av. Boyacá 2030</t>
+          <t>ZABALA 3573</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>809309606</t>
+          <t>808480549</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
@@ -3661,7 +3661,7 @@
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Corroida en base para recambio entro tambien como caso 3575</t>
         </is>
       </c>
       <c r="I43" t="n">
@@ -3683,14 +3683,14 @@
         </is>
       </c>
       <c r="M43" t="n">
-        <v>-58.471173</v>
+        <v>-58.457522</v>
       </c>
       <c r="N43" t="n">
-        <v>-34.60704</v>
+        <v>-34.579414</v>
       </c>
       <c r="O43" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P43" t="inlineStr">
@@ -3702,27 +3702,27 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>-575</t>
+          <t>6484</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>8/28/2025</t>
+          <t>7/24/2025</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Amenabar 3064</t>
+          <t>URIARTE 2396</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>809281299</t>
+          <t>808509373</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
@@ -3759,46 +3759,46 @@
         </is>
       </c>
       <c r="M44" t="n">
-        <v>-58.465984</v>
+        <v>-58.423934</v>
       </c>
       <c r="N44" t="n">
-        <v>-34.554869</v>
+        <v>-34.581562</v>
       </c>
       <c r="O44" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P44" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>5715</t>
+          <t>6512</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>5/1/2025</t>
+          <t>7/28/2025</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>CUENCA 4690</t>
+          <t>GASCON 1195</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>805579094</t>
+          <t>808571975</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
@@ -3813,7 +3813,7 @@
       </c>
       <c r="H45" t="inlineStr">
         <is>
-          <t>Aplomar poste</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I45" t="n">
@@ -3821,7 +3821,7 @@
       </c>
       <c r="J45" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K45" t="inlineStr">
@@ -3831,50 +3831,50 @@
       </c>
       <c r="L45" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M45" t="n">
-        <v>-58.506061</v>
+        <v>-58.423127</v>
       </c>
       <c r="N45" t="n">
-        <v>-34.588887</v>
+        <v>-34.596476</v>
       </c>
       <c r="O45" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P45" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>-569</t>
+          <t>6519</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>8/27/2025</t>
+          <t>7/28/2025</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Palpa 2862</t>
+          <t>SALGUERO, JERONIMO 2874</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>809257759</t>
+          <t>808571977</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
@@ -3889,7 +3889,7 @@
       </c>
       <c r="H46" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Reparar rienda</t>
         </is>
       </c>
       <c r="I46" t="n">
@@ -3897,7 +3897,7 @@
       </c>
       <c r="J46" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Tensor</t>
         </is>
       </c>
       <c r="K46" t="inlineStr">
@@ -3907,50 +3907,50 @@
       </c>
       <c r="L46" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M46" t="n">
-        <v>-58.449512</v>
+        <v>-58.407256</v>
       </c>
       <c r="N46" t="n">
-        <v>-34.573404</v>
+        <v>-34.578976</v>
       </c>
       <c r="O46" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P46" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>5656</t>
+          <t>-538</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>4/24/2025</t>
+          <t>7/31/2025</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>ECHEVERRIA 5893</t>
+          <t>Malabia 964</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>804922184</t>
+          <t>808609237</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
@@ -3965,7 +3965,7 @@
       </c>
       <c r="H47" t="inlineStr">
         <is>
-          <t>Poste con base quebrada</t>
+          <t>Cambiar poste mal estado por PRFV</t>
         </is>
       </c>
       <c r="I47" t="n">
@@ -3973,7 +3973,7 @@
       </c>
       <c r="J47" t="inlineStr">
         <is>
-          <t>Desmonte</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K47" t="inlineStr">
@@ -3987,46 +3987,46 @@
         </is>
       </c>
       <c r="M47" t="n">
-        <v>-58.489627</v>
+        <v>-58.433634</v>
       </c>
       <c r="N47" t="n">
-        <v>-34.583761</v>
+        <v>-34.595018</v>
       </c>
       <c r="O47" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P47" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>5624</t>
+          <t>-547</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>4/22/2025</t>
+          <t>8/6/2025</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>PINO, VIRREY DEL 3456</t>
+          <t>Habana 4210</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>804876043</t>
+          <t>808733921</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
@@ -4041,7 +4041,7 @@
       </c>
       <c r="H48" t="inlineStr">
         <is>
-          <t>Desmonte de poste</t>
+          <t>Cambiar poste dañado</t>
         </is>
       </c>
       <c r="I48" t="n">
@@ -4049,7 +4049,7 @@
       </c>
       <c r="J48" t="inlineStr">
         <is>
-          <t>Desmonte</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K48" t="inlineStr">
@@ -4063,14 +4063,14 @@
         </is>
       </c>
       <c r="M48" t="n">
-        <v>-58.464354</v>
+        <v>-58.515873</v>
       </c>
       <c r="N48" t="n">
-        <v>-34.572486</v>
+        <v>-34.599425</v>
       </c>
       <c r="O48" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P48" t="inlineStr">
@@ -4082,17 +4082,17 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>5599</t>
+          <t>6906</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>4/15/2025</t>
+          <t>8/12/2025</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>ESTOMBA 4052</t>
+          <t>MOSCONI GENERAL AV. 3163</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
@@ -4102,7 +4102,7 @@
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>804732246</t>
+          <t>808918685</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
@@ -4117,7 +4117,7 @@
       </c>
       <c r="H49" t="inlineStr">
         <is>
-          <t>Columna PRFV quedo inclinada (la hicieron como estomba 4056)</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I49" t="n">
@@ -4125,12 +4125,12 @@
       </c>
       <c r="J49" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K49" t="inlineStr">
         <is>
-          <t>Nodo TLC</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L49" t="inlineStr">
@@ -4139,14 +4139,14 @@
         </is>
       </c>
       <c r="M49" t="n">
-        <v>-58.485407</v>
+        <v>-58.505731</v>
       </c>
       <c r="N49" t="n">
-        <v>-34.552985</v>
+        <v>-34.588316</v>
       </c>
       <c r="O49" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P49" t="inlineStr">
@@ -4158,27 +4158,27 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>5590</t>
+          <t>6910</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>4/15/2025</t>
+          <t>8/12/2025</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>O'HIGGINS 2441</t>
+          <t>RIVAS, GRAL. 2345</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>804732275</t>
+          <t>808918698</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
@@ -4193,7 +4193,7 @@
       </c>
       <c r="H50" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I50" t="n">
@@ -4215,14 +4215,14 @@
         </is>
       </c>
       <c r="M50" t="n">
-        <v>-58.45573</v>
+        <v>-58.482497</v>
       </c>
       <c r="N50" t="n">
-        <v>-34.556576</v>
+        <v>-34.598714</v>
       </c>
       <c r="O50" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P50" t="inlineStr">
@@ -4234,27 +4234,27 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>-559</t>
+          <t>6928</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>8/21/2025</t>
+          <t>8/12/2025</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Av. Del Libertador 6736</t>
+          <t>ALBARELLOS AV. 3101</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>809098713</t>
+          <t>808918710</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
@@ -4291,14 +4291,14 @@
         </is>
       </c>
       <c r="M51" t="n">
-        <v>-58.453398</v>
+        <v>-58.512623</v>
       </c>
       <c r="N51" t="n">
-        <v>-34.550238</v>
+        <v>-34.579137</v>
       </c>
       <c r="O51" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P51" t="inlineStr">
@@ -4310,27 +4310,27 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>5589</t>
+          <t>-550</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>12/31/2023</t>
+          <t>8/12/2025</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>ARCOS 1520</t>
+          <t>Fitz roy 267</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>799540526</t>
+          <t>808918720</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
@@ -4340,16 +4340,16 @@
       </c>
       <c r="G52" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
+          <t>Pendiente</t>
         </is>
       </c>
       <c r="H52" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Aplomar columna</t>
         </is>
       </c>
       <c r="I52" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J52" t="inlineStr">
         <is>
@@ -4358,7 +4358,7 @@
       </c>
       <c r="K52" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L52" t="inlineStr">
@@ -4367,14 +4367,14 @@
         </is>
       </c>
       <c r="M52" t="n">
-        <v>-58.449125</v>
+        <v>-58.451378</v>
       </c>
       <c r="N52" t="n">
-        <v>-34.565958</v>
+        <v>-34.596195</v>
       </c>
       <c r="O52" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P52" t="inlineStr">
@@ -4386,17 +4386,17 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>5503</t>
+          <t>6943</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>8/22/2025</t>
+          <t>8/14/2025</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>CRAMER AV. 1771</t>
+          <t>SUPERI 1459</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
@@ -4406,7 +4406,7 @@
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>809102564</t>
+          <t>808972965</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
@@ -4421,7 +4421,7 @@
       </c>
       <c r="H53" t="inlineStr">
         <is>
-          <t>PIcada</t>
+          <t>Poste con base quebrada ver si es posible desmonte</t>
         </is>
       </c>
       <c r="I53" t="n">
@@ -4429,7 +4429,7 @@
       </c>
       <c r="J53" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Desmonte</t>
         </is>
       </c>
       <c r="K53" t="inlineStr">
@@ -4439,14 +4439,14 @@
       </c>
       <c r="L53" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M53" t="n">
-        <v>-58.458506</v>
+        <v>-58.460834</v>
       </c>
       <c r="N53" t="n">
-        <v>-34.56783</v>
+        <v>-34.573753</v>
       </c>
       <c r="O53" t="inlineStr">
         <is>
@@ -4462,27 +4462,27 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>-550</t>
+          <t>6971</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>8/12/2025</t>
+          <t>8/14/2025</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>Fitz roy 267</t>
+          <t>MAURE 1594</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>808918720</t>
+          <t>ICD30754530</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
@@ -4497,7 +4497,7 @@
       </c>
       <c r="H54" t="inlineStr">
         <is>
-          <t>Aplomar columna</t>
+          <t>Desmontar columna</t>
         </is>
       </c>
       <c r="I54" t="n">
@@ -4519,46 +4519,46 @@
         </is>
       </c>
       <c r="M54" t="n">
-        <v>-58.451378</v>
+        <v>-58.435072</v>
       </c>
       <c r="N54" t="n">
-        <v>-34.596195</v>
+        <v>-34.565732</v>
       </c>
       <c r="O54" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P54" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>5492</t>
+          <t>7000</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>4/4/2025</t>
+          <t>8/20/2025</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>ESTADO PLURINACIONAL DE BOLIVIA 5920</t>
+          <t>SCALABRINI ORTIZ, RAUL AV. 2106</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>804498035</t>
+          <t>809065867</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
@@ -4573,7 +4573,7 @@
       </c>
       <c r="H55" t="inlineStr">
         <is>
-          <t>aplomar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I55" t="n">
@@ -4581,7 +4581,7 @@
       </c>
       <c r="J55" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K55" t="inlineStr">
@@ -4591,50 +4591,50 @@
       </c>
       <c r="L55" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M55" t="n">
-        <v>-58.50751</v>
+        <v>-58.420109</v>
       </c>
       <c r="N55" t="n">
-        <v>-34.574543</v>
+        <v>-34.58764</v>
       </c>
       <c r="O55" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P55" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>-547</t>
+          <t>7003</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>8/6/2025</t>
+          <t>8/20/2025</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>Habana 4210</t>
+          <t>MELIAN AV. 2576</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>808733921</t>
+          <t>809065874</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
@@ -4649,7 +4649,7 @@
       </c>
       <c r="H56" t="inlineStr">
         <is>
-          <t>Cambiar poste dañado</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I56" t="n">
@@ -4667,18 +4667,18 @@
       </c>
       <c r="L56" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M56" t="n">
-        <v>-58.515873</v>
+        <v>-58.471943</v>
       </c>
       <c r="N56" t="n">
-        <v>-34.599425</v>
+        <v>-34.564948</v>
       </c>
       <c r="O56" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P56" t="inlineStr">
@@ -4690,27 +4690,27 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>5469</t>
+          <t>-559</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>4/4/2025</t>
+          <t>8/21/2025</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>ESTADO PLURINACIONAL DE BOLIVIA 5899</t>
+          <t>Av. Del Libertador 6736</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>804497887</t>
+          <t>809098713</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
@@ -4725,7 +4725,7 @@
       </c>
       <c r="H57" t="inlineStr">
         <is>
-          <t>Aplomar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I57" t="n">
@@ -4733,7 +4733,7 @@
       </c>
       <c r="J57" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K57" t="inlineStr">
@@ -4743,18 +4743,18 @@
       </c>
       <c r="L57" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M57" t="n">
-        <v>-58.507746</v>
+        <v>-58.453398</v>
       </c>
       <c r="N57" t="n">
-        <v>-34.574217</v>
+        <v>-34.550238</v>
       </c>
       <c r="O57" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P57" t="inlineStr">
@@ -4766,17 +4766,17 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>5464</t>
+          <t>5503</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>4/4/2025</t>
+          <t>8/22/2025</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>SUCRE, ANTONIO JOSE DE, MCAL. 3100</t>
+          <t>CRAMER AV. 1771</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
@@ -4786,7 +4786,7 @@
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>804497880</t>
+          <t>809102564</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
@@ -4801,7 +4801,7 @@
       </c>
       <c r="H58" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>PIcada</t>
         </is>
       </c>
       <c r="I58" t="n">
@@ -4819,14 +4819,14 @@
       </c>
       <c r="L58" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M58" t="n">
-        <v>-58.46161</v>
+        <v>-58.458506</v>
       </c>
       <c r="N58" t="n">
-        <v>-34.567849</v>
+        <v>-34.56783</v>
       </c>
       <c r="O58" t="inlineStr">
         <is>
@@ -4842,27 +4842,27 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>-538</t>
+          <t>7098</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>7/31/2025</t>
+          <t>8/25/2025</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>Malabia 964</t>
+          <t>UGARTE, MANUEL 3484</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>808609237</t>
+          <t>809126236</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
@@ -4877,7 +4877,7 @@
       </c>
       <c r="H59" t="inlineStr">
         <is>
-          <t>Cambiar poste mal estado por PRFV</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I59" t="n">
@@ -4895,40 +4895,40 @@
       </c>
       <c r="L59" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M59" t="n">
-        <v>-58.433634</v>
+        <v>-58.472869</v>
       </c>
       <c r="N59" t="n">
-        <v>-34.595018</v>
+        <v>-34.562</v>
       </c>
       <c r="O59" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P59" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>5053</t>
+          <t>7080</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>3/11/2025</t>
+          <t>8/25/2025</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>MENDOZA 1153</t>
+          <t>UGARTE, MANUEL 2196</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
@@ -4938,7 +4938,7 @@
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>803969314</t>
+          <t>809125906</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
@@ -4953,11 +4953,11 @@
       </c>
       <c r="H60" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I60" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J60" t="inlineStr">
         <is>
@@ -4971,14 +4971,14 @@
       </c>
       <c r="L60" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M60" t="n">
-        <v>-58.44463</v>
+        <v>-58.459402</v>
       </c>
       <c r="N60" t="n">
-        <v>-34.553354</v>
+        <v>-34.555262</v>
       </c>
       <c r="O60" t="inlineStr">
         <is>
@@ -4994,27 +4994,27 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>4862</t>
+          <t>7021</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>1/23/2025</t>
+          <t>8/25/2025</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>ARCOS 2263</t>
+          <t>VERA 445</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>802857379</t>
+          <t>809155622</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
@@ -5024,16 +5024,16 @@
       </c>
       <c r="G61" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
+          <t>Pendiente</t>
         </is>
       </c>
       <c r="H61" t="inlineStr">
         <is>
-          <t>picada</t>
+          <t>Correrla para sacarla del cantero</t>
         </is>
       </c>
       <c r="I61" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J61" t="inlineStr">
         <is>
@@ -5042,7 +5042,7 @@
       </c>
       <c r="K61" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L61" t="inlineStr">
@@ -5051,46 +5051,46 @@
         </is>
       </c>
       <c r="M61" t="n">
-        <v>-58.455082</v>
+        <v>-58.437181</v>
       </c>
       <c r="N61" t="n">
-        <v>-34.558883</v>
+        <v>-34.5995</v>
       </c>
       <c r="O61" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P61" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>-478</t>
+          <t>-569</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>6/15/2025</t>
+          <t>8/27/2025</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>Chivilcoy 4875</t>
+          <t>Palpa 2862</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>807508509</t>
+          <t>809257759</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
@@ -5105,7 +5105,7 @@
       </c>
       <c r="H62" t="inlineStr">
         <is>
-          <t>Poste podrido</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I62" t="n">
@@ -5123,18 +5123,18 @@
       </c>
       <c r="L62" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M62" t="n">
-        <v>-58.517389</v>
+        <v>-58.449512</v>
       </c>
       <c r="N62" t="n">
-        <v>-34.593541</v>
+        <v>-34.573404</v>
       </c>
       <c r="O62" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P62" t="inlineStr">
@@ -5146,27 +5146,27 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>4595</t>
+          <t>6465</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>1/15/2025</t>
+          <t>8/28/2025</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>PAROISSIEN 1806</t>
+          <t>AGUIRRE 368</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>802747617</t>
+          <t>809268249</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
@@ -5181,7 +5181,7 @@
       </c>
       <c r="H63" t="inlineStr">
         <is>
-          <t>Aplomar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I63" t="n">
@@ -5189,7 +5189,7 @@
       </c>
       <c r="J63" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K63" t="inlineStr">
@@ -5199,50 +5199,50 @@
       </c>
       <c r="L63" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M63" t="n">
-        <v>-58.464172</v>
+        <v>-58.434651</v>
       </c>
       <c r="N63" t="n">
-        <v>-34.543845</v>
+        <v>-34.598814</v>
       </c>
       <c r="O63" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P63" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>4528</t>
+          <t>7095</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>1/16/2025</t>
+          <t>8/28/2025</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>BARCO CENTENERA DEL 545</t>
+          <t>SAN MARTIN AV. 4515</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>802774521</t>
+          <t>809268240</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
@@ -5257,7 +5257,7 @@
       </c>
       <c r="H64" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Columna chocada</t>
         </is>
       </c>
       <c r="I64" t="n">
@@ -5275,50 +5275,50 @@
       </c>
       <c r="L64" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M64" t="n">
-        <v>-58.440625</v>
+        <v>-58.483415</v>
       </c>
       <c r="N64" t="n">
-        <v>-34.625499</v>
+        <v>-34.597663</v>
       </c>
       <c r="O64" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P64" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>-406</t>
+          <t>-575</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>5/8/2025</t>
+          <t>8/28/2025</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>Olof palme 4144</t>
+          <t>Amenabar 3064</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>805791925</t>
+          <t>809281299</t>
         </is>
       </c>
       <c r="F65" t="inlineStr">
@@ -5333,7 +5333,7 @@
       </c>
       <c r="H65" t="inlineStr">
         <is>
-          <t>Tensar 2 riendas a pique columna 168</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I65" t="n">
@@ -5341,7 +5341,7 @@
       </c>
       <c r="J65" t="inlineStr">
         <is>
-          <t>Tensor</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K65" t="inlineStr">
@@ -5351,14 +5351,14 @@
       </c>
       <c r="L65" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M65" t="n">
-        <v>-58.488252</v>
+        <v>-58.465984</v>
       </c>
       <c r="N65" t="n">
-        <v>-34.553391</v>
+        <v>-34.554869</v>
       </c>
       <c r="O65" t="inlineStr">
         <is>
@@ -5374,27 +5374,27 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>-404</t>
+          <t>-576</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>5/8/2025</t>
+          <t>8/29/2025</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>Amenabar 3048</t>
+          <t>Av. Boyacá 2030</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>805791896</t>
+          <t>809309606</t>
         </is>
       </c>
       <c r="F66" t="inlineStr">
@@ -5409,7 +5409,7 @@
       </c>
       <c r="H66" t="inlineStr">
         <is>
-          <t>Aplomar columna 114</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I66" t="n">
@@ -5417,7 +5417,7 @@
       </c>
       <c r="J66" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K66" t="inlineStr">
@@ -5431,14 +5431,14 @@
         </is>
       </c>
       <c r="M66" t="n">
-        <v>-58.46579</v>
+        <v>-58.471173</v>
       </c>
       <c r="N66" t="n">
-        <v>-34.555012</v>
+        <v>-34.60704</v>
       </c>
       <c r="O66" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P66" t="inlineStr">
@@ -5450,27 +5450,27 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>3839</t>
+          <t>7111</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>10/23/2024</t>
+          <t>9/1/2025</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>PICO 1511</t>
+          <t>VILELA 3699</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>798390296</t>
+          <t>809371823</t>
         </is>
       </c>
       <c r="F67" t="inlineStr">
@@ -5485,7 +5485,7 @@
       </c>
       <c r="H67" t="inlineStr">
         <is>
-          <t>Poste inclinado</t>
+          <t xml:space="preserve">Cambiar </t>
         </is>
       </c>
       <c r="I67" t="n">
@@ -5493,7 +5493,7 @@
       </c>
       <c r="J67" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K67" t="inlineStr">
@@ -5503,14 +5503,14 @@
       </c>
       <c r="L67" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M67" t="n">
-        <v>-58.465596</v>
+        <v>-58.482817</v>
       </c>
       <c r="N67" t="n">
-        <v>-34.53627</v>
+        <v>-34.550845</v>
       </c>
       <c r="O67" t="inlineStr">
         <is>
@@ -5526,17 +5526,17 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>3430</t>
+          <t>7118</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>4/1/2025</t>
+          <t>9/2/2025</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>MONROE 3838</t>
+          <t>CUBAS, JOSE 2211</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
@@ -5546,7 +5546,7 @@
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>804468442</t>
+          <t>809406168</t>
         </is>
       </c>
       <c r="F68" t="inlineStr">
@@ -5561,7 +5561,7 @@
       </c>
       <c r="H68" t="inlineStr">
         <is>
-          <t>Reparar rienda</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I68" t="n">
@@ -5569,7 +5569,7 @@
       </c>
       <c r="J68" t="inlineStr">
         <is>
-          <t>Tensor</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K68" t="inlineStr">
@@ -5579,18 +5579,18 @@
       </c>
       <c r="L68" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M68" t="n">
-        <v>-58.473659</v>
+        <v>-58.492448</v>
       </c>
       <c r="N68" t="n">
-        <v>-34.566979</v>
+        <v>-34.58372</v>
       </c>
       <c r="O68" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P68" t="inlineStr">
@@ -5602,27 +5602,27 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>3348</t>
+          <t>7211</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>3/27/2025</t>
+          <t>9/2/2025</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>ESTOMBA 2626</t>
+          <t>UGARTE, MANUEL 2318</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>804309704</t>
+          <t>809406177</t>
         </is>
       </c>
       <c r="F69" t="inlineStr">
@@ -5645,7 +5645,7 @@
       </c>
       <c r="J69" t="inlineStr">
         <is>
-          <t>Desmonte</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K69" t="inlineStr">
@@ -5659,14 +5659,14 @@
         </is>
       </c>
       <c r="M69" t="n">
-        <v>-58.47538</v>
+        <v>-58.460635</v>
       </c>
       <c r="N69" t="n">
-        <v>-34.566015</v>
+        <v>-34.555932</v>
       </c>
       <c r="O69" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P69" t="inlineStr">
@@ -5678,27 +5678,27 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>3299</t>
+          <t>7210</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>9/10/2024</t>
+          <t>9/2/2025</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>DIAZ COLODRERO 3309</t>
+          <t>RIVERA, PEDRO I., Dr. 2536</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>796186684</t>
+          <t>809406189</t>
         </is>
       </c>
       <c r="F70" t="inlineStr">
@@ -5708,12 +5708,12 @@
       </c>
       <c r="G70" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
+          <t>Pendiente</t>
         </is>
       </c>
       <c r="H70" t="inlineStr">
         <is>
-          <t>qap traspaso nodo TLC y Teco</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I70" t="n">
@@ -5726,7 +5726,7 @@
       </c>
       <c r="K70" t="inlineStr">
         <is>
-          <t>Nodo TLC</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L70" t="inlineStr">
@@ -5735,14 +5735,14 @@
         </is>
       </c>
       <c r="M70" t="n">
-        <v>-58.491722</v>
+        <v>-58.462327</v>
       </c>
       <c r="N70" t="n">
-        <v>-34.565845</v>
+        <v>-34.557565</v>
       </c>
       <c r="O70" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P70" t="inlineStr">
@@ -5754,27 +5754,27 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>-312</t>
+          <t>-579</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>3/29/2025</t>
+          <t>9/2/2025</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>MATIENZO BENJAMIN /ALT/ 1831</t>
+          <t>Pedro Rivera 2546</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>804333522</t>
+          <t>ICD30612785</t>
         </is>
       </c>
       <c r="F71" t="inlineStr">
@@ -5789,11 +5789,11 @@
       </c>
       <c r="H71" t="inlineStr">
         <is>
-          <t>Retirar columna ya traspasaron el nodo</t>
+          <t>Colocar R200 para pedir traspaso de equipos</t>
         </is>
       </c>
       <c r="I71" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J71" t="inlineStr">
         <is>
@@ -5811,46 +5811,46 @@
         </is>
       </c>
       <c r="M71" t="n">
-        <v>-58.434835</v>
+        <v>-58.462479</v>
       </c>
       <c r="N71" t="n">
-        <v>-34.569129</v>
+        <v>-34.55765</v>
       </c>
       <c r="O71" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P71" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>2485</t>
+          <t>-587</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>3/26/2025</t>
+          <t>9/8/2025</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>LA PLATA AV. 1095</t>
+          <t>ARIAS 4048</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>804302893</t>
+          <t>809526164</t>
         </is>
       </c>
       <c r="F72" t="inlineStr">
@@ -5865,7 +5865,7 @@
       </c>
       <c r="H72" t="inlineStr">
         <is>
-          <t>Sacar ancla de rienda vieja y cementar vereda</t>
+          <t>Cambiar 114 picada</t>
         </is>
       </c>
       <c r="I72" t="n">
@@ -5873,7 +5873,7 @@
       </c>
       <c r="J72" t="inlineStr">
         <is>
-          <t>Tensor</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K72" t="inlineStr">
@@ -5883,50 +5883,50 @@
       </c>
       <c r="L72" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M72" t="n">
-        <v>-58.426593</v>
+        <v>-58.488936</v>
       </c>
       <c r="N72" t="n">
-        <v>-34.628211</v>
+        <v>-34.549005</v>
       </c>
       <c r="O72" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P72" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>232</t>
+          <t>7220</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>5/9/2025</t>
+          <t>9/15/2025</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>Gorostiaga 2286</t>
+          <t>GUTENBERG 2901</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>805791858</t>
+          <t>809758870</t>
         </is>
       </c>
       <c r="F73" t="inlineStr">
@@ -5941,7 +5941,7 @@
       </c>
       <c r="H73" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Columna inclinada</t>
         </is>
       </c>
       <c r="I73" t="n">
@@ -5959,23 +5959,23 @@
       </c>
       <c r="L73" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M73" t="n">
-        <v>-58.441563</v>
+        <v>-58.496084</v>
       </c>
       <c r="N73" t="n">
-        <v>-34.569743</v>
+        <v>-34.593316</v>
       </c>
       <c r="O73" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P73" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-09-15 12:07:42)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_NEW.xlsx
+++ b/mapa_interactivo_NEW.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P73"/>
+  <dimension ref="A1:P74"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2030,27 +2030,27 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>6173</t>
+          <t>5715</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>4/29/2025</t>
+          <t>5/1/2025</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>ARMENIA 2321</t>
+          <t>CUENCA 4690</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>805507398</t>
+          <t>805579094</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
@@ -2065,7 +2065,7 @@
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>Picada volvio a entrar como caso 6325</t>
+          <t>Aplomar poste</t>
         </is>
       </c>
       <c r="I22" t="n">
@@ -2073,7 +2073,7 @@
       </c>
       <c r="J22" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K22" t="inlineStr">
@@ -2083,30 +2083,30 @@
       </c>
       <c r="L22" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M22" t="n">
-        <v>-58.420549</v>
+        <v>-58.506061</v>
       </c>
       <c r="N22" t="n">
-        <v>-34.585103</v>
+        <v>-34.588887</v>
       </c>
       <c r="O22" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P22" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>5715</t>
+          <t>6333</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -2116,17 +2116,17 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>CUENCA 4690</t>
+          <t>ORTEGA Y GASSET 1816</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>805579094</t>
+          <t>805655342</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
@@ -2141,7 +2141,7 @@
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>Aplomar poste</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I23" t="n">
@@ -2149,7 +2149,7 @@
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K23" t="inlineStr">
@@ -2159,40 +2159,40 @@
       </c>
       <c r="L23" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M23" t="n">
-        <v>-58.506061</v>
+        <v>-58.432556</v>
       </c>
       <c r="N23" t="n">
-        <v>-34.588887</v>
+        <v>-34.570279</v>
       </c>
       <c r="O23" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P23" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>6333</t>
+          <t>232</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>5/1/2025</t>
+          <t>5/9/2025</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>ORTEGA Y GASSET 1816</t>
+          <t>Gorostiaga 2286</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
@@ -2202,7 +2202,7 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>805655342</t>
+          <t>805791858</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
@@ -2239,10 +2239,10 @@
         </is>
       </c>
       <c r="M24" t="n">
-        <v>-58.432556</v>
+        <v>-58.441563</v>
       </c>
       <c r="N24" t="n">
-        <v>-34.570279</v>
+        <v>-34.569743</v>
       </c>
       <c r="O24" t="inlineStr">
         <is>
@@ -2258,27 +2258,27 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>232</t>
+          <t>-404</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>5/9/2025</t>
+          <t>5/8/2025</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Gorostiaga 2286</t>
+          <t>Amenabar 3048</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>805791858</t>
+          <t>805791896</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
@@ -2293,7 +2293,7 @@
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Aplomar columna 114</t>
         </is>
       </c>
       <c r="I25" t="n">
@@ -2301,7 +2301,7 @@
       </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K25" t="inlineStr">
@@ -2315,26 +2315,26 @@
         </is>
       </c>
       <c r="M25" t="n">
-        <v>-58.441563</v>
+        <v>-58.46579</v>
       </c>
       <c r="N25" t="n">
-        <v>-34.569743</v>
+        <v>-34.555012</v>
       </c>
       <c r="O25" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P25" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>-404</t>
+          <t>-406</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -2344,17 +2344,17 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Amenabar 3048</t>
+          <t>Olof palme 4144</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>805791896</t>
+          <t>805791925</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
@@ -2369,7 +2369,7 @@
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>Aplomar columna 114</t>
+          <t>Tensar 2 riendas a pique columna 168</t>
         </is>
       </c>
       <c r="I26" t="n">
@@ -2377,7 +2377,7 @@
       </c>
       <c r="J26" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Tensor</t>
         </is>
       </c>
       <c r="K26" t="inlineStr">
@@ -2387,14 +2387,14 @@
       </c>
       <c r="L26" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M26" t="n">
-        <v>-58.46579</v>
+        <v>-58.488252</v>
       </c>
       <c r="N26" t="n">
-        <v>-34.555012</v>
+        <v>-34.553391</v>
       </c>
       <c r="O26" t="inlineStr">
         <is>
@@ -2410,17 +2410,17 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>-406</t>
+          <t>5826</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>5/8/2025</t>
+          <t>5/19/2025</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Olof palme 4144</t>
+          <t>ALBARELLOS AV. 3180</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
@@ -2430,7 +2430,7 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>805791925</t>
+          <t>806926466</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
@@ -2445,7 +2445,7 @@
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>Tensar 2 riendas a pique columna 168</t>
+          <t>Columna (metal) inclinada</t>
         </is>
       </c>
       <c r="I27" t="n">
@@ -2453,7 +2453,7 @@
       </c>
       <c r="J27" t="inlineStr">
         <is>
-          <t>Tensor</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K27" t="inlineStr">
@@ -2467,14 +2467,14 @@
         </is>
       </c>
       <c r="M27" t="n">
-        <v>-58.488252</v>
+        <v>-58.513552</v>
       </c>
       <c r="N27" t="n">
-        <v>-34.553391</v>
+        <v>-34.579829</v>
       </c>
       <c r="O27" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P27" t="inlineStr">
@@ -2486,27 +2486,27 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>5826</t>
+          <t>6144</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>5/19/2025</t>
+          <t>6/11/2025</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>ALBARELLOS AV. 3180</t>
+          <t>TURIN 2990</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>806926466</t>
+          <t>807458282</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
@@ -2521,7 +2521,7 @@
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>Columna (metal) inclinada</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I28" t="n">
@@ -2529,7 +2529,7 @@
       </c>
       <c r="J28" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K28" t="inlineStr">
@@ -2539,14 +2539,14 @@
       </c>
       <c r="L28" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M28" t="n">
-        <v>-58.513552</v>
+        <v>-58.480925</v>
       </c>
       <c r="N28" t="n">
-        <v>-34.579829</v>
+        <v>-34.585471</v>
       </c>
       <c r="O28" t="inlineStr">
         <is>
@@ -2562,7 +2562,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>6144</t>
+          <t>6143</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -2572,7 +2572,7 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>TURIN 2990</t>
+          <t>SOLANO LOPEZ, F., MARISCAL 2845</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
@@ -2582,7 +2582,7 @@
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>807458282</t>
+          <t>807458296</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
@@ -2619,10 +2619,10 @@
         </is>
       </c>
       <c r="M29" t="n">
-        <v>-58.480925</v>
+        <v>-58.495071</v>
       </c>
       <c r="N29" t="n">
-        <v>-34.585471</v>
+        <v>-34.593122</v>
       </c>
       <c r="O29" t="inlineStr">
         <is>
@@ -2638,27 +2638,27 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>6143</t>
+          <t>-478</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>6/11/2025</t>
+          <t>6/15/2025</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>SOLANO LOPEZ, F., MARISCAL 2845</t>
+          <t>Chivilcoy 4875</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>807458296</t>
+          <t>807508509</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
@@ -2673,7 +2673,7 @@
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Poste podrido</t>
         </is>
       </c>
       <c r="I30" t="n">
@@ -2691,14 +2691,14 @@
       </c>
       <c r="L30" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M30" t="n">
-        <v>-58.495071</v>
+        <v>-58.517389</v>
       </c>
       <c r="N30" t="n">
-        <v>-34.593122</v>
+        <v>-34.593541</v>
       </c>
       <c r="O30" t="inlineStr">
         <is>
@@ -2714,27 +2714,27 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>-478</t>
+          <t>6171</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>6/15/2025</t>
+          <t>6/18/2025</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Chivilcoy 4875</t>
+          <t>CABELLO 3486</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>807508509</t>
+          <t>807658640</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
@@ -2749,7 +2749,7 @@
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>Poste podrido</t>
+          <t>Columna inclinada evaluar con inspector un corrimiento</t>
         </is>
       </c>
       <c r="I31" t="n">
@@ -2767,50 +2767,50 @@
       </c>
       <c r="L31" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M31" t="n">
-        <v>-58.517389</v>
+        <v>-58.409579</v>
       </c>
       <c r="N31" t="n">
-        <v>-34.593541</v>
+        <v>-34.581134</v>
       </c>
       <c r="O31" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P31" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>6171</t>
+          <t>6229</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>6/18/2025</t>
+          <t>6/24/2025</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>CABELLO 3486</t>
+          <t>ALVAREZ THOMAS AV. 309</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>807658640</t>
+          <t>807762987</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
@@ -2825,7 +2825,7 @@
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>Columna inclinada evaluar con inspector un corrimiento</t>
+          <t xml:space="preserve">Reparar rienda </t>
         </is>
       </c>
       <c r="I32" t="n">
@@ -2833,7 +2833,7 @@
       </c>
       <c r="J32" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Tensor</t>
         </is>
       </c>
       <c r="K32" t="inlineStr">
@@ -2843,14 +2843,14 @@
       </c>
       <c r="L32" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M32" t="n">
-        <v>-58.409579</v>
+        <v>-58.44848</v>
       </c>
       <c r="N32" t="n">
-        <v>-34.581134</v>
+        <v>-34.581338</v>
       </c>
       <c r="O32" t="inlineStr">
         <is>
@@ -2866,7 +2866,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>6230</t>
+          <t>6228</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -2876,17 +2876,17 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Santa maria de oro	2722</t>
+          <t>NEWBERY, JORGE AV. 3416</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>807763066</t>
+          <t>807762990</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
@@ -2901,7 +2901,7 @@
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Reparar rienda</t>
         </is>
       </c>
       <c r="I33" t="n">
@@ -2909,7 +2909,7 @@
       </c>
       <c r="J33" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Tensor</t>
         </is>
       </c>
       <c r="K33" t="inlineStr">
@@ -2919,30 +2919,30 @@
       </c>
       <c r="L33" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M33" t="n">
-        <v>-58.422315</v>
+        <v>-58.448496</v>
       </c>
       <c r="N33" t="n">
-        <v>-34.576988</v>
+        <v>-34.58182</v>
       </c>
       <c r="O33" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P33" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>6231</t>
+          <t>6230</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
@@ -2952,7 +2952,7 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Ciudad de la Paz 275</t>
+          <t>Santa maria de oro	2722</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
@@ -2962,7 +2962,7 @@
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>807763070</t>
+          <t>807763066</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
@@ -2977,7 +2977,7 @@
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>Aplomar o cambiar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I34" t="n">
@@ -2995,14 +2995,14 @@
       </c>
       <c r="L34" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M34" t="n">
-        <v>-58.441049</v>
+        <v>-58.422315</v>
       </c>
       <c r="N34" t="n">
-        <v>-34.574625</v>
+        <v>-34.576988</v>
       </c>
       <c r="O34" t="inlineStr">
         <is>
@@ -3018,7 +3018,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>6235</t>
+          <t>6231</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
@@ -3028,17 +3028,17 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>HUERGO 389</t>
+          <t>Ciudad de la Paz 275</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>807763078</t>
+          <t>807763070</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
@@ -3053,7 +3053,7 @@
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Aplomar o cambiar</t>
         </is>
       </c>
       <c r="I35" t="n">
@@ -3071,14 +3071,14 @@
       </c>
       <c r="L35" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M35" t="n">
-        <v>-58.432722</v>
+        <v>-58.441049</v>
       </c>
       <c r="N35" t="n">
-        <v>-34.572371</v>
+        <v>-34.574625</v>
       </c>
       <c r="O35" t="inlineStr">
         <is>
@@ -3094,27 +3094,27 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>6295</t>
+          <t>6235</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>6/30/2025</t>
+          <t>6/24/2025</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>SOLER 6017</t>
+          <t>HUERGO 389</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>807851636</t>
+          <t>807763078</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
@@ -3151,10 +3151,10 @@
         </is>
       </c>
       <c r="M36" t="n">
-        <v>-58.436808</v>
+        <v>-58.432722</v>
       </c>
       <c r="N36" t="n">
-        <v>-34.577464</v>
+        <v>-34.572371</v>
       </c>
       <c r="O36" t="inlineStr">
         <is>
@@ -3170,27 +3170,27 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>6308</t>
+          <t>6295</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>7/1/2025</t>
+          <t>6/30/2025</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Guayaquil 637</t>
+          <t>SOLER 6017</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>807896343</t>
+          <t>807851636</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
@@ -3227,14 +3227,14 @@
         </is>
       </c>
       <c r="M37" t="n">
-        <v>-58.437378</v>
+        <v>-58.436808</v>
       </c>
       <c r="N37" t="n">
-        <v>-34.62116</v>
+        <v>-34.577464</v>
       </c>
       <c r="O37" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P37" t="inlineStr">
@@ -3246,27 +3246,27 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>6332</t>
+          <t>6308</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>7/3/2025</t>
+          <t>7/1/2025</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>ARAOZ 2560</t>
+          <t>Guayaquil 637</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>807965818</t>
+          <t>807896343</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
@@ -3303,14 +3303,14 @@
         </is>
       </c>
       <c r="M38" t="n">
-        <v>-58.414507</v>
+        <v>-58.437378</v>
       </c>
       <c r="N38" t="n">
-        <v>-34.585377</v>
+        <v>-34.62116</v>
       </c>
       <c r="O38" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P38" t="inlineStr">
@@ -3322,27 +3322,27 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>6383</t>
+          <t>6332</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>7/8/2025</t>
+          <t>7/3/2025</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>FALCON, RAMON L.,CNEL. 1411</t>
+          <t>ARAOZ 2560</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>808099320</t>
+          <t>807965818</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
@@ -3379,14 +3379,14 @@
         </is>
       </c>
       <c r="M39" t="n">
-        <v>-58.448523</v>
+        <v>-58.414507</v>
       </c>
       <c r="N39" t="n">
-        <v>-34.62452</v>
+        <v>-34.585377</v>
       </c>
       <c r="O39" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P39" t="inlineStr">
@@ -3398,27 +3398,27 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>6506</t>
+          <t>6383</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>7/10/2025</t>
+          <t>7/8/2025</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Ohiggins 1611</t>
+          <t>FALCON, RAMON L.,CNEL. 1411</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>808148679</t>
+          <t>808099320</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
@@ -3433,7 +3433,7 @@
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t>Columna podrida en la base</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I40" t="n">
@@ -3446,7 +3446,7 @@
       </c>
       <c r="K40" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L40" t="inlineStr">
@@ -3455,46 +3455,46 @@
         </is>
       </c>
       <c r="M40" t="n">
-        <v>-58.448993</v>
+        <v>-58.448523</v>
       </c>
       <c r="N40" t="n">
-        <v>-34.564383</v>
+        <v>-34.62452</v>
       </c>
       <c r="O40" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P40" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>6437</t>
+          <t>6506</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>7/17/2025</t>
+          <t>7/10/2025</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>MILLER 4590</t>
+          <t>Ohiggins 1611</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>808400306</t>
+          <t>808148679</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
@@ -3509,7 +3509,7 @@
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>Columna corroida</t>
+          <t>Columna podrida en la base</t>
         </is>
       </c>
       <c r="I41" t="n">
@@ -3522,7 +3522,7 @@
       </c>
       <c r="K41" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L41" t="inlineStr">
@@ -3531,14 +3531,14 @@
         </is>
       </c>
       <c r="M41" t="n">
-        <v>-58.495482</v>
+        <v>-58.448993</v>
       </c>
       <c r="N41" t="n">
-        <v>-34.552614</v>
+        <v>-34.564383</v>
       </c>
       <c r="O41" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P41" t="inlineStr">
@@ -3550,7 +3550,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>6538</t>
+          <t>6437</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
@@ -3560,7 +3560,7 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Pedraza Manuela 4101</t>
+          <t>MILLER 4590</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
@@ -3570,7 +3570,7 @@
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>808400353</t>
+          <t>808400306</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
@@ -3585,7 +3585,7 @@
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t xml:space="preserve">Podrida en la base </t>
+          <t>Columna corroida</t>
         </is>
       </c>
       <c r="I42" t="n">
@@ -3607,10 +3607,10 @@
         </is>
       </c>
       <c r="M42" t="n">
-        <v>-58.481569</v>
+        <v>-58.495482</v>
       </c>
       <c r="N42" t="n">
-        <v>-34.559853</v>
+        <v>-34.552614</v>
       </c>
       <c r="O42" t="inlineStr">
         <is>
@@ -3626,27 +3626,27 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>7023</t>
+          <t>6538</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>7/22/2025</t>
+          <t>7/17/2025</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>ZABALA 3573</t>
+          <t>Pedraza Manuela 4101</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>808480549</t>
+          <t>808400353</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
@@ -3661,7 +3661,7 @@
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>Corroida en base para recambio entro tambien como caso 3575</t>
+          <t xml:space="preserve">Podrida en la base </t>
         </is>
       </c>
       <c r="I43" t="n">
@@ -3683,14 +3683,14 @@
         </is>
       </c>
       <c r="M43" t="n">
-        <v>-58.457522</v>
+        <v>-58.481569</v>
       </c>
       <c r="N43" t="n">
-        <v>-34.579414</v>
+        <v>-34.559853</v>
       </c>
       <c r="O43" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P43" t="inlineStr">
@@ -3702,27 +3702,27 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>6484</t>
+          <t>7023</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>7/24/2025</t>
+          <t>7/22/2025</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>URIARTE 2396</t>
+          <t>ZABALA 3573</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>808509373</t>
+          <t>808480549</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
@@ -3737,7 +3737,7 @@
       </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Corroida en base para recambio entro tambien como caso 3575</t>
         </is>
       </c>
       <c r="I44" t="n">
@@ -3759,36 +3759,36 @@
         </is>
       </c>
       <c r="M44" t="n">
-        <v>-58.423934</v>
+        <v>-58.457522</v>
       </c>
       <c r="N44" t="n">
-        <v>-34.581562</v>
+        <v>-34.579414</v>
       </c>
       <c r="O44" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P44" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>6512</t>
+          <t>6484</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>7/28/2025</t>
+          <t>7/24/2025</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>GASCON 1195</t>
+          <t>URIARTE 2396</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
@@ -3798,7 +3798,7 @@
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>808571975</t>
+          <t>808509373</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
@@ -3835,10 +3835,10 @@
         </is>
       </c>
       <c r="M45" t="n">
-        <v>-58.423127</v>
+        <v>-58.423934</v>
       </c>
       <c r="N45" t="n">
-        <v>-34.596476</v>
+        <v>-34.581562</v>
       </c>
       <c r="O45" t="inlineStr">
         <is>
@@ -3854,7 +3854,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>6519</t>
+          <t>6512</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
@@ -3864,7 +3864,7 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>SALGUERO, JERONIMO 2874</t>
+          <t>GASCON 1195</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
@@ -3874,7 +3874,7 @@
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>808571977</t>
+          <t>808571975</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
@@ -3889,7 +3889,7 @@
       </c>
       <c r="H46" t="inlineStr">
         <is>
-          <t>Reparar rienda</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I46" t="n">
@@ -3897,7 +3897,7 @@
       </c>
       <c r="J46" t="inlineStr">
         <is>
-          <t>Tensor</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K46" t="inlineStr">
@@ -3907,14 +3907,14 @@
       </c>
       <c r="L46" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M46" t="n">
-        <v>-58.407256</v>
+        <v>-58.423127</v>
       </c>
       <c r="N46" t="n">
-        <v>-34.578976</v>
+        <v>-34.596476</v>
       </c>
       <c r="O46" t="inlineStr">
         <is>
@@ -3930,27 +3930,27 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>-538</t>
+          <t>6519</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>7/31/2025</t>
+          <t>7/28/2025</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Malabia 964</t>
+          <t>SALGUERO, JERONIMO 2874</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>808609237</t>
+          <t>808571977</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
@@ -3965,7 +3965,7 @@
       </c>
       <c r="H47" t="inlineStr">
         <is>
-          <t>Cambiar poste mal estado por PRFV</t>
+          <t>Reparar rienda</t>
         </is>
       </c>
       <c r="I47" t="n">
@@ -3973,7 +3973,7 @@
       </c>
       <c r="J47" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Tensor</t>
         </is>
       </c>
       <c r="K47" t="inlineStr">
@@ -3983,14 +3983,14 @@
       </c>
       <c r="L47" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M47" t="n">
-        <v>-58.433634</v>
+        <v>-58.407256</v>
       </c>
       <c r="N47" t="n">
-        <v>-34.595018</v>
+        <v>-34.578976</v>
       </c>
       <c r="O47" t="inlineStr">
         <is>
@@ -4006,27 +4006,27 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>-547</t>
+          <t>-538</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>8/6/2025</t>
+          <t>7/31/2025</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Habana 4210</t>
+          <t>Malabia 964</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>808733921</t>
+          <t>808609237</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
@@ -4041,7 +4041,7 @@
       </c>
       <c r="H48" t="inlineStr">
         <is>
-          <t>Cambiar poste dañado</t>
+          <t>Cambiar poste mal estado por PRFV</t>
         </is>
       </c>
       <c r="I48" t="n">
@@ -4063,46 +4063,46 @@
         </is>
       </c>
       <c r="M48" t="n">
-        <v>-58.515873</v>
+        <v>-58.433634</v>
       </c>
       <c r="N48" t="n">
-        <v>-34.599425</v>
+        <v>-34.595018</v>
       </c>
       <c r="O48" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P48" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>6906</t>
+          <t>-547</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>8/12/2025</t>
+          <t>8/6/2025</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>MOSCONI GENERAL AV. 3163</t>
+          <t>Habana 4210</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>808918685</t>
+          <t>808733921</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
@@ -4117,7 +4117,7 @@
       </c>
       <c r="H49" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambiar poste dañado</t>
         </is>
       </c>
       <c r="I49" t="n">
@@ -4135,14 +4135,14 @@
       </c>
       <c r="L49" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M49" t="n">
-        <v>-58.505731</v>
+        <v>-58.515873</v>
       </c>
       <c r="N49" t="n">
-        <v>-34.588316</v>
+        <v>-34.599425</v>
       </c>
       <c r="O49" t="inlineStr">
         <is>
@@ -4158,7 +4158,7 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>6910</t>
+          <t>6906</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
@@ -4168,17 +4168,17 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>RIVAS, GRAL. 2345</t>
+          <t>MOSCONI GENERAL AV. 3163</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>808918698</t>
+          <t>808918685</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
@@ -4193,7 +4193,7 @@
       </c>
       <c r="H50" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I50" t="n">
@@ -4215,10 +4215,10 @@
         </is>
       </c>
       <c r="M50" t="n">
-        <v>-58.482497</v>
+        <v>-58.505731</v>
       </c>
       <c r="N50" t="n">
-        <v>-34.598714</v>
+        <v>-34.588316</v>
       </c>
       <c r="O50" t="inlineStr">
         <is>
@@ -4234,7 +4234,7 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>6928</t>
+          <t>6910</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
@@ -4244,17 +4244,17 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>ALBARELLOS AV. 3101</t>
+          <t>RIVAS, GRAL. 2345</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>808918710</t>
+          <t>808918698</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
@@ -4269,7 +4269,7 @@
       </c>
       <c r="H51" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I51" t="n">
@@ -4291,10 +4291,10 @@
         </is>
       </c>
       <c r="M51" t="n">
-        <v>-58.512623</v>
+        <v>-58.482497</v>
       </c>
       <c r="N51" t="n">
-        <v>-34.579137</v>
+        <v>-34.598714</v>
       </c>
       <c r="O51" t="inlineStr">
         <is>
@@ -4310,7 +4310,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>-550</t>
+          <t>6928</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
@@ -4320,17 +4320,17 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>Fitz roy 267</t>
+          <t>ALBARELLOS AV. 3101</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>808918720</t>
+          <t>808918710</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
@@ -4345,7 +4345,7 @@
       </c>
       <c r="H52" t="inlineStr">
         <is>
-          <t>Aplomar columna</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I52" t="n">
@@ -4367,10 +4367,10 @@
         </is>
       </c>
       <c r="M52" t="n">
-        <v>-58.451378</v>
+        <v>-58.512623</v>
       </c>
       <c r="N52" t="n">
-        <v>-34.596195</v>
+        <v>-34.579137</v>
       </c>
       <c r="O52" t="inlineStr">
         <is>
@@ -4386,27 +4386,27 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>6943</t>
+          <t>-550</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>8/14/2025</t>
+          <t>8/12/2025</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>SUPERI 1459</t>
+          <t>Fitz roy 267</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>808972965</t>
+          <t>808918720</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
@@ -4421,7 +4421,7 @@
       </c>
       <c r="H53" t="inlineStr">
         <is>
-          <t>Poste con base quebrada ver si es posible desmonte</t>
+          <t>Aplomar columna</t>
         </is>
       </c>
       <c r="I53" t="n">
@@ -4429,7 +4429,7 @@
       </c>
       <c r="J53" t="inlineStr">
         <is>
-          <t>Desmonte</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K53" t="inlineStr">
@@ -4439,18 +4439,18 @@
       </c>
       <c r="L53" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M53" t="n">
-        <v>-58.460834</v>
+        <v>-58.451378</v>
       </c>
       <c r="N53" t="n">
-        <v>-34.573753</v>
+        <v>-34.596195</v>
       </c>
       <c r="O53" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P53" t="inlineStr">
@@ -4462,7 +4462,7 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>6971</t>
+          <t>6943</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
@@ -4472,17 +4472,17 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>MAURE 1594</t>
+          <t>SUPERI 1459</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>ICD30754530</t>
+          <t>808972965</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
@@ -4497,7 +4497,7 @@
       </c>
       <c r="H54" t="inlineStr">
         <is>
-          <t>Desmontar columna</t>
+          <t>Poste con base quebrada ver si es posible desmonte</t>
         </is>
       </c>
       <c r="I54" t="n">
@@ -4505,7 +4505,7 @@
       </c>
       <c r="J54" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Desmonte</t>
         </is>
       </c>
       <c r="K54" t="inlineStr">
@@ -4515,40 +4515,40 @@
       </c>
       <c r="L54" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M54" t="n">
-        <v>-58.435072</v>
+        <v>-58.460834</v>
       </c>
       <c r="N54" t="n">
-        <v>-34.565732</v>
+        <v>-34.573753</v>
       </c>
       <c r="O54" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P54" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>7000</t>
+          <t>6971</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>8/20/2025</t>
+          <t>8/14/2025</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>SCALABRINI ORTIZ, RAUL AV. 2106</t>
+          <t>MAURE 1594</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
@@ -4558,7 +4558,7 @@
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>809065867</t>
+          <t>ICD30754530</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
@@ -4573,7 +4573,7 @@
       </c>
       <c r="H55" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Desmontar columna</t>
         </is>
       </c>
       <c r="I55" t="n">
@@ -4595,10 +4595,10 @@
         </is>
       </c>
       <c r="M55" t="n">
-        <v>-58.420109</v>
+        <v>-58.435072</v>
       </c>
       <c r="N55" t="n">
-        <v>-34.58764</v>
+        <v>-34.565732</v>
       </c>
       <c r="O55" t="inlineStr">
         <is>
@@ -4614,7 +4614,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>7003</t>
+          <t>7000</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
@@ -4624,17 +4624,17 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>MELIAN AV. 2576</t>
+          <t>SCALABRINI ORTIZ, RAUL AV. 2106</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>809065874</t>
+          <t>809065867</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
@@ -4671,46 +4671,46 @@
         </is>
       </c>
       <c r="M56" t="n">
-        <v>-58.471943</v>
+        <v>-58.420109</v>
       </c>
       <c r="N56" t="n">
-        <v>-34.564948</v>
+        <v>-34.58764</v>
       </c>
       <c r="O56" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P56" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>-559</t>
+          <t>7003</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>8/21/2025</t>
+          <t>8/20/2025</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>Av. Del Libertador 6736</t>
+          <t>MELIAN AV. 2576</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>809098713</t>
+          <t>809065874</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
@@ -4747,14 +4747,14 @@
         </is>
       </c>
       <c r="M57" t="n">
-        <v>-58.453398</v>
+        <v>-58.471943</v>
       </c>
       <c r="N57" t="n">
-        <v>-34.550238</v>
+        <v>-34.564948</v>
       </c>
       <c r="O57" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P57" t="inlineStr">
@@ -4766,17 +4766,17 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>5503</t>
+          <t>-559</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>8/22/2025</t>
+          <t>8/21/2025</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>CRAMER AV. 1771</t>
+          <t>Av. Del Libertador 6736</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
@@ -4786,7 +4786,7 @@
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>809102564</t>
+          <t>809098713</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
@@ -4801,7 +4801,7 @@
       </c>
       <c r="H58" t="inlineStr">
         <is>
-      